<commit_message>
feat: consolidate ingestSQL calls (#3)
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="204">
   <si>
     <t>ingest_session_id</t>
   </si>
@@ -57,7 +57,235 @@
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
   </si>
   <si>
-    <t>7bab389e-54af-5a13-a39f-079abdc73a48</t>
+    <t>168a34c7-d043-5ec4-a84a-c961f1a301ef</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_admin_demographic</t>
+  </si>
+  <si>
+    <t>1931dfcc-e8fc-597d-b1bc-65b4287e6fdf</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_screening</t>
+  </si>
+  <si>
+    <t>f90e1b86-1420-44d6-b5cc-30eaa9bf35b8</t>
+  </si>
+  <si>
+    <t>Missing Column</t>
+  </si>
+  <si>
+    <t>Required column PAT_MRN_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_MRN_ID"</t>
+  </si>
+  <si>
+    <t>47cae7da-f34b-4f30-a4a7-40cddb1f6edf</t>
+  </si>
+  <si>
+    <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
+  </si>
+  <si>
+    <t>ebee1f4a-ee7c-479c-8b07-89758cb1d73e</t>
+  </si>
+  <si>
+    <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
+  </si>
+  <si>
+    <t>87b75ddc-9bd3-4e0b-a329-8630956f260a</t>
+  </si>
+  <si>
+    <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
+  </si>
+  <si>
+    <t>71122c39-abfa-4f7a-a052-7b12dbc85209</t>
+  </si>
+  <si>
+    <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
+  </si>
+  <si>
+    <t>4d3ec647-4c81-4b82-9c4a-97c46b79da94</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>732ff8b5-04f4-4f64-a79e-3b70904ddc77</t>
+  </si>
+  <si>
+    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>f525abde-7b87-4938-b10f-0ba22a181d66</t>
+  </si>
+  <si>
+    <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
+  </si>
+  <si>
+    <t>cdcfa698-2b10-488e-b38b-5a0922968fcf</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>0436f804-5fa3-4376-a333-bdd660a1dcbf</t>
+  </si>
+  <si>
+    <t>Required column RECORDED_TIME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "RECORDED_TIME"</t>
+  </si>
+  <si>
+    <t>6b79ac35-5a81-404d-a6f4-0ac2d842180b</t>
+  </si>
+  <si>
+    <t>Required column QUESTION is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION"</t>
+  </si>
+  <si>
+    <t>ac240c17-7a9d-4b3f-9a57-0a7bab948de9</t>
+  </si>
+  <si>
+    <t>Required column MEAS_VALUE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEAS_VALUE"</t>
+  </si>
+  <si>
+    <t>65cb6487-0370-4c9f-a8c8-4fdcc72b5481</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION_CODE"</t>
+  </si>
+  <si>
+    <t>8ca30133-4a62-483b-adb5-73af19efffc0</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>1140d439-6c92-4031-97a7-11efb15a0b8f</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ANSWER_CODE"</t>
+  </si>
+  <si>
+    <t>806433ee-9244-4fa9-ae48-4241b64c73bb</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>c0a83f0f-8258-4839-956a-cc11924e897c</t>
+  </si>
+  <si>
+    <t>Required column SDOH_DOMAIN is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SDOH_DOMAIN"</t>
+  </si>
+  <si>
+    <t>ee11d8bd-5e1e-418d-9212-aba3d1464169</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>eeb5f9e9-640c-4a2a-89a1-ca18e0d1e2cc</t>
+  </si>
+  <si>
+    <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
+  </si>
+  <si>
+    <t>05608383-5739-4536-9956-0ee132c81df5</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>effc0021-0518-46f0-bd24-51c18ea2ef7c</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_q_e_admin_data</t>
+  </si>
+  <si>
+    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
@@ -66,10 +294,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>1d62090e-421c-4d2f-a79d-42d02218cd13</t>
-  </si>
-  <si>
-    <t>Missing Column</t>
+    <t>5fdee1e6-35b0-4957-a97a-144f6047a5fc</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -78,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>eb6c2120-4d30-4d74-b23b-8c2a111ab2ec</t>
+    <t>f6df354f-de42-45e8-b911-d8003e95da0a</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -87,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>adaedffc-0cda-43e9-abb8-1f7de065c73a</t>
+    <t>195b5ec4-0e29-4f0f-b947-b4aebf30db7e</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -96,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>76ffffb9-5275-4b4e-858f-f7e8278b8aad</t>
+    <t>ce61d386-d74e-4d57-88cb-c2d4841f2850</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -105,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>6433e280-0673-4eb4-973b-8edaac741f57</t>
+    <t>c870238a-6582-4143-b011-2bbcb815beba</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -114,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>84a0a784-467f-4b2e-a5f6-01ccaa2a51fc</t>
+    <t>fea81780-cea3-4276-b8c5-f614ddcae93c</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -123,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>8d3ba017-481f-4394-a158-d2fc5b8ab954</t>
+    <t>94b9747a-5851-416c-8dd0-c07a2a2fc357</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -132,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>3e68fef6-ccf4-48fe-a283-704e4eb75374</t>
+    <t>14e733df-0136-412e-aab0-feb8f220833f</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -141,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>cf377023-2d73-4db6-a120-86c867adaa99</t>
+    <t>06e8f683-8b7e-4282-8b3c-bba186c5d980</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -150,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>cffbab36-7f80-4846-a545-bcdf744ab69a</t>
+    <t>0186351e-151e-4b24-9d17-37a028982787</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -159,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>eceae89b-e0f5-4e6a-bc90-cf2ff7876032</t>
+    <t>78cc5f6b-1d37-49a9-a6a7-ff657c93a1dc</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -168,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>c436e2aa-31d9-4f87-9235-869999bb9cc3</t>
+    <t>353be5f1-42b4-4c21-8247-0058b5faef00</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -177,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>1dbe4f19-f975-459e-a8ae-813947feedd9</t>
+    <t>a5665d88-1b21-4fc5-969d-64b4e8325f6d</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -186,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>991cc8c7-6d8a-4cd1-97d6-c8cacd23ecd9</t>
+    <t>4862b8c6-ee43-41bf-87d8-c513a8df0af4</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -195,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>789dad0b-db42-4988-acaf-fd2ca520b223</t>
+    <t>c19e097c-e4db-41e1-bce2-b67c91de1f18</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -204,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>bb3fa37a-c79b-4aad-ab9a-4a2e072b44a7</t>
+    <t>e2a59c76-55b4-40b1-965f-8211316f5bc5</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -213,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>439fe7e6-7821-4af7-98ca-dbef52726fe6</t>
+    <t>3e58c098-cf2d-45d5-8e9b-5407e46f61c8</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -222,7 +447,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>c496d27a-cda0-40c7-858d-b0ed2845f744</t>
+    <t>77d0008e-108f-46b5-8ea0-ea43e7606017</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -231,7 +456,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>14fddde7-e2a1-4ca8-a39f-cee1beefcdc5</t>
+    <t>f25ac8c1-ef7c-4600-9858-271ef4f501d8</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -240,7 +465,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>ee301881-6874-4465-86cd-57003de5b101</t>
+    <t>680e74ef-c3a1-4247-9ac4-e950c9b6a540</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -249,7 +474,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>7879dbd7-da51-41f3-a35d-0387dc732480</t>
+    <t>f0c7a585-20a6-4e4e-892f-82c31eb69047</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -258,7 +483,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>1931dfcc-e8fc-597d-b1bc-65b4287e6fdf</t>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
@@ -267,7 +492,7 @@
     <t>ERROR</t>
   </si>
   <si>
-    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
   </si>
   <si>
     <t>Sheet Missing</t>
@@ -276,169 +501,25 @@
     <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
-  </si>
-  <si>
-    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
-  </si>
-  <si>
-    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
   </si>
   <si>
     <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>47277588-99e8-59f5-8384-b24344a86073</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_admin_demographic</t>
-  </si>
-  <si>
-    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
-  </si>
-  <si>
-    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_screening</t>
-  </si>
-  <si>
-    <t>a5efdefa-01df-4c18-a9af-bc1e8a7963e1</t>
-  </si>
-  <si>
-    <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
-  </si>
-  <si>
-    <t>9f8cc74d-65b7-4557-ba38-07aa21267699</t>
-  </si>
-  <si>
-    <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
-  </si>
-  <si>
-    <t>985842e7-03b6-4d7f-9fae-f5fcf95e6c35</t>
-  </si>
-  <si>
-    <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
-  </si>
-  <si>
-    <t>b37f730f-42e2-46c4-8263-bccbb681babd</t>
-  </si>
-  <si>
-    <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
-  </si>
-  <si>
-    <t>36eac8e0-d4c4-4ae6-af24-a4ca713f075c</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>b9a5d5ef-591d-42c4-b695-39b8345176c4</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>1373859a-be5b-44f1-b530-c5e24d016f3b</t>
-  </si>
-  <si>
-    <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
-  </si>
-  <si>
-    <t>124d2172-198a-401f-92db-cacb6e72799d</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>b709f71b-e3cb-4ba4-9960-c366e0a15fcc</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>7c3a5569-2b46-4935-bfa4-ed1cc0f2209c</t>
-  </si>
-  <si>
-    <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
-  </si>
-  <si>
-    <t>db99bb24-cd1f-4384-bae1-7f88124cda3e</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>15535506-368a-4157-bef7-88d1fd779d0d</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
-    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_q_e_admin_data</t>
-  </si>
-  <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
-  </si>
-  <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
-  </si>
-  <si>
-    <t>168a34c7-d043-5ec4-a84a-c961f1a301ef</t>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-12-12-2023-valid.csv</t>
@@ -447,7 +528,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>06c3b45a-4aff-45fd-ba15-80f369996a49</t>
+    <t>cd8b67a7-c8dc-4f31-a2f3-f91610e85683</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -465,82 +546,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>626c1816-cd7d-4505-99aa-bf71cebe592b</t>
-  </si>
-  <si>
-    <t>b885a317-be20-4ee7-b874-4c6ca1ff935b</t>
-  </si>
-  <si>
-    <t>222c7bd8-d4a7-4778-98d3-5e7f1e31744f</t>
-  </si>
-  <si>
-    <t>c16ed03a-195a-452f-b68e-99821d54a163</t>
-  </si>
-  <si>
-    <t>8aac74a7-c3ba-418e-a17e-b1ff95542e1a</t>
-  </si>
-  <si>
-    <t>15961aaf-b2a2-4efb-b716-778e397600d0</t>
-  </si>
-  <si>
-    <t>a190a2d6-c96e-412d-9591-1c4d44ba5e0d</t>
-  </si>
-  <si>
-    <t>32aaa5c0-d845-4a59-83ef-a643a21da229</t>
-  </si>
-  <si>
-    <t>d1cb4c90-c404-4fc7-adb7-4fb05ff6477b</t>
-  </si>
-  <si>
-    <t>5aaa57a7-e79f-4f44-b75a-9eefa9bd6bdb</t>
-  </si>
-  <si>
-    <t>18b4e536-e654-4cbb-8e5f-547260c1beae</t>
-  </si>
-  <si>
-    <t>199b5c69-3948-44af-8d94-d993e1d36f7f</t>
-  </si>
-  <si>
-    <t>82c54791-63ac-4efb-aa45-cee26dc17ee7</t>
-  </si>
-  <si>
-    <t>fc7bf867-c79c-4990-a622-aa125c7d0a94</t>
-  </si>
-  <si>
-    <t>b8283c56-2cbd-4e5e-a403-13a45e9e81a4</t>
-  </si>
-  <si>
-    <t>114d6152-7f13-4572-8597-f4161c51bea5</t>
-  </si>
-  <si>
-    <t>f5258407-2a4d-4301-bf82-15e3815523fa</t>
-  </si>
-  <si>
-    <t>bb04e070-c623-4e44-a208-fb2c70a1c33a</t>
-  </si>
-  <si>
-    <t>c506c02f-89f7-4c97-9ec0-860845a6b10f</t>
-  </si>
-  <si>
-    <t>66d3c8d8-1edc-414f-9e88-25834f83988a</t>
-  </si>
-  <si>
-    <t>ae54ba20-9b7f-4589-92af-99b7aafd4db5</t>
-  </si>
-  <si>
-    <t>f0dd4673-95c0-4d59-996f-a5bd4db0353b</t>
-  </si>
-  <si>
-    <t>ae3dc5f0-cfed-4b18-b458-16a024daed1c</t>
-  </si>
-  <si>
-    <t>75c85a15-8c82-4ee6-b237-c448e18e2eea</t>
-  </si>
-  <si>
-    <t>e7e8f864-6582-4dc7-8aca-5996e10ac2ed</t>
-  </si>
-  <si>
-    <t>b2ff6f13-91e7-4540-b4d9-8ae20c2d2153</t>
+    <t>f72fdf75-d3b3-4add-848a-191cc035c60d</t>
+  </si>
+  <si>
+    <t>75eb00b8-9402-409f-8983-1f0e97d3e4c4</t>
+  </si>
+  <si>
+    <t>55dc8960-6a04-429f-b1a3-b3fce6c6e75c</t>
+  </si>
+  <si>
+    <t>5ebc4583-ad62-47c7-9996-ab750dd08811</t>
+  </si>
+  <si>
+    <t>495b620f-285c-4b76-9ce8-a99f18f17a65</t>
+  </si>
+  <si>
+    <t>dc0c62b3-1162-4db7-a781-b1585589bfee</t>
+  </si>
+  <si>
+    <t>cd8c4076-948d-4420-967e-3504453d5955</t>
+  </si>
+  <si>
+    <t>c95612d9-a1cc-4bf3-8a42-dc782ff1d4bd</t>
+  </si>
+  <si>
+    <t>6dbd854a-95c5-461c-91b2-644d4919eecc</t>
+  </si>
+  <si>
+    <t>3327b9f7-d3d2-45cd-ac8b-f5b070a0483e</t>
+  </si>
+  <si>
+    <t>4009082a-e537-4eaf-a4c4-8362b8f78c7f</t>
+  </si>
+  <si>
+    <t>257d5876-1625-4393-a761-bd02a6abe550</t>
+  </si>
+  <si>
+    <t>bded3d74-be9a-42bc-aa8d-df54cdc25a38</t>
+  </si>
+  <si>
+    <t>86c1d72f-25a5-4f73-bac9-2914368dc3b5</t>
+  </si>
+  <si>
+    <t>fbd0bbda-fe05-4df4-8c5d-8c1e6f4a6363</t>
+  </si>
+  <si>
+    <t>28eeb640-ba4e-465a-8880-7217b4b9ec89</t>
+  </si>
+  <si>
+    <t>35066299-a398-424a-b398-39c25f325953</t>
+  </si>
+  <si>
+    <t>fccaf294-c9e8-4ec8-9938-4e13bf3e3b84</t>
+  </si>
+  <si>
+    <t>be56f5af-3490-4e82-a45b-d8863a71c6cd</t>
+  </si>
+  <si>
+    <t>c4f1c30d-06e9-437c-b406-d28e0e7c48af</t>
+  </si>
+  <si>
+    <t>890e4028-b12a-4cb6-ae4d-1ab6d44de8cd</t>
+  </si>
+  <si>
+    <t>60b35e5f-ed06-4a9c-83c7-b9d59042d715</t>
+  </si>
+  <si>
+    <t>31dbdff6-7e6b-4101-b186-c900de4ade12</t>
+  </si>
+  <si>
+    <t>5c4294b9-0d06-4e7e-8a8c-34932c7f829f</t>
+  </si>
+  <si>
+    <t>69cdacb8-5a84-4b02-9105-27c922ea59fa</t>
+  </si>
+  <si>
+    <t>2c1534ef-9073-4744-b9f0-4379cb69be52</t>
   </si>
 </sst>
 </file>
@@ -679,8 +760,8 @@
       <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
-        <v>21</v>
+      <c r="L2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
@@ -688,25 +769,25 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -714,25 +795,25 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -740,25 +821,25 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -766,25 +847,25 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -792,25 +873,25 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
@@ -818,25 +899,25 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9">
@@ -844,25 +925,25 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
@@ -870,25 +951,25 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
@@ -896,25 +977,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12">
@@ -922,25 +1003,25 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -948,25 +1029,25 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -974,25 +1055,25 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
@@ -1000,25 +1081,25 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16">
@@ -1026,25 +1107,25 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="M16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17">
@@ -1052,25 +1133,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18">
@@ -1078,25 +1159,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19">
@@ -1104,25 +1185,25 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
         <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
@@ -1130,25 +1211,25 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21">
@@ -1156,25 +1237,25 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
@@ -1182,25 +1263,25 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D22" t="s">
         <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M22" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23">
@@ -1208,25 +1289,25 @@
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
         <v>84</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" t="s">
         <v>85</v>
       </c>
-      <c r="H23" t="s">
+      <c r="M23" t="s">
         <v>86</v>
-      </c>
-      <c r="I23" t="s">
-        <v>87</v>
-      </c>
-      <c r="L23" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="24">
@@ -1234,25 +1315,25 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
         <v>88</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" t="s">
-        <v>84</v>
       </c>
       <c r="G24" t="s">
         <v>89</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="I24" t="s">
         <v>90</v>
       </c>
       <c r="L24" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25">
@@ -1263,22 +1344,22 @@
         <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H25" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>93</v>
-      </c>
-      <c r="L25" t="s">
-        <v>83</v>
+        <v>95</v>
+      </c>
+      <c r="M25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="26">
@@ -1286,25 +1367,25 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G26" t="s">
         <v>97</v>
       </c>
       <c r="H26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
         <v>98</v>
       </c>
-      <c r="I26" t="s">
+      <c r="M26" t="s">
         <v>99</v>
-      </c>
-      <c r="L26" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27">
@@ -1312,25 +1393,25 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" t="s">
         <v>100</v>
       </c>
-      <c r="D27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" t="s">
         <v>101</v>
       </c>
-      <c r="G27" t="s">
+      <c r="M27" t="s">
         <v>102</v>
-      </c>
-      <c r="H27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27" t="s">
-        <v>103</v>
-      </c>
-      <c r="M27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28">
@@ -1338,25 +1419,25 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" t="s">
+        <v>104</v>
+      </c>
+      <c r="M28" t="s">
         <v>105</v>
-      </c>
-      <c r="H28" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" t="s">
-        <v>106</v>
-      </c>
-      <c r="M28" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="29">
@@ -1364,25 +1445,25 @@
         <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G29" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" t="s">
+        <v>107</v>
+      </c>
+      <c r="M29" t="s">
         <v>108</v>
-      </c>
-      <c r="H29" t="s">
-        <v>19</v>
-      </c>
-      <c r="I29" t="s">
-        <v>109</v>
-      </c>
-      <c r="M29" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="30">
@@ -1390,25 +1471,25 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G30" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" t="s">
+        <v>110</v>
+      </c>
+      <c r="M30" t="s">
         <v>111</v>
-      </c>
-      <c r="H30" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" t="s">
-        <v>112</v>
-      </c>
-      <c r="M30" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="31">
@@ -1416,25 +1497,25 @@
         <v>14</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G31" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>113</v>
+      </c>
+      <c r="M31" t="s">
         <v>114</v>
-      </c>
-      <c r="H31" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" t="s">
-        <v>115</v>
-      </c>
-      <c r="M31" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="32">
@@ -1442,25 +1523,25 @@
         <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G32" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" t="s">
+        <v>116</v>
+      </c>
+      <c r="M32" t="s">
         <v>117</v>
-      </c>
-      <c r="H32" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" t="s">
-        <v>118</v>
-      </c>
-      <c r="M32" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="33">
@@ -1468,25 +1549,25 @@
         <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" t="s">
+        <v>119</v>
+      </c>
+      <c r="M33" t="s">
         <v>120</v>
-      </c>
-      <c r="H33" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" t="s">
-        <v>121</v>
-      </c>
-      <c r="M33" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34">
@@ -1494,25 +1575,25 @@
         <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" t="s">
+        <v>122</v>
+      </c>
+      <c r="M34" t="s">
         <v>123</v>
-      </c>
-      <c r="H34" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" t="s">
-        <v>124</v>
-      </c>
-      <c r="M34" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="35">
@@ -1520,25 +1601,25 @@
         <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E35" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H35" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" t="s">
+        <v>125</v>
+      </c>
+      <c r="M35" t="s">
         <v>126</v>
-      </c>
-      <c r="H35" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" t="s">
-        <v>127</v>
-      </c>
-      <c r="M35" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="36">
@@ -1546,25 +1627,25 @@
         <v>14</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E36" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G36" t="s">
+        <v>127</v>
+      </c>
+      <c r="H36" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" t="s">
+        <v>128</v>
+      </c>
+      <c r="M36" t="s">
         <v>129</v>
-      </c>
-      <c r="H36" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" t="s">
-        <v>130</v>
-      </c>
-      <c r="M36" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="37">
@@ -1572,25 +1653,25 @@
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G37" t="s">
+        <v>130</v>
+      </c>
+      <c r="H37" t="s">
+        <v>24</v>
+      </c>
+      <c r="I37" t="s">
+        <v>131</v>
+      </c>
+      <c r="M37" t="s">
         <v>132</v>
-      </c>
-      <c r="H37" t="s">
-        <v>19</v>
-      </c>
-      <c r="I37" t="s">
-        <v>133</v>
-      </c>
-      <c r="M37" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="38">
@@ -1598,25 +1679,25 @@
         <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E38" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G38" t="s">
+        <v>133</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I38" t="s">
+        <v>134</v>
+      </c>
+      <c r="M38" t="s">
         <v>135</v>
-      </c>
-      <c r="H38" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38" t="s">
-        <v>136</v>
-      </c>
-      <c r="M38" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="39">
@@ -1624,25 +1705,25 @@
         <v>14</v>
       </c>
       <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H39" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" t="s">
+        <v>137</v>
+      </c>
+      <c r="M39" t="s">
         <v>138</v>
-      </c>
-      <c r="D39" t="s">
-        <v>95</v>
-      </c>
-      <c r="E39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G39" t="s">
-        <v>140</v>
-      </c>
-      <c r="H39" t="s">
-        <v>98</v>
-      </c>
-      <c r="I39" t="s">
-        <v>141</v>
-      </c>
-      <c r="L39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="40">
@@ -1650,34 +1731,25 @@
         <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="E40" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="G40" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H40" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
       <c r="I40" t="s">
-        <v>147</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40" t="s">
-        <v>148</v>
-      </c>
-      <c r="L40" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="M40" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41">
@@ -1685,34 +1757,25 @@
         <v>14</v>
       </c>
       <c r="C41" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" t="s">
         <v>142</v>
       </c>
-      <c r="D41" t="s">
+      <c r="H41" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" t="s">
         <v>143</v>
       </c>
-      <c r="E41" t="s">
+      <c r="M41" t="s">
         <v>144</v>
-      </c>
-      <c r="G41" t="s">
-        <v>151</v>
-      </c>
-      <c r="H41" t="s">
-        <v>146</v>
-      </c>
-      <c r="I41" t="s">
-        <v>147</v>
-      </c>
-      <c r="J41">
-        <v>2</v>
-      </c>
-      <c r="K41" t="s">
-        <v>148</v>
-      </c>
-      <c r="L41" t="s">
-        <v>149</v>
-      </c>
-      <c r="M41" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="42">
@@ -1720,34 +1783,25 @@
         <v>14</v>
       </c>
       <c r="C42" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="G42" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H42" t="s">
+        <v>24</v>
+      </c>
+      <c r="I42" t="s">
         <v>146</v>
       </c>
-      <c r="I42" t="s">
+      <c r="M42" t="s">
         <v>147</v>
-      </c>
-      <c r="J42">
-        <v>3</v>
-      </c>
-      <c r="K42" t="s">
-        <v>148</v>
-      </c>
-      <c r="L42" t="s">
-        <v>149</v>
-      </c>
-      <c r="M42" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="43">
@@ -1755,30 +1809,21 @@
         <v>14</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="G43" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H43" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
       <c r="I43" t="s">
-        <v>147</v>
-      </c>
-      <c r="J43">
-        <v>4</v>
-      </c>
-      <c r="K43" t="s">
-        <v>148</v>
-      </c>
-      <c r="L43" t="s">
         <v>149</v>
       </c>
       <c r="M43" t="s">
@@ -1790,34 +1835,25 @@
         <v>14</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="E44" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="G44" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H44" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
       <c r="I44" t="s">
-        <v>147</v>
-      </c>
-      <c r="J44">
-        <v>5</v>
-      </c>
-      <c r="K44" t="s">
-        <v>148</v>
-      </c>
-      <c r="L44" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="M44" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45">
@@ -1825,34 +1861,25 @@
         <v>14</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="E45" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="G45" t="s">
+        <v>154</v>
+      </c>
+      <c r="H45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" t="s">
         <v>155</v>
       </c>
-      <c r="H45" t="s">
-        <v>146</v>
-      </c>
-      <c r="I45" t="s">
-        <v>147</v>
-      </c>
-      <c r="J45">
-        <v>6</v>
-      </c>
-      <c r="K45" t="s">
-        <v>148</v>
-      </c>
-      <c r="L45" t="s">
-        <v>149</v>
-      </c>
       <c r="M45" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46">
@@ -1860,34 +1887,25 @@
         <v>14</v>
       </c>
       <c r="C46" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="G46" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H46" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="I46" t="s">
-        <v>147</v>
-      </c>
-      <c r="J46">
-        <v>7</v>
-      </c>
-      <c r="K46" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="L46" t="s">
-        <v>149</v>
-      </c>
-      <c r="M46" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47">
@@ -1895,34 +1913,25 @@
         <v>14</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="G47" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="H47" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="I47" t="s">
-        <v>147</v>
-      </c>
-      <c r="J47">
-        <v>8</v>
-      </c>
-      <c r="K47" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="L47" t="s">
-        <v>149</v>
-      </c>
-      <c r="M47" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48">
@@ -1930,34 +1939,25 @@
         <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="E48" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="G48" t="s">
+        <v>167</v>
+      </c>
+      <c r="H48" t="s">
+        <v>161</v>
+      </c>
+      <c r="I48" t="s">
+        <v>168</v>
+      </c>
+      <c r="L48" t="s">
         <v>158</v>
-      </c>
-      <c r="H48" t="s">
-        <v>146</v>
-      </c>
-      <c r="I48" t="s">
-        <v>147</v>
-      </c>
-      <c r="J48">
-        <v>9</v>
-      </c>
-      <c r="K48" t="s">
-        <v>148</v>
-      </c>
-      <c r="L48" t="s">
-        <v>149</v>
-      </c>
-      <c r="M48" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="49">
@@ -1965,34 +1965,34 @@
         <v>14</v>
       </c>
       <c r="C49" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E49" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G49" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="H49" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I49" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J49">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K49" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L49" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M49" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50">
@@ -2000,34 +2000,34 @@
         <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E50" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G50" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="H50" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I50" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J50">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K50" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L50" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M50" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51">
@@ -2035,34 +2035,34 @@
         <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E51" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G51" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
       <c r="H51" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I51" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J51">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="K51" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L51" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M51" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52">
@@ -2070,34 +2070,34 @@
         <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E52" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G52" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="H52" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I52" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J52">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K52" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L52" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M52" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53">
@@ -2105,34 +2105,34 @@
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D53" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E53" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G53" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="H53" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I53" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J53">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="K53" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L53" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M53" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="54">
@@ -2140,34 +2140,34 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E54" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G54" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="H54" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I54" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J54">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="K54" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L54" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M54" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="55">
@@ -2175,34 +2175,34 @@
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D55" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E55" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G55" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="H55" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I55" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J55">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K55" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L55" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M55" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56">
@@ -2210,34 +2210,34 @@
         <v>14</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E56" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G56" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="H56" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I56" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J56">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="K56" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L56" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M56" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57">
@@ -2245,34 +2245,34 @@
         <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E57" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G57" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="H57" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I57" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J57">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="K57" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L57" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M57" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58">
@@ -2280,34 +2280,34 @@
         <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E58" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G58" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="H58" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I58" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J58">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="K58" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L58" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M58" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59">
@@ -2315,34 +2315,34 @@
         <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G59" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="H59" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I59" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J59">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K59" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L59" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M59" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60">
@@ -2350,34 +2350,34 @@
         <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D60" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E60" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G60" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="H60" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I60" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J60">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="K60" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L60" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M60" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61">
@@ -2385,34 +2385,34 @@
         <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D61" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E61" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G61" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="H61" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I61" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J61">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="K61" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L61" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M61" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62">
@@ -2420,34 +2420,34 @@
         <v>14</v>
       </c>
       <c r="C62" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E62" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G62" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="H62" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="I62" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J62">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="K62" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L62" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M62" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63">
@@ -2455,34 +2455,34 @@
         <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E63" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G63" t="s">
+        <v>191</v>
+      </c>
+      <c r="H63" t="s">
         <v>173</v>
       </c>
-      <c r="H63" t="s">
-        <v>146</v>
-      </c>
       <c r="I63" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J63">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K63" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L63" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M63" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="64">
@@ -2490,34 +2490,34 @@
         <v>14</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D64" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E64" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G64" t="s">
+        <v>192</v>
+      </c>
+      <c r="H64" t="s">
+        <v>173</v>
+      </c>
+      <c r="I64" t="s">
         <v>174</v>
       </c>
-      <c r="H64" t="s">
-        <v>146</v>
-      </c>
-      <c r="I64" t="s">
-        <v>147</v>
-      </c>
       <c r="J64">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="K64" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="L64" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M64" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65">
@@ -2525,34 +2525,34 @@
         <v>14</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E65" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G65" t="s">
+        <v>193</v>
+      </c>
+      <c r="H65" t="s">
+        <v>173</v>
+      </c>
+      <c r="I65" t="s">
+        <v>174</v>
+      </c>
+      <c r="J65">
+        <v>17</v>
+      </c>
+      <c r="K65" t="s">
         <v>175</v>
       </c>
-      <c r="H65" t="s">
-        <v>146</v>
-      </c>
-      <c r="I65" t="s">
-        <v>147</v>
-      </c>
-      <c r="J65">
-        <v>26</v>
-      </c>
-      <c r="K65" t="s">
-        <v>148</v>
-      </c>
       <c r="L65" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="M65" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66">
@@ -2560,34 +2560,349 @@
         <v>14</v>
       </c>
       <c r="C66" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="D66" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="G66" t="s">
+        <v>194</v>
+      </c>
+      <c r="H66" t="s">
+        <v>173</v>
+      </c>
+      <c r="I66" t="s">
+        <v>174</v>
+      </c>
+      <c r="J66">
+        <v>18</v>
+      </c>
+      <c r="K66" t="s">
+        <v>175</v>
+      </c>
+      <c r="L66" t="s">
         <v>176</v>
       </c>
-      <c r="H66" t="s">
-        <v>146</v>
-      </c>
-      <c r="I66" t="s">
-        <v>147</v>
-      </c>
-      <c r="J66">
+      <c r="M66" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" t="s">
+        <v>169</v>
+      </c>
+      <c r="D67" t="s">
+        <v>170</v>
+      </c>
+      <c r="E67" t="s">
+        <v>171</v>
+      </c>
+      <c r="G67" t="s">
+        <v>195</v>
+      </c>
+      <c r="H67" t="s">
+        <v>173</v>
+      </c>
+      <c r="I67" t="s">
+        <v>174</v>
+      </c>
+      <c r="J67">
+        <v>19</v>
+      </c>
+      <c r="K67" t="s">
+        <v>175</v>
+      </c>
+      <c r="L67" t="s">
+        <v>176</v>
+      </c>
+      <c r="M67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" t="s">
+        <v>169</v>
+      </c>
+      <c r="D68" t="s">
+        <v>170</v>
+      </c>
+      <c r="E68" t="s">
+        <v>171</v>
+      </c>
+      <c r="G68" t="s">
+        <v>196</v>
+      </c>
+      <c r="H68" t="s">
+        <v>173</v>
+      </c>
+      <c r="I68" t="s">
+        <v>174</v>
+      </c>
+      <c r="J68">
+        <v>20</v>
+      </c>
+      <c r="K68" t="s">
+        <v>175</v>
+      </c>
+      <c r="L68" t="s">
+        <v>176</v>
+      </c>
+      <c r="M68" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" t="s">
+        <v>169</v>
+      </c>
+      <c r="D69" t="s">
+        <v>170</v>
+      </c>
+      <c r="E69" t="s">
+        <v>171</v>
+      </c>
+      <c r="G69" t="s">
+        <v>197</v>
+      </c>
+      <c r="H69" t="s">
+        <v>173</v>
+      </c>
+      <c r="I69" t="s">
+        <v>174</v>
+      </c>
+      <c r="J69">
+        <v>21</v>
+      </c>
+      <c r="K69" t="s">
+        <v>175</v>
+      </c>
+      <c r="L69" t="s">
+        <v>176</v>
+      </c>
+      <c r="M69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" t="s">
+        <v>169</v>
+      </c>
+      <c r="D70" t="s">
+        <v>170</v>
+      </c>
+      <c r="E70" t="s">
+        <v>171</v>
+      </c>
+      <c r="G70" t="s">
+        <v>198</v>
+      </c>
+      <c r="H70" t="s">
+        <v>173</v>
+      </c>
+      <c r="I70" t="s">
+        <v>174</v>
+      </c>
+      <c r="J70">
+        <v>22</v>
+      </c>
+      <c r="K70" t="s">
+        <v>175</v>
+      </c>
+      <c r="L70" t="s">
+        <v>176</v>
+      </c>
+      <c r="M70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" t="s">
+        <v>169</v>
+      </c>
+      <c r="D71" t="s">
+        <v>170</v>
+      </c>
+      <c r="E71" t="s">
+        <v>171</v>
+      </c>
+      <c r="G71" t="s">
+        <v>199</v>
+      </c>
+      <c r="H71" t="s">
+        <v>173</v>
+      </c>
+      <c r="I71" t="s">
+        <v>174</v>
+      </c>
+      <c r="J71">
+        <v>23</v>
+      </c>
+      <c r="K71" t="s">
+        <v>175</v>
+      </c>
+      <c r="L71" t="s">
+        <v>176</v>
+      </c>
+      <c r="M71" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" t="s">
+        <v>169</v>
+      </c>
+      <c r="D72" t="s">
+        <v>170</v>
+      </c>
+      <c r="E72" t="s">
+        <v>171</v>
+      </c>
+      <c r="G72" t="s">
+        <v>200</v>
+      </c>
+      <c r="H72" t="s">
+        <v>173</v>
+      </c>
+      <c r="I72" t="s">
+        <v>174</v>
+      </c>
+      <c r="J72">
+        <v>24</v>
+      </c>
+      <c r="K72" t="s">
+        <v>175</v>
+      </c>
+      <c r="L72" t="s">
+        <v>176</v>
+      </c>
+      <c r="M72" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" t="s">
+        <v>170</v>
+      </c>
+      <c r="E73" t="s">
+        <v>171</v>
+      </c>
+      <c r="G73" t="s">
+        <v>201</v>
+      </c>
+      <c r="H73" t="s">
+        <v>173</v>
+      </c>
+      <c r="I73" t="s">
+        <v>174</v>
+      </c>
+      <c r="J73">
+        <v>25</v>
+      </c>
+      <c r="K73" t="s">
+        <v>175</v>
+      </c>
+      <c r="L73" t="s">
+        <v>176</v>
+      </c>
+      <c r="M73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C74" t="s">
+        <v>169</v>
+      </c>
+      <c r="D74" t="s">
+        <v>170</v>
+      </c>
+      <c r="E74" t="s">
+        <v>171</v>
+      </c>
+      <c r="G74" t="s">
+        <v>202</v>
+      </c>
+      <c r="H74" t="s">
+        <v>173</v>
+      </c>
+      <c r="I74" t="s">
+        <v>174</v>
+      </c>
+      <c r="J74">
+        <v>26</v>
+      </c>
+      <c r="K74" t="s">
+        <v>175</v>
+      </c>
+      <c r="L74" t="s">
+        <v>176</v>
+      </c>
+      <c r="M74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="C75" t="s">
+        <v>169</v>
+      </c>
+      <c r="D75" t="s">
+        <v>170</v>
+      </c>
+      <c r="E75" t="s">
+        <v>171</v>
+      </c>
+      <c r="G75" t="s">
+        <v>203</v>
+      </c>
+      <c r="H75" t="s">
+        <v>173</v>
+      </c>
+      <c r="I75" t="s">
+        <v>174</v>
+      </c>
+      <c r="J75">
         <v>27</v>
       </c>
-      <c r="K66" t="s">
-        <v>148</v>
-      </c>
-      <c r="L66" t="s">
-        <v>149</v>
-      </c>
-      <c r="M66" t="s">
-        <v>150</v>
+      <c r="K75" t="s">
+        <v>175</v>
+      </c>
+      <c r="L75" t="s">
+        <v>176</v>
+      </c>
+      <c r="M75" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Introduce SQLPage #6
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -123,7 +123,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>075edff5-a4e7-4ee3-8d19-cfd113748ac0</t>
+    <t>5c3046fa-bb76-4d07-b4d7-2cdfd85193a2</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -135,7 +135,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>6ca0effe-2584-4e52-a4c8-f0419e77b764</t>
+    <t>4882c6b1-77f1-4cba-ba86-c26e062dab71</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -144,7 +144,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>48efe1e7-3744-44e3-89c2-39386800a5ce</t>
+    <t>e6139de2-edd1-4516-a7c0-8828e6a6d4b3</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -153,7 +153,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>cd51142c-2eb5-468e-bc9b-0ccb3e58bf66</t>
+    <t>948d5ddb-caef-4683-af04-a9936974d326</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -162,7 +162,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>1c9d1659-2fa2-49a3-a148-175572b163b8</t>
+    <t>7f0fd156-d853-438e-a643-62156d1d8f90</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -171,7 +171,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>2545cca8-d5c8-4893-89d2-082b5624ef68</t>
+    <t>81ac8b91-89c0-4ec2-89ec-fa5d8ee36bc3</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -180,7 +180,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>96f2ece9-baca-4da9-8e46-d32d6c7a7f79</t>
+    <t>13a43ce9-da28-48a9-90aa-7a1ff58d7bab</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -189,7 +189,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>254ea412-be68-44e9-ac29-9cbe4374418b</t>
+    <t>a638ff45-26b4-46d9-81b2-ce35f105277f</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -198,7 +198,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>e632a328-5781-4643-9e66-428ae9953f3c</t>
+    <t>9c1b5ed8-c102-41c4-a8a7-1e9a9b5168a4</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -207,7 +207,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>97eb4167-9616-43dc-976a-3686d4b132ba</t>
+    <t>f96e38c5-a3e0-483e-ba36-5d5934b9503f</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -216,7 +216,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>bc25ec47-3825-45cd-804b-bcd5f7ec0a98</t>
+    <t>74b39964-6432-456d-8471-338dcd6d42e3</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -225,7 +225,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>f8aaddfe-ac87-4710-a869-4ff918b7b9d2</t>
+    <t>4000bd76-bd24-49e2-849a-839dabc51be8</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>52ee9024-14c7-4bb7-9052-db9e92bf4ecb</t>
+    <t>5cd2a955-9d69-42e9-aa54-03d3f2e1e1be</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -264,7 +264,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>1349ff77-41c8-4fac-867a-061d8904b9e0</t>
+    <t>e10797f7-b3cf-42c5-9ffc-f8fa529c89df</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -273,7 +273,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>b1092e59-9718-42e5-9dc6-616a87edff14</t>
+    <t>35190394-6745-4cf5-ac25-7637e9c1d08d</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -282,7 +282,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>668ac1f1-7c0e-44ca-94e9-01a791222d74</t>
+    <t>9e6b7969-254a-4e5a-a2b4-7844fb3bb0ec</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -291,7 +291,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>32388b9a-8bcd-4306-9b52-11e640030dcc</t>
+    <t>9a969bf1-b846-4f90-b8bc-995c5cbe0ca1</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -300,7 +300,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>643bb10c-584a-45ef-ac7a-2c378c7b461f</t>
+    <t>20074e00-8db4-4ced-950d-28dfc6a384a6</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -309,7 +309,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>a212a6ab-1097-4052-af76-640ad3ab449f</t>
+    <t>7c82d85a-a562-4a4c-be1d-eb3644f85357</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -318,7 +318,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>4f30e487-6b0b-4341-b9ce-d4c37bc3e503</t>
+    <t>1f2f3f60-99f7-489c-a320-87ec93cd091e</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -327,7 +327,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>8b3142b0-7eed-4b04-af98-f8ad3fd6917e</t>
+    <t>426b3fe4-013b-4d2e-a808-412399b989f4</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -336,7 +336,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>757746fe-3786-4d12-aa38-68a403161dd2</t>
+    <t>263b09ed-942a-4ab5-a387-7b65798bb7e1</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -345,7 +345,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>0faf29d3-d45d-4498-847a-d9a1058b0313</t>
+    <t>c52dbac0-2f05-461a-9f17-7460c1846953</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -354,7 +354,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>88b5519e-9d49-4054-892c-1c65948d1e5f</t>
+    <t>028f272c-4fb9-44b2-a253-ed1957e69daf</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -363,7 +363,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>3de7dd13-d26d-4ce5-9297-16e22313ec6a</t>
+    <t>7aecbcab-353a-4168-8661-21d361ca2c12</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -372,7 +372,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>7b8c600d-6011-43e7-a889-ae51561eda9a</t>
+    <t>1f05683a-c313-4d6c-ba3c-dab029472ba9</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -381,7 +381,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>c15a925c-8ac1-4fae-82d7-b44ea2ff7551</t>
+    <t>a736fbae-3a61-44f9-9a4c-ed4720b91762</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -390,7 +390,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>4c35bd4d-beaa-48ad-b21c-acf0c91c2296</t>
+    <t>76da67c9-4093-44cf-b3c4-5aa5dbe243f1</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -399,7 +399,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>f9f053aa-571d-47df-b497-5d2e9006fc4c</t>
+    <t>bc1fc326-08ba-4d2b-a7c5-3115ffca70a0</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -408,7 +408,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>ec6c0559-785d-407a-8dea-39cfb3c01e7c</t>
+    <t>6acfa2f1-2f37-4bd9-bd69-166a0bf82363</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -417,7 +417,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>7a33a23e-e341-40ae-8b33-4a10c7efcff1</t>
+    <t>57d1b10a-da42-45ab-96c7-590470dc3f3e</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -426,7 +426,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>1481d6a3-4f03-4121-a2b8-a51708188977</t>
+    <t>8b063687-59c5-4d4e-ab4b-6313e6c3f08f</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -435,7 +435,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>5c7575ce-8ecc-49d8-8d67-3f9a2879a7e5</t>
+    <t>e2c6ea89-c5e0-4d20-96d1-a2f5cb64efa2</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -453,7 +453,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>de4b7752-e1b2-4565-8cb2-36ca89a29716</t>
+    <t>3b3b86c0-dbbc-43ad-a21b-6f0704a8f8cc</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>28538fb5-50f2-4fb7-96e0-afd34871497e</t>
-  </si>
-  <si>
-    <t>c1f0ca21-12c8-4799-830c-6ef952daa3e3</t>
-  </si>
-  <si>
-    <t>045f0757-2df2-46b3-9df8-903511f59bfb</t>
-  </si>
-  <si>
-    <t>817681d8-2135-4dde-8e59-9be390da728e</t>
-  </si>
-  <si>
-    <t>2b0769ce-fd5e-4dfd-8943-f8ef22fc1d3a</t>
-  </si>
-  <si>
-    <t>dd828c06-a3ac-4674-a0c3-d87cf256db38</t>
-  </si>
-  <si>
-    <t>af83d49f-b21a-4b2f-80c7-bcdfaead8dbe</t>
-  </si>
-  <si>
-    <t>40875697-8dd4-4c57-8a74-d3b22815212a</t>
-  </si>
-  <si>
-    <t>a5d92603-f5e4-426d-a071-781530076db2</t>
-  </si>
-  <si>
-    <t>e8f71fc1-8f11-4b93-98b0-1ab532d5d28b</t>
-  </si>
-  <si>
-    <t>7421876f-56fa-4469-8e69-ecb5e8ce14ef</t>
-  </si>
-  <si>
-    <t>c92db077-1635-49bf-a1d1-41d62ff09f1f</t>
-  </si>
-  <si>
-    <t>20977389-0732-4fe9-b69a-b73c79c48175</t>
-  </si>
-  <si>
-    <t>12420baa-2d22-468f-92ed-9e28ba1e98a9</t>
-  </si>
-  <si>
-    <t>31c8f82b-4ad6-44f3-88ae-a2c17eb569c5</t>
-  </si>
-  <si>
-    <t>fb942859-6c04-4806-af3f-31151ce68e36</t>
-  </si>
-  <si>
-    <t>b1a13326-5ce8-44a5-bd4a-b0cf1b602505</t>
-  </si>
-  <si>
-    <t>b8864fc9-f5e3-484c-aed2-902c26eb25f9</t>
-  </si>
-  <si>
-    <t>b00be03f-6bd0-44ba-95c0-478aefda742d</t>
-  </si>
-  <si>
-    <t>9614eda2-92be-4ed6-a79a-22a856ce04fc</t>
-  </si>
-  <si>
-    <t>737e2212-2a8c-4e23-8a9a-0ca0abfa1b43</t>
-  </si>
-  <si>
-    <t>d088ffd4-a77e-4119-95c8-5e0a82641439</t>
-  </si>
-  <si>
-    <t>77580cd0-afaa-4ab0-bd9e-d001519da10b</t>
-  </si>
-  <si>
-    <t>1f877899-e8bf-4ac3-ad7b-545fdf7fd891</t>
-  </si>
-  <si>
-    <t>252b911b-5759-4128-be79-5867e98e5bbb</t>
-  </si>
-  <si>
-    <t>dff928ab-120d-4942-a528-026e0cf0838b</t>
+    <t>72b97a24-1c89-464d-a09a-71475050f108</t>
+  </si>
+  <si>
+    <t>f9466b39-f04e-4376-897e-cac3889791a7</t>
+  </si>
+  <si>
+    <t>15fb7579-253d-4914-9ccc-b506da18b409</t>
+  </si>
+  <si>
+    <t>c4149881-51a1-4dc9-acd0-3b7908637b04</t>
+  </si>
+  <si>
+    <t>0ac95d85-02ac-4bac-b097-dd5a41aa2936</t>
+  </si>
+  <si>
+    <t>6b1b8963-6c34-4a38-9742-940c8e52c170</t>
+  </si>
+  <si>
+    <t>df232722-5f3d-4282-ba45-e898f6d50fd7</t>
+  </si>
+  <si>
+    <t>c703b4fc-96a9-4bb1-8501-d81233b0e695</t>
+  </si>
+  <si>
+    <t>dfda3db0-757f-4520-b0fd-5c10769827e4</t>
+  </si>
+  <si>
+    <t>1dd59022-ffd2-4940-8604-fc004d3d8f34</t>
+  </si>
+  <si>
+    <t>eb72acdf-79a3-4f23-aa27-66b37674d5b6</t>
+  </si>
+  <si>
+    <t>a0ba7912-9cce-41d2-8e9e-5d6f05b31c5c</t>
+  </si>
+  <si>
+    <t>7f4ecbcd-d6b1-4ff3-80c5-333599aa0d36</t>
+  </si>
+  <si>
+    <t>a205f55e-562b-4eb2-bc42-9faaf3d6a3ab</t>
+  </si>
+  <si>
+    <t>7b56f30f-635a-41f1-91d6-522b2e939fdd</t>
+  </si>
+  <si>
+    <t>72d661e9-d76d-468e-8347-ed598c30b2a3</t>
+  </si>
+  <si>
+    <t>af2b1808-e6dd-49c5-9269-75664b0a3f75</t>
+  </si>
+  <si>
+    <t>a163e47d-eb17-4caf-82f3-3eae56538625</t>
+  </si>
+  <si>
+    <t>08e9bca4-b4d3-45fa-a5e2-d3e22f11c8d3</t>
+  </si>
+  <si>
+    <t>ac914fee-17eb-46bb-8ff3-10a0c2922076</t>
+  </si>
+  <si>
+    <t>9b7a113a-d186-42a6-a11b-38a2795dd6d4</t>
+  </si>
+  <si>
+    <t>c9eb4f53-a13c-475e-92b2-cf6049001957</t>
+  </si>
+  <si>
+    <t>e19f9abd-e119-4ff7-96bb-7d054beb18e0</t>
+  </si>
+  <si>
+    <t>e384b13a-654a-475f-a362-f625dbf5e10c</t>
+  </si>
+  <si>
+    <t>32372d09-9dd6-451c-b552-523c33d815ba</t>
+  </si>
+  <si>
+    <t>2d1121a6-2e34-4075-b1ff-c7bc514924e2</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: enhance SQLPage content #6
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -123,7 +123,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>5c3046fa-bb76-4d07-b4d7-2cdfd85193a2</t>
+    <t>c4b960e1-fd30-46a5-bb55-ef8f63a923e0</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -135,7 +135,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>4882c6b1-77f1-4cba-ba86-c26e062dab71</t>
+    <t>7b730162-4b11-489f-898d-5a58e3219854</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -144,7 +144,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>e6139de2-edd1-4516-a7c0-8828e6a6d4b3</t>
+    <t>192f0f5f-25c5-471f-adff-96f8b2076dd3</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -153,7 +153,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>948d5ddb-caef-4683-af04-a9936974d326</t>
+    <t>5253ce90-35af-474a-81a4-6306b99450d0</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -162,7 +162,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>7f0fd156-d853-438e-a643-62156d1d8f90</t>
+    <t>655c87f4-4de7-4ef5-9a94-ec7eae4be078</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -171,7 +171,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>81ac8b91-89c0-4ec2-89ec-fa5d8ee36bc3</t>
+    <t>cecf1905-e361-4f9f-9a3e-8781a2697bb5</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -180,7 +180,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>13a43ce9-da28-48a9-90aa-7a1ff58d7bab</t>
+    <t>d2487b2b-5cd4-425f-b155-842b1a8ede22</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -189,7 +189,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>a638ff45-26b4-46d9-81b2-ce35f105277f</t>
+    <t>19ab5051-0ac7-4848-a88a-a15cf2d94639</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -198,7 +198,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>9c1b5ed8-c102-41c4-a8a7-1e9a9b5168a4</t>
+    <t>068ec416-5a3b-432e-96d6-674dc6d51bbc</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -207,7 +207,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>f96e38c5-a3e0-483e-ba36-5d5934b9503f</t>
+    <t>8f2e32fd-f70d-46ed-a13b-db04fd7ca81e</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -216,7 +216,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>74b39964-6432-456d-8471-338dcd6d42e3</t>
+    <t>d35883ce-22ac-4d53-8f1d-0ef5295a5a0f</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -225,7 +225,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>4000bd76-bd24-49e2-849a-839dabc51be8</t>
+    <t>047f752e-a980-4b7b-9e88-5dfddd0b816a</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>5cd2a955-9d69-42e9-aa54-03d3f2e1e1be</t>
+    <t>798bde55-9ddc-4547-bdc1-17c9c7a31fc7</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -264,7 +264,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>e10797f7-b3cf-42c5-9ffc-f8fa529c89df</t>
+    <t>f86bf60a-5e26-4477-9ba1-54d33fa1ee3c</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -273,7 +273,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>35190394-6745-4cf5-ac25-7637e9c1d08d</t>
+    <t>0afbcfba-c4d1-481a-a9dc-964e35a863c3</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -282,7 +282,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>9e6b7969-254a-4e5a-a2b4-7844fb3bb0ec</t>
+    <t>bba7f884-5d02-4654-b115-378bf5d18cf8</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -291,7 +291,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>9a969bf1-b846-4f90-b8bc-995c5cbe0ca1</t>
+    <t>84a79d5e-ec17-49a6-aa05-32c42eccf353</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -300,7 +300,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>20074e00-8db4-4ced-950d-28dfc6a384a6</t>
+    <t>8e313eee-4a13-4a97-9e61-8659e2ae856d</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -309,7 +309,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>7c82d85a-a562-4a4c-be1d-eb3644f85357</t>
+    <t>14893e2f-48e4-4d56-86f9-7cebcebd8abe</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -318,7 +318,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>1f2f3f60-99f7-489c-a320-87ec93cd091e</t>
+    <t>18419899-347f-46b9-abc5-26fd42577096</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -327,7 +327,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>426b3fe4-013b-4d2e-a808-412399b989f4</t>
+    <t>a719c7d2-a392-4de4-adfd-060ef456cf3f</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -336,7 +336,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>263b09ed-942a-4ab5-a387-7b65798bb7e1</t>
+    <t>2400b7ae-df64-4b79-b31d-c3a422e6239b</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -345,7 +345,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>c52dbac0-2f05-461a-9f17-7460c1846953</t>
+    <t>837ff885-b7e2-45d6-9393-bf554a868fd2</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -354,7 +354,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>028f272c-4fb9-44b2-a253-ed1957e69daf</t>
+    <t>89b0767b-c4f7-4c6f-9884-d9d2595d4297</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -363,7 +363,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>7aecbcab-353a-4168-8661-21d361ca2c12</t>
+    <t>114a3068-c7bc-42bc-aa12-f5323dbdfdd8</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -372,7 +372,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>1f05683a-c313-4d6c-ba3c-dab029472ba9</t>
+    <t>bc0acb68-2440-4fc2-ae5c-b921d1147cc5</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -381,7 +381,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>a736fbae-3a61-44f9-9a4c-ed4720b91762</t>
+    <t>19bf6957-a07e-4295-842f-37837b344276</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -390,7 +390,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>76da67c9-4093-44cf-b3c4-5aa5dbe243f1</t>
+    <t>de407d20-bb55-4f18-b323-04bebec7f2ea</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -399,7 +399,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>bc1fc326-08ba-4d2b-a7c5-3115ffca70a0</t>
+    <t>cc6efe66-880a-495e-86e1-dc5be91e0f08</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -408,7 +408,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>6acfa2f1-2f37-4bd9-bd69-166a0bf82363</t>
+    <t>8245347a-da91-4584-a750-38527c9f7434</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -417,7 +417,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>57d1b10a-da42-45ab-96c7-590470dc3f3e</t>
+    <t>886ae2d0-f0bf-4e4b-ae84-01f0d7429f19</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -426,7 +426,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>8b063687-59c5-4d4e-ab4b-6313e6c3f08f</t>
+    <t>71828bf0-6318-41f3-84fb-59a6b6934cef</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -435,7 +435,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>e2c6ea89-c5e0-4d20-96d1-a2f5cb64efa2</t>
+    <t>8e1d44a6-593b-4a13-b0f0-6cddc32e1265</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -453,7 +453,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>3b3b86c0-dbbc-43ad-a21b-6f0704a8f8cc</t>
+    <t>25dc3071-3b26-451e-9c43-0789eeb536c9</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>72b97a24-1c89-464d-a09a-71475050f108</t>
-  </si>
-  <si>
-    <t>f9466b39-f04e-4376-897e-cac3889791a7</t>
-  </si>
-  <si>
-    <t>15fb7579-253d-4914-9ccc-b506da18b409</t>
-  </si>
-  <si>
-    <t>c4149881-51a1-4dc9-acd0-3b7908637b04</t>
-  </si>
-  <si>
-    <t>0ac95d85-02ac-4bac-b097-dd5a41aa2936</t>
-  </si>
-  <si>
-    <t>6b1b8963-6c34-4a38-9742-940c8e52c170</t>
-  </si>
-  <si>
-    <t>df232722-5f3d-4282-ba45-e898f6d50fd7</t>
-  </si>
-  <si>
-    <t>c703b4fc-96a9-4bb1-8501-d81233b0e695</t>
-  </si>
-  <si>
-    <t>dfda3db0-757f-4520-b0fd-5c10769827e4</t>
-  </si>
-  <si>
-    <t>1dd59022-ffd2-4940-8604-fc004d3d8f34</t>
-  </si>
-  <si>
-    <t>eb72acdf-79a3-4f23-aa27-66b37674d5b6</t>
-  </si>
-  <si>
-    <t>a0ba7912-9cce-41d2-8e9e-5d6f05b31c5c</t>
-  </si>
-  <si>
-    <t>7f4ecbcd-d6b1-4ff3-80c5-333599aa0d36</t>
-  </si>
-  <si>
-    <t>a205f55e-562b-4eb2-bc42-9faaf3d6a3ab</t>
-  </si>
-  <si>
-    <t>7b56f30f-635a-41f1-91d6-522b2e939fdd</t>
-  </si>
-  <si>
-    <t>72d661e9-d76d-468e-8347-ed598c30b2a3</t>
-  </si>
-  <si>
-    <t>af2b1808-e6dd-49c5-9269-75664b0a3f75</t>
-  </si>
-  <si>
-    <t>a163e47d-eb17-4caf-82f3-3eae56538625</t>
-  </si>
-  <si>
-    <t>08e9bca4-b4d3-45fa-a5e2-d3e22f11c8d3</t>
-  </si>
-  <si>
-    <t>ac914fee-17eb-46bb-8ff3-10a0c2922076</t>
-  </si>
-  <si>
-    <t>9b7a113a-d186-42a6-a11b-38a2795dd6d4</t>
-  </si>
-  <si>
-    <t>c9eb4f53-a13c-475e-92b2-cf6049001957</t>
-  </si>
-  <si>
-    <t>e19f9abd-e119-4ff7-96bb-7d054beb18e0</t>
-  </si>
-  <si>
-    <t>e384b13a-654a-475f-a362-f625dbf5e10c</t>
-  </si>
-  <si>
-    <t>32372d09-9dd6-451c-b552-523c33d815ba</t>
-  </si>
-  <si>
-    <t>2d1121a6-2e34-4075-b1ff-c7bc514924e2</t>
+    <t>782c8626-1d09-4236-98a2-4cfd033d73d1</t>
+  </si>
+  <si>
+    <t>9877a798-eb7a-4c29-99d1-1676a93b6529</t>
+  </si>
+  <si>
+    <t>a73cb25d-9c4d-48cf-9bb2-4836078210bf</t>
+  </si>
+  <si>
+    <t>8e7c4113-e945-4e00-b8c5-65225cd8b757</t>
+  </si>
+  <si>
+    <t>d84a476c-75bc-4262-a114-e2fa7baefd3b</t>
+  </si>
+  <si>
+    <t>68dd7cd1-d9ab-401a-88d6-72ab32668191</t>
+  </si>
+  <si>
+    <t>3bbe034e-dd99-4289-8b6b-29996f82ca44</t>
+  </si>
+  <si>
+    <t>a5069d3e-15df-45a7-b0c3-f2f52e92582a</t>
+  </si>
+  <si>
+    <t>16cd6a34-eece-4591-aee5-2a83664e94a6</t>
+  </si>
+  <si>
+    <t>6926d742-cf4d-4330-befa-6245e37dddff</t>
+  </si>
+  <si>
+    <t>a71bfbec-2103-4ba0-be15-d805cce4a7de</t>
+  </si>
+  <si>
+    <t>5a64905d-1672-42fc-a2b0-693f83a1239e</t>
+  </si>
+  <si>
+    <t>38d09dac-c9aa-416e-9f52-cbd0abec77fe</t>
+  </si>
+  <si>
+    <t>08b43517-8871-4dae-84e2-933085bbb7be</t>
+  </si>
+  <si>
+    <t>97495ed2-9357-4197-ace0-cdd6498ff09f</t>
+  </si>
+  <si>
+    <t>e9894dea-9c9c-468d-abb6-cb71b8cccbdd</t>
+  </si>
+  <si>
+    <t>416ffa1b-6282-4b60-829c-1ee0657fdbd7</t>
+  </si>
+  <si>
+    <t>a5912725-e15a-4168-a792-128af37b08c4</t>
+  </si>
+  <si>
+    <t>4b74c60e-9ac5-4bbe-83fc-0d177444b77d</t>
+  </si>
+  <si>
+    <t>f894a812-0ae6-485b-bbce-5e8bfa065f8c</t>
+  </si>
+  <si>
+    <t>ada6ced1-1f8a-4a62-8b26-bb6c64faf2cb</t>
+  </si>
+  <si>
+    <t>98f54b84-463b-45f0-8e6d-3cc31046f85f</t>
+  </si>
+  <si>
+    <t>ff18e9df-4613-43bb-abb2-bf17f6ebc5fe</t>
+  </si>
+  <si>
+    <t>83f1798e-4e8c-4ede-8d55-f9e810d55e05</t>
+  </si>
+  <si>
+    <t>d16337c2-2f93-454e-af03-39818e1f5034</t>
+  </si>
+  <si>
+    <t>4eab3580-c8c5-4bf2-8625-795f74ff59b2</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: introduce sample FHIR view
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -123,7 +123,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>c4b960e1-fd30-46a5-bb55-ef8f63a923e0</t>
+    <t>c633b3cf-d150-4007-88ac-d18907a85098</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -135,7 +135,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>7b730162-4b11-489f-898d-5a58e3219854</t>
+    <t>4d025129-d1ba-4cbb-ba9c-7720d2bc129c</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -144,7 +144,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>192f0f5f-25c5-471f-adff-96f8b2076dd3</t>
+    <t>39b8f6a9-937b-4166-bf55-d361e794afd7</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -153,7 +153,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>5253ce90-35af-474a-81a4-6306b99450d0</t>
+    <t>842f317d-f770-4665-9316-dc84e72a5bca</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -162,7 +162,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>655c87f4-4de7-4ef5-9a94-ec7eae4be078</t>
+    <t>2d26f2f3-b9d5-408e-8558-7443322ecb7c</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -171,7 +171,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>cecf1905-e361-4f9f-9a3e-8781a2697bb5</t>
+    <t>e9085274-1009-47b2-9031-6bbd6a7f7377</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -180,7 +180,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>d2487b2b-5cd4-425f-b155-842b1a8ede22</t>
+    <t>464b6b4e-839a-4bf0-b5a8-a77288e85245</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -189,7 +189,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>19ab5051-0ac7-4848-a88a-a15cf2d94639</t>
+    <t>2dadf332-c4d5-41fd-9192-68715d02610a</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -198,7 +198,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>068ec416-5a3b-432e-96d6-674dc6d51bbc</t>
+    <t>26a9f2ac-65c2-4f39-af08-1b26f402284f</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -207,7 +207,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>8f2e32fd-f70d-46ed-a13b-db04fd7ca81e</t>
+    <t>6e5c8133-7ae8-41e5-9edd-18e2c744288a</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -216,7 +216,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>d35883ce-22ac-4d53-8f1d-0ef5295a5a0f</t>
+    <t>3c080f0c-5745-4d05-b01b-0b4c4cd5ab9a</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -225,7 +225,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>047f752e-a980-4b7b-9e88-5dfddd0b816a</t>
+    <t>75f94655-9307-4ca3-aabb-8fce81454578</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>798bde55-9ddc-4547-bdc1-17c9c7a31fc7</t>
+    <t>40169ffd-6050-45e5-93a8-caed0c5a1ab7</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -264,7 +264,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>f86bf60a-5e26-4477-9ba1-54d33fa1ee3c</t>
+    <t>b286ce66-a092-4d45-a87b-fb1987d1b7fa</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -273,7 +273,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>0afbcfba-c4d1-481a-a9dc-964e35a863c3</t>
+    <t>6aaed81c-8cf6-428f-a675-1399b03b6d82</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -282,7 +282,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>bba7f884-5d02-4654-b115-378bf5d18cf8</t>
+    <t>ee155508-eadc-4039-a375-c17b671833d7</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -291,7 +291,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>84a79d5e-ec17-49a6-aa05-32c42eccf353</t>
+    <t>a6c775a1-d7d1-4ad4-924b-ef5ee0d1ef77</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -300,7 +300,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>8e313eee-4a13-4a97-9e61-8659e2ae856d</t>
+    <t>e659eb16-a838-440e-95f2-e824db80bef9</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -309,7 +309,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>14893e2f-48e4-4d56-86f9-7cebcebd8abe</t>
+    <t>f0bfb036-a45b-4573-bb2b-755504461ec2</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -318,7 +318,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>18419899-347f-46b9-abc5-26fd42577096</t>
+    <t>27e1948a-4d16-48a3-a5b6-feffe8301427</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -327,7 +327,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>a719c7d2-a392-4de4-adfd-060ef456cf3f</t>
+    <t>17faa7ec-5e65-48e6-9a41-f0819e681784</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -336,7 +336,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>2400b7ae-df64-4b79-b31d-c3a422e6239b</t>
+    <t>d8032654-96d3-4656-8472-8a07a099df9f</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -345,7 +345,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>837ff885-b7e2-45d6-9393-bf554a868fd2</t>
+    <t>f55d501a-e9dc-42ab-b77c-ed29b6c6c0ef</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -354,7 +354,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>89b0767b-c4f7-4c6f-9884-d9d2595d4297</t>
+    <t>6ee7c933-3b81-4dd7-88f7-33f3e837f737</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -363,7 +363,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>114a3068-c7bc-42bc-aa12-f5323dbdfdd8</t>
+    <t>2d2eae99-8fb3-446d-a2f8-e733d637e0d8</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -372,7 +372,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>bc0acb68-2440-4fc2-ae5c-b921d1147cc5</t>
+    <t>6ce1dd33-2777-40f5-949c-0043cd21f1dc</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -381,7 +381,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>19bf6957-a07e-4295-842f-37837b344276</t>
+    <t>b30078a9-76a6-493b-96b0-7de65272fdc2</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -390,7 +390,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>de407d20-bb55-4f18-b323-04bebec7f2ea</t>
+    <t>a51f96ac-4e2a-41b7-a3f5-2ac184a421d1</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -399,7 +399,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>cc6efe66-880a-495e-86e1-dc5be91e0f08</t>
+    <t>bcb2899d-7b3b-4aed-8536-8e24aecadc6e</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -408,7 +408,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>8245347a-da91-4584-a750-38527c9f7434</t>
+    <t>61b9d4fe-cec1-4171-9545-3adad30c8c41</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -417,7 +417,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>886ae2d0-f0bf-4e4b-ae84-01f0d7429f19</t>
+    <t>c0dd763c-f4bb-4d5b-93e0-e720bb183896</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -426,7 +426,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>71828bf0-6318-41f3-84fb-59a6b6934cef</t>
+    <t>a97fb3f2-382f-4c67-ac17-92a414689288</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -435,7 +435,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>8e1d44a6-593b-4a13-b0f0-6cddc32e1265</t>
+    <t>e7d8c6bd-f14a-4882-846c-c8ceae6204fe</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -453,7 +453,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>25dc3071-3b26-451e-9c43-0789eeb536c9</t>
+    <t>3a3dc980-8f95-4c78-ad5a-1d315d45e717</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>782c8626-1d09-4236-98a2-4cfd033d73d1</t>
-  </si>
-  <si>
-    <t>9877a798-eb7a-4c29-99d1-1676a93b6529</t>
-  </si>
-  <si>
-    <t>a73cb25d-9c4d-48cf-9bb2-4836078210bf</t>
-  </si>
-  <si>
-    <t>8e7c4113-e945-4e00-b8c5-65225cd8b757</t>
-  </si>
-  <si>
-    <t>d84a476c-75bc-4262-a114-e2fa7baefd3b</t>
-  </si>
-  <si>
-    <t>68dd7cd1-d9ab-401a-88d6-72ab32668191</t>
-  </si>
-  <si>
-    <t>3bbe034e-dd99-4289-8b6b-29996f82ca44</t>
-  </si>
-  <si>
-    <t>a5069d3e-15df-45a7-b0c3-f2f52e92582a</t>
-  </si>
-  <si>
-    <t>16cd6a34-eece-4591-aee5-2a83664e94a6</t>
-  </si>
-  <si>
-    <t>6926d742-cf4d-4330-befa-6245e37dddff</t>
-  </si>
-  <si>
-    <t>a71bfbec-2103-4ba0-be15-d805cce4a7de</t>
-  </si>
-  <si>
-    <t>5a64905d-1672-42fc-a2b0-693f83a1239e</t>
-  </si>
-  <si>
-    <t>38d09dac-c9aa-416e-9f52-cbd0abec77fe</t>
-  </si>
-  <si>
-    <t>08b43517-8871-4dae-84e2-933085bbb7be</t>
-  </si>
-  <si>
-    <t>97495ed2-9357-4197-ace0-cdd6498ff09f</t>
-  </si>
-  <si>
-    <t>e9894dea-9c9c-468d-abb6-cb71b8cccbdd</t>
-  </si>
-  <si>
-    <t>416ffa1b-6282-4b60-829c-1ee0657fdbd7</t>
-  </si>
-  <si>
-    <t>a5912725-e15a-4168-a792-128af37b08c4</t>
-  </si>
-  <si>
-    <t>4b74c60e-9ac5-4bbe-83fc-0d177444b77d</t>
-  </si>
-  <si>
-    <t>f894a812-0ae6-485b-bbce-5e8bfa065f8c</t>
-  </si>
-  <si>
-    <t>ada6ced1-1f8a-4a62-8b26-bb6c64faf2cb</t>
-  </si>
-  <si>
-    <t>98f54b84-463b-45f0-8e6d-3cc31046f85f</t>
-  </si>
-  <si>
-    <t>ff18e9df-4613-43bb-abb2-bf17f6ebc5fe</t>
-  </si>
-  <si>
-    <t>83f1798e-4e8c-4ede-8d55-f9e810d55e05</t>
-  </si>
-  <si>
-    <t>d16337c2-2f93-454e-af03-39818e1f5034</t>
-  </si>
-  <si>
-    <t>4eab3580-c8c5-4bf2-8625-795f74ff59b2</t>
+    <t>7377073d-93f7-42ce-b529-985b970397ce</t>
+  </si>
+  <si>
+    <t>a7f7818a-771c-4c1d-bc1a-512526b5a7ae</t>
+  </si>
+  <si>
+    <t>fe240662-989e-4984-aee0-1b8b83305bcb</t>
+  </si>
+  <si>
+    <t>fc009024-5c7e-4aa2-b583-8f18428a6be3</t>
+  </si>
+  <si>
+    <t>eccb1c32-c22b-4a8b-b699-01e01402d31b</t>
+  </si>
+  <si>
+    <t>7a6315d3-b727-4a2c-b6fc-9862024579b2</t>
+  </si>
+  <si>
+    <t>24200d78-47c6-41a5-b535-b77dd403e1ab</t>
+  </si>
+  <si>
+    <t>a77709f3-1888-430e-a108-6ab7320065a8</t>
+  </si>
+  <si>
+    <t>dcd52a6b-0684-4534-a8da-e262ab510d61</t>
+  </si>
+  <si>
+    <t>bbe68dc1-da98-4e00-844b-e6e851a800e2</t>
+  </si>
+  <si>
+    <t>8cd46abd-96ed-41da-90b2-d296365f18a9</t>
+  </si>
+  <si>
+    <t>75177149-3acf-44f9-bb6f-2804bdd02f63</t>
+  </si>
+  <si>
+    <t>ce84a5dc-1458-474b-a883-43df2e90e05b</t>
+  </si>
+  <si>
+    <t>50afc1e9-8994-4006-9fb2-60b4ff258514</t>
+  </si>
+  <si>
+    <t>cafe744b-c5fb-4561-b52c-3ab6002a05f5</t>
+  </si>
+  <si>
+    <t>6f95f12f-fd70-4d08-b5b7-befe7de06e0f</t>
+  </si>
+  <si>
+    <t>87d37215-2d02-4992-8725-1e5037655f97</t>
+  </si>
+  <si>
+    <t>82bdaedf-d4e4-4639-b3f1-095e65770c5c</t>
+  </si>
+  <si>
+    <t>e296eaa3-4bb2-474d-b797-114f43e83b59</t>
+  </si>
+  <si>
+    <t>258ef7f3-0676-4df9-8770-c8715c3b0da7</t>
+  </si>
+  <si>
+    <t>f581fb7b-4c62-4492-aa20-ce0e634754d2</t>
+  </si>
+  <si>
+    <t>b30db91d-38c5-403d-8eba-d48c4e9b621c</t>
+  </si>
+  <si>
+    <t>0519b8bf-ab6c-402e-81da-a60c36868381</t>
+  </si>
+  <si>
+    <t>d7895669-c69b-445d-a381-cbdf6e463222</t>
+  </si>
+  <si>
+    <t>d9d36687-6ace-4251-9007-f3d6693c23d5</t>
+  </si>
+  <si>
+    <t>9b5db90f-411d-46b1-bfca-90e8887c1c3c</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
refactor: rename "ingest" to "orchestrate"
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -12,7 +12,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="179">
   <si>
-    <t>ingest_session_id</t>
+    <t>orch_session_id</t>
   </si>
   <si>
     <t>device_id</t>
@@ -21,7 +21,7 @@
     <t>elaboration</t>
   </si>
   <si>
-    <t>ingest_session_entry_id</t>
+    <t>orch_session_entry_id</t>
   </si>
   <si>
     <t>ingest_src</t>
@@ -33,7 +33,7 @@
     <t>elaboration:1</t>
   </si>
   <si>
-    <t>ingest_session_issue_id</t>
+    <t>orch_session_issue_id</t>
   </si>
   <si>
     <t>issue_type</t>
@@ -123,7 +123,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>c633b3cf-d150-4007-88ac-d18907a85098</t>
+    <t>db54c94e-e025-4555-92df-3b0472d624b8</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -135,7 +135,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>4d025129-d1ba-4cbb-ba9c-7720d2bc129c</t>
+    <t>4c2d1bf8-0c52-4828-96ef-bf3f69d46d3d</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -144,7 +144,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>39b8f6a9-937b-4166-bf55-d361e794afd7</t>
+    <t>bd7aab99-46b7-449b-9155-b153985b713a</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -153,7 +153,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>842f317d-f770-4665-9316-dc84e72a5bca</t>
+    <t>93fe09ef-5ae8-4848-91ce-9fb9ab3d850b</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -162,7 +162,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>2d26f2f3-b9d5-408e-8558-7443322ecb7c</t>
+    <t>671d7155-1e1d-4126-a5eb-874ebc5d57e4</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -171,7 +171,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>e9085274-1009-47b2-9031-6bbd6a7f7377</t>
+    <t>baf75e04-d1ba-4794-bf82-467be42dcc75</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -180,7 +180,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>464b6b4e-839a-4bf0-b5a8-a77288e85245</t>
+    <t>4c9c7ddf-1e6a-43a6-8c51-3fc78c145b00</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -189,7 +189,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>2dadf332-c4d5-41fd-9192-68715d02610a</t>
+    <t>5a075599-6096-4961-8f04-96d8ef636f28</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -198,7 +198,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>26a9f2ac-65c2-4f39-af08-1b26f402284f</t>
+    <t>0a763e51-1479-429d-816c-2e3217ca63f0</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -207,7 +207,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>6e5c8133-7ae8-41e5-9edd-18e2c744288a</t>
+    <t>5032c177-7c52-47de-8741-7d88464bc6fb</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -216,7 +216,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>3c080f0c-5745-4d05-b01b-0b4c4cd5ab9a</t>
+    <t>d1626583-bba0-4ec9-9fab-8d3d2c87c1d1</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -225,7 +225,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>75f94655-9307-4ca3-aabb-8fce81454578</t>
+    <t>778b95c3-3fc5-4c42-ac1f-65ac9ffb337f</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>40169ffd-6050-45e5-93a8-caed0c5a1ab7</t>
+    <t>6116a37a-4e94-434c-be8d-fba574a57bce</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -264,7 +264,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>b286ce66-a092-4d45-a87b-fb1987d1b7fa</t>
+    <t>bb80d8cd-9031-4498-a11b-38ae517e03f9</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -273,7 +273,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>6aaed81c-8cf6-428f-a675-1399b03b6d82</t>
+    <t>57d5489c-47c5-4b5e-9d00-fc041385ae69</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -282,7 +282,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>ee155508-eadc-4039-a375-c17b671833d7</t>
+    <t>62687b89-afce-4bd1-9e6c-62223f7cda02</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -291,7 +291,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>a6c775a1-d7d1-4ad4-924b-ef5ee0d1ef77</t>
+    <t>9af44f4a-6258-4de2-97fb-ea9d8177f53a</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -300,7 +300,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>e659eb16-a838-440e-95f2-e824db80bef9</t>
+    <t>b3fc3589-7c0c-4771-a0d5-ad279731ed07</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -309,7 +309,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>f0bfb036-a45b-4573-bb2b-755504461ec2</t>
+    <t>88af3db6-67b0-4be4-b33f-994457cae455</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -318,7 +318,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>27e1948a-4d16-48a3-a5b6-feffe8301427</t>
+    <t>517e26e8-cc26-4f27-a93e-f56c69125462</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -327,7 +327,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>17faa7ec-5e65-48e6-9a41-f0819e681784</t>
+    <t>12bbdabc-2df6-4bb7-ae05-ce78637576d6</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -336,7 +336,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>d8032654-96d3-4656-8472-8a07a099df9f</t>
+    <t>d6de092b-1701-4af9-87b4-4071f1b58824</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -345,7 +345,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>f55d501a-e9dc-42ab-b77c-ed29b6c6c0ef</t>
+    <t>30dad59d-3b76-4375-9c0d-6497f09395ca</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -354,7 +354,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>6ee7c933-3b81-4dd7-88f7-33f3e837f737</t>
+    <t>3317574e-4eb9-41df-96d8-77f3f1d6c9c7</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -363,7 +363,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>2d2eae99-8fb3-446d-a2f8-e733d637e0d8</t>
+    <t>8b2d7596-295c-408b-8271-26af2725bd3c</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -372,7 +372,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>6ce1dd33-2777-40f5-949c-0043cd21f1dc</t>
+    <t>032d1455-a432-4455-866d-636379cc0113</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -381,7 +381,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>b30078a9-76a6-493b-96b0-7de65272fdc2</t>
+    <t>2421138d-c86c-40f8-8e39-0554a6102f76</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -390,7 +390,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>a51f96ac-4e2a-41b7-a3f5-2ac184a421d1</t>
+    <t>a58ce8f9-34a1-4af0-9a4a-d3a5529d0077</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -399,7 +399,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>bcb2899d-7b3b-4aed-8536-8e24aecadc6e</t>
+    <t>057d87d0-a510-46e2-8f78-9e338600eee8</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -408,7 +408,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>61b9d4fe-cec1-4171-9545-3adad30c8c41</t>
+    <t>cafc25aa-fc22-46ac-891b-499239ff5185</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -417,7 +417,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>c0dd763c-f4bb-4d5b-93e0-e720bb183896</t>
+    <t>50c4fd24-d066-4db3-af9b-edbf4b3f0492</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -426,7 +426,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>a97fb3f2-382f-4c67-ac17-92a414689288</t>
+    <t>7c58c117-1e20-4bfc-a928-5dfc96c7defe</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -435,7 +435,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>e7d8c6bd-f14a-4882-846c-c8ceae6204fe</t>
+    <t>69912e9f-389d-4309-a46a-108e5cf22159</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -453,7 +453,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>3a3dc980-8f95-4c78-ad5a-1d315d45e717</t>
+    <t>fd70db33-83de-4564-81a8-22016e1fb21b</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>7377073d-93f7-42ce-b529-985b970397ce</t>
-  </si>
-  <si>
-    <t>a7f7818a-771c-4c1d-bc1a-512526b5a7ae</t>
-  </si>
-  <si>
-    <t>fe240662-989e-4984-aee0-1b8b83305bcb</t>
-  </si>
-  <si>
-    <t>fc009024-5c7e-4aa2-b583-8f18428a6be3</t>
-  </si>
-  <si>
-    <t>eccb1c32-c22b-4a8b-b699-01e01402d31b</t>
-  </si>
-  <si>
-    <t>7a6315d3-b727-4a2c-b6fc-9862024579b2</t>
-  </si>
-  <si>
-    <t>24200d78-47c6-41a5-b535-b77dd403e1ab</t>
-  </si>
-  <si>
-    <t>a77709f3-1888-430e-a108-6ab7320065a8</t>
-  </si>
-  <si>
-    <t>dcd52a6b-0684-4534-a8da-e262ab510d61</t>
-  </si>
-  <si>
-    <t>bbe68dc1-da98-4e00-844b-e6e851a800e2</t>
-  </si>
-  <si>
-    <t>8cd46abd-96ed-41da-90b2-d296365f18a9</t>
-  </si>
-  <si>
-    <t>75177149-3acf-44f9-bb6f-2804bdd02f63</t>
-  </si>
-  <si>
-    <t>ce84a5dc-1458-474b-a883-43df2e90e05b</t>
-  </si>
-  <si>
-    <t>50afc1e9-8994-4006-9fb2-60b4ff258514</t>
-  </si>
-  <si>
-    <t>cafe744b-c5fb-4561-b52c-3ab6002a05f5</t>
-  </si>
-  <si>
-    <t>6f95f12f-fd70-4d08-b5b7-befe7de06e0f</t>
-  </si>
-  <si>
-    <t>87d37215-2d02-4992-8725-1e5037655f97</t>
-  </si>
-  <si>
-    <t>82bdaedf-d4e4-4639-b3f1-095e65770c5c</t>
-  </si>
-  <si>
-    <t>e296eaa3-4bb2-474d-b797-114f43e83b59</t>
-  </si>
-  <si>
-    <t>258ef7f3-0676-4df9-8770-c8715c3b0da7</t>
-  </si>
-  <si>
-    <t>f581fb7b-4c62-4492-aa20-ce0e634754d2</t>
-  </si>
-  <si>
-    <t>b30db91d-38c5-403d-8eba-d48c4e9b621c</t>
-  </si>
-  <si>
-    <t>0519b8bf-ab6c-402e-81da-a60c36868381</t>
-  </si>
-  <si>
-    <t>d7895669-c69b-445d-a381-cbdf6e463222</t>
-  </si>
-  <si>
-    <t>d9d36687-6ace-4251-9007-f3d6693c23d5</t>
-  </si>
-  <si>
-    <t>9b5db90f-411d-46b1-bfca-90e8887c1c3c</t>
+    <t>ac4b863f-7c12-4bc0-8385-a953e1ca6c22</t>
+  </si>
+  <si>
+    <t>c3ef3362-8bc0-427f-a20c-e74abf3f398e</t>
+  </si>
+  <si>
+    <t>165159a9-2592-401c-bd36-0621c4cc8b6d</t>
+  </si>
+  <si>
+    <t>fb89466b-6735-4a0d-a141-0e490d798c7b</t>
+  </si>
+  <si>
+    <t>cf44dd80-6825-4395-8237-be93d4e22374</t>
+  </si>
+  <si>
+    <t>40cb2fbe-db4e-4e00-9846-b7b9ae3d3a49</t>
+  </si>
+  <si>
+    <t>23108655-c46e-4507-aa83-96cd25985e8d</t>
+  </si>
+  <si>
+    <t>e89539f2-c751-4cf3-962c-c0cba00848b4</t>
+  </si>
+  <si>
+    <t>06f6ffd3-ef5c-409f-b990-137697918f42</t>
+  </si>
+  <si>
+    <t>70652dd0-f325-4b7a-981b-469e2453e8c1</t>
+  </si>
+  <si>
+    <t>81650c85-fd50-471e-8fc8-e9a15156448a</t>
+  </si>
+  <si>
+    <t>882d4a4b-6e7e-4822-878f-30a769069d3d</t>
+  </si>
+  <si>
+    <t>94dd2556-9e09-4f07-96df-401430c7ecd9</t>
+  </si>
+  <si>
+    <t>e99b5a98-6e87-4d94-a7b7-0eedc5b71a77</t>
+  </si>
+  <si>
+    <t>97c77468-b41c-4e4f-98bf-114f6a221b0b</t>
+  </si>
+  <si>
+    <t>6a14248a-eefb-429d-959c-e0ccd57c6ae2</t>
+  </si>
+  <si>
+    <t>50fda451-475b-448b-8b87-e70843e852f8</t>
+  </si>
+  <si>
+    <t>cf5a1b31-3567-4096-adc7-769e42e206e1</t>
+  </si>
+  <si>
+    <t>87ec150d-1cd3-476e-8cb4-38ca49c550a9</t>
+  </si>
+  <si>
+    <t>7772fe11-edb7-4004-8f15-7b6ada8d6282</t>
+  </si>
+  <si>
+    <t>61beca90-96cb-431f-ab58-d0122791fd81</t>
+  </si>
+  <si>
+    <t>b4d48c0f-1002-4492-ab15-94459a117702</t>
+  </si>
+  <si>
+    <t>601ad1d2-31e2-405d-8e4d-3c16008308a7</t>
+  </si>
+  <si>
+    <t>39b53120-1f5a-426b-b2a9-8533089e09c7</t>
+  </si>
+  <si>
+    <t>aa6fce67-0d05-422a-af60-fce41e223634</t>
+  </si>
+  <si>
+    <t>f59499c5-ddf1-451e-919a-0deae4bb1665</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: introduce cmd exec tracking
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="206">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -63,7 +63,433 @@
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
   </si>
   <si>
-    <t>1931dfcc-e8fc-597d-b1bc-65b4287e6fdf</t>
+    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_admin_demographic</t>
+  </si>
+  <si>
+    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_screening</t>
+  </si>
+  <si>
+    <t>1b857fd6-c4bd-4983-8895-838f0ca4d319</t>
+  </si>
+  <si>
+    <t>Missing Column</t>
+  </si>
+  <si>
+    <t>Required column PAT_MRN_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_MRN_ID"</t>
+  </si>
+  <si>
+    <t>9bc4ea2c-c958-4b9e-b3c4-895a095bc4bf</t>
+  </si>
+  <si>
+    <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
+  </si>
+  <si>
+    <t>fd737f42-e5c0-45c0-8bf6-38fd72ae1b74</t>
+  </si>
+  <si>
+    <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
+  </si>
+  <si>
+    <t>2c1574bc-9e82-405d-9c4c-d9a43cfe914f</t>
+  </si>
+  <si>
+    <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
+  </si>
+  <si>
+    <t>8f53f351-2986-4313-a3b0-edecd336154b</t>
+  </si>
+  <si>
+    <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
+  </si>
+  <si>
+    <t>1a3cbfc3-1b32-46c6-a309-f1b050970913</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>54a51c62-7734-48bb-bd6f-fbfaf8084c6a</t>
+  </si>
+  <si>
+    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>cc82261e-4b4e-4e3f-a555-572075329c66</t>
+  </si>
+  <si>
+    <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
+  </si>
+  <si>
+    <t>ac513692-e9e0-46b9-9d8e-b2ad467d3e44</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>d3cc2b49-759f-4607-bc23-402a37c006e7</t>
+  </si>
+  <si>
+    <t>Required column RECORDED_TIME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "RECORDED_TIME"</t>
+  </si>
+  <si>
+    <t>609dbcfc-b949-47f9-ac8d-387f5580ffc8</t>
+  </si>
+  <si>
+    <t>Required column QUESTION is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION"</t>
+  </si>
+  <si>
+    <t>05490ae4-e0fa-403f-ae68-67de963f80af</t>
+  </si>
+  <si>
+    <t>Required column MEAS_VALUE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEAS_VALUE"</t>
+  </si>
+  <si>
+    <t>376da591-5f92-4c2c-97b5-e8cc32efc5a5</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION_CODE"</t>
+  </si>
+  <si>
+    <t>b8265db7-06ac-4073-8b32-9345021ef32a</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>037449b9-513c-40df-b8ee-afd4da827671</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ANSWER_CODE"</t>
+  </si>
+  <si>
+    <t>94d23651-ae5c-4d48-8a5f-36984ee5fd6e</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>98306097-8a78-4ffc-92e7-554c8d95aed4</t>
+  </si>
+  <si>
+    <t>Required column SDOH_DOMAIN is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SDOH_DOMAIN"</t>
+  </si>
+  <si>
+    <t>d5341699-5ee3-4924-8c23-87a4e6ac2bad</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>6b8ddece-df67-4487-8b89-e895576a7249</t>
+  </si>
+  <si>
+    <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
+  </si>
+  <si>
+    <t>c89e55ee-a55f-4ecd-848c-878981fc4fac</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>5a8d83aa-36e4-4477-908c-04d3bff84bd6</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_q_e_admin_data</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
+  </si>
+  <si>
+    <t>synthetic_fail</t>
+  </si>
+  <si>
+    <t>c87dfe5d-1ab6-406f-bd07-fcf6c45511a4</t>
+  </si>
+  <si>
+    <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
+  </si>
+  <si>
+    <t>1a6980aa-0d43-4796-a784-03e0d319cd05</t>
+  </si>
+  <si>
+    <t>Required column FACILITY is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "FACILITY"</t>
+  </si>
+  <si>
+    <t>8cc7ce7b-d361-4502-b323-4a40f2ba2243</t>
+  </si>
+  <si>
+    <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
+  </si>
+  <si>
+    <t>be12ecbf-c08f-4dfb-a04f-af326ba4330e</t>
+  </si>
+  <si>
+    <t>Required column LAST_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
+  </si>
+  <si>
+    <t>7f034c48-78da-4631-8c7a-614b44f8f6ce</t>
+  </si>
+  <si>
+    <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
+  </si>
+  <si>
+    <t>b10805d2-0afd-4c40-91b7-c26d8d28a765</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>ede6a6c4-80e8-442b-be4f-f9917d29afd9</t>
+  </si>
+  <si>
+    <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>1d616170-d1b3-470b-9263-a1fe3bfce729</t>
+  </si>
+  <si>
+    <t>Required column SURVEY is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SURVEY"</t>
+  </si>
+  <si>
+    <t>4b7f6515-fb93-4a1a-99be-e3c0dd8c9ce1</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>4a0fddb2-8390-419f-9df5-91e28b6fc7a9</t>
+  </si>
+  <si>
+    <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
+  </si>
+  <si>
+    <t>34160cc4-2cb7-46fe-9a40-1f098bdb42b2</t>
+  </si>
+  <si>
+    <t>Required column QUESTION is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION"</t>
+  </si>
+  <si>
+    <t>d2e44b8d-b5f8-4b2d-ba41-d8a15da0071c</t>
+  </si>
+  <si>
+    <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
+  </si>
+  <si>
+    <t>296feb73-a822-40ee-91a8-f6160d065f12</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
+  </si>
+  <si>
+    <t>8674a4b5-ab7a-45a4-9ebc-61fc71c9ab79</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>07b2795f-dff3-4247-a716-4bac3f9fe2de</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
+  </si>
+  <si>
+    <t>f325d4a9-f19c-4f3d-be4e-580466135a99</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>fab6dee2-5c52-4477-907a-4f0b2d9ea5cb</t>
+  </si>
+  <si>
+    <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
+  </si>
+  <si>
+    <t>be07b70a-3caa-47e4-bc00-db2034cbc07d</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>94f01b29-959f-4ef7-a894-58830b5543be</t>
+  </si>
+  <si>
+    <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
+  </si>
+  <si>
+    <t>d7ef1e9f-cd90-4650-9d51-15b19d669afa</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>b5f5ee76-e7e4-4bcb-92f1-f59718839eb8</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
@@ -72,7 +498,7 @@
     <t>ERROR</t>
   </si>
   <si>
-    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
   </si>
   <si>
     <t>Sheet Missing</t>
@@ -81,370 +507,25 @@
     <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
-  </si>
-  <si>
-    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
-  </si>
-  <si>
-    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
   </si>
   <si>
     <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>47277588-99e8-59f5-8384-b24344a86073</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_admin_demographic</t>
-  </si>
-  <si>
-    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
-  </si>
-  <si>
-    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_screening</t>
-  </si>
-  <si>
-    <t>db54c94e-e025-4555-92df-3b0472d624b8</t>
-  </si>
-  <si>
-    <t>Missing Column</t>
-  </si>
-  <si>
-    <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
-  </si>
-  <si>
-    <t>4c2d1bf8-0c52-4828-96ef-bf3f69d46d3d</t>
-  </si>
-  <si>
-    <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
-  </si>
-  <si>
-    <t>bd7aab99-46b7-449b-9155-b153985b713a</t>
-  </si>
-  <si>
-    <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
-  </si>
-  <si>
-    <t>93fe09ef-5ae8-4848-91ce-9fb9ab3d850b</t>
-  </si>
-  <si>
-    <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
-  </si>
-  <si>
-    <t>671d7155-1e1d-4126-a5eb-874ebc5d57e4</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>baf75e04-d1ba-4794-bf82-467be42dcc75</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>4c9c7ddf-1e6a-43a6-8c51-3fc78c145b00</t>
-  </si>
-  <si>
-    <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
-  </si>
-  <si>
-    <t>5a075599-6096-4961-8f04-96d8ef636f28</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>0a763e51-1479-429d-816c-2e3217ca63f0</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>5032c177-7c52-47de-8741-7d88464bc6fb</t>
-  </si>
-  <si>
-    <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
-  </si>
-  <si>
-    <t>d1626583-bba0-4ec9-9fab-8d3d2c87c1d1</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>778b95c3-3fc5-4c42-ac1f-65ac9ffb337f</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
-    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_q_e_admin_data</t>
-  </si>
-  <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
-  </si>
-  <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
-  </si>
-  <si>
-    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
-  </si>
-  <si>
-    <t>synthetic_fail</t>
-  </si>
-  <si>
-    <t>6116a37a-4e94-434c-be8d-fba574a57bce</t>
-  </si>
-  <si>
-    <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
-  </si>
-  <si>
-    <t>bb80d8cd-9031-4498-a11b-38ae517e03f9</t>
-  </si>
-  <si>
-    <t>Required column FACILITY is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "FACILITY"</t>
-  </si>
-  <si>
-    <t>57d5489c-47c5-4b5e-9d00-fc041385ae69</t>
-  </si>
-  <si>
-    <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
-  </si>
-  <si>
-    <t>62687b89-afce-4bd1-9e6c-62223f7cda02</t>
-  </si>
-  <si>
-    <t>Required column LAST_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
-  </si>
-  <si>
-    <t>9af44f4a-6258-4de2-97fb-ea9d8177f53a</t>
-  </si>
-  <si>
-    <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
-  </si>
-  <si>
-    <t>b3fc3589-7c0c-4771-a0d5-ad279731ed07</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>88af3db6-67b0-4be4-b33f-994457cae455</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>517e26e8-cc26-4f27-a93e-f56c69125462</t>
-  </si>
-  <si>
-    <t>Required column SURVEY is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "SURVEY"</t>
-  </si>
-  <si>
-    <t>12bbdabc-2df6-4bb7-ae05-ce78637576d6</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>d6de092b-1701-4af9-87b4-4071f1b58824</t>
-  </si>
-  <si>
-    <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
-  </si>
-  <si>
-    <t>30dad59d-3b76-4375-9c0d-6497f09395ca</t>
-  </si>
-  <si>
-    <t>Required column QUESTION is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "QUESTION"</t>
-  </si>
-  <si>
-    <t>3317574e-4eb9-41df-96d8-77f3f1d6c9c7</t>
-  </si>
-  <si>
-    <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
-  </si>
-  <si>
-    <t>8b2d7596-295c-408b-8271-26af2725bd3c</t>
-  </si>
-  <si>
-    <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
-  </si>
-  <si>
-    <t>032d1455-a432-4455-866d-636379cc0113</t>
-  </si>
-  <si>
-    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
-  </si>
-  <si>
-    <t>2421138d-c86c-40f8-8e39-0554a6102f76</t>
-  </si>
-  <si>
-    <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
-  </si>
-  <si>
-    <t>a58ce8f9-34a1-4af0-9a4a-d3a5529d0077</t>
-  </si>
-  <si>
-    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
-  </si>
-  <si>
-    <t>057d87d0-a510-46e2-8f78-9e338600eee8</t>
-  </si>
-  <si>
-    <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
-  </si>
-  <si>
-    <t>cafc25aa-fc22-46ac-891b-499239ff5185</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>50c4fd24-d066-4db3-af9b-edbf4b3f0492</t>
-  </si>
-  <si>
-    <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
-  </si>
-  <si>
-    <t>7c58c117-1e20-4bfc-a928-5dfc96c7defe</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>69912e9f-389d-4309-a46a-108e5cf22159</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-12-12-2023-valid.csv</t>
@@ -453,7 +534,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>fd70db33-83de-4564-81a8-22016e1fb21b</t>
+    <t>636f92f8-6814-4edb-af3c-d99d67ddf391</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +552,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>ac4b863f-7c12-4bc0-8385-a953e1ca6c22</t>
-  </si>
-  <si>
-    <t>c3ef3362-8bc0-427f-a20c-e74abf3f398e</t>
-  </si>
-  <si>
-    <t>165159a9-2592-401c-bd36-0621c4cc8b6d</t>
-  </si>
-  <si>
-    <t>fb89466b-6735-4a0d-a141-0e490d798c7b</t>
-  </si>
-  <si>
-    <t>cf44dd80-6825-4395-8237-be93d4e22374</t>
-  </si>
-  <si>
-    <t>40cb2fbe-db4e-4e00-9846-b7b9ae3d3a49</t>
-  </si>
-  <si>
-    <t>23108655-c46e-4507-aa83-96cd25985e8d</t>
-  </si>
-  <si>
-    <t>e89539f2-c751-4cf3-962c-c0cba00848b4</t>
-  </si>
-  <si>
-    <t>06f6ffd3-ef5c-409f-b990-137697918f42</t>
-  </si>
-  <si>
-    <t>70652dd0-f325-4b7a-981b-469e2453e8c1</t>
-  </si>
-  <si>
-    <t>81650c85-fd50-471e-8fc8-e9a15156448a</t>
-  </si>
-  <si>
-    <t>882d4a4b-6e7e-4822-878f-30a769069d3d</t>
-  </si>
-  <si>
-    <t>94dd2556-9e09-4f07-96df-401430c7ecd9</t>
-  </si>
-  <si>
-    <t>e99b5a98-6e87-4d94-a7b7-0eedc5b71a77</t>
-  </si>
-  <si>
-    <t>97c77468-b41c-4e4f-98bf-114f6a221b0b</t>
-  </si>
-  <si>
-    <t>6a14248a-eefb-429d-959c-e0ccd57c6ae2</t>
-  </si>
-  <si>
-    <t>50fda451-475b-448b-8b87-e70843e852f8</t>
-  </si>
-  <si>
-    <t>cf5a1b31-3567-4096-adc7-769e42e206e1</t>
-  </si>
-  <si>
-    <t>87ec150d-1cd3-476e-8cb4-38ca49c550a9</t>
-  </si>
-  <si>
-    <t>7772fe11-edb7-4004-8f15-7b6ada8d6282</t>
-  </si>
-  <si>
-    <t>61beca90-96cb-431f-ab58-d0122791fd81</t>
-  </si>
-  <si>
-    <t>b4d48c0f-1002-4492-ab15-94459a117702</t>
-  </si>
-  <si>
-    <t>601ad1d2-31e2-405d-8e4d-3c16008308a7</t>
-  </si>
-  <si>
-    <t>39b53120-1f5a-426b-b2a9-8533089e09c7</t>
-  </si>
-  <si>
-    <t>aa6fce67-0d05-422a-af60-fce41e223634</t>
-  </si>
-  <si>
-    <t>f59499c5-ddf1-451e-919a-0deae4bb1665</t>
+    <t>a53ea21e-175e-4a87-9c41-acf3121a1bb1</t>
+  </si>
+  <si>
+    <t>23e8d74a-18ac-4ebe-b81f-0af71f51d3db</t>
+  </si>
+  <si>
+    <t>0ec176ea-8e64-464d-82b1-f91292ab1457</t>
+  </si>
+  <si>
+    <t>05537ddc-4abc-42cb-995f-a709757e2999</t>
+  </si>
+  <si>
+    <t>c5736093-046a-4fc1-8f62-f4b880b93bcd</t>
+  </si>
+  <si>
+    <t>746dace2-d191-4018-a49a-be453c122778</t>
+  </si>
+  <si>
+    <t>624a1a45-dd50-494e-8fa2-76273725cb80</t>
+  </si>
+  <si>
+    <t>12167f7e-ff5c-4b69-bda2-66d7bf1d9545</t>
+  </si>
+  <si>
+    <t>cb7b93f9-3e40-4560-a99d-ed983fb1dc4a</t>
+  </si>
+  <si>
+    <t>6c9ef092-2905-4e91-a70c-ce275a298cad</t>
+  </si>
+  <si>
+    <t>e41ec874-61d4-48fd-a7ce-dbb4e633c8f4</t>
+  </si>
+  <si>
+    <t>dde536f8-ee57-4c80-8b54-8e257b567bee</t>
+  </si>
+  <si>
+    <t>c5dc2c30-828f-436e-8768-862714d7dcbf</t>
+  </si>
+  <si>
+    <t>64749c98-ff94-43bf-82d2-eefaaac5cab0</t>
+  </si>
+  <si>
+    <t>ca5c2890-aac6-48e7-993a-bfc9434c9858</t>
+  </si>
+  <si>
+    <t>7ab8ff9f-3161-48bf-ad6a-2f18e2817bd2</t>
+  </si>
+  <si>
+    <t>c6a34c81-2d0b-4aa6-859b-2e1c40ddb40c</t>
+  </si>
+  <si>
+    <t>4803f10a-1652-4692-a096-c39859a0fd9a</t>
+  </si>
+  <si>
+    <t>c06f31d3-1407-40aa-9ec3-37536b752d6c</t>
+  </si>
+  <si>
+    <t>313b0d12-d0d8-4e71-92b1-c0e088245746</t>
+  </si>
+  <si>
+    <t>6caae179-c18f-4314-a88a-56de476644c2</t>
+  </si>
+  <si>
+    <t>fb80dc58-7e6d-4712-9723-b25b3d5147bc</t>
+  </si>
+  <si>
+    <t>77dd4874-123e-408f-9c0b-2128071893e2</t>
+  </si>
+  <si>
+    <t>a9744940-48d7-4230-909a-1280b44f1c74</t>
+  </si>
+  <si>
+    <t>f1eea481-1f08-4872-bfb9-980a26707ea2</t>
+  </si>
+  <si>
+    <t>93628a6a-23cc-4b1f-a736-aba583812f14</t>
   </si>
 </sst>
 </file>
@@ -710,19 +791,19 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4">
@@ -733,25 +814,25 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -762,25 +843,25 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
         <v>32</v>
       </c>
       <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>34</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -791,25 +872,25 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
         <v>36</v>
       </c>
-      <c r="H6" t="s">
+      <c r="N6" t="s">
         <v>37</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -820,25 +901,25 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="N7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
@@ -849,25 +930,25 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="N8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9">
@@ -878,25 +959,25 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="N9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -907,25 +988,25 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="N10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
@@ -936,25 +1017,25 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
@@ -965,25 +1046,25 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
@@ -994,25 +1075,25 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -1023,25 +1104,25 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15">
@@ -1052,25 +1133,25 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -1081,25 +1162,25 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="N16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
@@ -1110,25 +1191,25 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="N17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18">
@@ -1139,25 +1220,25 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>77</v>
-      </c>
-      <c r="M18" t="s">
-        <v>30</v>
+        <v>72</v>
+      </c>
+      <c r="N18" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19">
@@ -1168,25 +1249,25 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="H19" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="N19" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -1197,25 +1278,25 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" t="s">
         <v>78</v>
       </c>
-      <c r="E20" t="s">
+      <c r="N20" t="s">
         <v>79</v>
-      </c>
-      <c r="F20" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" t="s">
-        <v>84</v>
-      </c>
-      <c r="I20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" t="s">
-        <v>85</v>
-      </c>
-      <c r="N20" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -1226,25 +1307,25 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" t="s">
         <v>80</v>
       </c>
-      <c r="H21" t="s">
-        <v>87</v>
-      </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J21" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="N21" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
@@ -1255,25 +1336,25 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J22" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N22" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23">
@@ -1284,25 +1365,25 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="H23" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J23" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N23" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24">
@@ -1313,25 +1394,25 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="J24" t="s">
-        <v>97</v>
-      </c>
-      <c r="N24" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="M24" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25">
@@ -1342,25 +1423,25 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H25" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I25" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="N25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -1371,25 +1452,25 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I26" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="N26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27">
@@ -1400,25 +1481,25 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H27" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I27" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="N27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28">
@@ -1429,25 +1510,25 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H28" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I28" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29">
@@ -1458,25 +1539,25 @@
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F29" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I29" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N29" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
@@ -1487,25 +1568,25 @@
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F30" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31">
@@ -1516,25 +1597,25 @@
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I31" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32">
@@ -1545,25 +1626,25 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H32" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N32" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33">
@@ -1574,25 +1655,25 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E33" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I33" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="N33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34">
@@ -1603,25 +1684,25 @@
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F34" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H34" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I34" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N34" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35">
@@ -1632,25 +1713,25 @@
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F35" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H35" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I35" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J35" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N35" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36">
@@ -1661,25 +1742,25 @@
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F36" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H36" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37">
@@ -1690,25 +1771,25 @@
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F37" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H37" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I37" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J37" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N37" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38">
@@ -1719,25 +1800,25 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H38" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I38" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J38" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N38" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39">
@@ -1748,25 +1829,25 @@
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="H39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I39" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J39" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N39" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="40">
@@ -1777,34 +1858,25 @@
         <v>16</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="E40" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="F40" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="H40" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="I40" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="J40" t="s">
-        <v>149</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40" t="s">
-        <v>150</v>
-      </c>
-      <c r="M40" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="N40" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41">
@@ -1815,34 +1887,25 @@
         <v>16</v>
       </c>
       <c r="D41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F41" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41" t="s">
         <v>144</v>
       </c>
-      <c r="E41" t="s">
+      <c r="I41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" t="s">
         <v>145</v>
       </c>
-      <c r="F41" t="s">
+      <c r="N41" t="s">
         <v>146</v>
-      </c>
-      <c r="H41" t="s">
-        <v>153</v>
-      </c>
-      <c r="I41" t="s">
-        <v>148</v>
-      </c>
-      <c r="J41" t="s">
-        <v>149</v>
-      </c>
-      <c r="K41">
-        <v>2</v>
-      </c>
-      <c r="L41" t="s">
-        <v>150</v>
-      </c>
-      <c r="M41" t="s">
-        <v>151</v>
-      </c>
-      <c r="N41" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="42">
@@ -1853,34 +1916,25 @@
         <v>16</v>
       </c>
       <c r="D42" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="E42" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="F42" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="H42" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="I42" t="s">
+        <v>26</v>
+      </c>
+      <c r="J42" t="s">
         <v>148</v>
       </c>
-      <c r="J42" t="s">
+      <c r="N42" t="s">
         <v>149</v>
-      </c>
-      <c r="K42">
-        <v>3</v>
-      </c>
-      <c r="L42" t="s">
-        <v>150</v>
-      </c>
-      <c r="M42" t="s">
-        <v>151</v>
-      </c>
-      <c r="N42" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="43">
@@ -1891,30 +1945,21 @@
         <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="E43" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="F43" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="H43" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I43" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="J43" t="s">
-        <v>149</v>
-      </c>
-      <c r="K43">
-        <v>4</v>
-      </c>
-      <c r="L43" t="s">
-        <v>150</v>
-      </c>
-      <c r="M43" t="s">
         <v>151</v>
       </c>
       <c r="N43" t="s">
@@ -1929,34 +1974,25 @@
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="F44" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="H44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I44" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="J44" t="s">
-        <v>149</v>
-      </c>
-      <c r="K44">
-        <v>5</v>
-      </c>
-      <c r="L44" t="s">
-        <v>150</v>
-      </c>
-      <c r="M44" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N44" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45">
@@ -1967,34 +2003,25 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="E45" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="H45" t="s">
+        <v>156</v>
+      </c>
+      <c r="I45" t="s">
+        <v>26</v>
+      </c>
+      <c r="J45" t="s">
         <v>157</v>
       </c>
-      <c r="I45" t="s">
-        <v>148</v>
-      </c>
-      <c r="J45" t="s">
-        <v>149</v>
-      </c>
-      <c r="K45">
-        <v>6</v>
-      </c>
-      <c r="L45" t="s">
-        <v>150</v>
-      </c>
-      <c r="M45" t="s">
-        <v>151</v>
-      </c>
       <c r="N45" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46">
@@ -2005,34 +2032,25 @@
         <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="E46" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="F46" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="H46" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I46" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="J46" t="s">
-        <v>149</v>
-      </c>
-      <c r="K46">
-        <v>7</v>
-      </c>
-      <c r="L46" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="M46" t="s">
-        <v>151</v>
-      </c>
-      <c r="N46" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="47">
@@ -2043,34 +2061,25 @@
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="E47" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="F47" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="H47" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="I47" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="J47" t="s">
-        <v>149</v>
-      </c>
-      <c r="K47">
-        <v>8</v>
-      </c>
-      <c r="L47" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="M47" t="s">
-        <v>151</v>
-      </c>
-      <c r="N47" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48">
@@ -2081,34 +2090,25 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E48" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="F48" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="H48" t="s">
+        <v>169</v>
+      </c>
+      <c r="I48" t="s">
+        <v>163</v>
+      </c>
+      <c r="J48" t="s">
+        <v>170</v>
+      </c>
+      <c r="M48" t="s">
         <v>160</v>
-      </c>
-      <c r="I48" t="s">
-        <v>148</v>
-      </c>
-      <c r="J48" t="s">
-        <v>149</v>
-      </c>
-      <c r="K48">
-        <v>9</v>
-      </c>
-      <c r="L48" t="s">
-        <v>150</v>
-      </c>
-      <c r="M48" t="s">
-        <v>151</v>
-      </c>
-      <c r="N48" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="49">
@@ -2119,34 +2119,34 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E49" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F49" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H49" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="I49" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J49" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K49">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L49" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M49" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N49" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50">
@@ -2157,34 +2157,34 @@
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E50" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H50" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="I50" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J50" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K50">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="L50" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M50" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N50" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51">
@@ -2195,34 +2195,34 @@
         <v>16</v>
       </c>
       <c r="D51" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E51" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F51" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H51" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c r="I51" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J51" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K51">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L51" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M51" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N51" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52">
@@ -2233,34 +2233,34 @@
         <v>16</v>
       </c>
       <c r="D52" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E52" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F52" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H52" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c r="I52" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J52" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K52">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="L52" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M52" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N52" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53">
@@ -2271,34 +2271,34 @@
         <v>16</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F53" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H53" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="I53" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J53" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K53">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="L53" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M53" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N53" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54">
@@ -2309,34 +2309,34 @@
         <v>16</v>
       </c>
       <c r="D54" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E54" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F54" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H54" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="I54" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J54" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K54">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L54" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M54" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N54" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55">
@@ -2347,34 +2347,34 @@
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E55" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F55" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H55" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="I55" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J55" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K55">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="L55" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M55" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N55" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56">
@@ -2385,34 +2385,34 @@
         <v>16</v>
       </c>
       <c r="D56" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E56" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F56" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H56" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="I56" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J56" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K56">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="L56" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M56" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N56" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57">
@@ -2423,34 +2423,34 @@
         <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E57" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F57" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H57" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="I57" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J57" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K57">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="L57" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M57" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N57" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58">
@@ -2461,34 +2461,34 @@
         <v>16</v>
       </c>
       <c r="D58" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F58" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H58" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="I58" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J58" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K58">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="L58" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M58" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N58" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59">
@@ -2499,34 +2499,34 @@
         <v>16</v>
       </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F59" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H59" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="I59" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J59" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K59">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="L59" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M59" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N59" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60">
@@ -2537,34 +2537,34 @@
         <v>16</v>
       </c>
       <c r="D60" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E60" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F60" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H60" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="I60" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J60" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K60">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="L60" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M60" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N60" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61">
@@ -2575,34 +2575,34 @@
         <v>16</v>
       </c>
       <c r="D61" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E61" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F61" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H61" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
       <c r="I61" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J61" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K61">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="L61" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M61" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N61" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62">
@@ -2613,34 +2613,34 @@
         <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F62" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H62" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="I62" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="J62" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K62">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="L62" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M62" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N62" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63">
@@ -2651,34 +2651,34 @@
         <v>16</v>
       </c>
       <c r="D63" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E63" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F63" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H63" t="s">
+        <v>193</v>
+      </c>
+      <c r="I63" t="s">
         <v>175</v>
       </c>
-      <c r="I63" t="s">
-        <v>148</v>
-      </c>
       <c r="J63" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="K63">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L63" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M63" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N63" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64">
@@ -2689,34 +2689,34 @@
         <v>16</v>
       </c>
       <c r="D64" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E64" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F64" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H64" t="s">
+        <v>194</v>
+      </c>
+      <c r="I64" t="s">
+        <v>175</v>
+      </c>
+      <c r="J64" t="s">
         <v>176</v>
       </c>
-      <c r="I64" t="s">
-        <v>148</v>
-      </c>
-      <c r="J64" t="s">
-        <v>149</v>
-      </c>
       <c r="K64">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="L64" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="M64" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N64" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65">
@@ -2727,34 +2727,34 @@
         <v>16</v>
       </c>
       <c r="D65" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E65" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F65" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H65" t="s">
+        <v>195</v>
+      </c>
+      <c r="I65" t="s">
+        <v>175</v>
+      </c>
+      <c r="J65" t="s">
+        <v>176</v>
+      </c>
+      <c r="K65">
+        <v>17</v>
+      </c>
+      <c r="L65" t="s">
         <v>177</v>
       </c>
-      <c r="I65" t="s">
-        <v>148</v>
-      </c>
-      <c r="J65" t="s">
-        <v>149</v>
-      </c>
-      <c r="K65">
-        <v>26</v>
-      </c>
-      <c r="L65" t="s">
-        <v>150</v>
-      </c>
       <c r="M65" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="N65" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66">
@@ -2765,34 +2765,376 @@
         <v>16</v>
       </c>
       <c r="D66" t="s">
-        <v>144</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="F66" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="H66" t="s">
+        <v>196</v>
+      </c>
+      <c r="I66" t="s">
+        <v>175</v>
+      </c>
+      <c r="J66" t="s">
+        <v>176</v>
+      </c>
+      <c r="K66">
+        <v>18</v>
+      </c>
+      <c r="L66" t="s">
+        <v>177</v>
+      </c>
+      <c r="M66" t="s">
         <v>178</v>
       </c>
-      <c r="I66" t="s">
-        <v>148</v>
-      </c>
-      <c r="J66" t="s">
-        <v>149</v>
-      </c>
-      <c r="K66">
+      <c r="N66" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>15</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>171</v>
+      </c>
+      <c r="E67" t="s">
+        <v>172</v>
+      </c>
+      <c r="F67" t="s">
+        <v>173</v>
+      </c>
+      <c r="H67" t="s">
+        <v>197</v>
+      </c>
+      <c r="I67" t="s">
+        <v>175</v>
+      </c>
+      <c r="J67" t="s">
+        <v>176</v>
+      </c>
+      <c r="K67">
+        <v>19</v>
+      </c>
+      <c r="L67" t="s">
+        <v>177</v>
+      </c>
+      <c r="M67" t="s">
+        <v>178</v>
+      </c>
+      <c r="N67" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>15</v>
+      </c>
+      <c r="B68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68" t="s">
+        <v>171</v>
+      </c>
+      <c r="E68" t="s">
+        <v>172</v>
+      </c>
+      <c r="F68" t="s">
+        <v>173</v>
+      </c>
+      <c r="H68" t="s">
+        <v>198</v>
+      </c>
+      <c r="I68" t="s">
+        <v>175</v>
+      </c>
+      <c r="J68" t="s">
+        <v>176</v>
+      </c>
+      <c r="K68">
+        <v>20</v>
+      </c>
+      <c r="L68" t="s">
+        <v>177</v>
+      </c>
+      <c r="M68" t="s">
+        <v>178</v>
+      </c>
+      <c r="N68" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" t="s">
+        <v>171</v>
+      </c>
+      <c r="E69" t="s">
+        <v>172</v>
+      </c>
+      <c r="F69" t="s">
+        <v>173</v>
+      </c>
+      <c r="H69" t="s">
+        <v>199</v>
+      </c>
+      <c r="I69" t="s">
+        <v>175</v>
+      </c>
+      <c r="J69" t="s">
+        <v>176</v>
+      </c>
+      <c r="K69">
+        <v>21</v>
+      </c>
+      <c r="L69" t="s">
+        <v>177</v>
+      </c>
+      <c r="M69" t="s">
+        <v>178</v>
+      </c>
+      <c r="N69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>15</v>
+      </c>
+      <c r="B70" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" t="s">
+        <v>171</v>
+      </c>
+      <c r="E70" t="s">
+        <v>172</v>
+      </c>
+      <c r="F70" t="s">
+        <v>173</v>
+      </c>
+      <c r="H70" t="s">
+        <v>200</v>
+      </c>
+      <c r="I70" t="s">
+        <v>175</v>
+      </c>
+      <c r="J70" t="s">
+        <v>176</v>
+      </c>
+      <c r="K70">
+        <v>22</v>
+      </c>
+      <c r="L70" t="s">
+        <v>177</v>
+      </c>
+      <c r="M70" t="s">
+        <v>178</v>
+      </c>
+      <c r="N70" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" t="s">
+        <v>171</v>
+      </c>
+      <c r="E71" t="s">
+        <v>172</v>
+      </c>
+      <c r="F71" t="s">
+        <v>173</v>
+      </c>
+      <c r="H71" t="s">
+        <v>201</v>
+      </c>
+      <c r="I71" t="s">
+        <v>175</v>
+      </c>
+      <c r="J71" t="s">
+        <v>176</v>
+      </c>
+      <c r="K71">
+        <v>23</v>
+      </c>
+      <c r="L71" t="s">
+        <v>177</v>
+      </c>
+      <c r="M71" t="s">
+        <v>178</v>
+      </c>
+      <c r="N71" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" t="s">
+        <v>16</v>
+      </c>
+      <c r="D72" t="s">
+        <v>171</v>
+      </c>
+      <c r="E72" t="s">
+        <v>172</v>
+      </c>
+      <c r="F72" t="s">
+        <v>173</v>
+      </c>
+      <c r="H72" t="s">
+        <v>202</v>
+      </c>
+      <c r="I72" t="s">
+        <v>175</v>
+      </c>
+      <c r="J72" t="s">
+        <v>176</v>
+      </c>
+      <c r="K72">
+        <v>24</v>
+      </c>
+      <c r="L72" t="s">
+        <v>177</v>
+      </c>
+      <c r="M72" t="s">
+        <v>178</v>
+      </c>
+      <c r="N72" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" t="s">
+        <v>171</v>
+      </c>
+      <c r="E73" t="s">
+        <v>172</v>
+      </c>
+      <c r="F73" t="s">
+        <v>173</v>
+      </c>
+      <c r="H73" t="s">
+        <v>203</v>
+      </c>
+      <c r="I73" t="s">
+        <v>175</v>
+      </c>
+      <c r="J73" t="s">
+        <v>176</v>
+      </c>
+      <c r="K73">
+        <v>25</v>
+      </c>
+      <c r="L73" t="s">
+        <v>177</v>
+      </c>
+      <c r="M73" t="s">
+        <v>178</v>
+      </c>
+      <c r="N73" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>171</v>
+      </c>
+      <c r="E74" t="s">
+        <v>172</v>
+      </c>
+      <c r="F74" t="s">
+        <v>173</v>
+      </c>
+      <c r="H74" t="s">
+        <v>204</v>
+      </c>
+      <c r="I74" t="s">
+        <v>175</v>
+      </c>
+      <c r="J74" t="s">
+        <v>176</v>
+      </c>
+      <c r="K74">
+        <v>26</v>
+      </c>
+      <c r="L74" t="s">
+        <v>177</v>
+      </c>
+      <c r="M74" t="s">
+        <v>178</v>
+      </c>
+      <c r="N74" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
+        <v>171</v>
+      </c>
+      <c r="E75" t="s">
+        <v>172</v>
+      </c>
+      <c r="F75" t="s">
+        <v>173</v>
+      </c>
+      <c r="H75" t="s">
+        <v>205</v>
+      </c>
+      <c r="I75" t="s">
+        <v>175</v>
+      </c>
+      <c r="J75" t="s">
+        <v>176</v>
+      </c>
+      <c r="K75">
         <v>27</v>
       </c>
-      <c r="L66" t="s">
-        <v>150</v>
-      </c>
-      <c r="M66" t="s">
-        <v>151</v>
-      </c>
-      <c r="N66" t="s">
-        <v>152</v>
+      <c r="L75" t="s">
+        <v>177</v>
+      </c>
+      <c r="M75" t="s">
+        <v>178</v>
+      </c>
+      <c r="N75" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: use new SQLa type safety features
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -72,7 +72,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>25355414-e403-4a71-9f97-6080aa7bf3a2</t>
+    <t>38749fe7-b3cd-4f6e-97a2-c7f4e3f8fdf2</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -84,7 +84,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>1b56ef89-bbe2-4316-9053-88092657c1f1</t>
+    <t>61d9a7d6-09b4-4fa4-97c7-220513b0962f</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -93,7 +93,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>e2319144-804e-4b6e-9e1c-b4f3879f087e</t>
+    <t>72ee7100-3a87-4ffa-aef0-2640c5df8cfa</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -102,7 +102,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>6854ff25-99aa-4cfd-8f56-bb8555cd2907</t>
+    <t>ad3b3796-a803-481a-a257-b321bbf6d1bb</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -111,7 +111,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>8f598ae7-822d-4c83-982e-4ffbb6c659b0</t>
+    <t>ae8b6413-3631-4443-9d38-f9e073a456ad</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -120,7 +120,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>7e545c76-8575-4640-8f1d-19b211581e88</t>
+    <t>e75ba306-36f4-45af-9a08-0a5e544bc4a0</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -129,7 +129,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>2ff4dd2b-6851-41f3-b12c-d851ee7a48d8</t>
+    <t>60da1c0b-5068-4ac1-a523-891c5609d783</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -138,7 +138,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>81cde82d-dc27-4b05-bfb5-d8647e2567a5</t>
+    <t>3d5a282e-4e68-4ad2-a5ab-61a4d9f51f36</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -147,7 +147,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>e4664262-9986-4c1a-888c-de73c88ec7df</t>
+    <t>17e73e9c-ed54-4f14-a303-35942c0bf1a4</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -156,7 +156,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>c215c80d-a0fc-4cef-9b26-bd3395bb442e</t>
+    <t>112188d1-8d0a-46d8-81d5-a95331127302</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -165,7 +165,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>261d05e0-5f76-48a2-97a1-1ca728d5ab8a</t>
+    <t>424f0088-d833-465a-9e04-b82b9cef5847</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -174,7 +174,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>1a853360-4bee-4809-b696-8b450323cd4f</t>
+    <t>29552173-a34c-4876-b3d2-68bbe72b9f03</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -183,7 +183,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>6aff6844-8fa9-4df4-bc8d-44a219fa3aca</t>
+    <t>8632494b-90c5-4ad5-a9f5-610bc116ff9a</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -192,7 +192,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>f83f927c-1bc3-4945-91c1-cf1093672932</t>
+    <t>da3d4b96-64f1-4852-9050-3c33c85d73a2</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -201,7 +201,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>ef87acfe-68c3-429b-8899-2dd51e520782</t>
+    <t>06ef4839-7e61-4c95-90ef-0290f03fd23b</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -210,7 +210,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>23321b2a-c50f-4d54-854e-fd5d052cf775</t>
+    <t>27aeace6-65a0-4a33-8240-3694f7fa1f28</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -219,7 +219,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>5ababacc-22c3-4324-8191-32e38155389c</t>
+    <t>1b504d3f-18d7-482a-82c3-ac0ce2d4cc17</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -228,7 +228,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>fef18579-457a-4cc8-9545-4368a58aa2f7</t>
+    <t>1a6b4a7e-dd5d-46b7-885b-fa0ccfac5470</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -237,7 +237,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>3bde8af0-cd21-4b71-8ed5-e5c0e239ba46</t>
+    <t>82940c83-c0e9-4636-9e7b-9842532da0c0</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -246,7 +246,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>cdf71f13-ef66-48d8-88c3-be8ed69b67fe</t>
+    <t>6d9ff95f-3179-420b-b1c6-c0c5104e60e6</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -255,7 +255,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>5e9c72ef-9215-4fb8-8bf3-7e89d7723db6</t>
+    <t>1bbf963b-1188-4e4d-91af-6fd31bfae417</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -324,7 +324,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>41012e63-00c6-4517-a855-8a5f49bfaaca</t>
+    <t>117892cf-b527-401f-a916-1cd63b761a3e</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -333,7 +333,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>ef79d627-c51c-4286-bdd5-824d29a0fe60</t>
+    <t>73947d22-66c7-44fa-8b23-35c64dc10a23</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -342,7 +342,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>6adcc105-6856-42dc-9bd0-c58399db18ac</t>
+    <t>4358499b-2b79-4251-a3b4-6297f7d901fc</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -351,7 +351,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>3a02e275-c59f-4336-a1a5-eb53a5e17bac</t>
+    <t>0fb4bf12-5a94-4aa9-9481-0790070c4a7a</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -360,7 +360,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>6ef5cda9-8ba5-47ac-bc46-a45b3b79e73c</t>
+    <t>8208bb57-ff1a-4b53-8d71-e7313f90d59b</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -369,7 +369,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>65a20fd7-d9f1-46fc-85e9-11948c17376a</t>
+    <t>6014344d-23e6-41c3-8931-d3ae02cd786e</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -378,7 +378,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>cadff939-0510-4454-80dd-a3a3bad3bac2</t>
+    <t>58b9ecad-c9e9-4358-9fd2-3debb8224e16</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -387,7 +387,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>7a249006-c736-4bf7-8069-c33577b577ac</t>
+    <t>7bd902c7-513c-4514-acaa-bca929857511</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -396,7 +396,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>f5702bc4-e786-43d9-9709-5ca8ed9443a2</t>
+    <t>4ad23d64-7ad5-49a8-bc68-c02073093772</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -405,7 +405,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>fa2c1c05-b864-4bbe-8d8e-0721091f66f5</t>
+    <t>20ad9557-2e53-4b45-8f8d-732fce01b81d</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -414,7 +414,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>b6cd623c-869c-48a6-9548-fedf900c7b3d</t>
+    <t>eec2748c-967b-4cd7-bdce-c6249409416d</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -423,7 +423,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>ec1daff2-2c0d-4dba-a92e-14fe7ec05cea</t>
+    <t>dc8a448d-9e59-44ce-943b-d54d902b9ec5</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -453,7 +453,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>dbcf4d4f-ab9c-4420-b977-4a571e5854f3</t>
+    <t>a61ab194-a83f-4bcb-98dd-ad06b667e2bb</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>834c840c-2128-4230-9bb2-96c010c4ac50</t>
-  </si>
-  <si>
-    <t>cc0adc27-91ad-4954-9dd4-00c5caa065e2</t>
-  </si>
-  <si>
-    <t>23bd8653-47f0-4a96-8fe7-f65e772fd1dd</t>
-  </si>
-  <si>
-    <t>fedd488b-1912-4054-a35e-83a86e663a1b</t>
-  </si>
-  <si>
-    <t>2158ebdb-2bcc-4a89-acba-2fcf7aac09bf</t>
-  </si>
-  <si>
-    <t>d6d781a1-9b26-41e4-af2a-0a07a644a729</t>
-  </si>
-  <si>
-    <t>287cb160-6ce0-40b1-a377-d55259212842</t>
-  </si>
-  <si>
-    <t>2b23accd-af68-4489-8956-3c8f2f73c6df</t>
-  </si>
-  <si>
-    <t>2456e234-d97d-428e-ba67-74d639c2a5b4</t>
-  </si>
-  <si>
-    <t>68ace895-9b05-4372-b103-58d7276a08bd</t>
-  </si>
-  <si>
-    <t>41d7fd81-ca3d-43fc-a1d7-b4318cfbb035</t>
-  </si>
-  <si>
-    <t>5f85e3dc-4357-4881-acb4-e136cf871668</t>
-  </si>
-  <si>
-    <t>611faf43-28d4-4e1d-be20-d4e96ab0796f</t>
-  </si>
-  <si>
-    <t>69b16ba6-ca9c-4df6-9cf9-6ac0539560d9</t>
-  </si>
-  <si>
-    <t>b342bc4c-0d88-478f-943c-831652ae20c9</t>
-  </si>
-  <si>
-    <t>1619b1a9-30ba-43d8-af1e-94795affc4b5</t>
-  </si>
-  <si>
-    <t>93e45942-6ce2-4d19-a1f3-a73cf206bfeb</t>
-  </si>
-  <si>
-    <t>941e3870-a691-4ac4-9069-b52adbf72512</t>
-  </si>
-  <si>
-    <t>12248dd0-4cb7-4e97-9c3e-ee41c7ec7632</t>
-  </si>
-  <si>
-    <t>91e7c757-f144-4cc0-ae09-d646cecf4ff2</t>
-  </si>
-  <si>
-    <t>5cfb8357-271d-47a5-8e9d-8a22c038abc8</t>
-  </si>
-  <si>
-    <t>a479e402-6e8e-4431-af92-8457dc0b783e</t>
-  </si>
-  <si>
-    <t>44123e1c-b561-4fb1-944c-a7c10e0561dd</t>
-  </si>
-  <si>
-    <t>40c38ca1-859f-4722-900f-37521fdaffd1</t>
-  </si>
-  <si>
-    <t>cf312695-2492-4be3-9535-7033fa12be3b</t>
-  </si>
-  <si>
-    <t>ec57fcd2-1d19-4746-95dc-e68034fb1ad9</t>
+    <t>5b214c54-2e50-4e01-ae22-f0bb3e58a741</t>
+  </si>
+  <si>
+    <t>1034729c-f84d-486e-94fd-952cbd2fef7e</t>
+  </si>
+  <si>
+    <t>827fbffc-d9e7-403f-84fb-e152692ffd62</t>
+  </si>
+  <si>
+    <t>fdf0de5c-bc22-4b9d-9288-b51064314c88</t>
+  </si>
+  <si>
+    <t>067a5e3f-d138-4735-a96a-b0795c02af1a</t>
+  </si>
+  <si>
+    <t>788f51c2-447a-47b0-bb3c-89dfb0a183d5</t>
+  </si>
+  <si>
+    <t>8a4d4437-dcc9-474e-a21c-1fc98bdb9c39</t>
+  </si>
+  <si>
+    <t>8aa636d7-4e67-43cd-878a-8c670062131f</t>
+  </si>
+  <si>
+    <t>cc24ee55-84c2-410b-ae9b-e57f47975a3c</t>
+  </si>
+  <si>
+    <t>95d5d741-44eb-4c35-ba83-fd3a779823f5</t>
+  </si>
+  <si>
+    <t>01c5a162-4c1a-48a8-9a33-e02f5e5bdb9e</t>
+  </si>
+  <si>
+    <t>9432e199-654b-475c-b37c-6102f4a903e6</t>
+  </si>
+  <si>
+    <t>42b4cc12-b23d-4035-aa70-cb8fd1e023e2</t>
+  </si>
+  <si>
+    <t>ba0f9c27-ecf4-488f-9fbf-c53bc67a93f8</t>
+  </si>
+  <si>
+    <t>22c1e39d-d1e6-4836-a068-559369f60ff7</t>
+  </si>
+  <si>
+    <t>4e530af0-aa18-4d54-9ae6-d6b0107a5143</t>
+  </si>
+  <si>
+    <t>e667977b-8559-49eb-964c-ea8147517d71</t>
+  </si>
+  <si>
+    <t>4f8737d7-911d-41a1-8349-33247f90fb2c</t>
+  </si>
+  <si>
+    <t>9497e0a1-a4f9-4bce-8c17-aab924c62f08</t>
+  </si>
+  <si>
+    <t>fca586ac-95ae-4c20-a445-4178a2ff124d</t>
+  </si>
+  <si>
+    <t>a5d51571-6884-4e53-8603-f99816b808c2</t>
+  </si>
+  <si>
+    <t>85945493-6d00-4806-8a4a-0e19c11d14c1</t>
+  </si>
+  <si>
+    <t>51eeb4c9-f89c-44aa-a78b-8a85e1c4e0d1</t>
+  </si>
+  <si>
+    <t>1d531b7a-a791-4c50-98e1-d3afaf8edbc9</t>
+  </si>
+  <si>
+    <t>39372525-d66b-4f0d-8224-453c7b6e4956</t>
+  </si>
+  <si>
+    <t>c009beff-bc88-49cb-94ea-1431548b46b8</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: improve data previews / schema dosc
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -66,16 +66,196 @@
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
   </si>
   <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
+  </si>
+  <si>
+    <t>Sheet Missing</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_admin_demographic</t>
+  </si>
+  <si>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_screening</t>
+  </si>
+  <si>
+    <t>eed22197-3cd1-4be8-9814-cc66fecc63c8</t>
+  </si>
+  <si>
+    <t>Missing Column</t>
+  </si>
+  <si>
+    <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
+  </si>
+  <si>
+    <t>6a90386c-77d8-4f29-9f6f-4d11146138cd</t>
+  </si>
+  <si>
+    <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
+  </si>
+  <si>
+    <t>7712dd86-d28f-40a7-99c7-ece902728cee</t>
+  </si>
+  <si>
+    <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
+  </si>
+  <si>
+    <t>03216e2a-d9ec-4871-8b45-c98456896fa6</t>
+  </si>
+  <si>
+    <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
+  </si>
+  <si>
+    <t>a9938492-0961-49f4-9cbd-14bd764aecac</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>314f3bdd-3ce5-4ac9-b7e1-ebd0dd6d4ec9</t>
+  </si>
+  <si>
+    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>699656df-df56-4e75-bf86-0065358fa903</t>
+  </si>
+  <si>
+    <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
+  </si>
+  <si>
+    <t>e1e4603f-e16d-40b0-8906-99d413b95c90</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>3b9866ba-3c33-4579-a12a-79ab2a8e0c67</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>b2c909c7-a858-494a-8d1d-f813a4a2980a</t>
+  </si>
+  <si>
+    <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
+  </si>
+  <si>
+    <t>eca83dd0-20c1-42b7-9d90-425d259bf8d8</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>f1bbcbdb-584a-46ef-b0b6-5726aea93143</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
+  </si>
+  <si>
+    <t>ahc_hrsn_valid_01_q_e_admin_data</t>
+  </si>
+  <si>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+  </si>
+  <si>
+    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+  </si>
+  <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
   </si>
   <si>
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>38749fe7-b3cd-4f6e-97a2-c7f4e3f8fdf2</t>
-  </si>
-  <si>
-    <t>Missing Column</t>
+    <t>35f90d5d-bbdb-4fb2-b98e-14598e595179</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -84,7 +264,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>61d9a7d6-09b4-4fa4-97c7-220513b0962f</t>
+    <t>73fedf25-1977-4d52-88d3-a861f74c7f98</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -93,7 +273,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>72ee7100-3a87-4ffa-aef0-2640c5df8cfa</t>
+    <t>c523c015-6fde-4038-9dbd-6bb6cb6e28ea</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -102,7 +282,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>ad3b3796-a803-481a-a257-b321bbf6d1bb</t>
+    <t>b37e844f-c3fe-404f-b1c7-e5d37d363a50</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -111,7 +291,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>ae8b6413-3631-4443-9d38-f9e073a456ad</t>
+    <t>e6764a80-3d07-4aa0-8e49-16028fb46a47</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -120,7 +300,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>e75ba306-36f4-45af-9a08-0a5e544bc4a0</t>
+    <t>a774712b-68f0-4293-9ca6-a2686330b865</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -129,7 +309,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>60da1c0b-5068-4ac1-a523-891c5609d783</t>
+    <t>26afb567-e70a-4be8-b504-e8c711fdf74c</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -138,7 +318,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>3d5a282e-4e68-4ad2-a5ab-61a4d9f51f36</t>
+    <t>421370d6-32c4-40e0-b05e-c0bd98eaa89e</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -147,7 +327,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>17e73e9c-ed54-4f14-a303-35942c0bf1a4</t>
+    <t>f252a3b9-73a3-4d95-8663-c542a77a90b3</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -156,7 +336,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>112188d1-8d0a-46d8-81d5-a95331127302</t>
+    <t>56d2678b-5a94-40b1-acff-17256ded8442</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -165,7 +345,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>424f0088-d833-465a-9e04-b82b9cef5847</t>
+    <t>e17d719c-75c4-4506-b167-e2774c7e9fdb</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -174,7 +354,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>29552173-a34c-4876-b3d2-68bbe72b9f03</t>
+    <t>aef53175-75a6-4cbf-91a4-483c58645562</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -183,7 +363,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>8632494b-90c5-4ad5-a9f5-610bc116ff9a</t>
+    <t>21167f57-e247-42e2-9a64-595df2badc7d</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -192,7 +372,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>da3d4b96-64f1-4852-9050-3c33c85d73a2</t>
+    <t>b571acf8-2106-4955-80f7-a09503b17683</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -201,7 +381,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>06ef4839-7e61-4c95-90ef-0290f03fd23b</t>
+    <t>26b01308-2b71-43a4-9ecd-c9c056bacda4</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -210,7 +390,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>27aeace6-65a0-4a33-8240-3694f7fa1f28</t>
+    <t>2a63efb4-f527-49c5-88b7-8b42a88d7f75</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -219,7 +399,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>1b504d3f-18d7-482a-82c3-ac0ce2d4cc17</t>
+    <t>763f36a8-5042-4bde-adb1-181768859dc4</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -228,7 +408,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>1a6b4a7e-dd5d-46b7-885b-fa0ccfac5470</t>
+    <t>bf7a295d-77b5-4b2e-ab53-fb9ff938df53</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -237,7 +417,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>82940c83-c0e9-4636-9e7b-9842532da0c0</t>
+    <t>2ece34f1-d614-4217-8086-c3a750312d46</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -246,7 +426,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>6d9ff95f-3179-420b-b1c6-c0c5104e60e6</t>
+    <t>7c68beba-5a46-4b34-98f2-add9f4f74561</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -255,7 +435,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>1bbf963b-1188-4e4d-91af-6fd31bfae417</t>
+    <t>1abbab71-097a-4305-984b-0195703bc1b5</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -264,196 +444,16 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
-  </si>
-  <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
-  </si>
-  <si>
-    <t>Sheet Missing</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
-  </si>
-  <si>
-    <t>47277588-99e8-59f5-8384-b24344a86073</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
-  </si>
-  <si>
-    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_admin_demographic</t>
-  </si>
-  <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
-  </si>
-  <si>
-    <t>TODO</t>
-  </si>
-  <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
-  </si>
-  <si>
-    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_screening</t>
-  </si>
-  <si>
-    <t>117892cf-b527-401f-a916-1cd63b761a3e</t>
-  </si>
-  <si>
-    <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
-  </si>
-  <si>
-    <t>73947d22-66c7-44fa-8b23-35c64dc10a23</t>
-  </si>
-  <si>
-    <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
-  </si>
-  <si>
-    <t>4358499b-2b79-4251-a3b4-6297f7d901fc</t>
-  </si>
-  <si>
-    <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
-  </si>
-  <si>
-    <t>0fb4bf12-5a94-4aa9-9481-0790070c4a7a</t>
-  </si>
-  <si>
-    <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
-  </si>
-  <si>
-    <t>8208bb57-ff1a-4b53-8d71-e7313f90d59b</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>6014344d-23e6-41c3-8931-d3ae02cd786e</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>58b9ecad-c9e9-4358-9fd2-3debb8224e16</t>
-  </si>
-  <si>
-    <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
-  </si>
-  <si>
-    <t>7bd902c7-513c-4514-acaa-bca929857511</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>4ad23d64-7ad5-49a8-bc68-c02073093772</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>20ad9557-2e53-4b45-8f8d-732fce01b81d</t>
-  </si>
-  <si>
-    <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
-  </si>
-  <si>
-    <t>eec2748c-967b-4cd7-bdce-c6249409416d</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>dc8a448d-9e59-44ce-943b-d54d902b9ec5</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
-  </si>
-  <si>
-    <t>ahc_hrsn_valid_01_q_e_admin_data</t>
-  </si>
-  <si>
     <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
   </si>
   <si>
-    <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
-  </si>
-  <si>
-    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
-  </si>
-  <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-12-12-2023-valid.csv</t>
   </si>
   <si>
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>a61ab194-a83f-4bcb-98dd-ad06b667e2bb</t>
+    <t>104ac409-77c5-45e3-b1e3-7b60ca725814</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>5b214c54-2e50-4e01-ae22-f0bb3e58a741</t>
-  </si>
-  <si>
-    <t>1034729c-f84d-486e-94fd-952cbd2fef7e</t>
-  </si>
-  <si>
-    <t>827fbffc-d9e7-403f-84fb-e152692ffd62</t>
-  </si>
-  <si>
-    <t>fdf0de5c-bc22-4b9d-9288-b51064314c88</t>
-  </si>
-  <si>
-    <t>067a5e3f-d138-4735-a96a-b0795c02af1a</t>
-  </si>
-  <si>
-    <t>788f51c2-447a-47b0-bb3c-89dfb0a183d5</t>
-  </si>
-  <si>
-    <t>8a4d4437-dcc9-474e-a21c-1fc98bdb9c39</t>
-  </si>
-  <si>
-    <t>8aa636d7-4e67-43cd-878a-8c670062131f</t>
-  </si>
-  <si>
-    <t>cc24ee55-84c2-410b-ae9b-e57f47975a3c</t>
-  </si>
-  <si>
-    <t>95d5d741-44eb-4c35-ba83-fd3a779823f5</t>
-  </si>
-  <si>
-    <t>01c5a162-4c1a-48a8-9a33-e02f5e5bdb9e</t>
-  </si>
-  <si>
-    <t>9432e199-654b-475c-b37c-6102f4a903e6</t>
-  </si>
-  <si>
-    <t>42b4cc12-b23d-4035-aa70-cb8fd1e023e2</t>
-  </si>
-  <si>
-    <t>ba0f9c27-ecf4-488f-9fbf-c53bc67a93f8</t>
-  </si>
-  <si>
-    <t>22c1e39d-d1e6-4836-a068-559369f60ff7</t>
-  </si>
-  <si>
-    <t>4e530af0-aa18-4d54-9ae6-d6b0107a5143</t>
-  </si>
-  <si>
-    <t>e667977b-8559-49eb-964c-ea8147517d71</t>
-  </si>
-  <si>
-    <t>4f8737d7-911d-41a1-8349-33247f90fb2c</t>
-  </si>
-  <si>
-    <t>9497e0a1-a4f9-4bce-8c17-aab924c62f08</t>
-  </si>
-  <si>
-    <t>fca586ac-95ae-4c20-a445-4178a2ff124d</t>
-  </si>
-  <si>
-    <t>a5d51571-6884-4e53-8603-f99816b808c2</t>
-  </si>
-  <si>
-    <t>85945493-6d00-4806-8a4a-0e19c11d14c1</t>
-  </si>
-  <si>
-    <t>51eeb4c9-f89c-44aa-a78b-8a85e1c4e0d1</t>
-  </si>
-  <si>
-    <t>1d531b7a-a791-4c50-98e1-d3afaf8edbc9</t>
-  </si>
-  <si>
-    <t>39372525-d66b-4f0d-8224-453c7b6e4956</t>
-  </si>
-  <si>
-    <t>c009beff-bc88-49cb-94ea-1431548b46b8</t>
+    <t>f8036943-a46c-4a60-8444-2ffc42e27093</t>
+  </si>
+  <si>
+    <t>70ed8630-3cfc-435a-afdb-a6e82c247ed0</t>
+  </si>
+  <si>
+    <t>cc667c51-7016-423d-a2bd-ba2a9315eff1</t>
+  </si>
+  <si>
+    <t>872b306a-aee4-4394-8f3d-86a57626b83a</t>
+  </si>
+  <si>
+    <t>bef6c55a-c14b-492c-b384-3fc71084289b</t>
+  </si>
+  <si>
+    <t>514804d4-b385-4797-a0cb-04f4b417a8fd</t>
+  </si>
+  <si>
+    <t>e1aa4005-2c9c-4c1d-9871-b2950d438e64</t>
+  </si>
+  <si>
+    <t>4ac00108-677d-41b5-b563-f64a62473717</t>
+  </si>
+  <si>
+    <t>f35211f0-d3ee-467a-a575-7fb4241dcb3c</t>
+  </si>
+  <si>
+    <t>ab9be637-3a6b-4a37-84c2-074b6a6f3bd9</t>
+  </si>
+  <si>
+    <t>e0211115-25ec-40b2-826e-46d569e1cc47</t>
+  </si>
+  <si>
+    <t>ff843123-b7ad-4a02-8266-b6c9626578bb</t>
+  </si>
+  <si>
+    <t>9954fd97-9f6a-4daf-962c-2f7ef2fa4eae</t>
+  </si>
+  <si>
+    <t>88643542-0475-4909-81d0-225f43047331</t>
+  </si>
+  <si>
+    <t>93a34564-0628-40ac-9332-a54c2dbdf302</t>
+  </si>
+  <si>
+    <t>a3d3914f-4486-42e3-93cf-e7aef98abbad</t>
+  </si>
+  <si>
+    <t>2ac8c118-01c0-4c7a-b7cf-0d5fea0f7157</t>
+  </si>
+  <si>
+    <t>6e16f7d8-cfdd-45f0-ba45-890e5d2be188</t>
+  </si>
+  <si>
+    <t>1a950bd0-4ea4-4bf6-ba5e-b9a43130e78f</t>
+  </si>
+  <si>
+    <t>d752d6ee-9b11-44e7-a4c6-ee4d23d54e8d</t>
+  </si>
+  <si>
+    <t>46bf16f3-4f10-454c-bb79-69266493deb8</t>
+  </si>
+  <si>
+    <t>b0854e40-87d1-4875-9a24-9866e3c94b93</t>
+  </si>
+  <si>
+    <t>c484b02e-b787-4ba2-972b-e962ef91941f</t>
+  </si>
+  <si>
+    <t>7f181307-88a5-44ab-b6a1-06f3762340fc</t>
+  </si>
+  <si>
+    <t>ce2274a1-a43e-4c26-af5c-22c7b8344053</t>
+  </si>
+  <si>
+    <t>1d6611b4-6056-4fd1-a1a6-584d829406f6</t>
   </si>
 </sst>
 </file>
@@ -692,8 +692,8 @@
       <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
-        <v>23</v>
+      <c r="M2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
@@ -704,7 +704,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -721,8 +721,8 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="N3" t="s">
-        <v>26</v>
+      <c r="M3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
@@ -733,7 +733,7 @@
         <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
@@ -750,8 +750,8 @@
       <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="N4" t="s">
-        <v>29</v>
+      <c r="M4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
@@ -762,25 +762,25 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
         <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6">
@@ -791,25 +791,25 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="N6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7">
@@ -820,25 +820,25 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="N7" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -849,25 +849,25 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="N8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
@@ -878,25 +878,25 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
@@ -907,25 +907,25 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="N10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
@@ -936,25 +936,25 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="N11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
@@ -965,25 +965,25 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -994,25 +994,25 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -1023,25 +1023,25 @@
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J14" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
@@ -1052,25 +1052,25 @@
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="N15" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -1081,25 +1081,25 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J16" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="N16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -1110,25 +1110,25 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J17" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="N17" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18">
@@ -1139,25 +1139,25 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
-      </c>
-      <c r="N18" t="s">
-        <v>71</v>
+        <v>77</v>
+      </c>
+      <c r="M18" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19">
@@ -1168,25 +1168,25 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="N19" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -1197,25 +1197,25 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J20" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="N20" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21">
@@ -1226,25 +1226,25 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="I21" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J21" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="N21" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22">
@@ -1255,25 +1255,25 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J22" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="N22" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23">
@@ -1284,25 +1284,25 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H23" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I23" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="J23" t="s">
-        <v>89</v>
-      </c>
-      <c r="M23" t="s">
-        <v>85</v>
+        <v>94</v>
+      </c>
+      <c r="N23" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="24">
@@ -1313,25 +1313,25 @@
         <v>16</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="I24" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="J24" t="s">
-        <v>92</v>
-      </c>
-      <c r="M24" t="s">
-        <v>85</v>
+        <v>97</v>
+      </c>
+      <c r="N24" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="25">
@@ -1342,25 +1342,25 @@
         <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="I25" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="J25" t="s">
-        <v>95</v>
-      </c>
-      <c r="M25" t="s">
-        <v>85</v>
+        <v>100</v>
+      </c>
+      <c r="N25" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="26">
@@ -1371,25 +1371,25 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="H26" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I26" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>101</v>
-      </c>
-      <c r="M26" t="s">
-        <v>97</v>
+        <v>103</v>
+      </c>
+      <c r="N26" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -1400,25 +1400,25 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I27" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -1429,25 +1429,25 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I28" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J28" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -1458,25 +1458,25 @@
         <v>16</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H29" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I29" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N29" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30">
@@ -1487,25 +1487,25 @@
         <v>16</v>
       </c>
       <c r="D30" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F30" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I30" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J30" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31">
@@ -1516,25 +1516,25 @@
         <v>16</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F31" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I31" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32">
@@ -1545,25 +1545,25 @@
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E32" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F32" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I32" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33">
@@ -1574,25 +1574,25 @@
         <v>16</v>
       </c>
       <c r="D33" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E33" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F33" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I33" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J33" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34">
@@ -1603,25 +1603,25 @@
         <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E34" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H34" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I34" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J34" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N34" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35">
@@ -1632,25 +1632,25 @@
         <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E35" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I35" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J35" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36">
@@ -1661,25 +1661,25 @@
         <v>16</v>
       </c>
       <c r="D36" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F36" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H36" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I36" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N36" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37">
@@ -1690,25 +1690,25 @@
         <v>16</v>
       </c>
       <c r="D37" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E37" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H37" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I37" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J37" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N37" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38">
@@ -1719,25 +1719,25 @@
         <v>16</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E38" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F38" t="s">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="H38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I38" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="J38" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39">
@@ -1748,25 +1748,25 @@
         <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="E39" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="F39" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" t="s">
         <v>141</v>
       </c>
-      <c r="H39" t="s">
+      <c r="I39" t="s">
+        <v>38</v>
+      </c>
+      <c r="J39" t="s">
         <v>142</v>
       </c>
-      <c r="I39" t="s">
-        <v>100</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="N39" t="s">
         <v>143</v>
-      </c>
-      <c r="M39" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="40">

</xml_diff>

<commit_message>
feat: use new SQLa extensions autoloading
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -123,7 +123,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>eed22197-3cd1-4be8-9814-cc66fecc63c8</t>
+    <t>1c249b90-02ed-42e3-bc80-8bebe0b3f63b</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -135,7 +135,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>6a90386c-77d8-4f29-9f6f-4d11146138cd</t>
+    <t>41d3ee39-c1a6-4232-9e19-3c397bc28e67</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -144,7 +144,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>7712dd86-d28f-40a7-99c7-ece902728cee</t>
+    <t>65619ffc-d9fe-4b65-83d5-ef481cef90d2</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -153,7 +153,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>03216e2a-d9ec-4871-8b45-c98456896fa6</t>
+    <t>c5290207-8a38-422a-828a-ae6f20805f6c</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -162,7 +162,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>a9938492-0961-49f4-9cbd-14bd764aecac</t>
+    <t>740b7b5d-db7c-461f-8980-59e870a14963</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -171,7 +171,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>314f3bdd-3ce5-4ac9-b7e1-ebd0dd6d4ec9</t>
+    <t>130d8033-1979-4035-a8ca-828d9d071b1f</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -180,7 +180,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>699656df-df56-4e75-bf86-0065358fa903</t>
+    <t>42705ffe-03a5-4409-a55a-29eb3faa6365</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -189,7 +189,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>e1e4603f-e16d-40b0-8906-99d413b95c90</t>
+    <t>904da14c-df53-4397-82b2-edd4155d5d7a</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -198,7 +198,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>3b9866ba-3c33-4579-a12a-79ab2a8e0c67</t>
+    <t>d82c4a03-df84-4d87-958c-9b54baddeb2c</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -207,7 +207,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>b2c909c7-a858-494a-8d1d-f813a4a2980a</t>
+    <t>5fb4f10b-717a-4aa7-a937-a554d4e2b6f1</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -216,7 +216,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>eca83dd0-20c1-42b7-9d90-425d259bf8d8</t>
+    <t>7bddee20-67e2-4c3d-9d3b-adc300497d57</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -225,7 +225,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>f1bbcbdb-584a-46ef-b0b6-5726aea93143</t>
+    <t>b300f309-cb97-4c1e-9046-42c65feaed8b</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>35f90d5d-bbdb-4fb2-b98e-14598e595179</t>
+    <t>39ad14b9-3de2-4dea-9075-8182a9f7be7e</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -264,7 +264,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>73fedf25-1977-4d52-88d3-a861f74c7f98</t>
+    <t>b4d9c654-79c0-474e-8077-88549890405c</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -273,7 +273,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>c523c015-6fde-4038-9dbd-6bb6cb6e28ea</t>
+    <t>4b81795d-4e50-4f8b-b9d4-1d879522eef0</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -282,7 +282,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>b37e844f-c3fe-404f-b1c7-e5d37d363a50</t>
+    <t>17063d26-909d-4cf6-9063-d6a1e0dda382</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -291,7 +291,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>e6764a80-3d07-4aa0-8e49-16028fb46a47</t>
+    <t>2531d9ad-1bf1-4987-bedd-04baa40f9246</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -300,7 +300,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>a774712b-68f0-4293-9ca6-a2686330b865</t>
+    <t>51438f74-bab0-40d2-9810-83c888938960</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -309,7 +309,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>26afb567-e70a-4be8-b504-e8c711fdf74c</t>
+    <t>c1be0df4-8755-4667-8766-3aa8f61737a5</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -318,7 +318,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>421370d6-32c4-40e0-b05e-c0bd98eaa89e</t>
+    <t>6b54595c-8fc5-493c-bac5-078956ac90e3</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -327,7 +327,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>f252a3b9-73a3-4d95-8663-c542a77a90b3</t>
+    <t>fa0cc4d3-ea6d-4b2b-b507-48f1c541c42b</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -336,7 +336,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>56d2678b-5a94-40b1-acff-17256ded8442</t>
+    <t>76434d6d-fb85-401c-9383-9a6c18fa2c48</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -345,7 +345,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>e17d719c-75c4-4506-b167-e2774c7e9fdb</t>
+    <t>d2702766-09b6-4fed-8a0c-62be3bf50fef</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -354,7 +354,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>aef53175-75a6-4cbf-91a4-483c58645562</t>
+    <t>0f710509-bb46-4f6b-a48e-4a508a8c3fea</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -363,7 +363,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>21167f57-e247-42e2-9a64-595df2badc7d</t>
+    <t>439bf9e2-d6c0-41ad-a18b-fcd4590aafa9</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -372,7 +372,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>b571acf8-2106-4955-80f7-a09503b17683</t>
+    <t>c9b61112-d008-40bb-8ef0-51a1a60793fc</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -381,7 +381,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>26b01308-2b71-43a4-9ecd-c9c056bacda4</t>
+    <t>0f830419-702b-46ce-902f-f8ce101713a0</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -390,7 +390,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>2a63efb4-f527-49c5-88b7-8b42a88d7f75</t>
+    <t>cfde60f3-6ef4-4fe2-877d-8b34778687a4</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -399,7 +399,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>763f36a8-5042-4bde-adb1-181768859dc4</t>
+    <t>07168f2d-4495-48f0-98c1-01c3e1ebaab0</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -408,7 +408,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>bf7a295d-77b5-4b2e-ab53-fb9ff938df53</t>
+    <t>70c74ded-5d86-468d-a3db-218adaa673c3</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -417,7 +417,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>2ece34f1-d614-4217-8086-c3a750312d46</t>
+    <t>98ee1b1f-4b3d-405a-8cd2-db5df12212bf</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -426,7 +426,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>7c68beba-5a46-4b34-98f2-add9f4f74561</t>
+    <t>576d7063-64a0-42a4-ac5f-83110f349002</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -435,7 +435,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>1abbab71-097a-4305-984b-0195703bc1b5</t>
+    <t>1558afa6-3b96-4263-ba04-9585fba3091b</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -453,7 +453,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>104ac409-77c5-45e3-b1e3-7b60ca725814</t>
+    <t>621f07f6-3879-4616-bf35-ec0593be5d10</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -471,82 +471,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>f8036943-a46c-4a60-8444-2ffc42e27093</t>
-  </si>
-  <si>
-    <t>70ed8630-3cfc-435a-afdb-a6e82c247ed0</t>
-  </si>
-  <si>
-    <t>cc667c51-7016-423d-a2bd-ba2a9315eff1</t>
-  </si>
-  <si>
-    <t>872b306a-aee4-4394-8f3d-86a57626b83a</t>
-  </si>
-  <si>
-    <t>bef6c55a-c14b-492c-b384-3fc71084289b</t>
-  </si>
-  <si>
-    <t>514804d4-b385-4797-a0cb-04f4b417a8fd</t>
-  </si>
-  <si>
-    <t>e1aa4005-2c9c-4c1d-9871-b2950d438e64</t>
-  </si>
-  <si>
-    <t>4ac00108-677d-41b5-b563-f64a62473717</t>
-  </si>
-  <si>
-    <t>f35211f0-d3ee-467a-a575-7fb4241dcb3c</t>
-  </si>
-  <si>
-    <t>ab9be637-3a6b-4a37-84c2-074b6a6f3bd9</t>
-  </si>
-  <si>
-    <t>e0211115-25ec-40b2-826e-46d569e1cc47</t>
-  </si>
-  <si>
-    <t>ff843123-b7ad-4a02-8266-b6c9626578bb</t>
-  </si>
-  <si>
-    <t>9954fd97-9f6a-4daf-962c-2f7ef2fa4eae</t>
-  </si>
-  <si>
-    <t>88643542-0475-4909-81d0-225f43047331</t>
-  </si>
-  <si>
-    <t>93a34564-0628-40ac-9332-a54c2dbdf302</t>
-  </si>
-  <si>
-    <t>a3d3914f-4486-42e3-93cf-e7aef98abbad</t>
-  </si>
-  <si>
-    <t>2ac8c118-01c0-4c7a-b7cf-0d5fea0f7157</t>
-  </si>
-  <si>
-    <t>6e16f7d8-cfdd-45f0-ba45-890e5d2be188</t>
-  </si>
-  <si>
-    <t>1a950bd0-4ea4-4bf6-ba5e-b9a43130e78f</t>
-  </si>
-  <si>
-    <t>d752d6ee-9b11-44e7-a4c6-ee4d23d54e8d</t>
-  </si>
-  <si>
-    <t>46bf16f3-4f10-454c-bb79-69266493deb8</t>
-  </si>
-  <si>
-    <t>b0854e40-87d1-4875-9a24-9866e3c94b93</t>
-  </si>
-  <si>
-    <t>c484b02e-b787-4ba2-972b-e962ef91941f</t>
-  </si>
-  <si>
-    <t>7f181307-88a5-44ab-b6a1-06f3762340fc</t>
-  </si>
-  <si>
-    <t>ce2274a1-a43e-4c26-af5c-22c7b8344053</t>
-  </si>
-  <si>
-    <t>1d6611b4-6056-4fd1-a1a6-584d829406f6</t>
+    <t>bc082cab-267c-4b62-b13b-21446c9cb0c6</t>
+  </si>
+  <si>
+    <t>d77dd9b6-b1a0-4aac-a063-a3da778d82c9</t>
+  </si>
+  <si>
+    <t>c87bd9c4-815e-4878-a0d7-e043e70279ed</t>
+  </si>
+  <si>
+    <t>52ef1e71-a854-41a1-a20f-3ac2796927af</t>
+  </si>
+  <si>
+    <t>04801f92-7dae-47a6-820b-0b1e8524dd26</t>
+  </si>
+  <si>
+    <t>27dfe84b-85cd-4872-b8e6-ef705da3dddc</t>
+  </si>
+  <si>
+    <t>123cbf97-0400-4776-a15d-e181a9830a62</t>
+  </si>
+  <si>
+    <t>e5685493-d5e0-4dec-ae56-721d09fcddaf</t>
+  </si>
+  <si>
+    <t>2620e43a-0b92-46d8-b59e-7c2974a50a17</t>
+  </si>
+  <si>
+    <t>c7f44052-0361-429f-8e45-9023a9278099</t>
+  </si>
+  <si>
+    <t>cc9b2c17-185a-48a7-a7c7-0a432ae8e014</t>
+  </si>
+  <si>
+    <t>ac74606d-0e85-4b55-853e-50bca27c880e</t>
+  </si>
+  <si>
+    <t>83a12958-d579-4d25-8ed2-f8b1fa94b51c</t>
+  </si>
+  <si>
+    <t>d6a90ca6-379d-4844-984a-f84a0a631155</t>
+  </si>
+  <si>
+    <t>97e20099-328f-499a-a988-25d98e06f3f0</t>
+  </si>
+  <si>
+    <t>0cab18ab-0987-456e-a6a8-7346eaa87760</t>
+  </si>
+  <si>
+    <t>727e7674-fc47-44bc-9973-a68bf55d9cc8</t>
+  </si>
+  <si>
+    <t>854d1ffb-566a-4614-b9f8-f29306fce2fc</t>
+  </si>
+  <si>
+    <t>ed5eb2cb-ea5e-48dc-af61-f3baa15fa267</t>
+  </si>
+  <si>
+    <t>85173e0b-5c11-4d69-8349-e876776f4ef7</t>
+  </si>
+  <si>
+    <t>c01e2c32-e028-46d1-a0e7-7f520819fa60</t>
+  </si>
+  <si>
+    <t>6059ded4-437d-4a44-aa93-40d808e2f127</t>
+  </si>
+  <si>
+    <t>d8d44904-32b9-40d5-95d4-b05349628e30</t>
+  </si>
+  <si>
+    <t>558640af-39e9-48e3-87cf-907a383dfa0b</t>
+  </si>
+  <si>
+    <t>8fe53d94-1e80-42ae-8593-28b012c54a3e</t>
+  </si>
+  <si>
+    <t>51c7349b-81cf-4b9a-be85-9f1fbe2203a2</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
chore: format generated SQL
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -135,7 +135,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>f5e7c858-1724-4776-9e05-0703afa5b1b7</t>
+    <t>95b8b0b0-a12d-48c7-ac7d-b79791c1de3c</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -147,7 +147,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>20fa3903-4e4c-453c-a5af-f951ed63e446</t>
+    <t>2635d729-6559-464a-b0d6-7325018ffe36</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -156,7 +156,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>22c886fc-582d-4aca-90a9-3c4452477c9c</t>
+    <t>b9069bd0-8299-4b62-ab81-e287d88133be</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -165,7 +165,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>58f4c605-0155-4e88-9877-41b28d0cd3f9</t>
+    <t>ffd88615-fc9c-402f-8479-67df9fcff002</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -174,7 +174,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>49008b05-96c5-4d77-853c-985dfdc931bb</t>
+    <t>23166d7b-d6b5-4bf5-906e-c0350d65bcf1</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -183,7 +183,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>35da1f4b-46b0-4fe6-9f17-2afddca0614b</t>
+    <t>6f584c45-31fb-419e-9173-33dee34cffa9</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -192,7 +192,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>d02049a3-b3fb-4051-9bdc-ce53c7bc652f</t>
+    <t>6d58188e-2b9a-42db-b593-b578e796f775</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -201,7 +201,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>99d180dc-5253-4ecd-bf67-f5bc7139c065</t>
+    <t>ef252f02-7ff7-4fd4-9c14-f9e2508c6ffa</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -210,7 +210,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>067ce2a1-f0fa-4fcd-9fa9-91a7d3c30e22</t>
+    <t>cfeeb1dd-de6e-423c-9f9d-ce724e1979dd</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -219,7 +219,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>a517b1ab-65c8-4136-91b6-9f883fee3252</t>
+    <t>499b7f18-15d5-405a-9a99-830fcf1a67e7</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -228,7 +228,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>d1757744-1978-4843-8cba-786cb94b475d</t>
+    <t>57858b87-1b4d-4bec-870b-7bfe9bcbf4c6</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -237,7 +237,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>7740f706-7bba-4c00-80ed-85ddb717da70</t>
+    <t>fda5965b-8733-4cd7-8f38-46707a87000e</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -267,7 +267,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>c54a6bbf-ab56-4ca1-a8d8-c2059f603bf7</t>
+    <t>bbf9588f-c3b5-490f-8e1d-0b4d585a350a</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>b5571b11-e6e9-47ea-b0ae-b090a93bd9fc</t>
+    <t>3645688c-9317-4f40-b626-c4f2f55b9b2b</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>cc445e11-0b3e-4fdf-84a1-5f2d57d35f6b</t>
+    <t>7b6fcfa1-dab6-4c98-b71a-e2dcea765514</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>9e8b6232-c4de-43a4-a425-6900077b2b3d</t>
+    <t>9686114b-e3f3-4f48-a423-5fb7cfd98da6</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>e8da9fe9-6aa4-4111-ae3a-f6ae58bbb801</t>
+    <t>b11d057d-511d-4e08-b2a0-7956484b2bb4</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>7e43b5c0-4d17-4c98-a363-1ff2cfcc652e</t>
+    <t>b72d9b61-880e-48f9-b52a-3e2e80071be7</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>8f4b2d56-dea3-451f-8be0-b65f4f9c1792</t>
+    <t>23b92792-6856-4dd6-8f36-26291e6f7c3b</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>44e578e1-d222-4d0d-8ae5-a8afc1625985</t>
+    <t>0f74e96e-82c9-4553-b393-f514c76dcb21</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>54119e6a-a2f6-476c-b74c-7a7711eefa24</t>
+    <t>962da885-0a5f-40d9-bd3c-9787ed79257f</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>45aff83d-6869-42f4-a4c8-3823873df181</t>
+    <t>7647913f-db03-4601-af23-12d6bb2410dc</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>7edce13a-1249-444b-ae9b-329820606994</t>
+    <t>bb824194-3bd3-45d0-bd6b-673b34cf993b</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>658bc6a5-eb16-4470-ba8c-6cdab74b52ad</t>
+    <t>2599baf6-9da4-4128-8a54-934e6cadee6e</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>91c88db6-8424-4152-a3ff-e06ce481cfc0</t>
+    <t>05ae4641-e06a-4d39-9ebd-0935ad2e061b</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>b1b42cfd-7019-4358-931a-aff57164817d</t>
+    <t>9bc6e87f-e77f-4750-a7c9-b1b320902717</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>7b79132e-eccf-43c0-907c-7afa576c5ccc</t>
+    <t>4cf83cfc-cca5-4f4f-8c6e-f0e901ec1e67</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>a48822bb-e7b5-4162-8d62-0622f6eca25d</t>
+    <t>e773ff1a-56fe-4d8f-99e4-cfd83382a9e6</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>9e72fda2-1b28-4e0b-8090-1362c2c1e7b7</t>
+    <t>04a1b1b9-2e96-47c3-9ca4-f53d9194c2d1</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>57aa5b0d-37c9-46e2-a99f-33914c38e2da</t>
+    <t>5c2ca29d-4b10-47c0-8212-3150a077625a</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>0f895dd6-c10d-4dd2-b206-e55299ec1adf</t>
+    <t>dc5f13d6-c58f-440c-8b16-5187f61f1dbc</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>0d5141d3-15cb-43de-b7f0-edd06f4cf5f2</t>
+    <t>846e6fd6-9a03-4e19-8866-bcc60e15178a</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -447,7 +447,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>e8849f0c-9fe3-4cee-9416-26283075cc86</t>
+    <t>54f0d4e0-2a53-49c0-9871-ac29f241f5ff</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -465,7 +465,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>98f1eea4-eae8-4811-a66f-12323898e39e</t>
+    <t>66a4e63a-4cd2-47ff-8d31-fd14175a5169</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -483,82 +483,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>f01fd20e-b472-4427-b1a9-25e55684f475</t>
-  </si>
-  <si>
-    <t>267277ef-d745-4369-8d45-eec1a0781fbf</t>
-  </si>
-  <si>
-    <t>08fe024d-99a7-43c0-9eea-ec3b8f78a769</t>
-  </si>
-  <si>
-    <t>9472d8f8-07d2-4042-855a-b534fa580e99</t>
-  </si>
-  <si>
-    <t>decfc1b6-73a1-4511-a03d-ca657bc463c8</t>
-  </si>
-  <si>
-    <t>6dc9fb75-e565-4e72-abdd-f5481e8396fc</t>
-  </si>
-  <si>
-    <t>69b8fe00-781b-459f-a2d7-781335c2dfb9</t>
-  </si>
-  <si>
-    <t>83ba0f86-ecbb-428d-8c5c-f2d4d41f899c</t>
-  </si>
-  <si>
-    <t>fbdc7ce7-5535-46b3-a68d-fe54daa8484a</t>
-  </si>
-  <si>
-    <t>87cfffcd-5237-4439-bf89-f764d28f0f0a</t>
-  </si>
-  <si>
-    <t>c0e0f130-16a7-439b-b69b-ba935f2fe59c</t>
-  </si>
-  <si>
-    <t>118e0dfd-ba53-4966-8e70-ad512ce5b5df</t>
-  </si>
-  <si>
-    <t>78a38f6d-45cd-4017-841d-f0dde258aa1e</t>
-  </si>
-  <si>
-    <t>f590ee48-d78c-414f-b2cd-78f0018e51c1</t>
-  </si>
-  <si>
-    <t>0747bd3f-9170-48e4-ac88-8c542154f4ca</t>
-  </si>
-  <si>
-    <t>921a0fd9-9298-4a07-8034-562c853bfc02</t>
-  </si>
-  <si>
-    <t>9c3d91f2-b2fb-487d-b49c-a17c7fdd76d9</t>
-  </si>
-  <si>
-    <t>865e09da-db74-43f2-b0fd-cb12f4dc0654</t>
-  </si>
-  <si>
-    <t>1825722d-b575-463b-b5e1-f53780a23bf9</t>
-  </si>
-  <si>
-    <t>64797fb1-1839-4058-98de-816da4c8626a</t>
-  </si>
-  <si>
-    <t>d36db3fa-ffd9-42f2-b5b5-c65f4fa9a991</t>
-  </si>
-  <si>
-    <t>9e3b0c7c-87ab-4dc4-a1b9-0c67c3381733</t>
-  </si>
-  <si>
-    <t>1061be62-1ea5-434f-9dcd-21c995420c38</t>
-  </si>
-  <si>
-    <t>d40082e9-e9b5-4275-8a8d-a9ae82b0a8fa</t>
-  </si>
-  <si>
-    <t>a8a27bb7-4bac-477d-bc86-472a18428ab0</t>
-  </si>
-  <si>
-    <t>4778ac70-1139-4dfd-8dac-4872641153a7</t>
+    <t>c580c9af-cce5-4c1e-94aa-54625dd203e3</t>
+  </si>
+  <si>
+    <t>88bec9e8-b860-4b77-a028-80c29e53e247</t>
+  </si>
+  <si>
+    <t>edc93ddc-555f-4661-881e-b1bdbfde4d3a</t>
+  </si>
+  <si>
+    <t>af5f9e17-b5c1-4945-8069-ac7535280835</t>
+  </si>
+  <si>
+    <t>9fbea7ac-4085-4f12-8aae-d5f6212aaf6c</t>
+  </si>
+  <si>
+    <t>8255fed7-726b-4856-b95f-54780f6f26e7</t>
+  </si>
+  <si>
+    <t>6fa663c9-6616-41b2-9cb3-8e04ad299ac7</t>
+  </si>
+  <si>
+    <t>44af2d82-e3e2-4fbf-b43d-65a7b4863bf3</t>
+  </si>
+  <si>
+    <t>ae8b4b12-bc48-4f77-b3ba-bcdf37ed56ed</t>
+  </si>
+  <si>
+    <t>4edd6a35-2dd9-4580-ab45-9e2d7b4c962a</t>
+  </si>
+  <si>
+    <t>777c5e3b-469a-4d0a-baf5-76b83f79c3d4</t>
+  </si>
+  <si>
+    <t>5e5a732a-971e-41fd-9ec2-5ea31c167e7d</t>
+  </si>
+  <si>
+    <t>f180b0a2-8968-4324-899c-81d7805dc46b</t>
+  </si>
+  <si>
+    <t>a0dbf012-0e14-46b4-b284-835c7fde1d83</t>
+  </si>
+  <si>
+    <t>5556aa4f-0093-4423-b16b-ba324c3d003e</t>
+  </si>
+  <si>
+    <t>805e628a-64e0-4a8e-8a86-83ecd5d662cf</t>
+  </si>
+  <si>
+    <t>81338169-7388-4b32-911f-e552e099f102</t>
+  </si>
+  <si>
+    <t>f718546c-5f2a-48b7-a86c-fb7f9aaced33</t>
+  </si>
+  <si>
+    <t>361483ad-3fd1-4c32-8ab0-e6e8a2bb3b1a</t>
+  </si>
+  <si>
+    <t>924d09c8-a080-4da4-b566-4d1884148ec1</t>
+  </si>
+  <si>
+    <t>b859a5ff-f24c-4616-b10b-ee6a97d935d6</t>
+  </si>
+  <si>
+    <t>793aa431-f23c-48be-b929-50e1e2c164b1</t>
+  </si>
+  <si>
+    <t>6db8e041-81f3-4ddc-9b21-de3999a7f22f</t>
+  </si>
+  <si>
+    <t>8f3e0493-cdd9-4d9d-8a80-e85f36908d3b</t>
+  </si>
+  <si>
+    <t>70fc27e8-4c10-4045-858c-b294df3bde81</t>
+  </si>
+  <si>
+    <t>89be468e-3403-4958-a2cf-0284d7287d67</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: improve observability and lineage/state
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -135,7 +135,7 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>95b8b0b0-a12d-48c7-ac7d-b79791c1de3c</t>
+    <t>69f45ebf-bc69-444e-9e59-72e123d1afa4</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -147,7 +147,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>2635d729-6559-464a-b0d6-7325018ffe36</t>
+    <t>dbaf647a-d05a-455c-9ef3-94131b1a2f22</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -156,7 +156,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>b9069bd0-8299-4b62-ab81-e287d88133be</t>
+    <t>fc57ae5a-8d70-4b43-bb4c-0a513397997c</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -165,7 +165,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>ffd88615-fc9c-402f-8479-67df9fcff002</t>
+    <t>7d13ba6b-d02a-4a8c-b65a-83ca38438f05</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -174,7 +174,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>23166d7b-d6b5-4bf5-906e-c0350d65bcf1</t>
+    <t>eed40001-1933-455a-8e39-7e3892ed2ce5</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -183,7 +183,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>6f584c45-31fb-419e-9173-33dee34cffa9</t>
+    <t>9b3b923a-5646-427f-b0a3-18cf52bb974d</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -192,7 +192,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>6d58188e-2b9a-42db-b593-b578e796f775</t>
+    <t>f25dcc11-b4bc-4ae5-90da-17a8cb58c6eb</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -201,7 +201,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>ef252f02-7ff7-4fd4-9c14-f9e2508c6ffa</t>
+    <t>6ae02d52-1294-4e4c-9a4e-d93c28e27e9b</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -210,7 +210,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>cfeeb1dd-de6e-423c-9f9d-ce724e1979dd</t>
+    <t>850d23cc-ae5b-4e96-ad78-ff0d692ed313</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -219,7 +219,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>499b7f18-15d5-405a-9a99-830fcf1a67e7</t>
+    <t>e1165481-4678-48dd-8072-2d5a8d8994a6</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -228,7 +228,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>57858b87-1b4d-4bec-870b-7bfe9bcbf4c6</t>
+    <t>4dc156fa-eada-4fa7-a2f3-5aede98788eb</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -237,7 +237,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>fda5965b-8733-4cd7-8f38-46707a87000e</t>
+    <t>d86cd5a3-fa2d-4804-9fcb-81e349e4b166</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -246,19 +246,19 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
   </si>
   <si>
     <t>ahc_hrsn_valid_01_q_e_admin_data</t>
   </si>
   <si>
-    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
   </si>
   <si>
     <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
   </si>
   <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+    <t>591191c7-f693-5957-8734-ac87151ca981</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
@@ -267,7 +267,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>bbf9588f-c3b5-490f-8e1d-0b4d585a350a</t>
+    <t>ed7b1af2-3c5c-4259-a997-5eaeca20f2d5</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>3645688c-9317-4f40-b626-c4f2f55b9b2b</t>
+    <t>815b48f7-b310-4ff6-aa02-6b8f7c049bb1</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>7b6fcfa1-dab6-4c98-b71a-e2dcea765514</t>
+    <t>53dd6491-04c6-45f1-abf7-55cb5180a256</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>9686114b-e3f3-4f48-a423-5fb7cfd98da6</t>
+    <t>5846bdfe-fb03-4f05-87e7-641a2b943ff7</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>b11d057d-511d-4e08-b2a0-7956484b2bb4</t>
+    <t>54d572f5-f901-4688-8a27-c4f3db636f11</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>b72d9b61-880e-48f9-b52a-3e2e80071be7</t>
+    <t>9ad84ef6-184a-437f-8472-31563a623011</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>23b92792-6856-4dd6-8f36-26291e6f7c3b</t>
+    <t>494294b4-1d59-4221-9fa6-0ba460a71409</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>0f74e96e-82c9-4553-b393-f514c76dcb21</t>
+    <t>5225b69e-1ecc-4362-bd59-fa2bcc642317</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>962da885-0a5f-40d9-bd3c-9787ed79257f</t>
+    <t>a5ede658-f75d-4d73-9297-962e1f4b7d72</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>7647913f-db03-4601-af23-12d6bb2410dc</t>
+    <t>5e59c68e-51d4-4a57-bbca-ff8ec3ebe05f</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>bb824194-3bd3-45d0-bd6b-673b34cf993b</t>
+    <t>90ea63e8-a640-4b01-b573-e2924fc5f0ad</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>2599baf6-9da4-4128-8a54-934e6cadee6e</t>
+    <t>e8d424f3-5833-4603-819d-23cc9039c289</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>05ae4641-e06a-4d39-9ebd-0935ad2e061b</t>
+    <t>76865ebd-8524-4549-b034-3cbe130beb18</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>9bc6e87f-e77f-4750-a7c9-b1b320902717</t>
+    <t>f14ca97a-4bf1-46d4-8ca2-2eadf9e16556</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>4cf83cfc-cca5-4f4f-8c6e-f0e901ec1e67</t>
+    <t>07eedb66-f428-4be7-a42c-ae48c4c28c20</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>e773ff1a-56fe-4d8f-99e4-cfd83382a9e6</t>
+    <t>0dd7f6a8-0e76-4008-a21e-4a0a5de0ebc3</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>04a1b1b9-2e96-47c3-9ca4-f53d9194c2d1</t>
+    <t>6a9f8a4c-e08b-447d-9f3d-8d2ddd34979f</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>5c2ca29d-4b10-47c0-8212-3150a077625a</t>
+    <t>868b5676-29a9-48d8-ba3a-feed82e9caac</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>dc5f13d6-c58f-440c-8b16-5187f61f1dbc</t>
+    <t>59f3777c-bb08-442c-816b-9727ccfda685</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>846e6fd6-9a03-4e19-8866-bcc60e15178a</t>
+    <t>011c4358-b74a-42d7-b4ad-586c1217a7a3</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -447,7 +447,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>54f0d4e0-2a53-49c0-9871-ac29f241f5ff</t>
+    <t>1a8c1aad-0a8f-4bf0-9306-592948d513dd</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -456,7 +456,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+    <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-12-12-2023-valid.csv</t>
@@ -465,7 +465,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>66a4e63a-4cd2-47ff-8d31-fd14175a5169</t>
+    <t>fdee0ae4-6ff7-442e-b183-03041be75e7e</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -483,82 +483,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>c580c9af-cce5-4c1e-94aa-54625dd203e3</t>
-  </si>
-  <si>
-    <t>88bec9e8-b860-4b77-a028-80c29e53e247</t>
-  </si>
-  <si>
-    <t>edc93ddc-555f-4661-881e-b1bdbfde4d3a</t>
-  </si>
-  <si>
-    <t>af5f9e17-b5c1-4945-8069-ac7535280835</t>
-  </si>
-  <si>
-    <t>9fbea7ac-4085-4f12-8aae-d5f6212aaf6c</t>
-  </si>
-  <si>
-    <t>8255fed7-726b-4856-b95f-54780f6f26e7</t>
-  </si>
-  <si>
-    <t>6fa663c9-6616-41b2-9cb3-8e04ad299ac7</t>
-  </si>
-  <si>
-    <t>44af2d82-e3e2-4fbf-b43d-65a7b4863bf3</t>
-  </si>
-  <si>
-    <t>ae8b4b12-bc48-4f77-b3ba-bcdf37ed56ed</t>
-  </si>
-  <si>
-    <t>4edd6a35-2dd9-4580-ab45-9e2d7b4c962a</t>
-  </si>
-  <si>
-    <t>777c5e3b-469a-4d0a-baf5-76b83f79c3d4</t>
-  </si>
-  <si>
-    <t>5e5a732a-971e-41fd-9ec2-5ea31c167e7d</t>
-  </si>
-  <si>
-    <t>f180b0a2-8968-4324-899c-81d7805dc46b</t>
-  </si>
-  <si>
-    <t>a0dbf012-0e14-46b4-b284-835c7fde1d83</t>
-  </si>
-  <si>
-    <t>5556aa4f-0093-4423-b16b-ba324c3d003e</t>
-  </si>
-  <si>
-    <t>805e628a-64e0-4a8e-8a86-83ecd5d662cf</t>
-  </si>
-  <si>
-    <t>81338169-7388-4b32-911f-e552e099f102</t>
-  </si>
-  <si>
-    <t>f718546c-5f2a-48b7-a86c-fb7f9aaced33</t>
-  </si>
-  <si>
-    <t>361483ad-3fd1-4c32-8ab0-e6e8a2bb3b1a</t>
-  </si>
-  <si>
-    <t>924d09c8-a080-4da4-b566-4d1884148ec1</t>
-  </si>
-  <si>
-    <t>b859a5ff-f24c-4616-b10b-ee6a97d935d6</t>
-  </si>
-  <si>
-    <t>793aa431-f23c-48be-b929-50e1e2c164b1</t>
-  </si>
-  <si>
-    <t>6db8e041-81f3-4ddc-9b21-de3999a7f22f</t>
-  </si>
-  <si>
-    <t>8f3e0493-cdd9-4d9d-8a80-e85f36908d3b</t>
-  </si>
-  <si>
-    <t>70fc27e8-4c10-4045-858c-b294df3bde81</t>
-  </si>
-  <si>
-    <t>89be468e-3403-4958-a2cf-0284d7287d67</t>
+    <t>8f431b0e-0d9e-42ca-97ca-7b61d8824d20</t>
+  </si>
+  <si>
+    <t>2e79a982-fcdb-48c1-8752-ceee1aa77256</t>
+  </si>
+  <si>
+    <t>a9c9e4e4-7828-41bc-8fc2-d7bb69ccf364</t>
+  </si>
+  <si>
+    <t>2e33b845-3409-4bbf-9726-ee86617aa123</t>
+  </si>
+  <si>
+    <t>7f952548-16c3-43c2-a1e5-e24275633ca4</t>
+  </si>
+  <si>
+    <t>5f0237e5-b3c7-4951-842b-29f2ac710378</t>
+  </si>
+  <si>
+    <t>e858541e-93ec-4ab1-bb80-870030c8de10</t>
+  </si>
+  <si>
+    <t>e3e5a9eb-4f9a-41d9-8384-94781be61ce8</t>
+  </si>
+  <si>
+    <t>f9b91d43-617f-4bd6-908e-e25fbc4a09ca</t>
+  </si>
+  <si>
+    <t>48bfdaba-4762-477f-a736-b6048f4d54c1</t>
+  </si>
+  <si>
+    <t>489580e5-e745-46fb-a8e9-1066b955698f</t>
+  </si>
+  <si>
+    <t>13d70913-2ce9-4720-bb74-8e3e92266312</t>
+  </si>
+  <si>
+    <t>fdf7d612-4cfb-44c4-a1bc-05706f66d404</t>
+  </si>
+  <si>
+    <t>dd03acfd-5c0e-4411-be5c-92b4d78c5ec4</t>
+  </si>
+  <si>
+    <t>1f629815-2287-49ab-932b-077a154b1f97</t>
+  </si>
+  <si>
+    <t>4b5ede2d-7972-4025-b264-68ca35520a9d</t>
+  </si>
+  <si>
+    <t>c9bba00c-0c5a-4be2-b6ae-2a2a94c7578b</t>
+  </si>
+  <si>
+    <t>864968c5-c0f1-4a0c-9671-c0bb49a84693</t>
+  </si>
+  <si>
+    <t>a5a593ff-757e-48db-a620-1951939f9e70</t>
+  </si>
+  <si>
+    <t>3e5aeeef-7245-4a01-863b-b91e1341fc49</t>
+  </si>
+  <si>
+    <t>04afe5bb-edee-4c11-a2e0-daf54d508d28</t>
+  </si>
+  <si>
+    <t>da8a2660-535d-4430-b696-95f668ade476</t>
+  </si>
+  <si>
+    <t>aaacb190-7de5-4069-b422-6a3184f9e631</t>
+  </si>
+  <si>
+    <t>50d9b2ac-e7cd-4047-97f5-6c05d9bccd03</t>
+  </si>
+  <si>
+    <t>afc2bc99-bc4f-450e-800c-ccfe303e27dd</t>
+  </si>
+  <si>
+    <t>baacb865-a98a-4216-bfa0-8909c50afe23</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
test: add synthetic file from Jericho Road HC
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="193">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -78,40 +78,70 @@
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
   </si>
   <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
+  </si>
+  <si>
+    <t>Sheet Missing</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
   </si>
   <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>7b979b68-7227-53fd-b689-e4fe153afb76</t>
-  </si>
-  <si>
-    <t>Sheet Missing</t>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>abf5c680-a135-5d89-b871-fa5b9b99aed6</t>
-  </si>
-  <si>
-    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
-  </si>
-  <si>
-    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
   </si>
   <si>
     <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-valid-01.xlsx</t>
@@ -120,7 +150,7 @@
     <t>ahc_hrsn_valid_01_admin_demographic</t>
   </si>
   <si>
-    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
+    <t>591191c7-f693-5957-8734-ac87151ca981</t>
   </si>
   <si>
     <t>TODO</t>
@@ -129,13 +159,13 @@
     <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'Admin_Demographic' has not been implemented yet.</t>
   </si>
   <si>
-    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+    <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
   </si>
   <si>
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>69f45ebf-bc69-444e-9e59-72e123d1afa4</t>
+    <t>e8072bf2-b35a-43f7-acb0-e432ee838454</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -147,7 +177,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>dbaf647a-d05a-455c-9ef3-94131b1a2f22</t>
+    <t>4fb54c11-1a30-497c-b7f2-3eb781fdedc9</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -156,7 +186,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>fc57ae5a-8d70-4b43-bb4c-0a513397997c</t>
+    <t>75468089-d654-449b-8f54-1fed131c7f8e</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -165,7 +195,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>7d13ba6b-d02a-4a8c-b65a-83ca38438f05</t>
+    <t>93a3ef2f-7c03-4d54-9963-ffe23b558aff</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -174,7 +204,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>eed40001-1933-455a-8e39-7e3892ed2ce5</t>
+    <t>4c02d136-85f0-4aa3-a0f8-a8eaa36ecbbf</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
@@ -183,7 +213,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>9b3b923a-5646-427f-b0a3-18cf52bb974d</t>
+    <t>39cefa29-8080-4bcd-aedf-b3126d48e525</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -192,7 +222,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>f25dcc11-b4bc-4ae5-90da-17a8cb58c6eb</t>
+    <t>36f9f665-5cae-45ab-942a-866d651b982d</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -201,7 +231,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>6ae02d52-1294-4e4c-9a4e-d93c28e27e9b</t>
+    <t>ee5b41c4-17bb-4895-a53e-5de19f2bb425</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
@@ -210,7 +240,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>850d23cc-ae5b-4e96-ad78-ff0d692ed313</t>
+    <t>a906d5d1-1895-4062-8575-6b0315792fd3</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
@@ -219,7 +249,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>e1165481-4678-48dd-8072-2d5a8d8994a6</t>
+    <t>fb6a39c9-90fd-43f3-aedb-26b31d0c87a5</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -228,7 +258,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>4dc156fa-eada-4fa7-a2f3-5aede98788eb</t>
+    <t>3c51ef73-6c00-48fa-aaa8-ec2abed99acb</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -237,7 +267,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>d86cd5a3-fa2d-4804-9fcb-81e349e4b166</t>
+    <t>3a2d069f-04d3-4954-9b54-4142bcd0f467</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -246,19 +276,19 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+    <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
   </si>
   <si>
     <t>ahc_hrsn_valid_01_q_e_admin_data</t>
   </si>
   <si>
-    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+    <t>a3fe7098-8ae8-5612-81ac-cbe10780c19b</t>
   </si>
   <si>
     <t>Excel workbook 'ahc-hrsn-valid-01.xlsx' sheet 'QE_Admin_Data' has not been implemented yet.</t>
   </si>
   <si>
-    <t>591191c7-f693-5957-8734-ac87151ca981</t>
+    <t>99e72a60-96ab-5ef1-a3af-3e7759777664</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
@@ -267,7 +297,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>ed7b1af2-3c5c-4259-a997-5eaeca20f2d5</t>
+    <t>478df3f3-5634-4055-b749-a8194910501e</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -276,7 +306,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>815b48f7-b310-4ff6-aa02-6b8f7c049bb1</t>
+    <t>4c048f3b-2cee-4c9c-8244-45cb68b34de8</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -285,7 +315,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>53dd6491-04c6-45f1-abf7-55cb5180a256</t>
+    <t>6f223a56-4770-4967-a77b-ee913cc4e381</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -294,7 +324,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>5846bdfe-fb03-4f05-87e7-641a2b943ff7</t>
+    <t>3549d51c-7ed6-4efc-83a3-295b6b89a39a</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +333,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>54d572f5-f901-4688-8a27-c4f3db636f11</t>
+    <t>14fba79f-4bf3-40db-99ad-de7d3ff7c376</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -312,7 +342,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>9ad84ef6-184a-437f-8472-31563a623011</t>
+    <t>1a5e19a3-7824-4a10-b89d-a611da7f8fd0</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -321,7 +351,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>494294b4-1d59-4221-9fa6-0ba460a71409</t>
+    <t>4cb48244-cffe-4364-825e-270d560bd038</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -330,7 +360,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>5225b69e-1ecc-4362-bd59-fa2bcc642317</t>
+    <t>f2028828-18f4-4e93-b98e-bd1034c1e902</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -339,7 +369,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>a5ede658-f75d-4d73-9297-962e1f4b7d72</t>
+    <t>0990a6f3-9fdf-4c40-bc6a-595af64f8ce5</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -348,7 +378,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>5e59c68e-51d4-4a57-bbca-ff8ec3ebe05f</t>
+    <t>96bd7521-da8f-4bbf-a6d9-9952dceaff28</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -357,7 +387,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>90ea63e8-a640-4b01-b573-e2924fc5f0ad</t>
+    <t>d0e1e6d2-537a-4f30-8d50-efb9e5505259</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -366,7 +396,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>e8d424f3-5833-4603-819d-23cc9039c289</t>
+    <t>b46bab6a-1095-4edd-847f-1c27a60e5377</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -375,7 +405,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>76865ebd-8524-4549-b034-3cbe130beb18</t>
+    <t>955e5510-b7e9-4b46-a5e8-8c417bde1eaa</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -384,7 +414,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>f14ca97a-4bf1-46d4-8ca2-2eadf9e16556</t>
+    <t>6c72b864-b0ae-4f72-884c-341d0df2d6ae</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -393,7 +423,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>07eedb66-f428-4be7-a42c-ae48c4c28c20</t>
+    <t>fe18eecb-5a58-444e-9a6d-09537b5d49e7</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -402,7 +432,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>0dd7f6a8-0e76-4008-a21e-4a0a5de0ebc3</t>
+    <t>48adf76c-bf15-4d76-9250-e24ffe07c3e4</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -411,7 +441,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>6a9f8a4c-e08b-447d-9f3d-8d2ddd34979f</t>
+    <t>bfdc6088-c3a4-4917-8282-3212efefb5cd</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -420,7 +450,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>868b5676-29a9-48d8-ba3a-feed82e9caac</t>
+    <t>fce070ce-037c-46d6-9f9c-6885b791531b</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -429,7 +459,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>59f3777c-bb08-442c-816b-9727ccfda685</t>
+    <t>295a3da8-31e8-414a-b192-d52b506060a1</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +468,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>011c4358-b74a-42d7-b4ad-586c1217a7a3</t>
+    <t>b63679a7-5188-46c3-9b59-f7e586b88ff4</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -447,7 +477,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>1a8c1aad-0a8f-4bf0-9306-592948d513dd</t>
+    <t>84c22787-93a6-4b5c-a9a7-f63211d99868</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -456,7 +486,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
+    <t>c60cf3db-b1bf-5103-b278-b0c128ce924a</t>
   </si>
   <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-12-12-2023-valid.csv</t>
@@ -465,7 +495,7 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>fdee0ae4-6ff7-442e-b183-03041be75e7e</t>
+    <t>bdbe5b5a-e186-4b87-8918-796e1b5146d1</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -483,82 +513,82 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>8f431b0e-0d9e-42ca-97ca-7b61d8824d20</t>
-  </si>
-  <si>
-    <t>2e79a982-fcdb-48c1-8752-ceee1aa77256</t>
-  </si>
-  <si>
-    <t>a9c9e4e4-7828-41bc-8fc2-d7bb69ccf364</t>
-  </si>
-  <si>
-    <t>2e33b845-3409-4bbf-9726-ee86617aa123</t>
-  </si>
-  <si>
-    <t>7f952548-16c3-43c2-a1e5-e24275633ca4</t>
-  </si>
-  <si>
-    <t>5f0237e5-b3c7-4951-842b-29f2ac710378</t>
-  </si>
-  <si>
-    <t>e858541e-93ec-4ab1-bb80-870030c8de10</t>
-  </si>
-  <si>
-    <t>e3e5a9eb-4f9a-41d9-8384-94781be61ce8</t>
-  </si>
-  <si>
-    <t>f9b91d43-617f-4bd6-908e-e25fbc4a09ca</t>
-  </si>
-  <si>
-    <t>48bfdaba-4762-477f-a736-b6048f4d54c1</t>
-  </si>
-  <si>
-    <t>489580e5-e745-46fb-a8e9-1066b955698f</t>
-  </si>
-  <si>
-    <t>13d70913-2ce9-4720-bb74-8e3e92266312</t>
-  </si>
-  <si>
-    <t>fdf7d612-4cfb-44c4-a1bc-05706f66d404</t>
-  </si>
-  <si>
-    <t>dd03acfd-5c0e-4411-be5c-92b4d78c5ec4</t>
-  </si>
-  <si>
-    <t>1f629815-2287-49ab-932b-077a154b1f97</t>
-  </si>
-  <si>
-    <t>4b5ede2d-7972-4025-b264-68ca35520a9d</t>
-  </si>
-  <si>
-    <t>c9bba00c-0c5a-4be2-b6ae-2a2a94c7578b</t>
-  </si>
-  <si>
-    <t>864968c5-c0f1-4a0c-9671-c0bb49a84693</t>
-  </si>
-  <si>
-    <t>a5a593ff-757e-48db-a620-1951939f9e70</t>
-  </si>
-  <si>
-    <t>3e5aeeef-7245-4a01-863b-b91e1341fc49</t>
-  </si>
-  <si>
-    <t>04afe5bb-edee-4c11-a2e0-daf54d508d28</t>
-  </si>
-  <si>
-    <t>da8a2660-535d-4430-b696-95f668ade476</t>
-  </si>
-  <si>
-    <t>aaacb190-7de5-4069-b422-6a3184f9e631</t>
-  </si>
-  <si>
-    <t>50d9b2ac-e7cd-4047-97f5-6c05d9bccd03</t>
-  </si>
-  <si>
-    <t>afc2bc99-bc4f-450e-800c-ccfe303e27dd</t>
-  </si>
-  <si>
-    <t>baacb865-a98a-4216-bfa0-8909c50afe23</t>
+    <t>b36b3553-e7ac-4e16-9c0a-6f07a88a5373</t>
+  </si>
+  <si>
+    <t>3db2979f-913f-451e-a36e-c534abdeb4e0</t>
+  </si>
+  <si>
+    <t>1e91bc80-a5a9-48a2-82a4-27ea6d0158dd</t>
+  </si>
+  <si>
+    <t>b62c0483-6814-4abd-a54c-f5dd6444f171</t>
+  </si>
+  <si>
+    <t>d174ce5a-9baa-42d3-8f3e-8a23406b0662</t>
+  </si>
+  <si>
+    <t>0a4fbf7a-0e9d-4aa9-9339-eb5c6edaec39</t>
+  </si>
+  <si>
+    <t>33187aac-eeda-4649-8cb5-d177e002a244</t>
+  </si>
+  <si>
+    <t>ba704267-8f26-4568-88d7-20de7115419c</t>
+  </si>
+  <si>
+    <t>62dbc77b-b212-4555-b7ad-9a7ac4a9ebf9</t>
+  </si>
+  <si>
+    <t>33e9a0c1-3a63-4faf-99dd-8eada6bd463b</t>
+  </si>
+  <si>
+    <t>98ae6f47-0d61-44cb-ab2a-a0f8733d7149</t>
+  </si>
+  <si>
+    <t>b6e47942-9086-456b-8105-9a03c5374278</t>
+  </si>
+  <si>
+    <t>6587a497-e5da-45ab-86dc-44db98f3e460</t>
+  </si>
+  <si>
+    <t>695c3bfa-c1b9-455f-bf96-8b1d5d7524fd</t>
+  </si>
+  <si>
+    <t>0e2df081-9bac-4637-8808-05cf4da5b1c7</t>
+  </si>
+  <si>
+    <t>d11bc45e-14f6-4ec9-8e75-b957f76f5d85</t>
+  </si>
+  <si>
+    <t>2a40b763-bbe9-4c73-a242-ac1273918eb2</t>
+  </si>
+  <si>
+    <t>70262c9a-f47c-4409-b39c-e958b7f808fe</t>
+  </si>
+  <si>
+    <t>ae08bf13-7445-4ff8-a512-9393b05d0c15</t>
+  </si>
+  <si>
+    <t>4a09c8b7-d6a8-42a4-b7a6-41be06cc86f6</t>
+  </si>
+  <si>
+    <t>01465847-d973-4323-b2ed-87ecd6f6c3fa</t>
+  </si>
+  <si>
+    <t>1543e2ab-1380-4abe-9304-745303c6d216</t>
+  </si>
+  <si>
+    <t>4417d626-2f03-4f45-b6e4-ac139c7c25db</t>
+  </si>
+  <si>
+    <t>d3bae684-8b35-401a-a243-7252ddb95bd3</t>
+  </si>
+  <si>
+    <t>e5f3e2f8-23ce-4402-b210-cc21bf2023d2</t>
+  </si>
+  <si>
+    <t>294b1a56-4d03-4927-8928-31ff5b651103</t>
   </si>
 </sst>
 </file>
@@ -804,16 +834,16 @@
         <v>34</v>
       </c>
       <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
         <v>35</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" t="s">
         <v>36</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" t="s">
-        <v>38</v>
       </c>
       <c r="P5" t="s">
         <v>34</v>
@@ -830,25 +860,25 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -862,25 +892,25 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
         <v>42</v>
       </c>
-      <c r="M7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>47</v>
+      <c r="P7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -894,25 +924,25 @@
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="K8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" t="s">
         <v>48</v>
       </c>
-      <c r="L8" t="s">
-        <v>42</v>
-      </c>
-      <c r="M8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>50</v>
+      <c r="P8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9">
@@ -926,25 +956,25 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K9" t="s">
         <v>51</v>
       </c>
       <c r="L9" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10">
@@ -958,25 +988,25 @@
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L10" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11">
@@ -990,25 +1020,25 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -1022,25 +1052,25 @@
         <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I12" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L12" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -1054,25 +1084,25 @@
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -1086,25 +1116,25 @@
         <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I14" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
@@ -1118,25 +1148,25 @@
         <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K15" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L15" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -1150,25 +1180,25 @@
         <v>20</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I16" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L16" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Q16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -1182,25 +1212,25 @@
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I17" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L17" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18">
@@ -1214,25 +1244,25 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" t="s">
         <v>79</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" t="s">
         <v>80</v>
       </c>
-      <c r="L18" t="s">
-        <v>37</v>
-      </c>
-      <c r="M18" t="s">
+      <c r="Q18" t="s">
         <v>81</v>
-      </c>
-      <c r="P18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -1246,25 +1276,25 @@
         <v>20</v>
       </c>
       <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" t="s">
         <v>82</v>
       </c>
-      <c r="H19" t="s">
+      <c r="L19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" t="s">
         <v>83</v>
       </c>
-      <c r="I19" t="s">
+      <c r="Q19" t="s">
         <v>84</v>
-      </c>
-      <c r="K19" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" t="s">
-        <v>42</v>
-      </c>
-      <c r="M19" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20">
@@ -1278,25 +1308,25 @@
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="I20" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="K20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L20" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="Q20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
@@ -1310,25 +1340,25 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="K21" t="s">
+        <v>90</v>
+      </c>
+      <c r="L21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" t="s">
         <v>91</v>
       </c>
-      <c r="L21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M21" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>93</v>
+      <c r="P21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22">
@@ -1342,25 +1372,25 @@
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L22" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -1374,25 +1404,25 @@
         <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I23" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K23" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L23" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -1406,25 +1436,25 @@
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I24" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L24" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25">
@@ -1438,25 +1468,25 @@
         <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I25" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="L25" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26">
@@ -1470,25 +1500,25 @@
         <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I26" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L26" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M26" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27">
@@ -1502,25 +1532,25 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I27" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L27" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28">
@@ -1534,25 +1564,25 @@
         <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I28" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L28" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M28" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29">
@@ -1566,25 +1596,25 @@
         <v>20</v>
       </c>
       <c r="G29" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I29" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="L29" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M29" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Q29" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
@@ -1598,25 +1628,25 @@
         <v>20</v>
       </c>
       <c r="G30" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H30" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I30" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L30" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M30" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
@@ -1630,25 +1660,25 @@
         <v>20</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I31" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L31" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32">
@@ -1662,25 +1692,25 @@
         <v>20</v>
       </c>
       <c r="G32" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H32" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I32" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K32" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L32" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
@@ -1694,25 +1724,25 @@
         <v>20</v>
       </c>
       <c r="G33" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H33" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I33" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K33" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L33" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M33" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
@@ -1726,25 +1756,25 @@
         <v>20</v>
       </c>
       <c r="G34" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H34" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I34" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K34" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L34" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M34" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q34" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35">
@@ -1758,25 +1788,25 @@
         <v>20</v>
       </c>
       <c r="G35" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H35" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I35" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K35" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L35" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M35" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q35" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
@@ -1790,25 +1820,25 @@
         <v>20</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H36" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I36" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K36" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="L36" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Q36" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37">
@@ -1822,25 +1852,25 @@
         <v>20</v>
       </c>
       <c r="G37" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H37" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I37" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L37" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="Q37" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38">
@@ -1854,25 +1884,25 @@
         <v>20</v>
       </c>
       <c r="G38" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H38" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I38" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K38" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L38" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Q38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39">
@@ -1886,25 +1916,25 @@
         <v>20</v>
       </c>
       <c r="G39" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H39" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="I39" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K39" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L39" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="M39" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="Q39" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40">
@@ -1918,34 +1948,25 @@
         <v>20</v>
       </c>
       <c r="G40" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="H40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40" t="s">
+        <v>94</v>
+      </c>
+      <c r="K40" t="s">
         <v>149</v>
       </c>
-      <c r="I40" t="s">
+      <c r="L40" t="s">
+        <v>52</v>
+      </c>
+      <c r="M40" t="s">
         <v>150</v>
       </c>
-      <c r="K40" t="s">
+      <c r="Q40" t="s">
         <v>151</v>
-      </c>
-      <c r="L40" t="s">
-        <v>152</v>
-      </c>
-      <c r="M40" t="s">
-        <v>153</v>
-      </c>
-      <c r="N40">
-        <v>1</v>
-      </c>
-      <c r="O40" t="s">
-        <v>154</v>
-      </c>
-      <c r="P40" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="41">
@@ -1959,34 +1980,25 @@
         <v>20</v>
       </c>
       <c r="G41" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="H41" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="I41" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="K41" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="L41" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="M41" t="s">
         <v>153</v>
       </c>
-      <c r="N41">
-        <v>2</v>
-      </c>
-      <c r="O41" t="s">
+      <c r="Q41" t="s">
         <v>154</v>
-      </c>
-      <c r="P41" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="42">
@@ -2000,34 +2012,25 @@
         <v>20</v>
       </c>
       <c r="G42" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="H42" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="I42" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="K42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="L42" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="M42" t="s">
-        <v>153</v>
-      </c>
-      <c r="N42">
-        <v>3</v>
-      </c>
-      <c r="O42" t="s">
-        <v>154</v>
-      </c>
-      <c r="P42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="Q42" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43">
@@ -2041,34 +2044,34 @@
         <v>20</v>
       </c>
       <c r="G43" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H43" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I43" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L43" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M43" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P43" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q43" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44">
@@ -2082,34 +2085,34 @@
         <v>20</v>
       </c>
       <c r="G44" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H44" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I44" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K44" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="L44" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M44" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O44" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P44" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q44" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45">
@@ -2123,34 +2126,34 @@
         <v>20</v>
       </c>
       <c r="G45" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H45" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I45" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K45" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="L45" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M45" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N45">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O45" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P45" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q45" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46">
@@ -2164,34 +2167,34 @@
         <v>20</v>
       </c>
       <c r="G46" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H46" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I46" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K46" t="s">
+        <v>169</v>
+      </c>
+      <c r="L46" t="s">
         <v>162</v>
       </c>
-      <c r="L46" t="s">
-        <v>152</v>
-      </c>
       <c r="M46" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N46">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O46" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P46" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q46" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47">
@@ -2205,34 +2208,34 @@
         <v>20</v>
       </c>
       <c r="G47" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H47" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I47" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K47" t="s">
+        <v>170</v>
+      </c>
+      <c r="L47" t="s">
+        <v>162</v>
+      </c>
+      <c r="M47" t="s">
         <v>163</v>
       </c>
-      <c r="L47" t="s">
-        <v>152</v>
-      </c>
-      <c r="M47" t="s">
-        <v>153</v>
-      </c>
       <c r="N47">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O47" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P47" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q47" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48">
@@ -2246,34 +2249,34 @@
         <v>20</v>
       </c>
       <c r="G48" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H48" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I48" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K48" t="s">
+        <v>171</v>
+      </c>
+      <c r="L48" t="s">
+        <v>162</v>
+      </c>
+      <c r="M48" t="s">
+        <v>163</v>
+      </c>
+      <c r="N48">
+        <v>6</v>
+      </c>
+      <c r="O48" t="s">
         <v>164</v>
       </c>
-      <c r="L48" t="s">
-        <v>152</v>
-      </c>
-      <c r="M48" t="s">
-        <v>153</v>
-      </c>
-      <c r="N48">
-        <v>9</v>
-      </c>
-      <c r="O48" t="s">
-        <v>154</v>
-      </c>
       <c r="P48" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q48" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49">
@@ -2287,34 +2290,34 @@
         <v>20</v>
       </c>
       <c r="G49" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H49" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I49" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K49" t="s">
+        <v>172</v>
+      </c>
+      <c r="L49" t="s">
+        <v>162</v>
+      </c>
+      <c r="M49" t="s">
+        <v>163</v>
+      </c>
+      <c r="N49">
+        <v>7</v>
+      </c>
+      <c r="O49" t="s">
+        <v>164</v>
+      </c>
+      <c r="P49" t="s">
         <v>165</v>
       </c>
-      <c r="L49" t="s">
-        <v>152</v>
-      </c>
-      <c r="M49" t="s">
-        <v>153</v>
-      </c>
-      <c r="N49">
-        <v>10</v>
-      </c>
-      <c r="O49" t="s">
-        <v>154</v>
-      </c>
-      <c r="P49" t="s">
-        <v>155</v>
-      </c>
       <c r="Q49" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50">
@@ -2328,34 +2331,34 @@
         <v>20</v>
       </c>
       <c r="G50" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H50" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I50" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K50" t="s">
+        <v>173</v>
+      </c>
+      <c r="L50" t="s">
+        <v>162</v>
+      </c>
+      <c r="M50" t="s">
+        <v>163</v>
+      </c>
+      <c r="N50">
+        <v>8</v>
+      </c>
+      <c r="O50" t="s">
+        <v>164</v>
+      </c>
+      <c r="P50" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q50" t="s">
         <v>166</v>
-      </c>
-      <c r="L50" t="s">
-        <v>152</v>
-      </c>
-      <c r="M50" t="s">
-        <v>153</v>
-      </c>
-      <c r="N50">
-        <v>11</v>
-      </c>
-      <c r="O50" t="s">
-        <v>154</v>
-      </c>
-      <c r="P50" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="51">
@@ -2369,34 +2372,34 @@
         <v>20</v>
       </c>
       <c r="G51" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H51" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I51" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K51" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="L51" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M51" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N51">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="O51" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P51" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q51" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52">
@@ -2410,34 +2413,34 @@
         <v>20</v>
       </c>
       <c r="G52" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H52" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I52" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K52" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="L52" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M52" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N52">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="O52" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P52" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q52" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53">
@@ -2451,34 +2454,34 @@
         <v>20</v>
       </c>
       <c r="G53" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H53" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I53" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K53" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="L53" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M53" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N53">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="O53" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P53" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q53" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54">
@@ -2492,34 +2495,34 @@
         <v>20</v>
       </c>
       <c r="G54" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H54" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I54" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K54" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="L54" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M54" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N54">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O54" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P54" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q54" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55">
@@ -2533,34 +2536,34 @@
         <v>20</v>
       </c>
       <c r="G55" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H55" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I55" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K55" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="L55" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M55" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N55">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O55" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P55" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q55" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56">
@@ -2574,34 +2577,34 @@
         <v>20</v>
       </c>
       <c r="G56" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H56" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I56" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K56" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="L56" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M56" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N56">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O56" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P56" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q56" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57">
@@ -2615,34 +2618,34 @@
         <v>20</v>
       </c>
       <c r="G57" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H57" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I57" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K57" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="L57" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M57" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N57">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O57" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P57" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q57" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58">
@@ -2656,34 +2659,34 @@
         <v>20</v>
       </c>
       <c r="G58" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H58" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I58" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K58" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="L58" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M58" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N58">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="O58" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P58" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q58" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59">
@@ -2697,34 +2700,34 @@
         <v>20</v>
       </c>
       <c r="G59" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H59" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I59" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K59" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="L59" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M59" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N59">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O59" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P59" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q59" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60">
@@ -2738,34 +2741,34 @@
         <v>20</v>
       </c>
       <c r="G60" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H60" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I60" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K60" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="L60" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M60" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N60">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="O60" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P60" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q60" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="61">
@@ -2779,34 +2782,34 @@
         <v>20</v>
       </c>
       <c r="G61" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H61" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I61" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K61" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="L61" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M61" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N61">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="O61" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P61" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q61" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62">
@@ -2820,34 +2823,34 @@
         <v>20</v>
       </c>
       <c r="G62" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H62" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I62" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K62" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="L62" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M62" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N62">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="O62" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P62" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q62" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63">
@@ -2861,34 +2864,34 @@
         <v>20</v>
       </c>
       <c r="G63" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H63" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I63" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K63" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="L63" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M63" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N63">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O63" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P63" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q63" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64">
@@ -2902,34 +2905,34 @@
         <v>20</v>
       </c>
       <c r="G64" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H64" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I64" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K64" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="L64" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M64" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N64">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="O64" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P64" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q64" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65">
@@ -2943,34 +2946,34 @@
         <v>20</v>
       </c>
       <c r="G65" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H65" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I65" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K65" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="L65" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M65" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N65">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O65" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="P65" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="Q65" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66">
@@ -2984,34 +2987,157 @@
         <v>20</v>
       </c>
       <c r="G66" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="H66" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="I66" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="K66" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="L66" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="M66" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="N66">
+        <v>24</v>
+      </c>
+      <c r="O66" t="s">
+        <v>164</v>
+      </c>
+      <c r="P66" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" t="s">
+        <v>158</v>
+      </c>
+      <c r="H67" t="s">
+        <v>159</v>
+      </c>
+      <c r="I67" t="s">
+        <v>160</v>
+      </c>
+      <c r="K67" t="s">
+        <v>190</v>
+      </c>
+      <c r="L67" t="s">
+        <v>162</v>
+      </c>
+      <c r="M67" t="s">
+        <v>163</v>
+      </c>
+      <c r="N67">
+        <v>25</v>
+      </c>
+      <c r="O67" t="s">
+        <v>164</v>
+      </c>
+      <c r="P67" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" t="s">
+        <v>158</v>
+      </c>
+      <c r="H68" t="s">
+        <v>159</v>
+      </c>
+      <c r="I68" t="s">
+        <v>160</v>
+      </c>
+      <c r="K68" t="s">
+        <v>191</v>
+      </c>
+      <c r="L68" t="s">
+        <v>162</v>
+      </c>
+      <c r="M68" t="s">
+        <v>163</v>
+      </c>
+      <c r="N68">
+        <v>26</v>
+      </c>
+      <c r="O68" t="s">
+        <v>164</v>
+      </c>
+      <c r="P68" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>18</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" t="s">
+        <v>158</v>
+      </c>
+      <c r="H69" t="s">
+        <v>159</v>
+      </c>
+      <c r="I69" t="s">
+        <v>160</v>
+      </c>
+      <c r="K69" t="s">
+        <v>192</v>
+      </c>
+      <c r="L69" t="s">
+        <v>162</v>
+      </c>
+      <c r="M69" t="s">
+        <v>163</v>
+      </c>
+      <c r="N69">
         <v>27</v>
       </c>
-      <c r="O66" t="s">
-        <v>154</v>
-      </c>
-      <c r="P66" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>156</v>
+      <c r="O69" t="s">
+        <v>164</v>
+      </c>
+      <c r="P69" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: increase type-safety and add rules
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="245">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -165,19 +165,28 @@
     <t>ahc_hrsn_valid_01_screening</t>
   </si>
   <si>
-    <t>e8072bf2-b35a-43f7-acb0-e432ee838454</t>
+    <t>85efcea7-9bed-412f-99dd-7cc3fabdfe29</t>
   </si>
   <si>
     <t>Missing Column</t>
   </si>
   <si>
+    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>47eab19d-85d0-46cd-a578-6c53d0ca4801</t>
+  </si>
+  <si>
     <t>Required column FACILITY is missing in ahc_hrsn_valid_01_screening.</t>
   </si>
   <si>
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>4fb54c11-1a30-497c-b7f2-3eb781fdedc9</t>
+    <t>b8b900a9-7818-4991-a494-66b1331abfc9</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -186,7 +195,7 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>75468089-d654-449b-8f54-1fed131c7f8e</t>
+    <t>81c8f6b0-08db-4567-b2b7-de67cc03fcb0</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in ahc_hrsn_valid_01_screening.</t>
@@ -195,7 +204,25 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>93a3ef2f-7c03-4d54-9963-ffe23b558aff</t>
+    <t>efaa266f-9f05-4881-846f-36130d99f964</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>026baf29-d4aa-4bfa-a277-7431f0166cb6</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>e796270c-4dc2-43b9-a049-b9de29b0bb7f</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in ahc_hrsn_valid_01_screening.</t>
@@ -204,25 +231,16 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>4c02d136-85f0-4aa3-a0f8-a8eaa36ecbbf</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>39cefa29-8080-4bcd-aedf-b3126d48e525</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>36f9f665-5cae-45ab-942a-866d651b982d</t>
+    <t>fce2c712-c9bd-4baa-8161-197dfee1bd73</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>fb6a7d77-196c-4a72-b138-f19c22306fad</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in ahc_hrsn_valid_01_screening.</t>
@@ -231,25 +249,25 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>ee5b41c4-17bb-4895-a53e-5de19f2bb425</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>a906d5d1-1895-4062-8575-6b0315792fd3</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>fb6a39c9-90fd-43f3-aedb-26b31d0c87a5</t>
+    <t>7ae7670b-7815-4b52-beaa-4a191abe807f</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>b2d21057-8e99-44f9-951f-b678cc408988</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
+  </si>
+  <si>
+    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>f051d49a-c14f-4d30-85bf-0a689887d23a</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
@@ -258,24 +276,6 @@
     <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>3c51ef73-6c00-48fa-aaa8-ec2abed99acb</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>3a2d069f-04d3-4954-9b54-4142bcd0f467</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in ahc_hrsn_valid_01_screening.</t>
-  </si>
-  <si>
-    <t>Ensure ahc_hrsn_valid_01_screening contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
     <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
   </si>
   <si>
@@ -297,7 +297,97 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>478df3f3-5634-4055-b749-a8194910501e</t>
+    <t>738d4342-dbdd-4be7-90f5-a89a2d5e6f61</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>4730a786-f1bf-4fb9-9815-6e98d798c353</t>
+  </si>
+  <si>
+    <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
+  </si>
+  <si>
+    <t>73b79d3f-ac78-4252-b205-f3402579ac97</t>
+  </si>
+  <si>
+    <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
+  </si>
+  <si>
+    <t>17a0922f-bc1c-4d4e-b5b1-650c7c7d358f</t>
+  </si>
+  <si>
+    <t>Required column FACILITY is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "FACILITY"</t>
+  </si>
+  <si>
+    <t>3e35350e-8162-426d-86d2-4868d8dbbf08</t>
+  </si>
+  <si>
+    <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
+  </si>
+  <si>
+    <t>aeceebef-855e-4008-a227-85d2a8984b3a</t>
+  </si>
+  <si>
+    <t>Required column LAST_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
+  </si>
+  <si>
+    <t>7e19ff98-1234-4ffd-82ac-21fa291f04f1</t>
+  </si>
+  <si>
+    <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
+  </si>
+  <si>
+    <t>281ee6c7-1abf-403f-9e0f-95a2c917e393</t>
+  </si>
+  <si>
+    <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
+  </si>
+  <si>
+    <t>90ae75f0-a24b-42c9-87c8-910450de94c5</t>
+  </si>
+  <si>
+    <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
+  </si>
+  <si>
+    <t>bed84d18-b72f-4c63-b6d4-623a2cd2a0fd</t>
+  </si>
+  <si>
+    <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
+  </si>
+  <si>
+    <t>63ab1f6e-8c85-4f2b-8fae-297831ab45f0</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -306,61 +396,61 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>4c048f3b-2cee-4c9c-8244-45cb68b34de8</t>
-  </si>
-  <si>
-    <t>Required column FACILITY is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "FACILITY"</t>
-  </si>
-  <si>
-    <t>6f223a56-4770-4967-a77b-ee913cc4e381</t>
-  </si>
-  <si>
-    <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
-  </si>
-  <si>
-    <t>3549d51c-7ed6-4efc-83a3-295b6b89a39a</t>
-  </si>
-  <si>
-    <t>Required column LAST_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
-  </si>
-  <si>
-    <t>14fba79f-4bf3-40db-99ad-de7d3ff7c376</t>
-  </si>
-  <si>
-    <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
-  </si>
-  <si>
-    <t>1a5e19a3-7824-4a10-b89d-a611da7f8fd0</t>
-  </si>
-  <si>
-    <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
-  </si>
-  <si>
-    <t>4cb48244-cffe-4364-825e-270d560bd038</t>
-  </si>
-  <si>
-    <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
-  </si>
-  <si>
-    <t>f2028828-18f4-4e93-b98e-bd1034c1e902</t>
+    <t>b620850e-6999-4fee-8ba0-6d77b5028dff</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
+  </si>
+  <si>
+    <t>59f33c76-6866-4b86-bd99-4beb3ecb8a6e</t>
+  </si>
+  <si>
+    <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
+  </si>
+  <si>
+    <t>67a5b456-c42c-4b01-8410-4e03cf7e8219</t>
+  </si>
+  <si>
+    <t>Required column QUESTION is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "QUESTION"</t>
+  </si>
+  <si>
+    <t>5c92d010-f860-4e01-b961-8bbfafbc503b</t>
+  </si>
+  <si>
+    <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
+  </si>
+  <si>
+    <t>fc3fff70-dd9e-43d7-b27e-2c23d0fcc711</t>
+  </si>
+  <si>
+    <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
+  </si>
+  <si>
+    <t>ca1adda6-7b64-4545-8789-ad94530597b1</t>
+  </si>
+  <si>
+    <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
+  </si>
+  <si>
+    <t>bae92016-1f8b-4d73-9e64-47fc776b2d49</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -369,97 +459,25 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>0990a6f3-9fdf-4c40-bc6a-595af64f8ce5</t>
-  </si>
-  <si>
-    <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
-  </si>
-  <si>
-    <t>96bd7521-da8f-4bbf-a6d9-9952dceaff28</t>
-  </si>
-  <si>
-    <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
-  </si>
-  <si>
-    <t>d0e1e6d2-537a-4f30-8d50-efb9e5505259</t>
-  </si>
-  <si>
-    <t>Required column QUESTION is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "QUESTION"</t>
-  </si>
-  <si>
-    <t>b46bab6a-1095-4edd-847f-1c27a60e5377</t>
-  </si>
-  <si>
-    <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
-  </si>
-  <si>
-    <t>955e5510-b7e9-4b46-a5e8-8c417bde1eaa</t>
-  </si>
-  <si>
-    <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
-  </si>
-  <si>
-    <t>6c72b864-b0ae-4f72-884c-341d0df2d6ae</t>
-  </si>
-  <si>
-    <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
-  </si>
-  <si>
-    <t>fe18eecb-5a58-444e-9a6d-09537b5d49e7</t>
-  </si>
-  <si>
-    <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
-  </si>
-  <si>
-    <t>48adf76c-bf15-4d76-9250-e24ffe07c3e4</t>
-  </si>
-  <si>
-    <t>Required column ANSWER_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
-  </si>
-  <si>
-    <t>bfdc6088-c3a4-4917-8282-3212efefb5cd</t>
-  </si>
-  <si>
-    <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
-  </si>
-  <si>
-    <t>fce070ce-037c-46d6-9f9c-6885b791531b</t>
-  </si>
-  <si>
-    <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
-  </si>
-  <si>
-    <t>295a3da8-31e8-414a-b192-d52b506060a1</t>
+    <t>b262e432-56d5-455a-b122-02996609bd53</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
+  </si>
+  <si>
+    <t>cae20b66-d13e-4096-9102-b6eaa00ebba1</t>
+  </si>
+  <si>
+    <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
+  </si>
+  <si>
+    <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
+  </si>
+  <si>
+    <t>adc470a9-cc6c-4d6b-99e8-13929112bb59</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -468,24 +486,6 @@
     <t>Ensure synthetic_fail contains the column "VISIT_PART_2_FLAG"</t>
   </si>
   <si>
-    <t>b63679a7-5188-46c3-9b59-f7e586b88ff4</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
-  </si>
-  <si>
-    <t>84c22787-93a6-4b5c-a9a7-f63211d99868</t>
-  </si>
-  <si>
-    <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
-  </si>
-  <si>
-    <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
-  </si>
-  <si>
     <t>c60cf3db-b1bf-5103-b278-b0c128ce924a</t>
   </si>
   <si>
@@ -495,100 +495,256 @@
     <t>ahc_hrsn_12_12_2023_valid</t>
   </si>
   <si>
-    <t>bdbe5b5a-e186-4b87-8918-796e1b5146d1</t>
-  </si>
-  <si>
-    <t>Data Type Mismatch</t>
-  </si>
-  <si>
-    <t>Non-integer value "AHCHRSN01" found in SURVEY_ID</t>
-  </si>
-  <si>
-    <t>SURVEY_ID</t>
-  </si>
-  <si>
-    <t>AHCHRSN01</t>
-  </si>
-  <si>
-    <t>Convert non-integer values to INTEGER</t>
-  </si>
-  <si>
-    <t>b36b3553-e7ac-4e16-9c0a-6f07a88a5373</t>
-  </si>
-  <si>
-    <t>3db2979f-913f-451e-a36e-c534abdeb4e0</t>
-  </si>
-  <si>
-    <t>1e91bc80-a5a9-48a2-82a4-27ea6d0158dd</t>
-  </si>
-  <si>
-    <t>b62c0483-6814-4abd-a54c-f5dd6444f171</t>
-  </si>
-  <si>
-    <t>d174ce5a-9baa-42d3-8f3e-8a23406b0662</t>
-  </si>
-  <si>
-    <t>0a4fbf7a-0e9d-4aa9-9339-eb5c6edaec39</t>
-  </si>
-  <si>
-    <t>33187aac-eeda-4649-8cb5-d177e002a244</t>
-  </si>
-  <si>
-    <t>ba704267-8f26-4568-88d7-20de7115419c</t>
-  </si>
-  <si>
-    <t>62dbc77b-b212-4555-b7ad-9a7ac4a9ebf9</t>
-  </si>
-  <si>
-    <t>33e9a0c1-3a63-4faf-99dd-8eada6bd463b</t>
-  </si>
-  <si>
-    <t>98ae6f47-0d61-44cb-ab2a-a0f8733d7149</t>
-  </si>
-  <si>
-    <t>b6e47942-9086-456b-8105-9a03c5374278</t>
-  </si>
-  <si>
-    <t>6587a497-e5da-45ab-86dc-44db98f3e460</t>
-  </si>
-  <si>
-    <t>695c3bfa-c1b9-455f-bf96-8b1d5d7524fd</t>
-  </si>
-  <si>
-    <t>0e2df081-9bac-4637-8808-05cf4da5b1c7</t>
-  </si>
-  <si>
-    <t>d11bc45e-14f6-4ec9-8e75-b957f76f5d85</t>
-  </si>
-  <si>
-    <t>2a40b763-bbe9-4c73-a242-ac1273918eb2</t>
-  </si>
-  <si>
-    <t>70262c9a-f47c-4409-b39c-e958b7f808fe</t>
-  </si>
-  <si>
-    <t>ae08bf13-7445-4ff8-a512-9393b05d0c15</t>
-  </si>
-  <si>
-    <t>4a09c8b7-d6a8-42a4-b7a6-41be06cc86f6</t>
-  </si>
-  <si>
-    <t>01465847-d973-4323-b2ed-87ecd6f6c3fa</t>
-  </si>
-  <si>
-    <t>1543e2ab-1380-4abe-9304-745303c6d216</t>
-  </si>
-  <si>
-    <t>4417d626-2f03-4f45-b6e4-ac139c7c25db</t>
-  </si>
-  <si>
-    <t>d3bae684-8b35-401a-a243-7252ddb95bd3</t>
-  </si>
-  <si>
-    <t>e5f3e2f8-23ce-4402-b210-cc21bf2023d2</t>
-  </si>
-  <si>
-    <t>294b1a56-4d03-4927-8928-31ff5b651103</t>
+    <t>b5da270e-5e2f-4d3a-b9f0-29b2a6dca776</t>
+  </si>
+  <si>
+    <t>Invalid Value</t>
+  </si>
+  <si>
+    <t>Value 71802-3 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>QUESTION_CODE</t>
+  </si>
+  <si>
+    <t>71802-3</t>
+  </si>
+  <si>
+    <t>Use only allowed values 71802-3,96778-6 in QUESTION_CODE</t>
+  </si>
+  <si>
+    <t>6ce8d267-cc74-46b7-b20f-515289d015a3</t>
+  </si>
+  <si>
+    <t>Value 96778-6	 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>96778-6	</t>
+  </si>
+  <si>
+    <t>661f17bb-1159-446a-acd0-8bc8259c06fe</t>
+  </si>
+  <si>
+    <t>Value 88122-7 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>88122-7</t>
+  </si>
+  <si>
+    <t>8eb97664-3b83-41e6-acf7-ce756b2ada53</t>
+  </si>
+  <si>
+    <t>Value 88123-5 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>88123-5</t>
+  </si>
+  <si>
+    <t>4559fecd-fcf3-46f7-9371-10e128ac544f</t>
+  </si>
+  <si>
+    <t>Value 93030-5 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>93030-5</t>
+  </si>
+  <si>
+    <t>3d3ee8a0-4fa9-492d-9cf9-1e455b64bbfc</t>
+  </si>
+  <si>
+    <t>Value 96779-4 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>96779-4</t>
+  </si>
+  <si>
+    <t>7ab61fa7-4548-4fa4-9830-d97dad6b613e</t>
+  </si>
+  <si>
+    <t>Value 95618-5 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>95618-5</t>
+  </si>
+  <si>
+    <t>12fdeba6-cddd-4e50-8e4b-2eb849ba4072</t>
+  </si>
+  <si>
+    <t>Value 95617-7 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>95617-7</t>
+  </si>
+  <si>
+    <t>cf845311-0e1d-4eb5-9c01-b9dd5e7b6e7c</t>
+  </si>
+  <si>
+    <t>Value 95616-9 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>95616-9</t>
+  </si>
+  <si>
+    <t>fde2822a-5c93-43a9-ae5d-d8be243b559c</t>
+  </si>
+  <si>
+    <t>Value 95615-1 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>95615-1</t>
+  </si>
+  <si>
+    <t>52d66915-c7cf-46fd-8105-60bd160784dd</t>
+  </si>
+  <si>
+    <t>Value 76513-1 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>76513-1</t>
+  </si>
+  <si>
+    <t>1764264e-b081-4ed3-bb02-fb9570beb84e</t>
+  </si>
+  <si>
+    <t>Value 96780-2 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>96780-2</t>
+  </si>
+  <si>
+    <t>28384edd-a7b6-46c4-8f14-ebb427541d9d</t>
+  </si>
+  <si>
+    <t>Value 96781-0 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>96781-0</t>
+  </si>
+  <si>
+    <t>34542845-39da-4ce9-a67a-dd2c4b501043</t>
+  </si>
+  <si>
+    <t>Value 93159-2	 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>93159-2	</t>
+  </si>
+  <si>
+    <t>ac2520b3-041d-42f9-ac2f-ea28c42b69dd</t>
+  </si>
+  <si>
+    <t>Value 97027-7 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>97027-7</t>
+  </si>
+  <si>
+    <t>9793ad7d-bf28-40e8-bab3-468f2e70c125</t>
+  </si>
+  <si>
+    <t>Value 96782-8	 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>96782-8	</t>
+  </si>
+  <si>
+    <t>95ee2443-df5f-407e-a0f0-23d30be7d6a2</t>
+  </si>
+  <si>
+    <t>Value 89555-7 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>89555-7</t>
+  </si>
+  <si>
+    <t>6c30cb9c-60e4-40f6-989c-3c50243f7c78</t>
+  </si>
+  <si>
+    <t>Value 68516-4	 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>68516-4	</t>
+  </si>
+  <si>
+    <t>8d1553e0-4f5d-415c-8d03-7aaecef7bb7b</t>
+  </si>
+  <si>
+    <t>Value 68517-2 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>68517-2</t>
+  </si>
+  <si>
+    <t>b5cc4584-3f2f-42ee-a425-1d6d0ea9a442</t>
+  </si>
+  <si>
+    <t>Value 96842-0 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>96842-0</t>
+  </si>
+  <si>
+    <t>d38df34c-3da6-4f19-abb2-0730eb32ad1a</t>
+  </si>
+  <si>
+    <t>Value 95530-2 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>95530-2</t>
+  </si>
+  <si>
+    <t>cd6f1c94-1478-4803-aa84-193e093c3589</t>
+  </si>
+  <si>
+    <t>Value 68524-8 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>68524-8</t>
+  </si>
+  <si>
+    <t>babc94c0-82da-45d5-af10-f3f14b1d1220</t>
+  </si>
+  <si>
+    <t>Value 44250-9 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>44250-9</t>
+  </si>
+  <si>
+    <t>64297238-66ce-4dc6-9616-ba478a422439</t>
+  </si>
+  <si>
+    <t>Value 44255-8 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>44255-8</t>
+  </si>
+  <si>
+    <t>0b445a2c-2536-4c05-b98f-c74f5f732961</t>
+  </si>
+  <si>
+    <t>Value 93038-8 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>93038-8</t>
+  </si>
+  <si>
+    <t>c277b268-334b-435d-ace7-d42b52ac40d7</t>
+  </si>
+  <si>
+    <t>Value 69858-9 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>69858-9</t>
+  </si>
+  <si>
+    <t>c4cd6cd2-e97f-4afe-8796-ae5f87a3f776</t>
+  </si>
+  <si>
+    <t>Value 69861-3	 in QUESTION_CODE not in allowed list (71802-3,96778-6)</t>
+  </si>
+  <si>
+    <t>69861-3	</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2256,7 @@
         <v>162</v>
       </c>
       <c r="M44" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="N44">
         <v>2</v>
@@ -2109,7 +2265,7 @@
         <v>164</v>
       </c>
       <c r="P44" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="Q44" t="s">
         <v>166</v>
@@ -2135,13 +2291,13 @@
         <v>160</v>
       </c>
       <c r="K45" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="L45" t="s">
         <v>162</v>
       </c>
       <c r="M45" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="N45">
         <v>3</v>
@@ -2150,7 +2306,7 @@
         <v>164</v>
       </c>
       <c r="P45" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="Q45" t="s">
         <v>166</v>
@@ -2176,13 +2332,13 @@
         <v>160</v>
       </c>
       <c r="K46" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="L46" t="s">
         <v>162</v>
       </c>
       <c r="M46" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="N46">
         <v>4</v>
@@ -2191,7 +2347,7 @@
         <v>164</v>
       </c>
       <c r="P46" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="Q46" t="s">
         <v>166</v>
@@ -2217,13 +2373,13 @@
         <v>160</v>
       </c>
       <c r="K47" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="L47" t="s">
         <v>162</v>
       </c>
       <c r="M47" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="N47">
         <v>5</v>
@@ -2232,7 +2388,7 @@
         <v>164</v>
       </c>
       <c r="P47" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="Q47" t="s">
         <v>166</v>
@@ -2258,13 +2414,13 @@
         <v>160</v>
       </c>
       <c r="K48" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="L48" t="s">
         <v>162</v>
       </c>
       <c r="M48" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="N48">
         <v>6</v>
@@ -2273,7 +2429,7 @@
         <v>164</v>
       </c>
       <c r="P48" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="Q48" t="s">
         <v>166</v>
@@ -2299,13 +2455,13 @@
         <v>160</v>
       </c>
       <c r="K49" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="L49" t="s">
         <v>162</v>
       </c>
       <c r="M49" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="N49">
         <v>7</v>
@@ -2314,7 +2470,7 @@
         <v>164</v>
       </c>
       <c r="P49" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="Q49" t="s">
         <v>166</v>
@@ -2340,13 +2496,13 @@
         <v>160</v>
       </c>
       <c r="K50" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="L50" t="s">
         <v>162</v>
       </c>
       <c r="M50" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="N50">
         <v>8</v>
@@ -2355,7 +2511,7 @@
         <v>164</v>
       </c>
       <c r="P50" t="s">
-        <v>165</v>
+        <v>187</v>
       </c>
       <c r="Q50" t="s">
         <v>166</v>
@@ -2381,13 +2537,13 @@
         <v>160</v>
       </c>
       <c r="K51" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="L51" t="s">
         <v>162</v>
       </c>
       <c r="M51" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="N51">
         <v>9</v>
@@ -2396,7 +2552,7 @@
         <v>164</v>
       </c>
       <c r="P51" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="Q51" t="s">
         <v>166</v>
@@ -2422,13 +2578,13 @@
         <v>160</v>
       </c>
       <c r="K52" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="L52" t="s">
         <v>162</v>
       </c>
       <c r="M52" t="s">
-        <v>163</v>
+        <v>192</v>
       </c>
       <c r="N52">
         <v>10</v>
@@ -2437,7 +2593,7 @@
         <v>164</v>
       </c>
       <c r="P52" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="Q52" t="s">
         <v>166</v>
@@ -2463,13 +2619,13 @@
         <v>160</v>
       </c>
       <c r="K53" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="L53" t="s">
         <v>162</v>
       </c>
       <c r="M53" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="N53">
         <v>11</v>
@@ -2478,7 +2634,7 @@
         <v>164</v>
       </c>
       <c r="P53" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="Q53" t="s">
         <v>166</v>
@@ -2504,13 +2660,13 @@
         <v>160</v>
       </c>
       <c r="K54" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="L54" t="s">
         <v>162</v>
       </c>
       <c r="M54" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="N54">
         <v>12</v>
@@ -2519,7 +2675,7 @@
         <v>164</v>
       </c>
       <c r="P54" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="Q54" t="s">
         <v>166</v>
@@ -2545,13 +2701,13 @@
         <v>160</v>
       </c>
       <c r="K55" t="s">
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="L55" t="s">
         <v>162</v>
       </c>
       <c r="M55" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="N55">
         <v>13</v>
@@ -2560,7 +2716,7 @@
         <v>164</v>
       </c>
       <c r="P55" t="s">
-        <v>165</v>
+        <v>202</v>
       </c>
       <c r="Q55" t="s">
         <v>166</v>
@@ -2586,13 +2742,13 @@
         <v>160</v>
       </c>
       <c r="K56" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="L56" t="s">
         <v>162</v>
       </c>
       <c r="M56" t="s">
-        <v>163</v>
+        <v>204</v>
       </c>
       <c r="N56">
         <v>14</v>
@@ -2601,7 +2757,7 @@
         <v>164</v>
       </c>
       <c r="P56" t="s">
-        <v>165</v>
+        <v>205</v>
       </c>
       <c r="Q56" t="s">
         <v>166</v>
@@ -2627,13 +2783,13 @@
         <v>160</v>
       </c>
       <c r="K57" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="L57" t="s">
         <v>162</v>
       </c>
       <c r="M57" t="s">
-        <v>163</v>
+        <v>207</v>
       </c>
       <c r="N57">
         <v>15</v>
@@ -2642,7 +2798,7 @@
         <v>164</v>
       </c>
       <c r="P57" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="Q57" t="s">
         <v>166</v>
@@ -2668,13 +2824,13 @@
         <v>160</v>
       </c>
       <c r="K58" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="L58" t="s">
         <v>162</v>
       </c>
       <c r="M58" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="N58">
         <v>16</v>
@@ -2683,7 +2839,7 @@
         <v>164</v>
       </c>
       <c r="P58" t="s">
-        <v>165</v>
+        <v>211</v>
       </c>
       <c r="Q58" t="s">
         <v>166</v>
@@ -2709,13 +2865,13 @@
         <v>160</v>
       </c>
       <c r="K59" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="L59" t="s">
         <v>162</v>
       </c>
       <c r="M59" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="N59">
         <v>17</v>
@@ -2724,7 +2880,7 @@
         <v>164</v>
       </c>
       <c r="P59" t="s">
-        <v>165</v>
+        <v>214</v>
       </c>
       <c r="Q59" t="s">
         <v>166</v>
@@ -2750,13 +2906,13 @@
         <v>160</v>
       </c>
       <c r="K60" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
       <c r="L60" t="s">
         <v>162</v>
       </c>
       <c r="M60" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="N60">
         <v>18</v>
@@ -2765,7 +2921,7 @@
         <v>164</v>
       </c>
       <c r="P60" t="s">
-        <v>165</v>
+        <v>217</v>
       </c>
       <c r="Q60" t="s">
         <v>166</v>
@@ -2791,13 +2947,13 @@
         <v>160</v>
       </c>
       <c r="K61" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="L61" t="s">
         <v>162</v>
       </c>
       <c r="M61" t="s">
-        <v>163</v>
+        <v>219</v>
       </c>
       <c r="N61">
         <v>19</v>
@@ -2806,7 +2962,7 @@
         <v>164</v>
       </c>
       <c r="P61" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
       <c r="Q61" t="s">
         <v>166</v>
@@ -2832,13 +2988,13 @@
         <v>160</v>
       </c>
       <c r="K62" t="s">
-        <v>185</v>
+        <v>221</v>
       </c>
       <c r="L62" t="s">
         <v>162</v>
       </c>
       <c r="M62" t="s">
-        <v>163</v>
+        <v>222</v>
       </c>
       <c r="N62">
         <v>20</v>
@@ -2847,7 +3003,7 @@
         <v>164</v>
       </c>
       <c r="P62" t="s">
-        <v>165</v>
+        <v>223</v>
       </c>
       <c r="Q62" t="s">
         <v>166</v>
@@ -2873,13 +3029,13 @@
         <v>160</v>
       </c>
       <c r="K63" t="s">
-        <v>186</v>
+        <v>224</v>
       </c>
       <c r="L63" t="s">
         <v>162</v>
       </c>
       <c r="M63" t="s">
-        <v>163</v>
+        <v>225</v>
       </c>
       <c r="N63">
         <v>21</v>
@@ -2888,7 +3044,7 @@
         <v>164</v>
       </c>
       <c r="P63" t="s">
-        <v>165</v>
+        <v>226</v>
       </c>
       <c r="Q63" t="s">
         <v>166</v>
@@ -2914,13 +3070,13 @@
         <v>160</v>
       </c>
       <c r="K64" t="s">
-        <v>187</v>
+        <v>227</v>
       </c>
       <c r="L64" t="s">
         <v>162</v>
       </c>
       <c r="M64" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="N64">
         <v>22</v>
@@ -2929,7 +3085,7 @@
         <v>164</v>
       </c>
       <c r="P64" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="Q64" t="s">
         <v>166</v>
@@ -2955,13 +3111,13 @@
         <v>160</v>
       </c>
       <c r="K65" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="L65" t="s">
         <v>162</v>
       </c>
       <c r="M65" t="s">
-        <v>163</v>
+        <v>231</v>
       </c>
       <c r="N65">
         <v>23</v>
@@ -2970,7 +3126,7 @@
         <v>164</v>
       </c>
       <c r="P65" t="s">
-        <v>165</v>
+        <v>232</v>
       </c>
       <c r="Q65" t="s">
         <v>166</v>
@@ -2996,13 +3152,13 @@
         <v>160</v>
       </c>
       <c r="K66" t="s">
-        <v>189</v>
+        <v>233</v>
       </c>
       <c r="L66" t="s">
         <v>162</v>
       </c>
       <c r="M66" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="N66">
         <v>24</v>
@@ -3011,7 +3167,7 @@
         <v>164</v>
       </c>
       <c r="P66" t="s">
-        <v>165</v>
+        <v>235</v>
       </c>
       <c r="Q66" t="s">
         <v>166</v>
@@ -3037,13 +3193,13 @@
         <v>160</v>
       </c>
       <c r="K67" t="s">
-        <v>190</v>
+        <v>236</v>
       </c>
       <c r="L67" t="s">
         <v>162</v>
       </c>
       <c r="M67" t="s">
-        <v>163</v>
+        <v>237</v>
       </c>
       <c r="N67">
         <v>25</v>
@@ -3052,7 +3208,7 @@
         <v>164</v>
       </c>
       <c r="P67" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="Q67" t="s">
         <v>166</v>
@@ -3078,13 +3234,13 @@
         <v>160</v>
       </c>
       <c r="K68" t="s">
-        <v>191</v>
+        <v>239</v>
       </c>
       <c r="L68" t="s">
         <v>162</v>
       </c>
       <c r="M68" t="s">
-        <v>163</v>
+        <v>240</v>
       </c>
       <c r="N68">
         <v>26</v>
@@ -3093,7 +3249,7 @@
         <v>164</v>
       </c>
       <c r="P68" t="s">
-        <v>165</v>
+        <v>241</v>
       </c>
       <c r="Q68" t="s">
         <v>166</v>
@@ -3119,13 +3275,13 @@
         <v>160</v>
       </c>
       <c r="K69" t="s">
-        <v>192</v>
+        <v>242</v>
       </c>
       <c r="L69" t="s">
         <v>162</v>
       </c>
       <c r="M69" t="s">
-        <v>163</v>
+        <v>243</v>
       </c>
       <c r="N69">
         <v>27</v>
@@ -3134,7 +3290,7 @@
         <v>164</v>
       </c>
       <c r="P69" t="s">
-        <v>165</v>
+        <v>244</v>
       </c>
       <c r="Q69" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
feat: introduce SDLC compliance infrastructure
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -168,7 +168,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>5ebc4fc0-016b-4689-ba12-e0990f7273d0</t>
+    <t>e518da22-7605-49f9-8dec-9edfcc8ffad2</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -180,7 +180,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>1c3a7eb0-1db4-4392-89c4-7018ca2d7e25</t>
+    <t>8f550447-effe-4641-95c6-0a79caed6c81</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -189,7 +189,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>a1417bf0-00b5-4adc-9dea-5f835306d367</t>
+    <t>e24fac9e-1dea-4918-8527-eccc133dc297</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -198,7 +198,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>abbbb2b8-237b-431a-ae6a-583c4e4f4d04</t>
+    <t>0a5bf65c-a679-41b8-9476-b4610b35f8ee</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -207,7 +207,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>af975844-2476-4d90-9a77-280b515f82d0</t>
+    <t>7dfd62df-b658-44c1-9204-beac6686d8c2</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -216,7 +216,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>749373dd-68bb-4446-84d9-c2fef91b7078</t>
+    <t>a638b785-9e8f-4c94-9825-e18b6c067668</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -225,7 +225,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>d39ebb6c-4cb6-4b93-b53c-8ac86d45d8ff</t>
+    <t>2b4ee646-6072-4e28-8a53-2592dca481cf</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -234,7 +234,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>146e294e-3b61-4428-84ac-6f8f1b24f363</t>
+    <t>57cbfe6b-cdd1-48c0-8777-bdea1c3eebbc</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -243,7 +243,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>faf681d2-adbe-47b3-8ec4-770f3243b9e3</t>
+    <t>ce90fc5b-f7ad-45f5-a5f7-51636ee5d9e1</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -252,7 +252,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>9203972f-a22b-4629-9511-72f9edae5d94</t>
+    <t>29be68ad-ceee-4a8c-aca3-e69fa5e9c0fa</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -261,7 +261,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>07baa847-e339-40d3-86b2-97295c16dd0b</t>
+    <t>c54b6936-fd21-4752-a43d-4a835afe92a8</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -270,7 +270,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>a9f4c9bd-fcbc-4370-9767-835166f4d521</t>
+    <t>d6f82305-003b-42e7-bb42-8d5cb6cb5bf4</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -279,7 +279,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>14e87de7-f032-4d25-a37d-671f3c2e4541</t>
+    <t>9677d4af-7245-429b-8fe7-878a72c74e49</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -288,7 +288,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>3e6133b2-4010-41f5-b794-8e43d5439a86</t>
+    <t>6c21838d-3e6d-4549-aaff-433efcfc3278</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -297,7 +297,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>31f7a949-51c3-430b-a4d3-38befc47e9af</t>
+    <t>beaf8db1-94d5-4146-a032-345cee5fede9</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -306,7 +306,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>41c9cff1-2656-46f8-9cca-e16dc2e89880</t>
+    <t>c02fa68d-153f-4acc-97a1-5bd0d0514055</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -315,7 +315,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>de786c06-1d89-4178-9194-46e0587a464e</t>
+    <t>4db672f0-f4b3-4e81-b8ac-e6b8e01a5080</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -324,7 +324,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>d451e291-61e6-48c4-ad01-57251a36ef58</t>
+    <t>049f60d6-5b4f-4db5-b116-f4ad3c321c66</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -333,7 +333,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>2c809e37-7f76-4f29-9096-03a8c5e8756e</t>
+    <t>627e2ed0-034c-482a-a0c4-213f54e7d663</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -342,7 +342,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>f2fd64e7-3f88-4bca-93ad-0a56423dd560</t>
+    <t>bfe55423-2c4e-4903-bd9e-9c02f9c838e4</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -351,7 +351,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>f950dd2c-e0d7-41c6-b8eb-be8d5ce49301</t>
+    <t>830c5baa-c8b5-45d6-ac3b-b8449283d544</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>ahc_hrsn_2023_12_12_valid</t>
   </si>
   <si>
-    <t>ac640321-f55e-4e69-9db8-ccfd4e035337</t>
+    <t>fd59a27e-a6cc-44db-9148-373797f19f92</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -402,7 +402,7 @@
     <t>Use only allowed values '71802-3','96778-6' in QUESTION_CODE</t>
   </si>
   <si>
-    <t>312c5919-57ae-4ca1-b05c-52325e45ebcc</t>
+    <t>551f7746-171a-453e-b340-aae12b40caf6</t>
   </si>
   <si>
     <t>Value 88122-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -411,7 +411,7 @@
     <t>88122-7</t>
   </si>
   <si>
-    <t>e7c9edf9-4d5c-4839-9b14-7865bfacfb28</t>
+    <t>1630f993-7ad0-42f9-92c8-6c78534ad021</t>
   </si>
   <si>
     <t>Value 88123-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -420,7 +420,7 @@
     <t>88123-5</t>
   </si>
   <si>
-    <t>0b94ccba-f4b6-4463-b818-a9cc7f69aa6b</t>
+    <t>f2467db1-3ae0-425e-af49-469a67d4ac45</t>
   </si>
   <si>
     <t>Value 93030-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -429,7 +429,7 @@
     <t>93030-5</t>
   </si>
   <si>
-    <t>10a6167f-7789-493c-9743-f09a2e97ace2</t>
+    <t>92a4986d-4600-4e10-9154-078b1a29a65d</t>
   </si>
   <si>
     <t>Value 96779-4 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -438,7 +438,7 @@
     <t>96779-4</t>
   </si>
   <si>
-    <t>baca343c-0f93-4f83-ac72-ad99d0dcb5e9</t>
+    <t>d9a6454a-a0db-499f-8dc2-2994814404e1</t>
   </si>
   <si>
     <t>Value 95618-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -447,7 +447,7 @@
     <t>95618-5</t>
   </si>
   <si>
-    <t>f562fa4b-5c42-46b7-a3be-7152f722011d</t>
+    <t>3ce13d44-1548-4305-b1c4-fa90d76809fb</t>
   </si>
   <si>
     <t>Value 95617-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -456,7 +456,7 @@
     <t>95617-7</t>
   </si>
   <si>
-    <t>51944ea0-e609-4cbd-b7ed-a849107ab414</t>
+    <t>7b903a97-b7f5-4abe-bc04-b1578fb7802d</t>
   </si>
   <si>
     <t>Value 95616-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -465,7 +465,7 @@
     <t>95616-9</t>
   </si>
   <si>
-    <t>ef516127-81f1-44f2-b7f2-34a67290cd53</t>
+    <t>92e40b91-f92a-49e9-bb91-bf3c0b02f86c</t>
   </si>
   <si>
     <t>Value 95615-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -474,7 +474,7 @@
     <t>95615-1</t>
   </si>
   <si>
-    <t>001a3797-987d-4b8c-8fd1-79e35cb713ef</t>
+    <t>1134c277-c666-4bf8-b3fb-0222201050df</t>
   </si>
   <si>
     <t>Value 76513-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -483,7 +483,7 @@
     <t>76513-1</t>
   </si>
   <si>
-    <t>e9497990-f4d0-4842-825b-6242f4d53c86</t>
+    <t>c0bf7f6e-20ce-49b5-b911-8cca3f3840af</t>
   </si>
   <si>
     <t>Value 96780-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -492,7 +492,7 @@
     <t>96780-2</t>
   </si>
   <si>
-    <t>b4f8f8a5-b912-4aa8-8a8b-28d9bdc79d65</t>
+    <t>f2a5f9dd-490a-4741-a8a6-f84e6d14b0fd</t>
   </si>
   <si>
     <t>Value 96781-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -501,7 +501,7 @@
     <t>96781-0</t>
   </si>
   <si>
-    <t>4a18d131-5f28-45ef-b2cc-b50a708d785c</t>
+    <t>084c2d61-c30d-46a4-b365-5a8f1cc3f7b4</t>
   </si>
   <si>
     <t>Value 93159-2	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -510,7 +510,7 @@
     <t>93159-2	</t>
   </si>
   <si>
-    <t>1b9c8b1b-7695-4210-a8b2-26d6a668eb9f</t>
+    <t>e3632ccf-fc1e-415e-a516-0d3e57c53ace</t>
   </si>
   <si>
     <t>Value 97027-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -519,7 +519,7 @@
     <t>97027-7</t>
   </si>
   <si>
-    <t>1c315bf7-a353-4179-ac1c-bee85b336fb2</t>
+    <t>644d144d-33e2-4822-b324-d9efd7e2cd01</t>
   </si>
   <si>
     <t>Value 96782-8	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -528,7 +528,7 @@
     <t>96782-8	</t>
   </si>
   <si>
-    <t>3f044bed-713c-4f10-81b9-047f91ae53ba</t>
+    <t>591ad535-6713-46cd-8f86-27d27ac00765</t>
   </si>
   <si>
     <t>Value 89555-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -537,7 +537,7 @@
     <t>89555-7</t>
   </si>
   <si>
-    <t>5b41159b-c43a-49af-ae1d-36cc76640a43</t>
+    <t>ff871831-9c38-48f7-a02f-7ab16d74cd3f</t>
   </si>
   <si>
     <t>Value 68516-4	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -546,7 +546,7 @@
     <t>68516-4	</t>
   </si>
   <si>
-    <t>cd7c6bd1-1a16-4d96-b167-67d80ffe58d2</t>
+    <t>fd6e1127-afcf-4ed1-b629-428279d6dd8a</t>
   </si>
   <si>
     <t>Value 68517-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -555,7 +555,7 @@
     <t>68517-2</t>
   </si>
   <si>
-    <t>5287d0ea-2504-426b-98e5-0897feadfa79</t>
+    <t>dbacaa4a-3e9f-4a73-a641-d03f5261c083</t>
   </si>
   <si>
     <t>Value 96842-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -564,7 +564,7 @@
     <t>96842-0</t>
   </si>
   <si>
-    <t>d6288a87-319a-4ba0-aae9-3c31f94b58fd</t>
+    <t>bf9e4a66-25d8-4d88-bc09-dcfadd6fdaa6</t>
   </si>
   <si>
     <t>Value 95530-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -573,7 +573,7 @@
     <t>95530-2</t>
   </si>
   <si>
-    <t>af423e28-16c8-4208-9d7e-d1b14886b19c</t>
+    <t>f462174b-f95a-4b3d-aa63-16169b628b43</t>
   </si>
   <si>
     <t>Value 68524-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -582,7 +582,7 @@
     <t>68524-8</t>
   </si>
   <si>
-    <t>add8073e-ee50-448f-bcba-caeea509bb59</t>
+    <t>f2214c19-c93e-484c-8d82-31bb6248fe28</t>
   </si>
   <si>
     <t>Value 44250-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -591,7 +591,7 @@
     <t>44250-9</t>
   </si>
   <si>
-    <t>430d0ec6-b2bd-4319-af77-ceb2fb29b6b5</t>
+    <t>c07a1f2c-d772-4ad5-95c5-acd15fd0f0b0</t>
   </si>
   <si>
     <t>Value 44255-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -600,7 +600,7 @@
     <t>44255-8</t>
   </si>
   <si>
-    <t>f86fd75d-68f1-4f65-98d4-85ad1a705055</t>
+    <t>02c9b12e-b2f0-457b-b606-a430a4de96ce</t>
   </si>
   <si>
     <t>Value 93038-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -609,7 +609,7 @@
     <t>93038-8</t>
   </si>
   <si>
-    <t>27a38e34-7e9c-4a9d-8b46-3a0f66dfa80f</t>
+    <t>ac93e76d-b888-45bc-8460-95f1fc0207b4</t>
   </si>
   <si>
     <t>Value 69858-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -618,7 +618,7 @@
     <t>69858-9</t>
   </si>
   <si>
-    <t>2ce4a812-4a5b-4fee-a07f-f64c7182b1ab</t>
+    <t>8d392943-b9c9-4620-a8ab-c39d477397a1</t>
   </si>
   <si>
     <t>Value 69861-3	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -627,7 +627,7 @@
     <t>69861-3	</t>
   </si>
   <si>
-    <t>bf887974-cea5-4122-b65f-29d6947295fe</t>
+    <t>d96030f5-ebc5-4866-b1ca-e7cc7e28f244</t>
   </si>
   <si>
     <t>Value false in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -642,7 +642,7 @@
     <t>Use only allowed values 'TRUE','FALSE' in NEED_INDICATED</t>
   </si>
   <si>
-    <t>4d90a8a3-5246-4185-8c0a-6756187cf40f</t>
+    <t>825e173c-be20-407d-943d-0f6cf0946aed</t>
   </si>
   <si>
     <t>Value true in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -651,82 +651,82 @@
     <t>true</t>
   </si>
   <si>
-    <t>cf4e148b-f1da-45be-b1ca-73abe4561585</t>
-  </si>
-  <si>
-    <t>bab8003d-4e2b-4b52-9888-cb71eb40bd97</t>
-  </si>
-  <si>
-    <t>044e7c46-fbb7-41f1-944a-8cad797667ba</t>
-  </si>
-  <si>
-    <t>c382f781-909b-44ef-a2ba-486f4ccecd99</t>
-  </si>
-  <si>
-    <t>cf3f64d4-3497-48a5-a75e-00b67c4604a7</t>
-  </si>
-  <si>
-    <t>45cb578d-72ff-4a27-bb94-febb4c6ebfda</t>
-  </si>
-  <si>
-    <t>bf2d7b21-3514-41d8-a4d4-0a44c2d26d1e</t>
-  </si>
-  <si>
-    <t>9e0e1dda-5d66-4246-9952-8bdcc9f5720e</t>
-  </si>
-  <si>
-    <t>29488b82-de5a-4475-acdf-9915f5d26f6d</t>
-  </si>
-  <si>
-    <t>2afe8f59-6b45-4465-8f6e-8a0955d28b71</t>
-  </si>
-  <si>
-    <t>7e285f2f-cc1d-4e10-8c84-89f2a8a49eb6</t>
-  </si>
-  <si>
-    <t>1e5788a7-4421-4505-8766-922c6df64d7f</t>
-  </si>
-  <si>
-    <t>919652f2-594d-49b5-99a5-dbd697da4dc3</t>
-  </si>
-  <si>
-    <t>e5ee3662-76c9-4043-b01f-41d44970fbf6</t>
-  </si>
-  <si>
-    <t>c3702288-392c-4b9e-bc83-f0905a91fe7a</t>
-  </si>
-  <si>
-    <t>2a7bc95d-092d-408b-a82f-4c6f71e32e2f</t>
-  </si>
-  <si>
-    <t>265d1cab-2de5-47dd-9dcd-30fd0435230f</t>
-  </si>
-  <si>
-    <t>a08be98b-48e0-490c-a003-f9b55e740b57</t>
-  </si>
-  <si>
-    <t>f1d47771-4ee3-4c3d-9ebb-aadabd797112</t>
-  </si>
-  <si>
-    <t>ab16fd50-b80e-4957-b93d-4490435b5c68</t>
-  </si>
-  <si>
-    <t>cce0f24c-f199-4a39-90f8-2710b66b54ee</t>
-  </si>
-  <si>
-    <t>ecb1e955-d8de-422a-b073-566918ec7271</t>
-  </si>
-  <si>
-    <t>05c71b51-1123-48d8-a16b-1c52219bda30</t>
-  </si>
-  <si>
-    <t>6ada8a37-9cfa-40f6-85a1-c1fb566aa03d</t>
-  </si>
-  <si>
-    <t>af4a1f0e-a433-4b8b-ad4b-dcd34c9093ed</t>
-  </si>
-  <si>
-    <t>37f181d1-ecff-4c6e-be18-917041cbc970</t>
+    <t>2ff2e79b-5026-495a-a788-10556bb4bed5</t>
+  </si>
+  <si>
+    <t>adb4df45-12b0-456b-9564-f61ebd80bc11</t>
+  </si>
+  <si>
+    <t>b6843e68-aee9-44d5-a59b-30493679b0da</t>
+  </si>
+  <si>
+    <t>e6b24b4e-79b4-4e39-a1de-1a4e539f96b0</t>
+  </si>
+  <si>
+    <t>ffe7b8af-5086-45c2-8f09-967dc11a8116</t>
+  </si>
+  <si>
+    <t>808c1cfa-74d0-4c11-a61f-846b3e4c9fbf</t>
+  </si>
+  <si>
+    <t>c652c992-a245-41af-b62f-6b1ad24834d1</t>
+  </si>
+  <si>
+    <t>775beed9-d8db-4965-9951-5a08b6f02503</t>
+  </si>
+  <si>
+    <t>829f7c13-9441-4691-a46c-5783101eddf0</t>
+  </si>
+  <si>
+    <t>9dae920a-e4c7-47dc-bf53-069d7c3f7c9b</t>
+  </si>
+  <si>
+    <t>d21fa503-a91e-4d20-a46f-cdbe72b17258</t>
+  </si>
+  <si>
+    <t>cae2f65d-211f-4654-8dee-ba9f8bd777f1</t>
+  </si>
+  <si>
+    <t>392016a0-48f7-4a0b-9590-2a8e4a38c713</t>
+  </si>
+  <si>
+    <t>5724f630-d3e7-48ba-9fb8-d5826fbc2a48</t>
+  </si>
+  <si>
+    <t>2c4c5a6e-bacc-4249-95f5-fd0ddb2a4011</t>
+  </si>
+  <si>
+    <t>2cdf5767-a6e3-4dc1-90b1-7a5cfcb781d3</t>
+  </si>
+  <si>
+    <t>29a1adce-6154-4608-bd6c-4dce8cd28dd6</t>
+  </si>
+  <si>
+    <t>e5172afe-eb3d-40dd-8030-2e340e084b57</t>
+  </si>
+  <si>
+    <t>5e2afdeb-93a5-4425-b9dc-7f669e18ee95</t>
+  </si>
+  <si>
+    <t>74a70f46-5272-4334-8474-6fcfab21619a</t>
+  </si>
+  <si>
+    <t>fcd7eae4-95da-46a9-9aaf-47d8e2a6df9c</t>
+  </si>
+  <si>
+    <t>702182dd-492e-4490-a351-37413bd08820</t>
+  </si>
+  <si>
+    <t>378727ed-fc5e-442d-a0cc-86e57ea09474</t>
+  </si>
+  <si>
+    <t>d439f196-2dae-4bf5-acf6-43073845db0e</t>
+  </si>
+  <si>
+    <t>0b1b797b-e4ff-4fc9-983b-8dac71edc54e</t>
+  </si>
+  <si>
+    <t>9b02e550-2b91-4fc8-adf2-ac84971a239d</t>
   </si>
   <si>
     <t>Value false in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -738,88 +738,88 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_PART_2_FLAG</t>
   </si>
   <si>
-    <t>2e563537-fcfb-4f21-8d88-cb5725140963</t>
-  </si>
-  <si>
-    <t>614af384-0683-4912-8265-02061509948c</t>
-  </si>
-  <si>
-    <t>76cd2aa3-adbd-422a-9251-3d5786dfb19a</t>
-  </si>
-  <si>
-    <t>45b41c4d-b49d-499b-84fa-d543bc359ed6</t>
-  </si>
-  <si>
-    <t>6ec62e95-8c78-43d5-8277-657a616be7f2</t>
-  </si>
-  <si>
-    <t>2e080b92-cfdd-4365-9117-ce3836ead048</t>
-  </si>
-  <si>
-    <t>60197b0f-13b7-4b11-a24a-f7f2358484ce</t>
-  </si>
-  <si>
-    <t>68f49ea1-d186-4c60-8972-468e3bfa5012</t>
-  </si>
-  <si>
-    <t>f9ea6d13-43a8-459e-9896-517987f16570</t>
-  </si>
-  <si>
-    <t>f3fca671-6940-450f-8bb7-5340b7675292</t>
-  </si>
-  <si>
-    <t>735afe0c-5f8a-477a-89b1-531add950992</t>
-  </si>
-  <si>
-    <t>e5d7f9fa-e0aa-401f-a6cd-66d3f0aa2f97</t>
-  </si>
-  <si>
-    <t>02cd5695-0b81-4002-b4f7-2295dc6e9cdd</t>
-  </si>
-  <si>
-    <t>77580969-4a83-467e-b459-45f9e29416aa</t>
-  </si>
-  <si>
-    <t>e012a6e3-97d5-46db-be37-5a4a0ede973d</t>
-  </si>
-  <si>
-    <t>8de7e8c2-a964-49dd-a836-9d2c2e9769f6</t>
-  </si>
-  <si>
-    <t>131865e5-c7f8-4240-a787-bc30f8a866a4</t>
-  </si>
-  <si>
-    <t>04f4825b-0865-45f2-b846-fce12dbdab41</t>
+    <t>eb347056-4d59-41bb-9e54-d9cc7f257073</t>
+  </si>
+  <si>
+    <t>be0809cc-0076-4e2f-84aa-fa3e77ae5bee</t>
+  </si>
+  <si>
+    <t>d34fcb03-ca54-4aaf-9bc1-7affd3503464</t>
+  </si>
+  <si>
+    <t>c145e52c-679c-4cb0-9a3f-bf34e55be37e</t>
+  </si>
+  <si>
+    <t>ab6e3b68-728e-4d69-9cc2-cac0a4d72bd5</t>
+  </si>
+  <si>
+    <t>0b1b5600-84a9-4078-85b8-c3e3553d8d62</t>
+  </si>
+  <si>
+    <t>c2bc8f74-ca88-4c14-80c8-f6bf93e7922c</t>
+  </si>
+  <si>
+    <t>12857e81-6043-48bf-9e81-afeb32105ba7</t>
+  </si>
+  <si>
+    <t>9c24f12a-0c14-4ea6-bd82-8b69842d55ab</t>
+  </si>
+  <si>
+    <t>e5e585df-133e-4a6d-9cbe-383f620b794e</t>
+  </si>
+  <si>
+    <t>b2e17939-92a1-45fd-ac8c-36c44548c0d2</t>
+  </si>
+  <si>
+    <t>0c7fdc8d-e733-432a-958f-554a95a6c40a</t>
+  </si>
+  <si>
+    <t>baae2602-ce3f-4b5f-b06b-390f2f4ea970</t>
+  </si>
+  <si>
+    <t>f8d3d45f-3fa6-41de-94d3-78c018a4cd72</t>
+  </si>
+  <si>
+    <t>c580b111-cd5d-4edb-9ac7-92f37e3c62ba</t>
+  </si>
+  <si>
+    <t>76eb6d1c-9769-4100-b8dd-d0427ada6716</t>
+  </si>
+  <si>
+    <t>2efb8572-4513-4b81-afb9-28d7c501a317</t>
+  </si>
+  <si>
+    <t>c24028e0-6792-4c2e-82d8-fd45a3d17bb3</t>
   </si>
   <si>
     <t>Value true in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>9c0163c5-0a1b-4ddc-9294-43f392c79aae</t>
-  </si>
-  <si>
-    <t>2e1b58cd-35f2-4144-bd44-d43e6441d201</t>
-  </si>
-  <si>
-    <t>a9b2d02c-215b-4a67-b9a6-9648fd744dee</t>
-  </si>
-  <si>
-    <t>fc92ac16-a6ab-401d-a9ae-bf8b89b018fb</t>
-  </si>
-  <si>
-    <t>ddbcf09e-a04d-46fe-b5d7-0da4ab1ef46b</t>
-  </si>
-  <si>
-    <t>ab6c3481-f11a-44bc-aa62-dcb843147356</t>
-  </si>
-  <si>
-    <t>1ffdda96-f6c8-43ea-86fe-2614548ab35d</t>
-  </si>
-  <si>
-    <t>119481ef-8eea-4b47-b85c-38311fba13e5</t>
-  </si>
-  <si>
-    <t>062fe29b-b268-484e-84a0-c76d85ff8859</t>
+    <t>5c92ac7b-2ad6-46d5-b43e-9f9eeaf36e86</t>
+  </si>
+  <si>
+    <t>099023d5-cf0b-44a6-9b70-bc8f3705d057</t>
+  </si>
+  <si>
+    <t>1220a787-4540-4ae5-8e8a-5f41582abc61</t>
+  </si>
+  <si>
+    <t>f70d3aa1-8e56-40fd-a792-3604b8e900a7</t>
+  </si>
+  <si>
+    <t>3e74cc92-7168-4636-a459-75246e54696c</t>
+  </si>
+  <si>
+    <t>aff9c1cf-1b4a-4614-ab52-da2c8904fce1</t>
+  </si>
+  <si>
+    <t>e2d0987e-f1a8-41a9-81b6-dd5fb963bfca</t>
+  </si>
+  <si>
+    <t>3546d0ce-115b-43e1-9d42-ce0c366d43f8</t>
+  </si>
+  <si>
+    <t>33de157b-f82e-4ffc-a224-f59a2283480f</t>
   </si>
   <si>
     <t>Value false in VISIT_OMH_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -831,85 +831,85 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OMH_FLAG</t>
   </si>
   <si>
-    <t>9359c697-5194-451f-b6fd-6681e1066b20</t>
-  </si>
-  <si>
-    <t>18fe52e4-be89-4438-871f-42a501af4a43</t>
-  </si>
-  <si>
-    <t>a9248ff8-dafe-448d-884e-d7547dfe6278</t>
-  </si>
-  <si>
-    <t>d642b3d9-1e09-4705-9316-2848dc0e02db</t>
-  </si>
-  <si>
-    <t>c3a432f3-25bd-4ed8-941c-efe1f3d5a5be</t>
-  </si>
-  <si>
-    <t>96732b3b-30f8-4972-9f5e-59c7d0d10bb5</t>
-  </si>
-  <si>
-    <t>c2ae1217-7ccb-40c7-81b7-c709e77f3de0</t>
-  </si>
-  <si>
-    <t>87da3459-743e-401a-b6e7-64c4bc9ac4f8</t>
-  </si>
-  <si>
-    <t>946ffeb5-e0ea-4cb5-99d8-1ad44b05eef2</t>
-  </si>
-  <si>
-    <t>75e00c72-158e-4d84-810a-6187055c53f2</t>
-  </si>
-  <si>
-    <t>eef451fa-b807-4642-91e6-7565ad20a6ff</t>
-  </si>
-  <si>
-    <t>db1e537a-128c-4689-b67b-6ca68ec65d34</t>
-  </si>
-  <si>
-    <t>8c7a1a54-3d96-4d81-ac05-28a3b3fcf2b9</t>
-  </si>
-  <si>
-    <t>1c1620fd-fb94-400d-abdd-f5935506cb15</t>
-  </si>
-  <si>
-    <t>da96a47f-3487-49ea-ab99-12cc20e01793</t>
-  </si>
-  <si>
-    <t>66f6a70e-2d61-426e-994f-46cc309d2da2</t>
-  </si>
-  <si>
-    <t>e334c185-cc60-4556-9bb3-4a77ee840b3b</t>
-  </si>
-  <si>
-    <t>61edcd67-385f-4efe-815e-1f1be1709823</t>
-  </si>
-  <si>
-    <t>66bcafa1-a2d1-4a40-bee4-f2d88b31fa21</t>
-  </si>
-  <si>
-    <t>ed79eec7-2c0b-413b-818c-68b2bca1c508</t>
-  </si>
-  <si>
-    <t>574954a7-fd2c-4e02-b238-3bf0873b0272</t>
-  </si>
-  <si>
-    <t>eceaed2c-912e-4b3c-b865-68ceb3e2ffd3</t>
-  </si>
-  <si>
-    <t>9b8e01f2-be7d-4dfb-abe1-f75a6287adbe</t>
-  </si>
-  <si>
-    <t>814e26a4-3034-4121-9295-4862c18c5923</t>
-  </si>
-  <si>
-    <t>4733c8d1-0460-4edc-bb44-136bae3b4434</t>
-  </si>
-  <si>
-    <t>730bc7c0-5fa4-4a0b-8c3b-4dae8c7b567b</t>
-  </si>
-  <si>
-    <t>f2573c3d-2ec5-4b46-9ce7-199c61188ae6</t>
+    <t>39e3d96e-e397-42cf-8197-9ab3088f06e2</t>
+  </si>
+  <si>
+    <t>fb8e69b3-1641-4814-835e-6c8ae209b2fa</t>
+  </si>
+  <si>
+    <t>d00049aa-13d9-44ed-8ff9-c6ed03e76f08</t>
+  </si>
+  <si>
+    <t>b9d80d89-41c6-40db-87f2-422a2261295f</t>
+  </si>
+  <si>
+    <t>3593da9b-cb7b-490d-b51b-9839cba729e9</t>
+  </si>
+  <si>
+    <t>9fb2c0fb-1cfb-4a14-83df-fecf625ff99d</t>
+  </si>
+  <si>
+    <t>ad2b292a-2609-461b-b3cb-8260363c7283</t>
+  </si>
+  <si>
+    <t>9835a03b-1870-474c-9b8a-0cd414a112d8</t>
+  </si>
+  <si>
+    <t>62f9a9ac-fe7d-4567-9065-817cf9386d02</t>
+  </si>
+  <si>
+    <t>6b4b8ec1-fe18-4155-8dd2-accd8d7760de</t>
+  </si>
+  <si>
+    <t>8d313083-7c1a-4313-9090-e96de515474b</t>
+  </si>
+  <si>
+    <t>a46cc82e-a06d-4180-acd7-3540f1566d7a</t>
+  </si>
+  <si>
+    <t>ae3a9df7-a317-45e3-874f-7e38b5aa443a</t>
+  </si>
+  <si>
+    <t>e47b2b79-2744-47f6-b135-97ff65e0587e</t>
+  </si>
+  <si>
+    <t>05eee909-d66e-409d-a4fb-94438deb863e</t>
+  </si>
+  <si>
+    <t>2bab5b43-fa68-4d7b-9423-ca858fa777df</t>
+  </si>
+  <si>
+    <t>46ffb8e2-b3a0-45a1-adf3-7a895b348c94</t>
+  </si>
+  <si>
+    <t>0dad54e5-4465-47d1-aef3-b5e7af7df686</t>
+  </si>
+  <si>
+    <t>0e4c8b07-877e-423f-aa3f-d068085a7e1d</t>
+  </si>
+  <si>
+    <t>cae582bc-11fc-4f8c-b3e7-086775418454</t>
+  </si>
+  <si>
+    <t>e212d33a-77a7-4a76-8cfe-e806c30cc545</t>
+  </si>
+  <si>
+    <t>f2755be5-3ed1-4ff2-8b9d-d41d11f8af81</t>
+  </si>
+  <si>
+    <t>c7059314-725a-4903-8ae9-01d367fca374</t>
+  </si>
+  <si>
+    <t>99ae1a11-0864-48b4-b942-68a38bb65677</t>
+  </si>
+  <si>
+    <t>61cacdbb-19ae-4369-8cce-a505ddec6d41</t>
+  </si>
+  <si>
+    <t>4a5b2908-c441-4413-87b4-a66d8a0b6a3b</t>
+  </si>
+  <si>
+    <t>6767f088-3e86-4b37-bfbb-347d1d42ec4f</t>
   </si>
   <si>
     <t>Value false in VISIT_OPWDD_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -921,82 +921,82 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OPWDD_FLAG</t>
   </si>
   <si>
-    <t>d2355aa9-cf0b-4fde-b0df-97af21155cb0</t>
-  </si>
-  <si>
-    <t>b347fe79-9b88-46f6-92fb-6644ad97a51d</t>
-  </si>
-  <si>
-    <t>69f1f4f9-8553-4e52-9173-5b76e7668bce</t>
-  </si>
-  <si>
-    <t>b689524c-e75d-48e4-88b1-47b630057002</t>
-  </si>
-  <si>
-    <t>5a0132c5-4b35-42c7-847c-93f34b95cb2a</t>
-  </si>
-  <si>
-    <t>1d4c2b34-ade8-4f40-86b9-2844f125f414</t>
-  </si>
-  <si>
-    <t>39ebcc4c-ae9a-4475-a245-e22cb83b7db0</t>
-  </si>
-  <si>
-    <t>6e571c6a-c0b8-469d-b9a1-a4c7b9b77b15</t>
-  </si>
-  <si>
-    <t>fe579fb7-bd95-451e-8cc9-7152230d58a8</t>
-  </si>
-  <si>
-    <t>c87b4518-d486-4fb7-8848-03841f2b3828</t>
-  </si>
-  <si>
-    <t>502348cc-e376-4985-b5e2-05b88df2bee8</t>
-  </si>
-  <si>
-    <t>bf8d626f-1b63-4843-ac51-53260251eb9c</t>
-  </si>
-  <si>
-    <t>1a0600eb-7707-4a01-abc2-19da4cc28fee</t>
-  </si>
-  <si>
-    <t>4156525f-f30a-4cee-9062-b34eb0864d05</t>
-  </si>
-  <si>
-    <t>af54cdca-2523-4c2c-ba1a-ae02417f3201</t>
-  </si>
-  <si>
-    <t>987e70c3-0748-4571-a902-fb95c57ad529</t>
-  </si>
-  <si>
-    <t>21cece03-9500-4f17-bd04-a2223b859670</t>
-  </si>
-  <si>
-    <t>e50a787c-478a-40fd-a658-939e10a06de9</t>
-  </si>
-  <si>
-    <t>93f64d9e-46e0-4c3b-a848-6f0f6ee528b9</t>
-  </si>
-  <si>
-    <t>1e46463d-9424-45b0-bfd8-9f694c471953</t>
-  </si>
-  <si>
-    <t>252371eb-ee6b-4474-8f52-7ce9fe887e79</t>
-  </si>
-  <si>
-    <t>09ee9749-ce36-422d-a2a6-056ebcbe587a</t>
-  </si>
-  <si>
-    <t>f3601d28-f4b7-4072-9019-55a40ae36fa2</t>
-  </si>
-  <si>
-    <t>75ea2350-ee7b-4094-b9ba-170bfed78fb0</t>
-  </si>
-  <si>
-    <t>7b0653ef-0a8a-439e-a3c2-32fc8a98ff5e</t>
-  </si>
-  <si>
-    <t>a67dde2e-daa3-445f-acc9-4d23f27a3e30</t>
+    <t>2aac6e1a-55c9-43fb-a545-be7ba5fdffe0</t>
+  </si>
+  <si>
+    <t>b2268d0a-8e5c-415f-ba19-0cd629d6b659</t>
+  </si>
+  <si>
+    <t>09c460ee-a072-49f2-8909-9e1c430043de</t>
+  </si>
+  <si>
+    <t>62862959-e9d6-44ce-be0c-42662c6a5597</t>
+  </si>
+  <si>
+    <t>f3649465-2355-42fb-98c2-e9a7d88eacef</t>
+  </si>
+  <si>
+    <t>7617a61c-1247-4113-9298-8ecf38179d79</t>
+  </si>
+  <si>
+    <t>fa124174-f3c9-4c9c-b6b7-d4a9f64ac9ca</t>
+  </si>
+  <si>
+    <t>c7cd7b08-ad92-445b-aba9-bd89fbe38622</t>
+  </si>
+  <si>
+    <t>672190af-fa2c-4a6c-b0c9-218850ed5fb5</t>
+  </si>
+  <si>
+    <t>80613ece-8141-4f31-88b0-6e167a50cd5c</t>
+  </si>
+  <si>
+    <t>da1216a2-df2f-4ee8-a42f-947026d94cd7</t>
+  </si>
+  <si>
+    <t>6badad3f-ffcb-4726-9e71-bddccbf68c65</t>
+  </si>
+  <si>
+    <t>c9e0a7cc-5786-465a-a7d9-be18531c6bee</t>
+  </si>
+  <si>
+    <t>8b4a0ac4-07aa-4418-8b7f-60cfac25b356</t>
+  </si>
+  <si>
+    <t>3b763901-4f41-4f06-beab-5c89713a62d1</t>
+  </si>
+  <si>
+    <t>3b146bc1-ce40-45cb-a5cf-c55347b7268b</t>
+  </si>
+  <si>
+    <t>4992ebf3-0490-477b-b778-4a171fca9da0</t>
+  </si>
+  <si>
+    <t>ca0f973a-034f-4491-b626-791a8f4f9616</t>
+  </si>
+  <si>
+    <t>3ff03cb6-1fdf-470b-ba14-6fa71a65a48a</t>
+  </si>
+  <si>
+    <t>c9ded99e-b08b-4a18-a52f-b8b4348731e3</t>
+  </si>
+  <si>
+    <t>d67e19d3-80c3-441e-bf6f-fc363c98072c</t>
+  </si>
+  <si>
+    <t>d0dced2b-f1cd-4990-8e87-dc91d6c28add</t>
+  </si>
+  <si>
+    <t>0bde1737-9115-42d5-8c34-8f5ffc0fefb0</t>
+  </si>
+  <si>
+    <t>bdceb579-2ec7-4374-ad80-9844a8451a7e</t>
+  </si>
+  <si>
+    <t>cc41a941-018f-4931-9215-e5f0ed18270a</t>
+  </si>
+  <si>
+    <t>d5cc9da3-3fb6-4a07-b2d3-bdade7cd7f55</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -1005,7 +1005,7 @@
     <t>ahc_hrsn_2023_12_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>9468d4bd-a6e4-463b-b373-2762f829789e</t>
+    <t>7b6ea772-075e-4e78-8bc7-81aa18bb1b9e</t>
   </si>
   <si>
     <t>Pattern Mismatch</t>
@@ -1023,7 +1023,7 @@
     <t>Follow the pattern ^[A-Za-z]+$ in FIRST_NAME</t>
   </si>
   <si>
-    <t>31a41940-c446-4d4f-bb0f-17faffa1b039</t>
+    <t>d289c162-88c7-4ab4-8163-482b4fd5cfdc</t>
   </si>
   <si>
     <t>Value Patient Matching  in MIDDLE_NAME does not match the pattern ^[A-Za-z]+$</t>
@@ -1035,7 +1035,7 @@
     <t>Follow the pattern ^[A-Za-z]+$ in MIDDLE_NAME</t>
   </si>
   <si>
-    <t>ccecfba9-a510-49dc-ab66-0c90611c7b7d</t>
+    <t>fcb93c5f-43fe-4ce0-af51-b46ca63cc78e</t>
   </si>
   <si>
     <t>Value Patient Matching  in LAST_NAME does not match the pattern ^[A-Za-z]+$</t>
@@ -1053,7 +1053,7 @@
     <t>ahc_hrsn_2023_12_25_valid_screening</t>
   </si>
   <si>
-    <t>0787946b-b290-4eae-a7bf-112411043a52</t>
+    <t>9e414cb5-89d0-401b-9cb2-15af4cb79f0e</t>
   </si>
   <si>
     <t>Data Type Mismatch</t>
@@ -1071,7 +1071,7 @@
     <t>Convert non-integer values to INTEGER</t>
   </si>
   <si>
-    <t>55bf3ada-8238-4f18-a4eb-7bef9d281c66</t>
+    <t>80450310-4fce-4af2-907d-1876d8ff71fb</t>
   </si>
   <si>
     <t>Non-integer value "Yes" found in PAT_MRN_ID</t>
@@ -1080,7 +1080,7 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>089a47fd-b15e-4875-ae7a-8458f6813756</t>
+    <t>9289d862-432a-4fec-95fe-24d4309e346a</t>
   </si>
   <si>
     <t>Non-integer value "Facility" found in PAT_MRN_ID</t>
@@ -1089,7 +1089,7 @@
     <t>Facility</t>
   </si>
   <si>
-    <t>ec00b467-27ab-4aae-9aec-6a2edfa33352</t>
+    <t>d80f9215-778d-44aa-a470-f77164780a50</t>
   </si>
   <si>
     <t>Value Screening in SCREENING_METHOD not in allowed list ('In-Person', 'Phone', 'Website')</t>
@@ -1104,7 +1104,7 @@
     <t>Use only allowed values 'In-Person', 'Phone', 'Website' in SCREENING_METHOD</t>
   </si>
   <si>
-    <t>48eee97d-cb4a-4100-b3ce-bd0759b37f68</t>
+    <t>95717368-0f70-4abb-9aa6-fb0f89a0596f</t>
   </si>
   <si>
     <t>Value No in SCREENING_METHOD not in allowed list ('In-Person', 'Phone', 'Website')</t>
@@ -1113,13 +1113,13 @@
     <t>No</t>
   </si>
   <si>
-    <t>5dcf2909-c634-4667-88d9-fbbdd9ea1477</t>
+    <t>b93eb165-eaaa-4275-8d41-743399c60893</t>
   </si>
   <si>
     <t>Value Facility in SCREENING_METHOD not in allowed list ('In-Person', 'Phone', 'Website')</t>
   </si>
   <si>
-    <t>d76b78eb-d832-49f6-a763-91cd9d9d4a70</t>
+    <t>9f26fe4b-6ae5-43a2-baad-2bd092dc0fb9</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -1134,19 +1134,19 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>c1f19154-04bd-43a0-b27b-5bf4c624fb43</t>
+    <t>70a264c8-16bf-4fb0-98e6-c2c7a026766c</t>
   </si>
   <si>
     <t>Invalid timestamp "Yes" found in RECORDED_TIME</t>
   </si>
   <si>
-    <t>2be0b2b1-d08e-4043-b4e6-f1c1599a4e4d</t>
+    <t>e223054c-d42b-41e5-b1f4-761813ec71c1</t>
   </si>
   <si>
     <t>Invalid timestamp "Facility" found in RECORDED_TIME</t>
   </si>
   <si>
-    <t>843c79e7-8251-47ca-8dd5-0923ae05b0f0</t>
+    <t>a9590e1f-8bd0-448d-8037-6ed42458e6dc</t>
   </si>
   <si>
     <t>Value Screening in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
@@ -1155,13 +1155,13 @@
     <t>Use only allowed values '71802-3', '96778-6' in QUESTION_CODE</t>
   </si>
   <si>
-    <t>d2861e19-3e95-4fc9-87a3-cb5e936fb899</t>
+    <t>dbe96a4b-4612-4dd6-9df7-8ebf948382d2</t>
   </si>
   <si>
     <t>Value Yes in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>a7a2bc69-7bac-4457-91ed-c54283cc5f22</t>
+    <t>93e855ad-4af2-42b0-82ab-ffbaee40fe4b</t>
   </si>
   <si>
     <t>Value Facility/QE in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
@@ -1170,61 +1170,61 @@
     <t>Facility/QE</t>
   </si>
   <si>
-    <t>59929260-efdd-4254-b787-dff0a0096d5a</t>
+    <t>486e687b-ab65-466f-acbd-795bf967b33c</t>
   </si>
   <si>
     <t>Value 96778-6	 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>15a63c61-c12f-4df0-986a-380dfb0bb96e</t>
+    <t>2afd2868-fceb-4d75-8328-463250ed3976</t>
   </si>
   <si>
     <t>Value 88122-7 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>15ed3f8b-6150-424e-bcfd-693cd0c0fb71</t>
+    <t>ee82235e-0713-4fe7-b8cb-8f1fca6f6b46</t>
   </si>
   <si>
     <t>Value 88123-5 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>13f93424-eb06-4af7-8dc8-c165d2c36d9b</t>
+    <t>b5754f66-da15-47b9-a321-aff10a85d3f3</t>
   </si>
   <si>
     <t>Value 93030-5 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>1f08feca-977f-4786-a34a-8290b41da028</t>
+    <t>e3cc255c-fb5b-46fd-bfca-811092888bf4</t>
   </si>
   <si>
     <t>Value 96779-4 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>dcfbd318-e110-41cf-aacb-ac82ed2e42a9</t>
+    <t>9a47ec91-b693-4507-a125-03fe873f243b</t>
   </si>
   <si>
     <t>Value 95618-5 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>27e0930f-1cbc-41d9-886e-d32fc7a5907c</t>
+    <t>9df6c211-2e81-4acb-a7af-fa173006a569</t>
   </si>
   <si>
     <t>Value 95617-7 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>2285e352-c651-4b1c-ad2e-33a5bf9f5c1f</t>
+    <t>61963aa7-c82f-438a-8376-b9d53568d472</t>
   </si>
   <si>
     <t>Value 95616-9 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>34436dcb-25f0-45a3-bd55-6695074cb6a1</t>
+    <t>be980d3f-1776-44a6-8103-bf2c66629d8f</t>
   </si>
   <si>
     <t>Value 95615-1 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>41f2c79e-2cae-474d-bc22-4e4bc30079f3</t>
+    <t>3c380d90-2b54-40ee-b4e6-9803176e51ac</t>
   </si>
   <si>
     <t>Value 95614-4 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
@@ -1233,190 +1233,190 @@
     <t>95614-4</t>
   </si>
   <si>
-    <t>4453742d-5c2f-49ef-91cf-a9ae6649fdfa</t>
+    <t>269b710a-3c2a-4f7e-8948-7521e5df8cfb</t>
   </si>
   <si>
     <t>Value 76513-1 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>7afa44bc-89dc-4db6-b8bb-7ff91b242af1</t>
+    <t>bdd5b648-2699-4bbf-adc3-275c94939770</t>
   </si>
   <si>
     <t>Value 96780-2 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>9d2b7104-7fcf-4468-ab29-1fb866a02423</t>
+    <t>935ff2be-de81-4f8d-a0d3-8bd1804b0bde</t>
   </si>
   <si>
     <t>Value 96781-0 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>8e91ef71-cd8a-4d85-a46a-b776a15c577a</t>
+    <t>003b0905-63a6-4889-9526-e3f73f808629</t>
   </si>
   <si>
     <t>Value 93159-2	 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>01142220-1cc6-47fb-8844-c8e82b518242</t>
+    <t>a6c59902-9315-4dea-a61c-f654d9778546</t>
   </si>
   <si>
     <t>Value 97027-7 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>d5bb0aa5-2697-4947-9b96-4c1d6371c76e</t>
+    <t>e78b5157-aebe-49d3-bf56-40aa497163c7</t>
   </si>
   <si>
     <t>Value 96782-8	 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>b6f535b3-b4d6-446a-b0f2-e9b7a19c98e8</t>
+    <t>799974d9-86f0-44e8-a69a-172f23ad2f64</t>
   </si>
   <si>
     <t>Value 89555-7 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>2b78030a-6c26-473d-8f3c-5adff2bb6914</t>
+    <t>fd0bae23-326e-4c11-b4d4-56b68dc969a7</t>
   </si>
   <si>
     <t>Value 68516-4	 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>08dba4f9-d56b-469a-8628-26821207d2aa</t>
+    <t>6f338164-fd41-4f05-a7a0-f7369d31a1af</t>
   </si>
   <si>
     <t>Value 68517-2 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>b104235f-d01b-45aa-8273-6fe2f3ccf6b0</t>
+    <t>c58bb00d-040e-4ab3-8ebc-84cf7ef62477</t>
   </si>
   <si>
     <t>Value 96842-0 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>af6907e8-a664-4d7d-b483-2bb4b2f9c814</t>
+    <t>3fad102d-9fc8-48f9-8bfb-ff5189cb54ec</t>
   </si>
   <si>
     <t>Value 95530-2 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>6f6ee060-7f26-4b56-ab9d-bc46c900b037</t>
+    <t>567a74ae-5d17-4f8c-8feb-c650241bee7b</t>
   </si>
   <si>
     <t>Value 68524-8 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>3fcf7bc3-9257-4701-b901-f04ad089bbf7</t>
+    <t>fb1e7730-8c22-4e47-b441-df9fea431d60</t>
   </si>
   <si>
     <t>Value 44250-9 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>2dea9444-6bf9-4536-b595-87137539a436</t>
+    <t>b6b6b4b9-956d-4094-850e-fecf8a6b8614</t>
   </si>
   <si>
     <t>Value 44255-8 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>0340dd98-194d-4744-85b9-d619299efe19</t>
+    <t>02135fa6-cd59-4d68-bcb6-3d3d381da1e2</t>
   </si>
   <si>
     <t>Value 93038-8 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>06ecbb4c-06e0-4093-a68e-a02b3b222cd1</t>
+    <t>9d411f92-0ac7-454f-a6f0-cd1073de8b0e</t>
   </si>
   <si>
     <t>Value 69858-9 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>7d30e380-1a89-4852-b5b2-1bbbf509f6f8</t>
+    <t>0584381c-135c-48a1-8b89-78f23aa45795</t>
   </si>
   <si>
     <t>Value 69861-3	 in QUESTION_CODE not in allowed list ('71802-3', '96778-6')</t>
   </si>
   <si>
-    <t>38974086-003c-4a9f-a588-598e2720250a</t>
-  </si>
-  <si>
-    <t>d3977c66-6650-45e8-8445-dc5077f8d66c</t>
-  </si>
-  <si>
-    <t>3f717cc9-5f90-48e6-9214-6a0dbd625496</t>
-  </si>
-  <si>
-    <t>ca5192b3-ba90-4587-ae4e-1476934e4e7f</t>
-  </si>
-  <si>
-    <t>067708b7-5c28-48d4-a175-431fbc0114b5</t>
-  </si>
-  <si>
-    <t>03d8759f-7d96-4199-a836-dff1fc3fa078</t>
-  </si>
-  <si>
-    <t>f2a4ab72-905e-46be-9404-23c6412262a4</t>
-  </si>
-  <si>
-    <t>7135fa6e-691a-49d6-aa7f-fe49ea4bc4a3</t>
-  </si>
-  <si>
-    <t>00efcf47-e6c6-43af-bac1-748dd1f1848c</t>
-  </si>
-  <si>
-    <t>3d5d6f6b-5800-47f5-8dff-5d80573e2005</t>
-  </si>
-  <si>
-    <t>f2eb2899-130d-4623-917e-514b4d057840</t>
-  </si>
-  <si>
-    <t>f90d6fd4-5933-4bbb-a789-d6c346bda0f5</t>
-  </si>
-  <si>
-    <t>6303b2d6-4462-42de-b88a-911cdfcf59a4</t>
-  </si>
-  <si>
-    <t>f637cba2-ddd6-49d5-b14b-5cc56e0857ea</t>
-  </si>
-  <si>
-    <t>72ef73c1-0e0d-4bca-8cbd-d934d33b9167</t>
-  </si>
-  <si>
-    <t>ddbbfa3e-fe17-4dc4-9dff-197e61faeb13</t>
-  </si>
-  <si>
-    <t>3318ffc1-bb4c-4c8e-ac13-b668c68f45f6</t>
-  </si>
-  <si>
-    <t>89b92e17-8a79-4e75-a95c-f17ac0634af5</t>
-  </si>
-  <si>
-    <t>aa47561d-77c0-43d4-84d7-12c86ee9833d</t>
-  </si>
-  <si>
-    <t>8b3a2e22-98a8-4a43-8992-7ab2f245983b</t>
-  </si>
-  <si>
-    <t>9d3c8bc5-2938-4bf7-8d60-07c8c17a1992</t>
-  </si>
-  <si>
-    <t>76386d24-6b85-48d5-b1ae-babbc9256a67</t>
-  </si>
-  <si>
-    <t>98e0b775-fff0-4cf2-a19b-3747adfb81fc</t>
-  </si>
-  <si>
-    <t>189c855b-f0a1-4e45-8f34-899e9fd3202c</t>
-  </si>
-  <si>
-    <t>0d1d3512-bc67-4749-9125-e3220fdfbdde</t>
-  </si>
-  <si>
-    <t>1a3e5e02-d417-45f2-a0d7-cb9489bca1a8</t>
-  </si>
-  <si>
-    <t>4066648a-75c4-4dce-bd93-31f9bd95c989</t>
-  </si>
-  <si>
-    <t>0c7c3860-57ed-4f01-8c35-3a1ec46c2419</t>
+    <t>26527bc0-ea4d-4e61-99a3-39a7d12ec03d</t>
+  </si>
+  <si>
+    <t>e29714d0-9ca0-40b4-a609-9bf5537e37e8</t>
+  </si>
+  <si>
+    <t>6d92b61f-0911-434d-8c8a-2f3e4f4ca623</t>
+  </si>
+  <si>
+    <t>a744a2f7-4cc5-45c0-b96a-0838f5a95009</t>
+  </si>
+  <si>
+    <t>b6c801d7-475d-4ba9-8c95-552414529739</t>
+  </si>
+  <si>
+    <t>76caaaf6-4aeb-4ecc-8f7d-dd899d0ec400</t>
+  </si>
+  <si>
+    <t>f309aeaa-b5b0-42a6-8e84-5257331ccad6</t>
+  </si>
+  <si>
+    <t>09829048-c39b-4512-87f8-06b5493ce96c</t>
+  </si>
+  <si>
+    <t>b1c389d7-4e7f-4bfb-a5ae-190be865e111</t>
+  </si>
+  <si>
+    <t>61817c5e-dc31-49df-b338-8623b779807a</t>
+  </si>
+  <si>
+    <t>d9b4affe-dfe7-455c-ae84-17701165bf8e</t>
+  </si>
+  <si>
+    <t>f477e1c9-3ecc-4b91-b7d9-84ea741aa48e</t>
+  </si>
+  <si>
+    <t>3cc0f3ad-7d69-4a5d-bdef-940a835759fc</t>
+  </si>
+  <si>
+    <t>994ae494-7ef0-4147-b1a2-7ea6bb584b52</t>
+  </si>
+  <si>
+    <t>241bc2cd-6cc0-4a10-8097-6e86936d8f7c</t>
+  </si>
+  <si>
+    <t>639efdd8-a959-425b-bcec-af6dd743d7d7</t>
+  </si>
+  <si>
+    <t>beb346f6-c7b0-4b92-86aa-1c8db99636c3</t>
+  </si>
+  <si>
+    <t>699e8072-84a6-4892-98b7-5749f0038cce</t>
+  </si>
+  <si>
+    <t>45f6f853-c020-4827-8f92-6f1517623085</t>
+  </si>
+  <si>
+    <t>41bfb1fe-3245-47f4-9e90-7f7ee1d8c53f</t>
+  </si>
+  <si>
+    <t>16c80db3-91de-4372-9f1a-e90a3a6dcc66</t>
+  </si>
+  <si>
+    <t>4133b511-4e28-4080-9aa7-da767d5d1486</t>
+  </si>
+  <si>
+    <t>a3e41537-9533-473a-af72-1b800cee28cd</t>
+  </si>
+  <si>
+    <t>98644b15-7445-4d77-844e-06a9a3ec4d53</t>
+  </si>
+  <si>
+    <t>4051d474-e3aa-4749-ba0b-ed50cce9b2c9</t>
+  </si>
+  <si>
+    <t>a4cc7951-f97b-4dd1-9180-b3fc92fa8e50</t>
+  </si>
+  <si>
+    <t>be05b189-6097-46f6-87a2-123e4444bf0a</t>
+  </si>
+  <si>
+    <t>7a3deb48-1484-475c-8455-75d72f0324b6</t>
   </si>
   <si>
     <t>Value Screening in QUESTION_CODE_SYSTEM_NAME not in allowed list ('LN','LOIN')</t>
@@ -1428,19 +1428,19 @@
     <t>Use only allowed values 'LN','LOIN' in QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>88e84388-2375-43fd-8065-7cf49bb6cef5</t>
+    <t>0275e681-7d5b-4514-88b8-88e09d9bc82c</t>
   </si>
   <si>
     <t>Value Yes in QUESTION_CODE_SYSTEM_NAME not in allowed list ('LN','LOIN')</t>
   </si>
   <si>
-    <t>798c3b45-c9c0-4720-bff1-85c8a91b4840</t>
+    <t>a3c1003b-eedf-42f8-b5bc-f5dddae2c34a</t>
   </si>
   <si>
     <t>Value Facility/QE in QUESTION_CODE_SYSTEM_NAME not in allowed list ('LN','LOIN')</t>
   </si>
   <si>
-    <t>41f1eb79-8125-490d-a205-4068b5968414</t>
+    <t>d34cd608-74e7-4592-9090-aa35695c4f80</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -1455,10 +1455,10 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>27842d2c-88e5-4f54-99b4-f93cadb4cfaf</t>
-  </si>
-  <si>
-    <t>7b96e2fe-7770-45de-a7f7-7d15e8cd50aa</t>
+    <t>e1ac50f9-a3ea-4062-b4d0-26226655bc9f</t>
+  </si>
+  <si>
+    <t>94df092a-d6f0-4049-ba53-294cbde3d4b5</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -1470,10 +1470,10 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>cc6262ec-5f48-421e-a7c0-e60bc2250f55</t>
-  </si>
-  <si>
-    <t>1626d0f7-b2a1-4581-8d43-8e62b6ca3f57</t>
+    <t>dd8a3d35-8116-4d65-84ab-fd3f452923e6</t>
+  </si>
+  <si>
+    <t>929bec7b-2738-41a6-b27d-ea5e66c4fdf9</t>
   </si>
   <si>
     <t>Value Screening in ANSWER_CODE_SYSTEM_NAME not in allowed list ('LN','LOIN')</t>
@@ -1482,19 +1482,19 @@
     <t>Use only allowed values 'LN','LOIN' in ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>3be429de-9f40-47a1-a6cd-e8c990276af2</t>
+    <t>ff05ffa2-842d-482c-982c-c68171029d85</t>
   </si>
   <si>
     <t>Value Yes in ANSWER_CODE_SYSTEM_NAME not in allowed list ('LN','LOIN')</t>
   </si>
   <si>
-    <t>22992dbd-aeff-47bc-be10-803b4d6a097a</t>
+    <t>e8d7b4e9-bfe0-4f65-9f23-a9ceb36dc099</t>
   </si>
   <si>
     <t>Value Facility/QE in ANSWER_CODE_SYSTEM_NAME not in allowed list ('LN','LOIN')</t>
   </si>
   <si>
-    <t>35533f91-1a3d-4971-9bb9-b2f87bd7815f</t>
+    <t>aa5b1603-1ec6-49b1-bf32-f205cb3bda9b</t>
   </si>
   <si>
     <t>Mandatory field PARENT_QUESTION_CODE is empty</t>
@@ -1506,10 +1506,10 @@
     <t>Provide a value for PARENT_QUESTION_CODE</t>
   </si>
   <si>
-    <t>bb26c0fd-f139-487e-8405-6d7bca18df94</t>
-  </si>
-  <si>
-    <t>c8387961-4014-438c-9671-1afb771de60f</t>
+    <t>af92d2a3-5a3a-44b2-911a-653a7469b51c</t>
+  </si>
+  <si>
+    <t>d80b476c-ab30-4138-9428-7b16db04c251</t>
   </si>
   <si>
     <t>Value Screening in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
@@ -1518,19 +1518,19 @@
     <t>Use only allowed values '88122-7','88123-5' in PARENT_QUESTION_CODE</t>
   </si>
   <si>
-    <t>c3dbb954-40cb-4c3c-8a41-c1476f4c5ace</t>
+    <t>fc0a05b4-250b-4290-961d-ea66e3294773</t>
   </si>
   <si>
     <t>Value No in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>98a25f99-427c-4b05-b189-061c346d97a0</t>
+    <t>3f690bb4-3ba8-4274-9736-d277a446565a</t>
   </si>
   <si>
     <t>Value Facility/QE in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>7f749451-1759-4cff-b9d1-7a443d10e4d1</t>
+    <t>f6220339-fa4a-4461-8a72-f985fe2f2a7d</t>
   </si>
   <si>
     <t>Value 71802-3 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
@@ -1539,226 +1539,226 @@
     <t>71802-3</t>
   </si>
   <si>
-    <t>780e22d5-37c7-4118-8dc8-95affad6d30b</t>
+    <t>b15639f9-42bd-48ab-b45a-db89ae15f694</t>
   </si>
   <si>
     <t>Value 96778-6	 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>660d94ef-eff2-47c5-906f-a73e71665bbb</t>
+    <t>cc569f34-9171-4edc-804c-5e61fc91b587</t>
   </si>
   <si>
     <t>Value 93030-5 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>969ec130-f7ec-40c1-9d00-dfd1773e32be</t>
+    <t>e903ec20-cd4c-40fb-abab-029ebc8df7ac</t>
   </si>
   <si>
     <t>Value 96779-4 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>318a2853-1a14-4362-beec-a9f7fc024d06</t>
+    <t>39d8d0de-642e-4e04-a7ab-1aed5b5dd15e</t>
   </si>
   <si>
     <t>Value 95618-5 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>ea6b21ff-2f94-4104-922d-c02e1b21c8c5</t>
+    <t>e83a93d2-262b-4895-a0d0-8123884cba39</t>
   </si>
   <si>
     <t>Value 95617-7 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>72cd8006-8cef-4849-a7c2-d9945dbbed30</t>
+    <t>206d69fe-d9f3-4c10-95c1-84dddd347f9c</t>
   </si>
   <si>
     <t>Value 95616-9 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>99809c24-92b5-488d-9648-34d224b553c2</t>
+    <t>a9fbffd5-ea28-43f9-9fdd-7768a86c9b58</t>
   </si>
   <si>
     <t>Value 95615-1 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>bd599d26-2bc9-47d6-a8dc-ae19a6800f73</t>
+    <t>4c839d9f-1aac-4a65-9305-ce1d3c246747</t>
   </si>
   <si>
     <t>Value 76513-1 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>0f617441-1c78-4224-9192-09e03a4b6271</t>
+    <t>efb1a0d8-1bed-40ee-b51d-047996ba8eb3</t>
   </si>
   <si>
     <t>Value 96780-2 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>a2616ff5-acee-4212-8108-821407c8942a</t>
+    <t>37230072-0756-48b9-a339-ffec29646a69</t>
   </si>
   <si>
     <t>Value 96781-0 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>6bfaa509-21a0-4733-928d-b203dbaaca24</t>
+    <t>2b9f3efe-ba01-4021-8fe3-6cc81b080800</t>
   </si>
   <si>
     <t>Value 93159-2	 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>5fb5ae66-7525-4ffa-90a4-57e0c323d737</t>
+    <t>871f4486-f562-4bc8-932a-929e8dc0f3d4</t>
   </si>
   <si>
     <t>Value 97027-7 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>38e29654-2611-4932-8c1d-ee3639238ba0</t>
+    <t>d39eca02-2d38-43c0-9e9c-21b1a79029f6</t>
   </si>
   <si>
     <t>Value 96782-8	 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>b7c6017a-e853-4140-a87c-562fd0c45c9d</t>
+    <t>24d04094-3a7b-4e96-a231-294d28b539d1</t>
   </si>
   <si>
     <t>Value 89555-7 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>f1afac95-7d4f-4c83-bbc3-9ff3c731bdc8</t>
+    <t>5c427365-724a-45b4-b0b1-322152cdda13</t>
   </si>
   <si>
     <t>Value 68516-4	 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>c65f1f19-3d7c-4a6b-99ab-a7c0f111120d</t>
+    <t>3b838dd5-9042-456b-8c98-295c297c2a59</t>
   </si>
   <si>
     <t>Value 68517-2 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>e23c33e4-54bc-4283-b8b9-c6b63f5bcb2c</t>
+    <t>fc6dce9f-a52c-4ed6-94a9-cf2d3deda2ff</t>
   </si>
   <si>
     <t>Value 96842-0 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>0a7f3000-b7be-4c5b-b687-95dc409bd765</t>
+    <t>5e9d41f2-8333-4a6d-bc93-c457bed32f1a</t>
   </si>
   <si>
     <t>Value 95530-2 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>dcc94009-8bbf-46cd-9f1b-c30c884c893f</t>
+    <t>aa072d38-7e7f-4e71-a6f5-d1f3eeeb374d</t>
   </si>
   <si>
     <t>Value 68524-8 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>5654ad50-b284-448d-9c19-14048d775580</t>
+    <t>1ab02f42-e864-42d6-879a-d1f1f93f1c91</t>
   </si>
   <si>
     <t>Value 44250-9 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>b99061af-3dbb-4760-82d0-e01597c075b5</t>
+    <t>8a5426ab-b0df-4c3c-9ca7-306ed959343e</t>
   </si>
   <si>
     <t>Value 44255-8 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>b9f47b72-b1d6-43c5-9c00-15b0ef6ba93c</t>
+    <t>30cda042-fd1f-4fef-8b55-45362f924d10</t>
   </si>
   <si>
     <t>Value 93038-8 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>cf12733a-ed00-40b9-ab33-60c97b6bfbbb</t>
+    <t>c8340905-2e8e-4fb6-8c8d-71d06b26d082</t>
   </si>
   <si>
     <t>Value 69858-9 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>6540323b-69e3-4153-80d4-753136c90075</t>
+    <t>e452d24e-a2db-46fd-ab69-bd584aa4429e</t>
   </si>
   <si>
     <t>Value 69861-3	 in PARENT_QUESTION_CODE not in allowed list ('88122-7','88123-5')</t>
   </si>
   <si>
-    <t>a744c497-a788-41fa-9d31-6cf3194bc427</t>
-  </si>
-  <si>
-    <t>d61811c1-4f38-4189-b4a0-2ce50d29e790</t>
-  </si>
-  <si>
-    <t>7220137c-4fd9-4387-8865-8c15a99c8470</t>
-  </si>
-  <si>
-    <t>f9fb8daa-290c-4035-ac6e-7c675ec49ae1</t>
-  </si>
-  <si>
-    <t>1729eaf8-1c30-4b49-8c9f-4b10c8b6e505</t>
-  </si>
-  <si>
-    <t>690f1eec-c4c9-48f3-a942-efa7b851918b</t>
-  </si>
-  <si>
-    <t>dd680062-9271-4ab4-82e2-30102fa39377</t>
-  </si>
-  <si>
-    <t>e4f37e83-8fcb-4741-a592-e81fe3dc5a73</t>
-  </si>
-  <si>
-    <t>0284fb57-be05-4e78-92d4-6e3ccf2b87bd</t>
-  </si>
-  <si>
-    <t>a1046dd4-64df-4b40-b901-83402c75ddb0</t>
-  </si>
-  <si>
-    <t>a16cf83e-ad1d-488e-8d63-76d5aa5cc425</t>
-  </si>
-  <si>
-    <t>fbc1d3dc-0271-4118-be18-42d75850c95b</t>
-  </si>
-  <si>
-    <t>a82fd1ac-d07d-4ef7-85fe-27fc9ceba83d</t>
-  </si>
-  <si>
-    <t>602b6680-dadb-4042-9f9c-5b06e07bb835</t>
-  </si>
-  <si>
-    <t>2f1c687e-06d3-4d5f-af4d-d94d3559fb7e</t>
-  </si>
-  <si>
-    <t>6070a1c5-16a4-446d-bde8-3831f5936ef2</t>
-  </si>
-  <si>
-    <t>36502c90-642d-4094-9c8c-c9d5face7eb0</t>
-  </si>
-  <si>
-    <t>e5f563d5-a444-41d6-a3b5-c796ed9ecd47</t>
-  </si>
-  <si>
-    <t>8c7661a0-7640-4898-b815-f064d6e09bc5</t>
-  </si>
-  <si>
-    <t>b141d58e-6cb8-4a11-a096-a94d76b19378</t>
-  </si>
-  <si>
-    <t>9a7b65af-bbdd-480b-a78e-62413b07590e</t>
-  </si>
-  <si>
-    <t>67ab8f69-6f2f-4da8-9a92-24f552149cc8</t>
-  </si>
-  <si>
-    <t>bff20af7-4941-4966-992f-6b53876f546b</t>
-  </si>
-  <si>
-    <t>95c6037c-1187-43c6-b7a2-392661ad04ca</t>
-  </si>
-  <si>
-    <t>8b411dbe-dc7d-4505-bb8c-3dfb6342c885</t>
-  </si>
-  <si>
-    <t>832920fe-443e-477b-8ee9-ad5cb2da9d02</t>
+    <t>332d4ce6-47f1-4b2a-a786-a113f4b20c05</t>
+  </si>
+  <si>
+    <t>f515c1cb-e445-49af-84c8-ae9177f29fce</t>
+  </si>
+  <si>
+    <t>06a0648b-f27d-4f71-8cc8-58dc14892334</t>
+  </si>
+  <si>
+    <t>62f0d5d7-46f3-424b-8c57-731061d9da9f</t>
+  </si>
+  <si>
+    <t>34c822f1-9c72-45c8-95fd-d21acfeec01c</t>
+  </si>
+  <si>
+    <t>e3272ec3-98d9-4264-8980-bd1bcfdd9fcd</t>
+  </si>
+  <si>
+    <t>9655c471-e0f1-4747-814e-dee7768e9eee</t>
+  </si>
+  <si>
+    <t>05553a12-ef69-4b17-a52e-d8c7b2e02a1f</t>
+  </si>
+  <si>
+    <t>a48e6d54-6d74-4b36-bdb1-80e31660624e</t>
+  </si>
+  <si>
+    <t>b5ee5d32-7aad-49ec-ab9e-f6622594a0d7</t>
+  </si>
+  <si>
+    <t>2938c9c7-7d8a-4861-ba7e-451b1097dc84</t>
+  </si>
+  <si>
+    <t>a5274b07-6941-494b-b5dc-d3ff11de1fb3</t>
+  </si>
+  <si>
+    <t>8036c1c8-0600-4c10-a44d-c53de09da85c</t>
+  </si>
+  <si>
+    <t>dcaa8eb9-7fe3-48b3-9145-5e48e59baaee</t>
+  </si>
+  <si>
+    <t>4c632b19-99a9-4fc4-8f81-47d08ad4387d</t>
+  </si>
+  <si>
+    <t>31eca3a0-d7e5-4592-a405-2c566a63d283</t>
+  </si>
+  <si>
+    <t>f0f03ba7-3950-4646-9d94-0eb70fb57743</t>
+  </si>
+  <si>
+    <t>476c1979-f51d-4055-a546-8c4f8a4afe98</t>
+  </si>
+  <si>
+    <t>1f19653f-b182-4da9-96fb-f2131512c23f</t>
+  </si>
+  <si>
+    <t>fea14bdf-f2cb-4c9d-8754-bef036c97092</t>
+  </si>
+  <si>
+    <t>45a4af2e-90b0-49ff-bb9f-1e0fc8b5c681</t>
+  </si>
+  <si>
+    <t>89cab61b-ed63-4b7a-b8bd-f8ef63c26638</t>
+  </si>
+  <si>
+    <t>354ae5c5-5aa2-4628-98d3-bad14f0de63f</t>
+  </si>
+  <si>
+    <t>8deaa94c-5cd1-4ea3-8d5a-b7d1bfd98793</t>
+  </si>
+  <si>
+    <t>e23f3234-0dfe-4c01-a6b0-360907be281c</t>
+  </si>
+  <si>
+    <t>395328cf-283d-44a1-a234-1458fca6ccb4</t>
   </si>
   <si>
     <t>Mandatory field SDOH_DOMAIN is empty</t>
@@ -1770,7 +1770,7 @@
     <t>Provide a value for SDOH_DOMAIN</t>
   </si>
   <si>
-    <t>2cd2d72b-0217-4b97-be6d-55de97c0972b</t>
+    <t>2240535e-78cf-49ed-ad64-557b2eaf1d8d</t>
   </si>
   <si>
     <t>Mandatory field POTENTIAL_NEED_INDICATED is empty</t>
@@ -1782,13 +1782,13 @@
     <t>Provide a value for POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>eb43c3db-11d9-4553-b1bd-f8c65572b261</t>
-  </si>
-  <si>
-    <t>c1905e12-a7db-4be5-8298-c083608a5cdc</t>
-  </si>
-  <si>
-    <t>55c7f555-10d7-492e-afdf-3c8d70e93585</t>
+    <t>1957cb6e-3382-4ea6-8a9b-6308051fe741</t>
+  </si>
+  <si>
+    <t>b5acc5d0-d75f-4e84-a2e2-9bcbd73f328c</t>
+  </si>
+  <si>
+    <t>d49e92ab-d9a1-4bea-92ca-d59a21c2ad3c</t>
   </si>
   <si>
     <t>Value Screening in POTENTIAL_NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -1797,121 +1797,121 @@
     <t>Use only allowed values 'TRUE','FALSE' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>308c3240-ee8f-4851-92a1-997057487d4e</t>
+    <t>f741253a-4837-4e9e-835e-bc2837cb84ed</t>
   </si>
   <si>
     <t>Value Yes in POTENTIAL_NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>eef0b629-9eb0-4165-a961-351d3e980fb2</t>
+    <t>7adfe1fb-afee-435f-bc2f-86b8ca2a6d1a</t>
   </si>
   <si>
     <t>Value Facility/QE in POTENTIAL_NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>de4367de-45a7-4885-b08e-a5fe6f775260</t>
+    <t>de3a92fb-f702-4ff5-8cfd-72cd6b1ec2f6</t>
   </si>
   <si>
     <t>Value No in POTENTIAL_NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>12f6e5f6-487a-449b-93f2-6835e02355ba</t>
-  </si>
-  <si>
-    <t>de2ad364-cdb0-4aa2-a01e-3307d0e6df5c</t>
-  </si>
-  <si>
-    <t>9eb0e6a5-7d3f-4ab8-af0b-eea83959a739</t>
-  </si>
-  <si>
-    <t>b5c9e2e7-7af7-483b-94be-755704d2bd24</t>
-  </si>
-  <si>
-    <t>35e08085-542c-4e77-ad5d-d013b289eaf8</t>
-  </si>
-  <si>
-    <t>ccb0ebcf-d995-43f2-822b-0eb77a265eb3</t>
-  </si>
-  <si>
-    <t>9e0b7579-7197-492c-aa11-d41c3cac9773</t>
-  </si>
-  <si>
-    <t>c3007cb9-26de-4383-846b-cdedcd824b65</t>
-  </si>
-  <si>
-    <t>1690eb75-f259-4900-9e77-7420bdf629dd</t>
-  </si>
-  <si>
-    <t>ed2a6f98-8f92-4bd0-9658-1be867a0815e</t>
-  </si>
-  <si>
-    <t>c1cd7e6b-3d16-4e5a-8ab9-27bb617e3e9f</t>
-  </si>
-  <si>
-    <t>ce632b30-4f2d-4b75-a7c1-c1be1c6625f7</t>
-  </si>
-  <si>
-    <t>c5b88ce1-1daa-4842-9c86-8514d25878a3</t>
-  </si>
-  <si>
-    <t>16ad7299-16c5-4d69-96c2-c590904109dd</t>
-  </si>
-  <si>
-    <t>d6d935c6-0630-4b37-b145-b6e1f7916d47</t>
-  </si>
-  <si>
-    <t>f320c7fe-0fa8-4df1-a5e4-dff6117c7ee1</t>
-  </si>
-  <si>
-    <t>134e05ef-f97a-451b-8152-2d347f19bf05</t>
-  </si>
-  <si>
-    <t>5fbfb0f5-ae70-44f2-8b41-d417e5b9ce7e</t>
-  </si>
-  <si>
-    <t>4825a7d7-8465-4913-8cfe-9b70fc8f75c4</t>
-  </si>
-  <si>
-    <t>a434561c-896a-45f7-93f9-51c3d44f4158</t>
-  </si>
-  <si>
-    <t>37f3bc1c-eb40-4307-bab9-7f359e304cae</t>
-  </si>
-  <si>
-    <t>cf281daf-31c7-43f5-8d9f-c816829b3c5e</t>
-  </si>
-  <si>
-    <t>6a6bd3d9-fbfa-4e37-97a3-185f7c8e08f6</t>
-  </si>
-  <si>
-    <t>dc4f3b5e-9d98-4d58-bba3-ada37ea06106</t>
-  </si>
-  <si>
-    <t>5061ea72-b890-42c2-8392-7921cdea120a</t>
-  </si>
-  <si>
-    <t>04f45139-902c-4c27-ad79-fcf5a5c6dd69</t>
-  </si>
-  <si>
-    <t>f98264e2-bee4-4b65-8e76-0f26e49f8c1f</t>
-  </si>
-  <si>
-    <t>3cd9de31-5831-4c55-a9e7-9e7546484d13</t>
-  </si>
-  <si>
-    <t>7a904d30-9976-4c2c-8caf-9f7ad94e45e6</t>
-  </si>
-  <si>
-    <t>f631c6cc-cafc-455c-ae54-0d0cb7df4188</t>
-  </si>
-  <si>
-    <t>752878ab-252b-4a9c-8acf-8f6dfb819eb3</t>
-  </si>
-  <si>
-    <t>ab8eae61-8e22-40ee-9e71-9dbb61c4b3ea</t>
-  </si>
-  <si>
-    <t>aadd8b48-381c-414c-910d-82134242f9fe</t>
+    <t>aafd9ca1-2b5b-4a28-b712-d6e9c79f35ff</t>
+  </si>
+  <si>
+    <t>d5652869-b8e6-4c7a-8eb0-5278931d069c</t>
+  </si>
+  <si>
+    <t>3a34cbd8-418d-4ce8-b924-97f502c1272d</t>
+  </si>
+  <si>
+    <t>e100136f-9a6c-4ac5-b887-980c802c7723</t>
+  </si>
+  <si>
+    <t>53df4adf-8bdf-4357-8f73-13675ee2e020</t>
+  </si>
+  <si>
+    <t>bcd4b770-6ca0-40ff-bafe-42ba8cb59c55</t>
+  </si>
+  <si>
+    <t>901269bb-f4ba-45ad-bafa-3ba222c94d02</t>
+  </si>
+  <si>
+    <t>a32a74b9-97d6-47a1-864d-f08676411f00</t>
+  </si>
+  <si>
+    <t>c82f1bfc-98a7-46a2-9543-55dbe0bc4d0d</t>
+  </si>
+  <si>
+    <t>71efc060-e883-4bc5-9897-c867a6dedc74</t>
+  </si>
+  <si>
+    <t>8830b9e3-011f-4065-b31c-740213d1b920</t>
+  </si>
+  <si>
+    <t>7d586283-349f-4cf2-b44f-3f193ea45173</t>
+  </si>
+  <si>
+    <t>80c2b8be-a26b-4e28-8491-61666fe96f8c</t>
+  </si>
+  <si>
+    <t>2bf97164-38a2-4731-95e2-66d349569c68</t>
+  </si>
+  <si>
+    <t>e2e7d857-ecbd-4f1f-a6c4-5a5cd2f71a8a</t>
+  </si>
+  <si>
+    <t>6c5beca4-83f0-46c3-a2e7-dea3f54e84c6</t>
+  </si>
+  <si>
+    <t>cccc374b-33c8-45f8-8be0-cccb8c154552</t>
+  </si>
+  <si>
+    <t>ef9565a0-f403-4797-b114-b0beb5f64163</t>
+  </si>
+  <si>
+    <t>78f0fcb5-58fa-48d4-ac88-262a57c6a39e</t>
+  </si>
+  <si>
+    <t>6001ba8e-fe38-4a24-800c-5595d6d71afa</t>
+  </si>
+  <si>
+    <t>5697d839-8a4e-480b-b6f5-196fd9c5b995</t>
+  </si>
+  <si>
+    <t>bdad3e98-1c3a-4ed8-bb1d-3606249deaec</t>
+  </si>
+  <si>
+    <t>55119a18-e0f7-48b2-b675-19ef37057b9b</t>
+  </si>
+  <si>
+    <t>563d28b3-9d6e-43e0-a101-ac73929f1d60</t>
+  </si>
+  <si>
+    <t>1b4c4b17-ead1-40b0-9769-d617fe3070b6</t>
+  </si>
+  <si>
+    <t>c15bf57b-f8d7-48b5-91c6-cd90040d88f3</t>
+  </si>
+  <si>
+    <t>6bf3a775-8d07-41c7-bf88-4516517b9c7f</t>
+  </si>
+  <si>
+    <t>3eb31175-d71c-479a-beb2-8e9585be3067</t>
+  </si>
+  <si>
+    <t>a49db34a-76a1-4073-808d-7ef2a7b4cac0</t>
+  </si>
+  <si>
+    <t>823e2083-06b1-47da-96e1-e76dc3a83c1b</t>
+  </si>
+  <si>
+    <t>bc6d0ba6-8b82-4c09-9cbb-ea09fab2009a</t>
+  </si>
+  <si>
+    <t>aabc36c6-9dda-44f1-bc08-8a7bc4ed4c8a</t>
+  </si>
+  <si>
+    <t>3105b48d-1d6a-4300-a793-39882f9ebad8</t>
   </si>
   <si>
     <t>Value NA in POTENTIAL_NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -1920,64 +1920,64 @@
     <t>NA</t>
   </si>
   <si>
-    <t>1e119763-67e3-4628-8d32-cb685daf3aab</t>
-  </si>
-  <si>
-    <t>81501deb-0fc9-472b-9d49-3890f79d31c8</t>
-  </si>
-  <si>
-    <t>0141d97a-9454-4fea-ab60-7db68d8b3aad</t>
-  </si>
-  <si>
-    <t>1a8fb113-93e1-4cfa-ae18-3a015757506e</t>
-  </si>
-  <si>
-    <t>1b0a4d80-c51d-45fd-8e57-07c32471e05b</t>
-  </si>
-  <si>
-    <t>ff3874fa-a724-4e4f-ad19-619def0472b6</t>
-  </si>
-  <si>
-    <t>1da1b89c-1bee-4a80-a7de-35c505463381</t>
-  </si>
-  <si>
-    <t>19e0e310-7677-4f85-b87c-c600947ff325</t>
-  </si>
-  <si>
-    <t>5ddf8486-31c4-41fe-96e2-186f1833cc79</t>
-  </si>
-  <si>
-    <t>ff1f790c-838c-46cd-b56a-9743310e6041</t>
-  </si>
-  <si>
-    <t>f296775f-9c74-4e43-89ad-3c3d1787952e</t>
-  </si>
-  <si>
-    <t>52d64245-3b94-4e4a-9ff0-8bc653e50210</t>
-  </si>
-  <si>
-    <t>d885660a-1c40-4dc9-8f5a-2e0346520196</t>
-  </si>
-  <si>
-    <t>be0b41f7-8d59-4011-ae3f-f32e5c2cecda</t>
-  </si>
-  <si>
-    <t>b7db5983-fe48-4590-97fd-216bc09ea72a</t>
-  </si>
-  <si>
-    <t>f79ef6d6-fe86-4daf-87c3-0efbb68606c0</t>
-  </si>
-  <si>
-    <t>81c0efe8-8f01-4e02-b265-1d2d9eead1c6</t>
-  </si>
-  <si>
-    <t>4b340c90-ed78-4609-a8a1-fc972b2f1427</t>
-  </si>
-  <si>
-    <t>33ba75af-5d75-4ed4-91d0-8d110c6387c8</t>
-  </si>
-  <si>
-    <t>317502aa-0d04-4dc3-99d2-03987b43b8c6</t>
+    <t>a23db935-d731-405a-82f0-8e8e8b6adff2</t>
+  </si>
+  <si>
+    <t>75ce15aa-3cec-4759-b74e-cd7d1ac1f654</t>
+  </si>
+  <si>
+    <t>dd64f0a3-1a75-499a-8d31-26fa0361d066</t>
+  </si>
+  <si>
+    <t>12f04100-3374-4411-a385-d68f5d586c5c</t>
+  </si>
+  <si>
+    <t>39ff3d23-4643-4b7b-a319-72593e84f94a</t>
+  </si>
+  <si>
+    <t>f5624527-2a4d-4b9f-8f7e-d76d44fe287d</t>
+  </si>
+  <si>
+    <t>07e3a4f2-09fe-4504-b27a-27da75467dcf</t>
+  </si>
+  <si>
+    <t>655cd85c-c9c0-41bc-a404-2727cfab02df</t>
+  </si>
+  <si>
+    <t>2bab02d8-5539-4dfd-a53a-1e643954dccb</t>
+  </si>
+  <si>
+    <t>899eb2a3-55a4-4924-8df0-5f2915a619ae</t>
+  </si>
+  <si>
+    <t>295a0b02-bfc5-47d3-b38b-318ef2e45c25</t>
+  </si>
+  <si>
+    <t>c2c7dfe5-f233-452a-81ad-b7ba33e488a3</t>
+  </si>
+  <si>
+    <t>fc74ced2-d849-4257-9d19-4133b1b0bee2</t>
+  </si>
+  <si>
+    <t>613c9ef1-0486-4435-a62f-e1e1f7679580</t>
+  </si>
+  <si>
+    <t>040fe9db-ffa7-488c-afff-06c626c28479</t>
+  </si>
+  <si>
+    <t>e107a92e-8934-4057-a7cc-7c9e47c08bc9</t>
+  </si>
+  <si>
+    <t>572c2721-2e1a-47a6-81fc-9b0cc41ec7e6</t>
+  </si>
+  <si>
+    <t>5d2c0c46-fd72-43cc-8198-ced7969aacad</t>
+  </si>
+  <si>
+    <t>ff9d45ca-57c7-4e1f-a08b-2b0f97634d5b</t>
+  </si>
+  <si>
+    <t>83d833a9-8c9e-42b6-ab43-196f0b6ca9a4</t>
   </si>
   <si>
     <t>Value Screening in ASSISTANCE_REQUESTED not in allowed list ('YES','NO')</t>
@@ -1989,178 +1989,178 @@
     <t>Use only allowed values 'YES','NO' in ASSISTANCE_REQUESTED</t>
   </si>
   <si>
-    <t>f47026d5-ea81-47f2-8408-5cde25180d8d</t>
+    <t>5e3c8bd3-bf45-4f04-b672-259baa22db4d</t>
   </si>
   <si>
     <t>Value No in ASSISTANCE_REQUESTED not in allowed list ('YES','NO')</t>
   </si>
   <si>
-    <t>389c0529-c537-4ba4-b42f-2148998571ee</t>
+    <t>bc59c2ed-8231-439b-b681-438536b0b290</t>
   </si>
   <si>
     <t>Value Facility in ASSISTANCE_REQUESTED not in allowed list ('YES','NO')</t>
   </si>
   <si>
-    <t>2dc94d68-ca78-4c85-a575-58b8668d653e</t>
-  </si>
-  <si>
-    <t>b10a6713-9d47-4b79-a6f7-d7888421be73</t>
+    <t>a5d14fb1-fd6d-494b-8ae9-8568072e7df1</t>
+  </si>
+  <si>
+    <t>80a6e7dd-f4b4-495f-9ec4-cc181309bf1d</t>
   </si>
   <si>
     <t>Value Yes in ASSISTANCE_REQUESTED not in allowed list ('YES','NO')</t>
   </si>
   <si>
-    <t>d68be8ca-e8ee-429f-bed4-0b782e4fab05</t>
-  </si>
-  <si>
-    <t>c6370d70-9bb6-4854-966b-05df81808c60</t>
-  </si>
-  <si>
-    <t>f8ae1ac6-375f-43ad-9585-4d339b7d776b</t>
-  </si>
-  <si>
-    <t>681e2b68-d709-4ae9-a57a-6b7cd46b8810</t>
-  </si>
-  <si>
-    <t>1abe929a-fda0-4f95-9c34-d5a6d9ae6005</t>
-  </si>
-  <si>
-    <t>792ab3dd-0345-48bd-9b78-c25970251778</t>
-  </si>
-  <si>
-    <t>6af390e7-dc46-417b-b1d9-7d8c55c66442</t>
-  </si>
-  <si>
-    <t>89b668f1-cb1b-4747-8ba4-3c49f30375a9</t>
-  </si>
-  <si>
-    <t>85ac4e2b-841f-4d7e-8539-b73ed54bbb26</t>
-  </si>
-  <si>
-    <t>70e1f8af-2456-44b1-8270-d3292a513ad4</t>
-  </si>
-  <si>
-    <t>f7edb1f6-e49d-4351-8039-cf1e2fe28219</t>
-  </si>
-  <si>
-    <t>91b1d6ee-6692-42e3-950d-d5d09b23f497</t>
-  </si>
-  <si>
-    <t>8a23abde-5e97-41a7-9a88-e1eaa4ebb65f</t>
-  </si>
-  <si>
-    <t>30aead09-2609-4e33-a1c3-378a9d36b26a</t>
-  </si>
-  <si>
-    <t>83274d64-11ae-4e14-9660-66ad3fc5016d</t>
-  </si>
-  <si>
-    <t>640e55f4-3da1-4616-9f75-e7d9b68b77f8</t>
-  </si>
-  <si>
-    <t>dc9ac82e-e2a5-4b42-9d25-07a3eb507873</t>
-  </si>
-  <si>
-    <t>f0d727a5-a63f-4edc-81cf-c95952366d68</t>
-  </si>
-  <si>
-    <t>16524547-4256-4951-a8f8-0f1b4f94e73a</t>
-  </si>
-  <si>
-    <t>b8197f0e-9d4f-4199-99cf-b17ec3c2d6a7</t>
-  </si>
-  <si>
-    <t>859c3964-05cf-4a29-b691-2be25eefad91</t>
-  </si>
-  <si>
-    <t>0970c4a5-9e08-4822-b237-4db49867fe3d</t>
-  </si>
-  <si>
-    <t>baf305c9-e456-4352-a4d6-953e7efda776</t>
-  </si>
-  <si>
-    <t>f05ee76d-76bf-4291-bbfe-1f7d54178cbe</t>
-  </si>
-  <si>
-    <t>f931cb2c-c275-4f26-991e-e97fdb3c902d</t>
-  </si>
-  <si>
-    <t>17719023-2763-4ccd-8cce-81888e7a7b4f</t>
-  </si>
-  <si>
-    <t>aeb447ab-88a4-46d1-987d-784d7238e744</t>
-  </si>
-  <si>
-    <t>f2588ef9-d01b-4a16-9648-e50a0e6bfb1f</t>
-  </si>
-  <si>
-    <t>e0215140-8e3a-4487-ad6f-07995b3e9c89</t>
-  </si>
-  <si>
-    <t>0b34bef0-ed49-453e-9948-348292567dd1</t>
-  </si>
-  <si>
-    <t>6b93555f-e008-4ead-8609-e7b7d9d8aa03</t>
-  </si>
-  <si>
-    <t>f21d6677-e753-46a8-b22c-dd9fda2a63f9</t>
-  </si>
-  <si>
-    <t>b2f5aa97-077c-4635-84e6-f7a2bca5d11d</t>
-  </si>
-  <si>
-    <t>b3dae95e-7dd5-4173-80e5-61918625dea4</t>
-  </si>
-  <si>
-    <t>7b91243d-b7cf-49ac-aaf9-6b2c66179feb</t>
-  </si>
-  <si>
-    <t>40ccd979-5b2d-4d1e-90b9-2a2119e961f0</t>
-  </si>
-  <si>
-    <t>5996a27f-a5bd-4c22-b576-65c7b6f68f80</t>
-  </si>
-  <si>
-    <t>a76971ff-f3f1-482c-9b36-86cc779a1398</t>
-  </si>
-  <si>
-    <t>b82edaed-c4a4-40ad-afec-8917d049354e</t>
-  </si>
-  <si>
-    <t>cba6076b-6069-475a-a9a1-3861ed3f0cc7</t>
-  </si>
-  <si>
-    <t>933531a9-d8b5-4644-aaf7-b1d9991c6b7b</t>
-  </si>
-  <si>
-    <t>d5dd4186-84bc-4fc6-a8a0-3b77aaf313a8</t>
-  </si>
-  <si>
-    <t>e4361437-f31f-4ea0-9b41-30be7ab0f76f</t>
-  </si>
-  <si>
-    <t>2219b8c4-ef7b-4a9a-9c7c-c83bcb1b0238</t>
-  </si>
-  <si>
-    <t>a96bf27a-3712-4e81-b20f-cd68ea8b9ced</t>
-  </si>
-  <si>
-    <t>6ced0b8c-2e3a-43c9-aede-4810e48fa337</t>
-  </si>
-  <si>
-    <t>66016131-c9ed-4150-8ac6-0736ceabd2d5</t>
-  </si>
-  <si>
-    <t>8f5a35b2-1ba0-40c5-86c3-63e2c42b94ae</t>
-  </si>
-  <si>
-    <t>576bbea7-a0c3-4b26-a92a-c97294634889</t>
-  </si>
-  <si>
-    <t>c9dd1b74-db1b-41f9-9e8c-3757504a0491</t>
-  </si>
-  <si>
-    <t>a2cdfe11-3773-4766-8609-3ca5b21b9292</t>
+    <t>4d5906e3-1cc7-4126-bb02-2843c80b13ba</t>
+  </si>
+  <si>
+    <t>8d41f62e-5e83-473f-acbc-570c4f986a96</t>
+  </si>
+  <si>
+    <t>923f7e76-e87e-4bd3-832f-67f5a65a6604</t>
+  </si>
+  <si>
+    <t>ac11cbda-9dbe-4bbd-affa-e2e8e7c182a1</t>
+  </si>
+  <si>
+    <t>846bff51-866b-42b4-8207-39dd2bdf600a</t>
+  </si>
+  <si>
+    <t>bbd6d20c-ed8c-4111-a560-66b90bf54247</t>
+  </si>
+  <si>
+    <t>8b4584f1-6f40-4455-8777-ca1e93823f0c</t>
+  </si>
+  <si>
+    <t>b97385ca-b622-45bd-a3de-1a0428ab5661</t>
+  </si>
+  <si>
+    <t>8bf41ece-ea44-4832-9815-861eedbda300</t>
+  </si>
+  <si>
+    <t>0ace56a3-e41b-44c1-a99f-abb32f42b3f8</t>
+  </si>
+  <si>
+    <t>6c2eeb5d-c252-44b1-8070-109b922461dd</t>
+  </si>
+  <si>
+    <t>15306d85-e21b-4001-8b7d-184f133a9035</t>
+  </si>
+  <si>
+    <t>76fc8a80-c378-488b-8c9b-795bf9b21c17</t>
+  </si>
+  <si>
+    <t>faa34206-f29e-4aba-bddc-18a0ff83dce8</t>
+  </si>
+  <si>
+    <t>ce9588b1-af8f-4753-beb8-8ed356b82177</t>
+  </si>
+  <si>
+    <t>b0e83252-a0d7-4bb0-958a-dfb1ba4f8861</t>
+  </si>
+  <si>
+    <t>f3cabe94-6889-410c-81d2-103df605ec07</t>
+  </si>
+  <si>
+    <t>b18880ce-7479-41d8-ba02-4b79d4d87caa</t>
+  </si>
+  <si>
+    <t>90336469-7565-471f-aa8e-60c08bfef1d5</t>
+  </si>
+  <si>
+    <t>c8014044-c4e8-417f-a44a-e2985011fb2a</t>
+  </si>
+  <si>
+    <t>bc6b7923-b989-4256-ac4e-23cad2444827</t>
+  </si>
+  <si>
+    <t>fe977195-d4c6-473d-9155-11aa447a9cf2</t>
+  </si>
+  <si>
+    <t>67fba97b-d944-4552-84a0-1e9d4ce65739</t>
+  </si>
+  <si>
+    <t>c4f355bc-54c2-4db2-a4ed-93032e2a76af</t>
+  </si>
+  <si>
+    <t>8baddda1-57c9-45bc-85fe-df741ce2fc39</t>
+  </si>
+  <si>
+    <t>991fa6fa-a982-458e-8548-fda62db006e6</t>
+  </si>
+  <si>
+    <t>87c376c4-f752-468e-abf6-46784910e18c</t>
+  </si>
+  <si>
+    <t>beccab57-7325-4568-b2e6-116cb8c2da76</t>
+  </si>
+  <si>
+    <t>4ad6cb20-f003-4e64-a888-bead2b4b9467</t>
+  </si>
+  <si>
+    <t>d66a73f4-a838-4d30-a537-68aa84dbbe86</t>
+  </si>
+  <si>
+    <t>86ec84e0-2e8f-457a-a7c7-99f0e27a7156</t>
+  </si>
+  <si>
+    <t>032c9ad4-b50c-4d83-b0be-e0d791dcb381</t>
+  </si>
+  <si>
+    <t>1eae5ad9-82b4-4b17-b991-d06d96738658</t>
+  </si>
+  <si>
+    <t>761763cc-bc7d-4140-8d87-79ed5cbbd888</t>
+  </si>
+  <si>
+    <t>8f78cf6a-3827-4962-bcdf-ddb84da39c8a</t>
+  </si>
+  <si>
+    <t>ac80f75e-d144-4684-8167-699fd3531147</t>
+  </si>
+  <si>
+    <t>7027bff6-03c7-4cfc-be7b-61919e3968b7</t>
+  </si>
+  <si>
+    <t>5523d645-5abd-4bd2-a4bf-ba7fb72b6339</t>
+  </si>
+  <si>
+    <t>7b056635-e72f-4698-a10e-bf85517158fd</t>
+  </si>
+  <si>
+    <t>cada0b53-6313-4804-ac39-cacbdac62d81</t>
+  </si>
+  <si>
+    <t>20272608-34db-4783-881f-6cf62c8aa5c6</t>
+  </si>
+  <si>
+    <t>fec05eac-eaff-4eb1-a4f3-702d4b278539</t>
+  </si>
+  <si>
+    <t>1cbb9414-1c07-4f43-8ee8-c20228341a46</t>
+  </si>
+  <si>
+    <t>0ae0f1b7-ec8c-4b07-be76-a14319afc76d</t>
+  </si>
+  <si>
+    <t>a7e42b03-bae7-4c1d-ac6e-71371441c861</t>
+  </si>
+  <si>
+    <t>652b0220-bf1e-4846-845d-b0198aef2239</t>
+  </si>
+  <si>
+    <t>f3cb6df0-209e-491f-a0bb-c09dc18ef04a</t>
+  </si>
+  <si>
+    <t>af1d67fb-d7a3-4061-8100-e54a34660d1a</t>
+  </si>
+  <si>
+    <t>faade35d-d46d-4d1e-b29f-6ec51c0d2599</t>
+  </si>
+  <si>
+    <t>342e8b6b-cbd7-4a5a-9112-efb75a1ed647</t>
+  </si>
+  <si>
+    <t>da801e0f-8f0b-4527-a73d-6d9a224a6ff9</t>
   </si>
   <si>
     <t>fa7874f6-f848-572b-a9ab-9db4c8d5e959</t>
@@ -2169,13 +2169,13 @@
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>8b1d9cf6-bbc3-46a9-a2e9-a5a6d64539c2</t>
-  </si>
-  <si>
-    <t>b12be08b-a35d-4d56-a838-36b32a450960</t>
-  </si>
-  <si>
-    <t>62403b1b-f023-441c-a374-3a26c3ed8618</t>
+    <t>84e68bd2-b8b2-4ffa-8aa1-3e67bd14083d</t>
+  </si>
+  <si>
+    <t>2ce39488-6fa2-4d4c-bb18-2bfe42272865</t>
+  </si>
+  <si>
+    <t>7a517147-30f8-475b-8634-ec1801de7ede</t>
   </si>
   <si>
     <t>78d6a904-035e-54ae-8ac2-ca5cdf3f75f7</t>
@@ -2184,16 +2184,16 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>46cc743c-36d8-4a5d-b9e3-4e6ef546e8ca</t>
-  </si>
-  <si>
-    <t>e5f4e1a8-ba41-44d7-bad5-8e412a1247ec</t>
-  </si>
-  <si>
-    <t>f45db706-a546-4810-b9b5-1716a8e8ff73</t>
-  </si>
-  <si>
-    <t>73f74500-6a83-40f4-b755-1541155f508e</t>
+    <t>2c7f8c58-fa8b-47f1-995f-8d03e5123500</t>
+  </si>
+  <si>
+    <t>1f29a59c-9010-4320-a7e6-8fbaab7c38d5</t>
+  </si>
+  <si>
+    <t>c012ddfe-f148-43a1-82ee-93a633288528</t>
+  </si>
+  <si>
+    <t>6be9a464-3748-4d6c-acf8-befb69bc86fc</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE_SYSTEM_NAME is empty</t>
@@ -2205,16 +2205,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>82e3c097-9751-4277-83c5-72710d617d8c</t>
-  </si>
-  <si>
-    <t>833cd281-8471-4ded-991a-1506aa4040e8</t>
-  </si>
-  <si>
-    <t>638bd86a-2159-4218-899b-344df9e1329b</t>
-  </si>
-  <si>
-    <t>8b9c28f7-de84-463e-a80a-3192f0aefff0</t>
+    <t>bbe04bce-b2e3-48eb-8360-1d6fab208bc8</t>
+  </si>
+  <si>
+    <t>7023934a-a783-4b6e-b0d3-937257a68ad5</t>
+  </si>
+  <si>
+    <t>09c244e6-362c-424a-bfb4-0b9701f652c2</t>
+  </si>
+  <si>
+    <t>0f5128b7-7052-466c-9faf-aff2dd26aad2</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -2226,34 +2226,34 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>1c3c9aa4-70bc-4e3a-9a0b-64070b640dee</t>
-  </si>
-  <si>
-    <t>8340cdb1-ae9d-4338-90e9-642131139409</t>
-  </si>
-  <si>
-    <t>81b8bde1-8d6c-453b-9ec0-3d8c2f32c8aa</t>
-  </si>
-  <si>
-    <t>dfde182e-bd37-4850-ad80-7778e31ddb74</t>
-  </si>
-  <si>
-    <t>3d8a946f-6a15-4010-8e01-68055e608ac0</t>
-  </si>
-  <si>
-    <t>b3f51dcd-dbd4-4c9c-9050-792a92b91fbd</t>
-  </si>
-  <si>
-    <t>62ee105b-23db-47bc-9e04-bef68e71d5a0</t>
-  </si>
-  <si>
-    <t>5aa1dea6-d2dc-4fad-84f6-bceb9b0509e5</t>
-  </si>
-  <si>
-    <t>dcb5a357-3485-4730-965f-37255acb84fa</t>
-  </si>
-  <si>
-    <t>82df1752-baf8-4c06-97e2-9380981d90d3</t>
+    <t>eced7b5d-7b2d-496e-abb9-e6ba28d00b00</t>
+  </si>
+  <si>
+    <t>792452e0-b4ec-433e-b0a5-060e71e16813</t>
+  </si>
+  <si>
+    <t>ed2538f4-6a91-43ce-ab5a-ba5b640bd125</t>
+  </si>
+  <si>
+    <t>b81f05c9-c1c9-46e0-b9e7-4c4738603163</t>
+  </si>
+  <si>
+    <t>63dc668d-b886-496c-9db1-f30745463ec5</t>
+  </si>
+  <si>
+    <t>9ed8d1e2-3062-4d83-8d55-3e98bbb7d233</t>
+  </si>
+  <si>
+    <t>25d74c6c-7582-4fd8-82b6-16321e25d1bb</t>
+  </si>
+  <si>
+    <t>93b2c359-681f-4608-a0e2-69c5614a6f99</t>
+  </si>
+  <si>
+    <t>5af3be13-ccb9-4e03-8440-26974e88a522</t>
+  </si>
+  <si>
+    <t>927117f9-b5b8-4219-9fd8-aa2f86d2dda2</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -2262,187 +2262,187 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>aec182dc-4f83-4aac-aab6-7180d7b78a7a</t>
-  </si>
-  <si>
-    <t>9773a4fb-bde1-402e-8875-0a71d89f4fac</t>
-  </si>
-  <si>
-    <t>3f4996a2-1cdf-4db5-bde1-eb5db16d366e</t>
-  </si>
-  <si>
-    <t>f0bfecf8-7b38-4473-bbcb-72e45daf0b1f</t>
-  </si>
-  <si>
-    <t>f051251e-0848-452d-8389-994cdb49205e</t>
-  </si>
-  <si>
-    <t>dfdae050-e9da-44be-bc14-11f7632af6b2</t>
-  </si>
-  <si>
-    <t>fca1effe-ac4c-4e90-b491-81dc406d7e61</t>
-  </si>
-  <si>
-    <t>69c11927-bed7-4429-bc8d-127a9140187c</t>
-  </si>
-  <si>
-    <t>dee1b723-c885-403d-8a6f-7893f979b82d</t>
-  </si>
-  <si>
-    <t>d3e75c5b-5c15-4054-9aec-e71f544448a1</t>
-  </si>
-  <si>
-    <t>4e060503-977e-4118-920d-ef103dddc184</t>
-  </si>
-  <si>
-    <t>24744533-eeff-4572-8207-e1adaae2ce8d</t>
-  </si>
-  <si>
-    <t>6b0da9ca-ada9-4415-a794-4d74692d40c2</t>
-  </si>
-  <si>
-    <t>dcc0c124-6622-4166-8c0c-87f634f7d3ef</t>
-  </si>
-  <si>
-    <t>ee76ccd6-c64f-4d87-94c8-0cb33db32be4</t>
-  </si>
-  <si>
-    <t>8fd4d91b-9a41-4a1a-9ea5-356f7c1b0323</t>
-  </si>
-  <si>
-    <t>efdd0084-4f4d-4204-8405-a453c8d8e684</t>
-  </si>
-  <si>
-    <t>a35f904e-61e9-4b44-8149-214e7138ba7e</t>
-  </si>
-  <si>
-    <t>73412153-dc3f-42ea-ae77-03fa664b08dc</t>
-  </si>
-  <si>
-    <t>f23e3241-0526-4696-a941-332c86207265</t>
-  </si>
-  <si>
-    <t>40962737-05da-4d0f-b479-8f381d21befc</t>
-  </si>
-  <si>
-    <t>1e8d9a37-0a86-4091-8f79-715d42dd4b5d</t>
-  </si>
-  <si>
-    <t>7a8ca2c3-c48e-41da-aa77-26215df2510d</t>
-  </si>
-  <si>
-    <t>69a95cd2-9b60-483e-b9e7-d37262dadb04</t>
-  </si>
-  <si>
-    <t>e31b42c1-a2ce-4d9b-9a2d-2db8f74820b0</t>
-  </si>
-  <si>
-    <t>56ed2dac-2c5b-485c-b17a-1b456577d911</t>
-  </si>
-  <si>
-    <t>9b311566-4027-43a1-9955-5243ffa0adee</t>
-  </si>
-  <si>
-    <t>421091db-c8ef-478e-b3d8-f5e3c92cd3f5</t>
-  </si>
-  <si>
-    <t>5c65014a-51df-4999-8466-d219a8c5332c</t>
-  </si>
-  <si>
-    <t>6430990b-6244-47c8-8ad5-b21117269ed8</t>
-  </si>
-  <si>
-    <t>a082c212-929b-419e-8c65-85db0e32a425</t>
-  </si>
-  <si>
-    <t>942e8bc0-6cfd-4ed1-ab73-b2751f331369</t>
-  </si>
-  <si>
-    <t>c2383ba9-41c2-420c-9576-c6320ebc0ea5</t>
-  </si>
-  <si>
-    <t>b9571e43-ed79-404e-83a4-5f579a64681e</t>
-  </si>
-  <si>
-    <t>0f14662a-2fd3-460e-bf98-57459a815280</t>
-  </si>
-  <si>
-    <t>b198f186-9522-41d4-9de5-80a53b575268</t>
-  </si>
-  <si>
-    <t>d71b8b89-6758-40f3-ba3a-afc24e4d87db</t>
-  </si>
-  <si>
-    <t>528cdc3f-1da6-4101-9477-3171c4a3ef0a</t>
-  </si>
-  <si>
-    <t>f8eb4cb3-4069-437e-8988-a158b9f7fa95</t>
-  </si>
-  <si>
-    <t>f57673bb-ca5e-4228-9e2e-92a33a5a98c2</t>
-  </si>
-  <si>
-    <t>2f3dcb80-c00d-4091-93ee-093a1f34f040</t>
-  </si>
-  <si>
-    <t>aa8449e2-164a-4a40-accf-0922b1c4b332</t>
-  </si>
-  <si>
-    <t>2c3af0c9-7445-4c44-9219-b07398a1d7b9</t>
-  </si>
-  <si>
-    <t>76a715a2-1d27-43c9-a1ec-f8fbfe83b42a</t>
-  </si>
-  <si>
-    <t>f79c4d2d-3541-4a55-9550-cbdce273c377</t>
-  </si>
-  <si>
-    <t>a9a6de65-02c4-4df5-ac0c-0d3c4b563ec6</t>
-  </si>
-  <si>
-    <t>e17f474a-264d-4fc5-9704-547d5431a360</t>
-  </si>
-  <si>
-    <t>15100216-4039-4f10-b9e7-8ef084ef16a9</t>
-  </si>
-  <si>
-    <t>3bd36e35-6a29-4288-be91-f21328ee8add</t>
-  </si>
-  <si>
-    <t>6438120b-3fdf-4ea8-94fa-5d85d93fd92d</t>
-  </si>
-  <si>
-    <t>ce692293-aa93-4905-aef2-33171d21e62d</t>
-  </si>
-  <si>
-    <t>4b630c7f-8196-4ec3-85ce-483497e39359</t>
-  </si>
-  <si>
-    <t>e6447d63-723e-413a-acb7-eaee65340469</t>
-  </si>
-  <si>
-    <t>d0c2f9af-1a2a-4505-87b6-15205dae93f6</t>
-  </si>
-  <si>
-    <t>6dfafbac-b56b-47e8-aaaf-886885aa69f6</t>
-  </si>
-  <si>
-    <t>6976b534-43d7-4e2b-9377-168ab774c1c1</t>
-  </si>
-  <si>
-    <t>3b6f2864-a6f1-4d42-bd3e-28a6d59aefca</t>
-  </si>
-  <si>
-    <t>43dfec2f-3d87-477b-bab8-f9810e1ac3cc</t>
-  </si>
-  <si>
-    <t>033fad95-5893-4efc-b6a6-c04d8a0e5652</t>
-  </si>
-  <si>
-    <t>a8c55587-21a1-4697-88c3-3486a7e3a4b9</t>
-  </si>
-  <si>
-    <t>b7105ef2-54d5-45b6-bbb5-df23ae6ccdf3</t>
+    <t>ee296699-6aa3-44fa-adc1-a1c63f51f0cb</t>
+  </si>
+  <si>
+    <t>f63af899-0729-49ba-aacc-27f769d9ad7c</t>
+  </si>
+  <si>
+    <t>f08a4c6b-9c21-49c9-9e2d-f30e4c1e55f5</t>
+  </si>
+  <si>
+    <t>adb72684-7dbf-40ec-a3b5-aaba862abacf</t>
+  </si>
+  <si>
+    <t>0992a1bc-feaa-4c4f-ad1f-19c4dea94522</t>
+  </si>
+  <si>
+    <t>d42e8abf-4ed2-4f69-b247-28e41c3e48ff</t>
+  </si>
+  <si>
+    <t>a5214520-72e2-427a-a9a9-c0be99ecc4be</t>
+  </si>
+  <si>
+    <t>6f008a06-5d64-4543-b323-e75d2fda7152</t>
+  </si>
+  <si>
+    <t>f291474a-81f1-4eb4-b263-ac5f36d8ae3a</t>
+  </si>
+  <si>
+    <t>501c7d52-5c4c-4f79-937e-6852ae5b0f30</t>
+  </si>
+  <si>
+    <t>fcd55452-d965-483e-a9c3-7052c969167a</t>
+  </si>
+  <si>
+    <t>9d336d37-98b2-4d3a-958d-c8dbab36de9a</t>
+  </si>
+  <si>
+    <t>20fd30cd-32e0-4381-a24a-916759967175</t>
+  </si>
+  <si>
+    <t>1db3ffdd-aa95-44ef-9d74-8c157363f56d</t>
+  </si>
+  <si>
+    <t>bd87631a-dd09-4926-ba17-2d9c87ff4d95</t>
+  </si>
+  <si>
+    <t>6414ba67-0cad-43ea-9a44-d7020b3b7fd8</t>
+  </si>
+  <si>
+    <t>9c9460cb-7a2f-4a65-a89d-0019d20bfed5</t>
+  </si>
+  <si>
+    <t>29cf2c0f-ede7-46ba-a4db-28d91103aea8</t>
+  </si>
+  <si>
+    <t>6a9f1481-ead7-4c5d-b1f2-b301d0cbb6e6</t>
+  </si>
+  <si>
+    <t>68ae00c5-e5ac-451a-8854-1dee036a9194</t>
+  </si>
+  <si>
+    <t>7fe66c3c-0db5-4b21-b4bf-1a1f7aa4f49f</t>
+  </si>
+  <si>
+    <t>64f378dc-e79f-4262-ba65-00d2e27e84e3</t>
+  </si>
+  <si>
+    <t>425f9371-4d6f-4e23-8179-3ea7b32c3310</t>
+  </si>
+  <si>
+    <t>884eedf6-7afd-4e27-a7e9-61fe995bae04</t>
+  </si>
+  <si>
+    <t>0594012b-108b-4ac3-9b8b-b6f58a638000</t>
+  </si>
+  <si>
+    <t>fec473ee-7510-4e32-96ee-90e917e9c753</t>
+  </si>
+  <si>
+    <t>8bde32f0-8095-4388-8d68-e9ed2c36d4b6</t>
+  </si>
+  <si>
+    <t>c8fe944a-fd3e-43ad-bec7-1e10b6eb82fb</t>
+  </si>
+  <si>
+    <t>02ead437-3893-4363-8984-fcd423531326</t>
+  </si>
+  <si>
+    <t>0a44ea0b-efeb-48dc-9133-9570ce2a4c0c</t>
+  </si>
+  <si>
+    <t>562456cc-0589-4ce3-ad15-d2d2eb23796c</t>
+  </si>
+  <si>
+    <t>d5ac72a0-8466-4d8b-b5cd-06e136386464</t>
+  </si>
+  <si>
+    <t>96d057d8-8d99-4124-a244-1c906fa829ff</t>
+  </si>
+  <si>
+    <t>1063b2d6-3c81-4c6a-8e10-2e5d7df2fe3c</t>
+  </si>
+  <si>
+    <t>2a0f6682-3620-4630-b9cb-dd7a3a61810e</t>
+  </si>
+  <si>
+    <t>a5348e86-af47-4b3e-bb1b-8ac6fcb97976</t>
+  </si>
+  <si>
+    <t>ceb8c9dd-f861-4064-be29-35969bcfc6fa</t>
+  </si>
+  <si>
+    <t>8cf714f8-14e7-49cf-94e5-92c8cdedaa4d</t>
+  </si>
+  <si>
+    <t>83a89223-71b0-4d20-8b2f-ff1642b7a202</t>
+  </si>
+  <si>
+    <t>abb1c1ee-23d1-449f-a95e-f88d139b0376</t>
+  </si>
+  <si>
+    <t>901331e4-3183-4e6d-aa1d-5929eaebcf02</t>
+  </si>
+  <si>
+    <t>049e6ee4-d426-4701-9fd5-496d7fd62ef8</t>
+  </si>
+  <si>
+    <t>46b04317-3011-46a6-94a0-42639234af04</t>
+  </si>
+  <si>
+    <t>a1349472-8df4-40f5-8f7f-d1da1be569e7</t>
+  </si>
+  <si>
+    <t>edf76ee8-a812-4683-b127-f954869dc6e1</t>
+  </si>
+  <si>
+    <t>a67954e4-21f1-484b-b4d6-34301bc2b3d5</t>
+  </si>
+  <si>
+    <t>c357b710-5b13-4c16-8dd6-7469ba1daf68</t>
+  </si>
+  <si>
+    <t>ccd2bd57-aa4b-418f-a3ee-323af75f62b5</t>
+  </si>
+  <si>
+    <t>90c306c8-f0b2-4df9-b2f7-f780af1e5754</t>
+  </si>
+  <si>
+    <t>b3ed8af2-e501-461d-b448-b11a58694dde</t>
+  </si>
+  <si>
+    <t>f5ca4891-8e09-47fc-97b0-c6571d10a2f3</t>
+  </si>
+  <si>
+    <t>26b1fb0c-3bc2-4c0a-9143-3fde5bd3a101</t>
+  </si>
+  <si>
+    <t>6228c990-947d-40f6-ada1-31291bb5f4a5</t>
+  </si>
+  <si>
+    <t>0cb50657-f18e-4de6-a12b-f9def1119e26</t>
+  </si>
+  <si>
+    <t>9a7097ca-7e4c-428a-bb32-fc3ab242c48c</t>
+  </si>
+  <si>
+    <t>7c80e616-b191-4678-b839-f210e9179676</t>
+  </si>
+  <si>
+    <t>af8f31a8-bbf7-4faf-864a-867ab8a5f658</t>
+  </si>
+  <si>
+    <t>5b3af13e-061d-4704-a7da-4a4ed54d128f</t>
+  </si>
+  <si>
+    <t>c6ed9cf8-7266-44a9-90d2-076677be5ace</t>
+  </si>
+  <si>
+    <t>77901bc1-0642-4054-90fc-b67d7917c0bf</t>
+  </si>
+  <si>
+    <t>303d1a64-70c8-44cd-b920-79bc79d21ab6</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -2451,631 +2451,631 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>16fc97e9-e188-4b65-a5b3-b70ab246683c</t>
-  </si>
-  <si>
-    <t>ee29daaa-5838-4254-9263-832f02c8c9ac</t>
-  </si>
-  <si>
-    <t>f67be1eb-0dca-4dd4-980e-6fbbddbef015</t>
-  </si>
-  <si>
-    <t>41808857-579f-4adc-99d4-e495f8598e08</t>
-  </si>
-  <si>
-    <t>b009e6f9-6294-44a8-ac6b-e06944cd026a</t>
-  </si>
-  <si>
-    <t>31f1ab70-9c87-45dd-8e3b-20738c477d6b</t>
-  </si>
-  <si>
-    <t>d72277a8-7c91-4102-9836-a92b223288ad</t>
-  </si>
-  <si>
-    <t>7286fc5e-2be3-4c44-8aae-22ccedc4d3d2</t>
-  </si>
-  <si>
-    <t>3c6be758-9827-4406-89c3-e233e5eff92c</t>
-  </si>
-  <si>
-    <t>1696a250-47fa-4d30-8a8d-1ee196a0746f</t>
-  </si>
-  <si>
-    <t>1c9759cc-d1d6-451d-b434-9c79b69d74fa</t>
-  </si>
-  <si>
-    <t>4e1212f8-a8aa-478d-9b1f-efd5071cc331</t>
-  </si>
-  <si>
-    <t>e83eb228-6997-40bd-85d5-094d4df6a637</t>
-  </si>
-  <si>
-    <t>77e82b85-59e2-4dbb-b00a-83c3cd568567</t>
-  </si>
-  <si>
-    <t>a2b604c4-68a5-435b-9d01-4b5f1d0d6900</t>
-  </si>
-  <si>
-    <t>72958069-32d8-4df1-b394-581998ad142f</t>
-  </si>
-  <si>
-    <t>676d29b7-852d-475c-81bd-7c2aaae116c0</t>
-  </si>
-  <si>
-    <t>faa6b513-19bf-4bb0-a51c-fbf71349f321</t>
-  </si>
-  <si>
-    <t>4edaa6bd-b74a-4db6-a8cb-db4518c869e6</t>
-  </si>
-  <si>
-    <t>99b64dfd-d1eb-4a7f-8415-54db68838c6a</t>
-  </si>
-  <si>
-    <t>d6d798a6-8f4d-4ea3-ae69-632c8fc5bb0c</t>
-  </si>
-  <si>
-    <t>eba98ec7-6f5d-4394-a32e-788a4a0b1881</t>
-  </si>
-  <si>
-    <t>c822a0fa-bc0e-431a-8ee1-625f4a3db735</t>
-  </si>
-  <si>
-    <t>caa17b15-43fa-4712-9ba0-08334e5cc992</t>
-  </si>
-  <si>
-    <t>31bfe40b-e70c-49e5-864f-472cc82cdae3</t>
-  </si>
-  <si>
-    <t>74fa516a-7822-4d83-b86a-cb045637f3a4</t>
-  </si>
-  <si>
-    <t>fba8fd6e-f051-4649-8747-446723214a5d</t>
-  </si>
-  <si>
-    <t>e3b50883-c4bc-40e4-a53b-22f7e44478fc</t>
-  </si>
-  <si>
-    <t>5ff9c482-40c5-4edf-a315-306985c29034</t>
-  </si>
-  <si>
-    <t>c4a08925-c701-4e74-a9be-3bd37d46d6ef</t>
-  </si>
-  <si>
-    <t>31997883-1051-480c-ac1e-ed85a5a7a2ef</t>
-  </si>
-  <si>
-    <t>d56b8e14-0f71-481d-a49f-e567aabf434b</t>
-  </si>
-  <si>
-    <t>bd178eb4-e598-4b9c-9fa2-c3f96e5877ad</t>
-  </si>
-  <si>
-    <t>bde5d12f-428f-4c29-8515-ebcc9fa1cfc2</t>
-  </si>
-  <si>
-    <t>d0de49e6-df49-4da9-9ddf-c7d01537cb78</t>
-  </si>
-  <si>
-    <t>4f05e62d-a90c-4f13-b346-b6555abdb9c8</t>
-  </si>
-  <si>
-    <t>3e30f389-0b09-4c01-859a-0b7ec9bdae87</t>
-  </si>
-  <si>
-    <t>05c02b94-eea2-40ac-bb0b-4d7e786475f7</t>
-  </si>
-  <si>
-    <t>32ec65de-0883-4492-82a7-3030b2b7525e</t>
-  </si>
-  <si>
-    <t>25b9c8b6-ee82-42a4-8819-c54b4a523388</t>
-  </si>
-  <si>
-    <t>4f6f80c0-eb76-4a00-a8ba-9fb8efe971b5</t>
-  </si>
-  <si>
-    <t>42dd1262-9f52-420b-b80f-3187b7d960de</t>
-  </si>
-  <si>
-    <t>331cee6c-7f88-41c7-862d-738091356a18</t>
-  </si>
-  <si>
-    <t>6e307cd5-a0bb-44c8-acab-9843f36f7704</t>
-  </si>
-  <si>
-    <t>0c5ce709-da88-4647-b2a8-87b32c76be34</t>
-  </si>
-  <si>
-    <t>98966fe2-b5e7-4507-b16d-91552ae8f450</t>
-  </si>
-  <si>
-    <t>a93ba99b-42dd-4623-8011-caa0249222a2</t>
-  </si>
-  <si>
-    <t>39baccc2-c657-468e-af5a-5ee769d9fe07</t>
-  </si>
-  <si>
-    <t>f35676a7-e3d4-4dd1-b603-fb3f333473c0</t>
-  </si>
-  <si>
-    <t>3ef4ca2f-3c2f-4fa5-b5c5-af9d6d263212</t>
-  </si>
-  <si>
-    <t>5bad1bc5-f317-48bb-945c-c27f90404455</t>
-  </si>
-  <si>
-    <t>a77102cd-0119-4d07-9909-ca1884564a42</t>
-  </si>
-  <si>
-    <t>ab73083e-26bf-4f01-940e-502513b57861</t>
-  </si>
-  <si>
-    <t>bafd0de1-ea8f-4b4a-ad82-387b94335402</t>
-  </si>
-  <si>
-    <t>35932fbf-e9a2-43bc-9ba5-acee23cc71e2</t>
-  </si>
-  <si>
-    <t>9153e966-92c4-4701-97f9-42e99bf901b4</t>
-  </si>
-  <si>
-    <t>d6960644-a58e-45c7-957b-7ecca1347106</t>
-  </si>
-  <si>
-    <t>704511d4-9339-47fa-81c1-33dd025a8ed1</t>
-  </si>
-  <si>
-    <t>bccaf7c8-7518-4fd9-ae6a-f6b4bca658d4</t>
-  </si>
-  <si>
-    <t>96e286ad-42e4-4d5f-9e60-b5b058386818</t>
-  </si>
-  <si>
-    <t>98ed307e-f61b-429a-a92d-2993076b9c04</t>
-  </si>
-  <si>
-    <t>7a9838d0-829f-4288-9142-65c08be948d4</t>
-  </si>
-  <si>
-    <t>2411657b-bea0-4748-bf86-9b9d9b010a1f</t>
-  </si>
-  <si>
-    <t>f2e74018-b0b6-4193-8e62-b219657d9123</t>
-  </si>
-  <si>
-    <t>a62aa6b5-d15b-464f-aefd-6af1f9be335d</t>
-  </si>
-  <si>
-    <t>11cabe01-c2fc-4726-9881-b7c9222646fa</t>
-  </si>
-  <si>
-    <t>9ff704bb-5d79-4e2c-baaa-eddc30c53e15</t>
-  </si>
-  <si>
-    <t>342e8481-6530-4447-b815-04ced37cc10a</t>
-  </si>
-  <si>
-    <t>d2626fd6-b86a-403f-ae73-af27604aead8</t>
-  </si>
-  <si>
-    <t>ec0283c5-d728-48cc-b764-0ba26cb3f365</t>
-  </si>
-  <si>
-    <t>a47548eb-cbf8-4af2-bd38-571f05a17242</t>
-  </si>
-  <si>
-    <t>4167c884-fe1e-444f-aea5-392f453a9407</t>
-  </si>
-  <si>
-    <t>99be632b-cc95-4a44-94d6-c7e550d65601</t>
-  </si>
-  <si>
-    <t>64761fb0-b146-42bb-8805-0deb7c68b9d1</t>
-  </si>
-  <si>
-    <t>a4f2f36e-147f-4a09-b427-b3a1735eda11</t>
-  </si>
-  <si>
-    <t>c75b6ede-3872-4b9d-9329-aad92f2a6027</t>
-  </si>
-  <si>
-    <t>73f9183f-cdfd-4db5-9b16-10ea974ef720</t>
-  </si>
-  <si>
-    <t>8aa1b4cd-9a6e-4354-a985-bfc5b5931d01</t>
-  </si>
-  <si>
-    <t>7f10a26c-afaf-4bf9-bff9-3838697d2fc9</t>
-  </si>
-  <si>
-    <t>3ff68311-7b1c-43d5-bc59-b5e184dbcbe7</t>
-  </si>
-  <si>
-    <t>cd3005c9-1a18-47ec-a1e3-ab9389c7a83d</t>
-  </si>
-  <si>
-    <t>102f41dd-0d45-4ce7-a6af-5c2d1f842c26</t>
-  </si>
-  <si>
-    <t>bfa70dda-39b0-482c-9f19-175138110498</t>
-  </si>
-  <si>
-    <t>6fbba649-363d-4099-b8f9-b6067bea0afd</t>
-  </si>
-  <si>
-    <t>b1a1a81c-1d86-41fa-af48-ffc6abe5b059</t>
-  </si>
-  <si>
-    <t>2cfcb1d7-6fd7-4eef-9585-3e9b09bf6488</t>
-  </si>
-  <si>
-    <t>acbf10f7-de24-4343-a728-e8c826669236</t>
-  </si>
-  <si>
-    <t>89cfdcbd-e2ce-4c16-ac41-fed5a128b66b</t>
-  </si>
-  <si>
-    <t>7cca863c-66f6-442a-b8ec-b8c4922bba20</t>
-  </si>
-  <si>
-    <t>657dc1f9-b0d0-44ce-9ad2-dd6fbab80fd0</t>
-  </si>
-  <si>
-    <t>322d1ad1-b094-4283-b491-14093254f650</t>
-  </si>
-  <si>
-    <t>43d03565-5ed1-4da3-9a08-1b9ed2b47fe9</t>
-  </si>
-  <si>
-    <t>31a4c801-09ee-4880-8fc7-702efcd4c0f2</t>
-  </si>
-  <si>
-    <t>fe9800c6-fbcb-4717-8842-5201b13ebdcc</t>
-  </si>
-  <si>
-    <t>cc0dc483-59af-4feb-a418-27322d84b491</t>
-  </si>
-  <si>
-    <t>b45df614-1b68-41ee-b30a-a1abbedef451</t>
-  </si>
-  <si>
-    <t>13fa0773-4ff4-44cd-83ea-dd1c8fb4be7d</t>
-  </si>
-  <si>
-    <t>274f1af7-3822-4b31-81a4-8eba582c891d</t>
-  </si>
-  <si>
-    <t>f63a83ae-061b-473a-8337-a1302592c15e</t>
-  </si>
-  <si>
-    <t>738bbb79-ae83-4e84-9133-69c2ebf52343</t>
-  </si>
-  <si>
-    <t>d1675715-e03e-4c49-b7bb-0a66ee4d33e0</t>
-  </si>
-  <si>
-    <t>1289b502-1083-447b-88ba-139e208fe965</t>
-  </si>
-  <si>
-    <t>8f6949f0-2095-4454-94be-484fa7bc5231</t>
-  </si>
-  <si>
-    <t>54a99b8d-e7b6-4c65-8779-dff0b5324252</t>
-  </si>
-  <si>
-    <t>5a90b684-8cdf-44e3-9e98-c15eb00eb936</t>
-  </si>
-  <si>
-    <t>90302c74-7e08-4b1a-8245-12e8c69c0e5c</t>
-  </si>
-  <si>
-    <t>18d2f2fc-e670-4da8-ad9b-547c8b948841</t>
-  </si>
-  <si>
-    <t>913fe345-f3cf-4256-9737-c96376b86db3</t>
-  </si>
-  <si>
-    <t>ac7a3b7b-dbfa-410b-8f7e-0cc9b794dd0f</t>
-  </si>
-  <si>
-    <t>f75f2727-0a1f-49f8-bac2-80f343fd61ab</t>
-  </si>
-  <si>
-    <t>2333fe94-b78e-4920-b0ff-00b44a6bf31a</t>
-  </si>
-  <si>
-    <t>ae110049-9103-4cda-9400-69954df0cdee</t>
-  </si>
-  <si>
-    <t>aa6448bb-d2a0-4258-9d12-1a1b333a716e</t>
-  </si>
-  <si>
-    <t>3b0bc9e7-3e4a-4e74-b176-cd55c1c5460c</t>
-  </si>
-  <si>
-    <t>32136308-2b82-4bca-abaf-906278eaa398</t>
-  </si>
-  <si>
-    <t>bff3cb45-386b-4db1-a009-bd948450c280</t>
-  </si>
-  <si>
-    <t>acc73c54-5a70-4b29-97ae-bbb59e53f78f</t>
-  </si>
-  <si>
-    <t>62d4ed6d-d248-456f-a636-324d00672383</t>
-  </si>
-  <si>
-    <t>d481a342-eb03-410f-8284-c82c267d275a</t>
-  </si>
-  <si>
-    <t>15f6574d-e0e4-486c-97da-f640be9112a2</t>
-  </si>
-  <si>
-    <t>773de992-a93b-4cb8-bdb9-e08e5f1df15c</t>
-  </si>
-  <si>
-    <t>747bf828-3413-4258-87f6-677a67cf8254</t>
-  </si>
-  <si>
-    <t>592bb940-ab4a-4e10-bbe1-184ed3682441</t>
-  </si>
-  <si>
-    <t>6d7bd00d-76fe-4a60-8a9b-00c6fd63dac6</t>
-  </si>
-  <si>
-    <t>16e58e2b-610a-4c02-a35d-b96482b70250</t>
-  </si>
-  <si>
-    <t>78f69063-7a1f-4366-94b3-4998cac85e9c</t>
-  </si>
-  <si>
-    <t>f5f74798-5b6d-47cd-9db4-ed9a441270ed</t>
-  </si>
-  <si>
-    <t>639ff48e-05fc-4d4a-92ba-3f1ae345e62e</t>
-  </si>
-  <si>
-    <t>13ae3718-ada0-4e99-b1fb-7260c1031a0e</t>
-  </si>
-  <si>
-    <t>ae559464-a101-412a-977e-e90e7537da4b</t>
-  </si>
-  <si>
-    <t>e19154e2-4e5c-4aac-9157-7dc7a8a9c367</t>
-  </si>
-  <si>
-    <t>059a4218-9175-4b89-9220-70ea93410073</t>
-  </si>
-  <si>
-    <t>ca766758-4f4a-498c-acca-586d3ca825a6</t>
-  </si>
-  <si>
-    <t>e0920e6a-6194-4d0f-bf09-34e1c23d228c</t>
-  </si>
-  <si>
-    <t>ea20072b-af3d-47b5-b9a1-f1d1715a8ce3</t>
-  </si>
-  <si>
-    <t>c176b499-4d1a-4520-9c8a-05f9f5a7b598</t>
-  </si>
-  <si>
-    <t>5e92c621-061c-4bba-9556-a28f12423c0b</t>
-  </si>
-  <si>
-    <t>15bf9c75-057b-4141-bd2e-5fe79228d944</t>
-  </si>
-  <si>
-    <t>157b675a-9ae7-49d5-a1c8-1e541589704a</t>
-  </si>
-  <si>
-    <t>e888432e-83f6-40d2-b73e-3efcdbc97a38</t>
-  </si>
-  <si>
-    <t>dd4a5739-9e5d-4d46-b649-a733109dc4b9</t>
-  </si>
-  <si>
-    <t>fa5175e6-960f-4a60-9dfa-fa654f790407</t>
-  </si>
-  <si>
-    <t>4df21dec-1183-470b-bdb1-4b7143cac73d</t>
-  </si>
-  <si>
-    <t>7d2175ad-21cb-4bcf-a439-ffb6485d66c5</t>
-  </si>
-  <si>
-    <t>9ee93e58-ee70-4e68-9891-d0458a98c154</t>
-  </si>
-  <si>
-    <t>bf5eb3b5-f8f6-441f-891f-a4799dab54e2</t>
-  </si>
-  <si>
-    <t>da2d951d-d64c-4ee1-bddd-f401f230e3a8</t>
-  </si>
-  <si>
-    <t>cea598b5-2955-409c-ab96-bc7a118892d1</t>
-  </si>
-  <si>
-    <t>9a665307-e9be-4fba-b8d5-2750339e5a5c</t>
+    <t>1288895d-d470-4dae-84a1-d5e3ebd619f4</t>
+  </si>
+  <si>
+    <t>4c7163a6-d9aa-47cf-9e3a-9fa2bd81ea78</t>
+  </si>
+  <si>
+    <t>96f91c97-93f8-4513-b513-bd2bdd5361d6</t>
+  </si>
+  <si>
+    <t>5c008b69-f937-4d9c-ad27-baa202c5b0ba</t>
+  </si>
+  <si>
+    <t>4c8b6184-2219-43f7-b506-65dd9ad6cc12</t>
+  </si>
+  <si>
+    <t>14625a44-4935-4590-b6bc-b5a7a211ee7a</t>
+  </si>
+  <si>
+    <t>81eeaad8-cd7a-4c18-96cb-68a8cf50ad49</t>
+  </si>
+  <si>
+    <t>9855d45c-cd3c-4545-8397-46d00a98b04c</t>
+  </si>
+  <si>
+    <t>85c4a92f-1dd5-467c-977f-8d2d18d702cb</t>
+  </si>
+  <si>
+    <t>0e244627-1bbd-42cb-a128-7d0ce82af781</t>
+  </si>
+  <si>
+    <t>1b9eb44c-404a-46cb-94b2-99ca1b9a6e83</t>
+  </si>
+  <si>
+    <t>1c32af25-7c0b-4359-a7ec-e65ee767732b</t>
+  </si>
+  <si>
+    <t>9e2e6da4-f86f-4224-826c-6dad93d0f940</t>
+  </si>
+  <si>
+    <t>7c8bfea7-6cf3-4922-bd02-1eaadbe74ef9</t>
+  </si>
+  <si>
+    <t>3a8a2016-94b6-45de-ad48-d5fdc94d2475</t>
+  </si>
+  <si>
+    <t>2db8c139-2cc3-42b8-bcf0-e1056b6ef285</t>
+  </si>
+  <si>
+    <t>ceb91f4f-e943-4ef6-b661-7df87e34d420</t>
+  </si>
+  <si>
+    <t>eec49e3c-3546-40f3-92e9-40c8b51ff9c9</t>
+  </si>
+  <si>
+    <t>a8c7bcec-1a7f-46bd-9553-1875699fb4cb</t>
+  </si>
+  <si>
+    <t>a98d65ab-baa5-4cb3-b351-dff773fe0a9e</t>
+  </si>
+  <si>
+    <t>e4f871f6-8e7d-40c3-89bd-c4796734d877</t>
+  </si>
+  <si>
+    <t>ed28eba3-38a1-44a4-90a0-2e402284c9c3</t>
+  </si>
+  <si>
+    <t>93ff639f-791b-49ac-a795-cc241aca60a6</t>
+  </si>
+  <si>
+    <t>ac60623f-f1cb-4336-bf58-834b79f03023</t>
+  </si>
+  <si>
+    <t>6e64a0b9-bbb2-4acc-854c-1926772372d1</t>
+  </si>
+  <si>
+    <t>11a059d4-296e-4b0a-b883-b136826163e1</t>
+  </si>
+  <si>
+    <t>b10058e4-5c70-43e1-8e70-33d21791afee</t>
+  </si>
+  <si>
+    <t>96f30cc2-3764-418e-bba6-cc904f5fc7f7</t>
+  </si>
+  <si>
+    <t>a8fedd01-29a6-4e02-b225-990b75f527c0</t>
+  </si>
+  <si>
+    <t>04d497b0-317d-4f0c-a29b-dfee6cc9b1af</t>
+  </si>
+  <si>
+    <t>0910a672-f938-4fa0-a6f2-976b59956483</t>
+  </si>
+  <si>
+    <t>83a2cbd7-2555-45c3-bd37-115a37fe4f45</t>
+  </si>
+  <si>
+    <t>1f29a78d-9da2-4368-bd80-8f3ea823d464</t>
+  </si>
+  <si>
+    <t>29b9463f-f2bf-4583-b7c2-11adc7476f81</t>
+  </si>
+  <si>
+    <t>ff39f9f8-07ee-4a0c-bf67-70f7501b0dc5</t>
+  </si>
+  <si>
+    <t>d547fd43-f2c3-4b59-a26d-4b1f85599e84</t>
+  </si>
+  <si>
+    <t>0ac96154-f845-48d9-99ec-0b9c97bc98d4</t>
+  </si>
+  <si>
+    <t>bf287adb-ed87-41ff-ad96-d9f7f124ad64</t>
+  </si>
+  <si>
+    <t>9e960f58-72c3-4e50-99e9-fc30bf9f4749</t>
+  </si>
+  <si>
+    <t>d0d904c4-5961-43f8-8ee7-ea74c8775222</t>
+  </si>
+  <si>
+    <t>01da5d39-b4b3-473f-90a9-c9223953598c</t>
+  </si>
+  <si>
+    <t>acf84fab-d406-4a0d-a041-419d0275c69d</t>
+  </si>
+  <si>
+    <t>2c29f477-9f89-4da6-9004-3dc77f66330f</t>
+  </si>
+  <si>
+    <t>9a332b7d-0317-47a7-ac92-9d66970a7d86</t>
+  </si>
+  <si>
+    <t>bbcd54b0-7897-4623-aafb-017054f08edf</t>
+  </si>
+  <si>
+    <t>b79ad985-6623-47a3-ba17-c8e6c956f41e</t>
+  </si>
+  <si>
+    <t>6c5d016c-db3a-4d1c-98eb-7e8bef49ae51</t>
+  </si>
+  <si>
+    <t>64c43668-1c16-4dd0-a318-945d8421e8f8</t>
+  </si>
+  <si>
+    <t>a3ee44c9-42f5-4afa-9807-03b0240ea2e1</t>
+  </si>
+  <si>
+    <t>54616e96-30db-4e44-bc4d-c49117cefc3a</t>
+  </si>
+  <si>
+    <t>102a1db9-6ecc-4d09-add0-f21a2f8e9a4e</t>
+  </si>
+  <si>
+    <t>63f0bb6d-0552-40e1-9204-3e759278d487</t>
+  </si>
+  <si>
+    <t>bdfd3a25-91fd-4418-8481-1b69fa6b793a</t>
+  </si>
+  <si>
+    <t>c22ae7d5-cd7f-4883-b6d6-e77361a9eca9</t>
+  </si>
+  <si>
+    <t>6393dbbb-e8a7-431b-ae79-e4870cc59e52</t>
+  </si>
+  <si>
+    <t>2a52dcb9-e211-49f0-90dd-95a39b2c181f</t>
+  </si>
+  <si>
+    <t>803cd07c-271b-429b-a07a-94226eb2f8cb</t>
+  </si>
+  <si>
+    <t>42c37760-22b9-4040-a209-a46c9052212c</t>
+  </si>
+  <si>
+    <t>2ca78489-91fe-447f-a554-6a234ffa8322</t>
+  </si>
+  <si>
+    <t>1bd2a640-4bbf-46ef-849d-38c6ea3828c7</t>
+  </si>
+  <si>
+    <t>b7daa608-db48-4ca7-8efc-a7d5890107f1</t>
+  </si>
+  <si>
+    <t>3200c502-9c50-4039-8815-3d04a636973e</t>
+  </si>
+  <si>
+    <t>b6fff1dc-f1ba-4475-8254-6df16e573145</t>
+  </si>
+  <si>
+    <t>145170ee-c5b1-40bd-8a66-fb1aa9559857</t>
+  </si>
+  <si>
+    <t>bf934751-4c32-4a90-8e5e-0b2735b3234d</t>
+  </si>
+  <si>
+    <t>6405f4ae-0523-436c-b91d-5ab039f927b5</t>
+  </si>
+  <si>
+    <t>1db2c34e-522c-4fa1-a183-a7ff3db0e1d7</t>
+  </si>
+  <si>
+    <t>9adce9b6-8eca-406e-be89-7acd85171185</t>
+  </si>
+  <si>
+    <t>a48f6107-36b9-4ec1-a597-4a7f20bb0ef2</t>
+  </si>
+  <si>
+    <t>a26ef1cd-5628-4e9b-b706-c7330a5bb11f</t>
+  </si>
+  <si>
+    <t>b37bb4d1-7c0d-46c5-820b-2b8c3f2fce43</t>
+  </si>
+  <si>
+    <t>8dce6d44-9e0f-4ab8-b473-24d65b2e3f55</t>
+  </si>
+  <si>
+    <t>c231897d-73fa-4a66-9683-7b15d30beaaa</t>
+  </si>
+  <si>
+    <t>c917fe6f-738c-4f8c-bc4f-f3fcca99cc76</t>
+  </si>
+  <si>
+    <t>843f32fc-41ff-4b6e-be28-133bf88f9b65</t>
+  </si>
+  <si>
+    <t>3625004f-6ab2-4c56-8748-882ae0b161e1</t>
+  </si>
+  <si>
+    <t>0a6b5c94-787e-4b68-a1ef-6a25626f59ef</t>
+  </si>
+  <si>
+    <t>cb319f22-3d46-4039-acdd-a9c165120511</t>
+  </si>
+  <si>
+    <t>64b6de64-f343-4f4b-a90a-76a801520400</t>
+  </si>
+  <si>
+    <t>87b2b202-41c4-4d0f-be9c-60decd1e451c</t>
+  </si>
+  <si>
+    <t>32751de4-756b-453e-bc60-5bd4f862050a</t>
+  </si>
+  <si>
+    <t>560d49c9-786f-4c1c-bf25-fe5a78eb1064</t>
+  </si>
+  <si>
+    <t>3238ffed-bd33-436b-8781-a354c7d197c4</t>
+  </si>
+  <si>
+    <t>5b6f279c-b4a0-4669-b42f-d3634f4d48d3</t>
+  </si>
+  <si>
+    <t>d7e9d93a-4b67-4786-8814-8aa0feefaf9e</t>
+  </si>
+  <si>
+    <t>76116a90-1430-45f9-92cb-f060e758b354</t>
+  </si>
+  <si>
+    <t>cca2bbe1-a503-4e75-aa4b-1fd4b84e45f5</t>
+  </si>
+  <si>
+    <t>68b69369-387d-4b71-be40-cf8366f1f79b</t>
+  </si>
+  <si>
+    <t>749292ac-4019-43c8-b721-1481b2777f4c</t>
+  </si>
+  <si>
+    <t>eb5f64ac-f0be-47c5-8622-434f79f8a015</t>
+  </si>
+  <si>
+    <t>c070f040-419c-4700-95eb-4cd3f2ae7745</t>
+  </si>
+  <si>
+    <t>9644b4ea-a794-44c0-adb4-2dbca29ac115</t>
+  </si>
+  <si>
+    <t>4eee3a36-79c1-41e3-8b3e-c8fe248f1ff3</t>
+  </si>
+  <si>
+    <t>355a5067-9a3c-4a95-87f2-5d89ecbf0ec0</t>
+  </si>
+  <si>
+    <t>d802ecd4-d88b-4ac8-857f-03545b973a2e</t>
+  </si>
+  <si>
+    <t>9bd4291c-999b-4120-9af1-f424052a244d</t>
+  </si>
+  <si>
+    <t>95442059-9484-43d0-81bf-581abbb5d88a</t>
+  </si>
+  <si>
+    <t>7ebee5e3-2cc3-4af0-8f70-9b825cd9f6fd</t>
+  </si>
+  <si>
+    <t>7bf2911f-42fa-4fce-a80c-413ebf491037</t>
+  </si>
+  <si>
+    <t>ffb6b0ac-467b-40ee-9e9f-7dc2090b5caa</t>
+  </si>
+  <si>
+    <t>a0016f59-e8c1-4382-86e9-9298c01ff072</t>
+  </si>
+  <si>
+    <t>4d5da2b4-0737-4016-af77-4e239f9071c3</t>
+  </si>
+  <si>
+    <t>12d35a4f-7331-4dc6-afaa-eb6884296a91</t>
+  </si>
+  <si>
+    <t>1d56e282-8e97-4bd6-be7e-f2c7319a0c90</t>
+  </si>
+  <si>
+    <t>91862b5e-8f7c-427d-91cd-1d50df601b10</t>
+  </si>
+  <si>
+    <t>58a10f15-8593-4392-a238-047d88126e3b</t>
+  </si>
+  <si>
+    <t>b9b32d08-a6df-4349-8b76-ba7384d4f85d</t>
+  </si>
+  <si>
+    <t>5d1c71c4-7513-4abf-9ec3-46ee8a53d92f</t>
+  </si>
+  <si>
+    <t>a348a183-a548-4731-80f3-613214437d1f</t>
+  </si>
+  <si>
+    <t>4885b611-83d2-416f-a1ba-e5175535e3af</t>
+  </si>
+  <si>
+    <t>cb342ed8-df2b-4726-b18a-cf249f3fec31</t>
+  </si>
+  <si>
+    <t>c7cb6da6-5241-410c-b9e3-929f9eb32404</t>
+  </si>
+  <si>
+    <t>7d36523e-ec63-4cc8-80e0-cfc2c3505c46</t>
+  </si>
+  <si>
+    <t>d18102a5-986c-40a2-af53-74c264d5d97e</t>
+  </si>
+  <si>
+    <t>9880f09c-ab11-4d01-ae57-06e8208564c1</t>
+  </si>
+  <si>
+    <t>f5473a1b-02bd-4a03-a2e5-0a13cd2a394f</t>
+  </si>
+  <si>
+    <t>27145a40-9391-4697-bfb9-5fa0e118b576</t>
+  </si>
+  <si>
+    <t>6ee180b3-3c71-4b19-8b2a-505d631b20c5</t>
+  </si>
+  <si>
+    <t>8418bcfd-0b19-490b-88f2-8d64511d4a25</t>
+  </si>
+  <si>
+    <t>7dda387b-7c7a-4cd1-9846-4ccde454f111</t>
+  </si>
+  <si>
+    <t>2242847e-6355-40ff-9fff-c44e19750222</t>
+  </si>
+  <si>
+    <t>8d27c115-90fd-4737-8801-fdbdbb8bed0a</t>
+  </si>
+  <si>
+    <t>1cca39e0-8bb6-4637-80e4-aeaebd990bc0</t>
+  </si>
+  <si>
+    <t>27645f81-1de5-4344-ae25-dcb06a691a52</t>
+  </si>
+  <si>
+    <t>2981b055-8023-49a8-8cae-72cd9ac14027</t>
+  </si>
+  <si>
+    <t>e91e2519-9cba-4eec-8cd6-9764aa67e347</t>
+  </si>
+  <si>
+    <t>305ae574-8500-43c5-ad64-31f05e6c24f2</t>
+  </si>
+  <si>
+    <t>d80a2475-8fc0-4871-b30f-06a6998b62b4</t>
+  </si>
+  <si>
+    <t>99c87f2b-1f0d-4766-aaff-cd392a943766</t>
+  </si>
+  <si>
+    <t>ad4acc8e-21c5-411b-bbed-5d9a0b9565fd</t>
+  </si>
+  <si>
+    <t>57c44bd3-3852-4995-9971-8abf29d82b5e</t>
+  </si>
+  <si>
+    <t>fceaf1b6-29e9-4b5f-9830-bacdedbbad5e</t>
+  </si>
+  <si>
+    <t>baea87ee-7ab3-4d0b-ba64-4716968f302d</t>
+  </si>
+  <si>
+    <t>cb968ca5-5e2b-4d0a-a974-3f87bebaf4b6</t>
+  </si>
+  <si>
+    <t>aa1b4e1d-728d-4202-aecf-d388576e98c7</t>
+  </si>
+  <si>
+    <t>bc42ab3e-92c2-407b-b157-66690958984d</t>
+  </si>
+  <si>
+    <t>30fb4b6d-86a5-485a-abbb-313dafac42ab</t>
+  </si>
+  <si>
+    <t>c2d3f5e0-70ef-47a9-b4e1-da37be86b605</t>
+  </si>
+  <si>
+    <t>b6cf6439-c5e7-4bdb-af86-cd9f96d7f8bc</t>
+  </si>
+  <si>
+    <t>d035dfd0-f719-4843-9f51-d8d7563cac28</t>
+  </si>
+  <si>
+    <t>cfb8f3e3-23a2-49ea-935c-c92a673d4972</t>
+  </si>
+  <si>
+    <t>be47d0d1-3561-47df-9223-8f6c8512f7e2</t>
+  </si>
+  <si>
+    <t>91ef45d7-76e7-4b44-8ab4-cd1bb6a6457a</t>
+  </si>
+  <si>
+    <t>e6dcd986-dab0-48de-bd6b-2c0660ef136b</t>
+  </si>
+  <si>
+    <t>5d9b3eb0-204c-4e15-b143-7e0f44a6d7bf</t>
+  </si>
+  <si>
+    <t>b20d42f3-8efe-4e1f-a9ab-a3d9599bd67e</t>
+  </si>
+  <si>
+    <t>5048b0c0-e993-487f-8435-b8178d0e833e</t>
+  </si>
+  <si>
+    <t>3d805d8a-ccff-4891-832a-f42ad83e7111</t>
+  </si>
+  <si>
+    <t>83a72e67-a1ab-4679-bada-5c5295b5cd69</t>
   </si>
   <si>
     <t>Value NA in ASSISTANCE_REQUESTED not in allowed list ('YES','NO')</t>
   </si>
   <si>
-    <t>16899917-eecd-4635-8725-606e5f31be16</t>
-  </si>
-  <si>
-    <t>48181a68-0854-465f-88c9-0e22e04fecfa</t>
-  </si>
-  <si>
-    <t>21e682ba-4c7a-4af3-b111-40b5e9e3fd47</t>
-  </si>
-  <si>
-    <t>bcaac1cb-b6c5-4f92-9ad5-836778c07456</t>
-  </si>
-  <si>
-    <t>07a02f02-63b0-4b3b-b30f-b68265ad5861</t>
-  </si>
-  <si>
-    <t>0a0f9232-425e-47df-b2d1-df0560ee208d</t>
-  </si>
-  <si>
-    <t>ac7c52a5-025e-400c-81c1-fef571d3d998</t>
-  </si>
-  <si>
-    <t>b073fcdd-b71f-429e-b0f1-3aad865d577f</t>
-  </si>
-  <si>
-    <t>95b4f80d-dba3-4749-b821-5318423ea01a</t>
-  </si>
-  <si>
-    <t>a8f48410-3f0e-4db4-a86b-e0663c6d051e</t>
-  </si>
-  <si>
-    <t>c1ec72d4-ef29-4466-8e79-0ed12e6558fe</t>
-  </si>
-  <si>
-    <t>18efaacd-f900-4423-9d5a-32c4d7c909b1</t>
-  </si>
-  <si>
-    <t>114241c1-4a6c-4c5c-a462-6f92184acc61</t>
-  </si>
-  <si>
-    <t>e5e24fe9-c96a-46fe-8378-e3d023f9c03b</t>
-  </si>
-  <si>
-    <t>7bec8945-d2de-42e5-aedc-b4063a9ef1e3</t>
-  </si>
-  <si>
-    <t>f73d3a86-6ef3-40be-85f6-5db00a0a5d71</t>
-  </si>
-  <si>
-    <t>3eac893a-60d1-43ea-a3e3-1a772f4158bb</t>
-  </si>
-  <si>
-    <t>0e11ff0d-5d75-4952-a6b3-170a7c402562</t>
-  </si>
-  <si>
-    <t>e523f4f6-127a-4e27-a1be-ef747d3023eb</t>
-  </si>
-  <si>
-    <t>4e6174bf-7675-4116-bcd1-53a1aac2ae3e</t>
-  </si>
-  <si>
-    <t>eaedcf38-761d-4509-9243-1ee3c852b111</t>
-  </si>
-  <si>
-    <t>d064b055-5a1e-4a89-8734-9f52f3a35606</t>
-  </si>
-  <si>
-    <t>eea3e96d-fcbd-4798-9888-79075e80a9fb</t>
-  </si>
-  <si>
-    <t>cf98ab22-da3d-4da3-b918-5b5dd6b61fd9</t>
-  </si>
-  <si>
-    <t>c69a0aef-8cc3-4e30-9003-3ac816172f4b</t>
-  </si>
-  <si>
-    <t>644d2337-6102-43ea-b195-f27f3cc01cbe</t>
-  </si>
-  <si>
-    <t>0f4802d5-51c9-4ace-a974-d268df1970e6</t>
-  </si>
-  <si>
-    <t>1aa8dde9-6380-4073-90d2-e1caed1260cb</t>
-  </si>
-  <si>
-    <t>f617ab50-caed-4e55-befa-1083a8db549b</t>
-  </si>
-  <si>
-    <t>00e346ef-3e28-4a69-a3a7-ffb3d945b051</t>
-  </si>
-  <si>
-    <t>0a743264-f74e-4479-aa4c-dc9f3ba87f7f</t>
-  </si>
-  <si>
-    <t>d3fad977-474f-46d2-baea-304e48cfbde6</t>
-  </si>
-  <si>
-    <t>2470451f-929e-41c4-8ab8-40728361b434</t>
-  </si>
-  <si>
-    <t>b96037de-9910-467f-8f33-e52ffa1b254d</t>
-  </si>
-  <si>
-    <t>35b47d7d-ef5e-41bc-8672-21ce892c8486</t>
-  </si>
-  <si>
-    <t>6efb2092-8514-4568-ad86-654e1b6aa441</t>
-  </si>
-  <si>
-    <t>d0f60ed4-f905-4326-802a-0f63cc00dd46</t>
-  </si>
-  <si>
-    <t>02e19ed1-2376-4740-9ec4-c96e933c27c6</t>
-  </si>
-  <si>
-    <t>746d15e9-c38a-4340-a68a-f73cb2af61ed</t>
-  </si>
-  <si>
-    <t>27f54394-0737-4e59-a62a-bfd0aab32ce2</t>
-  </si>
-  <si>
-    <t>2e30b91a-8782-471c-a33b-5838e56cd732</t>
-  </si>
-  <si>
-    <t>9df1c277-fc7b-4ed8-82ab-58191e73e9ac</t>
-  </si>
-  <si>
-    <t>1292f261-3964-4371-a05f-ce5202525ac6</t>
-  </si>
-  <si>
-    <t>00995032-bb64-4748-8d42-a58aa528ac25</t>
-  </si>
-  <si>
-    <t>5bd30868-ccb1-420a-8ea5-588543f69b03</t>
-  </si>
-  <si>
-    <t>f3d6d1d3-ac54-4d03-8c45-c5beb9665275</t>
-  </si>
-  <si>
-    <t>0a0cae76-ffc5-419f-8fe9-0f33ca05c91b</t>
-  </si>
-  <si>
-    <t>56659399-1b47-466e-8dbb-f0d6cfdfa508</t>
-  </si>
-  <si>
-    <t>8a26fd96-3bcb-486c-886a-ebead4b98f1d</t>
-  </si>
-  <si>
-    <t>ebd37160-4510-432f-848e-d5d9e34ed21c</t>
-  </si>
-  <si>
-    <t>33ba86b2-fd91-4a6e-b911-29e514ade927</t>
-  </si>
-  <si>
-    <t>90812b32-17f1-4c53-9411-953ce08fbadc</t>
-  </si>
-  <si>
-    <t>1dc217b7-ca84-457b-8460-3e32a7e826fe</t>
-  </si>
-  <si>
-    <t>09c391ab-9f3a-439e-b7d7-6ab75879b46b</t>
-  </si>
-  <si>
-    <t>44875512-7148-41b0-9017-42e64560ecd2</t>
-  </si>
-  <si>
-    <t>84721eae-fb04-4db1-b6ce-a5aebf51301a</t>
-  </si>
-  <si>
-    <t>25207b0a-f238-46b6-84ad-6c8d4b0dcf83</t>
-  </si>
-  <si>
-    <t>5e2cda43-fd3e-4de4-85ea-6e664c43dda5</t>
-  </si>
-  <si>
-    <t>7c5cf17c-42dc-477d-bb04-279d4cf13f6f</t>
+    <t>a81ea571-e9e9-4cb2-8ded-add1fe77eaa0</t>
+  </si>
+  <si>
+    <t>3e6d7410-7bab-4719-bf6f-ff7f5e321d02</t>
+  </si>
+  <si>
+    <t>00b7bb88-9c40-45fb-ba1a-df0f49c3d817</t>
+  </si>
+  <si>
+    <t>2fdee946-c4f4-46ac-aab9-fe8a5bac588e</t>
+  </si>
+  <si>
+    <t>3cd1d54a-d3b9-4413-9ce8-f6b29bf3bd7a</t>
+  </si>
+  <si>
+    <t>2440e066-0085-451d-bff3-ec68c339dc01</t>
+  </si>
+  <si>
+    <t>66bcbbeb-c56c-4ef8-9ff9-b5208ef41446</t>
+  </si>
+  <si>
+    <t>c6be2714-860e-489f-94c9-673c4eed05c0</t>
+  </si>
+  <si>
+    <t>eb779c4a-acfd-47fe-b049-086c378503ed</t>
+  </si>
+  <si>
+    <t>6057b14e-c1e6-4a27-8aca-1bc287ec00d8</t>
+  </si>
+  <si>
+    <t>daedfab6-bf91-488f-8cc4-0c93e7269021</t>
+  </si>
+  <si>
+    <t>e4874016-a12b-4ae6-8a59-498e4e718061</t>
+  </si>
+  <si>
+    <t>20799606-e361-4484-871d-7e02002517f7</t>
+  </si>
+  <si>
+    <t>fff6de5d-a60a-4b8e-8cb2-52070a6ca5d3</t>
+  </si>
+  <si>
+    <t>bded1efc-c3f0-4a75-8884-180f6f6dc60d</t>
+  </si>
+  <si>
+    <t>51469c6a-1b60-471e-a0f1-6fc96f392522</t>
+  </si>
+  <si>
+    <t>d28dffb7-07e4-4a37-9466-54369983d1c3</t>
+  </si>
+  <si>
+    <t>60fd09d2-9926-499e-bbf8-60f447c7a7ea</t>
+  </si>
+  <si>
+    <t>ac73f958-aac5-48e7-a49b-e563ce2f7bd8</t>
+  </si>
+  <si>
+    <t>73279d26-95af-42f0-beb4-680d3561c74d</t>
+  </si>
+  <si>
+    <t>d871710b-69c0-46f5-a7bf-d0b8e33f5f80</t>
+  </si>
+  <si>
+    <t>723c4096-a9b3-4816-a467-457c8a78e119</t>
+  </si>
+  <si>
+    <t>d09d19e2-707a-409c-ac4f-15c61603979f</t>
+  </si>
+  <si>
+    <t>58faf8ea-6a15-4788-acd5-d125938fd449</t>
+  </si>
+  <si>
+    <t>32b9e95e-219d-4c1b-b8a8-8d3f3b57f7ed</t>
+  </si>
+  <si>
+    <t>1e344a1b-2129-41c9-9e50-e75d165349ce</t>
+  </si>
+  <si>
+    <t>e84bf4c1-7df1-44e1-9d4a-1cb8c8942c2f</t>
+  </si>
+  <si>
+    <t>71c77cbd-764f-4d49-b3df-02b172a2659c</t>
+  </si>
+  <si>
+    <t>34067f77-bd7f-4c7f-8d3f-6f90306a6c01</t>
+  </si>
+  <si>
+    <t>6696342c-a3bb-48c8-8840-186c4e6795de</t>
+  </si>
+  <si>
+    <t>86a29338-44eb-45fb-93e1-47326e147579</t>
+  </si>
+  <si>
+    <t>0857756e-a7b6-4f4c-a421-a546049384ba</t>
+  </si>
+  <si>
+    <t>c5894a7c-da58-47de-a7f6-7a7efb39be6d</t>
+  </si>
+  <si>
+    <t>80264d3e-d0e6-4386-9f24-4dba318090c8</t>
+  </si>
+  <si>
+    <t>0a47eea3-7e97-4158-acf0-d1dca5ad745c</t>
+  </si>
+  <si>
+    <t>34ade936-d50c-4b8d-b240-07708a10496a</t>
+  </si>
+  <si>
+    <t>16bdf127-c860-472c-990f-09c3a75d74c6</t>
+  </si>
+  <si>
+    <t>11564a2f-0eeb-4c03-86bf-c18ecd5c1102</t>
+  </si>
+  <si>
+    <t>370875c3-01d4-4a2c-9f2f-5dce37eff55f</t>
+  </si>
+  <si>
+    <t>1ed16ef2-7c36-486a-9c0f-c3564152f610</t>
+  </si>
+  <si>
+    <t>a67486e7-263a-4ca6-8b6d-0bb632281f51</t>
+  </si>
+  <si>
+    <t>5eb56ce5-933d-48a2-9c45-304be7dc1bec</t>
+  </si>
+  <si>
+    <t>9efe841a-e38c-4b05-a346-a615de2650a6</t>
+  </si>
+  <si>
+    <t>00fd8543-9059-4d39-a720-340139b2c3dd</t>
+  </si>
+  <si>
+    <t>553b6df8-dbef-4e40-b3da-5bf919296a97</t>
+  </si>
+  <si>
+    <t>e1449fa0-6f7c-4e48-866b-cb8f22172065</t>
+  </si>
+  <si>
+    <t>a15fc3f3-5a0c-42f0-8397-b1a168d7732b</t>
+  </si>
+  <si>
+    <t>d33eb40b-3861-4b37-91c6-ecfb3a73b865</t>
+  </si>
+  <si>
+    <t>da2bf171-ddc3-436d-9994-cb9a1f77871c</t>
+  </si>
+  <si>
+    <t>f6230d6b-fb26-4e98-8c33-86ec2c8295ea</t>
+  </si>
+  <si>
+    <t>1aa78e34-d587-47e3-a321-85f06fa7acd3</t>
+  </si>
+  <si>
+    <t>de6c6c68-ffec-4948-9b57-904a00f6b6ae</t>
+  </si>
+  <si>
+    <t>562df619-456c-4a51-9a6c-aa06db370dde</t>
+  </si>
+  <si>
+    <t>37818824-1eb0-4253-85b3-7f60a4177ffa</t>
+  </si>
+  <si>
+    <t>a47e2bcb-699d-45f6-b521-97b6475bf32b</t>
+  </si>
+  <si>
+    <t>39cc9eed-1173-4bc7-9ea0-6702473ac823</t>
+  </si>
+  <si>
+    <t>bdec8c69-e0ae-424b-a714-ea75048e8e0f</t>
+  </si>
+  <si>
+    <t>9a0ddb48-9d07-4e3c-91cd-6b38928e3d7b</t>
+  </si>
+  <si>
+    <t>7d076da4-9c99-4aab-9c0f-0b6cf70a4ff0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
feat: prepare for orchestration ingestion fs watch
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -66,19 +66,19 @@
     <t>elaboration:2</t>
   </si>
   <si>
-    <t>05e8feaa-0bed-5909-a817-39812494b361</t>
-  </si>
-  <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
   </si>
   <si>
-    <t>Session 05e8feaa-0bed-5909-a817-39812494b361 markdown diagnostics not provided (not completed?)</t>
+    <t>7bab389e-54af-5a13-a39f-079abdc73a48</t>
+  </si>
+  <si>
+    <t>Session 05269d28-15ae-5bd6-bd88-f949ccfa52d7 markdown diagnostics not provided (not completed?)</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx</t>
   </si>
   <si>
     <t>ERROR</t>
@@ -132,7 +132,7 @@
     <t>591191c7-f693-5957-8734-ac87151ca981</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-25-valid.xlsx</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-25-valid.xlsx</t>
   </si>
   <si>
     <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
@@ -153,7 +153,7 @@
     <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
   </si>
   <si>
     <t>a3fe7098-8ae8-5612-81ac-cbe10780c19b</t>
@@ -201,7 +201,7 @@
     <t>c302047e-21cf-5059-a32c-e81a9bd3a9b9</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
   </si>
   <si>
     <t>3252fee6-3a9a-5f4c-81c6-739201046d79</t>
@@ -249,13 +249,13 @@
     <t>0adb81bc-3df2-5f86-99cc-2d20e1dd5efd</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
   </si>
   <si>
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>14ec0063-7360-4d62-be4c-2f49738e623f</t>
+    <t>17843c58-37af-452e-b0bf-c9344cc4a18b</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -267,7 +267,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>6e9d04bb-4f75-4883-8639-20ae9b86180e</t>
+    <t>0a92581a-dec5-46cb-af86-7aafa636ff8d</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>30caaf6c-03b3-4c0d-8def-03af6b48e515</t>
+    <t>1c61c3d9-f2db-47d4-9749-1b36b377d8be</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>443f5916-49c0-4036-a957-77016ca8cc23</t>
+    <t>d9562870-0850-48cb-975a-85c582c89288</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>d4632564-4dc6-4961-a164-9b7b291d8760</t>
+    <t>38d66903-9b78-4151-a5cd-fa0e11d476d4</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>e28b592c-0f1a-4be1-94a7-943895a4176a</t>
+    <t>f532deaa-e41f-4315-976f-25365e8595a5</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>c6cb5fe2-8832-4f68-bfcc-66ccd8e55b17</t>
+    <t>aed4f471-ddad-429a-8cac-93094e9b20e8</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>8116555c-8307-4773-8b0e-e293c5d4dc04</t>
+    <t>43885a11-1961-4001-8aed-5572eec05074</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>85e71def-7059-4002-9cfb-f23de73e6417</t>
+    <t>08c627b8-3cf8-4560-9c8e-89beefee38ce</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>d02b7e19-a3ed-428c-96d1-87af9526d558</t>
+    <t>847ff20a-0686-4e95-a53b-747a70ae3948</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>5b3e8525-f32a-4787-bda0-9c1c3925efc7</t>
+    <t>6eed13f5-a146-4498-b33e-1228cf4b852b</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>df8cb8ef-e5f6-4ff2-81ee-c4e8b67b76df</t>
+    <t>a395d15e-2bfd-40b6-b69c-2c359d90ae87</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>9b151a91-f66d-424c-9415-dd53f54bfa48</t>
+    <t>eaf67770-2fb7-4855-bd5f-7be64a39f428</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>3f25232e-f6ee-40dc-96e9-bfd05436839b</t>
+    <t>a7c02631-3023-4ad3-a0e0-06701d1e65c0</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>4625e5be-dbe8-4926-88f2-4ae020a2d6df</t>
+    <t>3bf41967-9a22-4859-bf91-bfd1b82a802a</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>6a8a558c-7827-4b0b-82ce-41aaa2000dac</t>
+    <t>bdf91f6e-02a0-4a43-80a6-cfd902965e5d</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>83f4c510-032b-45bd-8748-58831f88ae38</t>
+    <t>32183022-6aec-46a2-9068-1efdb23ff741</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>f2ec62c5-6d98-4a28-8b41-2f3e9a98fef6</t>
+    <t>27af204a-d36f-44a6-9542-d6ee7b97275e</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>c8dba378-3986-49aa-bde4-3e66a7b799e1</t>
+    <t>acc7468f-7bc2-45dc-9c07-d7d489e7784e</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>ec9e6a0b-bd83-4d8f-83c9-197e6a3823a8</t>
+    <t>1946d1e7-a043-4263-bbb0-21f71f6ac997</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>8b46621d-0bbe-4d3f-a429-2a126c5fdf17</t>
+    <t>ef91eaf4-b32f-4ab9-8516-4d30a0b3a521</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -450,13 +450,13 @@
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-12-valid.csv</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-12-valid.csv</t>
   </si>
   <si>
     <t>ahc_hrsn_2023_12_12_valid</t>
   </si>
   <si>
-    <t>bf7580e1-db19-49b9-a246-8042e874e917</t>
+    <t>89a58da9-df99-42c3-b76a-fee16b2afa62</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -474,7 +474,7 @@
     <t>Use only allowed values '71802-3','96778-6' in QUESTION_CODE</t>
   </si>
   <si>
-    <t>d7bfe5ab-7d4d-45a2-8412-6d9cd37e1276</t>
+    <t>c7c06103-01a3-4dc2-9692-aa54b2563314</t>
   </si>
   <si>
     <t>Value 88122-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -483,7 +483,7 @@
     <t>88122-7</t>
   </si>
   <si>
-    <t>dcacec96-3e03-4750-b889-bf1aa5be2eaf</t>
+    <t>a0e3f342-c04c-4e3b-9550-d28702132752</t>
   </si>
   <si>
     <t>Value 88123-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -492,7 +492,7 @@
     <t>88123-5</t>
   </si>
   <si>
-    <t>4a65b050-9ff3-4402-8796-a2dce938eae8</t>
+    <t>d6cb33a7-9c17-4272-98c4-91085fe44fb0</t>
   </si>
   <si>
     <t>Value 93030-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -501,7 +501,7 @@
     <t>93030-5</t>
   </si>
   <si>
-    <t>4f6d275c-d68d-4d2d-bf51-d069b9ad8d55</t>
+    <t>29b8baec-dde3-49de-a272-59d9f8f2dc29</t>
   </si>
   <si>
     <t>Value 96779-4 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -510,7 +510,7 @@
     <t>96779-4</t>
   </si>
   <si>
-    <t>07508de0-5216-4155-96b6-66dab7e225df</t>
+    <t>98882e18-7bc8-4162-80d0-849c48f9341a</t>
   </si>
   <si>
     <t>Value 95618-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -519,7 +519,7 @@
     <t>95618-5</t>
   </si>
   <si>
-    <t>1670cdd4-53eb-49ce-81c1-5bdabe3a89eb</t>
+    <t>8b41abc1-ff92-496d-a8ff-91712209c47a</t>
   </si>
   <si>
     <t>Value 95617-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -528,7 +528,7 @@
     <t>95617-7</t>
   </si>
   <si>
-    <t>77cfa47f-5697-4993-aa78-56bd911fb347</t>
+    <t>b8b45cf2-5f1b-4102-af20-fb3b6148a697</t>
   </si>
   <si>
     <t>Value 95616-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -537,7 +537,7 @@
     <t>95616-9</t>
   </si>
   <si>
-    <t>fc58f097-cd42-4d17-a6f0-d564c45d6697</t>
+    <t>adf5776d-8785-4b00-b9bf-1498f36be75d</t>
   </si>
   <si>
     <t>Value 95615-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -546,7 +546,7 @@
     <t>95615-1</t>
   </si>
   <si>
-    <t>bc51a352-9d2e-47b7-8805-8cc56d7ff429</t>
+    <t>7e9dedf3-995a-4e36-b3ad-2139f1f990a1</t>
   </si>
   <si>
     <t>Value 76513-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -555,7 +555,7 @@
     <t>76513-1</t>
   </si>
   <si>
-    <t>c47237b7-e08d-46c1-bb9c-5232484e88b2</t>
+    <t>59de9820-bce8-4694-a50c-60238f5b6cdc</t>
   </si>
   <si>
     <t>Value 96780-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -564,7 +564,7 @@
     <t>96780-2</t>
   </si>
   <si>
-    <t>56778f4b-43b5-4d74-af88-c6032b360bfe</t>
+    <t>6d9fb301-17bd-4360-9e94-a41c76178c05</t>
   </si>
   <si>
     <t>Value 96781-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -573,7 +573,7 @@
     <t>96781-0</t>
   </si>
   <si>
-    <t>016bc7cd-06e8-4fe6-aa21-45463e9f8283</t>
+    <t>9e3d981f-4e7e-49e9-98ad-2352118f2c10</t>
   </si>
   <si>
     <t>Value 93159-2	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -582,7 +582,7 @@
     <t>93159-2	</t>
   </si>
   <si>
-    <t>5f22c57d-bde3-4df5-a673-84c1464507e9</t>
+    <t>06bee207-f171-493f-bac9-0f2595e99308</t>
   </si>
   <si>
     <t>Value 97027-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -591,7 +591,7 @@
     <t>97027-7</t>
   </si>
   <si>
-    <t>997f92ac-cebe-4aa2-a293-5ccee9d9bf1e</t>
+    <t>ac51bcdb-1729-42cc-a5e0-8cc052967dad</t>
   </si>
   <si>
     <t>Value 96782-8	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -600,7 +600,7 @@
     <t>96782-8	</t>
   </si>
   <si>
-    <t>33816771-a419-4f72-bf9a-22aea27299e6</t>
+    <t>8208472d-aab3-458d-8635-d2ba521a56aa</t>
   </si>
   <si>
     <t>Value 89555-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -609,7 +609,7 @@
     <t>89555-7</t>
   </si>
   <si>
-    <t>b8fb5dca-89af-4ae6-8b99-b3d128965b27</t>
+    <t>e808a3e6-0b6f-4d64-a7e9-1b689ecd7718</t>
   </si>
   <si>
     <t>Value 68516-4	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -618,7 +618,7 @@
     <t>68516-4	</t>
   </si>
   <si>
-    <t>2d0c71c3-87de-4296-b083-a0b65a072832</t>
+    <t>1bc09197-07ba-447f-a2cb-1a96f88b2593</t>
   </si>
   <si>
     <t>Value 68517-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -627,7 +627,7 @@
     <t>68517-2</t>
   </si>
   <si>
-    <t>f1ec6400-4dcb-4a2d-af5c-a3840376d25f</t>
+    <t>62477dc6-e4c8-46c8-9ac9-5ae4e13042e8</t>
   </si>
   <si>
     <t>Value 96842-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -636,7 +636,7 @@
     <t>96842-0</t>
   </si>
   <si>
-    <t>0dd88bbf-a190-4ae7-a3b2-7af71e0b4a9e</t>
+    <t>2e55d592-ee8e-40da-ab23-e8552bce17de</t>
   </si>
   <si>
     <t>Value 95530-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -645,7 +645,7 @@
     <t>95530-2</t>
   </si>
   <si>
-    <t>6cef0fe9-49fc-4fee-8980-543be3096482</t>
+    <t>a52cb32c-4978-4067-b1d2-cf4cc4bb1a7d</t>
   </si>
   <si>
     <t>Value 68524-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -654,7 +654,7 @@
     <t>68524-8</t>
   </si>
   <si>
-    <t>f6b0b9c1-2292-44f4-8fcb-e195a9850c67</t>
+    <t>619ffaf9-c38e-40fa-b85b-e499b2de57b1</t>
   </si>
   <si>
     <t>Value 44250-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -663,7 +663,7 @@
     <t>44250-9</t>
   </si>
   <si>
-    <t>ca23be51-73d4-4944-bfe5-8c2cb7c4c0ca</t>
+    <t>d66ce610-6f17-43d4-bea6-5d017c21b78d</t>
   </si>
   <si>
     <t>Value 44255-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -672,7 +672,7 @@
     <t>44255-8</t>
   </si>
   <si>
-    <t>e68affc6-37e8-4a92-a3d3-44d3a91d3bdf</t>
+    <t>d05e89d4-756c-4c0f-b347-bb553c75a658</t>
   </si>
   <si>
     <t>Value 93038-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -681,7 +681,7 @@
     <t>93038-8</t>
   </si>
   <si>
-    <t>f3002fad-585b-4cb6-8dc8-080fc8f3dd52</t>
+    <t>4766624d-ae36-45b9-8bfe-635d8ec19293</t>
   </si>
   <si>
     <t>Value 69858-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -690,7 +690,7 @@
     <t>69858-9</t>
   </si>
   <si>
-    <t>6b4efeee-4ef8-475f-b23b-e3e5bc564b1b</t>
+    <t>183e7b05-a7fc-4c36-a27c-b8977b0b0871</t>
   </si>
   <si>
     <t>Value 69861-3	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -699,7 +699,7 @@
     <t>69861-3	</t>
   </si>
   <si>
-    <t>9de688ba-1689-42e8-be03-ff743ab3532d</t>
+    <t>db64ac39-6a9d-4c3b-bcae-fe0c36afb29d</t>
   </si>
   <si>
     <t>Value false in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -714,7 +714,7 @@
     <t>Use only allowed values 'TRUE','FALSE' in NEED_INDICATED</t>
   </si>
   <si>
-    <t>9691e872-a4c3-4bde-8856-3fb0ecd68842</t>
+    <t>d84afcf9-a556-408e-89ca-8794030bf58e</t>
   </si>
   <si>
     <t>Value true in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -723,82 +723,82 @@
     <t>true</t>
   </si>
   <si>
-    <t>532da32b-d5c7-43b6-a552-e48fa6380647</t>
-  </si>
-  <si>
-    <t>c006148d-119e-44b2-87ac-b46ed05758d5</t>
-  </si>
-  <si>
-    <t>07b724b5-9a90-4aa2-86be-10fc5924ba28</t>
-  </si>
-  <si>
-    <t>3b675de0-1e34-4af2-830e-fdd0bc69cd08</t>
-  </si>
-  <si>
-    <t>84df1af5-1ac1-4dae-8e8a-510d62655cb0</t>
-  </si>
-  <si>
-    <t>cc7054ef-59a3-4ddf-beb2-cd77692fb48e</t>
-  </si>
-  <si>
-    <t>e15080a2-d606-46bb-b50f-88b7d86bbd30</t>
-  </si>
-  <si>
-    <t>a9b62951-e355-44bc-8b5b-7ef60815964f</t>
-  </si>
-  <si>
-    <t>cfec4c9b-a179-4c66-8423-91ed77f95615</t>
-  </si>
-  <si>
-    <t>59430f20-be6b-4c56-8e74-08e823db6a59</t>
-  </si>
-  <si>
-    <t>e9c7fb96-3d04-40de-948a-7e7dde9cd97c</t>
-  </si>
-  <si>
-    <t>f9550486-ac29-4300-a971-7a2bffc156ec</t>
-  </si>
-  <si>
-    <t>80241bb7-acf3-4812-8ec2-42ec79d5ad37</t>
-  </si>
-  <si>
-    <t>c0eff7f1-08e3-4974-8e44-0032826f0688</t>
-  </si>
-  <si>
-    <t>c614a04b-51cd-4c15-b83e-ebff802545c6</t>
-  </si>
-  <si>
-    <t>8e2fbb3e-c4a9-487e-aec7-5e0ff3985128</t>
-  </si>
-  <si>
-    <t>b3870cf7-a3ed-46be-9089-6715016216cc</t>
-  </si>
-  <si>
-    <t>df53d0e6-86b3-4c00-9475-ebadcaa6346b</t>
-  </si>
-  <si>
-    <t>277a8288-5e78-49e7-be55-e732ce0552b8</t>
-  </si>
-  <si>
-    <t>aba1dd8b-7607-4ec9-b60a-41c90df63a19</t>
-  </si>
-  <si>
-    <t>87c58629-b4ca-4f25-9457-329c9af7d3c3</t>
-  </si>
-  <si>
-    <t>62d5abf7-679a-4fca-a3f4-d3f7ca55fd7b</t>
-  </si>
-  <si>
-    <t>855321f0-faa7-4cab-99ed-f3de993f1b66</t>
-  </si>
-  <si>
-    <t>fff6a39e-e4dc-429d-84cb-77c9e320ed2e</t>
-  </si>
-  <si>
-    <t>acce33c6-f021-494a-956e-2ec710bc1bfe</t>
-  </si>
-  <si>
-    <t>a27cd1db-8bef-4aa0-82ad-a9ccccff2443</t>
+    <t>5c5360f0-6375-44a0-affb-0b9d552d5a8a</t>
+  </si>
+  <si>
+    <t>3bdbf3dc-59d4-4852-a337-912975f7ae6d</t>
+  </si>
+  <si>
+    <t>3fa03bd0-30a7-439c-a5b0-34512397ca6f</t>
+  </si>
+  <si>
+    <t>80a6af0a-9fc2-4bf8-bdf4-4e232212eca4</t>
+  </si>
+  <si>
+    <t>f1d0d809-e010-4186-95a8-ee9878dc0f9f</t>
+  </si>
+  <si>
+    <t>1f16d526-7339-494f-aab4-3875d148b6c3</t>
+  </si>
+  <si>
+    <t>2ea57ef8-5310-4130-a2f3-242d2fb80ba2</t>
+  </si>
+  <si>
+    <t>9b42b1a0-8546-4b7c-8ace-4f8eb3df86aa</t>
+  </si>
+  <si>
+    <t>84c02511-9f22-43e7-bb7d-d2aef579d770</t>
+  </si>
+  <si>
+    <t>5cf87805-b8c0-4e69-899e-55f339f2b6eb</t>
+  </si>
+  <si>
+    <t>d226e490-a5ff-428e-9518-0a1dffcbe3bb</t>
+  </si>
+  <si>
+    <t>3995a99e-9eee-41e6-b7bb-8e2da0d24914</t>
+  </si>
+  <si>
+    <t>bfcff5a9-6894-4399-9192-92de2c62b2a2</t>
+  </si>
+  <si>
+    <t>dee8dced-3caf-4f36-929a-d2123cabf98a</t>
+  </si>
+  <si>
+    <t>e8797b8b-3555-4c05-b6fe-d30a6733baeb</t>
+  </si>
+  <si>
+    <t>e8660fe8-7fd4-4227-a735-95987aeca07c</t>
+  </si>
+  <si>
+    <t>e68c6908-94c8-49df-b266-b9d5229d0eaf</t>
+  </si>
+  <si>
+    <t>892911e3-4612-4a19-a87e-409c086c3260</t>
+  </si>
+  <si>
+    <t>43ca2da9-9eb7-40f1-98e4-5f6f2bd7e4a1</t>
+  </si>
+  <si>
+    <t>7a8dd1c4-ee17-48ba-b5f1-5fa86ca61868</t>
+  </si>
+  <si>
+    <t>ef555323-7236-473e-86c1-5d7496d5742e</t>
+  </si>
+  <si>
+    <t>9a64f9e2-02dd-4e3b-88fd-816e327f4547</t>
+  </si>
+  <si>
+    <t>5efc1d85-305d-4dd5-af3e-d5916567aaa0</t>
+  </si>
+  <si>
+    <t>dc5ff1f0-6458-4395-ad43-6f48fd64bccd</t>
+  </si>
+  <si>
+    <t>8b45852d-cbe1-422c-ac53-1a6964613ef0</t>
+  </si>
+  <si>
+    <t>57256237-8c6e-4d22-b567-45898b75de45</t>
   </si>
   <si>
     <t>Value false in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -810,88 +810,88 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_PART_2_FLAG</t>
   </si>
   <si>
-    <t>4e26ce61-8b36-4760-9e7e-0e7bf26d9b61</t>
-  </si>
-  <si>
-    <t>d6152c6a-e576-4f98-82e3-ffa728cef819</t>
-  </si>
-  <si>
-    <t>99541add-5bbe-4494-b93d-ec4c161a2158</t>
-  </si>
-  <si>
-    <t>01d10c12-1e92-49fc-94cc-efec8745ad48</t>
-  </si>
-  <si>
-    <t>9bd6b31a-c02c-4537-9a84-d51ad94c3f43</t>
-  </si>
-  <si>
-    <t>f847b89b-f104-40b7-8e18-2382bb548bc6</t>
-  </si>
-  <si>
-    <t>b7227633-e8bd-45a7-a2ee-3607f7e37238</t>
-  </si>
-  <si>
-    <t>f6735c18-f409-4186-9f51-c3fbc3443108</t>
-  </si>
-  <si>
-    <t>db93b0de-94cc-4046-abf2-f53a930897fb</t>
-  </si>
-  <si>
-    <t>aafcfbdf-8fd4-41e4-9f59-6c1d0d61b4a6</t>
-  </si>
-  <si>
-    <t>3750a0c0-1e16-47aa-a856-2b07857a6d09</t>
-  </si>
-  <si>
-    <t>13f8b0e1-7367-4142-bec8-a9f562b95410</t>
-  </si>
-  <si>
-    <t>b6696ede-9b75-457c-89c9-87756da47b2f</t>
-  </si>
-  <si>
-    <t>dbefcd27-0ba4-4a16-9e89-6aae065bc703</t>
-  </si>
-  <si>
-    <t>a703665d-d7bd-458b-9122-e6e819c3353a</t>
-  </si>
-  <si>
-    <t>6f02b2f4-aff6-4ed6-87aa-cdf647c4c280</t>
-  </si>
-  <si>
-    <t>5f92a6cb-7e24-452e-b406-556e2d7895a9</t>
-  </si>
-  <si>
-    <t>44641ffc-c997-434c-aae7-729e564b28d6</t>
+    <t>e506eae1-b00e-4b33-8b79-79703aa0f376</t>
+  </si>
+  <si>
+    <t>ddb9cc13-26c9-4b4f-9641-12ff1f35949f</t>
+  </si>
+  <si>
+    <t>9d834fe8-4025-4946-9b8c-6d7fbff0fd3f</t>
+  </si>
+  <si>
+    <t>a48d4e41-18cc-4177-a18c-d43280d75092</t>
+  </si>
+  <si>
+    <t>2c84e46e-a24b-4c1a-b884-c7353e5dd3af</t>
+  </si>
+  <si>
+    <t>2fd2b503-3f2b-458f-ad99-751c698ab140</t>
+  </si>
+  <si>
+    <t>b06863e8-f899-412e-ba7f-21164b582bf1</t>
+  </si>
+  <si>
+    <t>b1b36f69-3658-4ba2-872e-891affef3386</t>
+  </si>
+  <si>
+    <t>6305d06d-989f-4465-aba1-7a9cce4aace2</t>
+  </si>
+  <si>
+    <t>b4156a2b-5d30-4e0e-b97e-524fd115c092</t>
+  </si>
+  <si>
+    <t>f239a9ba-28db-4cdd-b452-e9e9ee8c3db1</t>
+  </si>
+  <si>
+    <t>7b2d0185-8fae-4656-af9f-44f04cbf6694</t>
+  </si>
+  <si>
+    <t>fc3abcad-e617-438d-bd80-7004f48fe803</t>
+  </si>
+  <si>
+    <t>4dcb099d-ea04-4c72-8825-9ee33e6e7fe4</t>
+  </si>
+  <si>
+    <t>dbe5d442-5564-46b5-911a-4a222ba3a151</t>
+  </si>
+  <si>
+    <t>541f4528-591c-4d3a-b638-11890686723c</t>
+  </si>
+  <si>
+    <t>a7d916bd-d667-4286-8507-48ec50609c04</t>
+  </si>
+  <si>
+    <t>dbdafaaa-9b17-4f9d-a120-64b7415b3afe</t>
   </si>
   <si>
     <t>Value true in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>bca6eb55-efb5-4462-9eba-92a20a1f0783</t>
-  </si>
-  <si>
-    <t>8a14b893-a9f6-4da9-a1cb-1ec971073bda</t>
-  </si>
-  <si>
-    <t>13d2a611-6c16-45b4-b981-a00612b73e65</t>
-  </si>
-  <si>
-    <t>65e85ac9-a671-4bd7-8592-c5da9e1c366f</t>
-  </si>
-  <si>
-    <t>d464f746-ca7d-4f0c-b00b-461800dea81e</t>
-  </si>
-  <si>
-    <t>2163ac01-1018-4b1b-928c-eb1751367a69</t>
-  </si>
-  <si>
-    <t>01ab071d-8014-4b50-a430-b284e2474e99</t>
-  </si>
-  <si>
-    <t>c8fbf66b-adac-495c-932a-359ce5280bb7</t>
-  </si>
-  <si>
-    <t>fcf78422-0d38-4a3b-8c38-7b5cb0730df0</t>
+    <t>98c1c338-7af1-449c-ba12-a727d2522993</t>
+  </si>
+  <si>
+    <t>0ab71565-f1ea-4eeb-9295-6ae1e53dff51</t>
+  </si>
+  <si>
+    <t>5cb26a8a-110d-400b-b158-de8c5321588a</t>
+  </si>
+  <si>
+    <t>c315c9b2-374a-4e16-a323-42718f345c4e</t>
+  </si>
+  <si>
+    <t>2566b618-5c8c-46ef-a985-0e0dd1295953</t>
+  </si>
+  <si>
+    <t>ebc58797-ed8f-4227-b65e-0e301a265afe</t>
+  </si>
+  <si>
+    <t>24002e76-2637-4212-8d1b-18276fdc855f</t>
+  </si>
+  <si>
+    <t>014a0d29-b9f9-4359-ba37-eea733062058</t>
+  </si>
+  <si>
+    <t>20030643-c1d4-4c0a-bbf8-923c17e6860a</t>
   </si>
   <si>
     <t>Value false in VISIT_OMH_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -903,85 +903,85 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OMH_FLAG</t>
   </si>
   <si>
-    <t>e7bfa653-9134-44f0-9591-72bb7c2e7e36</t>
-  </si>
-  <si>
-    <t>fb3d4ebb-309e-4a5e-a75c-042544c51cbc</t>
-  </si>
-  <si>
-    <t>d0d6c95b-7c0c-49de-8931-5537e5855623</t>
-  </si>
-  <si>
-    <t>e9e0d8f8-0825-465f-8986-8e5eab8441cb</t>
-  </si>
-  <si>
-    <t>066317b0-03ec-4be1-8b12-86e913f400cd</t>
-  </si>
-  <si>
-    <t>a83c2c9f-68f0-4627-ac7f-48f60a4a2a89</t>
-  </si>
-  <si>
-    <t>0d8a47fa-f9de-4646-b846-ecee263f0ef0</t>
-  </si>
-  <si>
-    <t>3a35dc46-1907-4aa3-af3f-ebbf0988e55c</t>
-  </si>
-  <si>
-    <t>7490f57b-5e20-475e-aa64-c14a748beb10</t>
-  </si>
-  <si>
-    <t>5c80ad05-4ffa-4b9c-9cad-f28100d558f5</t>
-  </si>
-  <si>
-    <t>1b2eb20f-2a39-4ce2-b3af-034eed4130d6</t>
-  </si>
-  <si>
-    <t>df4aaca7-b299-46b4-91b7-f6ddf3f9d345</t>
-  </si>
-  <si>
-    <t>bd776ee8-56de-42f7-983d-9a0e6e9f0f55</t>
-  </si>
-  <si>
-    <t>3e03b210-2358-40cd-9777-844151841617</t>
-  </si>
-  <si>
-    <t>3296a73d-9a98-490f-b664-53f13a02f3ac</t>
-  </si>
-  <si>
-    <t>0de23669-60cc-4098-9a7e-774f631a78f7</t>
-  </si>
-  <si>
-    <t>c7c406ff-7de6-4490-bddc-21c2ab27a2a7</t>
-  </si>
-  <si>
-    <t>6a738b1e-91e4-4b2b-ba07-6b28988ce878</t>
-  </si>
-  <si>
-    <t>7c2bed61-be6c-4611-85a5-4ab673f2e8df</t>
-  </si>
-  <si>
-    <t>fd0e1e13-24b3-4cf3-ad94-80db90d8c807</t>
-  </si>
-  <si>
-    <t>dd9f5a76-e49d-4651-ad5f-fd71c16e8b0e</t>
-  </si>
-  <si>
-    <t>c261709c-4144-4d3b-af2a-826196a562c4</t>
-  </si>
-  <si>
-    <t>293c374d-a8fc-44cb-a5c9-5960faf0805a</t>
-  </si>
-  <si>
-    <t>35a270e2-6332-4085-8f55-d3b1bff3dd9d</t>
-  </si>
-  <si>
-    <t>3435e18e-d959-4a7e-bdd6-de4111b37bd3</t>
-  </si>
-  <si>
-    <t>5d0e915a-5823-4efc-8fa5-98e1e6d315eb</t>
-  </si>
-  <si>
-    <t>2403b547-a1aa-484d-a33f-e1dad268f89d</t>
+    <t>ed2ab7b2-a7dc-4a41-a7db-c173fc95f918</t>
+  </si>
+  <si>
+    <t>e1ff200e-740c-4b14-a100-486bf0701bd6</t>
+  </si>
+  <si>
+    <t>659721b1-02ab-405f-890b-5e01ecb29277</t>
+  </si>
+  <si>
+    <t>15924218-8df9-4aae-b4f0-05c2bea986c4</t>
+  </si>
+  <si>
+    <t>7391a520-72b3-4017-9707-16f7dff6a1a6</t>
+  </si>
+  <si>
+    <t>9d6d80a4-4509-4bbf-b464-6dc6d9237f5b</t>
+  </si>
+  <si>
+    <t>0d755d21-b40e-452b-9523-535726b8bc28</t>
+  </si>
+  <si>
+    <t>9691a743-0cca-489a-bf1b-d792fa25564f</t>
+  </si>
+  <si>
+    <t>22d84121-b050-43cd-94f9-c4c1bd6c8935</t>
+  </si>
+  <si>
+    <t>ea39fa8d-74a5-458e-ba72-ce9973491ac3</t>
+  </si>
+  <si>
+    <t>e2acc918-b8e4-4a4a-8302-c8e97a9211ad</t>
+  </si>
+  <si>
+    <t>24ab0104-cd26-46f4-8ea0-d2818068510f</t>
+  </si>
+  <si>
+    <t>95c0492e-041b-418b-bfeb-14a1e1186659</t>
+  </si>
+  <si>
+    <t>8f9c0aea-70b7-416f-8eea-22087a702e38</t>
+  </si>
+  <si>
+    <t>3a47254f-441a-44df-958d-d3466b8235e6</t>
+  </si>
+  <si>
+    <t>94ca6c28-b324-42d8-9329-781e3ba71f43</t>
+  </si>
+  <si>
+    <t>08939bcd-0abc-44c4-8c68-559969d59082</t>
+  </si>
+  <si>
+    <t>271831a4-b175-4a48-a173-8e42a6024ae9</t>
+  </si>
+  <si>
+    <t>0e2edefd-b282-4f60-8b35-5d0d6ece4452</t>
+  </si>
+  <si>
+    <t>630a6eae-1b5b-4adf-82bc-44484bd4c047</t>
+  </si>
+  <si>
+    <t>999831ba-914b-4b33-8fda-831f800a17ad</t>
+  </si>
+  <si>
+    <t>f8fda3f7-56c3-48ae-878d-0952adb674b3</t>
+  </si>
+  <si>
+    <t>97063eee-9ce7-44a6-9ba1-781c7dfa464f</t>
+  </si>
+  <si>
+    <t>a946323a-23de-4eff-9bfc-5bc6e49d4740</t>
+  </si>
+  <si>
+    <t>c997e735-9326-4805-9ea8-2e4ffb727131</t>
+  </si>
+  <si>
+    <t>72e6ab00-eb68-4f5a-ab6d-1d1b54b7e406</t>
+  </si>
+  <si>
+    <t>52131706-0693-4472-9056-fc17fdc378f1</t>
   </si>
   <si>
     <t>Value false in VISIT_OPWDD_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -993,94 +993,94 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OPWDD_FLAG</t>
   </si>
   <si>
-    <t>3a2d1d25-7119-48a4-b1c5-c7592c57dd2d</t>
-  </si>
-  <si>
-    <t>ee7cc3e7-d7d1-4d81-849b-17e963b95805</t>
-  </si>
-  <si>
-    <t>068a6af7-aee0-426c-ae43-fa7ccf15b953</t>
-  </si>
-  <si>
-    <t>bc914fd7-6c19-49a6-8564-2815ac85dc86</t>
-  </si>
-  <si>
-    <t>072adcd8-eeaf-4d2a-9bd9-04b772c28318</t>
-  </si>
-  <si>
-    <t>d5a9d024-4c89-4d21-896e-93a137e3b763</t>
-  </si>
-  <si>
-    <t>2af4fc60-1ddb-4c3d-8095-d08f042602a4</t>
-  </si>
-  <si>
-    <t>d6becdbc-ff60-4bfc-ab19-b4a1c5a8c0df</t>
-  </si>
-  <si>
-    <t>a14f6919-48b5-40dc-9758-f31d6b40014d</t>
-  </si>
-  <si>
-    <t>3e5c6126-7845-4780-886d-a98457fab9fc</t>
-  </si>
-  <si>
-    <t>b46433ee-8dfa-4a1d-b508-1b65d24a41c8</t>
-  </si>
-  <si>
-    <t>68528729-9373-42c0-a5f6-7b21bdcf379b</t>
-  </si>
-  <si>
-    <t>509e1d69-7c56-4dcb-9b8b-521e7d4adba0</t>
-  </si>
-  <si>
-    <t>39ccb274-092f-426d-a272-ebe9873be003</t>
-  </si>
-  <si>
-    <t>f3698f3d-e146-4946-bac4-50b614d91081</t>
-  </si>
-  <si>
-    <t>e4d90173-35dd-48d3-9100-7cd5f08d8831</t>
-  </si>
-  <si>
-    <t>bcd0e33d-6457-41a7-9c33-9e0ceba77fe6</t>
-  </si>
-  <si>
-    <t>96083645-4cbf-4897-9b40-a7384e7da0af</t>
-  </si>
-  <si>
-    <t>a5715e74-0c8e-4c5f-ad88-4c0f62d6df44</t>
-  </si>
-  <si>
-    <t>dba97425-67d4-491a-ace7-3f8d3e924001</t>
-  </si>
-  <si>
-    <t>a995802d-fbf9-4e7b-a6d7-05b7b111eccb</t>
-  </si>
-  <si>
-    <t>7dee9a10-9734-4b04-a171-cf3132522d74</t>
-  </si>
-  <si>
-    <t>2c49db87-79b6-421c-88fe-0ca5239faaff</t>
-  </si>
-  <si>
-    <t>7ac82e84-91ed-401f-970e-103deab42c90</t>
-  </si>
-  <si>
-    <t>92200336-6da8-42de-bf12-9995f411a504</t>
-  </si>
-  <si>
-    <t>6d354ad0-c99b-46d7-9134-06661ff06337</t>
+    <t>f6c35bcc-c382-4841-90a5-93d871af4c3a</t>
+  </si>
+  <si>
+    <t>d7f90076-a178-430a-8bcc-2df768552a81</t>
+  </si>
+  <si>
+    <t>a8c90640-ad29-48e9-b69b-ba2d5362b5f2</t>
+  </si>
+  <si>
+    <t>97c9e81b-1710-4bad-9a08-eeada19821f3</t>
+  </si>
+  <si>
+    <t>470684a2-20d0-430e-a8cb-b8f53aee6ed8</t>
+  </si>
+  <si>
+    <t>964aeb1e-f7a0-447c-a970-4dbf23a94507</t>
+  </si>
+  <si>
+    <t>bde06c67-16b6-4064-9ed5-9bcd51073561</t>
+  </si>
+  <si>
+    <t>f4164dc2-db4f-4480-87e0-31f4d43a99ce</t>
+  </si>
+  <si>
+    <t>67c7f9b9-4534-4532-a409-734aa8deca9a</t>
+  </si>
+  <si>
+    <t>586f298e-1cd2-41b3-b899-752d5bc91257</t>
+  </si>
+  <si>
+    <t>c567371b-1e91-4a7f-8a8c-7780a4f34376</t>
+  </si>
+  <si>
+    <t>fe6e972c-e8fd-44bc-8dc4-e9ad92daf0a3</t>
+  </si>
+  <si>
+    <t>620e21a6-d994-4cb7-82a8-4bc6e4706e1d</t>
+  </si>
+  <si>
+    <t>6976077c-99ef-4134-8e50-8554c4b7dc8c</t>
+  </si>
+  <si>
+    <t>d69e8517-1055-461f-a29f-218c713e770e</t>
+  </si>
+  <si>
+    <t>ffc205f6-18e3-4159-88e3-bb584ff03d2d</t>
+  </si>
+  <si>
+    <t>5d19ce3a-4fe6-433f-9060-eb22401f86cc</t>
+  </si>
+  <si>
+    <t>2a0ebcd7-fd16-4763-a79f-1751cc5c4c47</t>
+  </si>
+  <si>
+    <t>a0091998-cc46-4a05-8f30-1639db791c87</t>
+  </si>
+  <si>
+    <t>705034d9-6803-4333-89c9-f6009a554304</t>
+  </si>
+  <si>
+    <t>68d76074-9074-4523-8780-72a9462f6631</t>
+  </si>
+  <si>
+    <t>a0c4b587-2836-4635-935e-68828776ed69</t>
+  </si>
+  <si>
+    <t>52ad3ae7-dc25-42b6-a2e1-b799fc1c473a</t>
+  </si>
+  <si>
+    <t>3e218b23-e99c-4e0c-a9bf-e3ae7c72a4c6</t>
+  </si>
+  <si>
+    <t>e746683d-88ee-44d6-9d25-2b63c4633625</t>
+  </si>
+  <si>
+    <t>ae90c72b-7e19-4740-8e26-9a586603ea22</t>
   </si>
   <si>
     <t>2afb3098-bcfd-5a54-8ebb-4d65d399c55e</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2024-01-25-valid.xlsx</t>
+    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2024-01-25-valid.xlsx</t>
   </si>
   <si>
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>643d07ef-94e3-4e21-bcae-a06e9c5d5ecf</t>
+    <t>c6b9bfcb-6a70-4953-b237-71d5b5ebfa78</t>
   </si>
   <si>
     <t>Value 	20430005 in SEXUAL_ORIENTATION_CODE not in allowed list ('42035005','20430005','38628009','OTH','UNK')</t>
@@ -1101,7 +1101,7 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>4ab9aef8-9b0c-43e8-9f64-e4f8b9374608</t>
+    <t>1d96dfd3-050f-4985-a7ab-4d14a4d0dd0a</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -1116,16 +1116,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>2b7908ba-a2df-4370-9daf-6e36705373bf</t>
-  </si>
-  <si>
-    <t>edb06f65-2c77-4387-b17a-8a3d8b9f23fa</t>
-  </si>
-  <si>
-    <t>a81db5f5-cbc1-43b6-a7a1-70a98d172900</t>
-  </si>
-  <si>
-    <t>b79b5d17-8798-4a03-9287-143d5bc95184</t>
+    <t>07059d07-4a45-4012-a233-cbf818a935e1</t>
+  </si>
+  <si>
+    <t>c2ccbc63-3294-4df6-b4a2-516dc4909288</t>
+  </si>
+  <si>
+    <t>72e0854e-f751-4968-9fc9-7cb27768ceb3</t>
+  </si>
+  <si>
+    <t>d3c24e24-e8fd-46f8-af92-40b2c4dba5f5</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -1137,16 +1137,16 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>4eab8df1-814c-4d07-93e8-64e040077f15</t>
-  </si>
-  <si>
-    <t>e3f50c6e-dfd0-415f-a3f3-6adc8e245723</t>
-  </si>
-  <si>
-    <t>f37a2977-08ef-45b7-9a32-055dfeeda462</t>
-  </si>
-  <si>
-    <t>984823b3-5b3b-4668-8d78-874dfd3f8598</t>
+    <t>e1b6190c-38bd-418f-a1ba-8fbfc5a7b575</t>
+  </si>
+  <si>
+    <t>9c83dbe1-fb40-428c-a3f4-7d76ed833129</t>
+  </si>
+  <si>
+    <t>005fdf80-24f2-4682-9c61-c80544c7f587</t>
+  </si>
+  <si>
+    <t>effb11b5-9bdf-498d-9302-a5ab23410e26</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -1155,16 +1155,16 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>daaea8b7-1583-4ff3-a0ca-a8a309973caa</t>
-  </si>
-  <si>
-    <t>9ef8f528-d4e2-478d-a22a-b67cf9ac8f47</t>
-  </si>
-  <si>
-    <t>91b2ded0-fc04-4e01-af19-85c39d556575</t>
-  </si>
-  <si>
-    <t>3053f961-dca4-4c5a-a194-3cef7422093d</t>
+    <t>5f6333ac-3555-405b-97d8-ee962008e50f</t>
+  </si>
+  <si>
+    <t>2f0fba0c-4c81-4446-819c-cb189950b666</t>
+  </si>
+  <si>
+    <t>f318d1b5-fd8f-425b-af14-718e0ac0dad3</t>
+  </si>
+  <si>
+    <t>c4aae64e-fd2c-49e8-804d-669d063aa4e6</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -1176,16 +1176,16 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>480ac37c-f156-4d0e-a220-ccac781e9886</t>
-  </si>
-  <si>
-    <t>7c813564-25eb-45a0-a132-015c9bbb0800</t>
-  </si>
-  <si>
-    <t>6f6ef3f9-ca9d-445f-93e4-b386dee97216</t>
-  </si>
-  <si>
-    <t>54755b8b-578a-4836-8d9c-285dcbc3505c</t>
+    <t>70245c4c-d217-45a7-8de8-be3b0b5021f8</t>
+  </si>
+  <si>
+    <t>8e4ef763-a972-4151-9f88-e40d373d91e3</t>
+  </si>
+  <si>
+    <t>4594712d-de19-45ea-9548-fe605b57b1ec</t>
+  </si>
+  <si>
+    <t>772953ad-4cf2-4913-9851-00cc16e1c6f5</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE is empty</t>
@@ -1197,22 +1197,22 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>36bfc93a-44c7-430c-8cfa-20abefb7d931</t>
-  </si>
-  <si>
-    <t>35d57d74-9c7b-4f43-8286-03db5431b373</t>
-  </si>
-  <si>
-    <t>5c545327-475e-4493-9e0d-fb2eef511012</t>
-  </si>
-  <si>
-    <t>176cba14-39ac-4441-b61c-ca75cb146cc2</t>
-  </si>
-  <si>
-    <t>6cb43f17-ec2c-484b-9219-453012573cf3</t>
-  </si>
-  <si>
-    <t>3ced12ec-0845-4d92-abdc-aa6daa0fd73f</t>
+    <t>baa8e05a-7cb3-4b7d-aee3-ad14fe172266</t>
+  </si>
+  <si>
+    <t>4e952ace-93e2-4cf6-944d-52d54a32e22a</t>
+  </si>
+  <si>
+    <t>f9d3a06a-0943-4204-ab7b-67ab83cdc11b</t>
+  </si>
+  <si>
+    <t>65f28648-421b-4e40-bdc7-9cd45bf9053a</t>
+  </si>
+  <si>
+    <t>58890c7a-b578-48a7-aa20-acb7a3bb3197</t>
+  </si>
+  <si>
+    <t>4b74a565-ef30-4ef3-b6aa-e8d474c4cc13</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -1224,19 +1224,19 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>ef6db1d5-28ef-4885-b937-8dc91baa6735</t>
-  </si>
-  <si>
-    <t>ac5ab3d3-9f6b-4750-b693-ca46bf0b48bd</t>
-  </si>
-  <si>
-    <t>1b14c808-8400-4fb1-80f8-765150e34cb7</t>
-  </si>
-  <si>
-    <t>740665fb-3ca0-47f7-a26a-80f7d57d2797</t>
-  </si>
-  <si>
-    <t>257593fb-7479-49dd-b750-945f7f90fd20</t>
+    <t>a05fb005-80cc-4e90-a720-73a0e37ec5d2</t>
+  </si>
+  <si>
+    <t>13e76153-6c76-4f3d-932d-82c4986ad74a</t>
+  </si>
+  <si>
+    <t>1b25ed25-417c-4ca6-a4c3-f27e760cbc54</t>
+  </si>
+  <si>
+    <t>1df3ab74-0549-4c4b-bcd8-540c7c3e7202</t>
+  </si>
+  <si>
+    <t>ff909909-e244-4afc-8425-44a99dc83635</t>
   </si>
   <si>
     <t>86ff3ab6-900d-5474-b63c-cbcac3c66f1a</t>

</xml_diff>

<commit_message>
feat: continue ingestion fs watch prep
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>17843c58-37af-452e-b0bf-c9344cc4a18b</t>
+    <t>47391431-8b8d-44f7-b7ad-0a5ec9457269</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -267,7 +267,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>0a92581a-dec5-46cb-af86-7aafa636ff8d</t>
+    <t>adeec7a6-f457-468b-acc0-14c234096f3f</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>1c61c3d9-f2db-47d4-9749-1b36b377d8be</t>
+    <t>e7f84daa-fb8f-488c-81af-6219d6576eb1</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>d9562870-0850-48cb-975a-85c582c89288</t>
+    <t>d72c715a-79f6-47ed-ad4e-2d66acf93cac</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>38d66903-9b78-4151-a5cd-fa0e11d476d4</t>
+    <t>a43e7f17-0dd3-49f2-b7f0-c58c055e6cf1</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>f532deaa-e41f-4315-976f-25365e8595a5</t>
+    <t>b3abf54b-92fb-4d98-bc83-ef06155da0fd</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>aed4f471-ddad-429a-8cac-93094e9b20e8</t>
+    <t>cd244eeb-4d4a-43b5-a731-eff45d554045</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>43885a11-1961-4001-8aed-5572eec05074</t>
+    <t>af60ef36-c9f4-418c-baba-c818bf994d70</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>08c627b8-3cf8-4560-9c8e-89beefee38ce</t>
+    <t>476ba583-78a2-413c-a5c8-f98cafc6ca57</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>847ff20a-0686-4e95-a53b-747a70ae3948</t>
+    <t>e7609f3d-0642-4220-8c7c-142a2f019fa2</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>6eed13f5-a146-4498-b33e-1228cf4b852b</t>
+    <t>e3dfe3da-cabe-407d-9aa4-aa2b999d0438</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>a395d15e-2bfd-40b6-b69c-2c359d90ae87</t>
+    <t>b8050943-12a1-4bcd-8e92-f60f46b69ee7</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>eaf67770-2fb7-4855-bd5f-7be64a39f428</t>
+    <t>e5e4ac78-a598-464d-838c-83640ad49ad3</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>a7c02631-3023-4ad3-a0e0-06701d1e65c0</t>
+    <t>61f9406e-02ec-4c72-9617-3a59754a9f89</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>3bf41967-9a22-4859-bf91-bfd1b82a802a</t>
+    <t>f6a5644a-e164-43a4-934f-1753738ff750</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>bdf91f6e-02a0-4a43-80a6-cfd902965e5d</t>
+    <t>0f59a624-3b9f-4229-ab73-c470b4222558</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>32183022-6aec-46a2-9068-1efdb23ff741</t>
+    <t>872c338e-4e3b-448d-87c7-d3f745faf15e</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>27af204a-d36f-44a6-9542-d6ee7b97275e</t>
+    <t>aaf428d1-9873-4aef-ba7c-f41be0ae38f4</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>acc7468f-7bc2-45dc-9c07-d7d489e7784e</t>
+    <t>38ef7636-40ed-4ffe-ae51-197bff0364c1</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>1946d1e7-a043-4263-bbb0-21f71f6ac997</t>
+    <t>62afc447-4e5a-411d-a647-e49c460e827e</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>ef91eaf4-b32f-4ab9-8516-4d30a0b3a521</t>
+    <t>9e3df00e-a382-408a-be43-68717b43f067</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -456,7 +456,7 @@
     <t>ahc_hrsn_2023_12_12_valid</t>
   </si>
   <si>
-    <t>89a58da9-df99-42c3-b76a-fee16b2afa62</t>
+    <t>06c107ff-205b-4798-adea-162e0143af35</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -474,7 +474,7 @@
     <t>Use only allowed values '71802-3','96778-6' in QUESTION_CODE</t>
   </si>
   <si>
-    <t>c7c06103-01a3-4dc2-9692-aa54b2563314</t>
+    <t>da49021d-c649-41be-b39a-50905078c486</t>
   </si>
   <si>
     <t>Value 88122-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -483,7 +483,7 @@
     <t>88122-7</t>
   </si>
   <si>
-    <t>a0e3f342-c04c-4e3b-9550-d28702132752</t>
+    <t>f03a21a0-548f-41b1-a349-75f4c4f7a337</t>
   </si>
   <si>
     <t>Value 88123-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -492,7 +492,7 @@
     <t>88123-5</t>
   </si>
   <si>
-    <t>d6cb33a7-9c17-4272-98c4-91085fe44fb0</t>
+    <t>f0807d98-04e3-4d13-bc3c-6d3355c49e30</t>
   </si>
   <si>
     <t>Value 93030-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -501,7 +501,7 @@
     <t>93030-5</t>
   </si>
   <si>
-    <t>29b8baec-dde3-49de-a272-59d9f8f2dc29</t>
+    <t>fe2fdabb-14b2-4aea-9302-844edaf389be</t>
   </si>
   <si>
     <t>Value 96779-4 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -510,7 +510,7 @@
     <t>96779-4</t>
   </si>
   <si>
-    <t>98882e18-7bc8-4162-80d0-849c48f9341a</t>
+    <t>fb7182d3-8208-48e2-97b2-a82677a88137</t>
   </si>
   <si>
     <t>Value 95618-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -519,7 +519,7 @@
     <t>95618-5</t>
   </si>
   <si>
-    <t>8b41abc1-ff92-496d-a8ff-91712209c47a</t>
+    <t>3a815c1a-89bc-402b-95be-2bf8fa45127c</t>
   </si>
   <si>
     <t>Value 95617-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -528,7 +528,7 @@
     <t>95617-7</t>
   </si>
   <si>
-    <t>b8b45cf2-5f1b-4102-af20-fb3b6148a697</t>
+    <t>b478654f-41a9-4bb9-a955-74b9b1973254</t>
   </si>
   <si>
     <t>Value 95616-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -537,7 +537,7 @@
     <t>95616-9</t>
   </si>
   <si>
-    <t>adf5776d-8785-4b00-b9bf-1498f36be75d</t>
+    <t>182b91db-d9c7-45fc-86f9-71d19e0488b9</t>
   </si>
   <si>
     <t>Value 95615-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -546,7 +546,7 @@
     <t>95615-1</t>
   </si>
   <si>
-    <t>7e9dedf3-995a-4e36-b3ad-2139f1f990a1</t>
+    <t>1d5de0af-cbba-42ad-a544-c8e24da0e7f5</t>
   </si>
   <si>
     <t>Value 76513-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -555,7 +555,7 @@
     <t>76513-1</t>
   </si>
   <si>
-    <t>59de9820-bce8-4694-a50c-60238f5b6cdc</t>
+    <t>2d77c3bd-a11d-4df0-a430-35958315e396</t>
   </si>
   <si>
     <t>Value 96780-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -564,7 +564,7 @@
     <t>96780-2</t>
   </si>
   <si>
-    <t>6d9fb301-17bd-4360-9e94-a41c76178c05</t>
+    <t>18c30399-3dbb-4de5-b597-1624032543ed</t>
   </si>
   <si>
     <t>Value 96781-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -573,7 +573,7 @@
     <t>96781-0</t>
   </si>
   <si>
-    <t>9e3d981f-4e7e-49e9-98ad-2352118f2c10</t>
+    <t>11291398-953c-4424-a7ba-04dd2287d832</t>
   </si>
   <si>
     <t>Value 93159-2	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -582,7 +582,7 @@
     <t>93159-2	</t>
   </si>
   <si>
-    <t>06bee207-f171-493f-bac9-0f2595e99308</t>
+    <t>0355cee1-21b7-4ac5-81cc-fbaf5ab9eaaf</t>
   </si>
   <si>
     <t>Value 97027-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -591,7 +591,7 @@
     <t>97027-7</t>
   </si>
   <si>
-    <t>ac51bcdb-1729-42cc-a5e0-8cc052967dad</t>
+    <t>edca6e0f-4cdd-4991-94c8-fd988333e204</t>
   </si>
   <si>
     <t>Value 96782-8	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -600,7 +600,7 @@
     <t>96782-8	</t>
   </si>
   <si>
-    <t>8208472d-aab3-458d-8635-d2ba521a56aa</t>
+    <t>2deb080a-192c-404d-99df-49f5a59b9f1a</t>
   </si>
   <si>
     <t>Value 89555-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -609,7 +609,7 @@
     <t>89555-7</t>
   </si>
   <si>
-    <t>e808a3e6-0b6f-4d64-a7e9-1b689ecd7718</t>
+    <t>c510ecf4-9ec8-44db-8754-fa5b1cee19aa</t>
   </si>
   <si>
     <t>Value 68516-4	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -618,7 +618,7 @@
     <t>68516-4	</t>
   </si>
   <si>
-    <t>1bc09197-07ba-447f-a2cb-1a96f88b2593</t>
+    <t>54c9bca9-9bfe-48fc-875c-fb36249a32e8</t>
   </si>
   <si>
     <t>Value 68517-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -627,7 +627,7 @@
     <t>68517-2</t>
   </si>
   <si>
-    <t>62477dc6-e4c8-46c8-9ac9-5ae4e13042e8</t>
+    <t>7f311a74-46f2-4fb0-a277-b3f0ee077039</t>
   </si>
   <si>
     <t>Value 96842-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -636,7 +636,7 @@
     <t>96842-0</t>
   </si>
   <si>
-    <t>2e55d592-ee8e-40da-ab23-e8552bce17de</t>
+    <t>5262e0c3-3ac9-4d97-9f76-271bef997ed8</t>
   </si>
   <si>
     <t>Value 95530-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -645,7 +645,7 @@
     <t>95530-2</t>
   </si>
   <si>
-    <t>a52cb32c-4978-4067-b1d2-cf4cc4bb1a7d</t>
+    <t>c775d037-dd35-4fc1-a7da-92cc60ff14bf</t>
   </si>
   <si>
     <t>Value 68524-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -654,7 +654,7 @@
     <t>68524-8</t>
   </si>
   <si>
-    <t>619ffaf9-c38e-40fa-b85b-e499b2de57b1</t>
+    <t>e03f9c8c-2eb8-4996-bd54-ad5977925aaf</t>
   </si>
   <si>
     <t>Value 44250-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -663,7 +663,7 @@
     <t>44250-9</t>
   </si>
   <si>
-    <t>d66ce610-6f17-43d4-bea6-5d017c21b78d</t>
+    <t>3850e254-e0b2-4f1f-a5e3-2a3945cf708c</t>
   </si>
   <si>
     <t>Value 44255-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -672,7 +672,7 @@
     <t>44255-8</t>
   </si>
   <si>
-    <t>d05e89d4-756c-4c0f-b347-bb553c75a658</t>
+    <t>456f6795-55b5-4293-a322-644303880bc3</t>
   </si>
   <si>
     <t>Value 93038-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -681,7 +681,7 @@
     <t>93038-8</t>
   </si>
   <si>
-    <t>4766624d-ae36-45b9-8bfe-635d8ec19293</t>
+    <t>7b2ede7b-8be3-4dec-bb67-68ba12c7e9c2</t>
   </si>
   <si>
     <t>Value 69858-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -690,7 +690,7 @@
     <t>69858-9</t>
   </si>
   <si>
-    <t>183e7b05-a7fc-4c36-a27c-b8977b0b0871</t>
+    <t>3ff3f2ec-58eb-455c-8c87-e707e9fd62ad</t>
   </si>
   <si>
     <t>Value 69861-3	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -699,7 +699,7 @@
     <t>69861-3	</t>
   </si>
   <si>
-    <t>db64ac39-6a9d-4c3b-bcae-fe0c36afb29d</t>
+    <t>c1871143-53b1-4f3e-bf83-1282c3ff03d1</t>
   </si>
   <si>
     <t>Value false in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -714,7 +714,7 @@
     <t>Use only allowed values 'TRUE','FALSE' in NEED_INDICATED</t>
   </si>
   <si>
-    <t>d84afcf9-a556-408e-89ca-8794030bf58e</t>
+    <t>ad9b41e7-b17d-4526-9950-4cbe27acd0a1</t>
   </si>
   <si>
     <t>Value true in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -723,82 +723,82 @@
     <t>true</t>
   </si>
   <si>
-    <t>5c5360f0-6375-44a0-affb-0b9d552d5a8a</t>
-  </si>
-  <si>
-    <t>3bdbf3dc-59d4-4852-a337-912975f7ae6d</t>
-  </si>
-  <si>
-    <t>3fa03bd0-30a7-439c-a5b0-34512397ca6f</t>
-  </si>
-  <si>
-    <t>80a6af0a-9fc2-4bf8-bdf4-4e232212eca4</t>
-  </si>
-  <si>
-    <t>f1d0d809-e010-4186-95a8-ee9878dc0f9f</t>
-  </si>
-  <si>
-    <t>1f16d526-7339-494f-aab4-3875d148b6c3</t>
-  </si>
-  <si>
-    <t>2ea57ef8-5310-4130-a2f3-242d2fb80ba2</t>
-  </si>
-  <si>
-    <t>9b42b1a0-8546-4b7c-8ace-4f8eb3df86aa</t>
-  </si>
-  <si>
-    <t>84c02511-9f22-43e7-bb7d-d2aef579d770</t>
-  </si>
-  <si>
-    <t>5cf87805-b8c0-4e69-899e-55f339f2b6eb</t>
-  </si>
-  <si>
-    <t>d226e490-a5ff-428e-9518-0a1dffcbe3bb</t>
-  </si>
-  <si>
-    <t>3995a99e-9eee-41e6-b7bb-8e2da0d24914</t>
-  </si>
-  <si>
-    <t>bfcff5a9-6894-4399-9192-92de2c62b2a2</t>
-  </si>
-  <si>
-    <t>dee8dced-3caf-4f36-929a-d2123cabf98a</t>
-  </si>
-  <si>
-    <t>e8797b8b-3555-4c05-b6fe-d30a6733baeb</t>
-  </si>
-  <si>
-    <t>e8660fe8-7fd4-4227-a735-95987aeca07c</t>
-  </si>
-  <si>
-    <t>e68c6908-94c8-49df-b266-b9d5229d0eaf</t>
-  </si>
-  <si>
-    <t>892911e3-4612-4a19-a87e-409c086c3260</t>
-  </si>
-  <si>
-    <t>43ca2da9-9eb7-40f1-98e4-5f6f2bd7e4a1</t>
-  </si>
-  <si>
-    <t>7a8dd1c4-ee17-48ba-b5f1-5fa86ca61868</t>
-  </si>
-  <si>
-    <t>ef555323-7236-473e-86c1-5d7496d5742e</t>
-  </si>
-  <si>
-    <t>9a64f9e2-02dd-4e3b-88fd-816e327f4547</t>
-  </si>
-  <si>
-    <t>5efc1d85-305d-4dd5-af3e-d5916567aaa0</t>
-  </si>
-  <si>
-    <t>dc5ff1f0-6458-4395-ad43-6f48fd64bccd</t>
-  </si>
-  <si>
-    <t>8b45852d-cbe1-422c-ac53-1a6964613ef0</t>
-  </si>
-  <si>
-    <t>57256237-8c6e-4d22-b567-45898b75de45</t>
+    <t>cd5b096f-12e3-4759-8db1-bc940700b4ba</t>
+  </si>
+  <si>
+    <t>1267af75-db75-4c07-af88-0219b368cd29</t>
+  </si>
+  <si>
+    <t>99c8f004-6630-4a3a-8ae2-dea34bcc7ee4</t>
+  </si>
+  <si>
+    <t>ef1fd2ce-91fa-45b4-bf6d-8b22473d7549</t>
+  </si>
+  <si>
+    <t>d0fe2cab-29b8-4e57-a220-316fe8cba5f0</t>
+  </si>
+  <si>
+    <t>b02006cd-5783-4e07-92db-6585fd28d124</t>
+  </si>
+  <si>
+    <t>e042ec16-31d9-4b71-b364-9136d7ef15ce</t>
+  </si>
+  <si>
+    <t>9e29983e-d1f1-4a67-af58-5ffae83cc9a1</t>
+  </si>
+  <si>
+    <t>d567b3ee-615b-4619-909d-a3fe4a67e101</t>
+  </si>
+  <si>
+    <t>97ef1762-406a-40b0-aff0-87e482e130ec</t>
+  </si>
+  <si>
+    <t>62a4bf91-69ad-4db5-ac5b-2d0442015d6b</t>
+  </si>
+  <si>
+    <t>97afe996-b24b-4434-8c8e-58a5568e9bd7</t>
+  </si>
+  <si>
+    <t>73a2cb8e-26b5-4404-a3bf-9f3218481e65</t>
+  </si>
+  <si>
+    <t>17984a6e-5ea0-43e1-ade0-3b1968c4f7b2</t>
+  </si>
+  <si>
+    <t>6c430adb-7d08-49b7-937f-69ec0eb34ff7</t>
+  </si>
+  <si>
+    <t>6740aba6-d156-43ff-b2e5-a3224e4c6653</t>
+  </si>
+  <si>
+    <t>0c0d1b67-6658-4c54-ba88-3b165321bd5a</t>
+  </si>
+  <si>
+    <t>665bf2b7-9340-4ee3-b683-be59b83937d8</t>
+  </si>
+  <si>
+    <t>768fdb55-38ef-4ca8-84b2-8320d9d8887d</t>
+  </si>
+  <si>
+    <t>645d6845-d222-4885-a73c-3025ca61c7b3</t>
+  </si>
+  <si>
+    <t>8d3402b3-3e92-44eb-aee9-f52891d7bd8f</t>
+  </si>
+  <si>
+    <t>c03e7b45-9bff-4e0a-a828-c63b8ce9360c</t>
+  </si>
+  <si>
+    <t>25c8d8d9-861b-4990-946f-96f9d8451b0c</t>
+  </si>
+  <si>
+    <t>50c2d4c1-123e-4713-824b-46606bc82218</t>
+  </si>
+  <si>
+    <t>e3da68f2-742c-41c7-b3a6-6f0ed3a00feb</t>
+  </si>
+  <si>
+    <t>aac10f11-16ea-49ca-a068-e95331c179e0</t>
   </si>
   <si>
     <t>Value false in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -810,88 +810,88 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_PART_2_FLAG</t>
   </si>
   <si>
-    <t>e506eae1-b00e-4b33-8b79-79703aa0f376</t>
-  </si>
-  <si>
-    <t>ddb9cc13-26c9-4b4f-9641-12ff1f35949f</t>
-  </si>
-  <si>
-    <t>9d834fe8-4025-4946-9b8c-6d7fbff0fd3f</t>
-  </si>
-  <si>
-    <t>a48d4e41-18cc-4177-a18c-d43280d75092</t>
-  </si>
-  <si>
-    <t>2c84e46e-a24b-4c1a-b884-c7353e5dd3af</t>
-  </si>
-  <si>
-    <t>2fd2b503-3f2b-458f-ad99-751c698ab140</t>
-  </si>
-  <si>
-    <t>b06863e8-f899-412e-ba7f-21164b582bf1</t>
-  </si>
-  <si>
-    <t>b1b36f69-3658-4ba2-872e-891affef3386</t>
-  </si>
-  <si>
-    <t>6305d06d-989f-4465-aba1-7a9cce4aace2</t>
-  </si>
-  <si>
-    <t>b4156a2b-5d30-4e0e-b97e-524fd115c092</t>
-  </si>
-  <si>
-    <t>f239a9ba-28db-4cdd-b452-e9e9ee8c3db1</t>
-  </si>
-  <si>
-    <t>7b2d0185-8fae-4656-af9f-44f04cbf6694</t>
-  </si>
-  <si>
-    <t>fc3abcad-e617-438d-bd80-7004f48fe803</t>
-  </si>
-  <si>
-    <t>4dcb099d-ea04-4c72-8825-9ee33e6e7fe4</t>
-  </si>
-  <si>
-    <t>dbe5d442-5564-46b5-911a-4a222ba3a151</t>
-  </si>
-  <si>
-    <t>541f4528-591c-4d3a-b638-11890686723c</t>
-  </si>
-  <si>
-    <t>a7d916bd-d667-4286-8507-48ec50609c04</t>
-  </si>
-  <si>
-    <t>dbdafaaa-9b17-4f9d-a120-64b7415b3afe</t>
+    <t>aa6d7557-ba2d-4075-bcba-16bd752673bf</t>
+  </si>
+  <si>
+    <t>a12b97b5-4c90-483e-a985-83bfd4d58e9c</t>
+  </si>
+  <si>
+    <t>7596300e-dc51-4c9e-a087-161b2ee68228</t>
+  </si>
+  <si>
+    <t>f7880c0c-dd84-4626-a183-79e9bf825516</t>
+  </si>
+  <si>
+    <t>cd1aa848-7be2-4fb6-91d0-f4b061e04b61</t>
+  </si>
+  <si>
+    <t>48fc0545-03db-44aa-84b2-d676e33097b7</t>
+  </si>
+  <si>
+    <t>52618c20-a107-47c9-ac75-8e4f3b04452e</t>
+  </si>
+  <si>
+    <t>10001626-db05-458b-90f7-afa3390e0f81</t>
+  </si>
+  <si>
+    <t>ddd9fb44-f233-46bc-a8be-e62fd965c0b3</t>
+  </si>
+  <si>
+    <t>9032b043-018f-453d-ba35-4d8c38e11c6d</t>
+  </si>
+  <si>
+    <t>ac88504d-4e29-4cd0-96de-a5ad7290d412</t>
+  </si>
+  <si>
+    <t>43d1304b-cc0c-4d5e-a28a-2a7817733494</t>
+  </si>
+  <si>
+    <t>db4fb6cc-c032-4c7c-8231-b51065f0d5e0</t>
+  </si>
+  <si>
+    <t>61040ec1-cc3c-4bf5-8552-ae8c544ee703</t>
+  </si>
+  <si>
+    <t>562f9b33-4948-48ea-989d-3a5e11adc25c</t>
+  </si>
+  <si>
+    <t>2b4c0f28-ca07-4cfb-b6fe-5da3c719abb9</t>
+  </si>
+  <si>
+    <t>c674c04e-d16e-4a8d-ad5e-b089d977189e</t>
+  </si>
+  <si>
+    <t>91dc4ad0-a587-4092-b533-b13705680707</t>
   </si>
   <si>
     <t>Value true in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>98c1c338-7af1-449c-ba12-a727d2522993</t>
-  </si>
-  <si>
-    <t>0ab71565-f1ea-4eeb-9295-6ae1e53dff51</t>
-  </si>
-  <si>
-    <t>5cb26a8a-110d-400b-b158-de8c5321588a</t>
-  </si>
-  <si>
-    <t>c315c9b2-374a-4e16-a323-42718f345c4e</t>
-  </si>
-  <si>
-    <t>2566b618-5c8c-46ef-a985-0e0dd1295953</t>
-  </si>
-  <si>
-    <t>ebc58797-ed8f-4227-b65e-0e301a265afe</t>
-  </si>
-  <si>
-    <t>24002e76-2637-4212-8d1b-18276fdc855f</t>
-  </si>
-  <si>
-    <t>014a0d29-b9f9-4359-ba37-eea733062058</t>
-  </si>
-  <si>
-    <t>20030643-c1d4-4c0a-bbf8-923c17e6860a</t>
+    <t>a5f45702-0192-4550-ae5d-b6d24eb7c1b3</t>
+  </si>
+  <si>
+    <t>dec3e3c7-ad92-4726-af4f-6ede46b091f9</t>
+  </si>
+  <si>
+    <t>03e0f46e-a9df-4ba5-8a3d-7d505d43f2e6</t>
+  </si>
+  <si>
+    <t>1e325f72-9f46-4b8f-993a-4e1e6dcbd6d4</t>
+  </si>
+  <si>
+    <t>994c7d58-d3ec-402b-a2ed-a71c41cab968</t>
+  </si>
+  <si>
+    <t>c4546a9b-4c03-41eb-8139-38b396cd7a90</t>
+  </si>
+  <si>
+    <t>55d6b53e-57b9-4c30-bd65-6a399fa243bc</t>
+  </si>
+  <si>
+    <t>2c94ec91-d26a-4c72-b451-ef7f26c43930</t>
+  </si>
+  <si>
+    <t>8ae744ad-f7b4-4442-b7c4-eb6b5ec122ea</t>
   </si>
   <si>
     <t>Value false in VISIT_OMH_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -903,85 +903,85 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OMH_FLAG</t>
   </si>
   <si>
-    <t>ed2ab7b2-a7dc-4a41-a7db-c173fc95f918</t>
-  </si>
-  <si>
-    <t>e1ff200e-740c-4b14-a100-486bf0701bd6</t>
-  </si>
-  <si>
-    <t>659721b1-02ab-405f-890b-5e01ecb29277</t>
-  </si>
-  <si>
-    <t>15924218-8df9-4aae-b4f0-05c2bea986c4</t>
-  </si>
-  <si>
-    <t>7391a520-72b3-4017-9707-16f7dff6a1a6</t>
-  </si>
-  <si>
-    <t>9d6d80a4-4509-4bbf-b464-6dc6d9237f5b</t>
-  </si>
-  <si>
-    <t>0d755d21-b40e-452b-9523-535726b8bc28</t>
-  </si>
-  <si>
-    <t>9691a743-0cca-489a-bf1b-d792fa25564f</t>
-  </si>
-  <si>
-    <t>22d84121-b050-43cd-94f9-c4c1bd6c8935</t>
-  </si>
-  <si>
-    <t>ea39fa8d-74a5-458e-ba72-ce9973491ac3</t>
-  </si>
-  <si>
-    <t>e2acc918-b8e4-4a4a-8302-c8e97a9211ad</t>
-  </si>
-  <si>
-    <t>24ab0104-cd26-46f4-8ea0-d2818068510f</t>
-  </si>
-  <si>
-    <t>95c0492e-041b-418b-bfeb-14a1e1186659</t>
-  </si>
-  <si>
-    <t>8f9c0aea-70b7-416f-8eea-22087a702e38</t>
-  </si>
-  <si>
-    <t>3a47254f-441a-44df-958d-d3466b8235e6</t>
-  </si>
-  <si>
-    <t>94ca6c28-b324-42d8-9329-781e3ba71f43</t>
-  </si>
-  <si>
-    <t>08939bcd-0abc-44c4-8c68-559969d59082</t>
-  </si>
-  <si>
-    <t>271831a4-b175-4a48-a173-8e42a6024ae9</t>
-  </si>
-  <si>
-    <t>0e2edefd-b282-4f60-8b35-5d0d6ece4452</t>
-  </si>
-  <si>
-    <t>630a6eae-1b5b-4adf-82bc-44484bd4c047</t>
-  </si>
-  <si>
-    <t>999831ba-914b-4b33-8fda-831f800a17ad</t>
-  </si>
-  <si>
-    <t>f8fda3f7-56c3-48ae-878d-0952adb674b3</t>
-  </si>
-  <si>
-    <t>97063eee-9ce7-44a6-9ba1-781c7dfa464f</t>
-  </si>
-  <si>
-    <t>a946323a-23de-4eff-9bfc-5bc6e49d4740</t>
-  </si>
-  <si>
-    <t>c997e735-9326-4805-9ea8-2e4ffb727131</t>
-  </si>
-  <si>
-    <t>72e6ab00-eb68-4f5a-ab6d-1d1b54b7e406</t>
-  </si>
-  <si>
-    <t>52131706-0693-4472-9056-fc17fdc378f1</t>
+    <t>ecf37f45-081f-4a8a-becc-6dabb0ab5fed</t>
+  </si>
+  <si>
+    <t>a101ea39-a97c-443f-86cd-d42116c682c8</t>
+  </si>
+  <si>
+    <t>9186c474-21de-4ed2-8a0c-a54563fa41fd</t>
+  </si>
+  <si>
+    <t>9cd84164-3eb8-4838-930a-97275f1f7c30</t>
+  </si>
+  <si>
+    <t>c7c97874-6b9a-4fcd-bdd3-ce64b74dd9fb</t>
+  </si>
+  <si>
+    <t>211b5b91-185a-47a9-9fe4-d81ec0212b06</t>
+  </si>
+  <si>
+    <t>faedc5e4-ebba-421f-b868-6a3e7c219cf9</t>
+  </si>
+  <si>
+    <t>877e5fac-ac96-463d-91ce-ac6fe1d0d49e</t>
+  </si>
+  <si>
+    <t>3f03a5bd-7af0-49a5-9b49-6a1e851045c6</t>
+  </si>
+  <si>
+    <t>711e11a1-e097-4dad-8cac-f92e9572b6be</t>
+  </si>
+  <si>
+    <t>bcf5b66b-eda8-437c-8e5b-73b73f60e937</t>
+  </si>
+  <si>
+    <t>64465f09-cabd-4457-9279-6dc26a9f4fd6</t>
+  </si>
+  <si>
+    <t>1aeaf602-55e2-44e2-9924-6b793aebb69c</t>
+  </si>
+  <si>
+    <t>1acffa15-8021-4a8b-bb75-802861427ee0</t>
+  </si>
+  <si>
+    <t>d0a7aec8-c0f5-4e5b-8635-68ff44f658d1</t>
+  </si>
+  <si>
+    <t>4b0f38b5-68df-4d48-8293-be32c645e0b4</t>
+  </si>
+  <si>
+    <t>d76ca0fa-2b40-44bc-88da-a1ca980c40c1</t>
+  </si>
+  <si>
+    <t>8f3e80d8-d996-4455-826d-a4fae88cdeda</t>
+  </si>
+  <si>
+    <t>78a1d30b-ca68-43e2-ad5d-742968b5c4e2</t>
+  </si>
+  <si>
+    <t>f2f28807-b8de-4b4d-a85a-ee74c4475337</t>
+  </si>
+  <si>
+    <t>45132a92-2e13-42f3-b227-bf6b223ccc30</t>
+  </si>
+  <si>
+    <t>4aba9bf5-0d92-4044-9dba-667eb4f9498d</t>
+  </si>
+  <si>
+    <t>515488cf-bafa-4142-90d3-cca671935987</t>
+  </si>
+  <si>
+    <t>8b1b7a6d-e4c0-439c-ac30-d76cb293bd64</t>
+  </si>
+  <si>
+    <t>5b65f0ca-3e39-425c-9b3d-a9521bbae9f3</t>
+  </si>
+  <si>
+    <t>538f8ba4-06cf-4e77-b3c6-34a674dfc307</t>
+  </si>
+  <si>
+    <t>52e9a4b6-3d6f-459c-a52f-25fdb2c1cc0f</t>
   </si>
   <si>
     <t>Value false in VISIT_OPWDD_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -993,82 +993,82 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OPWDD_FLAG</t>
   </si>
   <si>
-    <t>f6c35bcc-c382-4841-90a5-93d871af4c3a</t>
-  </si>
-  <si>
-    <t>d7f90076-a178-430a-8bcc-2df768552a81</t>
-  </si>
-  <si>
-    <t>a8c90640-ad29-48e9-b69b-ba2d5362b5f2</t>
-  </si>
-  <si>
-    <t>97c9e81b-1710-4bad-9a08-eeada19821f3</t>
-  </si>
-  <si>
-    <t>470684a2-20d0-430e-a8cb-b8f53aee6ed8</t>
-  </si>
-  <si>
-    <t>964aeb1e-f7a0-447c-a970-4dbf23a94507</t>
-  </si>
-  <si>
-    <t>bde06c67-16b6-4064-9ed5-9bcd51073561</t>
-  </si>
-  <si>
-    <t>f4164dc2-db4f-4480-87e0-31f4d43a99ce</t>
-  </si>
-  <si>
-    <t>67c7f9b9-4534-4532-a409-734aa8deca9a</t>
-  </si>
-  <si>
-    <t>586f298e-1cd2-41b3-b899-752d5bc91257</t>
-  </si>
-  <si>
-    <t>c567371b-1e91-4a7f-8a8c-7780a4f34376</t>
-  </si>
-  <si>
-    <t>fe6e972c-e8fd-44bc-8dc4-e9ad92daf0a3</t>
-  </si>
-  <si>
-    <t>620e21a6-d994-4cb7-82a8-4bc6e4706e1d</t>
-  </si>
-  <si>
-    <t>6976077c-99ef-4134-8e50-8554c4b7dc8c</t>
-  </si>
-  <si>
-    <t>d69e8517-1055-461f-a29f-218c713e770e</t>
-  </si>
-  <si>
-    <t>ffc205f6-18e3-4159-88e3-bb584ff03d2d</t>
-  </si>
-  <si>
-    <t>5d19ce3a-4fe6-433f-9060-eb22401f86cc</t>
-  </si>
-  <si>
-    <t>2a0ebcd7-fd16-4763-a79f-1751cc5c4c47</t>
-  </si>
-  <si>
-    <t>a0091998-cc46-4a05-8f30-1639db791c87</t>
-  </si>
-  <si>
-    <t>705034d9-6803-4333-89c9-f6009a554304</t>
-  </si>
-  <si>
-    <t>68d76074-9074-4523-8780-72a9462f6631</t>
-  </si>
-  <si>
-    <t>a0c4b587-2836-4635-935e-68828776ed69</t>
-  </si>
-  <si>
-    <t>52ad3ae7-dc25-42b6-a2e1-b799fc1c473a</t>
-  </si>
-  <si>
-    <t>3e218b23-e99c-4e0c-a9bf-e3ae7c72a4c6</t>
-  </si>
-  <si>
-    <t>e746683d-88ee-44d6-9d25-2b63c4633625</t>
-  </si>
-  <si>
-    <t>ae90c72b-7e19-4740-8e26-9a586603ea22</t>
+    <t>b1f55aae-fd97-4531-b068-4d412134cfbf</t>
+  </si>
+  <si>
+    <t>2deed5e9-d6a3-4363-b9f1-7955e01876a5</t>
+  </si>
+  <si>
+    <t>45edd0f3-163d-430a-9ca5-96799e81d72d</t>
+  </si>
+  <si>
+    <t>f509e77d-16c8-4739-b4ae-005b1ad8c27a</t>
+  </si>
+  <si>
+    <t>ec141418-942c-439a-92f1-34424612ff4a</t>
+  </si>
+  <si>
+    <t>a668ca97-07f0-4362-a84e-808bff8de94b</t>
+  </si>
+  <si>
+    <t>1b2c1c50-63f9-4a47-8275-0071de32b6be</t>
+  </si>
+  <si>
+    <t>1ecc83cd-4e42-4914-a5db-22cdd027ee9e</t>
+  </si>
+  <si>
+    <t>844c3154-b6ba-474b-92dd-122f02e12fd2</t>
+  </si>
+  <si>
+    <t>71835028-2616-4c24-aa65-76c14725442d</t>
+  </si>
+  <si>
+    <t>0e8f2e18-8d28-410b-9032-c2a034d499a0</t>
+  </si>
+  <si>
+    <t>69fde92c-3dfd-4c68-853b-b25231ccfbf6</t>
+  </si>
+  <si>
+    <t>067925b4-ff2b-41c8-9656-18e4fcfb2189</t>
+  </si>
+  <si>
+    <t>350f50bb-9d56-4289-9631-434f3e6ef6b6</t>
+  </si>
+  <si>
+    <t>c94d3dd1-2777-4c27-9609-6c514b2e13c7</t>
+  </si>
+  <si>
+    <t>dff9ba69-d523-4c7f-bd8d-4779c3e542fe</t>
+  </si>
+  <si>
+    <t>81a47774-facd-4ccf-8267-94e1c12e8b13</t>
+  </si>
+  <si>
+    <t>a1f59058-494e-40bf-b1fb-4c9c04970216</t>
+  </si>
+  <si>
+    <t>3d16878b-3c2c-48f8-8ef0-3a1a26961f98</t>
+  </si>
+  <si>
+    <t>6792c429-0203-4624-8970-4430b1efc4fb</t>
+  </si>
+  <si>
+    <t>5b28a8a7-e506-492e-975d-b7739838e93a</t>
+  </si>
+  <si>
+    <t>f222b01b-47b2-462d-9c25-d40f24b78e96</t>
+  </si>
+  <si>
+    <t>fc85c3e1-5c95-4037-afe1-037ec414169e</t>
+  </si>
+  <si>
+    <t>1d82ccc2-f41a-4114-b3d2-6c756ac312e5</t>
+  </si>
+  <si>
+    <t>ab25c6e7-0c1f-424f-a3a9-64509cf7fd0e</t>
+  </si>
+  <si>
+    <t>efc9abd3-7689-42e0-af36-315e20412e37</t>
   </si>
   <si>
     <t>2afb3098-bcfd-5a54-8ebb-4d65d399c55e</t>
@@ -1080,7 +1080,7 @@
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>c6b9bfcb-6a70-4953-b237-71d5b5ebfa78</t>
+    <t>0bfd672c-260b-499d-ad8d-70442e586806</t>
   </si>
   <si>
     <t>Value 	20430005 in SEXUAL_ORIENTATION_CODE not in allowed list ('42035005','20430005','38628009','OTH','UNK')</t>
@@ -1101,7 +1101,7 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>1d96dfd3-050f-4985-a7ab-4d14a4d0dd0a</t>
+    <t>c796a36d-3fd3-461b-9f4f-d79e30335bff</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -1116,16 +1116,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>07059d07-4a45-4012-a233-cbf818a935e1</t>
-  </si>
-  <si>
-    <t>c2ccbc63-3294-4df6-b4a2-516dc4909288</t>
-  </si>
-  <si>
-    <t>72e0854e-f751-4968-9fc9-7cb27768ceb3</t>
-  </si>
-  <si>
-    <t>d3c24e24-e8fd-46f8-af92-40b2c4dba5f5</t>
+    <t>3474d363-f086-4760-8f98-227864ab055c</t>
+  </si>
+  <si>
+    <t>f91e1895-fa7c-4df9-82a9-39379062b0bc</t>
+  </si>
+  <si>
+    <t>127558cb-8bb1-486c-b127-27a52256e9eb</t>
+  </si>
+  <si>
+    <t>5b4f9220-a142-4de0-9ef8-c51e243a315e</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -1137,16 +1137,16 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>e1b6190c-38bd-418f-a1ba-8fbfc5a7b575</t>
-  </si>
-  <si>
-    <t>9c83dbe1-fb40-428c-a3f4-7d76ed833129</t>
-  </si>
-  <si>
-    <t>005fdf80-24f2-4682-9c61-c80544c7f587</t>
-  </si>
-  <si>
-    <t>effb11b5-9bdf-498d-9302-a5ab23410e26</t>
+    <t>8a3ce826-600c-4929-a598-1d579ac0b1a0</t>
+  </si>
+  <si>
+    <t>08cc3aa4-3a68-4f75-a33c-988ffa7d2c27</t>
+  </si>
+  <si>
+    <t>061f891a-9d62-4b9a-9e7a-94c7ab3fbb94</t>
+  </si>
+  <si>
+    <t>0a9433ad-150a-4fc1-9bfa-80fa95d72d92</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -1155,16 +1155,16 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>5f6333ac-3555-405b-97d8-ee962008e50f</t>
-  </si>
-  <si>
-    <t>2f0fba0c-4c81-4446-819c-cb189950b666</t>
-  </si>
-  <si>
-    <t>f318d1b5-fd8f-425b-af14-718e0ac0dad3</t>
-  </si>
-  <si>
-    <t>c4aae64e-fd2c-49e8-804d-669d063aa4e6</t>
+    <t>613b7841-ec05-4dc2-8f60-0ef0191f1832</t>
+  </si>
+  <si>
+    <t>cd08e268-d48a-4564-88ee-97288babeb74</t>
+  </si>
+  <si>
+    <t>3306f96a-3c06-4d1e-ab0d-a9e0414b39bb</t>
+  </si>
+  <si>
+    <t>fe422644-8791-4e73-a392-21c5910469d7</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -1176,16 +1176,16 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>70245c4c-d217-45a7-8de8-be3b0b5021f8</t>
-  </si>
-  <si>
-    <t>8e4ef763-a972-4151-9f88-e40d373d91e3</t>
-  </si>
-  <si>
-    <t>4594712d-de19-45ea-9548-fe605b57b1ec</t>
-  </si>
-  <si>
-    <t>772953ad-4cf2-4913-9851-00cc16e1c6f5</t>
+    <t>dde6ef84-7491-42cf-9341-f154afa964a1</t>
+  </si>
+  <si>
+    <t>d9840dbb-51b2-4602-9569-790bb5065775</t>
+  </si>
+  <si>
+    <t>f516fccb-a4db-4c94-9912-ed60467e8906</t>
+  </si>
+  <si>
+    <t>6c8154bb-ce8a-4193-8b30-74817589f5ee</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE is empty</t>
@@ -1197,22 +1197,22 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>baa8e05a-7cb3-4b7d-aee3-ad14fe172266</t>
-  </si>
-  <si>
-    <t>4e952ace-93e2-4cf6-944d-52d54a32e22a</t>
-  </si>
-  <si>
-    <t>f9d3a06a-0943-4204-ab7b-67ab83cdc11b</t>
-  </si>
-  <si>
-    <t>65f28648-421b-4e40-bdc7-9cd45bf9053a</t>
-  </si>
-  <si>
-    <t>58890c7a-b578-48a7-aa20-acb7a3bb3197</t>
-  </si>
-  <si>
-    <t>4b74a565-ef30-4ef3-b6aa-e8d474c4cc13</t>
+    <t>f4b2d979-0846-43fe-87f7-aaa1a8b882b0</t>
+  </si>
+  <si>
+    <t>56511bb5-4b56-43c1-8f1c-1ed82664016c</t>
+  </si>
+  <si>
+    <t>2a9da0c2-f754-4f24-9857-d7cbbc668853</t>
+  </si>
+  <si>
+    <t>f1aa86f8-d476-49dc-887c-23e4a934c884</t>
+  </si>
+  <si>
+    <t>cc2dfe63-1674-46b1-826d-9498a9952866</t>
+  </si>
+  <si>
+    <t>569ffd82-32f7-40ad-904f-e61825bcd14d</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -1224,19 +1224,19 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>a05fb005-80cc-4e90-a720-73a0e37ec5d2</t>
-  </si>
-  <si>
-    <t>13e76153-6c76-4f3d-932d-82c4986ad74a</t>
-  </si>
-  <si>
-    <t>1b25ed25-417c-4ca6-a4c3-f27e760cbc54</t>
-  </si>
-  <si>
-    <t>1df3ab74-0549-4c4b-bcd8-540c7c3e7202</t>
-  </si>
-  <si>
-    <t>ff909909-e244-4afc-8425-44a99dc83635</t>
+    <t>bdd64e84-1cbd-4ffe-a2d4-455dc2ed23c3</t>
+  </si>
+  <si>
+    <t>ef0ebf61-3f2d-441a-93a7-e3a026ca338f</t>
+  </si>
+  <si>
+    <t>831016b2-caa0-4f36-83fb-eb9511085c95</t>
+  </si>
+  <si>
+    <t>79718a15-5d27-4ef5-b758-e2cf8502b30c</t>
+  </si>
+  <si>
+    <t>ceba7a1e-afd1-4741-bb7b-869755ae23f2</t>
   </si>
   <si>
     <t>86ff3ab6-900d-5474-b63c-cbcac3c66f1a</t>

</xml_diff>

<commit_message>
feat: switch to SQLa ingestion fs watch
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -255,7 +255,7 @@
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>47391431-8b8d-44f7-b7ad-0a5ec9457269</t>
+    <t>a58b9b5d-bc24-4331-a0e3-9a640e331705</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -267,7 +267,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>adeec7a6-f457-468b-acc0-14c234096f3f</t>
+    <t>3860d091-d94d-4ac4-a9ee-7841494c22b9</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>e7f84daa-fb8f-488c-81af-6219d6576eb1</t>
+    <t>41ddcc8c-cdea-4339-a796-23a100ebc9bf</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>d72c715a-79f6-47ed-ad4e-2d66acf93cac</t>
+    <t>ff0c36d7-cbb9-45d2-80a8-9ea8967646aa</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>a43e7f17-0dd3-49f2-b7f0-c58c055e6cf1</t>
+    <t>816c9a41-536e-482a-a1e2-cfc3a9ff839c</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>b3abf54b-92fb-4d98-bc83-ef06155da0fd</t>
+    <t>ec4115d4-882b-47bf-92c9-d3e01d2152ea</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>cd244eeb-4d4a-43b5-a731-eff45d554045</t>
+    <t>c1358876-388b-4ecd-a4cf-d22577045e6e</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>af60ef36-c9f4-418c-baba-c818bf994d70</t>
+    <t>11f6a6ac-a621-466e-af0e-795201617eb0</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>476ba583-78a2-413c-a5c8-f98cafc6ca57</t>
+    <t>49d19ca5-ff15-47b4-8dd1-ff7178dafb69</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>e7609f3d-0642-4220-8c7c-142a2f019fa2</t>
+    <t>36124f7d-6013-4d54-8bd1-b62b75cd070e</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>e3dfe3da-cabe-407d-9aa4-aa2b999d0438</t>
+    <t>e9be76dd-ddc0-48bb-b9e7-6c52a7283472</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>b8050943-12a1-4bcd-8e92-f60f46b69ee7</t>
+    <t>75dbaf65-57e9-49e8-b835-dd6de3e56d97</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>e5e4ac78-a598-464d-838c-83640ad49ad3</t>
+    <t>9bad977a-e9e5-472b-81f7-9ec4d6cf1721</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>61f9406e-02ec-4c72-9617-3a59754a9f89</t>
+    <t>baa4f65c-5fbe-4e4f-8948-b8e47b485ea2</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>f6a5644a-e164-43a4-934f-1753738ff750</t>
+    <t>c5c52f1f-22bc-4e11-8864-17783c9a80f4</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>0f59a624-3b9f-4229-ab73-c470b4222558</t>
+    <t>c65ab026-cadc-42f2-b317-b4fa5f532d28</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>872c338e-4e3b-448d-87c7-d3f745faf15e</t>
+    <t>cded0d34-2904-4693-bd3b-fc45f0d2bd12</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>aaf428d1-9873-4aef-ba7c-f41be0ae38f4</t>
+    <t>bc938a0e-8f37-4aeb-a45d-a80eb219e904</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>38ef7636-40ed-4ffe-ae51-197bff0364c1</t>
+    <t>ecefa7cd-5ec6-4781-b4d8-4a1cdee286c3</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>62afc447-4e5a-411d-a647-e49c460e827e</t>
+    <t>965f300a-8cfb-413f-a6fb-7b862dcefc2d</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>9e3df00e-a382-408a-be43-68717b43f067</t>
+    <t>9839803c-c8b3-4a32-8cdb-47ac28c43ca3</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -456,7 +456,7 @@
     <t>ahc_hrsn_2023_12_12_valid</t>
   </si>
   <si>
-    <t>06c107ff-205b-4798-adea-162e0143af35</t>
+    <t>222df9d5-2ccd-4ba6-b5df-54894aa9bdbc</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -474,7 +474,7 @@
     <t>Use only allowed values '71802-3','96778-6' in QUESTION_CODE</t>
   </si>
   <si>
-    <t>da49021d-c649-41be-b39a-50905078c486</t>
+    <t>68be5a76-9ae9-47f0-a2ec-81d0682f2b51</t>
   </si>
   <si>
     <t>Value 88122-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -483,7 +483,7 @@
     <t>88122-7</t>
   </si>
   <si>
-    <t>f03a21a0-548f-41b1-a349-75f4c4f7a337</t>
+    <t>e6b40756-db9c-49a6-984a-1df62cfbe7e8</t>
   </si>
   <si>
     <t>Value 88123-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -492,7 +492,7 @@
     <t>88123-5</t>
   </si>
   <si>
-    <t>f0807d98-04e3-4d13-bc3c-6d3355c49e30</t>
+    <t>802ef63a-e1da-4309-9b7c-8956beb142e1</t>
   </si>
   <si>
     <t>Value 93030-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -501,7 +501,7 @@
     <t>93030-5</t>
   </si>
   <si>
-    <t>fe2fdabb-14b2-4aea-9302-844edaf389be</t>
+    <t>de6dcf64-e504-4c0b-bebb-fbcc517f823a</t>
   </si>
   <si>
     <t>Value 96779-4 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -510,7 +510,7 @@
     <t>96779-4</t>
   </si>
   <si>
-    <t>fb7182d3-8208-48e2-97b2-a82677a88137</t>
+    <t>6e39b643-e1c9-49a5-a130-e7ee09223efb</t>
   </si>
   <si>
     <t>Value 95618-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -519,7 +519,7 @@
     <t>95618-5</t>
   </si>
   <si>
-    <t>3a815c1a-89bc-402b-95be-2bf8fa45127c</t>
+    <t>a599a953-0257-4c23-9216-7eba9b8e825f</t>
   </si>
   <si>
     <t>Value 95617-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -528,7 +528,7 @@
     <t>95617-7</t>
   </si>
   <si>
-    <t>b478654f-41a9-4bb9-a955-74b9b1973254</t>
+    <t>bf2cc2e5-214f-4177-8b73-c4be58002e45</t>
   </si>
   <si>
     <t>Value 95616-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -537,7 +537,7 @@
     <t>95616-9</t>
   </si>
   <si>
-    <t>182b91db-d9c7-45fc-86f9-71d19e0488b9</t>
+    <t>48117ff7-4689-48f4-a195-cf6b69198051</t>
   </si>
   <si>
     <t>Value 95615-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -546,7 +546,7 @@
     <t>95615-1</t>
   </si>
   <si>
-    <t>1d5de0af-cbba-42ad-a544-c8e24da0e7f5</t>
+    <t>d8fc6ae2-ebbe-485f-b204-2393ea3ec994</t>
   </si>
   <si>
     <t>Value 76513-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -555,7 +555,7 @@
     <t>76513-1</t>
   </si>
   <si>
-    <t>2d77c3bd-a11d-4df0-a430-35958315e396</t>
+    <t>4acfc863-3e1b-4aa1-a2b2-283c1fe8c364</t>
   </si>
   <si>
     <t>Value 96780-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -564,7 +564,7 @@
     <t>96780-2</t>
   </si>
   <si>
-    <t>18c30399-3dbb-4de5-b597-1624032543ed</t>
+    <t>f3e5d0c0-817b-43b9-820c-c4952bcacef0</t>
   </si>
   <si>
     <t>Value 96781-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -573,7 +573,7 @@
     <t>96781-0</t>
   </si>
   <si>
-    <t>11291398-953c-4424-a7ba-04dd2287d832</t>
+    <t>7d8396ca-80b5-4b36-91b4-4a98c8819ec1</t>
   </si>
   <si>
     <t>Value 93159-2	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -582,7 +582,7 @@
     <t>93159-2	</t>
   </si>
   <si>
-    <t>0355cee1-21b7-4ac5-81cc-fbaf5ab9eaaf</t>
+    <t>bf54f5db-adb2-49cc-8bcb-28a44126ee48</t>
   </si>
   <si>
     <t>Value 97027-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -591,7 +591,7 @@
     <t>97027-7</t>
   </si>
   <si>
-    <t>edca6e0f-4cdd-4991-94c8-fd988333e204</t>
+    <t>9198619b-ec93-4fec-b269-4c0a4aae8452</t>
   </si>
   <si>
     <t>Value 96782-8	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -600,7 +600,7 @@
     <t>96782-8	</t>
   </si>
   <si>
-    <t>2deb080a-192c-404d-99df-49f5a59b9f1a</t>
+    <t>fe955683-66f1-4276-80a7-a21349991ed7</t>
   </si>
   <si>
     <t>Value 89555-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -609,7 +609,7 @@
     <t>89555-7</t>
   </si>
   <si>
-    <t>c510ecf4-9ec8-44db-8754-fa5b1cee19aa</t>
+    <t>22188e21-8580-40e5-b452-51ad68fd59c3</t>
   </si>
   <si>
     <t>Value 68516-4	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -618,7 +618,7 @@
     <t>68516-4	</t>
   </si>
   <si>
-    <t>54c9bca9-9bfe-48fc-875c-fb36249a32e8</t>
+    <t>53a6982a-18cb-4036-8c82-05d4acd74d2f</t>
   </si>
   <si>
     <t>Value 68517-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -627,7 +627,7 @@
     <t>68517-2</t>
   </si>
   <si>
-    <t>7f311a74-46f2-4fb0-a277-b3f0ee077039</t>
+    <t>30f2c836-a651-465d-a41e-959b890b3896</t>
   </si>
   <si>
     <t>Value 96842-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -636,7 +636,7 @@
     <t>96842-0</t>
   </si>
   <si>
-    <t>5262e0c3-3ac9-4d97-9f76-271bef997ed8</t>
+    <t>99c07054-1037-4c19-9c40-41048c93896a</t>
   </si>
   <si>
     <t>Value 95530-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -645,7 +645,7 @@
     <t>95530-2</t>
   </si>
   <si>
-    <t>c775d037-dd35-4fc1-a7da-92cc60ff14bf</t>
+    <t>fffc3ca7-555b-473a-9bfb-c26522f4b970</t>
   </si>
   <si>
     <t>Value 68524-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -654,7 +654,7 @@
     <t>68524-8</t>
   </si>
   <si>
-    <t>e03f9c8c-2eb8-4996-bd54-ad5977925aaf</t>
+    <t>ec14109b-db1a-4c1c-a456-5ccfd93937e5</t>
   </si>
   <si>
     <t>Value 44250-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -663,7 +663,7 @@
     <t>44250-9</t>
   </si>
   <si>
-    <t>3850e254-e0b2-4f1f-a5e3-2a3945cf708c</t>
+    <t>74f8798e-d50f-449e-b786-9771a07becf6</t>
   </si>
   <si>
     <t>Value 44255-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -672,7 +672,7 @@
     <t>44255-8</t>
   </si>
   <si>
-    <t>456f6795-55b5-4293-a322-644303880bc3</t>
+    <t>b551d98b-4234-42a1-95af-0975f3622a72</t>
   </si>
   <si>
     <t>Value 93038-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -681,7 +681,7 @@
     <t>93038-8</t>
   </si>
   <si>
-    <t>7b2ede7b-8be3-4dec-bb67-68ba12c7e9c2</t>
+    <t>e7956b29-2f1f-44d0-b677-189dafecd9d9</t>
   </si>
   <si>
     <t>Value 69858-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -690,7 +690,7 @@
     <t>69858-9</t>
   </si>
   <si>
-    <t>3ff3f2ec-58eb-455c-8c87-e707e9fd62ad</t>
+    <t>9c0829f6-a638-4840-9bf7-e8f093975adf</t>
   </si>
   <si>
     <t>Value 69861-3	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -699,7 +699,7 @@
     <t>69861-3	</t>
   </si>
   <si>
-    <t>c1871143-53b1-4f3e-bf83-1282c3ff03d1</t>
+    <t>c4497746-4c72-41c3-9d9d-60bdc468e3b0</t>
   </si>
   <si>
     <t>Value false in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -714,7 +714,7 @@
     <t>Use only allowed values 'TRUE','FALSE' in NEED_INDICATED</t>
   </si>
   <si>
-    <t>ad9b41e7-b17d-4526-9950-4cbe27acd0a1</t>
+    <t>33ef191c-3f9d-4cae-8e16-1a912e7a0297</t>
   </si>
   <si>
     <t>Value true in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -723,82 +723,82 @@
     <t>true</t>
   </si>
   <si>
-    <t>cd5b096f-12e3-4759-8db1-bc940700b4ba</t>
-  </si>
-  <si>
-    <t>1267af75-db75-4c07-af88-0219b368cd29</t>
-  </si>
-  <si>
-    <t>99c8f004-6630-4a3a-8ae2-dea34bcc7ee4</t>
-  </si>
-  <si>
-    <t>ef1fd2ce-91fa-45b4-bf6d-8b22473d7549</t>
-  </si>
-  <si>
-    <t>d0fe2cab-29b8-4e57-a220-316fe8cba5f0</t>
-  </si>
-  <si>
-    <t>b02006cd-5783-4e07-92db-6585fd28d124</t>
-  </si>
-  <si>
-    <t>e042ec16-31d9-4b71-b364-9136d7ef15ce</t>
-  </si>
-  <si>
-    <t>9e29983e-d1f1-4a67-af58-5ffae83cc9a1</t>
-  </si>
-  <si>
-    <t>d567b3ee-615b-4619-909d-a3fe4a67e101</t>
-  </si>
-  <si>
-    <t>97ef1762-406a-40b0-aff0-87e482e130ec</t>
-  </si>
-  <si>
-    <t>62a4bf91-69ad-4db5-ac5b-2d0442015d6b</t>
-  </si>
-  <si>
-    <t>97afe996-b24b-4434-8c8e-58a5568e9bd7</t>
-  </si>
-  <si>
-    <t>73a2cb8e-26b5-4404-a3bf-9f3218481e65</t>
-  </si>
-  <si>
-    <t>17984a6e-5ea0-43e1-ade0-3b1968c4f7b2</t>
-  </si>
-  <si>
-    <t>6c430adb-7d08-49b7-937f-69ec0eb34ff7</t>
-  </si>
-  <si>
-    <t>6740aba6-d156-43ff-b2e5-a3224e4c6653</t>
-  </si>
-  <si>
-    <t>0c0d1b67-6658-4c54-ba88-3b165321bd5a</t>
-  </si>
-  <si>
-    <t>665bf2b7-9340-4ee3-b683-be59b83937d8</t>
-  </si>
-  <si>
-    <t>768fdb55-38ef-4ca8-84b2-8320d9d8887d</t>
-  </si>
-  <si>
-    <t>645d6845-d222-4885-a73c-3025ca61c7b3</t>
-  </si>
-  <si>
-    <t>8d3402b3-3e92-44eb-aee9-f52891d7bd8f</t>
-  </si>
-  <si>
-    <t>c03e7b45-9bff-4e0a-a828-c63b8ce9360c</t>
-  </si>
-  <si>
-    <t>25c8d8d9-861b-4990-946f-96f9d8451b0c</t>
-  </si>
-  <si>
-    <t>50c2d4c1-123e-4713-824b-46606bc82218</t>
-  </si>
-  <si>
-    <t>e3da68f2-742c-41c7-b3a6-6f0ed3a00feb</t>
-  </si>
-  <si>
-    <t>aac10f11-16ea-49ca-a068-e95331c179e0</t>
+    <t>5b1f6de3-fbc1-4408-a5f4-956ebb2dbf0f</t>
+  </si>
+  <si>
+    <t>e8cd7114-9a4e-4d2e-a15e-28e4476b101f</t>
+  </si>
+  <si>
+    <t>0eb3110f-a449-4ff7-bcab-2ac7dedf3d89</t>
+  </si>
+  <si>
+    <t>efd68e98-0e9a-42fc-8f70-44b463f76909</t>
+  </si>
+  <si>
+    <t>5d19937a-8e9e-4458-82b2-4a5a8eba3875</t>
+  </si>
+  <si>
+    <t>a88aa407-e882-4de8-a77b-633d9be385a3</t>
+  </si>
+  <si>
+    <t>3b2e6e58-3bd9-4ef9-b5c6-0d230f3093a1</t>
+  </si>
+  <si>
+    <t>689254d0-8d54-4139-bbe5-2cce40402c95</t>
+  </si>
+  <si>
+    <t>4df92f6a-5c3d-48c1-8d61-d35f87590a9c</t>
+  </si>
+  <si>
+    <t>99a1d552-e1f0-49b8-9436-92312b83a702</t>
+  </si>
+  <si>
+    <t>c443fe65-5aea-4500-a478-7787e8fc75ca</t>
+  </si>
+  <si>
+    <t>208c46be-9921-414c-80fd-08479ada70c9</t>
+  </si>
+  <si>
+    <t>7ae50078-e75b-4959-9ce3-cca8b0a14220</t>
+  </si>
+  <si>
+    <t>a66c191c-f875-4cc2-961a-021bb0165004</t>
+  </si>
+  <si>
+    <t>5882c1a7-1b9f-42ec-90ee-d7ff735ae92f</t>
+  </si>
+  <si>
+    <t>29453799-f1dd-40da-a9cb-a8a2c5f09fde</t>
+  </si>
+  <si>
+    <t>5beca73d-4da4-41e2-8e27-561e143e2b24</t>
+  </si>
+  <si>
+    <t>7ad17783-7e6f-4e49-8ff9-12266ff26197</t>
+  </si>
+  <si>
+    <t>753d3576-0aeb-4abc-a439-b807ad817e79</t>
+  </si>
+  <si>
+    <t>c4bc2a82-3507-4c0d-92c4-9281d2f3ab84</t>
+  </si>
+  <si>
+    <t>d04472d0-fb57-4079-b2ea-0feb4eb08556</t>
+  </si>
+  <si>
+    <t>d752a0fe-4241-49a8-9c0e-73a0d1519ae2</t>
+  </si>
+  <si>
+    <t>836c5c42-7a57-4a84-85ce-a134073148b3</t>
+  </si>
+  <si>
+    <t>675b9c7d-b87c-4e05-ac38-a9c73b50ff3e</t>
+  </si>
+  <si>
+    <t>b5d078d2-0796-4228-8584-158eb75da5a3</t>
+  </si>
+  <si>
+    <t>15398f62-cf2c-4688-9a8f-ca5fbf1cd956</t>
   </si>
   <si>
     <t>Value false in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -810,88 +810,88 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_PART_2_FLAG</t>
   </si>
   <si>
-    <t>aa6d7557-ba2d-4075-bcba-16bd752673bf</t>
-  </si>
-  <si>
-    <t>a12b97b5-4c90-483e-a985-83bfd4d58e9c</t>
-  </si>
-  <si>
-    <t>7596300e-dc51-4c9e-a087-161b2ee68228</t>
-  </si>
-  <si>
-    <t>f7880c0c-dd84-4626-a183-79e9bf825516</t>
-  </si>
-  <si>
-    <t>cd1aa848-7be2-4fb6-91d0-f4b061e04b61</t>
-  </si>
-  <si>
-    <t>48fc0545-03db-44aa-84b2-d676e33097b7</t>
-  </si>
-  <si>
-    <t>52618c20-a107-47c9-ac75-8e4f3b04452e</t>
-  </si>
-  <si>
-    <t>10001626-db05-458b-90f7-afa3390e0f81</t>
-  </si>
-  <si>
-    <t>ddd9fb44-f233-46bc-a8be-e62fd965c0b3</t>
-  </si>
-  <si>
-    <t>9032b043-018f-453d-ba35-4d8c38e11c6d</t>
-  </si>
-  <si>
-    <t>ac88504d-4e29-4cd0-96de-a5ad7290d412</t>
-  </si>
-  <si>
-    <t>43d1304b-cc0c-4d5e-a28a-2a7817733494</t>
-  </si>
-  <si>
-    <t>db4fb6cc-c032-4c7c-8231-b51065f0d5e0</t>
-  </si>
-  <si>
-    <t>61040ec1-cc3c-4bf5-8552-ae8c544ee703</t>
-  </si>
-  <si>
-    <t>562f9b33-4948-48ea-989d-3a5e11adc25c</t>
-  </si>
-  <si>
-    <t>2b4c0f28-ca07-4cfb-b6fe-5da3c719abb9</t>
-  </si>
-  <si>
-    <t>c674c04e-d16e-4a8d-ad5e-b089d977189e</t>
-  </si>
-  <si>
-    <t>91dc4ad0-a587-4092-b533-b13705680707</t>
+    <t>d0ae63d4-3e0f-4689-b14c-95192c8c63eb</t>
+  </si>
+  <si>
+    <t>5b734123-2187-4e89-9000-6bb499729b26</t>
+  </si>
+  <si>
+    <t>a7c2720a-4676-437f-b71b-647ddcef3fed</t>
+  </si>
+  <si>
+    <t>e93a9f72-7950-43c7-b8a5-eddf589d5f69</t>
+  </si>
+  <si>
+    <t>84057b79-6f2a-4a01-a893-221f274310a4</t>
+  </si>
+  <si>
+    <t>1c599dcf-14c0-4615-8f2b-df97f3cc7b18</t>
+  </si>
+  <si>
+    <t>a457c865-81e1-40f9-aca0-4effdb5feace</t>
+  </si>
+  <si>
+    <t>911fed0e-aac1-4729-ab5f-3a1272c2feb8</t>
+  </si>
+  <si>
+    <t>46baddad-7fe4-4d43-b6e6-e32ab4dbb420</t>
+  </si>
+  <si>
+    <t>59f688fe-346c-4283-b596-b939621258c9</t>
+  </si>
+  <si>
+    <t>625546ec-3494-4304-b601-16374913ce24</t>
+  </si>
+  <si>
+    <t>5bb55b83-f88f-4e75-918f-2d24e49741f1</t>
+  </si>
+  <si>
+    <t>0997f571-5549-487f-8f9c-99e05acd1dce</t>
+  </si>
+  <si>
+    <t>adfc9ba1-2517-4658-ac38-2a468a0bfaa8</t>
+  </si>
+  <si>
+    <t>d0af56ea-93bb-4e01-a94c-007c71a5d973</t>
+  </si>
+  <si>
+    <t>7e4063a8-4f84-4cff-b152-c91800cfef40</t>
+  </si>
+  <si>
+    <t>3b2f4967-c6ca-40ce-921e-1dc981ad7849</t>
+  </si>
+  <si>
+    <t>345d502d-2ce9-4efa-8060-8c4a7621fddb</t>
   </si>
   <si>
     <t>Value true in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>a5f45702-0192-4550-ae5d-b6d24eb7c1b3</t>
-  </si>
-  <si>
-    <t>dec3e3c7-ad92-4726-af4f-6ede46b091f9</t>
-  </si>
-  <si>
-    <t>03e0f46e-a9df-4ba5-8a3d-7d505d43f2e6</t>
-  </si>
-  <si>
-    <t>1e325f72-9f46-4b8f-993a-4e1e6dcbd6d4</t>
-  </si>
-  <si>
-    <t>994c7d58-d3ec-402b-a2ed-a71c41cab968</t>
-  </si>
-  <si>
-    <t>c4546a9b-4c03-41eb-8139-38b396cd7a90</t>
-  </si>
-  <si>
-    <t>55d6b53e-57b9-4c30-bd65-6a399fa243bc</t>
-  </si>
-  <si>
-    <t>2c94ec91-d26a-4c72-b451-ef7f26c43930</t>
-  </si>
-  <si>
-    <t>8ae744ad-f7b4-4442-b7c4-eb6b5ec122ea</t>
+    <t>1312c867-b24c-4f5d-89a5-096a81753765</t>
+  </si>
+  <si>
+    <t>da715ba9-8f22-4b80-b9fa-1f4e64237210</t>
+  </si>
+  <si>
+    <t>459a1b7b-2468-44eb-a337-2ffcb43e29c3</t>
+  </si>
+  <si>
+    <t>2edcd505-7ffc-43f0-bf4c-9e8fa2fd07a7</t>
+  </si>
+  <si>
+    <t>9ed92dcf-5c39-4a1d-8e28-faa42c44c383</t>
+  </si>
+  <si>
+    <t>9b03eee0-24f8-41e9-8ad9-f8e57f07a9d3</t>
+  </si>
+  <si>
+    <t>3e1dcb58-6e66-4555-8c00-eaba3bcc6eff</t>
+  </si>
+  <si>
+    <t>9b891b6f-eb49-4114-a83d-c984f92dbe93</t>
+  </si>
+  <si>
+    <t>173dc2a1-8175-4cdb-8d3e-2d129215813c</t>
   </si>
   <si>
     <t>Value false in VISIT_OMH_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -903,85 +903,85 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OMH_FLAG</t>
   </si>
   <si>
-    <t>ecf37f45-081f-4a8a-becc-6dabb0ab5fed</t>
-  </si>
-  <si>
-    <t>a101ea39-a97c-443f-86cd-d42116c682c8</t>
-  </si>
-  <si>
-    <t>9186c474-21de-4ed2-8a0c-a54563fa41fd</t>
-  </si>
-  <si>
-    <t>9cd84164-3eb8-4838-930a-97275f1f7c30</t>
-  </si>
-  <si>
-    <t>c7c97874-6b9a-4fcd-bdd3-ce64b74dd9fb</t>
-  </si>
-  <si>
-    <t>211b5b91-185a-47a9-9fe4-d81ec0212b06</t>
-  </si>
-  <si>
-    <t>faedc5e4-ebba-421f-b868-6a3e7c219cf9</t>
-  </si>
-  <si>
-    <t>877e5fac-ac96-463d-91ce-ac6fe1d0d49e</t>
-  </si>
-  <si>
-    <t>3f03a5bd-7af0-49a5-9b49-6a1e851045c6</t>
-  </si>
-  <si>
-    <t>711e11a1-e097-4dad-8cac-f92e9572b6be</t>
-  </si>
-  <si>
-    <t>bcf5b66b-eda8-437c-8e5b-73b73f60e937</t>
-  </si>
-  <si>
-    <t>64465f09-cabd-4457-9279-6dc26a9f4fd6</t>
-  </si>
-  <si>
-    <t>1aeaf602-55e2-44e2-9924-6b793aebb69c</t>
-  </si>
-  <si>
-    <t>1acffa15-8021-4a8b-bb75-802861427ee0</t>
-  </si>
-  <si>
-    <t>d0a7aec8-c0f5-4e5b-8635-68ff44f658d1</t>
-  </si>
-  <si>
-    <t>4b0f38b5-68df-4d48-8293-be32c645e0b4</t>
-  </si>
-  <si>
-    <t>d76ca0fa-2b40-44bc-88da-a1ca980c40c1</t>
-  </si>
-  <si>
-    <t>8f3e80d8-d996-4455-826d-a4fae88cdeda</t>
-  </si>
-  <si>
-    <t>78a1d30b-ca68-43e2-ad5d-742968b5c4e2</t>
-  </si>
-  <si>
-    <t>f2f28807-b8de-4b4d-a85a-ee74c4475337</t>
-  </si>
-  <si>
-    <t>45132a92-2e13-42f3-b227-bf6b223ccc30</t>
-  </si>
-  <si>
-    <t>4aba9bf5-0d92-4044-9dba-667eb4f9498d</t>
-  </si>
-  <si>
-    <t>515488cf-bafa-4142-90d3-cca671935987</t>
-  </si>
-  <si>
-    <t>8b1b7a6d-e4c0-439c-ac30-d76cb293bd64</t>
-  </si>
-  <si>
-    <t>5b65f0ca-3e39-425c-9b3d-a9521bbae9f3</t>
-  </si>
-  <si>
-    <t>538f8ba4-06cf-4e77-b3c6-34a674dfc307</t>
-  </si>
-  <si>
-    <t>52e9a4b6-3d6f-459c-a52f-25fdb2c1cc0f</t>
+    <t>f3e1bda2-63fe-49c7-9fd9-0a86b8ce3682</t>
+  </si>
+  <si>
+    <t>bada0d52-c0f9-4a56-8dff-29b9ce12be6c</t>
+  </si>
+  <si>
+    <t>03b4b01b-3e78-4518-a92b-7a669484a5f3</t>
+  </si>
+  <si>
+    <t>43d6e5f2-d832-4cae-ab87-65759218a9f8</t>
+  </si>
+  <si>
+    <t>4d230d85-c67e-4b26-9aca-23ab70aa44d7</t>
+  </si>
+  <si>
+    <t>6e6fbab4-9cf0-412c-8458-6812336e090a</t>
+  </si>
+  <si>
+    <t>c16a5219-c048-46b9-a8fa-0ee344e1b7f4</t>
+  </si>
+  <si>
+    <t>eb8299ca-1bec-4a8b-a69c-eb80b23a51ce</t>
+  </si>
+  <si>
+    <t>70d625d5-32d0-4bb3-bb2f-6aeb2b660755</t>
+  </si>
+  <si>
+    <t>68104db7-1081-4d59-8fee-827765fbd71c</t>
+  </si>
+  <si>
+    <t>8e7e334b-4c92-4b16-8ee4-7a71a61adcea</t>
+  </si>
+  <si>
+    <t>34ed810c-acd2-4e25-a89d-7e39bf3f23b2</t>
+  </si>
+  <si>
+    <t>f71bcad1-bca8-4901-9294-4cd7db7693f8</t>
+  </si>
+  <si>
+    <t>8d36586c-0b11-4c22-b249-b05f5da5a54d</t>
+  </si>
+  <si>
+    <t>fc24824f-404b-4945-a907-e4503e7475df</t>
+  </si>
+  <si>
+    <t>cedde292-b624-46ac-aa2f-0e0d1129d28f</t>
+  </si>
+  <si>
+    <t>6a1363e0-1b06-4b1e-896b-f05deab75041</t>
+  </si>
+  <si>
+    <t>a94fb550-9355-46de-803a-6803115d16da</t>
+  </si>
+  <si>
+    <t>0faa1afb-3322-4152-aab4-0167fd0b8ed9</t>
+  </si>
+  <si>
+    <t>b76adcae-95f5-4a8b-bb14-dc5e9a5d4b1e</t>
+  </si>
+  <si>
+    <t>770ed0e2-886d-4fae-b60c-ae4d563f2469</t>
+  </si>
+  <si>
+    <t>872b5d08-c726-4d1e-a207-2439c3029daa</t>
+  </si>
+  <si>
+    <t>2f5f8358-41ba-4cf3-a3eb-b626e99afe59</t>
+  </si>
+  <si>
+    <t>484fe084-e063-4aee-bb7b-b328917fdaeb</t>
+  </si>
+  <si>
+    <t>23339f9a-f7be-41c7-9604-accffe337b0a</t>
+  </si>
+  <si>
+    <t>80a87d81-e5f1-4fd6-84a8-491193a6cf0e</t>
+  </si>
+  <si>
+    <t>7b8c16f3-24de-4499-9cb7-9f53ddf359b9</t>
   </si>
   <si>
     <t>Value false in VISIT_OPWDD_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -993,82 +993,82 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OPWDD_FLAG</t>
   </si>
   <si>
-    <t>b1f55aae-fd97-4531-b068-4d412134cfbf</t>
-  </si>
-  <si>
-    <t>2deed5e9-d6a3-4363-b9f1-7955e01876a5</t>
-  </si>
-  <si>
-    <t>45edd0f3-163d-430a-9ca5-96799e81d72d</t>
-  </si>
-  <si>
-    <t>f509e77d-16c8-4739-b4ae-005b1ad8c27a</t>
-  </si>
-  <si>
-    <t>ec141418-942c-439a-92f1-34424612ff4a</t>
-  </si>
-  <si>
-    <t>a668ca97-07f0-4362-a84e-808bff8de94b</t>
-  </si>
-  <si>
-    <t>1b2c1c50-63f9-4a47-8275-0071de32b6be</t>
-  </si>
-  <si>
-    <t>1ecc83cd-4e42-4914-a5db-22cdd027ee9e</t>
-  </si>
-  <si>
-    <t>844c3154-b6ba-474b-92dd-122f02e12fd2</t>
-  </si>
-  <si>
-    <t>71835028-2616-4c24-aa65-76c14725442d</t>
-  </si>
-  <si>
-    <t>0e8f2e18-8d28-410b-9032-c2a034d499a0</t>
-  </si>
-  <si>
-    <t>69fde92c-3dfd-4c68-853b-b25231ccfbf6</t>
-  </si>
-  <si>
-    <t>067925b4-ff2b-41c8-9656-18e4fcfb2189</t>
-  </si>
-  <si>
-    <t>350f50bb-9d56-4289-9631-434f3e6ef6b6</t>
-  </si>
-  <si>
-    <t>c94d3dd1-2777-4c27-9609-6c514b2e13c7</t>
-  </si>
-  <si>
-    <t>dff9ba69-d523-4c7f-bd8d-4779c3e542fe</t>
-  </si>
-  <si>
-    <t>81a47774-facd-4ccf-8267-94e1c12e8b13</t>
-  </si>
-  <si>
-    <t>a1f59058-494e-40bf-b1fb-4c9c04970216</t>
-  </si>
-  <si>
-    <t>3d16878b-3c2c-48f8-8ef0-3a1a26961f98</t>
-  </si>
-  <si>
-    <t>6792c429-0203-4624-8970-4430b1efc4fb</t>
-  </si>
-  <si>
-    <t>5b28a8a7-e506-492e-975d-b7739838e93a</t>
-  </si>
-  <si>
-    <t>f222b01b-47b2-462d-9c25-d40f24b78e96</t>
-  </si>
-  <si>
-    <t>fc85c3e1-5c95-4037-afe1-037ec414169e</t>
-  </si>
-  <si>
-    <t>1d82ccc2-f41a-4114-b3d2-6c756ac312e5</t>
-  </si>
-  <si>
-    <t>ab25c6e7-0c1f-424f-a3a9-64509cf7fd0e</t>
-  </si>
-  <si>
-    <t>efc9abd3-7689-42e0-af36-315e20412e37</t>
+    <t>58b3495d-925f-4c35-8d73-5a1be9a95c4f</t>
+  </si>
+  <si>
+    <t>34c5b6b8-a92a-438b-b425-3953556876af</t>
+  </si>
+  <si>
+    <t>395d497a-0e8e-4dc4-b5c4-91060afd969c</t>
+  </si>
+  <si>
+    <t>556e09fb-719b-4350-92ea-7e66d70e8994</t>
+  </si>
+  <si>
+    <t>09393601-1eff-48b3-b81c-0c500fa42136</t>
+  </si>
+  <si>
+    <t>72a1e7bc-b366-4d60-9dd6-84c350ff35b3</t>
+  </si>
+  <si>
+    <t>9f77d07a-9b43-4564-a83b-13aac3313c73</t>
+  </si>
+  <si>
+    <t>6740d6f9-06db-447c-a593-77f9ded0c5e2</t>
+  </si>
+  <si>
+    <t>a49b2702-7f52-4e73-a15b-4fe6a9a10499</t>
+  </si>
+  <si>
+    <t>b075a877-3a40-4235-8cc0-ce666cd6d168</t>
+  </si>
+  <si>
+    <t>689c9134-f5bb-47a6-82f9-9a6b715d6d8e</t>
+  </si>
+  <si>
+    <t>d2492bea-bda9-4dec-a44a-045296d9623a</t>
+  </si>
+  <si>
+    <t>966190b7-11de-4e08-ae12-84c4e181ebef</t>
+  </si>
+  <si>
+    <t>b7d07a9b-4472-4566-8340-cad030b50cf8</t>
+  </si>
+  <si>
+    <t>4edc647b-d63b-473d-8355-18df8ff504d0</t>
+  </si>
+  <si>
+    <t>9178c936-e288-4784-9b06-7f3144fc544e</t>
+  </si>
+  <si>
+    <t>0e2320ee-261f-49a9-bd5c-d9225b01a937</t>
+  </si>
+  <si>
+    <t>1ef4ed47-63fe-45ec-9382-1d4eb3a04a5e</t>
+  </si>
+  <si>
+    <t>4154334a-0d73-4501-861f-8461b7d8e03d</t>
+  </si>
+  <si>
+    <t>751239b2-b6a4-48a7-80c2-af9f55bbed7e</t>
+  </si>
+  <si>
+    <t>a1e3a8ae-6883-4cfa-a266-f11d79c55c19</t>
+  </si>
+  <si>
+    <t>5dacbd20-4279-4b36-8b4d-b9443981863b</t>
+  </si>
+  <si>
+    <t>b55ab072-2992-4bc5-ab48-bf7ee069876c</t>
+  </si>
+  <si>
+    <t>df86d8dd-c1d2-449a-aedf-eba74c3c9c1c</t>
+  </si>
+  <si>
+    <t>054bafaa-e4f0-461f-8a82-88e0c25dd03e</t>
+  </si>
+  <si>
+    <t>667647ed-6e03-4a01-a02b-051b17b9e85e</t>
   </si>
   <si>
     <t>2afb3098-bcfd-5a54-8ebb-4d65d399c55e</t>
@@ -1080,7 +1080,7 @@
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>0bfd672c-260b-499d-ad8d-70442e586806</t>
+    <t>73405275-9054-4dba-8c76-4a3f7e97bc92</t>
   </si>
   <si>
     <t>Value 	20430005 in SEXUAL_ORIENTATION_CODE not in allowed list ('42035005','20430005','38628009','OTH','UNK')</t>
@@ -1101,7 +1101,7 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>c796a36d-3fd3-461b-9f4f-d79e30335bff</t>
+    <t>91722004-9020-4eb6-bab5-909de59b04eb</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -1116,16 +1116,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>3474d363-f086-4760-8f98-227864ab055c</t>
-  </si>
-  <si>
-    <t>f91e1895-fa7c-4df9-82a9-39379062b0bc</t>
-  </si>
-  <si>
-    <t>127558cb-8bb1-486c-b127-27a52256e9eb</t>
-  </si>
-  <si>
-    <t>5b4f9220-a142-4de0-9ef8-c51e243a315e</t>
+    <t>f7e9a73c-e8c6-482c-9cd1-d35a7050be00</t>
+  </si>
+  <si>
+    <t>6763e66d-e77a-4b16-a2ef-efeb757ceee4</t>
+  </si>
+  <si>
+    <t>63ca0389-77d9-412d-8330-80e7d5a8b59f</t>
+  </si>
+  <si>
+    <t>64f7eaaa-a5e0-43a8-938c-e00faf146855</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -1137,16 +1137,16 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>8a3ce826-600c-4929-a598-1d579ac0b1a0</t>
-  </si>
-  <si>
-    <t>08cc3aa4-3a68-4f75-a33c-988ffa7d2c27</t>
-  </si>
-  <si>
-    <t>061f891a-9d62-4b9a-9e7a-94c7ab3fbb94</t>
-  </si>
-  <si>
-    <t>0a9433ad-150a-4fc1-9bfa-80fa95d72d92</t>
+    <t>0326f614-ad3e-43b9-bf5b-e7c59a1b0411</t>
+  </si>
+  <si>
+    <t>129949c0-37d0-4611-a97b-e6095f882d9c</t>
+  </si>
+  <si>
+    <t>cb970457-300d-4a00-9415-702035eeca0d</t>
+  </si>
+  <si>
+    <t>f0871593-a570-4b87-b125-27708eaf198b</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -1155,16 +1155,16 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>613b7841-ec05-4dc2-8f60-0ef0191f1832</t>
-  </si>
-  <si>
-    <t>cd08e268-d48a-4564-88ee-97288babeb74</t>
-  </si>
-  <si>
-    <t>3306f96a-3c06-4d1e-ab0d-a9e0414b39bb</t>
-  </si>
-  <si>
-    <t>fe422644-8791-4e73-a392-21c5910469d7</t>
+    <t>03a0d417-0724-4a66-9b54-803473080d0b</t>
+  </si>
+  <si>
+    <t>72e9c77e-c78e-4792-a707-cb284b158e6a</t>
+  </si>
+  <si>
+    <t>11602052-a7ea-4e2b-9367-d1b907d117fa</t>
+  </si>
+  <si>
+    <t>9cebe92d-c5ab-4efe-9c93-f0b87dd354e9</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -1176,16 +1176,16 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>dde6ef84-7491-42cf-9341-f154afa964a1</t>
-  </si>
-  <si>
-    <t>d9840dbb-51b2-4602-9569-790bb5065775</t>
-  </si>
-  <si>
-    <t>f516fccb-a4db-4c94-9912-ed60467e8906</t>
-  </si>
-  <si>
-    <t>6c8154bb-ce8a-4193-8b30-74817589f5ee</t>
+    <t>d8ed4451-eaad-48c2-bc14-79951d522edc</t>
+  </si>
+  <si>
+    <t>367208b3-ae91-4873-a297-d5d4a36bea26</t>
+  </si>
+  <si>
+    <t>07959b46-d913-4753-bf5d-696af801237e</t>
+  </si>
+  <si>
+    <t>ec7d9603-a7ef-4112-be67-e598e0b67da0</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE is empty</t>
@@ -1197,22 +1197,22 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>f4b2d979-0846-43fe-87f7-aaa1a8b882b0</t>
-  </si>
-  <si>
-    <t>56511bb5-4b56-43c1-8f1c-1ed82664016c</t>
-  </si>
-  <si>
-    <t>2a9da0c2-f754-4f24-9857-d7cbbc668853</t>
-  </si>
-  <si>
-    <t>f1aa86f8-d476-49dc-887c-23e4a934c884</t>
-  </si>
-  <si>
-    <t>cc2dfe63-1674-46b1-826d-9498a9952866</t>
-  </si>
-  <si>
-    <t>569ffd82-32f7-40ad-904f-e61825bcd14d</t>
+    <t>2f946053-6387-4466-b9c7-44f11e985f4a</t>
+  </si>
+  <si>
+    <t>037bbebc-9b6a-43a9-9744-d9e183dd0f3b</t>
+  </si>
+  <si>
+    <t>e84e31e9-911e-44cf-96f8-3473ac2d881d</t>
+  </si>
+  <si>
+    <t>68db9b57-561d-4549-ba4b-122753659610</t>
+  </si>
+  <si>
+    <t>ef806370-d294-4900-af73-668d4e6c549a</t>
+  </si>
+  <si>
+    <t>aa7e72f2-80d9-4163-aaca-ecb0d8e37220</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -1224,19 +1224,19 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>bdd64e84-1cbd-4ffe-a2d4-455dc2ed23c3</t>
-  </si>
-  <si>
-    <t>ef0ebf61-3f2d-441a-93a7-e3a026ca338f</t>
-  </si>
-  <si>
-    <t>831016b2-caa0-4f36-83fb-eb9511085c95</t>
-  </si>
-  <si>
-    <t>79718a15-5d27-4ef5-b758-e2cf8502b30c</t>
-  </si>
-  <si>
-    <t>ceba7a1e-afd1-4741-bb7b-869755ae23f2</t>
+    <t>07bc494d-508b-4682-9819-393969403c63</t>
+  </si>
+  <si>
+    <t>46b25d0d-4385-43b7-b0d4-1278541c47cb</t>
+  </si>
+  <si>
+    <t>ca04bbf9-610b-4131-be63-31333a04d75a</t>
+  </si>
+  <si>
+    <t>06d1a211-bb43-4ceb-93b2-3815c3af1478</t>
+  </si>
+  <si>
+    <t>99a5a44c-57c2-4eb1-ba92-78b7e0e86d22</t>
   </si>
   <si>
     <t>86ff3ab6-900d-5474-b63c-cbcac3c66f1a</t>

</xml_diff>

<commit_message>
feat: implement initial SFTP structure #12
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -78,7 +78,7 @@
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx</t>
   </si>
   <si>
     <t>ERROR</t>
@@ -132,7 +132,7 @@
     <t>591191c7-f693-5957-8734-ac87151ca981</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-25-valid.xlsx</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-25-valid.xlsx</t>
   </si>
   <si>
     <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
@@ -153,7 +153,7 @@
     <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
   </si>
   <si>
     <t>a3fe7098-8ae8-5612-81ac-cbe10780c19b</t>
@@ -201,7 +201,7 @@
     <t>c302047e-21cf-5059-a32c-e81a9bd3a9b9</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
   </si>
   <si>
     <t>3252fee6-3a9a-5f4c-81c6-739201046d79</t>
@@ -249,13 +249,13 @@
     <t>0adb81bc-3df2-5f86-99cc-2d20e1dd5efd</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail.csv</t>
   </si>
   <si>
     <t>synthetic_fail</t>
   </si>
   <si>
-    <t>a58b9b5d-bc24-4331-a0e3-9a640e331705</t>
+    <t>fd45e704-6f67-4135-b40d-f5428cac3200</t>
   </si>
   <si>
     <t>Missing Column</t>
@@ -267,7 +267,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>3860d091-d94d-4ac4-a9ee-7841494c22b9</t>
+    <t>edf8b4bf-75b5-4596-b0f4-01a5abcaa68a</t>
   </si>
   <si>
     <t>Required column ANSWER_CODE is missing in synthetic_fail.</t>
@@ -276,7 +276,7 @@
     <t>Ensure synthetic_fail contains the column "ANSWER_CODE"</t>
   </si>
   <si>
-    <t>41ddcc8c-cdea-4339-a796-23a100ebc9bf</t>
+    <t>f371a846-47c5-4685-8372-c60b11f0e591</t>
   </si>
   <si>
     <t>Required column ENCOUNTER_ID is missing in synthetic_fail.</t>
@@ -285,7 +285,7 @@
     <t>Ensure synthetic_fail contains the column "ENCOUNTER_ID"</t>
   </si>
   <si>
-    <t>ff0c36d7-cbb9-45d2-80a8-9ea8967646aa</t>
+    <t>67679e9d-7296-436d-b5a6-670a2773c6ef</t>
   </si>
   <si>
     <t>Required column FACILITY is missing in synthetic_fail.</t>
@@ -294,7 +294,7 @@
     <t>Ensure synthetic_fail contains the column "FACILITY"</t>
   </si>
   <si>
-    <t>816c9a41-536e-482a-a1e2-cfc3a9ff839c</t>
+    <t>81c5126f-3da7-426f-9da3-68e32d731988</t>
   </si>
   <si>
     <t>Required column FIRST_NAME is missing in synthetic_fail.</t>
@@ -303,7 +303,7 @@
     <t>Ensure synthetic_fail contains the column "FIRST_NAME"</t>
   </si>
   <si>
-    <t>ec4115d4-882b-47bf-92c9-d3e01d2152ea</t>
+    <t>a7e02a37-3d31-41fc-add9-b6f4bef30a1a</t>
   </si>
   <si>
     <t>Required column LAST_NAME is missing in synthetic_fail.</t>
@@ -312,7 +312,7 @@
     <t>Ensure synthetic_fail contains the column "LAST_NAME"</t>
   </si>
   <si>
-    <t>c1358876-388b-4ecd-a4cf-d22577045e6e</t>
+    <t>641e4602-1526-41c7-a780-550c273a4e60</t>
   </si>
   <si>
     <t>Required column MEAS_VALUE is missing in synthetic_fail.</t>
@@ -321,7 +321,7 @@
     <t>Ensure synthetic_fail contains the column "MEAS_VALUE"</t>
   </si>
   <si>
-    <t>11f6a6ac-a621-466e-af0e-795201617eb0</t>
+    <t>4159ca7e-bb65-402b-b895-4f370ceee01c</t>
   </si>
   <si>
     <t>Required column MEDICAID_CIN is missing in synthetic_fail.</t>
@@ -330,7 +330,7 @@
     <t>Ensure synthetic_fail contains the column "MEDICAID_CIN"</t>
   </si>
   <si>
-    <t>49d19ca5-ff15-47b4-8dd1-ff7178dafb69</t>
+    <t>ada38788-42d4-4ff5-9166-5be3fe036551</t>
   </si>
   <si>
     <t>Required column NEED_INDICATED is missing in synthetic_fail.</t>
@@ -339,7 +339,7 @@
     <t>Ensure synthetic_fail contains the column "NEED_INDICATED"</t>
   </si>
   <si>
-    <t>36124f7d-6013-4d54-8bd1-b62b75cd070e</t>
+    <t>6d3db944-fa21-4571-8fca-d0b2815c299d</t>
   </si>
   <si>
     <t>Required column PAT_BIRTH_DATE is missing in synthetic_fail.</t>
@@ -348,7 +348,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_BIRTH_DATE"</t>
   </si>
   <si>
-    <t>e9be76dd-ddc0-48bb-b9e7-6c52a7283472</t>
+    <t>d23ea33f-d32e-436e-8ac3-893f152a7ccc</t>
   </si>
   <si>
     <t>Required column PAT_MRN_ID is missing in synthetic_fail.</t>
@@ -357,7 +357,7 @@
     <t>Ensure synthetic_fail contains the column "PAT_MRN_ID"</t>
   </si>
   <si>
-    <t>75dbaf65-57e9-49e8-b835-dd6de3e56d97</t>
+    <t>23d43e2a-dd0c-4dda-bd80-35460abd2886</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE_SYSTEM_NAME is missing in synthetic_fail.</t>
@@ -366,7 +366,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE_SYSTEM_NAME"</t>
   </si>
   <si>
-    <t>9bad977a-e9e5-472b-81f7-9ec4d6cf1721</t>
+    <t>e9c8d7ce-46af-4594-9227-644a6fb446de</t>
   </si>
   <si>
     <t>Required column QUESTION_CODE is missing in synthetic_fail.</t>
@@ -375,7 +375,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION_CODE"</t>
   </si>
   <si>
-    <t>baa4f65c-5fbe-4e4f-8948-b8e47b485ea2</t>
+    <t>ff7ec8e6-93af-4ed8-b189-3bd22d4e2f91</t>
   </si>
   <si>
     <t>Required column QUESTION is missing in synthetic_fail.</t>
@@ -384,7 +384,7 @@
     <t>Ensure synthetic_fail contains the column "QUESTION"</t>
   </si>
   <si>
-    <t>c5c52f1f-22bc-4e11-8864-17783c9a80f4</t>
+    <t>83b916f1-f25c-431e-8c81-9429805ccd90</t>
   </si>
   <si>
     <t>Required column RECORDED_TIME is missing in synthetic_fail.</t>
@@ -393,7 +393,7 @@
     <t>Ensure synthetic_fail contains the column "RECORDED_TIME"</t>
   </si>
   <si>
-    <t>c65ab026-cadc-42f2-b317-b4fa5f532d28</t>
+    <t>2879b173-8018-4f57-8ca3-23fbd9a807a1</t>
   </si>
   <si>
     <t>Required column SDOH_DOMAIN is missing in synthetic_fail.</t>
@@ -402,7 +402,7 @@
     <t>Ensure synthetic_fail contains the column "SDOH_DOMAIN"</t>
   </si>
   <si>
-    <t>cded0d34-2904-4693-bd3b-fc45f0d2bd12</t>
+    <t>76bbbdb0-f884-4859-bfc8-cceaf3c73d84</t>
   </si>
   <si>
     <t>Required column SURVEY_ID is missing in synthetic_fail.</t>
@@ -411,7 +411,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY_ID"</t>
   </si>
   <si>
-    <t>bc938a0e-8f37-4aeb-a45d-a80eb219e904</t>
+    <t>5f8194da-2398-4fc8-bf8a-091c8eaa6144</t>
   </si>
   <si>
     <t>Required column SURVEY is missing in synthetic_fail.</t>
@@ -420,7 +420,7 @@
     <t>Ensure synthetic_fail contains the column "SURVEY"</t>
   </si>
   <si>
-    <t>ecefa7cd-5ec6-4781-b4d8-4a1cdee286c3</t>
+    <t>cf005ab3-b5eb-4edb-8704-f831129fe06c</t>
   </si>
   <si>
     <t>Required column VISIT_OMH_FLAG is missing in synthetic_fail.</t>
@@ -429,7 +429,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OMH_FLAG"</t>
   </si>
   <si>
-    <t>965f300a-8cfb-413f-a6fb-7b862dcefc2d</t>
+    <t>4d4d98ac-42b8-415d-9776-7e75b1e47ceb</t>
   </si>
   <si>
     <t>Required column VISIT_OPWDD_FLAG is missing in synthetic_fail.</t>
@@ -438,7 +438,7 @@
     <t>Ensure synthetic_fail contains the column "VISIT_OPWDD_FLAG"</t>
   </si>
   <si>
-    <t>9839803c-c8b3-4a32-8cdb-47ac28c43ca3</t>
+    <t>7af6fba4-5837-4681-af39-469b08d33236</t>
   </si>
   <si>
     <t>Required column VISIT_PART_2_FLAG is missing in synthetic_fail.</t>
@@ -450,13 +450,13 @@
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-12-valid.csv</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2023-12-12-valid.csv</t>
   </si>
   <si>
     <t>ahc_hrsn_2023_12_12_valid</t>
   </si>
   <si>
-    <t>222df9d5-2ccd-4ba6-b5df-54894aa9bdbc</t>
+    <t>467f221d-83ad-44e8-9af9-f25d263122c3</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -474,7 +474,7 @@
     <t>Use only allowed values '71802-3','96778-6' in QUESTION_CODE</t>
   </si>
   <si>
-    <t>68be5a76-9ae9-47f0-a2ec-81d0682f2b51</t>
+    <t>65fa2e8f-d2a7-454f-be5f-e35dccb6d9e0</t>
   </si>
   <si>
     <t>Value 88122-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -483,7 +483,7 @@
     <t>88122-7</t>
   </si>
   <si>
-    <t>e6b40756-db9c-49a6-984a-1df62cfbe7e8</t>
+    <t>048d15ed-2b7c-43fc-b076-5186300aaaf9</t>
   </si>
   <si>
     <t>Value 88123-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -492,7 +492,7 @@
     <t>88123-5</t>
   </si>
   <si>
-    <t>802ef63a-e1da-4309-9b7c-8956beb142e1</t>
+    <t>86df3636-8843-4d09-9ee8-03945c221fa6</t>
   </si>
   <si>
     <t>Value 93030-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -501,7 +501,7 @@
     <t>93030-5</t>
   </si>
   <si>
-    <t>de6dcf64-e504-4c0b-bebb-fbcc517f823a</t>
+    <t>905fe86f-ad0e-41ed-b395-357cf0dbba3f</t>
   </si>
   <si>
     <t>Value 96779-4 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -510,7 +510,7 @@
     <t>96779-4</t>
   </si>
   <si>
-    <t>6e39b643-e1c9-49a5-a130-e7ee09223efb</t>
+    <t>86c5de7f-95b4-451a-a3bc-91e634bfdf06</t>
   </si>
   <si>
     <t>Value 95618-5 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -519,7 +519,7 @@
     <t>95618-5</t>
   </si>
   <si>
-    <t>a599a953-0257-4c23-9216-7eba9b8e825f</t>
+    <t>d2c44957-b54f-495e-92c2-69bc755dfe4a</t>
   </si>
   <si>
     <t>Value 95617-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -528,7 +528,7 @@
     <t>95617-7</t>
   </si>
   <si>
-    <t>bf2cc2e5-214f-4177-8b73-c4be58002e45</t>
+    <t>6a773c17-4179-4106-8a52-4eafc7ffb10e</t>
   </si>
   <si>
     <t>Value 95616-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -537,7 +537,7 @@
     <t>95616-9</t>
   </si>
   <si>
-    <t>48117ff7-4689-48f4-a195-cf6b69198051</t>
+    <t>1561c18e-6bc5-4d43-af29-c5c9f40c42a4</t>
   </si>
   <si>
     <t>Value 95615-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -546,7 +546,7 @@
     <t>95615-1</t>
   </si>
   <si>
-    <t>d8fc6ae2-ebbe-485f-b204-2393ea3ec994</t>
+    <t>a880766d-001f-435a-802a-5e8d629807bd</t>
   </si>
   <si>
     <t>Value 76513-1 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -555,7 +555,7 @@
     <t>76513-1</t>
   </si>
   <si>
-    <t>4acfc863-3e1b-4aa1-a2b2-283c1fe8c364</t>
+    <t>0eb0a9ec-5ff5-4a8d-9dde-057c6826dbd1</t>
   </si>
   <si>
     <t>Value 96780-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -564,7 +564,7 @@
     <t>96780-2</t>
   </si>
   <si>
-    <t>f3e5d0c0-817b-43b9-820c-c4952bcacef0</t>
+    <t>6a85e144-02d6-4e9d-af23-0968c51dac8e</t>
   </si>
   <si>
     <t>Value 96781-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -573,7 +573,7 @@
     <t>96781-0</t>
   </si>
   <si>
-    <t>7d8396ca-80b5-4b36-91b4-4a98c8819ec1</t>
+    <t>69426ba9-3b4d-4034-98b0-edbaea74536c</t>
   </si>
   <si>
     <t>Value 93159-2	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -582,7 +582,7 @@
     <t>93159-2	</t>
   </si>
   <si>
-    <t>bf54f5db-adb2-49cc-8bcb-28a44126ee48</t>
+    <t>38d69217-6de3-46af-9259-c9cb8875c33e</t>
   </si>
   <si>
     <t>Value 97027-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -591,7 +591,7 @@
     <t>97027-7</t>
   </si>
   <si>
-    <t>9198619b-ec93-4fec-b269-4c0a4aae8452</t>
+    <t>202439c9-8c59-4876-bd93-3980a795cbdb</t>
   </si>
   <si>
     <t>Value 96782-8	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -600,7 +600,7 @@
     <t>96782-8	</t>
   </si>
   <si>
-    <t>fe955683-66f1-4276-80a7-a21349991ed7</t>
+    <t>4fdc1daa-d789-4520-a8da-f2c0914ae282</t>
   </si>
   <si>
     <t>Value 89555-7 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -609,7 +609,7 @@
     <t>89555-7</t>
   </si>
   <si>
-    <t>22188e21-8580-40e5-b452-51ad68fd59c3</t>
+    <t>031af154-e38e-4de9-be10-5d104083b46c</t>
   </si>
   <si>
     <t>Value 68516-4	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -618,7 +618,7 @@
     <t>68516-4	</t>
   </si>
   <si>
-    <t>53a6982a-18cb-4036-8c82-05d4acd74d2f</t>
+    <t>390639ab-f156-4e60-b87c-af6bb23f5078</t>
   </si>
   <si>
     <t>Value 68517-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -627,7 +627,7 @@
     <t>68517-2</t>
   </si>
   <si>
-    <t>30f2c836-a651-465d-a41e-959b890b3896</t>
+    <t>219774d2-6bf0-4ee9-940f-3a92e928100c</t>
   </si>
   <si>
     <t>Value 96842-0 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -636,7 +636,7 @@
     <t>96842-0</t>
   </si>
   <si>
-    <t>99c07054-1037-4c19-9c40-41048c93896a</t>
+    <t>d94e1e1a-2a41-47ed-a099-d81c6e531ed5</t>
   </si>
   <si>
     <t>Value 95530-2 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -645,7 +645,7 @@
     <t>95530-2</t>
   </si>
   <si>
-    <t>fffc3ca7-555b-473a-9bfb-c26522f4b970</t>
+    <t>836967b5-c12a-4518-9d52-1564fd349add</t>
   </si>
   <si>
     <t>Value 68524-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -654,7 +654,7 @@
     <t>68524-8</t>
   </si>
   <si>
-    <t>ec14109b-db1a-4c1c-a456-5ccfd93937e5</t>
+    <t>4233083a-f220-4df5-8bf2-f6e587991636</t>
   </si>
   <si>
     <t>Value 44250-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -663,7 +663,7 @@
     <t>44250-9</t>
   </si>
   <si>
-    <t>74f8798e-d50f-449e-b786-9771a07becf6</t>
+    <t>f66ca25b-0c58-4699-acdf-f43da57d02fc</t>
   </si>
   <si>
     <t>Value 44255-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -672,7 +672,7 @@
     <t>44255-8</t>
   </si>
   <si>
-    <t>b551d98b-4234-42a1-95af-0975f3622a72</t>
+    <t>c3d69f6e-dcf3-4215-ae05-319e587c1021</t>
   </si>
   <si>
     <t>Value 93038-8 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -681,7 +681,7 @@
     <t>93038-8</t>
   </si>
   <si>
-    <t>e7956b29-2f1f-44d0-b677-189dafecd9d9</t>
+    <t>54ed73df-0078-4f4f-a226-0e67ba4cab48</t>
   </si>
   <si>
     <t>Value 69858-9 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -690,7 +690,7 @@
     <t>69858-9</t>
   </si>
   <si>
-    <t>9c0829f6-a638-4840-9bf7-e8f093975adf</t>
+    <t>055e6834-be48-467f-9b01-b7bb737e6922</t>
   </si>
   <si>
     <t>Value 69861-3	 in QUESTION_CODE not in allowed list ('71802-3','96778-6')</t>
@@ -699,7 +699,7 @@
     <t>69861-3	</t>
   </si>
   <si>
-    <t>c4497746-4c72-41c3-9d9d-60bdc468e3b0</t>
+    <t>944716ac-18cf-4083-97d5-bbd8db094942</t>
   </si>
   <si>
     <t>Value false in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -714,7 +714,7 @@
     <t>Use only allowed values 'TRUE','FALSE' in NEED_INDICATED</t>
   </si>
   <si>
-    <t>33ef191c-3f9d-4cae-8e16-1a912e7a0297</t>
+    <t>5f2b3556-861d-4e92-8104-6b4f0438f9ea</t>
   </si>
   <si>
     <t>Value true in NEED_INDICATED not in allowed list ('TRUE','FALSE')</t>
@@ -723,82 +723,82 @@
     <t>true</t>
   </si>
   <si>
-    <t>5b1f6de3-fbc1-4408-a5f4-956ebb2dbf0f</t>
-  </si>
-  <si>
-    <t>e8cd7114-9a4e-4d2e-a15e-28e4476b101f</t>
-  </si>
-  <si>
-    <t>0eb3110f-a449-4ff7-bcab-2ac7dedf3d89</t>
-  </si>
-  <si>
-    <t>efd68e98-0e9a-42fc-8f70-44b463f76909</t>
-  </si>
-  <si>
-    <t>5d19937a-8e9e-4458-82b2-4a5a8eba3875</t>
-  </si>
-  <si>
-    <t>a88aa407-e882-4de8-a77b-633d9be385a3</t>
-  </si>
-  <si>
-    <t>3b2e6e58-3bd9-4ef9-b5c6-0d230f3093a1</t>
-  </si>
-  <si>
-    <t>689254d0-8d54-4139-bbe5-2cce40402c95</t>
-  </si>
-  <si>
-    <t>4df92f6a-5c3d-48c1-8d61-d35f87590a9c</t>
-  </si>
-  <si>
-    <t>99a1d552-e1f0-49b8-9436-92312b83a702</t>
-  </si>
-  <si>
-    <t>c443fe65-5aea-4500-a478-7787e8fc75ca</t>
-  </si>
-  <si>
-    <t>208c46be-9921-414c-80fd-08479ada70c9</t>
-  </si>
-  <si>
-    <t>7ae50078-e75b-4959-9ce3-cca8b0a14220</t>
-  </si>
-  <si>
-    <t>a66c191c-f875-4cc2-961a-021bb0165004</t>
-  </si>
-  <si>
-    <t>5882c1a7-1b9f-42ec-90ee-d7ff735ae92f</t>
-  </si>
-  <si>
-    <t>29453799-f1dd-40da-a9cb-a8a2c5f09fde</t>
-  </si>
-  <si>
-    <t>5beca73d-4da4-41e2-8e27-561e143e2b24</t>
-  </si>
-  <si>
-    <t>7ad17783-7e6f-4e49-8ff9-12266ff26197</t>
-  </si>
-  <si>
-    <t>753d3576-0aeb-4abc-a439-b807ad817e79</t>
-  </si>
-  <si>
-    <t>c4bc2a82-3507-4c0d-92c4-9281d2f3ab84</t>
-  </si>
-  <si>
-    <t>d04472d0-fb57-4079-b2ea-0feb4eb08556</t>
-  </si>
-  <si>
-    <t>d752a0fe-4241-49a8-9c0e-73a0d1519ae2</t>
-  </si>
-  <si>
-    <t>836c5c42-7a57-4a84-85ce-a134073148b3</t>
-  </si>
-  <si>
-    <t>675b9c7d-b87c-4e05-ac38-a9c73b50ff3e</t>
-  </si>
-  <si>
-    <t>b5d078d2-0796-4228-8584-158eb75da5a3</t>
-  </si>
-  <si>
-    <t>15398f62-cf2c-4688-9a8f-ca5fbf1cd956</t>
+    <t>431477d3-46d1-4274-a925-65cce87c6460</t>
+  </si>
+  <si>
+    <t>d28357ec-dae3-4b2b-8b4a-d9217e4b2e5e</t>
+  </si>
+  <si>
+    <t>b92ccedd-84e0-42cf-9c74-a400f7c58fb0</t>
+  </si>
+  <si>
+    <t>56090832-a692-48af-8932-2b98f97b9972</t>
+  </si>
+  <si>
+    <t>4b859029-fc30-4a35-814d-2f71db0e5316</t>
+  </si>
+  <si>
+    <t>b8d1cb5c-212a-4ec0-9aee-22e1a1a33ec4</t>
+  </si>
+  <si>
+    <t>964f5199-246b-4fed-8348-d769e06c46e7</t>
+  </si>
+  <si>
+    <t>ba7d9348-8740-49f1-9cb5-9ddd8603d1c1</t>
+  </si>
+  <si>
+    <t>ebfc12df-90e2-4761-a58f-d64903cab4fc</t>
+  </si>
+  <si>
+    <t>a084baf0-7b79-4278-9342-9f50dbf29420</t>
+  </si>
+  <si>
+    <t>87b4ca91-9068-4406-89b3-295248206c32</t>
+  </si>
+  <si>
+    <t>8e33128c-32c6-45f1-9124-d125ce05b905</t>
+  </si>
+  <si>
+    <t>23166c2c-5202-44f8-8a10-981161d2802f</t>
+  </si>
+  <si>
+    <t>0558d3ca-4549-477b-91ce-0abc52bd4c06</t>
+  </si>
+  <si>
+    <t>45318512-91b9-435b-b250-8e91e666fb1a</t>
+  </si>
+  <si>
+    <t>0fc8046a-1290-4c02-8c83-d028df0fb871</t>
+  </si>
+  <si>
+    <t>345c53f8-9f9b-497f-8068-26e432869101</t>
+  </si>
+  <si>
+    <t>39fa9cd8-5a3c-4466-bd85-a96ccc00a448</t>
+  </si>
+  <si>
+    <t>2c64bafe-42f8-40ff-b585-421638a51295</t>
+  </si>
+  <si>
+    <t>6d3bb2b2-0840-4376-abc1-09eb1d54c505</t>
+  </si>
+  <si>
+    <t>653799b2-81f2-4787-95ca-eda695cec43f</t>
+  </si>
+  <si>
+    <t>aa44de87-e3f1-416f-8d45-7c0aaa2dc55d</t>
+  </si>
+  <si>
+    <t>a58a8251-1675-4388-8714-c27cd7093f55</t>
+  </si>
+  <si>
+    <t>9c9e4498-4bc7-473c-80f7-88076063c391</t>
+  </si>
+  <si>
+    <t>64c71703-ebdc-42f2-87ea-f5422de87c21</t>
+  </si>
+  <si>
+    <t>b862c4ca-2f02-49ee-be25-88c0dec798f6</t>
   </si>
   <si>
     <t>Value false in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -810,88 +810,88 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_PART_2_FLAG</t>
   </si>
   <si>
-    <t>d0ae63d4-3e0f-4689-b14c-95192c8c63eb</t>
-  </si>
-  <si>
-    <t>5b734123-2187-4e89-9000-6bb499729b26</t>
-  </si>
-  <si>
-    <t>a7c2720a-4676-437f-b71b-647ddcef3fed</t>
-  </si>
-  <si>
-    <t>e93a9f72-7950-43c7-b8a5-eddf589d5f69</t>
-  </si>
-  <si>
-    <t>84057b79-6f2a-4a01-a893-221f274310a4</t>
-  </si>
-  <si>
-    <t>1c599dcf-14c0-4615-8f2b-df97f3cc7b18</t>
-  </si>
-  <si>
-    <t>a457c865-81e1-40f9-aca0-4effdb5feace</t>
-  </si>
-  <si>
-    <t>911fed0e-aac1-4729-ab5f-3a1272c2feb8</t>
-  </si>
-  <si>
-    <t>46baddad-7fe4-4d43-b6e6-e32ab4dbb420</t>
-  </si>
-  <si>
-    <t>59f688fe-346c-4283-b596-b939621258c9</t>
-  </si>
-  <si>
-    <t>625546ec-3494-4304-b601-16374913ce24</t>
-  </si>
-  <si>
-    <t>5bb55b83-f88f-4e75-918f-2d24e49741f1</t>
-  </si>
-  <si>
-    <t>0997f571-5549-487f-8f9c-99e05acd1dce</t>
-  </si>
-  <si>
-    <t>adfc9ba1-2517-4658-ac38-2a468a0bfaa8</t>
-  </si>
-  <si>
-    <t>d0af56ea-93bb-4e01-a94c-007c71a5d973</t>
-  </si>
-  <si>
-    <t>7e4063a8-4f84-4cff-b152-c91800cfef40</t>
-  </si>
-  <si>
-    <t>3b2f4967-c6ca-40ce-921e-1dc981ad7849</t>
-  </si>
-  <si>
-    <t>345d502d-2ce9-4efa-8060-8c4a7621fddb</t>
+    <t>db6d0fe9-9c98-4a96-80f9-3b0023a02f58</t>
+  </si>
+  <si>
+    <t>6d550e73-68d2-4c12-8236-caa1faa9001e</t>
+  </si>
+  <si>
+    <t>68e73aea-5bd7-47df-9b98-37b28831f602</t>
+  </si>
+  <si>
+    <t>4e7f155e-fd35-48b4-9f90-2daf35c0fb99</t>
+  </si>
+  <si>
+    <t>30dd24ba-b35b-459a-9258-0a179d97005a</t>
+  </si>
+  <si>
+    <t>13578c07-ce5a-47bd-a5b0-094d4d7fd79b</t>
+  </si>
+  <si>
+    <t>0a7ddcf1-c49e-4822-b5bd-f4d2d90718ff</t>
+  </si>
+  <si>
+    <t>0a396f03-0aa9-4723-889b-edbf83daea15</t>
+  </si>
+  <si>
+    <t>e177ccb9-aec2-4839-80ac-2ccf20b2a941</t>
+  </si>
+  <si>
+    <t>d81f1c31-095c-416d-a06e-9bee88402d61</t>
+  </si>
+  <si>
+    <t>8ca922b5-ee08-4631-90c4-deed702432a6</t>
+  </si>
+  <si>
+    <t>93d78cbd-c0c6-490a-97ea-f37c2437d433</t>
+  </si>
+  <si>
+    <t>82b14e91-d4ae-4908-89db-8e5f4fe8b47e</t>
+  </si>
+  <si>
+    <t>3ba96f80-a7d5-4584-af64-d8ff03e23ef1</t>
+  </si>
+  <si>
+    <t>0d4d4ff2-7f18-4789-8f35-81cb1c50e6f8</t>
+  </si>
+  <si>
+    <t>5d051cae-f787-41aa-b95d-3478426bf582</t>
+  </si>
+  <si>
+    <t>037238dc-955b-4b37-b728-1fe8fd890273</t>
+  </si>
+  <si>
+    <t>c0ee53f8-64ef-4746-9f97-ee8f1d49f9e1</t>
   </si>
   <si>
     <t>Value true in VISIT_PART_2_FLAG not in allowed list ('TRUE','FALSE')</t>
   </si>
   <si>
-    <t>1312c867-b24c-4f5d-89a5-096a81753765</t>
-  </si>
-  <si>
-    <t>da715ba9-8f22-4b80-b9fa-1f4e64237210</t>
-  </si>
-  <si>
-    <t>459a1b7b-2468-44eb-a337-2ffcb43e29c3</t>
-  </si>
-  <si>
-    <t>2edcd505-7ffc-43f0-bf4c-9e8fa2fd07a7</t>
-  </si>
-  <si>
-    <t>9ed92dcf-5c39-4a1d-8e28-faa42c44c383</t>
-  </si>
-  <si>
-    <t>9b03eee0-24f8-41e9-8ad9-f8e57f07a9d3</t>
-  </si>
-  <si>
-    <t>3e1dcb58-6e66-4555-8c00-eaba3bcc6eff</t>
-  </si>
-  <si>
-    <t>9b891b6f-eb49-4114-a83d-c984f92dbe93</t>
-  </si>
-  <si>
-    <t>173dc2a1-8175-4cdb-8d3e-2d129215813c</t>
+    <t>2a09c25f-31e1-4059-9716-c7bd3f08c827</t>
+  </si>
+  <si>
+    <t>48a5b32d-babb-44c8-83a3-9bc217ba6004</t>
+  </si>
+  <si>
+    <t>68295c3c-e87c-45d0-bb83-7ed1e05534e1</t>
+  </si>
+  <si>
+    <t>30dd3efc-39db-4fa0-8fc4-d9f986ce9fba</t>
+  </si>
+  <si>
+    <t>5e653786-c039-4a54-b093-07b0cf519896</t>
+  </si>
+  <si>
+    <t>775129ef-7ed8-43e6-be63-a5f447ed0d50</t>
+  </si>
+  <si>
+    <t>5a147ae9-117e-4f8f-882a-5d143a03b4a1</t>
+  </si>
+  <si>
+    <t>a3e42822-2f44-4ecb-adc2-7a7f18b910d1</t>
+  </si>
+  <si>
+    <t>49b2745c-9808-4f43-88c5-4f795266769c</t>
   </si>
   <si>
     <t>Value false in VISIT_OMH_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -903,85 +903,85 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OMH_FLAG</t>
   </si>
   <si>
-    <t>f3e1bda2-63fe-49c7-9fd9-0a86b8ce3682</t>
-  </si>
-  <si>
-    <t>bada0d52-c0f9-4a56-8dff-29b9ce12be6c</t>
-  </si>
-  <si>
-    <t>03b4b01b-3e78-4518-a92b-7a669484a5f3</t>
-  </si>
-  <si>
-    <t>43d6e5f2-d832-4cae-ab87-65759218a9f8</t>
-  </si>
-  <si>
-    <t>4d230d85-c67e-4b26-9aca-23ab70aa44d7</t>
-  </si>
-  <si>
-    <t>6e6fbab4-9cf0-412c-8458-6812336e090a</t>
-  </si>
-  <si>
-    <t>c16a5219-c048-46b9-a8fa-0ee344e1b7f4</t>
-  </si>
-  <si>
-    <t>eb8299ca-1bec-4a8b-a69c-eb80b23a51ce</t>
-  </si>
-  <si>
-    <t>70d625d5-32d0-4bb3-bb2f-6aeb2b660755</t>
-  </si>
-  <si>
-    <t>68104db7-1081-4d59-8fee-827765fbd71c</t>
-  </si>
-  <si>
-    <t>8e7e334b-4c92-4b16-8ee4-7a71a61adcea</t>
-  </si>
-  <si>
-    <t>34ed810c-acd2-4e25-a89d-7e39bf3f23b2</t>
-  </si>
-  <si>
-    <t>f71bcad1-bca8-4901-9294-4cd7db7693f8</t>
-  </si>
-  <si>
-    <t>8d36586c-0b11-4c22-b249-b05f5da5a54d</t>
-  </si>
-  <si>
-    <t>fc24824f-404b-4945-a907-e4503e7475df</t>
-  </si>
-  <si>
-    <t>cedde292-b624-46ac-aa2f-0e0d1129d28f</t>
-  </si>
-  <si>
-    <t>6a1363e0-1b06-4b1e-896b-f05deab75041</t>
-  </si>
-  <si>
-    <t>a94fb550-9355-46de-803a-6803115d16da</t>
-  </si>
-  <si>
-    <t>0faa1afb-3322-4152-aab4-0167fd0b8ed9</t>
-  </si>
-  <si>
-    <t>b76adcae-95f5-4a8b-bb14-dc5e9a5d4b1e</t>
-  </si>
-  <si>
-    <t>770ed0e2-886d-4fae-b60c-ae4d563f2469</t>
-  </si>
-  <si>
-    <t>872b5d08-c726-4d1e-a207-2439c3029daa</t>
-  </si>
-  <si>
-    <t>2f5f8358-41ba-4cf3-a3eb-b626e99afe59</t>
-  </si>
-  <si>
-    <t>484fe084-e063-4aee-bb7b-b328917fdaeb</t>
-  </si>
-  <si>
-    <t>23339f9a-f7be-41c7-9604-accffe337b0a</t>
-  </si>
-  <si>
-    <t>80a87d81-e5f1-4fd6-84a8-491193a6cf0e</t>
-  </si>
-  <si>
-    <t>7b8c16f3-24de-4499-9cb7-9f53ddf359b9</t>
+    <t>f40efa01-fcf9-49ad-bf4f-76710e8ea3fb</t>
+  </si>
+  <si>
+    <t>b8dba63d-64dd-467a-95eb-12dee7767f8a</t>
+  </si>
+  <si>
+    <t>2f42d80d-b187-4447-913f-3cb7fb3f4dec</t>
+  </si>
+  <si>
+    <t>50133f7e-1838-4723-b3c0-ece159cc3ef9</t>
+  </si>
+  <si>
+    <t>0634126e-1f22-46af-bb41-e56fc8dd7f94</t>
+  </si>
+  <si>
+    <t>823c104a-b1e5-4eda-b3ba-fc3bfb0c645b</t>
+  </si>
+  <si>
+    <t>92e764f9-38b5-4cfb-aecf-ceddf3f15b41</t>
+  </si>
+  <si>
+    <t>e805ec8e-586b-463b-8e44-6e70cbdda858</t>
+  </si>
+  <si>
+    <t>38438400-b781-4977-9036-ca921d3e3be4</t>
+  </si>
+  <si>
+    <t>401d3934-b3b1-49ad-b94c-9436ac1ab9c4</t>
+  </si>
+  <si>
+    <t>7f132f2a-b41f-41f8-bbfa-1b976d0e3824</t>
+  </si>
+  <si>
+    <t>ad4b79b6-27f4-42f6-9b24-7c0d97bbbfe2</t>
+  </si>
+  <si>
+    <t>8c3afdc2-36f5-4c40-b9b1-fa979d2f5d14</t>
+  </si>
+  <si>
+    <t>3e4dab5a-c1c7-43d9-a30d-4e2b1b1e935b</t>
+  </si>
+  <si>
+    <t>f13cd8c5-0d42-46d2-88cb-0951900284a7</t>
+  </si>
+  <si>
+    <t>66a86182-c4f1-495d-bb51-da4fc23394ae</t>
+  </si>
+  <si>
+    <t>fbd861c8-ee2d-42df-bca2-91eb19088fc1</t>
+  </si>
+  <si>
+    <t>6d500bf7-18d4-4e35-8d6f-0f87946cffa1</t>
+  </si>
+  <si>
+    <t>9dd28fed-9e61-4a25-90a5-f159ec4ce5a0</t>
+  </si>
+  <si>
+    <t>245df81e-ef4a-4a61-a66a-36b95fb8b83a</t>
+  </si>
+  <si>
+    <t>43b02858-7bb4-4790-8c7c-ebf97ddf67bc</t>
+  </si>
+  <si>
+    <t>8ad937cb-f6bb-4329-b3ec-90fb28475aa9</t>
+  </si>
+  <si>
+    <t>55184d24-ab4f-4b14-abc5-8a5fa2c5826c</t>
+  </si>
+  <si>
+    <t>79ecbb21-9380-487c-b8c6-4a279d4f416a</t>
+  </si>
+  <si>
+    <t>773f6128-e1a2-4d72-bc3f-97b8f5f6ea37</t>
+  </si>
+  <si>
+    <t>5d69ad98-39ee-4513-a723-27f12e9d7311</t>
+  </si>
+  <si>
+    <t>0d0a2286-5f68-44ff-b110-aee2b8a34ed7</t>
   </si>
   <si>
     <t>Value false in VISIT_OPWDD_FLAG not in allowed list ('TRUE','FALSE')</t>
@@ -993,94 +993,94 @@
     <t>Use only allowed values 'TRUE','FALSE' in VISIT_OPWDD_FLAG</t>
   </si>
   <si>
-    <t>58b3495d-925f-4c35-8d73-5a1be9a95c4f</t>
-  </si>
-  <si>
-    <t>34c5b6b8-a92a-438b-b425-3953556876af</t>
-  </si>
-  <si>
-    <t>395d497a-0e8e-4dc4-b5c4-91060afd969c</t>
-  </si>
-  <si>
-    <t>556e09fb-719b-4350-92ea-7e66d70e8994</t>
-  </si>
-  <si>
-    <t>09393601-1eff-48b3-b81c-0c500fa42136</t>
-  </si>
-  <si>
-    <t>72a1e7bc-b366-4d60-9dd6-84c350ff35b3</t>
-  </si>
-  <si>
-    <t>9f77d07a-9b43-4564-a83b-13aac3313c73</t>
-  </si>
-  <si>
-    <t>6740d6f9-06db-447c-a593-77f9ded0c5e2</t>
-  </si>
-  <si>
-    <t>a49b2702-7f52-4e73-a15b-4fe6a9a10499</t>
-  </si>
-  <si>
-    <t>b075a877-3a40-4235-8cc0-ce666cd6d168</t>
-  </si>
-  <si>
-    <t>689c9134-f5bb-47a6-82f9-9a6b715d6d8e</t>
-  </si>
-  <si>
-    <t>d2492bea-bda9-4dec-a44a-045296d9623a</t>
-  </si>
-  <si>
-    <t>966190b7-11de-4e08-ae12-84c4e181ebef</t>
-  </si>
-  <si>
-    <t>b7d07a9b-4472-4566-8340-cad030b50cf8</t>
-  </si>
-  <si>
-    <t>4edc647b-d63b-473d-8355-18df8ff504d0</t>
-  </si>
-  <si>
-    <t>9178c936-e288-4784-9b06-7f3144fc544e</t>
-  </si>
-  <si>
-    <t>0e2320ee-261f-49a9-bd5c-d9225b01a937</t>
-  </si>
-  <si>
-    <t>1ef4ed47-63fe-45ec-9382-1d4eb3a04a5e</t>
-  </si>
-  <si>
-    <t>4154334a-0d73-4501-861f-8461b7d8e03d</t>
-  </si>
-  <si>
-    <t>751239b2-b6a4-48a7-80c2-af9f55bbed7e</t>
-  </si>
-  <si>
-    <t>a1e3a8ae-6883-4cfa-a266-f11d79c55c19</t>
-  </si>
-  <si>
-    <t>5dacbd20-4279-4b36-8b4d-b9443981863b</t>
-  </si>
-  <si>
-    <t>b55ab072-2992-4bc5-ab48-bf7ee069876c</t>
-  </si>
-  <si>
-    <t>df86d8dd-c1d2-449a-aedf-eba74c3c9c1c</t>
-  </si>
-  <si>
-    <t>054bafaa-e4f0-461f-8a82-88e0c25dd03e</t>
-  </si>
-  <si>
-    <t>667647ed-6e03-4a01-a02b-051b17b9e85e</t>
+    <t>1f37c31a-172f-4c45-8bf1-e7439093a612</t>
+  </si>
+  <si>
+    <t>9161c72d-909b-470b-81c2-4a48616bcec8</t>
+  </si>
+  <si>
+    <t>b6128705-93d7-4abf-ab17-5466b3899630</t>
+  </si>
+  <si>
+    <t>7bb9ca8e-7bf1-4a8c-8296-d87978a7e2a7</t>
+  </si>
+  <si>
+    <t>6a8d998b-efc5-42e3-a2f0-752d596bdcd4</t>
+  </si>
+  <si>
+    <t>28d3bf5e-d84d-433c-8f0a-a0b51a8ef07e</t>
+  </si>
+  <si>
+    <t>c696a8a7-f7a9-47d8-994b-0d9a1c4621c5</t>
+  </si>
+  <si>
+    <t>14ffa4ea-5b83-4400-bb8f-48b79adcfe09</t>
+  </si>
+  <si>
+    <t>89638681-1790-48ae-a688-3cc79efb8aef</t>
+  </si>
+  <si>
+    <t>325cbafd-076e-4216-924e-0241c4443487</t>
+  </si>
+  <si>
+    <t>1a74f5cf-18dd-4075-ae1a-dcc231f25f36</t>
+  </si>
+  <si>
+    <t>21126f73-ebac-424e-82d1-f0a3cb7003f1</t>
+  </si>
+  <si>
+    <t>f943957e-b616-412f-b5fd-029e38e24b70</t>
+  </si>
+  <si>
+    <t>e780cb51-5833-4f39-9d73-2d6e52d52378</t>
+  </si>
+  <si>
+    <t>6b9528e9-512f-4a77-ba48-a8b3fdf68523</t>
+  </si>
+  <si>
+    <t>84df4029-9c7d-4999-b927-700051e565e4</t>
+  </si>
+  <si>
+    <t>c611836c-f6a3-4136-9a5f-0fab7b91a135</t>
+  </si>
+  <si>
+    <t>26530df2-d505-49b6-8874-5eaaf938aec4</t>
+  </si>
+  <si>
+    <t>899f2c82-9d9f-4f07-acec-ce5ca68b02ea</t>
+  </si>
+  <si>
+    <t>a6e6aef8-d36b-4567-8768-8aed6a98091c</t>
+  </si>
+  <si>
+    <t>f28d0b04-fd71-4a0b-b52b-7b45777d3235</t>
+  </si>
+  <si>
+    <t>8f9db998-9649-4bba-99b1-25be8ff35d55</t>
+  </si>
+  <si>
+    <t>23787d48-6afa-4905-a8d8-bc802eb8a969</t>
+  </si>
+  <si>
+    <t>e9d96d3b-c5e5-4d26-9a85-01727b0e1d72</t>
+  </si>
+  <si>
+    <t>6112342f-4740-4497-994b-b249371adc12</t>
+  </si>
+  <si>
+    <t>ec9df83d-c8b6-4b53-a4f7-51d81b46023d</t>
   </si>
   <si>
     <t>2afb3098-bcfd-5a54-8ebb-4d65d399c55e</t>
   </si>
   <si>
-    <t>/home/snshah/workspaces/github.com/qe-collaborative-services/1115-hub/support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2024-01-25-valid.xlsx</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/ahc-hrsn-2024-01-25-valid.xlsx</t>
   </si>
   <si>
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>73405275-9054-4dba-8c76-4a3f7e97bc92</t>
+    <t>eddd3845-7b27-408b-8ab6-f35e78a7a68f</t>
   </si>
   <si>
     <t>Value 	20430005 in SEXUAL_ORIENTATION_CODE not in allowed list ('42035005','20430005','38628009','OTH','UNK')</t>
@@ -1101,7 +1101,7 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>91722004-9020-4eb6-bab5-909de59b04eb</t>
+    <t>de72bb8f-3cae-4756-8b31-719f2c2014af</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -1116,16 +1116,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>f7e9a73c-e8c6-482c-9cd1-d35a7050be00</t>
-  </si>
-  <si>
-    <t>6763e66d-e77a-4b16-a2ef-efeb757ceee4</t>
-  </si>
-  <si>
-    <t>63ca0389-77d9-412d-8330-80e7d5a8b59f</t>
-  </si>
-  <si>
-    <t>64f7eaaa-a5e0-43a8-938c-e00faf146855</t>
+    <t>182ba2b6-b6ac-440c-a8fa-596c311910fc</t>
+  </si>
+  <si>
+    <t>1bee9ba4-381e-4d32-8c77-db534d5b62c9</t>
+  </si>
+  <si>
+    <t>7f5b51f6-d230-424d-8b31-98e6f65e0851</t>
+  </si>
+  <si>
+    <t>14c77d8e-c715-4f67-9c9f-283a11f3b6ff</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -1137,16 +1137,16 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>0326f614-ad3e-43b9-bf5b-e7c59a1b0411</t>
-  </si>
-  <si>
-    <t>129949c0-37d0-4611-a97b-e6095f882d9c</t>
-  </si>
-  <si>
-    <t>cb970457-300d-4a00-9415-702035eeca0d</t>
-  </si>
-  <si>
-    <t>f0871593-a570-4b87-b125-27708eaf198b</t>
+    <t>0ef14305-a472-4e81-945b-b720e8d5e2ab</t>
+  </si>
+  <si>
+    <t>dbb86d90-4d2e-434b-a8ac-5ddb73c9aa31</t>
+  </si>
+  <si>
+    <t>4e6dcd5d-6e1d-458c-ad0b-fc5df4a1222e</t>
+  </si>
+  <si>
+    <t>81f5bc07-3b5f-4ee5-8f6a-d1261e5a54a0</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -1155,16 +1155,16 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>03a0d417-0724-4a66-9b54-803473080d0b</t>
-  </si>
-  <si>
-    <t>72e9c77e-c78e-4792-a707-cb284b158e6a</t>
-  </si>
-  <si>
-    <t>11602052-a7ea-4e2b-9367-d1b907d117fa</t>
-  </si>
-  <si>
-    <t>9cebe92d-c5ab-4efe-9c93-f0b87dd354e9</t>
+    <t>32475d64-1cc2-4208-827f-c142721b3de8</t>
+  </si>
+  <si>
+    <t>5794c0e7-7f06-46f7-9574-de9d844d7573</t>
+  </si>
+  <si>
+    <t>3da3798d-6512-459a-8e3a-ca656f1a7ec8</t>
+  </si>
+  <si>
+    <t>23953516-979a-4422-95f7-b4639cab53ed</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -1176,16 +1176,16 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>d8ed4451-eaad-48c2-bc14-79951d522edc</t>
-  </si>
-  <si>
-    <t>367208b3-ae91-4873-a297-d5d4a36bea26</t>
-  </si>
-  <si>
-    <t>07959b46-d913-4753-bf5d-696af801237e</t>
-  </si>
-  <si>
-    <t>ec7d9603-a7ef-4112-be67-e598e0b67da0</t>
+    <t>dd9845a9-3f49-4e05-8ea2-bf334699c5ed</t>
+  </si>
+  <si>
+    <t>f5f671fd-f9e5-40e4-8bed-11c016c33430</t>
+  </si>
+  <si>
+    <t>2f5120bb-4917-4730-b1bd-f0f80e6f84c5</t>
+  </si>
+  <si>
+    <t>0c01dddd-1f4d-4a1f-8e4c-bdf191227197</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE is empty</t>
@@ -1197,22 +1197,22 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>2f946053-6387-4466-b9c7-44f11e985f4a</t>
-  </si>
-  <si>
-    <t>037bbebc-9b6a-43a9-9744-d9e183dd0f3b</t>
-  </si>
-  <si>
-    <t>e84e31e9-911e-44cf-96f8-3473ac2d881d</t>
-  </si>
-  <si>
-    <t>68db9b57-561d-4549-ba4b-122753659610</t>
-  </si>
-  <si>
-    <t>ef806370-d294-4900-af73-668d4e6c549a</t>
-  </si>
-  <si>
-    <t>aa7e72f2-80d9-4163-aaca-ecb0d8e37220</t>
+    <t>db6f820d-1125-4b36-a95b-e713fa8b560b</t>
+  </si>
+  <si>
+    <t>785102dc-1994-4895-8b9d-36a7e9186cac</t>
+  </si>
+  <si>
+    <t>21903c48-e896-42b8-bd2c-bdb5e81a2c77</t>
+  </si>
+  <si>
+    <t>899289fe-bc27-407f-9e11-4e3a67f4463e</t>
+  </si>
+  <si>
+    <t>01379e06-d895-4f8e-85e6-3c4ddd10e561</t>
+  </si>
+  <si>
+    <t>24832ebf-2914-4c25-8272-f7d010ff0841</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -1224,19 +1224,19 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>07bc494d-508b-4682-9819-393969403c63</t>
-  </si>
-  <si>
-    <t>46b25d0d-4385-43b7-b0d4-1278541c47cb</t>
-  </si>
-  <si>
-    <t>ca04bbf9-610b-4131-be63-31333a04d75a</t>
-  </si>
-  <si>
-    <t>06d1a211-bb43-4ceb-93b2-3815c3af1478</t>
-  </si>
-  <si>
-    <t>99a5a44c-57c2-4eb1-ba92-78b7e0e86d22</t>
+    <t>f19e1dfe-ee96-41c5-9873-dd6a1cdf2f87</t>
+  </si>
+  <si>
+    <t>18c63dcb-2228-4ac4-87f1-2002acf92a79</t>
+  </si>
+  <si>
+    <t>239901e6-5b5a-4177-a75b-11c45485efc0</t>
+  </si>
+  <si>
+    <t>24ee30d6-2be7-4dd7-a662-76ff65948e77</t>
+  </si>
+  <si>
+    <t>c83cf69c-5488-4f2c-9084-58f5f0441d07</t>
   </si>
   <si>
     <t>86ff3ab6-900d-5474-b63c-cbcac3c66f1a</t>

</xml_diff>

<commit_message>
feat: refactor reference data ingestion
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -282,7 +282,7 @@
     <t>screening_2_01hpkty3hctk826tvx5tasga55</t>
   </si>
   <si>
-    <t>b1e8f805-1372-46b6-b46b-b56f9c52de30</t>
+    <t>c7c69ba0-f858-4e90-aa64-a6dcd57a8fcb</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -297,16 +297,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>3b274bc0-391c-4340-8265-0f4e5cfe69f9</t>
-  </si>
-  <si>
-    <t>82bbb7fe-c6e8-4bc9-81f6-696fcf344b2b</t>
-  </si>
-  <si>
-    <t>62836633-ea1b-42f0-9ee2-4e09018d68f1</t>
-  </si>
-  <si>
-    <t>fe098e07-a22b-4f8b-bca9-a522a5830680</t>
+    <t>0e352222-93c8-4557-a641-9158c83c6477</t>
+  </si>
+  <si>
+    <t>202d2b17-8cf8-4215-a471-c9c07fe2f42e</t>
+  </si>
+  <si>
+    <t>a606f389-719e-43ff-9785-e23ebb0511a1</t>
+  </si>
+  <si>
+    <t>22714e1c-6534-4305-bb9f-1d27e47b7e42</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -318,16 +318,16 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>49c5d95c-6a07-4635-ba60-2e3491a7094d</t>
-  </si>
-  <si>
-    <t>a241a926-62c8-4e62-8003-2ccae04890f0</t>
-  </si>
-  <si>
-    <t>a44dc398-be46-465d-8f4d-9291d5e2f5e7</t>
-  </si>
-  <si>
-    <t>483b6b10-2508-4f50-bbc5-ea8a45f8eb88</t>
+    <t>51b35066-9c15-4914-bc9c-514d19b09dd5</t>
+  </si>
+  <si>
+    <t>a896ecfc-80df-41e8-acd5-bc2653941ff5</t>
+  </si>
+  <si>
+    <t>3b6941b2-e0be-4591-9231-c35bd19e2c92</t>
+  </si>
+  <si>
+    <t>466b36f1-86ad-4d4c-b856-a1689bd39f77</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -345,94 +345,94 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>7ef5f20f-61d5-4d2d-9385-b690ede3dd1d</t>
-  </si>
-  <si>
-    <t>bb1e2dc6-55b7-4cae-b82d-adb3650939b0</t>
-  </si>
-  <si>
-    <t>285250e3-5233-48de-8152-28714b29b36a</t>
-  </si>
-  <si>
-    <t>e3944935-3da3-4c18-b6bc-0c79083e2eec</t>
-  </si>
-  <si>
-    <t>f59cb819-0af8-41d9-aae3-cbf40acd2173</t>
-  </si>
-  <si>
-    <t>9d8f6c62-9bcc-4a5f-a666-3064a27c61e4</t>
-  </si>
-  <si>
-    <t>7a723d0e-9b8f-43df-af54-a2cd1d570427</t>
-  </si>
-  <si>
-    <t>62af1a07-d420-46d0-8404-49b9acdef74a</t>
-  </si>
-  <si>
-    <t>6ed211be-25a2-4af0-a780-70b26405827c</t>
-  </si>
-  <si>
-    <t>efa0dcfc-2823-4379-bbec-a2ddcac188a5</t>
-  </si>
-  <si>
-    <t>baba8d89-c410-4b9f-872b-70950756c455</t>
-  </si>
-  <si>
-    <t>79e2efca-a593-4aae-983f-29dafe147401</t>
-  </si>
-  <si>
-    <t>ce309d50-5cc2-45cb-9304-f0713fe724fc</t>
-  </si>
-  <si>
-    <t>b49f1fee-0677-47fd-9ce4-c73ad90ee569</t>
-  </si>
-  <si>
-    <t>e8654306-bbb4-40fd-a55d-39628a7452a9</t>
-  </si>
-  <si>
-    <t>735be803-1681-4c9f-8fcf-cf413a4a6479</t>
-  </si>
-  <si>
-    <t>428d4c44-a549-4daa-b844-a23ca982911d</t>
-  </si>
-  <si>
-    <t>0749feed-4224-470c-8145-9eda5202b718</t>
-  </si>
-  <si>
-    <t>2e6cb585-8402-4a47-b507-e87ed182cabc</t>
-  </si>
-  <si>
-    <t>f6634aeb-8334-4b56-832d-ee67732ce2c8</t>
-  </si>
-  <si>
-    <t>be2ffc50-8da1-4d66-9194-9a619d319486</t>
-  </si>
-  <si>
-    <t>5b793654-719c-444f-8934-400d01483e2d</t>
-  </si>
-  <si>
-    <t>4ee59a66-a8b6-480a-959e-ff0497cd1f67</t>
-  </si>
-  <si>
-    <t>1fa04d8f-56c6-4284-8a4b-62d7cfe90441</t>
-  </si>
-  <si>
-    <t>6f68e286-69d6-42f4-aa39-35fae5b202ba</t>
-  </si>
-  <si>
-    <t>0ba2fd47-eae0-4250-99dc-63232a41037c</t>
-  </si>
-  <si>
-    <t>8adb112c-3377-4151-91d8-440b68788d72</t>
-  </si>
-  <si>
-    <t>558c9340-3846-415c-b4e2-b019e85f33f0</t>
-  </si>
-  <si>
-    <t>97f67b38-32b3-4655-9fc5-ce0c25a64d6a</t>
-  </si>
-  <si>
-    <t>6eaba49b-800d-43b1-9245-43ef52c00249</t>
+    <t>6e0e1568-9aac-444b-8814-b460028af9e8</t>
+  </si>
+  <si>
+    <t>6268d063-41cd-4f4e-93eb-7f8680b0a253</t>
+  </si>
+  <si>
+    <t>9cb81b78-f5cf-4d73-80d3-a09470b3e4c1</t>
+  </si>
+  <si>
+    <t>bcb64404-e307-41c2-b7ea-a45beb781eb5</t>
+  </si>
+  <si>
+    <t>97c1251c-860b-42a0-befc-d73e32fb9784</t>
+  </si>
+  <si>
+    <t>67632208-780a-469c-94e5-00005c442d32</t>
+  </si>
+  <si>
+    <t>488407d6-5457-4863-a8de-3610e941c486</t>
+  </si>
+  <si>
+    <t>f8975d05-dcf2-47fc-b4ba-edc92ffe9f09</t>
+  </si>
+  <si>
+    <t>ab39d8fb-27e8-4d34-866b-d0bfed43c99c</t>
+  </si>
+  <si>
+    <t>56bdf120-34a3-4546-93ad-53f00a5ea289</t>
+  </si>
+  <si>
+    <t>0dbe55c0-164d-4bd1-b150-9d7ad8f95666</t>
+  </si>
+  <si>
+    <t>6005387c-55d9-426d-944e-db531a3e5e2b</t>
+  </si>
+  <si>
+    <t>954981de-5187-4c3f-8e39-77d9af36d9c8</t>
+  </si>
+  <si>
+    <t>1adad4cb-b05c-4692-b1ee-4ff26c8ba110</t>
+  </si>
+  <si>
+    <t>41070fbc-c819-4bd2-b840-f9d5a8cebbd8</t>
+  </si>
+  <si>
+    <t>98062f52-6acf-4df6-bbb3-4e6bcc9673d8</t>
+  </si>
+  <si>
+    <t>32fd55b4-3397-438d-a9e8-d8df046e4b9b</t>
+  </si>
+  <si>
+    <t>b68a60b4-6656-45a5-bc5d-ecf7ac3c9d4e</t>
+  </si>
+  <si>
+    <t>7b5b33f6-b5a1-40c3-afeb-d56a34c7822f</t>
+  </si>
+  <si>
+    <t>781c1c32-229e-46f1-a11f-bb8086fe4d62</t>
+  </si>
+  <si>
+    <t>68da8bd6-6a43-446e-9668-07d4e6fed358</t>
+  </si>
+  <si>
+    <t>dfe986ef-f14b-4521-abcc-9744e57f97b8</t>
+  </si>
+  <si>
+    <t>2bbe56cc-d76d-4f6a-8e1f-6564c7e74099</t>
+  </si>
+  <si>
+    <t>630d39ae-d04b-48e4-a540-489be79757a9</t>
+  </si>
+  <si>
+    <t>f341e321-a51f-4bb4-80d5-b7e15ad06c0d</t>
+  </si>
+  <si>
+    <t>1e80f7a7-a503-4d0c-9452-789b2378c40b</t>
+  </si>
+  <si>
+    <t>aa3ecc24-9883-413e-920b-c57a6712f2f9</t>
+  </si>
+  <si>
+    <t>0203acab-2899-46dc-b7d7-2464587fa1fc</t>
+  </si>
+  <si>
+    <t>f21f6279-fec9-496c-be0a-2084ab209892</t>
+  </si>
+  <si>
+    <t>6b71b40a-baca-46c4-ae49-2017d69fe829</t>
   </si>
   <si>
     <t>Invalid timestamp "2023152  2:38:06 PM" found in RECORDED_TIME</t>
@@ -441,94 +441,94 @@
     <t>2023152  2:38:06 PM</t>
   </si>
   <si>
-    <t>e562126e-2f50-4d64-b175-f4dc837de4a2</t>
-  </si>
-  <si>
-    <t>bc1e059c-4233-412e-b7e6-a894dcd7571e</t>
-  </si>
-  <si>
-    <t>ad769353-6a3b-4976-8cfe-c9e72560a238</t>
-  </si>
-  <si>
-    <t>a8bda894-631a-439a-98fd-7ef9b4f547c5</t>
-  </si>
-  <si>
-    <t>c9e2c6f3-ab68-4e78-87cd-1ef4258b2c1e</t>
-  </si>
-  <si>
-    <t>76400075-78cb-4d81-a476-9aae2ebbb66b</t>
-  </si>
-  <si>
-    <t>b8831a2f-64a9-4840-8d52-ba53a2f34c02</t>
-  </si>
-  <si>
-    <t>8dce82f7-e472-4644-98b3-60804e0805a0</t>
-  </si>
-  <si>
-    <t>e03ae580-eb2e-48e4-bf72-2b937c1b70c0</t>
-  </si>
-  <si>
-    <t>e0d96555-ed44-4b55-a107-01b2f6db7bae</t>
-  </si>
-  <si>
-    <t>282db258-490a-4c63-bf2e-4bd639101c41</t>
-  </si>
-  <si>
-    <t>a6e8eaf6-f3b8-4be1-8ad2-e0924b2be23a</t>
-  </si>
-  <si>
-    <t>b923267f-23f0-40e4-853f-2de072b6101e</t>
-  </si>
-  <si>
-    <t>82c8abb4-0179-434c-bb3a-046abd4333d7</t>
-  </si>
-  <si>
-    <t>35328533-8527-4aa7-af43-664e033c14cd</t>
-  </si>
-  <si>
-    <t>45a70b1f-7bcc-40cd-af52-db4ec50f64e4</t>
-  </si>
-  <si>
-    <t>76abf82f-3753-4883-994d-c76e235d0892</t>
-  </si>
-  <si>
-    <t>99e48503-6146-4915-b00b-ecee87fa167b</t>
-  </si>
-  <si>
-    <t>19bc3e30-db6b-4c40-993a-d51a35d817c1</t>
-  </si>
-  <si>
-    <t>fcee4836-ed0e-441e-9a8e-5bafb25d2a07</t>
-  </si>
-  <si>
-    <t>1ca990f8-8c15-4d1a-88ca-39435d9c44aa</t>
-  </si>
-  <si>
-    <t>946e38f4-37b2-467d-8d07-10f7d99d7db9</t>
-  </si>
-  <si>
-    <t>8d48ce82-ce89-41c6-8592-7733b1f48ae4</t>
-  </si>
-  <si>
-    <t>6336a989-a4d7-467b-85b8-0023861347c9</t>
-  </si>
-  <si>
-    <t>0fa877ed-b611-4fce-a04a-d1cb66493e9b</t>
-  </si>
-  <si>
-    <t>3658da22-6c42-4e78-9ff8-4ea20551bda8</t>
-  </si>
-  <si>
-    <t>cfd24335-2229-43f5-be88-991c4805cf5a</t>
-  </si>
-  <si>
-    <t>8d7e638d-3821-4181-9102-6c7fd4696c2c</t>
-  </si>
-  <si>
-    <t>a85ea834-7fe9-491f-a306-63462e15d63f</t>
-  </si>
-  <si>
-    <t>040020fc-ede5-4670-8075-e6fd0f918e1e</t>
+    <t>34767309-75b8-4710-8d4e-8bc4d2e6b45c</t>
+  </si>
+  <si>
+    <t>027ddff8-b1b6-47a2-8c51-c897c9089ce3</t>
+  </si>
+  <si>
+    <t>68697c64-13db-4735-b1ce-3bbea7c08739</t>
+  </si>
+  <si>
+    <t>dae0cd7d-6942-474b-995d-0dd20acacdc9</t>
+  </si>
+  <si>
+    <t>720ae89c-daf0-44c4-8745-ab7bf875ac10</t>
+  </si>
+  <si>
+    <t>b40c8afc-cc1b-4be8-ad63-59321edecf31</t>
+  </si>
+  <si>
+    <t>31815b6f-c96e-43c9-8fb6-7fcbaaa63f14</t>
+  </si>
+  <si>
+    <t>e2d46a1a-4e7a-4e8f-8957-2408eb3a60e0</t>
+  </si>
+  <si>
+    <t>a3fb126f-285d-46f0-89c1-bafe1df05623</t>
+  </si>
+  <si>
+    <t>97435109-e58d-4e5e-b476-4a2848ff8a7b</t>
+  </si>
+  <si>
+    <t>2a9773a4-c60d-4dc3-a4f5-cffdaceb6f83</t>
+  </si>
+  <si>
+    <t>840f4e8a-148c-424a-9ccd-251896ca737d</t>
+  </si>
+  <si>
+    <t>9eb8c6eb-14bd-48a4-a8df-b84d3a8562fe</t>
+  </si>
+  <si>
+    <t>ea561f9b-7b77-416a-b970-2882e408a0c5</t>
+  </si>
+  <si>
+    <t>452efb45-239a-4c2e-84b2-6a733c59183d</t>
+  </si>
+  <si>
+    <t>6f5aedb4-f2db-4134-8ed9-e85d8d63a002</t>
+  </si>
+  <si>
+    <t>38dd49b7-a478-47fb-8aae-f7e38b3adc67</t>
+  </si>
+  <si>
+    <t>d1794036-118e-4e4b-938c-aebdce18dbd3</t>
+  </si>
+  <si>
+    <t>5cd83bdd-91f1-4c8e-bd85-c78357d0c588</t>
+  </si>
+  <si>
+    <t>a45db671-f0ab-43dd-9f0d-0f3521dc6335</t>
+  </si>
+  <si>
+    <t>87e6e272-b9bc-48f5-a758-e3c1808e9aef</t>
+  </si>
+  <si>
+    <t>ae3b9b1b-4ca5-472b-a8bc-4e6024d12740</t>
+  </si>
+  <si>
+    <t>9e8819cb-9d7b-4eb4-835d-04248f9502ef</t>
+  </si>
+  <si>
+    <t>907bcec3-c618-40e0-9494-cf805e290ee8</t>
+  </si>
+  <si>
+    <t>7fad2beb-db26-4441-9d2d-c5b1cab67ac7</t>
+  </si>
+  <si>
+    <t>41e23d15-c190-410f-85f6-9e4c62d4f8aa</t>
+  </si>
+  <si>
+    <t>c31921e3-fdc8-4dd2-8b2e-d421f580c183</t>
+  </si>
+  <si>
+    <t>e32650be-23c7-4380-befb-8716e8d23196</t>
+  </si>
+  <si>
+    <t>61b0dbb4-7332-4162-b830-4ff3b696a8f0</t>
+  </si>
+  <si>
+    <t>8a05fa10-8a9c-4064-9868-52e526fb1e4a</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -540,16 +540,16 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>ee661250-14da-4004-8ff0-11d39d22b07b</t>
-  </si>
-  <si>
-    <t>87cd65a5-48d8-4b5d-9434-6f99ae6fbe8b</t>
-  </si>
-  <si>
-    <t>4db46032-79ee-4c0b-b1fd-dd4f6df0efa2</t>
-  </si>
-  <si>
-    <t>0c3c5015-3279-4a38-bd46-324690828096</t>
+    <t>20deaa51-651b-4923-9fba-392e6cb41bc8</t>
+  </si>
+  <si>
+    <t>d469a47a-5f43-4816-94e4-319c8e9241ea</t>
+  </si>
+  <si>
+    <t>6cc8d07a-9051-4615-8b46-8f354fd6d186</t>
+  </si>
+  <si>
+    <t>8e82ef9d-8778-4a87-9565-312af629bee5</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -561,16 +561,16 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>5a119ded-ad20-4261-b152-c5ad9587d9b0</t>
-  </si>
-  <si>
-    <t>54499a0b-9ff5-4c42-a670-b18999998369</t>
-  </si>
-  <si>
-    <t>d1a80c25-ea8d-456b-b204-d4b63dd208fd</t>
-  </si>
-  <si>
-    <t>3b17c0f3-485d-4845-aa32-adaaefa02367</t>
+    <t>19a0239a-aefe-4e3b-a3ee-ce54461b124c</t>
+  </si>
+  <si>
+    <t>83f16d06-c095-4392-b5fb-d0455f800897</t>
+  </si>
+  <si>
+    <t>b91b9c08-954b-4498-b2a3-4c56fd09fce8</t>
+  </si>
+  <si>
+    <t>89eadf09-6d6d-403d-9667-084794ec1103</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE is empty</t>
@@ -582,22 +582,22 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>bfcb83f5-c2eb-49fc-a40c-a7adaeae7933</t>
-  </si>
-  <si>
-    <t>c4807a1c-ef41-4dfb-a9b9-2d82df47e8bf</t>
-  </si>
-  <si>
-    <t>6e97f819-5ae9-475a-94d3-536f5123d9d3</t>
-  </si>
-  <si>
-    <t>2b427257-d432-402c-ad18-4a1b5b98eb43</t>
-  </si>
-  <si>
-    <t>795670ea-c579-47ba-9428-3b64fa58bb73</t>
-  </si>
-  <si>
-    <t>721d067c-ebda-441a-9cea-a7aa243ea481</t>
+    <t>3c433083-e284-4cec-bdbd-5095b4ae66ac</t>
+  </si>
+  <si>
+    <t>02bbfea6-1016-466a-b3df-ef24c42f1d7f</t>
+  </si>
+  <si>
+    <t>c7b08b01-dacd-424e-8711-7779f02486c0</t>
+  </si>
+  <si>
+    <t>b3abbd32-b6ee-48a4-baf5-c56e6eaa093f</t>
+  </si>
+  <si>
+    <t>55d7c9cb-f6ea-40d3-b3f1-3e452ec0217c</t>
+  </si>
+  <si>
+    <t>55324869-d02e-4a88-b841-b7ad372ee148</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -609,19 +609,19 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>716c09e4-63f3-463b-beab-ce1117fbcb3b</t>
-  </si>
-  <si>
-    <t>dae87729-0843-4475-bfc5-1d05fb16627d</t>
-  </si>
-  <si>
-    <t>394a44f4-2ea9-4b29-bd73-70f725d212f5</t>
-  </si>
-  <si>
-    <t>90198ae3-1104-42b3-b63d-9f746e96f7ad</t>
-  </si>
-  <si>
-    <t>dcf4a540-55ad-4378-bf12-eaba6ed4ca8a</t>
+    <t>418f562d-fe9b-44aa-9b00-636f9da04aa8</t>
+  </si>
+  <si>
+    <t>8e02ad38-bb3e-403c-baf0-a3c476cdfb3d</t>
+  </si>
+  <si>
+    <t>1bb7ca21-9b29-4af2-ad84-4a42756e061c</t>
+  </si>
+  <si>
+    <t>2ffd5191-70cd-45c3-b3ac-054369dc5136</t>
+  </si>
+  <si>
+    <t>0dd6a98f-deb5-492c-9ae6-177877b5092f</t>
   </si>
   <si>
     <t>5b77d127-e62a-50a9-acee-bea63ff64dd5</t>
@@ -633,7 +633,7 @@
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>ad15e050-9877-4842-bf0c-e072f6d75322</t>
+    <t>a6b6a0ab-d615-45fa-950b-f31cc2be6c01</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -657,88 +657,88 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>8d81d446-4829-44e8-9423-4f32308f1fcb</t>
-  </si>
-  <si>
-    <t>5208ae96-002f-48ae-b0f0-a22e35c98f0d</t>
-  </si>
-  <si>
-    <t>5d1d7d11-500b-4e1e-bf41-9e7e33f83be5</t>
-  </si>
-  <si>
-    <t>d30057fb-c172-4ffd-8355-022461f5c678</t>
-  </si>
-  <si>
-    <t>c1821f00-34c3-4219-9648-e1bb9acbf6b8</t>
-  </si>
-  <si>
-    <t>c16d6795-2545-440b-a159-e11e8c6d59da</t>
-  </si>
-  <si>
-    <t>b63a4252-51d3-40e3-b5da-c853e0b62b8d</t>
-  </si>
-  <si>
-    <t>453b1236-0c6d-438a-bdf0-f12204f737a8</t>
-  </si>
-  <si>
-    <t>f0d70413-f4db-4332-91d4-0895f8d44778</t>
-  </si>
-  <si>
-    <t>49e7d211-7fb6-44fc-9d51-b1fd392d65ac</t>
-  </si>
-  <si>
-    <t>e5b95487-7833-41c5-9f6e-160810284b99</t>
-  </si>
-  <si>
-    <t>ec33acf8-5e6d-46aa-a053-076bc1bfa203</t>
-  </si>
-  <si>
-    <t>33d62e26-2575-4ae8-838e-05ac02a4420a</t>
-  </si>
-  <si>
-    <t>56421bca-4e37-4197-8677-36c19f13806d</t>
-  </si>
-  <si>
-    <t>13c920e3-06ea-4b73-b2e3-1eacedcd101d</t>
-  </si>
-  <si>
-    <t>f513a313-b990-4196-8c8d-a15f8a85fd95</t>
-  </si>
-  <si>
-    <t>c9ac8b4b-2544-432d-8493-0f3b4c0deb18</t>
-  </si>
-  <si>
-    <t>1168c218-92d2-4855-9a1c-3ca9b8f38f73</t>
-  </si>
-  <si>
-    <t>4f95b720-7848-4a5f-874e-e2460e0ab5d7</t>
-  </si>
-  <si>
-    <t>9f727189-605a-4317-8d50-17eacc675d72</t>
-  </si>
-  <si>
-    <t>5c1567db-166e-47f4-add8-a7f303a7c3b2</t>
-  </si>
-  <si>
-    <t>b86bb2c2-6ebe-415b-a140-ef15f7a89784</t>
-  </si>
-  <si>
-    <t>0efd8cab-9648-4563-b2d5-863ca581bc6a</t>
-  </si>
-  <si>
-    <t>36139345-d31b-469e-ad25-abc5bcacc950</t>
-  </si>
-  <si>
-    <t>a4e920b1-8976-447b-99af-555fa9c49bb2</t>
-  </si>
-  <si>
-    <t>b520e33f-7fc0-4508-851e-d395b41f7026</t>
-  </si>
-  <si>
-    <t>e23f3a01-6b85-49f0-b6d7-feddc4d41914</t>
-  </si>
-  <si>
-    <t>8a0d51b8-8d0a-4600-abf7-7c1c646e5afd</t>
+    <t>64a5dcc4-625f-4c09-a535-79ff35cd3d5a</t>
+  </si>
+  <si>
+    <t>201b7405-3603-44a0-967b-0483a81cb937</t>
+  </si>
+  <si>
+    <t>94d1af43-19ba-4cf6-b438-7db42772068a</t>
+  </si>
+  <si>
+    <t>7067fc04-1f8a-41f2-a41f-fca30d872f50</t>
+  </si>
+  <si>
+    <t>4639ff42-71a3-4bc3-891e-e9a0c3b122cd</t>
+  </si>
+  <si>
+    <t>9288295b-a41c-4fdf-b488-7c20b467f5e5</t>
+  </si>
+  <si>
+    <t>4c8f738f-0c83-4350-80b4-0a9ed20d4799</t>
+  </si>
+  <si>
+    <t>e2b4adb3-0c0f-4411-9ea1-4e4726acaa6b</t>
+  </si>
+  <si>
+    <t>38038d0e-91a7-469b-8d15-c59962b507b2</t>
+  </si>
+  <si>
+    <t>ce5ba600-35b8-4697-86d3-d37108e9cb0a</t>
+  </si>
+  <si>
+    <t>e3e0cf5d-1075-437d-b12d-8326671dccb4</t>
+  </si>
+  <si>
+    <t>1a80c7fa-39d4-42eb-bb2f-d6da49e527be</t>
+  </si>
+  <si>
+    <t>b395917a-423e-44d5-8c78-384d04931861</t>
+  </si>
+  <si>
+    <t>095d52a4-2eb9-486e-89d8-724353ac08e6</t>
+  </si>
+  <si>
+    <t>9d056191-a091-4af0-b693-e06d96f85bff</t>
+  </si>
+  <si>
+    <t>7a8bd44d-615a-4cc3-940e-fd214a499d15</t>
+  </si>
+  <si>
+    <t>148ab7fb-1eb7-4f8b-a32e-5b614b7b4683</t>
+  </si>
+  <si>
+    <t>eae3afe6-adec-40b6-9b49-01d00c84971d</t>
+  </si>
+  <si>
+    <t>b4edc9eb-f96d-48d5-beaa-14bdca734be4</t>
+  </si>
+  <si>
+    <t>be569bbf-0fda-415b-866b-d9e4b9ccaefd</t>
+  </si>
+  <si>
+    <t>4b5e09fc-9370-436c-aee7-6a5ff5107628</t>
+  </si>
+  <si>
+    <t>8153de51-2609-446a-98da-55c7ec1aec91</t>
+  </si>
+  <si>
+    <t>f7d07424-e9bd-4c42-b905-5a4db6cd6336</t>
+  </si>
+  <si>
+    <t>70e4d562-c243-4a32-bacf-9dc8f86b8f5b</t>
+  </si>
+  <si>
+    <t>b2ea2d37-4870-423f-8fc2-fb978f2bf09d</t>
+  </si>
+  <si>
+    <t>94f9454c-a5f6-4912-a012-acfc819000e7</t>
+  </si>
+  <si>
+    <t>0571fba4-406d-4357-93a2-54eaca25740b</t>
+  </si>
+  <si>
+    <t>dbdf1164-ed8c-45f4-9223-20343968fe4e</t>
   </si>
   <si>
     <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>

</xml_diff>

<commit_message>
feat: improve validation with ref data
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -282,7 +282,7 @@
     <t>screening_2_01hpkty3hctk826tvx5tasga55</t>
   </si>
   <si>
-    <t>c7c69ba0-f858-4e90-aa64-a6dcd57a8fcb</t>
+    <t>372cb3aa-d3cc-455b-a905-55d42e516ed1</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -297,16 +297,16 @@
     <t>Provide a value for SCREENING_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>0e352222-93c8-4557-a641-9158c83c6477</t>
-  </si>
-  <si>
-    <t>202d2b17-8cf8-4215-a471-c9c07fe2f42e</t>
-  </si>
-  <si>
-    <t>a606f389-719e-43ff-9785-e23ebb0511a1</t>
-  </si>
-  <si>
-    <t>22714e1c-6534-4305-bb9f-1d27e47b7e42</t>
+    <t>0ed122a5-5c70-4cad-9cec-53362f0d714b</t>
+  </si>
+  <si>
+    <t>0637a275-a245-4bd1-904d-38462b3f8c12</t>
+  </si>
+  <si>
+    <t>c812b8c4-786a-4566-84b2-207142fe1175</t>
+  </si>
+  <si>
+    <t>85c0de35-8816-4631-abfb-2d3a290d3d59</t>
   </si>
   <si>
     <t>Mandatory field SCREENING_CODE is empty</t>
@@ -318,16 +318,16 @@
     <t>Provide a value for SCREENING_CODE</t>
   </si>
   <si>
-    <t>51b35066-9c15-4914-bc9c-514d19b09dd5</t>
-  </si>
-  <si>
-    <t>a896ecfc-80df-41e8-acd5-bc2653941ff5</t>
-  </si>
-  <si>
-    <t>3b6941b2-e0be-4591-9231-c35bd19e2c92</t>
-  </si>
-  <si>
-    <t>466b36f1-86ad-4d4c-b856-a1689bd39f77</t>
+    <t>a2ae6296-de2b-45e3-862a-a1fa81caed99</t>
+  </si>
+  <si>
+    <t>83c2aa69-9cd6-4379-bf1c-58680e3a79e1</t>
+  </si>
+  <si>
+    <t>0041ec7b-0505-4fd9-9cf1-98bab786f898</t>
+  </si>
+  <si>
+    <t>4372dc0b-137f-425e-862b-8779645a1edd</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -345,94 +345,94 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>6e0e1568-9aac-444b-8814-b460028af9e8</t>
-  </si>
-  <si>
-    <t>6268d063-41cd-4f4e-93eb-7f8680b0a253</t>
-  </si>
-  <si>
-    <t>9cb81b78-f5cf-4d73-80d3-a09470b3e4c1</t>
-  </si>
-  <si>
-    <t>bcb64404-e307-41c2-b7ea-a45beb781eb5</t>
-  </si>
-  <si>
-    <t>97c1251c-860b-42a0-befc-d73e32fb9784</t>
-  </si>
-  <si>
-    <t>67632208-780a-469c-94e5-00005c442d32</t>
-  </si>
-  <si>
-    <t>488407d6-5457-4863-a8de-3610e941c486</t>
-  </si>
-  <si>
-    <t>f8975d05-dcf2-47fc-b4ba-edc92ffe9f09</t>
-  </si>
-  <si>
-    <t>ab39d8fb-27e8-4d34-866b-d0bfed43c99c</t>
-  </si>
-  <si>
-    <t>56bdf120-34a3-4546-93ad-53f00a5ea289</t>
-  </si>
-  <si>
-    <t>0dbe55c0-164d-4bd1-b150-9d7ad8f95666</t>
-  </si>
-  <si>
-    <t>6005387c-55d9-426d-944e-db531a3e5e2b</t>
-  </si>
-  <si>
-    <t>954981de-5187-4c3f-8e39-77d9af36d9c8</t>
-  </si>
-  <si>
-    <t>1adad4cb-b05c-4692-b1ee-4ff26c8ba110</t>
-  </si>
-  <si>
-    <t>41070fbc-c819-4bd2-b840-f9d5a8cebbd8</t>
-  </si>
-  <si>
-    <t>98062f52-6acf-4df6-bbb3-4e6bcc9673d8</t>
-  </si>
-  <si>
-    <t>32fd55b4-3397-438d-a9e8-d8df046e4b9b</t>
-  </si>
-  <si>
-    <t>b68a60b4-6656-45a5-bc5d-ecf7ac3c9d4e</t>
-  </si>
-  <si>
-    <t>7b5b33f6-b5a1-40c3-afeb-d56a34c7822f</t>
-  </si>
-  <si>
-    <t>781c1c32-229e-46f1-a11f-bb8086fe4d62</t>
-  </si>
-  <si>
-    <t>68da8bd6-6a43-446e-9668-07d4e6fed358</t>
-  </si>
-  <si>
-    <t>dfe986ef-f14b-4521-abcc-9744e57f97b8</t>
-  </si>
-  <si>
-    <t>2bbe56cc-d76d-4f6a-8e1f-6564c7e74099</t>
-  </si>
-  <si>
-    <t>630d39ae-d04b-48e4-a540-489be79757a9</t>
-  </si>
-  <si>
-    <t>f341e321-a51f-4bb4-80d5-b7e15ad06c0d</t>
-  </si>
-  <si>
-    <t>1e80f7a7-a503-4d0c-9452-789b2378c40b</t>
-  </si>
-  <si>
-    <t>aa3ecc24-9883-413e-920b-c57a6712f2f9</t>
-  </si>
-  <si>
-    <t>0203acab-2899-46dc-b7d7-2464587fa1fc</t>
-  </si>
-  <si>
-    <t>f21f6279-fec9-496c-be0a-2084ab209892</t>
-  </si>
-  <si>
-    <t>6b71b40a-baca-46c4-ae49-2017d69fe829</t>
+    <t>2daf847a-7c6c-4430-a71d-ec28c5fea551</t>
+  </si>
+  <si>
+    <t>9bdc4625-b04c-4ff8-b01f-cf79aa0adf7d</t>
+  </si>
+  <si>
+    <t>701dc41b-d2c1-4d97-bf1c-d348b334904b</t>
+  </si>
+  <si>
+    <t>2159dc03-98c8-4bd5-ae57-525d75881eba</t>
+  </si>
+  <si>
+    <t>ae3bbbe0-944c-44e7-926a-50915cfc6e1f</t>
+  </si>
+  <si>
+    <t>3a591750-d1ce-4d62-9669-efbf6ee90631</t>
+  </si>
+  <si>
+    <t>db8aabcb-8085-4dbd-8e49-ebd9364c181f</t>
+  </si>
+  <si>
+    <t>ed0a18d5-11cd-4fc4-ba5d-adf873b7595c</t>
+  </si>
+  <si>
+    <t>b96fd29f-efae-45c4-ac8a-80420a6c5936</t>
+  </si>
+  <si>
+    <t>cd278cf5-384d-4729-996c-0420f5d9d628</t>
+  </si>
+  <si>
+    <t>9a3a41b1-2a42-452a-8c27-b29fe55214f4</t>
+  </si>
+  <si>
+    <t>d70754be-cc55-41ec-b06d-96243a529b1e</t>
+  </si>
+  <si>
+    <t>24a5bcc3-ddb9-4a9e-b730-0bebd0b42617</t>
+  </si>
+  <si>
+    <t>73706993-b444-4171-bca6-566335e3fffc</t>
+  </si>
+  <si>
+    <t>0046b82e-9ab4-43c5-bf80-ecd54c160e30</t>
+  </si>
+  <si>
+    <t>bab249b5-51eb-444b-818b-de6dc059ff41</t>
+  </si>
+  <si>
+    <t>d92f112a-93d1-4bdd-bc82-ac2f0d8d5d2e</t>
+  </si>
+  <si>
+    <t>6a4ec714-33e6-44e3-a238-0e60838c8a8c</t>
+  </si>
+  <si>
+    <t>59aa3cc6-efe0-40b3-b430-92f4278e0a3a</t>
+  </si>
+  <si>
+    <t>d0197805-5078-40ff-82da-52ab10602dbf</t>
+  </si>
+  <si>
+    <t>975f06e4-d477-4015-9a9d-9ddf165ed0c9</t>
+  </si>
+  <si>
+    <t>b1fcdaf0-bcb4-464b-8e6d-b8e2abb5ccc8</t>
+  </si>
+  <si>
+    <t>0e5864ae-9696-49dd-866b-1224bb8ca615</t>
+  </si>
+  <si>
+    <t>2907bfbd-9c8b-45d4-bc74-12fb54d3fd24</t>
+  </si>
+  <si>
+    <t>b4a27f1e-19fe-4c6b-8ce8-3e60f9d85655</t>
+  </si>
+  <si>
+    <t>9f36a0c8-3e4e-4ee5-9a83-a905decfa0d8</t>
+  </si>
+  <si>
+    <t>82c3873f-b121-42e2-9bf0-9806370453b3</t>
+  </si>
+  <si>
+    <t>72929b93-50b1-4489-8a67-73bb09af0ff2</t>
+  </si>
+  <si>
+    <t>c72075d5-a03f-4a50-9f7c-3674efc50f8a</t>
+  </si>
+  <si>
+    <t>b084fa4d-c34b-4e49-bef4-6088df401a96</t>
   </si>
   <si>
     <t>Invalid timestamp "2023152  2:38:06 PM" found in RECORDED_TIME</t>
@@ -441,94 +441,94 @@
     <t>2023152  2:38:06 PM</t>
   </si>
   <si>
-    <t>34767309-75b8-4710-8d4e-8bc4d2e6b45c</t>
-  </si>
-  <si>
-    <t>027ddff8-b1b6-47a2-8c51-c897c9089ce3</t>
-  </si>
-  <si>
-    <t>68697c64-13db-4735-b1ce-3bbea7c08739</t>
-  </si>
-  <si>
-    <t>dae0cd7d-6942-474b-995d-0dd20acacdc9</t>
-  </si>
-  <si>
-    <t>720ae89c-daf0-44c4-8745-ab7bf875ac10</t>
-  </si>
-  <si>
-    <t>b40c8afc-cc1b-4be8-ad63-59321edecf31</t>
-  </si>
-  <si>
-    <t>31815b6f-c96e-43c9-8fb6-7fcbaaa63f14</t>
-  </si>
-  <si>
-    <t>e2d46a1a-4e7a-4e8f-8957-2408eb3a60e0</t>
-  </si>
-  <si>
-    <t>a3fb126f-285d-46f0-89c1-bafe1df05623</t>
-  </si>
-  <si>
-    <t>97435109-e58d-4e5e-b476-4a2848ff8a7b</t>
-  </si>
-  <si>
-    <t>2a9773a4-c60d-4dc3-a4f5-cffdaceb6f83</t>
-  </si>
-  <si>
-    <t>840f4e8a-148c-424a-9ccd-251896ca737d</t>
-  </si>
-  <si>
-    <t>9eb8c6eb-14bd-48a4-a8df-b84d3a8562fe</t>
-  </si>
-  <si>
-    <t>ea561f9b-7b77-416a-b970-2882e408a0c5</t>
-  </si>
-  <si>
-    <t>452efb45-239a-4c2e-84b2-6a733c59183d</t>
-  </si>
-  <si>
-    <t>6f5aedb4-f2db-4134-8ed9-e85d8d63a002</t>
-  </si>
-  <si>
-    <t>38dd49b7-a478-47fb-8aae-f7e38b3adc67</t>
-  </si>
-  <si>
-    <t>d1794036-118e-4e4b-938c-aebdce18dbd3</t>
-  </si>
-  <si>
-    <t>5cd83bdd-91f1-4c8e-bd85-c78357d0c588</t>
-  </si>
-  <si>
-    <t>a45db671-f0ab-43dd-9f0d-0f3521dc6335</t>
-  </si>
-  <si>
-    <t>87e6e272-b9bc-48f5-a758-e3c1808e9aef</t>
-  </si>
-  <si>
-    <t>ae3b9b1b-4ca5-472b-a8bc-4e6024d12740</t>
-  </si>
-  <si>
-    <t>9e8819cb-9d7b-4eb4-835d-04248f9502ef</t>
-  </si>
-  <si>
-    <t>907bcec3-c618-40e0-9494-cf805e290ee8</t>
-  </si>
-  <si>
-    <t>7fad2beb-db26-4441-9d2d-c5b1cab67ac7</t>
-  </si>
-  <si>
-    <t>41e23d15-c190-410f-85f6-9e4c62d4f8aa</t>
-  </si>
-  <si>
-    <t>c31921e3-fdc8-4dd2-8b2e-d421f580c183</t>
-  </si>
-  <si>
-    <t>e32650be-23c7-4380-befb-8716e8d23196</t>
-  </si>
-  <si>
-    <t>61b0dbb4-7332-4162-b830-4ff3b696a8f0</t>
-  </si>
-  <si>
-    <t>8a05fa10-8a9c-4064-9868-52e526fb1e4a</t>
+    <t>763b57a5-c33c-442b-88d3-f2a9b1a99213</t>
+  </si>
+  <si>
+    <t>ac910329-0262-4d62-84a8-d2c6bd40638e</t>
+  </si>
+  <si>
+    <t>91b551a8-6f96-433e-bd34-4a8744009d83</t>
+  </si>
+  <si>
+    <t>dc749e63-1e6d-44b8-9c79-361abed985a7</t>
+  </si>
+  <si>
+    <t>ad3004cb-1002-40b9-baca-169df14c1700</t>
+  </si>
+  <si>
+    <t>c94524a8-53a1-4f75-8aba-a3e137cef2e6</t>
+  </si>
+  <si>
+    <t>d746cfb4-4bfc-4dfd-9d8d-eaa011bec22b</t>
+  </si>
+  <si>
+    <t>49899fc0-ad1a-4a1e-b72d-0b9e1888b952</t>
+  </si>
+  <si>
+    <t>378a9579-bd6a-44d0-b9cb-bdcd2ff88270</t>
+  </si>
+  <si>
+    <t>ecdd500f-7b06-40da-b868-c3bb5ca413d4</t>
+  </si>
+  <si>
+    <t>0f9eaa0e-6b7e-4b54-a464-27abcd79d613</t>
+  </si>
+  <si>
+    <t>c9e048e4-389e-4274-b9c4-11e86d7337ee</t>
+  </si>
+  <si>
+    <t>2ee0b975-83d1-4fe6-9a2a-7cabbbd15cb9</t>
+  </si>
+  <si>
+    <t>8f62aacd-7797-482e-bf40-adebd0532de2</t>
+  </si>
+  <si>
+    <t>c4e64aa2-49a1-4f3d-9074-90f7f756e3fd</t>
+  </si>
+  <si>
+    <t>0b981b84-11ed-4c66-b8c5-75626c99d5e7</t>
+  </si>
+  <si>
+    <t>d735378e-eb64-42a4-80f4-fc4e175fa6aa</t>
+  </si>
+  <si>
+    <t>4a31bde2-3396-4e79-92dd-6cd9f3a9f21a</t>
+  </si>
+  <si>
+    <t>025cabee-24af-4ff9-99a8-31c9c1adde43</t>
+  </si>
+  <si>
+    <t>554e4017-bd12-4917-847c-b755f3b47824</t>
+  </si>
+  <si>
+    <t>f90c2bef-ee88-44e6-b475-f9cff7f97a65</t>
+  </si>
+  <si>
+    <t>d4ce1835-46f4-49c7-a8a9-7447a67b6b16</t>
+  </si>
+  <si>
+    <t>693431ed-8f29-4f7f-8906-48b117729456</t>
+  </si>
+  <si>
+    <t>9f8d9646-eaf1-4ec4-8434-4a2c1a70ec40</t>
+  </si>
+  <si>
+    <t>e26a68bc-aa42-4fc5-9bc8-d669f2d8366a</t>
+  </si>
+  <si>
+    <t>a62f8413-a713-4c95-9a7e-2093a36e58ad</t>
+  </si>
+  <si>
+    <t>4da7cbcb-8083-483a-be7c-67c7a6baac6a</t>
+  </si>
+  <si>
+    <t>70c885bf-80a6-42d8-b0d4-c8897471757e</t>
+  </si>
+  <si>
+    <t>4929f468-ab9f-46db-81f7-c5c368329ce0</t>
+  </si>
+  <si>
+    <t>2fcf07f2-20fd-47c8-8218-6a92d1109299</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE is empty</t>
@@ -540,16 +540,16 @@
     <t>Provide a value for QUESTION_CODE</t>
   </si>
   <si>
-    <t>20deaa51-651b-4923-9fba-392e6cb41bc8</t>
-  </si>
-  <si>
-    <t>d469a47a-5f43-4816-94e4-319c8e9241ea</t>
-  </si>
-  <si>
-    <t>6cc8d07a-9051-4615-8b46-8f354fd6d186</t>
-  </si>
-  <si>
-    <t>8e82ef9d-8778-4a87-9565-312af629bee5</t>
+    <t>37af9c50-b101-4988-92bc-7c32844139d1</t>
+  </si>
+  <si>
+    <t>1f4c623b-b4cd-439a-ab5c-43b4cefae2d3</t>
+  </si>
+  <si>
+    <t>09da1850-3489-471e-aa5a-b062ba695ff3</t>
+  </si>
+  <si>
+    <t>56cf1db1-c906-4a84-a31f-d3cd405132bc</t>
   </si>
   <si>
     <t>Mandatory field QUESTION_CODE_SYSTEM_NAME is empty</t>
@@ -561,16 +561,16 @@
     <t>Provide a value for QUESTION_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>19a0239a-aefe-4e3b-a3ee-ce54461b124c</t>
-  </si>
-  <si>
-    <t>83f16d06-c095-4392-b5fb-d0455f800897</t>
-  </si>
-  <si>
-    <t>b91b9c08-954b-4498-b2a3-4c56fd09fce8</t>
-  </si>
-  <si>
-    <t>89eadf09-6d6d-403d-9667-084794ec1103</t>
+    <t>f4c55d4e-ddcc-4948-9bdb-772896b2630f</t>
+  </si>
+  <si>
+    <t>71f17a13-d9a6-46fe-932f-0d0cfbf4cd66</t>
+  </si>
+  <si>
+    <t>97b346ef-5a26-42a9-be25-4820c856a724</t>
+  </si>
+  <si>
+    <t>2076b7b3-18b8-401a-a8ce-df6031bec2d8</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE is empty</t>
@@ -582,22 +582,22 @@
     <t>Provide a value for ANSWER_CODE</t>
   </si>
   <si>
-    <t>3c433083-e284-4cec-bdbd-5095b4ae66ac</t>
-  </si>
-  <si>
-    <t>02bbfea6-1016-466a-b3df-ef24c42f1d7f</t>
-  </si>
-  <si>
-    <t>c7b08b01-dacd-424e-8711-7779f02486c0</t>
-  </si>
-  <si>
-    <t>b3abbd32-b6ee-48a4-baf5-c56e6eaa093f</t>
-  </si>
-  <si>
-    <t>55d7c9cb-f6ea-40d3-b3f1-3e452ec0217c</t>
-  </si>
-  <si>
-    <t>55324869-d02e-4a88-b841-b7ad372ee148</t>
+    <t>bbc9b991-5063-4394-bd46-c4cce43d9bcb</t>
+  </si>
+  <si>
+    <t>54e0d1e2-b526-4ff8-b88b-1bb3eb75947b</t>
+  </si>
+  <si>
+    <t>efaaa067-0e50-47e6-acd9-0ab3a5ce05fc</t>
+  </si>
+  <si>
+    <t>3fdab6c9-39a3-4905-9019-33f3dd3711db</t>
+  </si>
+  <si>
+    <t>c2b2ec59-31ba-4ab4-a006-2c95b3cb0dd8</t>
+  </si>
+  <si>
+    <t>0593ced6-b74c-4d75-a958-59f034317205</t>
   </si>
   <si>
     <t>Mandatory field ANSWER_CODE_SYSTEM_NAME is empty</t>
@@ -609,19 +609,19 @@
     <t>Provide a value for ANSWER_CODE_SYSTEM_NAME</t>
   </si>
   <si>
-    <t>418f562d-fe9b-44aa-9b00-636f9da04aa8</t>
-  </si>
-  <si>
-    <t>8e02ad38-bb3e-403c-baf0-a3c476cdfb3d</t>
-  </si>
-  <si>
-    <t>1bb7ca21-9b29-4af2-ad84-4a42756e061c</t>
-  </si>
-  <si>
-    <t>2ffd5191-70cd-45c3-b3ac-054369dc5136</t>
-  </si>
-  <si>
-    <t>0dd6a98f-deb5-492c-9ae6-177877b5092f</t>
+    <t>419a5c1d-c836-4e6e-9870-97c855ea29fa</t>
+  </si>
+  <si>
+    <t>3f7f17e7-56e7-4b1d-be14-bb1e9239d956</t>
+  </si>
+  <si>
+    <t>3f89b6b0-4b5d-49f7-9b11-81f91f9511ca</t>
+  </si>
+  <si>
+    <t>b47ecb57-539e-4fcb-8fbc-a1a1fe0c6c67</t>
+  </si>
+  <si>
+    <t>8d5a54ef-5289-4c7f-80a0-48359746709f</t>
   </si>
   <si>
     <t>5b77d127-e62a-50a9-acee-bea63ff64dd5</t>
@@ -633,7 +633,7 @@
     <t>ahc_hrsn_2024_01_25_valid_admin_demographic</t>
   </si>
   <si>
-    <t>a6b6a0ab-d615-45fa-950b-f31cc2be6c01</t>
+    <t>3ab0389a-057e-4eef-9135-78fa900f5810</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -657,88 +657,88 @@
     <t>ahc_hrsn_2024_01_25_valid_screening</t>
   </si>
   <si>
-    <t>64a5dcc4-625f-4c09-a535-79ff35cd3d5a</t>
-  </si>
-  <si>
-    <t>201b7405-3603-44a0-967b-0483a81cb937</t>
-  </si>
-  <si>
-    <t>94d1af43-19ba-4cf6-b438-7db42772068a</t>
-  </si>
-  <si>
-    <t>7067fc04-1f8a-41f2-a41f-fca30d872f50</t>
-  </si>
-  <si>
-    <t>4639ff42-71a3-4bc3-891e-e9a0c3b122cd</t>
-  </si>
-  <si>
-    <t>9288295b-a41c-4fdf-b488-7c20b467f5e5</t>
-  </si>
-  <si>
-    <t>4c8f738f-0c83-4350-80b4-0a9ed20d4799</t>
-  </si>
-  <si>
-    <t>e2b4adb3-0c0f-4411-9ea1-4e4726acaa6b</t>
-  </si>
-  <si>
-    <t>38038d0e-91a7-469b-8d15-c59962b507b2</t>
-  </si>
-  <si>
-    <t>ce5ba600-35b8-4697-86d3-d37108e9cb0a</t>
-  </si>
-  <si>
-    <t>e3e0cf5d-1075-437d-b12d-8326671dccb4</t>
-  </si>
-  <si>
-    <t>1a80c7fa-39d4-42eb-bb2f-d6da49e527be</t>
-  </si>
-  <si>
-    <t>b395917a-423e-44d5-8c78-384d04931861</t>
-  </si>
-  <si>
-    <t>095d52a4-2eb9-486e-89d8-724353ac08e6</t>
-  </si>
-  <si>
-    <t>9d056191-a091-4af0-b693-e06d96f85bff</t>
-  </si>
-  <si>
-    <t>7a8bd44d-615a-4cc3-940e-fd214a499d15</t>
-  </si>
-  <si>
-    <t>148ab7fb-1eb7-4f8b-a32e-5b614b7b4683</t>
-  </si>
-  <si>
-    <t>eae3afe6-adec-40b6-9b49-01d00c84971d</t>
-  </si>
-  <si>
-    <t>b4edc9eb-f96d-48d5-beaa-14bdca734be4</t>
-  </si>
-  <si>
-    <t>be569bbf-0fda-415b-866b-d9e4b9ccaefd</t>
-  </si>
-  <si>
-    <t>4b5e09fc-9370-436c-aee7-6a5ff5107628</t>
-  </si>
-  <si>
-    <t>8153de51-2609-446a-98da-55c7ec1aec91</t>
-  </si>
-  <si>
-    <t>f7d07424-e9bd-4c42-b905-5a4db6cd6336</t>
-  </si>
-  <si>
-    <t>70e4d562-c243-4a32-bacf-9dc8f86b8f5b</t>
-  </si>
-  <si>
-    <t>b2ea2d37-4870-423f-8fc2-fb978f2bf09d</t>
-  </si>
-  <si>
-    <t>94f9454c-a5f6-4912-a012-acfc819000e7</t>
-  </si>
-  <si>
-    <t>0571fba4-406d-4357-93a2-54eaca25740b</t>
-  </si>
-  <si>
-    <t>dbdf1164-ed8c-45f4-9223-20343968fe4e</t>
+    <t>83257be3-215b-4065-a54a-0ad6682cf23a</t>
+  </si>
+  <si>
+    <t>32a94177-aa6e-4e52-bb40-4da5966c144c</t>
+  </si>
+  <si>
+    <t>6568617e-58a7-405d-b583-ed4e86551044</t>
+  </si>
+  <si>
+    <t>1ac97b52-297e-4ecb-bdac-c34828e7d60c</t>
+  </si>
+  <si>
+    <t>7acdac34-7ae3-4e42-95b9-dc3ec74e5f1a</t>
+  </si>
+  <si>
+    <t>b2c22bec-fa9a-4ed8-a546-de2835af7776</t>
+  </si>
+  <si>
+    <t>67066532-86a1-4645-87d5-0ce62b34d801</t>
+  </si>
+  <si>
+    <t>2a75fb98-d523-47ba-9141-598845efde37</t>
+  </si>
+  <si>
+    <t>79575c63-9e16-41db-8e95-febc68cdb703</t>
+  </si>
+  <si>
+    <t>f6ff5e47-86a5-4afa-a442-b19a87d2f3b9</t>
+  </si>
+  <si>
+    <t>e5b5e157-8fe5-43c0-9649-6ccd9af6aa44</t>
+  </si>
+  <si>
+    <t>3a9eb28a-f9fc-4b1a-a3c5-7eacfe0f5188</t>
+  </si>
+  <si>
+    <t>9b6d9dcd-e9ad-45cb-90c5-88c941a832c7</t>
+  </si>
+  <si>
+    <t>770bccb5-9e72-4e5f-b2ed-7016cd145c75</t>
+  </si>
+  <si>
+    <t>267f305b-6cd0-40af-bb69-76c45cd358e2</t>
+  </si>
+  <si>
+    <t>73af36cd-a77a-4e3d-8840-503958201bc0</t>
+  </si>
+  <si>
+    <t>619d6334-c993-408c-a7a6-1cf7ed1db415</t>
+  </si>
+  <si>
+    <t>5c3cad25-d713-4d4f-9ca3-fc8275069a71</t>
+  </si>
+  <si>
+    <t>6c8ff5fa-9e7d-4de7-b381-1b66b81672bb</t>
+  </si>
+  <si>
+    <t>f3cf86ad-0b3a-43a9-8733-d548e2094dad</t>
+  </si>
+  <si>
+    <t>ad9bfcd1-e193-496e-8756-27c8d38ea84a</t>
+  </si>
+  <si>
+    <t>b110e34b-b1a5-46ee-9971-7d4535561f28</t>
+  </si>
+  <si>
+    <t>9df52aea-f06e-403a-a82e-9010d3adc9d2</t>
+  </si>
+  <si>
+    <t>2597f3e4-7cd9-44ff-8159-2da33dfbfcc9</t>
+  </si>
+  <si>
+    <t>c97455cd-54b3-495f-b762-10a1a960415f</t>
+  </si>
+  <si>
+    <t>1885623d-c36a-41f7-8fed-9f303a0897b1</t>
+  </si>
+  <si>
+    <t>c0ea0aa3-962f-4869-aa6b-fc368a8cc634</t>
+  </si>
+  <si>
+    <t>34a0f612-b3f8-4888-86ce-28ca5ba496fd</t>
   </si>
   <si>
     <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>

</xml_diff>

<commit_message>
feat: add validation rules #53
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="122">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -87,79 +87,115 @@
     <t>Session 05269d28-15ae-5bd6-bd88-f949ccfa52d7 markdown diagnostics not provided (not completed?)</t>
   </si>
   <si>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/SCREENING_20240307.csv</t>
+  </si>
+  <si>
+    <t>screening_20240307</t>
+  </si>
+  <si>
+    <t>9e04c08e-ce47-42f1-b0e6-ea2faa81ef86</t>
+  </si>
+  <si>
+    <t>Invalid Date</t>
+  </si>
+  <si>
+    <t>Invalid timestamp "01/27/02 15:42" found in RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>01/27/02 15:42</t>
+  </si>
+  <si>
+    <t>Please be sure to provide both a valid date and time (Format: YYYYMMDD HH:MM:SS).</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>9cfbd778-d553-48b6-b13d-c13109798043</t>
+  </si>
+  <si>
+    <t>Invalid Answer Code</t>
+  </si>
+  <si>
+    <t>Invalid Answer Code "LA32-8" for Question Code "69861-3" found in ANSWER_CODE</t>
+  </si>
+  <si>
+    <t>ANSWER_CODE</t>
+  </si>
+  <si>
+    <t>LA32-8</t>
+  </si>
+  <si>
+    <t>Validate Question Code and Answer Code with ahc cross walk reference data</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>Resolved By QE/QCS</t>
+  </si>
+  <si>
+    <t>5ce08072-9956-4dc3-815d-185daf2def62</t>
+  </si>
+  <si>
+    <t>Missing Mandatory Value</t>
+  </si>
+  <si>
+    <t>Mandatory field POTENTIAL_NEED_INDICATED is empty</t>
+  </si>
+  <si>
+    <t>POTENTIAL_NEED_INDICATED</t>
+  </si>
+  <si>
+    <t>Provide a value for POTENTIAL_NEED_INDICATED</t>
+  </si>
+  <si>
+    <t>REJECTION</t>
+  </si>
+  <si>
     <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/SCREENING_healthix-20240307-testcase1.csv</t>
-  </si>
-  <si>
-    <t>screening_healthix_20240307_testcase1</t>
-  </si>
-  <si>
-    <t>77fffdfe-e7a8-4b61-8541-b079f6e39b1c</t>
-  </si>
-  <si>
-    <t>Invalid Date</t>
-  </si>
-  <si>
-    <t>Invalid timestamp "1988-05-30 01:09:07" found in RECORDED_TIME</t>
-  </si>
-  <si>
-    <t>RECORDED_TIME</t>
-  </si>
-  <si>
-    <t>1988-05-30 01:09:07</t>
-  </si>
-  <si>
-    <t>Please be sure to provide both a valid date and time (Format: YYYYMMDD HH:MM:SS).</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>8a2ea7b1-6b5d-4261-80ff-c0d8b1b100fe</t>
-  </si>
-  <si>
-    <t>Invalid value in QUESTION_CODE</t>
-  </si>
-  <si>
-    <t>Balnk/Empty value for QUESTION_CODE_DESCRIPTION "Do you speak a language other than English at home?" found in QUESTION_CODE</t>
-  </si>
-  <si>
-    <t>QUESTION_CODE</t>
-  </si>
-  <si>
-    <t>Do you speak a language other than English at home?</t>
-  </si>
-  <si>
-    <t>The required field value QUESTION_CODE is missing</t>
-  </si>
-  <si>
-    <t>WARNING</t>
-  </si>
-  <si>
-    <t>Resolved By QE/QCS</t>
-  </si>
-  <si>
-    <t>cb45537b-1d88-476c-a4dd-d0b7f65f9d77</t>
-  </si>
-  <si>
-    <t>Invalid Answer Code</t>
-  </si>
-  <si>
-    <t>Invalid Answer Code "LA32-8" for Question Code "69861-3" found in ANSWER_CODE</t>
-  </si>
-  <si>
-    <t>ANSWER_CODE</t>
-  </si>
-  <si>
-    <t>LA32-8</t>
-  </si>
-  <si>
-    <t>Validate Question Code and Answer Code with ahc cross walk reference data</t>
-  </si>
-  <si>
-    <t>64b154e9-98d3-4e42-bcd3-66a6e03c5537</t>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/DEMOGRAPHIC_DATA_20240307.csv</t>
+  </si>
+  <si>
+    <t>admin_demographics_20240307</t>
+  </si>
+  <si>
+    <t>294b0491-31dd-4be7-91d3-3003d31f9e30</t>
+  </si>
+  <si>
+    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" found in SEX_AT_BIRTH_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SEX_AT_BIRTH_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
+  </si>
+  <si>
+    <t>78c1b73d-1fad-4f32-b450-19f3f3a6c6c5</t>
+  </si>
+  <si>
+    <t>bbfa8aa7-72de-4516-a0cc-bcaaa736e610</t>
+  </si>
+  <si>
+    <t>9f5d6783-d15d-4fc8-9d5c-38f65689f510</t>
+  </si>
+  <si>
+    <t>dd053beb-145e-4db0-86dd-79d13f7139eb</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -168,247 +204,178 @@
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA')</t>
   </si>
   <si>
-    <t>POTENTIAL_NEED_INDICATED</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Use only allowed values 'Yes','No','NA' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>REJECTION</t>
+    <t>8251c962-311d-4b2e-abd2-35bb6081364e</t>
+  </si>
+  <si>
+    <t>bf006df1-137b-4380-94e7-6270f8580d7f</t>
+  </si>
+  <si>
+    <t>de324845-e6ad-4adb-b478-d988166efc9d</t>
+  </si>
+  <si>
+    <t>fbcab063-caf1-4534-8966-69689f5e9bd0</t>
+  </si>
+  <si>
+    <t>ab832d16-7982-4f5a-9fbd-594f52de55e2</t>
+  </si>
+  <si>
+    <t>d0ca0bbc-d440-416d-8589-ca9bebed39f5</t>
+  </si>
+  <si>
+    <t>a3f719df-8c38-4b38-9183-ec22d71f6329</t>
+  </si>
+  <si>
+    <t>75fd5f77-02ab-410f-87e2-4f14325131ca</t>
+  </si>
+  <si>
+    <t>2565ffdd-00e2-49d0-a37f-69fb18a58b58</t>
+  </si>
+  <si>
+    <t>4a9a9347-5057-437f-8e6e-555bddd11328</t>
+  </si>
+  <si>
+    <t>a0251d0c-869f-472c-89b2-cc429df93b7a</t>
+  </si>
+  <si>
+    <t>7b821f3d-63d4-4706-9a85-de3dce2f77a9</t>
+  </si>
+  <si>
+    <t>dd09ee58-27ac-4935-961f-d558309ae066</t>
+  </si>
+  <si>
+    <t>80d6e4f1-f10c-4c74-874d-3f07bd7fdc8a</t>
+  </si>
+  <si>
+    <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>03/05/94 13:08</t>
+  </si>
+  <si>
+    <t>3ca38a70-ac64-4035-845a-4c1d0154348e</t>
+  </si>
+  <si>
+    <t>be6986e1-e466-4927-8371-373a029574f6</t>
+  </si>
+  <si>
+    <t>2f42b780-25a4-44a5-8d4c-fcfdf813ed3a</t>
+  </si>
+  <si>
+    <t>05c81f04-3639-4a92-8cc9-0089cd548cc2</t>
+  </si>
+  <si>
+    <t>8989d84d-32ed-4575-8d9d-c51f07840a4b</t>
+  </si>
+  <si>
+    <t>6cedce8e-d18c-4636-922b-75feeff36db9</t>
+  </si>
+  <si>
+    <t>dd360ca8-eb17-4c9c-9a52-52b797d160ea</t>
+  </si>
+  <si>
+    <t>eddbc773-dae5-49b7-9a4d-8bdf89f53e3a</t>
+  </si>
+  <si>
+    <t>71311173-4497-4ab1-a86b-505ee8afc99c</t>
+  </si>
+  <si>
+    <t>186986b1-3b32-4298-91a9-8a868a852be1</t>
+  </si>
+  <si>
+    <t>906b9e45-9277-4ec9-aeba-6bc5932b50d0</t>
+  </si>
+  <si>
+    <t>11a8345b-fdf3-4dbb-88a7-81dba0654a0f</t>
+  </si>
+  <si>
+    <t>51f52e0b-f0b6-45b2-a07a-3af86befae27</t>
+  </si>
+  <si>
+    <t>2f8c2b78-0364-433c-bf76-f48b91d43f04</t>
+  </si>
+  <si>
+    <t>bc2a1c4f-e021-4a8b-92dc-01fa84eddae5</t>
+  </si>
+  <si>
+    <t>d1696b90-357c-4430-9111-a2a1b2074680</t>
+  </si>
+  <si>
+    <t>a0ecd25b-80a7-4ed7-9002-a00d6799d48a</t>
+  </si>
+  <si>
+    <t>7da5ebc6-4077-45ca-a1b3-a0a7da3139aa</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+  </si>
+  <si>
+    <t>Sheet Missing</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+  </si>
+  <si>
+    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>591191c7-f693-5957-8734-ac87151ca981</t>
+  </si>
+  <si>
+    <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>071f8fe1-4899-5c71-9c86-7d7377661d45</t>
   </si>
   <si>
     <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/DEMOGRAPHIC_DATA_healthix-20240307-testcase1.csv</t>
-  </si>
-  <si>
-    <t>admin_demographics_healthix_20240307_testcase1</t>
-  </si>
-  <si>
-    <t>4e28c9f2-4bb2-4a0f-b273-8cc294c2d8d0</t>
-  </si>
-  <si>
-    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION "other" found in SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
-  </si>
-  <si>
-    <t>c4c20e42-108c-416d-af8e-f6af1061df9e</t>
-  </si>
-  <si>
-    <t>Value urn:oid:2.16.840.1.113883.6.238 in RACE_CODE_SYSTEM_NAME not in allowed list ('CDC','CDCRE','2.16.840.1.113883.6.23')</t>
-  </si>
-  <si>
-    <t>RACE_CODE_SYSTEM_NAME</t>
-  </si>
-  <si>
-    <t>urn:oid:2.16.840.1.113883.6.238</t>
-  </si>
-  <si>
-    <t>Use only allowed values 'CDC','CDCRE','2.16.840.1.113883.6.23' in RACE_CODE_SYSTEM_NAME</t>
-  </si>
-  <si>
-    <t>dc3bb706-5336-432e-b456-b7f91359c6ec</t>
-  </si>
-  <si>
-    <t>Value urn:oid:2.16.840.1.113883.6.238 in ETHNICITY_CODE_SYSTEM_NAME not in allowed list ('CDC','CDCRE','2.16.840.1.113883.6.23')</t>
-  </si>
-  <si>
-    <t>ETHNICITY_CODE_SYSTEM_NAME</t>
-  </si>
-  <si>
-    <t>Use only allowed values 'CDC','CDCRE','2.16.840.1.113883.6.23' in ETHNICITY_CODE_SYSTEM_NAME</t>
-  </si>
-  <si>
-    <t>5565385a-4c6f-42c2-b74c-63852fa99cce</t>
-  </si>
-  <si>
-    <t>f7affba8-f0e2-4e45-82d2-220f94df0d80</t>
-  </si>
-  <si>
-    <t>Invalid Answer Code "LA10139-6" for Question Code "89555-7" found in ANSWER_CODE</t>
-  </si>
-  <si>
-    <t>LA10139-6</t>
-  </si>
-  <si>
-    <t>6506cbdd-a46f-46a7-8574-5e35493b36e5</t>
-  </si>
-  <si>
-    <t>19732e2d-7c74-4dcc-88e4-aeef6edb4829</t>
-  </si>
-  <si>
-    <t>e1374640-e45a-4e3f-8b92-d886188d0545</t>
-  </si>
-  <si>
-    <t>1315388f-d745-4ca5-8e3b-91fc8af459dc</t>
-  </si>
-  <si>
-    <t>21e0a270-5c6d-4db0-be24-b6d51dff5aae</t>
-  </si>
-  <si>
-    <t>95b9b606-0d8a-4164-b594-331c59569ffc</t>
-  </si>
-  <si>
-    <t>3690a92b-d6e3-4b2f-b20d-05fb89b7173b</t>
-  </si>
-  <si>
-    <t>c4bebf80-cd28-4371-b50c-6066e75860d4</t>
-  </si>
-  <si>
-    <t>95d05c4d-c412-41e8-9553-66224c93bb4b</t>
-  </si>
-  <si>
-    <t>619866d1-da69-4bec-9ca6-96b90a50926c</t>
-  </si>
-  <si>
-    <t>227b870a-7a0e-422f-893d-341ec9002f45</t>
-  </si>
-  <si>
-    <t>263a2cd3-019b-4cab-9f54-db4d0dea6fa8</t>
-  </si>
-  <si>
-    <t>4fd81d8a-f79a-451e-9394-131c4bfaab6e</t>
-  </si>
-  <si>
-    <t>d528bb43-387c-4828-a411-db7bc0c401c3</t>
-  </si>
-  <si>
-    <t>6810671a-17ab-42e0-89ad-e6c513f6bcc4</t>
-  </si>
-  <si>
-    <t>70bf9234-742b-40e1-9448-0efaf498bbaf</t>
-  </si>
-  <si>
-    <t>3cf8b4b9-343b-4514-835e-9450f6cac31a</t>
-  </si>
-  <si>
-    <t>Invalid timestamp "2000-06-05 20:25:02" found in RECORDED_TIME</t>
-  </si>
-  <si>
-    <t>2000-06-05 20:25:02</t>
-  </si>
-  <si>
-    <t>920165c6-575b-47d9-aae8-35653a4385c9</t>
-  </si>
-  <si>
-    <t>e30ed58f-df22-4bef-b7c7-0c3658059070</t>
-  </si>
-  <si>
-    <t>1076ce6d-6430-49ed-9c95-8a6ad994c129</t>
-  </si>
-  <si>
-    <t>d8f14533-9fe7-4716-91a5-0eb680f46bb7</t>
-  </si>
-  <si>
-    <t>fc108e30-f341-418f-8ff3-ec4baedd1811</t>
-  </si>
-  <si>
-    <t>946accf0-cdb9-4500-8546-50cb86d00eb2</t>
-  </si>
-  <si>
-    <t>c43c377e-fd5b-4348-ad6f-94d4e4ce01c9</t>
-  </si>
-  <si>
-    <t>35ac73bb-0aea-4d1b-b526-cf3a6bbbacd5</t>
-  </si>
-  <si>
-    <t>f49c8221-e5b6-48a4-b36c-920f74f45166</t>
-  </si>
-  <si>
-    <t>0d02ef1f-ad9f-4629-aca8-6eb61c7416f3</t>
-  </si>
-  <si>
-    <t>d358ccfc-02b9-4783-9a15-f8fee2585a5e</t>
-  </si>
-  <si>
-    <t>1f03b8b1-7058-4209-a1ef-20c95e8a24e7</t>
-  </si>
-  <si>
-    <t>d4b079e2-4907-4c68-b1c2-873119b56dd4</t>
-  </si>
-  <si>
-    <t>0cfbaab2-2c0b-4213-bebb-3edbee573804</t>
-  </si>
-  <si>
-    <t>aa29a908-6d26-438c-8f5d-2b3c94badfac</t>
-  </si>
-  <si>
-    <t>5193b0f7-2abf-46b0-b0df-5ad178de6c59</t>
-  </si>
-  <si>
-    <t>00a92b20-67ca-4fa6-9c38-f3b934d7ee68</t>
-  </si>
-  <si>
-    <t>733d532b-b48f-4142-8f56-61a035957cc0</t>
-  </si>
-  <si>
-    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
-  </si>
-  <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
-  </si>
-  <si>
-    <t>Sheet Missing</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
-  </si>
-  <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
-  </si>
-  <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
-  </si>
-  <si>
-    <t>591191c7-f693-5957-8734-ac87151ca981</t>
-  </si>
-  <si>
     <t>Excel workbook sheet 'Question_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
-  </si>
-  <si>
-    <t>071f8fe1-4899-5c71-9c86-7d7377661d45</t>
+    <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
+  </si>
+  <si>
+    <t>a3fe7098-8ae8-5612-81ac-cbe10780c19b</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>b2f9fd0b-01c6-41ba-8fe6-a7b469e06227</t>
+  </si>
+  <si>
+    <t>Mandatory field CONSENT is empty</t>
+  </si>
+  <si>
+    <t>CONSENT</t>
+  </si>
+  <si>
+    <t>Provide a value for CONSENT</t>
   </si>
 </sst>
 </file>
@@ -632,7 +599,7 @@
         <v>37</v>
       </c>
       <c r="O3">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="P3" t="s">
         <v>38</v>
@@ -682,22 +649,16 @@
         <v>45</v>
       </c>
       <c r="O4">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="P4" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>47</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>48</v>
-      </c>
-      <c r="T4" t="s">
-        <v>41</v>
-      </c>
-      <c r="U4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5">
@@ -714,37 +675,37 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="R5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="T5" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -761,34 +722,34 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
         <v>58</v>
       </c>
-      <c r="L6" t="s">
-        <v>59</v>
-      </c>
       <c r="M6" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="N6" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="Q6" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="R6" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="T6" t="s">
         <v>34</v>
@@ -808,37 +769,34 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="N7" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="R7" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="T7" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8">
@@ -855,34 +813,34 @@
         <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="I8" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="N8" t="s">
-        <v>71</v>
+        <v>30</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="Q8" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="R8" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="T8" t="s">
         <v>34</v>
@@ -911,28 +869,28 @@
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N9" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="O9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="P9" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="Q9" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="R9" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="T9" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10">
@@ -958,31 +916,28 @@
         <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="N10" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="O10">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="P10" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="Q10" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="R10" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="T10" t="s">
-        <v>41</v>
-      </c>
-      <c r="U10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -1008,28 +963,28 @@
         <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N11" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O11">
         <v>8</v>
       </c>
       <c r="P11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q11" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="R11" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T11" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
@@ -1055,7 +1010,7 @@
         <v>27</v>
       </c>
       <c r="L12" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="M12" t="s">
         <v>29</v>
@@ -1064,7 +1019,7 @@
         <v>30</v>
       </c>
       <c r="O12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P12" t="s">
         <v>31</v>
@@ -1102,28 +1057,28 @@
         <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="M13" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N13" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O13">
         <v>9</v>
       </c>
       <c r="P13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q13" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="R13" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T13" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
@@ -1149,7 +1104,7 @@
         <v>27</v>
       </c>
       <c r="L14" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="M14" t="s">
         <v>29</v>
@@ -1158,7 +1113,7 @@
         <v>30</v>
       </c>
       <c r="O14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P14" t="s">
         <v>31</v>
@@ -1196,28 +1151,28 @@
         <v>27</v>
       </c>
       <c r="L15" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="M15" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N15" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O15">
         <v>10</v>
       </c>
       <c r="P15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q15" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="R15" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T15" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
@@ -1243,7 +1198,7 @@
         <v>27</v>
       </c>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="M16" t="s">
         <v>29</v>
@@ -1252,7 +1207,7 @@
         <v>30</v>
       </c>
       <c r="O16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P16" t="s">
         <v>31</v>
@@ -1290,28 +1245,28 @@
         <v>27</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="M17" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N17" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O17">
         <v>18</v>
       </c>
       <c r="P17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q17" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="R17" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18">
@@ -1337,7 +1292,7 @@
         <v>27</v>
       </c>
       <c r="L18" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="M18" t="s">
         <v>29</v>
@@ -1346,7 +1301,7 @@
         <v>30</v>
       </c>
       <c r="O18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P18" t="s">
         <v>31</v>
@@ -1384,28 +1339,28 @@
         <v>27</v>
       </c>
       <c r="L19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="M19" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="N19" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O19">
         <v>19</v>
       </c>
       <c r="P19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="Q19" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="R19" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="T19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20">
@@ -1431,7 +1386,7 @@
         <v>27</v>
       </c>
       <c r="L20" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="M20" t="s">
         <v>29</v>
@@ -1440,7 +1395,7 @@
         <v>30</v>
       </c>
       <c r="O20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P20" t="s">
         <v>31</v>
@@ -1478,28 +1433,28 @@
         <v>27</v>
       </c>
       <c r="L21" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="M21" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="N21" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="O21">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P21" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="Q21" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="R21" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="T21" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22">
@@ -1525,7 +1480,7 @@
         <v>27</v>
       </c>
       <c r="L22" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="M22" t="s">
         <v>29</v>
@@ -1534,7 +1489,7 @@
         <v>30</v>
       </c>
       <c r="O22">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P22" t="s">
         <v>31</v>
@@ -1572,28 +1527,28 @@
         <v>27</v>
       </c>
       <c r="L23" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="M23" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="N23" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="O23">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="P23" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="Q23" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="R23" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="T23" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
@@ -1619,22 +1574,22 @@
         <v>27</v>
       </c>
       <c r="L24" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="M24" t="s">
         <v>29</v>
       </c>
       <c r="N24" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="O24">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P24" t="s">
         <v>31</v>
       </c>
       <c r="Q24" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="R24" t="s">
         <v>33</v>
@@ -1666,22 +1621,22 @@
         <v>27</v>
       </c>
       <c r="L25" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="M25" t="s">
         <v>29</v>
       </c>
       <c r="N25" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="O25">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P25" t="s">
         <v>31</v>
       </c>
       <c r="Q25" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="R25" t="s">
         <v>33</v>
@@ -1713,22 +1668,22 @@
         <v>27</v>
       </c>
       <c r="L26" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="M26" t="s">
         <v>29</v>
       </c>
       <c r="N26" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="O26">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="P26" t="s">
         <v>31</v>
       </c>
       <c r="Q26" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="R26" t="s">
         <v>33</v>
@@ -1760,22 +1715,22 @@
         <v>27</v>
       </c>
       <c r="L27" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="M27" t="s">
         <v>29</v>
       </c>
       <c r="N27" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O27">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P27" t="s">
         <v>31</v>
       </c>
       <c r="Q27" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R27" t="s">
         <v>33</v>
@@ -1807,22 +1762,22 @@
         <v>27</v>
       </c>
       <c r="L28" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="M28" t="s">
         <v>29</v>
       </c>
       <c r="N28" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O28">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
       </c>
       <c r="Q28" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R28" t="s">
         <v>33</v>
@@ -1854,22 +1809,22 @@
         <v>27</v>
       </c>
       <c r="L29" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="M29" t="s">
         <v>29</v>
       </c>
       <c r="N29" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O29">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="P29" t="s">
         <v>31</v>
       </c>
       <c r="Q29" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R29" t="s">
         <v>33</v>
@@ -1901,22 +1856,22 @@
         <v>27</v>
       </c>
       <c r="L30" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="M30" t="s">
         <v>29</v>
       </c>
       <c r="N30" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O30">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="P30" t="s">
         <v>31</v>
       </c>
       <c r="Q30" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R30" t="s">
         <v>33</v>
@@ -1948,22 +1903,22 @@
         <v>27</v>
       </c>
       <c r="L31" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="M31" t="s">
         <v>29</v>
       </c>
       <c r="N31" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O31">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="P31" t="s">
         <v>31</v>
       </c>
       <c r="Q31" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R31" t="s">
         <v>33</v>
@@ -1995,22 +1950,22 @@
         <v>27</v>
       </c>
       <c r="L32" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="M32" t="s">
         <v>29</v>
       </c>
       <c r="N32" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O32">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="P32" t="s">
         <v>31</v>
       </c>
       <c r="Q32" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R32" t="s">
         <v>33</v>
@@ -2042,22 +1997,22 @@
         <v>27</v>
       </c>
       <c r="L33" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="M33" t="s">
         <v>29</v>
       </c>
       <c r="N33" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O33">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="P33" t="s">
         <v>31</v>
       </c>
       <c r="Q33" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R33" t="s">
         <v>33</v>
@@ -2089,22 +2044,22 @@
         <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="M34" t="s">
         <v>29</v>
       </c>
       <c r="N34" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O34">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="P34" t="s">
         <v>31</v>
       </c>
       <c r="Q34" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R34" t="s">
         <v>33</v>
@@ -2136,22 +2091,22 @@
         <v>27</v>
       </c>
       <c r="L35" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="M35" t="s">
         <v>29</v>
       </c>
       <c r="N35" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O35">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="P35" t="s">
         <v>31</v>
       </c>
       <c r="Q35" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R35" t="s">
         <v>33</v>
@@ -2183,22 +2138,22 @@
         <v>27</v>
       </c>
       <c r="L36" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="M36" t="s">
         <v>29</v>
       </c>
       <c r="N36" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O36">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="P36" t="s">
         <v>31</v>
       </c>
       <c r="Q36" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R36" t="s">
         <v>33</v>
@@ -2230,22 +2185,22 @@
         <v>27</v>
       </c>
       <c r="L37" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="M37" t="s">
         <v>29</v>
       </c>
       <c r="N37" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O37">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="P37" t="s">
         <v>31</v>
       </c>
       <c r="Q37" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R37" t="s">
         <v>33</v>
@@ -2277,22 +2232,22 @@
         <v>27</v>
       </c>
       <c r="L38" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="M38" t="s">
         <v>29</v>
       </c>
       <c r="N38" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O38">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="P38" t="s">
         <v>31</v>
       </c>
       <c r="Q38" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R38" t="s">
         <v>33</v>
@@ -2324,22 +2279,22 @@
         <v>27</v>
       </c>
       <c r="L39" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="M39" t="s">
         <v>29</v>
       </c>
       <c r="N39" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O39">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="P39" t="s">
         <v>31</v>
       </c>
       <c r="Q39" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R39" t="s">
         <v>33</v>
@@ -2371,22 +2326,22 @@
         <v>27</v>
       </c>
       <c r="L40" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="M40" t="s">
         <v>29</v>
       </c>
       <c r="N40" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O40">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="P40" t="s">
         <v>31</v>
       </c>
       <c r="Q40" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R40" t="s">
         <v>33</v>
@@ -2418,22 +2373,22 @@
         <v>27</v>
       </c>
       <c r="L41" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="M41" t="s">
         <v>29</v>
       </c>
       <c r="N41" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O41">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="P41" t="s">
         <v>31</v>
       </c>
       <c r="Q41" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="R41" t="s">
         <v>33</v>
@@ -2456,37 +2411,25 @@
         <v>24</v>
       </c>
       <c r="H42" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="I42" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="J42" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="L42" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="M42" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="N42" t="s">
-        <v>95</v>
-      </c>
-      <c r="O42">
-        <v>27</v>
-      </c>
-      <c r="P42" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="Q42" t="s">
-        <v>96</v>
-      </c>
-      <c r="R42" t="s">
-        <v>33</v>
-      </c>
-      <c r="T42" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43">
@@ -2503,37 +2446,25 @@
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="I43" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="J43" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="L43" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="M43" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="N43" t="s">
-        <v>95</v>
-      </c>
-      <c r="O43">
-        <v>28</v>
-      </c>
-      <c r="P43" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="Q43" t="s">
-        <v>96</v>
-      </c>
-      <c r="R43" t="s">
-        <v>33</v>
-      </c>
-      <c r="T43" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44">
@@ -2550,37 +2481,25 @@
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>25</v>
+        <v>109</v>
       </c>
       <c r="I44" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="J44" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="L44" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M44" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="N44" t="s">
-        <v>95</v>
-      </c>
-      <c r="O44">
-        <v>29</v>
-      </c>
-      <c r="P44" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="Q44" t="s">
-        <v>96</v>
-      </c>
-      <c r="R44" t="s">
-        <v>33</v>
-      </c>
-      <c r="T44" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45">
@@ -2597,37 +2516,25 @@
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="I45" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="J45" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="L45" t="s">
+        <v>113</v>
+      </c>
+      <c r="M45" t="s">
+        <v>104</v>
+      </c>
+      <c r="N45" t="s">
         <v>114</v>
       </c>
-      <c r="M45" t="s">
-        <v>29</v>
-      </c>
-      <c r="N45" t="s">
-        <v>95</v>
-      </c>
-      <c r="O45">
-        <v>30</v>
-      </c>
-      <c r="P45" t="s">
-        <v>31</v>
-      </c>
       <c r="Q45" t="s">
-        <v>96</v>
-      </c>
-      <c r="R45" t="s">
-        <v>33</v>
-      </c>
-      <c r="T45" t="s">
-        <v>34</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46">
@@ -2647,22 +2554,22 @@
         <v>115</v>
       </c>
       <c r="I46" t="s">
+        <v>101</v>
+      </c>
+      <c r="J46" t="s">
+        <v>102</v>
+      </c>
+      <c r="L46" t="s">
         <v>116</v>
       </c>
-      <c r="J46" t="s">
+      <c r="M46" t="s">
+        <v>104</v>
+      </c>
+      <c r="N46" t="s">
         <v>117</v>
       </c>
-      <c r="L46" t="s">
-        <v>118</v>
-      </c>
-      <c r="M46" t="s">
-        <v>119</v>
-      </c>
-      <c r="N46" t="s">
-        <v>120</v>
-      </c>
       <c r="Q46" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47">
@@ -2679,130 +2586,31 @@
         <v>24</v>
       </c>
       <c r="H47" t="s">
+        <v>49</v>
+      </c>
+      <c r="I47" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" t="s">
+        <v>51</v>
+      </c>
+      <c r="L47" t="s">
+        <v>118</v>
+      </c>
+      <c r="M47" t="s">
+        <v>44</v>
+      </c>
+      <c r="N47" t="s">
+        <v>119</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47" t="s">
+        <v>120</v>
+      </c>
+      <c r="R47" t="s">
         <v>121</v>
-      </c>
-      <c r="I47" t="s">
-        <v>116</v>
-      </c>
-      <c r="J47" t="s">
-        <v>117</v>
-      </c>
-      <c r="L47" t="s">
-        <v>122</v>
-      </c>
-      <c r="M47" t="s">
-        <v>119</v>
-      </c>
-      <c r="N47" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>21</v>
-      </c>
-      <c r="B48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" t="s">
-        <v>23</v>
-      </c>
-      <c r="G48" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" t="s">
-        <v>124</v>
-      </c>
-      <c r="I48" t="s">
-        <v>116</v>
-      </c>
-      <c r="J48" t="s">
-        <v>117</v>
-      </c>
-      <c r="L48" t="s">
-        <v>125</v>
-      </c>
-      <c r="M48" t="s">
-        <v>119</v>
-      </c>
-      <c r="N48" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>21</v>
-      </c>
-      <c r="B49" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" t="s">
-        <v>23</v>
-      </c>
-      <c r="G49" t="s">
-        <v>24</v>
-      </c>
-      <c r="H49" t="s">
-        <v>127</v>
-      </c>
-      <c r="I49" t="s">
-        <v>116</v>
-      </c>
-      <c r="J49" t="s">
-        <v>117</v>
-      </c>
-      <c r="L49" t="s">
-        <v>128</v>
-      </c>
-      <c r="M49" t="s">
-        <v>119</v>
-      </c>
-      <c r="N49" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B50" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" t="s">
-        <v>130</v>
-      </c>
-      <c r="I50" t="s">
-        <v>116</v>
-      </c>
-      <c r="J50" t="s">
-        <v>117</v>
-      </c>
-      <c r="L50" t="s">
-        <v>131</v>
-      </c>
-      <c r="M50" t="s">
-        <v>119</v>
-      </c>
-      <c r="N50" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: updates and fixes for generating FHIR Bundle based on SHINNY IG specification #67 #69
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -81,247 +81,382 @@
     <t>7bab389e-54af-5a13-a39f-079abdc73a48</t>
   </si>
   <si>
-    <t>0.8.0</t>
+    <t>0.8.2</t>
   </si>
   <si>
     <t>Session 05269d28-15ae-5bd6-bd88-f949ccfa52d7 markdown diagnostics not provided (not completed?)</t>
   </si>
   <si>
+    <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/SCREENING_20240307.csv</t>
+  </si>
+  <si>
+    <t>screening_20240307</t>
+  </si>
+  <si>
+    <t>79455500-9915-4c11-936f-5840f098a231</t>
+  </si>
+  <si>
+    <t>Invalid Date</t>
+  </si>
+  <si>
+    <t>Invalid timestamp "01/27/02 15:42" found in RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>01/27/02 15:42</t>
+  </si>
+  <si>
+    <t>Please be sure to provide both a valid date and time (Format: YYYY-MM-DDTHH:MM:SS.000Z).</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>742748e5-f3f9-49ea-9dd5-227aa5383a65</t>
+  </si>
+  <si>
+    <t>Missing Mandatory Value</t>
+  </si>
+  <si>
+    <t>Mandatory field POTENTIAL_NEED_INDICATED is empty</t>
+  </si>
+  <si>
+    <t>POTENTIAL_NEED_INDICATED</t>
+  </si>
+  <si>
+    <t>Provide a value for POTENTIAL_NEED_INDICATED</t>
+  </si>
+  <si>
+    <t>REJECTION</t>
+  </si>
+  <si>
+    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/DEMOGRAPHIC_DATA_20240307.csv</t>
+  </si>
+  <si>
+    <t>admin_demographics_20240307</t>
+  </si>
+  <si>
+    <t>2d8b7e3d-27a7-49bb-9252-9b39c2065df4</t>
+  </si>
+  <si>
+    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" found in SEX_AT_BIRTH_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>SEX_AT_BIRTH_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
+  </si>
+  <si>
+    <t>af71efe7-b375-4057-a1cd-61eb5b6dada5</t>
+  </si>
+  <si>
+    <t>Invalid RACE CODE DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Invalid RACE CODE DESCRIPTION "Coquille" found in RACE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>RACE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Coquille</t>
+  </si>
+  <si>
+    <t>Validate RACE CODE DESCRIPTION with race reference data</t>
+  </si>
+  <si>
+    <t>d4b74416-6fdd-4f27-b2d9-794c792bfd6a</t>
+  </si>
+  <si>
+    <t>2108ec21-561f-465b-84fa-64ef33a441ad</t>
+  </si>
+  <si>
+    <t>667cc0df-1825-4e00-9d03-d916e84e89c1</t>
+  </si>
+  <si>
+    <t>cab24d3a-a25a-4635-927e-35c4face85bb</t>
+  </si>
+  <si>
+    <t>Invalid Value</t>
+  </si>
+  <si>
+    <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA')</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Use only allowed values 'Yes','No','NA' in POTENTIAL_NEED_INDICATED</t>
+  </si>
+  <si>
+    <t>ac4e23cc-b7ee-4dbe-8731-efdb07398dba</t>
+  </si>
+  <si>
+    <t>753a48ee-23e2-4212-85fb-4c3eaa376005</t>
+  </si>
+  <si>
+    <t>1af5c88b-638e-402c-86d3-61f045a53daa</t>
+  </si>
+  <si>
+    <t>cbd53a72-c77e-4027-a3d7-66283e2dcedb</t>
+  </si>
+  <si>
+    <t>879099c8-671b-494d-847c-6dc2c5a5b33c</t>
+  </si>
+  <si>
+    <t>aad9ad7f-5cfc-426f-b655-536c4849193d</t>
+  </si>
+  <si>
+    <t>3bf5593e-776b-43dc-b765-55b9d1e9bc2a</t>
+  </si>
+  <si>
+    <t>e28895f8-8fdb-4d8e-a66a-fd85b19d8bff</t>
+  </si>
+  <si>
+    <t>f310e1a3-ed3b-4697-ac7b-cb1c6c1d98c1</t>
+  </si>
+  <si>
+    <t>ba23d574-a236-4018-8d46-9b09fa6c0288</t>
+  </si>
+  <si>
+    <t>fae38e27-c700-400c-83cc-a4ac40244493</t>
+  </si>
+  <si>
+    <t>5eab58b6-7d33-4e09-816f-20b719bd61d5</t>
+  </si>
+  <si>
+    <t>0ff7b2db-6998-47eb-bd2d-a72f98766d33</t>
+  </si>
+  <si>
+    <t>8b5cf674-6a0a-4fd7-96e7-c0e640801894</t>
+  </si>
+  <si>
+    <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>03/05/94 13:08</t>
+  </si>
+  <si>
+    <t>a9d6fa36-725a-425d-b2be-16fdbed731ee</t>
+  </si>
+  <si>
+    <t>52844900-2e98-4624-a79e-fd6729735b4e</t>
+  </si>
+  <si>
+    <t>0cd2d3b4-598c-45af-be14-869b03ddc029</t>
+  </si>
+  <si>
+    <t>7df69de1-5c35-4463-a713-cdb4ee2cd4c1</t>
+  </si>
+  <si>
+    <t>e90e5431-7721-461e-9774-515a02c0b325</t>
+  </si>
+  <si>
+    <t>a8d8737f-7ddf-4f5c-97ed-f9dd3aeb6a8c</t>
+  </si>
+  <si>
+    <t>88ceb88f-f851-4e51-97e9-42622f1c98e6</t>
+  </si>
+  <si>
+    <t>0aaef67b-5dfc-47b9-8bf9-b0dd0786fc62</t>
+  </si>
+  <si>
+    <t>6a008556-e84c-4f8d-811e-6d6f5d7a4aae</t>
+  </si>
+  <si>
+    <t>9add894b-3758-4b2f-9c83-5d2be4368967</t>
+  </si>
+  <si>
+    <t>d38eaf2b-6ad5-427c-8e9d-7318b7088393</t>
+  </si>
+  <si>
+    <t>eb1ac4f9-ff60-4517-a9bd-1242fcf800d5</t>
+  </si>
+  <si>
+    <t>b7a098dc-245b-4c52-b493-ae1c2fe97d36</t>
+  </si>
+  <si>
+    <t>c7883f8d-c753-45ea-9d4f-431b9316d8aa</t>
+  </si>
+  <si>
+    <t>0c994e63-ed24-44c0-85d8-8eacf5fd3a6a</t>
+  </si>
+  <si>
+    <t>6cfea61e-c2c0-49b0-8e4b-3292b43501c6</t>
+  </si>
+  <si>
+    <t>7c3b44ee-ffb2-4bae-8bed-4f9787fbe8c9</t>
+  </si>
+  <si>
+    <t>7fa2fc5a-3d96-4093-9c96-3eb323df7376</t>
+  </si>
+  <si>
+    <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>Sheet Missing</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+  </si>
+  <si>
     <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
   </si>
   <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/SCREENING_20240307.csv</t>
-  </si>
-  <si>
-    <t>screening_20240307</t>
-  </si>
-  <si>
-    <t>f6947fba-efb6-413b-a794-b37a10d4b6fe</t>
-  </si>
-  <si>
-    <t>Invalid Date</t>
-  </si>
-  <si>
-    <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
-  </si>
-  <si>
-    <t>RECORDED_TIME</t>
-  </si>
-  <si>
-    <t>03/05/94 13:08</t>
-  </si>
-  <si>
-    <t>Please be sure to provide both a valid date and time (Format: YYYY-MM-DDTHH:MM:SS.000Z).</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>034bf5e2-9294-466a-b14f-6994cb150368</t>
-  </si>
-  <si>
-    <t>Missing Mandatory Value</t>
-  </si>
-  <si>
-    <t>Mandatory field POTENTIAL_NEED_INDICATED is empty</t>
-  </si>
-  <si>
-    <t>POTENTIAL_NEED_INDICATED</t>
-  </si>
-  <si>
-    <t>Provide a value for POTENTIAL_NEED_INDICATED</t>
-  </si>
-  <si>
-    <t>REJECTION</t>
-  </si>
-  <si>
-    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/DEMOGRAPHIC_DATA_20240307.csv</t>
-  </si>
-  <si>
-    <t>admin_demographics_20240307</t>
-  </si>
-  <si>
-    <t>26f09f30-078a-48b5-8946-6479a7331e4d</t>
-  </si>
-  <si>
-    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" found in SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
-  </si>
-  <si>
-    <t>f5da1c86-67d5-4787-ad8f-fe543ddf4a23</t>
-  </si>
-  <si>
-    <t>Invalid RACE CODE DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Invalid RACE CODE DESCRIPTION "Coquille" found in RACE_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>RACE_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Coquille</t>
-  </si>
-  <si>
-    <t>Validate RACE CODE DESCRIPTION with race reference data</t>
-  </si>
-  <si>
-    <t>30e0b720-1468-4220-9228-f7bffe885b0b</t>
-  </si>
-  <si>
-    <t>ddc72b43-0266-4b35-a793-7263b1206e17</t>
-  </si>
-  <si>
-    <t>2bcd30e2-6b8b-4d0a-bd7d-7e01ef39ffbf</t>
-  </si>
-  <si>
-    <t>286fa4e7-58cf-4834-8842-0b3541d5b5df</t>
-  </si>
-  <si>
-    <t>Invalid Value</t>
-  </si>
-  <si>
-    <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA')</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Use only allowed values 'Yes','No','NA' in POTENTIAL_NEED_INDICATED</t>
-  </si>
-  <si>
-    <t>6c9efe99-dbd4-4b45-b261-e0beef238916</t>
-  </si>
-  <si>
-    <t>5cb9f0c9-0f14-4077-9b6b-2abef60d1f42</t>
-  </si>
-  <si>
-    <t>a4c75b20-0161-4d7f-aa21-0eb5e279f5e2</t>
-  </si>
-  <si>
-    <t>f3293c17-6e1b-4dff-8d06-b6bf5973a5d3</t>
-  </si>
-  <si>
-    <t>c89fa242-36ea-4bec-a2e5-aa30eed157c0</t>
-  </si>
-  <si>
-    <t>9d1edf10-2987-4acc-8188-cf77ac17e24d</t>
-  </si>
-  <si>
-    <t>16cfe7be-b9d5-41bb-b665-d8c0ba23a5f4</t>
-  </si>
-  <si>
-    <t>72d83e16-1ec2-497b-9ad3-e3170dde7c4f</t>
-  </si>
-  <si>
-    <t>71f89f84-f9c9-45aa-bc4d-70a906cbc1fa</t>
-  </si>
-  <si>
-    <t>3f201b0e-0719-4b5c-bb30-38f8bda4493a</t>
-  </si>
-  <si>
-    <t>ca0fda07-54e3-4569-b08a-80382588bc21</t>
-  </si>
-  <si>
-    <t>d828ce2d-097e-467d-9e52-dd3fd1b324c9</t>
-  </si>
-  <si>
-    <t>708bd762-68c8-4e02-af19-dc0ca7b9d00e</t>
-  </si>
-  <si>
-    <t>491a785b-86d0-460e-847f-ba7684144766</t>
-  </si>
-  <si>
-    <t>374ac1da-ad47-4bac-9fe2-bb69ffd62dc6</t>
-  </si>
-  <si>
-    <t>817533d7-56ad-411f-b3ca-550834003125</t>
-  </si>
-  <si>
-    <t>8ef5dd35-afd7-45f2-b112-479d046f48fa</t>
-  </si>
-  <si>
-    <t>dccb1c29-7117-48ab-8029-cf323d5947c9</t>
-  </si>
-  <si>
-    <t>41115e57-157b-42ba-8a82-e9c11443bd0b</t>
-  </si>
-  <si>
-    <t>bf4e670e-c661-47ea-87ab-5efdb6e69f0e</t>
-  </si>
-  <si>
-    <t>5b556c00-78cb-4c93-88cb-666955f2c40f</t>
+    <t>Excel workbook sheet 'Screening' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
+  </si>
+  <si>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
+  </si>
+  <si>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
   </si>
   <si>
     <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
   </si>
   <si>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Question_Reference' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+  </si>
+  <si>
+    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Answer_Reference' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
+  </si>
+  <si>
+    <t>99e72a60-96ab-5ef1-a3af-3e7759777664</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
+  </si>
+  <si>
+    <t>e36daa69-3c63-5384-b6a7-03fa3b00641d</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>89f7ec04-277a-5799-afaa-a70d0f2a8ed5</t>
+  </si>
+  <si>
+    <t>c60cf3db-b1bf-5103-b278-b0c128ce924a</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>b2a7c7e8-5ffe-5f28-8112-4eb7abb6397f</t>
+  </si>
+  <si>
+    <t>b10e248d-8c94-59ec-83fc-a1249dd3b111</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>5222b730-9add-5b52-b0c9-6f2506b0af9d</t>
+  </si>
+  <si>
+    <t>fa7874f6-f848-572b-a9ab-9db4c8d5e959</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Question_Reference' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>c302047e-21cf-5059-a32c-e81a9bd3a9b9</t>
+  </si>
+  <si>
+    <t>3252fee6-3a9a-5f4c-81c6-739201046d79</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Answer_Reference' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>78d6a904-035e-54ae-8ac2-ca5cdf3f75f7</t>
+  </si>
+  <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
   </si>
   <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
-  </si>
-  <si>
-    <t>Sheet Missing</t>
+    <t>9860873a-c387-5d98-9930-4ff296eb7192</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
-  </si>
-  <si>
-    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+    <t>d5d6e25d-81b4-5f98-8b91-ea2dbc155a9c</t>
+  </si>
+  <si>
+    <t>46171763-bd21-57a8-a403-0785f72643cf</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>591191c7-f693-5957-8734-ac87151ca981</t>
-  </si>
-  <si>
-    <t>3b4eb0e5-6239-537a-8e67-e50e172e72a2</t>
+    <t>4971a2f5-06a3-5898-823d-364145d3b9a5</t>
+  </si>
+  <si>
+    <t>c2c0cbca-70cb-54f6-9dc7-66b47c4f3157</t>
   </si>
   <si>
     <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>071f8fe1-4899-5c71-9c86-7d7377661d45</t>
-  </si>
-  <si>
-    <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
+    <t>8640a4b5-53ef-506e-bcde-83f00315d4b2</t>
+  </si>
+  <si>
+    <t>544998d3-58c5-5f65-9dc8-9f998508495f</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Question_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
-  </si>
-  <si>
-    <t>a3fe7098-8ae8-5612-81ac-cbe10780c19b</t>
+    <t>0adb81bc-3df2-5f86-99cc-2d20e1dd5efd</t>
+  </si>
+  <si>
+    <t>10d0290c-b2eb-581e-b627-b5b8fcbb830f</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>849cfea8-7c12-4092-a122-0d57a5d4a451</t>
+    <t>bed34595-89ee-4f43-8c4e-0dae5f1dc086</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>
@@ -507,7 +642,7 @@
         <v>30</v>
       </c>
       <c r="O2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="P2" t="s">
         <v>31</v>
@@ -692,7 +827,7 @@
         <v>30</v>
       </c>
       <c r="O6">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="P6" t="s">
         <v>31</v>
@@ -783,7 +918,7 @@
         <v>30</v>
       </c>
       <c r="O8">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="P8" t="s">
         <v>31</v>
@@ -877,7 +1012,7 @@
         <v>30</v>
       </c>
       <c r="O10">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="P10" t="s">
         <v>31</v>
@@ -971,7 +1106,7 @@
         <v>30</v>
       </c>
       <c r="O12">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P12" t="s">
         <v>31</v>
@@ -1065,7 +1200,7 @@
         <v>30</v>
       </c>
       <c r="O14">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="P14" t="s">
         <v>31</v>
@@ -1159,7 +1294,7 @@
         <v>30</v>
       </c>
       <c r="O16">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P16" t="s">
         <v>31</v>
@@ -1253,7 +1388,7 @@
         <v>30</v>
       </c>
       <c r="O18">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="P18" t="s">
         <v>31</v>
@@ -1347,7 +1482,7 @@
         <v>30</v>
       </c>
       <c r="O20">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="P20" t="s">
         <v>31</v>
@@ -1394,7 +1529,7 @@
         <v>30</v>
       </c>
       <c r="O21">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="P21" t="s">
         <v>31</v>
@@ -1441,7 +1576,7 @@
         <v>30</v>
       </c>
       <c r="O22">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="P22" t="s">
         <v>31</v>
@@ -1485,16 +1620,16 @@
         <v>29</v>
       </c>
       <c r="N23" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O23">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="P23" t="s">
         <v>31</v>
       </c>
       <c r="Q23" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R23" t="s">
         <v>33</v>
@@ -1526,22 +1661,22 @@
         <v>27</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M24" t="s">
         <v>29</v>
       </c>
       <c r="N24" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O24">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="P24" t="s">
         <v>31</v>
       </c>
       <c r="Q24" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R24" t="s">
         <v>33</v>
@@ -1573,22 +1708,22 @@
         <v>27</v>
       </c>
       <c r="L25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M25" t="s">
         <v>29</v>
       </c>
       <c r="N25" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O25">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="P25" t="s">
         <v>31</v>
       </c>
       <c r="Q25" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R25" t="s">
         <v>33</v>
@@ -1620,22 +1755,22 @@
         <v>27</v>
       </c>
       <c r="L26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M26" t="s">
         <v>29</v>
       </c>
       <c r="N26" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O26">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="P26" t="s">
         <v>31</v>
       </c>
       <c r="Q26" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R26" t="s">
         <v>33</v>
@@ -1667,22 +1802,22 @@
         <v>27</v>
       </c>
       <c r="L27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="M27" t="s">
         <v>29</v>
       </c>
       <c r="N27" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O27">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="P27" t="s">
         <v>31</v>
       </c>
       <c r="Q27" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R27" t="s">
         <v>33</v>
@@ -1714,22 +1849,22 @@
         <v>27</v>
       </c>
       <c r="L28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="M28" t="s">
         <v>29</v>
       </c>
       <c r="N28" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O28">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
       </c>
       <c r="Q28" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R28" t="s">
         <v>33</v>
@@ -1761,22 +1896,22 @@
         <v>27</v>
       </c>
       <c r="L29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M29" t="s">
         <v>29</v>
       </c>
       <c r="N29" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O29">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="P29" t="s">
         <v>31</v>
       </c>
       <c r="Q29" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R29" t="s">
         <v>33</v>
@@ -1808,22 +1943,22 @@
         <v>27</v>
       </c>
       <c r="L30" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M30" t="s">
         <v>29</v>
       </c>
       <c r="N30" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="O30">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="P30" t="s">
         <v>31</v>
       </c>
       <c r="Q30" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="R30" t="s">
         <v>33</v>
@@ -1846,25 +1981,37 @@
         <v>24</v>
       </c>
       <c r="H31" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="I31" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="J31" t="s">
+        <v>27</v>
+      </c>
+      <c r="L31" t="s">
         <v>87</v>
       </c>
-      <c r="L31" t="s">
-        <v>88</v>
-      </c>
       <c r="M31" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="N31" t="s">
-        <v>90</v>
+        <v>78</v>
+      </c>
+      <c r="O31">
+        <v>20</v>
+      </c>
+      <c r="P31" t="s">
+        <v>31</v>
       </c>
       <c r="Q31" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="R31" t="s">
+        <v>33</v>
+      </c>
+      <c r="T31" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32">
@@ -1881,25 +2028,37 @@
         <v>24</v>
       </c>
       <c r="H32" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="I32" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="J32" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="L32" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M32" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="N32" t="s">
-        <v>93</v>
+        <v>78</v>
+      </c>
+      <c r="O32">
+        <v>21</v>
+      </c>
+      <c r="P32" t="s">
+        <v>31</v>
       </c>
       <c r="Q32" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="R32" t="s">
+        <v>33</v>
+      </c>
+      <c r="T32" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33">
@@ -1916,25 +2075,37 @@
         <v>24</v>
       </c>
       <c r="H33" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="I33" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="J33" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="L33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="M33" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="N33" t="s">
-        <v>96</v>
+        <v>78</v>
+      </c>
+      <c r="O33">
+        <v>22</v>
+      </c>
+      <c r="P33" t="s">
+        <v>31</v>
       </c>
       <c r="Q33" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="R33" t="s">
+        <v>33</v>
+      </c>
+      <c r="T33" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34">
@@ -1951,25 +2122,37 @@
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="I34" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="J34" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="M34" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="N34" t="s">
-        <v>99</v>
+        <v>78</v>
+      </c>
+      <c r="O34">
+        <v>23</v>
+      </c>
+      <c r="P34" t="s">
+        <v>31</v>
       </c>
       <c r="Q34" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="R34" t="s">
+        <v>33</v>
+      </c>
+      <c r="T34" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35">
@@ -1986,25 +2169,37 @@
         <v>24</v>
       </c>
       <c r="H35" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="I35" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="J35" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="L35" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="M35" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="N35" t="s">
-        <v>102</v>
+        <v>78</v>
+      </c>
+      <c r="O35">
+        <v>24</v>
+      </c>
+      <c r="P35" t="s">
+        <v>31</v>
       </c>
       <c r="Q35" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="R35" t="s">
+        <v>33</v>
+      </c>
+      <c r="T35" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36">
@@ -2021,31 +2216,838 @@
         <v>24</v>
       </c>
       <c r="H36" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J36" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" t="s">
+        <v>92</v>
+      </c>
+      <c r="M36" t="s">
+        <v>29</v>
+      </c>
+      <c r="N36" t="s">
+        <v>78</v>
+      </c>
+      <c r="O36">
+        <v>25</v>
+      </c>
+      <c r="P36" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>79</v>
+      </c>
+      <c r="R36" t="s">
+        <v>33</v>
+      </c>
+      <c r="T36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="G37" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" t="s">
+        <v>93</v>
+      </c>
+      <c r="M37" t="s">
+        <v>29</v>
+      </c>
+      <c r="N37" t="s">
+        <v>78</v>
+      </c>
+      <c r="O37">
+        <v>26</v>
+      </c>
+      <c r="P37" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>79</v>
+      </c>
+      <c r="R37" t="s">
+        <v>33</v>
+      </c>
+      <c r="T37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="G38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" t="s">
+        <v>27</v>
+      </c>
+      <c r="L38" t="s">
+        <v>94</v>
+      </c>
+      <c r="M38" t="s">
+        <v>29</v>
+      </c>
+      <c r="N38" t="s">
+        <v>78</v>
+      </c>
+      <c r="O38">
+        <v>27</v>
+      </c>
+      <c r="P38" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>79</v>
+      </c>
+      <c r="R38" t="s">
+        <v>33</v>
+      </c>
+      <c r="T38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
+        <v>25</v>
+      </c>
+      <c r="I39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" t="s">
+        <v>27</v>
+      </c>
+      <c r="L39" t="s">
+        <v>95</v>
+      </c>
+      <c r="M39" t="s">
+        <v>29</v>
+      </c>
+      <c r="N39" t="s">
+        <v>78</v>
+      </c>
+      <c r="O39">
+        <v>28</v>
+      </c>
+      <c r="P39" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>79</v>
+      </c>
+      <c r="R39" t="s">
+        <v>33</v>
+      </c>
+      <c r="T39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" t="s">
+        <v>25</v>
+      </c>
+      <c r="I40" t="s">
+        <v>26</v>
+      </c>
+      <c r="J40" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" t="s">
+        <v>96</v>
+      </c>
+      <c r="M40" t="s">
+        <v>29</v>
+      </c>
+      <c r="N40" t="s">
+        <v>78</v>
+      </c>
+      <c r="O40">
+        <v>29</v>
+      </c>
+      <c r="P40" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>79</v>
+      </c>
+      <c r="R40" t="s">
+        <v>33</v>
+      </c>
+      <c r="T40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" t="s">
+        <v>97</v>
+      </c>
+      <c r="M41" t="s">
+        <v>29</v>
+      </c>
+      <c r="N41" t="s">
+        <v>78</v>
+      </c>
+      <c r="O41">
+        <v>30</v>
+      </c>
+      <c r="P41" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>79</v>
+      </c>
+      <c r="R41" t="s">
+        <v>33</v>
+      </c>
+      <c r="T41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42" t="s">
+        <v>99</v>
+      </c>
+      <c r="J42" t="s">
+        <v>100</v>
+      </c>
+      <c r="L42" t="s">
+        <v>101</v>
+      </c>
+      <c r="M42" t="s">
+        <v>102</v>
+      </c>
+      <c r="N42" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" t="s">
+        <v>104</v>
+      </c>
+      <c r="I43" t="s">
+        <v>99</v>
+      </c>
+      <c r="J43" t="s">
+        <v>100</v>
+      </c>
+      <c r="L43" t="s">
+        <v>105</v>
+      </c>
+      <c r="M43" t="s">
+        <v>102</v>
+      </c>
+      <c r="N43" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44" t="s">
+        <v>107</v>
+      </c>
+      <c r="I44" t="s">
+        <v>99</v>
+      </c>
+      <c r="J44" t="s">
+        <v>100</v>
+      </c>
+      <c r="L44" t="s">
+        <v>108</v>
+      </c>
+      <c r="M44" t="s">
+        <v>102</v>
+      </c>
+      <c r="N44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" t="s">
+        <v>24</v>
+      </c>
+      <c r="H45" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" t="s">
+        <v>99</v>
+      </c>
+      <c r="J45" t="s">
+        <v>100</v>
+      </c>
+      <c r="L45" t="s">
+        <v>111</v>
+      </c>
+      <c r="M45" t="s">
+        <v>102</v>
+      </c>
+      <c r="N45" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" t="s">
+        <v>24</v>
+      </c>
+      <c r="H46" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" t="s">
+        <v>99</v>
+      </c>
+      <c r="J46" t="s">
+        <v>100</v>
+      </c>
+      <c r="L46" t="s">
+        <v>114</v>
+      </c>
+      <c r="M46" t="s">
+        <v>102</v>
+      </c>
+      <c r="N46" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H47" t="s">
+        <v>116</v>
+      </c>
+      <c r="I47" t="s">
+        <v>117</v>
+      </c>
+      <c r="J47" t="s">
+        <v>100</v>
+      </c>
+      <c r="L47" t="s">
+        <v>118</v>
+      </c>
+      <c r="M47" t="s">
+        <v>102</v>
+      </c>
+      <c r="N47" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" t="s">
+        <v>24</v>
+      </c>
+      <c r="H48" t="s">
+        <v>120</v>
+      </c>
+      <c r="I48" t="s">
+        <v>117</v>
+      </c>
+      <c r="J48" t="s">
+        <v>100</v>
+      </c>
+      <c r="L48" t="s">
+        <v>121</v>
+      </c>
+      <c r="M48" t="s">
+        <v>102</v>
+      </c>
+      <c r="N48" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" t="s">
+        <v>24</v>
+      </c>
+      <c r="H49" t="s">
+        <v>123</v>
+      </c>
+      <c r="I49" t="s">
+        <v>117</v>
+      </c>
+      <c r="J49" t="s">
+        <v>100</v>
+      </c>
+      <c r="L49" t="s">
+        <v>124</v>
+      </c>
+      <c r="M49" t="s">
+        <v>102</v>
+      </c>
+      <c r="N49" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>24</v>
+      </c>
+      <c r="H50" t="s">
+        <v>126</v>
+      </c>
+      <c r="I50" t="s">
+        <v>117</v>
+      </c>
+      <c r="J50" t="s">
+        <v>100</v>
+      </c>
+      <c r="L50" t="s">
+        <v>127</v>
+      </c>
+      <c r="M50" t="s">
+        <v>102</v>
+      </c>
+      <c r="N50" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" t="s">
+        <v>129</v>
+      </c>
+      <c r="I51" t="s">
+        <v>117</v>
+      </c>
+      <c r="J51" t="s">
+        <v>100</v>
+      </c>
+      <c r="L51" t="s">
+        <v>130</v>
+      </c>
+      <c r="M51" t="s">
+        <v>102</v>
+      </c>
+      <c r="N51" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G52" t="s">
+        <v>24</v>
+      </c>
+      <c r="H52" t="s">
+        <v>132</v>
+      </c>
+      <c r="I52" t="s">
+        <v>133</v>
+      </c>
+      <c r="J52" t="s">
+        <v>100</v>
+      </c>
+      <c r="L52" t="s">
+        <v>134</v>
+      </c>
+      <c r="M52" t="s">
+        <v>102</v>
+      </c>
+      <c r="N52" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G53" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" t="s">
+        <v>136</v>
+      </c>
+      <c r="I53" t="s">
+        <v>133</v>
+      </c>
+      <c r="J53" t="s">
+        <v>100</v>
+      </c>
+      <c r="L53" t="s">
+        <v>137</v>
+      </c>
+      <c r="M53" t="s">
+        <v>102</v>
+      </c>
+      <c r="N53" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="G54" t="s">
+        <v>24</v>
+      </c>
+      <c r="H54" t="s">
+        <v>139</v>
+      </c>
+      <c r="I54" t="s">
+        <v>133</v>
+      </c>
+      <c r="J54" t="s">
+        <v>100</v>
+      </c>
+      <c r="L54" t="s">
+        <v>140</v>
+      </c>
+      <c r="M54" t="s">
+        <v>102</v>
+      </c>
+      <c r="N54" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="G55" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" t="s">
+        <v>142</v>
+      </c>
+      <c r="I55" t="s">
+        <v>133</v>
+      </c>
+      <c r="J55" t="s">
+        <v>100</v>
+      </c>
+      <c r="L55" t="s">
+        <v>143</v>
+      </c>
+      <c r="M55" t="s">
+        <v>102</v>
+      </c>
+      <c r="N55" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>23</v>
+      </c>
+      <c r="G56" t="s">
+        <v>24</v>
+      </c>
+      <c r="H56" t="s">
+        <v>145</v>
+      </c>
+      <c r="I56" t="s">
+        <v>133</v>
+      </c>
+      <c r="J56" t="s">
+        <v>100</v>
+      </c>
+      <c r="L56" t="s">
+        <v>146</v>
+      </c>
+      <c r="M56" t="s">
+        <v>102</v>
+      </c>
+      <c r="N56" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" t="s">
+        <v>23</v>
+      </c>
+      <c r="G57" t="s">
+        <v>24</v>
+      </c>
+      <c r="H57" t="s">
         <v>41</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I57" t="s">
         <v>42</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J57" t="s">
         <v>43</v>
       </c>
-      <c r="L36" t="s">
-        <v>103</v>
-      </c>
-      <c r="M36" t="s">
+      <c r="L57" t="s">
+        <v>148</v>
+      </c>
+      <c r="M57" t="s">
         <v>36</v>
       </c>
-      <c r="N36" t="s">
-        <v>104</v>
-      </c>
-      <c r="O36">
+      <c r="N57" t="s">
+        <v>149</v>
+      </c>
+      <c r="O57">
         <v>1</v>
       </c>
-      <c r="P36" t="s">
-        <v>105</v>
-      </c>
-      <c r="R36" t="s">
-        <v>106</v>
+      <c r="P57" t="s">
+        <v>150</v>
+      </c>
+      <c r="R57" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add data validation #66
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="228">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -96,31 +96,124 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>79455500-9915-4c11-936f-5840f098a231</t>
+    <t>71deb9f6-3bcf-4690-b6fb-61b850c19d94</t>
+  </si>
+  <si>
+    <t>Missing Mandatory Value</t>
+  </si>
+  <si>
+    <t>Mandatory field ENCOUNTER_CLASS_CODE is empty</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_CLASS_CODE</t>
+  </si>
+  <si>
+    <t>Provide a value for ENCOUNTER_CLASS_CODE</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>Resolved By QE/QCS</t>
+  </si>
+  <si>
+    <t>cba6f08d-acfa-4f40-8a47-3562f75b7bb5</t>
+  </si>
+  <si>
+    <t>Combination Not Matching</t>
+  </si>
+  <si>
+    <t>Invalid value "inpatient non-acute" found in ENCOUNTER_CLASS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_CLASS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>inpatient non-acute</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_CLASS_CODE_DESCRIPTION "inpatient non-acute" of ENCOUNTER_CLASS_CODE "ACUTE" is not matching with the ENCOUNTER_CLASS_CODE_DESCRIPTION of ENCOUNTER_CLASS_CODE in reference data</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>cb44aab8-103c-4147-b881-6e3adb9c73be</t>
+  </si>
+  <si>
+    <t>Mandatory field ENCOUNTER_STATUS_CODE is empty</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>Provide a value for ENCOUNTER_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>04beb0b1-7d98-41f8-adba-34dffe720dc9</t>
+  </si>
+  <si>
+    <t>Invalid value "Unknown" found in ENCOUNTER_STATUS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_STATUS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_STATUS_CODE_DESCRIPTION "Unknown" of ENCOUNTER_STATUS_CODE "entered-in-error" is not matching with the ENCOUNTER_STATUS_CODE_DESCRIPTION of ENCOUNTER_STATUS_CODE in reference data</t>
+  </si>
+  <si>
+    <t>04640aa8-0218-466f-949f-5523d3d98a7c</t>
+  </si>
+  <si>
+    <t>Invalid value "185317003" found in ENCOUNTER_TYPE_CODE</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_TYPE_CODE</t>
+  </si>
+  <si>
+    <t>185317003</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_TYPE_CODE "185317003" of ENCOUNTER_TYPE_CODE_DESCRIPTION "History taking, self-administered, questionnaire" is not matching with the ENCOUNTER_TYPE_CODE of ENCOUNTER_TYPE_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>df37a164-3665-46fe-83ef-a0d614b35db3</t>
+  </si>
+  <si>
+    <t>Invalid value "In-person encounter" found in ENCOUNTER_TYPE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_TYPE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>In-person encounter</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_TYPE_CODE_DESCRIPTION "In-person encounter" of ENCOUNTER_TYPE_CODE "32166003" is not matching with the ENCOUNTER_TYPE_CODE_DESCRIPTION of ENCOUNTER_TYPE_CODE in reference data</t>
+  </si>
+  <si>
+    <t>60616f01-9491-4f0b-a38e-e7b69bf5b20b</t>
   </si>
   <si>
     <t>Invalid Date</t>
   </si>
   <si>
-    <t>Invalid timestamp "01/27/02 15:42" found in RECORDED_TIME</t>
+    <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
   </si>
   <si>
     <t>RECORDED_TIME</t>
   </si>
   <si>
-    <t>01/27/02 15:42</t>
-  </si>
-  <si>
-    <t>Please be sure to provide both a valid date and time (Format: YYYY-MM-DDTHH:MM:SS.000Z).</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>742748e5-f3f9-49ea-9dd5-227aa5383a65</t>
-  </si>
-  <si>
-    <t>Missing Mandatory Value</t>
+    <t>03/05/94 13:08</t>
+  </si>
+  <si>
+    <t>Please be sure to provide both a valid date and time.</t>
+  </si>
+  <si>
+    <t>c31be6eb-6233-4b86-b203-48bd076d8ad0</t>
   </si>
   <si>
     <t>Mandatory field POTENTIAL_NEED_INDICATED is empty</t>
@@ -144,7 +237,22 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>2d8b7e3d-27a7-49bb-9252-9b39c2065df4</t>
+    <t>d387023f-c351-4931-86ab-e1869b06a346</t>
+  </si>
+  <si>
+    <t>Invalid value "UNK" found in SEX_AT_BIRTH_CODE</t>
+  </si>
+  <si>
+    <t>SEX_AT_BIRTH_CODE</t>
+  </si>
+  <si>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t>The SEX_AT_BIRTH_CODE "UNK" of SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" is not matching with the SEX_AT_BIRTH_CODE of SEX_AT_BIRTH_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>0cfd0b0f-ac89-4afa-90e4-d0fe6227be9a</t>
   </si>
   <si>
     <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
@@ -162,7 +270,22 @@
     <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
   </si>
   <si>
-    <t>af71efe7-b375-4057-a1cd-61eb5b6dada5</t>
+    <t>bbb9fdc3-e68b-4dc1-b49b-db6d484d1f68</t>
+  </si>
+  <si>
+    <t>Invalid value "1142-9" found in RACE_CODE</t>
+  </si>
+  <si>
+    <t>RACE_CODE</t>
+  </si>
+  <si>
+    <t>1142-9</t>
+  </si>
+  <si>
+    <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>3bc6f543-8444-4e59-8c91-2b60fe6e58c5</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -180,16 +303,106 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>d4b74416-6fdd-4f27-b2d9-794c792bfd6a</t>
-  </si>
-  <si>
-    <t>2108ec21-561f-465b-84fa-64ef33a441ad</t>
-  </si>
-  <si>
-    <t>667cc0df-1825-4e00-9d03-d916e84e89c1</t>
-  </si>
-  <si>
-    <t>cab24d3a-a25a-4635-927e-35c4face85bb</t>
+    <t>5d1126c4-b72a-4b1b-b62d-deeda85f41dd</t>
+  </si>
+  <si>
+    <t>f3082526-a5de-415c-8f79-6bcd2dc6456a</t>
+  </si>
+  <si>
+    <t>Invalid value "pre-admission" found in ENCOUNTER_CLASS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>pre-admission</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_CLASS_CODE_DESCRIPTION "pre-admission" of ENCOUNTER_CLASS_CODE "IMP" is not matching with the ENCOUNTER_CLASS_CODE_DESCRIPTION of ENCOUNTER_CLASS_CODE in reference data</t>
+  </si>
+  <si>
+    <t>06ebfbf1-535d-406d-b055-c50d59bde4da</t>
+  </si>
+  <si>
+    <t>424c4575-77f3-42d4-859c-c73db0057957</t>
+  </si>
+  <si>
+    <t>Invalid value "Entered in Error" found in ENCOUNTER_STATUS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Entered in Error</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_STATUS_CODE_DESCRIPTION "Entered in Error" of ENCOUNTER_STATUS_CODE "discontinued" is not matching with the ENCOUNTER_STATUS_CODE_DESCRIPTION of ENCOUNTER_STATUS_CODE in reference data</t>
+  </si>
+  <si>
+    <t>39c39e9c-2436-4117-8fef-9f84f593857a</t>
+  </si>
+  <si>
+    <t>Invalid value "32166003" found in ENCOUNTER_TYPE_CODE</t>
+  </si>
+  <si>
+    <t>32166003</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_TYPE_CODE "32166003" of ENCOUNTER_TYPE_CODE_DESCRIPTION "In-person encounter" is not matching with the ENCOUNTER_TYPE_CODE of ENCOUNTER_TYPE_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>55ee7873-727b-417f-8db2-75ed9cda797c</t>
+  </si>
+  <si>
+    <t>Invalid value "History taking, self-administered, questionnaire" found in ENCOUNTER_TYPE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>History taking, self-administered, questionnaire</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_TYPE_CODE_DESCRIPTION "History taking, self-administered, questionnaire" of ENCOUNTER_TYPE_CODE "185317003" is not matching with the ENCOUNTER_TYPE_CODE_DESCRIPTION of ENCOUNTER_TYPE_CODE in reference data</t>
+  </si>
+  <si>
+    <t>6df1cd15-e806-4b2c-a7d1-cc8cafaa3767</t>
+  </si>
+  <si>
+    <t>6320c0bd-28ce-4a7b-9625-67a3386a998a</t>
+  </si>
+  <si>
+    <t>d488667a-dd64-45e8-bbec-124f95cddf01</t>
+  </si>
+  <si>
+    <t>Invalid value "EMER" found in ENCOUNTER_CLASS_CODE</t>
+  </si>
+  <si>
+    <t>EMER</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_CLASS_CODE "EMER" of ENCOUNTER_CLASS_CODE_DESCRIPTION "inpatient acute" is not matching with the ENCOUNTER_CLASS_CODE of ENCOUNTER_CLASS_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>ae54abe1-68b8-46c9-b0f1-7334976b600f</t>
+  </si>
+  <si>
+    <t>Invalid value "inpatient acute" found in ENCOUNTER_CLASS_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>inpatient acute</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_CLASS_CODE_DESCRIPTION "inpatient acute" of ENCOUNTER_CLASS_CODE "EMER" is not matching with the ENCOUNTER_CLASS_CODE_DESCRIPTION of ENCOUNTER_CLASS_CODE in reference data</t>
+  </si>
+  <si>
+    <t>d99e20d4-f610-42d6-8502-16c3276d7a08</t>
+  </si>
+  <si>
+    <t>Invalid value "discontinued" found in ENCOUNTER_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>discontinued</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_STATUS_CODE "discontinued" of ENCOUNTER_STATUS_CODE_DESCRIPTION "Entered in Error" is not matching with the ENCOUNTER_STATUS_CODE of ENCOUNTER_STATUS_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>ccb99cfe-99bf-4018-a5d8-4689bb9b86cc</t>
+  </si>
+  <si>
+    <t>56a676a1-96d1-4b7a-ad5e-b401201cc310</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -204,106 +417,121 @@
     <t>Use only allowed values 'Yes','No','NA' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>ac4e23cc-b7ee-4dbe-8731-efdb07398dba</t>
-  </si>
-  <si>
-    <t>753a48ee-23e2-4212-85fb-4c3eaa376005</t>
-  </si>
-  <si>
-    <t>1af5c88b-638e-402c-86d3-61f045a53daa</t>
-  </si>
-  <si>
-    <t>cbd53a72-c77e-4027-a3d7-66283e2dcedb</t>
-  </si>
-  <si>
-    <t>879099c8-671b-494d-847c-6dc2c5a5b33c</t>
-  </si>
-  <si>
-    <t>aad9ad7f-5cfc-426f-b655-536c4849193d</t>
-  </si>
-  <si>
-    <t>3bf5593e-776b-43dc-b765-55b9d1e9bc2a</t>
-  </si>
-  <si>
-    <t>e28895f8-8fdb-4d8e-a66a-fd85b19d8bff</t>
-  </si>
-  <si>
-    <t>f310e1a3-ed3b-4697-ac7b-cb1c6c1d98c1</t>
-  </si>
-  <si>
-    <t>ba23d574-a236-4018-8d46-9b09fa6c0288</t>
-  </si>
-  <si>
-    <t>fae38e27-c700-400c-83cc-a4ac40244493</t>
-  </si>
-  <si>
-    <t>5eab58b6-7d33-4e09-816f-20b719bd61d5</t>
-  </si>
-  <si>
-    <t>0ff7b2db-6998-47eb-bd2d-a72f98766d33</t>
-  </si>
-  <si>
-    <t>8b5cf674-6a0a-4fd7-96e7-c0e640801894</t>
-  </si>
-  <si>
-    <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
-  </si>
-  <si>
-    <t>03/05/94 13:08</t>
-  </si>
-  <si>
-    <t>a9d6fa36-725a-425d-b2be-16fdbed731ee</t>
-  </si>
-  <si>
-    <t>52844900-2e98-4624-a79e-fd6729735b4e</t>
-  </si>
-  <si>
-    <t>0cd2d3b4-598c-45af-be14-869b03ddc029</t>
-  </si>
-  <si>
-    <t>7df69de1-5c35-4463-a713-cdb4ee2cd4c1</t>
-  </si>
-  <si>
-    <t>e90e5431-7721-461e-9774-515a02c0b325</t>
-  </si>
-  <si>
-    <t>a8d8737f-7ddf-4f5c-97ed-f9dd3aeb6a8c</t>
-  </si>
-  <si>
-    <t>88ceb88f-f851-4e51-97e9-42622f1c98e6</t>
-  </si>
-  <si>
-    <t>0aaef67b-5dfc-47b9-8bf9-b0dd0786fc62</t>
-  </si>
-  <si>
-    <t>6a008556-e84c-4f8d-811e-6d6f5d7a4aae</t>
-  </si>
-  <si>
-    <t>9add894b-3758-4b2f-9c83-5d2be4368967</t>
-  </si>
-  <si>
-    <t>d38eaf2b-6ad5-427c-8e9d-7318b7088393</t>
-  </si>
-  <si>
-    <t>eb1ac4f9-ff60-4517-a9bd-1242fcf800d5</t>
-  </si>
-  <si>
-    <t>b7a098dc-245b-4c52-b493-ae1c2fe97d36</t>
-  </si>
-  <si>
-    <t>c7883f8d-c753-45ea-9d4f-431b9316d8aa</t>
-  </si>
-  <si>
-    <t>0c994e63-ed24-44c0-85d8-8eacf5fd3a6a</t>
-  </si>
-  <si>
-    <t>6cfea61e-c2c0-49b0-8e4b-3292b43501c6</t>
-  </si>
-  <si>
-    <t>7c3b44ee-ffb2-4bae-8bed-4f9787fbe8c9</t>
-  </si>
-  <si>
-    <t>7fa2fc5a-3d96-4093-9c96-3eb323df7376</t>
+    <t>2cc917b2-96b0-4400-9ae1-cd4dca2705d4</t>
+  </si>
+  <si>
+    <t>Invalid value "IMP" found in ENCOUNTER_CLASS_CODE</t>
+  </si>
+  <si>
+    <t>IMP</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_CLASS_CODE "IMP" of ENCOUNTER_CLASS_CODE_DESCRIPTION "pre-admission" is not matching with the ENCOUNTER_CLASS_CODE of ENCOUNTER_CLASS_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>0aafc770-0e0b-456e-bb55-9aa4783c0e4a</t>
+  </si>
+  <si>
+    <t>Invalid value "entered-in-error" found in ENCOUNTER_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>entered-in-error</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_STATUS_CODE "entered-in-error" of ENCOUNTER_STATUS_CODE_DESCRIPTION "Unknown" is not matching with the ENCOUNTER_STATUS_CODE of ENCOUNTER_STATUS_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>f86eb570-5152-4756-a79d-067e57310e19</t>
+  </si>
+  <si>
+    <t>68630e44-cec7-4100-81f8-0fc18598036c</t>
+  </si>
+  <si>
+    <t>ebfa9351-726c-41cf-8505-1b40d2017e2b</t>
+  </si>
+  <si>
+    <t>Invalid value "ACUTE" found in ENCOUNTER_CLASS_CODE</t>
+  </si>
+  <si>
+    <t>ACUTE</t>
+  </si>
+  <si>
+    <t>The ENCOUNTER_CLASS_CODE "ACUTE" of ENCOUNTER_CLASS_CODE_DESCRIPTION "inpatient non-acute" is not matching with the ENCOUNTER_CLASS_CODE of ENCOUNTER_CLASS_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>8ceedfad-3ede-46de-b4c6-423b8d49b491</t>
+  </si>
+  <si>
+    <t>6a99b10e-8eaf-4642-a804-e60b771d2919</t>
+  </si>
+  <si>
+    <t>b0f7aeed-807f-4195-b192-310942322f88</t>
+  </si>
+  <si>
+    <t>23d1981f-17f0-461d-ac36-690c94f95e46</t>
+  </si>
+  <si>
+    <t>adc2f12e-c8e0-4181-ade1-ca16a3f620a7</t>
+  </si>
+  <si>
+    <t>65242383-d63d-4004-848a-b3de99556695</t>
+  </si>
+  <si>
+    <t>601538aa-4fe5-4d0f-b317-45bbca859531</t>
+  </si>
+  <si>
+    <t>e0bd95e9-9021-44ae-8fc0-e155f466d746</t>
+  </si>
+  <si>
+    <t>73a62ab3-df0e-4af2-8fdb-21e7d5afa6dc</t>
+  </si>
+  <si>
+    <t>f62fe2b3-8dbc-4a5f-86b3-017cc2659175</t>
+  </si>
+  <si>
+    <t>7bc3a739-04ad-4e61-a2ee-4117b6953d9a</t>
+  </si>
+  <si>
+    <t>138cb6bc-5c67-446d-a879-2446cada9942</t>
+  </si>
+  <si>
+    <t>32615edd-f094-4564-b2a4-71f757c64894</t>
+  </si>
+  <si>
+    <t>cafe24d2-f087-4eff-a810-1e38c427f8f1</t>
+  </si>
+  <si>
+    <t>812e110e-0f9d-4fa4-9ed3-38bc2b939513</t>
+  </si>
+  <si>
+    <t>d4760d6d-79c5-44f7-8518-ca3d2aab1317</t>
+  </si>
+  <si>
+    <t>09f3a0ee-68fa-410a-8e1a-77b916f2b1e3</t>
+  </si>
+  <si>
+    <t>ff6b7b59-ea8b-4c9f-99db-6ae8bbbaf99d</t>
+  </si>
+  <si>
+    <t>96930927-20d4-4936-9c6e-e2627dd5aa71</t>
+  </si>
+  <si>
+    <t>b2e7b30b-f027-4780-8137-71ada604597b</t>
+  </si>
+  <si>
+    <t>Invalid timestamp "2023-02-02" found in RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>2023-02-02</t>
+  </si>
+  <si>
+    <t>6eeeb0e0-dc5a-4c0b-91a0-a62f903c70c8</t>
+  </si>
+  <si>
+    <t>Invalid timestamp "2021-02-02T13:40:12.000Z" found in RECORDED_TIME</t>
+  </si>
+  <si>
+    <t>2021-02-02T13:40:12.000Z</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -456,7 +684,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>bed34595-89ee-4f43-8c4e-0dae5f1dc086</t>
+    <t>d691f880-40f4-4549-983b-2093d9b6eca4</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>
@@ -642,18 +870,18 @@
         <v>30</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>32</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -689,16 +917,22 @@
         <v>37</v>
       </c>
       <c r="O3">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="P3" t="s">
         <v>38</v>
       </c>
+      <c r="Q3" t="s">
+        <v>39</v>
+      </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="U3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -715,36 +949,36 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" t="s">
         <v>43</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4">
+        <v>9</v>
+      </c>
+      <c r="P4" t="s">
         <v>44</v>
       </c>
-      <c r="M4" t="s">
+      <c r="R4" t="s">
         <v>45</v>
       </c>
-      <c r="N4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" t="s">
-        <v>49</v>
-      </c>
       <c r="T4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -762,36 +996,39 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T5" t="s">
         <v>41</v>
       </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>54</v>
-      </c>
-      <c r="R5" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -818,28 +1055,28 @@
         <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="O6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="Q6" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="R6" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="T6" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -865,25 +1102,28 @@
         <v>27</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M7" t="s">
         <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="O7">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="P7" t="s">
-        <v>38</v>
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>59</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="T7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
@@ -909,28 +1149,28 @@
         <v>27</v>
       </c>
       <c r="L8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N8" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="O8">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="P8" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q8" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="R8" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T8" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9">
@@ -956,28 +1196,25 @@
         <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="M9" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="O9">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="R9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="T9" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
@@ -994,37 +1231,37 @@
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="O10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="R10" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="T10" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11">
@@ -1041,37 +1278,37 @@
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="M11" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="O11">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="Q11" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="R11" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="T11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
@@ -1088,37 +1325,37 @@
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="J12" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="L12" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="O12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="Q12" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="R12" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="T12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
@@ -1135,37 +1372,37 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="L13" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="M13" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="N13" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="O13">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P13" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="Q13" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="R13" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="T13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
@@ -1191,7 +1428,7 @@
         <v>27</v>
       </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="M14" t="s">
         <v>29</v>
@@ -1205,13 +1442,13 @@
       <c r="P14" t="s">
         <v>31</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>32</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>33</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1238,28 +1475,31 @@
         <v>27</v>
       </c>
       <c r="L15" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="M15" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="N15" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="O15">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="P15" t="s">
         <v>38</v>
       </c>
       <c r="Q15" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="R15" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="T15" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="U15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -1285,27 +1525,27 @@
         <v>27</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="M16" t="s">
         <v>29</v>
       </c>
       <c r="N16" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O16">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="P16" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="R16" t="s">
+        <v>45</v>
+      </c>
+      <c r="T16" t="s">
         <v>33</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1332,28 +1572,31 @@
         <v>27</v>
       </c>
       <c r="L17" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="M17" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="N17" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="O17">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="P17" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="Q17" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="R17" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="T17" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="U17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -1379,28 +1622,28 @@
         <v>27</v>
       </c>
       <c r="L18" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="M18" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N18" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="O18">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="P18" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="Q18" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="R18" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="T18" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
@@ -1426,28 +1669,28 @@
         <v>27</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="M19" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="N19" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="O19">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="P19" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="Q19" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="R19" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="T19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
@@ -1473,28 +1716,28 @@
         <v>27</v>
       </c>
       <c r="L20" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="M20" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N20" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="O20">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="P20" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q20" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="R20" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T20" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21">
@@ -1520,28 +1763,25 @@
         <v>27</v>
       </c>
       <c r="L21" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="M21" t="s">
         <v>29</v>
       </c>
       <c r="N21" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="O21">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="P21" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="R21" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="T21" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22">
@@ -1567,27 +1807,30 @@
         <v>27</v>
       </c>
       <c r="L22" t="s">
-        <v>76</v>
+        <v>117</v>
       </c>
       <c r="M22" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N22" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="O22">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="P22" t="s">
         <v>31</v>
       </c>
       <c r="Q22" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="R22" t="s">
+        <v>120</v>
+      </c>
+      <c r="T22" t="s">
         <v>33</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1614,27 +1857,30 @@
         <v>27</v>
       </c>
       <c r="L23" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="M23" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N23" t="s">
-        <v>78</v>
+        <v>122</v>
       </c>
       <c r="O23">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="Q23" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
       <c r="R23" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="T23" t="s">
+        <v>41</v>
+      </c>
+      <c r="U23" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1661,27 +1907,30 @@
         <v>27</v>
       </c>
       <c r="L24" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="M24" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N24" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="O24">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="P24" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="Q24" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="R24" t="s">
+        <v>128</v>
+      </c>
+      <c r="T24" t="s">
         <v>33</v>
       </c>
-      <c r="T24" t="s">
+      <c r="U24" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1708,28 +1957,28 @@
         <v>27</v>
       </c>
       <c r="L25" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="M25" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N25" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O25">
         <v>14</v>
       </c>
       <c r="P25" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q25" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R25" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T25" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26">
@@ -1755,28 +2004,28 @@
         <v>27</v>
       </c>
       <c r="L26" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="M26" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="N26" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O26">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="P26" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="Q26" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="R26" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T26" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27">
@@ -1802,27 +2051,30 @@
         <v>27</v>
       </c>
       <c r="L27" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="M27" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N27" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="O27">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="P27" t="s">
         <v>31</v>
       </c>
       <c r="Q27" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="R27" t="s">
+        <v>138</v>
+      </c>
+      <c r="T27" t="s">
         <v>33</v>
       </c>
-      <c r="T27" t="s">
+      <c r="U27" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1849,27 +2101,30 @@
         <v>27</v>
       </c>
       <c r="L28" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="M28" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N28" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="O28">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="P28" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="Q28" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="R28" t="s">
+        <v>142</v>
+      </c>
+      <c r="T28" t="s">
         <v>33</v>
       </c>
-      <c r="T28" t="s">
+      <c r="U28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1896,28 +2151,28 @@
         <v>27</v>
       </c>
       <c r="L29" t="s">
-        <v>85</v>
+        <v>143</v>
       </c>
       <c r="M29" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N29" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O29">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="P29" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q29" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R29" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T29" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30">
@@ -1943,28 +2198,28 @@
         <v>27</v>
       </c>
       <c r="L30" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="M30" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="N30" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O30">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="P30" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="Q30" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="R30" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T30" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31">
@@ -1990,27 +2245,30 @@
         <v>27</v>
       </c>
       <c r="L31" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="M31" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="N31" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="O31">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="P31" t="s">
         <v>31</v>
       </c>
       <c r="Q31" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="R31" t="s">
+        <v>148</v>
+      </c>
+      <c r="T31" t="s">
         <v>33</v>
       </c>
-      <c r="T31" t="s">
+      <c r="U31" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2037,28 +2295,28 @@
         <v>27</v>
       </c>
       <c r="L32" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="M32" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N32" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O32">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="P32" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q32" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R32" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T32" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
@@ -2084,28 +2342,28 @@
         <v>27</v>
       </c>
       <c r="L33" t="s">
-        <v>89</v>
+        <v>150</v>
       </c>
       <c r="M33" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="N33" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O33">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="P33" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="Q33" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="R33" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T33" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34">
@@ -2131,28 +2389,28 @@
         <v>27</v>
       </c>
       <c r="L34" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="M34" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N34" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O34">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="P34" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q34" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R34" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T34" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35">
@@ -2178,28 +2436,28 @@
         <v>27</v>
       </c>
       <c r="L35" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="M35" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="N35" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O35">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="P35" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="Q35" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="R35" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T35" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36">
@@ -2225,28 +2483,28 @@
         <v>27</v>
       </c>
       <c r="L36" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="M36" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N36" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O36">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="P36" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q36" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R36" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T36" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37">
@@ -2272,28 +2530,28 @@
         <v>27</v>
       </c>
       <c r="L37" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="M37" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="N37" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O37">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="P37" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="Q37" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="R37" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T37" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38">
@@ -2319,28 +2577,28 @@
         <v>27</v>
       </c>
       <c r="L38" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="M38" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N38" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O38">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="P38" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q38" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R38" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T38" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39">
@@ -2366,28 +2624,28 @@
         <v>27</v>
       </c>
       <c r="L39" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="M39" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="N39" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="O39">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="P39" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="Q39" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="R39" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="T39" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40">
@@ -2413,28 +2671,28 @@
         <v>27</v>
       </c>
       <c r="L40" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="M40" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N40" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O40">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="P40" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q40" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R40" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T40" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41">
@@ -2460,28 +2718,28 @@
         <v>27</v>
       </c>
       <c r="L41" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="M41" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="N41" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="O41">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="P41" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="Q41" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="R41" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="T41" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42">
@@ -2498,25 +2756,37 @@
         <v>24</v>
       </c>
       <c r="H42" t="s">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="I42" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="J42" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L42" t="s">
-        <v>101</v>
+        <v>159</v>
       </c>
       <c r="M42" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N42" t="s">
-        <v>103</v>
+        <v>63</v>
+      </c>
+      <c r="O42">
+        <v>22</v>
+      </c>
+      <c r="P42" t="s">
+        <v>64</v>
       </c>
       <c r="Q42" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="R42" t="s">
+        <v>66</v>
+      </c>
+      <c r="T42" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="43">
@@ -2533,25 +2803,37 @@
         <v>24</v>
       </c>
       <c r="H43" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="I43" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="J43" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L43" t="s">
-        <v>105</v>
+        <v>160</v>
       </c>
       <c r="M43" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N43" t="s">
-        <v>106</v>
+        <v>63</v>
+      </c>
+      <c r="O43">
+        <v>23</v>
+      </c>
+      <c r="P43" t="s">
+        <v>64</v>
       </c>
       <c r="Q43" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="R43" t="s">
+        <v>66</v>
+      </c>
+      <c r="T43" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44">
@@ -2568,25 +2850,37 @@
         <v>24</v>
       </c>
       <c r="H44" t="s">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="I44" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="J44" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L44" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="M44" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N44" t="s">
-        <v>109</v>
+        <v>63</v>
+      </c>
+      <c r="O44">
+        <v>24</v>
+      </c>
+      <c r="P44" t="s">
+        <v>64</v>
       </c>
       <c r="Q44" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="R44" t="s">
+        <v>66</v>
+      </c>
+      <c r="T44" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="45">
@@ -2603,25 +2897,37 @@
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>110</v>
+        <v>25</v>
       </c>
       <c r="I45" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="J45" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L45" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
       <c r="M45" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N45" t="s">
-        <v>112</v>
+        <v>63</v>
+      </c>
+      <c r="O45">
+        <v>25</v>
+      </c>
+      <c r="P45" t="s">
+        <v>64</v>
       </c>
       <c r="Q45" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="R45" t="s">
+        <v>66</v>
+      </c>
+      <c r="T45" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="46">
@@ -2638,25 +2944,37 @@
         <v>24</v>
       </c>
       <c r="H46" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="I46" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="J46" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L46" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="M46" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N46" t="s">
-        <v>115</v>
+        <v>63</v>
+      </c>
+      <c r="O46">
+        <v>26</v>
+      </c>
+      <c r="P46" t="s">
+        <v>64</v>
       </c>
       <c r="Q46" t="s">
-        <v>99</v>
+        <v>65</v>
+      </c>
+      <c r="R46" t="s">
+        <v>66</v>
+      </c>
+      <c r="T46" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="47">
@@ -2673,25 +2991,37 @@
         <v>24</v>
       </c>
       <c r="H47" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="I47" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="J47" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L47" t="s">
-        <v>118</v>
+        <v>164</v>
       </c>
       <c r="M47" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N47" t="s">
-        <v>119</v>
+        <v>63</v>
+      </c>
+      <c r="O47">
+        <v>27</v>
+      </c>
+      <c r="P47" t="s">
+        <v>64</v>
       </c>
       <c r="Q47" t="s">
-        <v>117</v>
+        <v>65</v>
+      </c>
+      <c r="R47" t="s">
+        <v>66</v>
+      </c>
+      <c r="T47" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="48">
@@ -2708,25 +3038,37 @@
         <v>24</v>
       </c>
       <c r="H48" t="s">
-        <v>120</v>
+        <v>25</v>
       </c>
       <c r="I48" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="J48" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L48" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="M48" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N48" t="s">
-        <v>122</v>
+        <v>63</v>
+      </c>
+      <c r="O48">
+        <v>28</v>
+      </c>
+      <c r="P48" t="s">
+        <v>64</v>
       </c>
       <c r="Q48" t="s">
-        <v>117</v>
+        <v>65</v>
+      </c>
+      <c r="R48" t="s">
+        <v>66</v>
+      </c>
+      <c r="T48" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="49">
@@ -2743,25 +3085,37 @@
         <v>24</v>
       </c>
       <c r="H49" t="s">
-        <v>123</v>
+        <v>25</v>
       </c>
       <c r="I49" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="J49" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L49" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="M49" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N49" t="s">
-        <v>125</v>
+        <v>63</v>
+      </c>
+      <c r="O49">
+        <v>29</v>
+      </c>
+      <c r="P49" t="s">
+        <v>64</v>
       </c>
       <c r="Q49" t="s">
-        <v>117</v>
+        <v>65</v>
+      </c>
+      <c r="R49" t="s">
+        <v>66</v>
+      </c>
+      <c r="T49" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="50">
@@ -2778,25 +3132,37 @@
         <v>24</v>
       </c>
       <c r="H50" t="s">
-        <v>126</v>
+        <v>25</v>
       </c>
       <c r="I50" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="J50" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L50" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="M50" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N50" t="s">
-        <v>128</v>
+        <v>63</v>
+      </c>
+      <c r="O50">
+        <v>30</v>
+      </c>
+      <c r="P50" t="s">
+        <v>64</v>
       </c>
       <c r="Q50" t="s">
-        <v>117</v>
+        <v>65</v>
+      </c>
+      <c r="R50" t="s">
+        <v>66</v>
+      </c>
+      <c r="T50" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="51">
@@ -2813,25 +3179,37 @@
         <v>24</v>
       </c>
       <c r="H51" t="s">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="I51" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="J51" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L51" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="M51" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N51" t="s">
-        <v>131</v>
+        <v>169</v>
+      </c>
+      <c r="O51">
+        <v>7</v>
+      </c>
+      <c r="P51" t="s">
+        <v>64</v>
       </c>
       <c r="Q51" t="s">
-        <v>117</v>
+        <v>170</v>
+      </c>
+      <c r="R51" t="s">
+        <v>66</v>
+      </c>
+      <c r="T51" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="52">
@@ -2848,25 +3226,37 @@
         <v>24</v>
       </c>
       <c r="H52" t="s">
-        <v>132</v>
+        <v>25</v>
       </c>
       <c r="I52" t="s">
-        <v>133</v>
+        <v>26</v>
       </c>
       <c r="J52" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="L52" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="M52" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="N52" t="s">
-        <v>135</v>
+        <v>172</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52" t="s">
+        <v>64</v>
       </c>
       <c r="Q52" t="s">
-        <v>133</v>
+        <v>173</v>
+      </c>
+      <c r="R52" t="s">
+        <v>66</v>
+      </c>
+      <c r="T52" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="53">
@@ -2883,25 +3273,25 @@
         <v>24</v>
       </c>
       <c r="H53" t="s">
-        <v>136</v>
+        <v>174</v>
       </c>
       <c r="I53" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="J53" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="L53" t="s">
-        <v>137</v>
+        <v>177</v>
       </c>
       <c r="M53" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="N53" t="s">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="Q53" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54">
@@ -2918,25 +3308,25 @@
         <v>24</v>
       </c>
       <c r="H54" t="s">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="I54" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="J54" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="L54" t="s">
-        <v>140</v>
+        <v>181</v>
       </c>
       <c r="M54" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="N54" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
       <c r="Q54" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55">
@@ -2953,25 +3343,25 @@
         <v>24</v>
       </c>
       <c r="H55" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
       <c r="I55" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="J55" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="L55" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="M55" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="N55" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="Q55" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56">
@@ -2988,25 +3378,25 @@
         <v>24</v>
       </c>
       <c r="H56" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="I56" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
       <c r="J56" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="L56" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="M56" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
       <c r="N56" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="Q56" t="s">
-        <v>133</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57">
@@ -3023,31 +3413,416 @@
         <v>24</v>
       </c>
       <c r="H57" t="s">
-        <v>41</v>
+        <v>189</v>
       </c>
       <c r="I57" t="s">
-        <v>42</v>
+        <v>175</v>
       </c>
       <c r="J57" t="s">
-        <v>43</v>
+        <v>176</v>
       </c>
       <c r="L57" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="M57" t="s">
-        <v>36</v>
+        <v>178</v>
       </c>
       <c r="N57" t="s">
-        <v>149</v>
-      </c>
-      <c r="O57">
+        <v>191</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" t="s">
+        <v>192</v>
+      </c>
+      <c r="I58" t="s">
+        <v>193</v>
+      </c>
+      <c r="J58" t="s">
+        <v>176</v>
+      </c>
+      <c r="L58" t="s">
+        <v>194</v>
+      </c>
+      <c r="M58" t="s">
+        <v>178</v>
+      </c>
+      <c r="N58" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" t="s">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" t="s">
+        <v>196</v>
+      </c>
+      <c r="I59" t="s">
+        <v>193</v>
+      </c>
+      <c r="J59" t="s">
+        <v>176</v>
+      </c>
+      <c r="L59" t="s">
+        <v>197</v>
+      </c>
+      <c r="M59" t="s">
+        <v>178</v>
+      </c>
+      <c r="N59" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+      <c r="G60" t="s">
+        <v>24</v>
+      </c>
+      <c r="H60" t="s">
+        <v>199</v>
+      </c>
+      <c r="I60" t="s">
+        <v>193</v>
+      </c>
+      <c r="J60" t="s">
+        <v>176</v>
+      </c>
+      <c r="L60" t="s">
+        <v>200</v>
+      </c>
+      <c r="M60" t="s">
+        <v>178</v>
+      </c>
+      <c r="N60" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" t="s">
+        <v>202</v>
+      </c>
+      <c r="I61" t="s">
+        <v>193</v>
+      </c>
+      <c r="J61" t="s">
+        <v>176</v>
+      </c>
+      <c r="L61" t="s">
+        <v>203</v>
+      </c>
+      <c r="M61" t="s">
+        <v>178</v>
+      </c>
+      <c r="N61" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" t="s">
+        <v>205</v>
+      </c>
+      <c r="I62" t="s">
+        <v>193</v>
+      </c>
+      <c r="J62" t="s">
+        <v>176</v>
+      </c>
+      <c r="L62" t="s">
+        <v>206</v>
+      </c>
+      <c r="M62" t="s">
+        <v>178</v>
+      </c>
+      <c r="N62" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" t="s">
+        <v>208</v>
+      </c>
+      <c r="I63" t="s">
+        <v>209</v>
+      </c>
+      <c r="J63" t="s">
+        <v>176</v>
+      </c>
+      <c r="L63" t="s">
+        <v>210</v>
+      </c>
+      <c r="M63" t="s">
+        <v>178</v>
+      </c>
+      <c r="N63" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" t="s">
+        <v>24</v>
+      </c>
+      <c r="H64" t="s">
+        <v>212</v>
+      </c>
+      <c r="I64" t="s">
+        <v>209</v>
+      </c>
+      <c r="J64" t="s">
+        <v>176</v>
+      </c>
+      <c r="L64" t="s">
+        <v>213</v>
+      </c>
+      <c r="M64" t="s">
+        <v>178</v>
+      </c>
+      <c r="N64" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65" t="s">
+        <v>215</v>
+      </c>
+      <c r="I65" t="s">
+        <v>209</v>
+      </c>
+      <c r="J65" t="s">
+        <v>176</v>
+      </c>
+      <c r="L65" t="s">
+        <v>216</v>
+      </c>
+      <c r="M65" t="s">
+        <v>178</v>
+      </c>
+      <c r="N65" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66" t="s">
+        <v>218</v>
+      </c>
+      <c r="I66" t="s">
+        <v>209</v>
+      </c>
+      <c r="J66" t="s">
+        <v>176</v>
+      </c>
+      <c r="L66" t="s">
+        <v>219</v>
+      </c>
+      <c r="M66" t="s">
+        <v>178</v>
+      </c>
+      <c r="N66" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" t="s">
+        <v>22</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" t="s">
+        <v>221</v>
+      </c>
+      <c r="I67" t="s">
+        <v>209</v>
+      </c>
+      <c r="J67" t="s">
+        <v>176</v>
+      </c>
+      <c r="L67" t="s">
+        <v>222</v>
+      </c>
+      <c r="M67" t="s">
+        <v>178</v>
+      </c>
+      <c r="N67" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" t="s">
+        <v>72</v>
+      </c>
+      <c r="I68" t="s">
+        <v>73</v>
+      </c>
+      <c r="J68" t="s">
+        <v>74</v>
+      </c>
+      <c r="L68" t="s">
+        <v>224</v>
+      </c>
+      <c r="M68" t="s">
+        <v>29</v>
+      </c>
+      <c r="N68" t="s">
+        <v>225</v>
+      </c>
+      <c r="O68">
         <v>1</v>
       </c>
-      <c r="P57" t="s">
-        <v>150</v>
-      </c>
-      <c r="R57" t="s">
-        <v>151</v>
+      <c r="P68" t="s">
+        <v>226</v>
+      </c>
+      <c r="R68" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add preferred language reference ingestion #66 - add preferred language reference csv data
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>6fe6f3ba-15d5-4c14-9cee-05f9055fa85c</t>
+    <t>a1bcd225-38c1-41dc-ba77-02cd2193d596</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -117,7 +117,7 @@
     <t/>
   </si>
   <si>
-    <t>6cd57301-72ee-45b2-a89e-7c64505e493c</t>
+    <t>2dbd073c-6684-4224-bb4c-a91ca15222a4</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -141,7 +141,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>42289c37-5242-44ac-844b-bc027714c711</t>
+    <t>0244304a-5deb-48da-875a-627182e9e89b</t>
   </si>
   <si>
     <t>Invalid value "LA6729-3" found in ANSWER_CODE</t>
@@ -156,7 +156,7 @@
     <t>The ANSWER_CODE "LA6729-3" of ANSWER_CODE_DESCRIPTION "Sometimes true" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>247e9575-fa58-4fd5-ac10-6818afc1f1a5</t>
+    <t>026f475b-1f07-4fda-b482-105264f86fd2</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -186,7 +186,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>b2efd78e-a606-412c-9e75-9e63c310f277</t>
+    <t>7b8faadd-6850-401c-8b0c-2ac7dd11c42c</t>
   </si>
   <si>
     <t>Invalid value "UNK" found in SEX_AT_BIRTH_CODE</t>
@@ -201,7 +201,7 @@
     <t>The SEX_AT_BIRTH_CODE "UNK" of SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" is not matching with the SEX_AT_BIRTH_CODE of SEX_AT_BIRTH_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>6e449d32-c1d8-4040-977e-a5a23b025518</t>
+    <t>6625dac4-cae1-4679-82c2-0917df6bf522</t>
   </si>
   <si>
     <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
@@ -219,7 +219,7 @@
     <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
   </si>
   <si>
-    <t>f3120386-3344-401f-941f-514a4dc1d3dc</t>
+    <t>3ce331ee-5dc8-42d7-a7f7-b97ffd1c5751</t>
   </si>
   <si>
     <t>Invalid value "1142-9" found in RACE_CODE</t>
@@ -234,7 +234,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>7ea7272c-ca5d-4a76-9a8f-6a52d1fc6171</t>
+    <t>33d51eb2-8ad2-4328-824a-1f8b5f795cde</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -252,25 +252,25 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>dc3f0bfc-debf-47e0-82af-20d9619d2103</t>
-  </si>
-  <si>
-    <t>68b7f069-6cb0-4611-8a75-a41074c545a6</t>
-  </si>
-  <si>
-    <t>859addfe-2ffe-4f28-b739-b302a4a12e9a</t>
-  </si>
-  <si>
-    <t>8d1799a3-7233-41d6-943f-e1cfbb8a5cc9</t>
-  </si>
-  <si>
-    <t>7e4b58ae-4370-4549-831e-a4aa75a32943</t>
-  </si>
-  <si>
-    <t>1c46bd54-2a52-4d35-b332-8666da8d7aea</t>
-  </si>
-  <si>
-    <t>f5c0c5ee-9216-413e-8031-8f3e9112053e</t>
+    <t>2dcf1ec1-b9cd-4130-8f25-94815546c0eb</t>
+  </si>
+  <si>
+    <t>44463e7d-a7dc-419c-9637-6a35ea551d02</t>
+  </si>
+  <si>
+    <t>3011a340-e82b-4b7e-b2de-1c6ce6d7a64b</t>
+  </si>
+  <si>
+    <t>dbbad070-10bc-4ba3-8ab0-2ed53fb5db9b</t>
+  </si>
+  <si>
+    <t>7b0ebc60-137d-4566-91e6-3ccfc897a2fb</t>
+  </si>
+  <si>
+    <t>4b5d504e-fcaf-460a-9e41-d767f2be504f</t>
+  </si>
+  <si>
+    <t>28f5cba4-6f00-4644-9da8-7d0bd9552050</t>
   </si>
   <si>
     <t>Invalid value "LA6571-9" found in ANSWER_CODE</t>
@@ -282,16 +282,16 @@
     <t>The ANSWER_CODE "LA6571-9" of ANSWER_CODE_DESCRIPTION "Nearly every day" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>9381c195-36c2-446e-a23b-8166f7038c0a</t>
-  </si>
-  <si>
-    <t>3e0d3620-571f-418b-a0e4-a1df981c5719</t>
-  </si>
-  <si>
-    <t>f45562e3-6074-432e-90b2-21a6b6d8d30d</t>
-  </si>
-  <si>
-    <t>6e6ac80f-6859-4d98-909e-1d550e57d8ab</t>
+    <t>89f31848-70e7-4d5c-9c2a-73ca02e3cdb7</t>
+  </si>
+  <si>
+    <t>b9e6e10f-eb9a-49e5-a3fa-6dea8584ecdc</t>
+  </si>
+  <si>
+    <t>d886d3e9-fc19-414d-b847-0ba764eaa70e</t>
+  </si>
+  <si>
+    <t>c4996409-8355-45b6-95a8-b721d815150a</t>
   </si>
   <si>
     <t>Invalid value "LA6569-3" found in ANSWER_CODE</t>
@@ -303,25 +303,25 @@
     <t>The ANSWER_CODE "LA6569-3" of ANSWER_CODE_DESCRIPTION "Several days" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>8ec5f7e4-57c9-4c01-ac0b-16d7d3c0688c</t>
-  </si>
-  <si>
-    <t>472431c3-727a-4392-a6f4-c7164101cd5d</t>
-  </si>
-  <si>
-    <t>db78d6f8-1d41-4c69-bf4c-1b0af2bb40c7</t>
-  </si>
-  <si>
-    <t>6069b482-c551-458d-a460-34f55b97ff05</t>
-  </si>
-  <si>
-    <t>66ae6e97-2424-48db-baaf-279e749c11d4</t>
-  </si>
-  <si>
-    <t>61018a01-9f0f-4968-ae86-6f80e5e0d3d9</t>
-  </si>
-  <si>
-    <t>dd4f3549-ff00-45bc-a0ed-83b4f681085e</t>
+    <t>32556711-1f15-48ee-8b47-22aa919daab9</t>
+  </si>
+  <si>
+    <t>028f835f-37d1-4395-b2b1-de57d76803cd</t>
+  </si>
+  <si>
+    <t>efd473db-0aba-47e4-b2fb-01b4fa608999</t>
+  </si>
+  <si>
+    <t>23dd376f-566f-4e49-abbd-2779b2028319</t>
+  </si>
+  <si>
+    <t>d146a4dd-00da-442d-ba17-1fab3b3d84ac</t>
+  </si>
+  <si>
+    <t>013363e2-fe12-49f6-ba93-6c6afa64e762</t>
+  </si>
+  <si>
+    <t>64354630-7e22-48eb-a5ec-9b400ebbc5e9</t>
   </si>
   <si>
     <t>Invalid value "69861-3" found in QUESTION_CODE</t>
@@ -333,19 +333,19 @@
     <t>The QUESTION_CODE "69861-3" of QUESTION_CODE_DESCRIPTION "Because of a physical, mental, or emotional condition, do you have difficulty doing errands alone such as visiting a physician's office or shopping" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>48d32e54-e949-4ebd-9a1c-28337ae5516b</t>
-  </si>
-  <si>
-    <t>d3263673-9b38-409d-afd9-4bedf39458ad</t>
-  </si>
-  <si>
-    <t>d23cf982-273a-465b-8988-9f4ec7eb677a</t>
-  </si>
-  <si>
-    <t>36c0650d-9f85-4624-ad2c-0fa0da80abf1</t>
-  </si>
-  <si>
-    <t>2a8e077b-5cbf-448f-8cc8-d400894ab689</t>
+    <t>5147668f-02fa-43bf-a232-411b0011f374</t>
+  </si>
+  <si>
+    <t>356ca88d-410a-4803-ac69-47f536f47977</t>
+  </si>
+  <si>
+    <t>fa2ec750-ef9b-430e-accc-09a037cf049f</t>
+  </si>
+  <si>
+    <t>04f1fc8d-fe47-4689-80e1-3a6af42f3a25</t>
+  </si>
+  <si>
+    <t>99f54569-f1ed-4cf8-8b23-fb5f259ddd2a</t>
   </si>
   <si>
     <t>Invalid value "LA31983-2" found in ANSWER_CODE</t>
@@ -357,7 +357,7 @@
     <t>The ANSWER_CODE "LA31983-2" of ANSWER_CODE_DESCRIPTION "I do not need or want help" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>0cf58aaa-d22c-439e-ac43-cbb9579fc44f</t>
+    <t>afb5a289-b43c-448d-be33-ec669bf1ff4b</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -369,10 +369,10 @@
     <t>Provide a value for POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>c974ee29-12cf-41e8-942c-3576575d19b9</t>
-  </si>
-  <si>
-    <t>4ff52ec2-b4a9-40a5-b57a-13a03d08e0e9</t>
+    <t>824464b1-0c1b-45f9-9d9c-e4a5116e20ee</t>
+  </si>
+  <si>
+    <t>d86d77e9-84b1-4d75-b7d6-82b100461f48</t>
   </si>
   <si>
     <t>Invalid value "69858-9" found in QUESTION_CODE</t>
@@ -384,7 +384,7 @@
     <t>The QUESTION_CODE "69858-9" of QUESTION_CODE_DESCRIPTION "Because of a physical, mental, or emotional condition, do you have serious difficulty concentrating, remembering, or making decisions?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>98bcf9f1-ae48-4cd3-8e2f-134a57acc426</t>
+    <t>f6452619-643c-4803-9934-d8fd5e3f39ce</t>
   </si>
   <si>
     <t>Invalid value "LA16644-9" found in ANSWER_CODE</t>
@@ -396,22 +396,22 @@
     <t>The ANSWER_CODE "LA16644-9" of ANSWER_CODE_DESCRIPTION "Fairly often" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>6cc4f247-ad9c-45e8-8b64-ec51ad7c6e97</t>
-  </si>
-  <si>
-    <t>92a1e0a7-42dc-45c8-aab8-1b656faaf505</t>
-  </si>
-  <si>
-    <t>78bc4e30-9ebf-4b0a-a2e9-214efdeeaf5d</t>
-  </si>
-  <si>
-    <t>487ab317-914a-45a4-95dc-5d27081df473</t>
-  </si>
-  <si>
-    <t>3efe3ac1-d6ca-43fb-a7f9-ee1de492b3c0</t>
-  </si>
-  <si>
-    <t>dfd88fdf-ae1c-4077-8e7d-834db21ea29c</t>
+    <t>bbf0765f-ffa2-4700-9509-0d826e427157</t>
+  </si>
+  <si>
+    <t>d45208ae-beec-4494-a328-196bd7bdbc79</t>
+  </si>
+  <si>
+    <t>526116c7-4e05-4dc3-8a2b-549d9b3b2fe3</t>
+  </si>
+  <si>
+    <t>80b4e25d-ba60-43f3-8c30-894d9de52a3a</t>
+  </si>
+  <si>
+    <t>5b032a52-619d-40fd-b0bd-06faeee229f7</t>
+  </si>
+  <si>
+    <t>8654345f-2c5d-491d-8c4e-486967444406</t>
   </si>
   <si>
     <t>Invalid value "93038-8" found in QUESTION_CODE</t>
@@ -423,25 +423,25 @@
     <t>The QUESTION_CODE "93038-8" of QUESTION_CODE_DESCRIPTION "Stress means a situation in which a person feels tense, restless, nervous, or anxious, or is unable to sleep at night because his or her mind is troubled all the time. Do you feel this kind of stress these days?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>4d1532eb-9e13-4868-80a9-8f3d3bc4fbdd</t>
-  </si>
-  <si>
-    <t>2f2aa9fc-5561-4991-8d0c-24769cf5322f</t>
-  </si>
-  <si>
-    <t>719127e3-96aa-43e3-b08d-634b1332e766</t>
-  </si>
-  <si>
-    <t>d9ed0aa6-4cd2-4c1d-90bc-36555e4e4ae6</t>
-  </si>
-  <si>
-    <t>a93d837a-fd74-44e6-9cf6-525eba837994</t>
-  </si>
-  <si>
-    <t>1c614f0b-6d6e-4889-be9a-0a7cd6dceb8b</t>
-  </si>
-  <si>
-    <t>353c84d2-2b9c-4f59-853a-fde73bf0c6a3</t>
+    <t>767f2996-7ca0-4966-9d26-2ace48e272e6</t>
+  </si>
+  <si>
+    <t>93e03c23-a563-4441-bf83-da1750557c44</t>
+  </si>
+  <si>
+    <t>dc82faa1-2368-4be5-adb4-3bf887f76457</t>
+  </si>
+  <si>
+    <t>3abde441-aed7-4571-85af-52117905b126</t>
+  </si>
+  <si>
+    <t>eff18ffb-c6c3-4a47-8585-144989e29b43</t>
+  </si>
+  <si>
+    <t>40514b18-159d-4a5f-ac16-2adf6bde21da</t>
+  </si>
+  <si>
+    <t>312ef8f2-102c-457f-8acb-32dcdee2ade1</t>
   </si>
   <si>
     <t>Invalid value "LA32002-0" found in ANSWER_CODE</t>
@@ -453,31 +453,31 @@
     <t>The ANSWER_CODE "LA32002-0" of ANSWER_CODE_DESCRIPTION "Already shut off" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>736a20dd-544b-44e3-abbd-0052945a2d75</t>
-  </si>
-  <si>
-    <t>cec958a2-1421-4107-b675-b5eaa6a45ca0</t>
-  </si>
-  <si>
-    <t>e4c7c565-f393-4980-9e30-bc297defbe95</t>
-  </si>
-  <si>
-    <t>7c3e9b9d-a33f-4977-ac9c-893f4e5e1a9e</t>
-  </si>
-  <si>
-    <t>7231c125-06bf-4d21-aa89-ee551cfa67a0</t>
-  </si>
-  <si>
-    <t>1138f0e3-7f5b-46ac-84b9-69e9c31250a4</t>
-  </si>
-  <si>
-    <t>dcc10036-cc8c-48df-a50f-da428ca79d8d</t>
-  </si>
-  <si>
-    <t>f6eddaf5-6f1e-42ee-9d1f-4dc0ab0d5898</t>
-  </si>
-  <si>
-    <t>56e30650-888d-40b9-b4eb-7aba2ffc9cef</t>
+    <t>40a6be8c-599c-458b-b9d5-84d852ca15b1</t>
+  </si>
+  <si>
+    <t>0c65eae8-d47c-4e00-b2cb-99c76621a0ec</t>
+  </si>
+  <si>
+    <t>4f70c607-e509-43b4-937d-5806775ba5cf</t>
+  </si>
+  <si>
+    <t>aba6753f-52d0-4a2d-acf1-cbdeff656287</t>
+  </si>
+  <si>
+    <t>d07efb67-2f11-4c57-a7b1-5118a03327b4</t>
+  </si>
+  <si>
+    <t>cec0699f-5a01-4cc5-bc7e-c5e688240bbc</t>
+  </si>
+  <si>
+    <t>2630f5fd-b9a5-4a7c-b8c7-bb7b9897d473</t>
+  </si>
+  <si>
+    <t>25266ec9-5a20-42e9-bd8b-598c4123d7c4</t>
+  </si>
+  <si>
+    <t>c1599033-6475-48e4-862b-0394eb7a66cc</t>
   </si>
   <si>
     <t>Invalid value "LA31997-2" found in ANSWER_CODE</t>
@@ -489,10 +489,10 @@
     <t>The ANSWER_CODE "LA31997-2" of ANSWER_CODE_DESCRIPTION "Lead paint or pipes" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>ba4e94ec-810d-42d5-a6ef-d95da261a429</t>
-  </si>
-  <si>
-    <t>094bb63b-5074-494e-8716-93cd019338be</t>
+    <t>de1c606d-8abc-455a-947b-b0cf82c11418</t>
+  </si>
+  <si>
+    <t>d10943bf-66d3-43cd-ba7b-c48f5faf9b10</t>
   </si>
   <si>
     <t>Invalid value "44255-8" found in QUESTION_CODE</t>
@@ -504,7 +504,7 @@
     <t>The QUESTION_CODE "44255-8" of QUESTION_CODE_DESCRIPTION "Feeling down, depressed, or hopeless?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>b89184fb-839f-4cd6-a03e-b42409e56dfe</t>
+    <t>f421ac6a-f469-4e56-855f-375546663940</t>
   </si>
   <si>
     <t>Invalid value "LA31994-9" found in ANSWER_CODE</t>
@@ -516,25 +516,25 @@
     <t>The ANSWER_CODE "LA31994-9" of ANSWER_CODE_DESCRIPTION "I have a place to live today, but I am worried about losing it in the future" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>3352d97b-75b8-4d00-b5b6-b0242fc96403</t>
-  </si>
-  <si>
-    <t>2eb73d30-d76b-42f9-8f3f-2a28b51d7509</t>
-  </si>
-  <si>
-    <t>b4f9f53d-d245-41b5-a666-8ff65ea7c21c</t>
-  </si>
-  <si>
-    <t>d30b951f-bd95-43ca-a1d7-2c91394c84a6</t>
-  </si>
-  <si>
-    <t>176d6daf-0c60-4d72-8e23-b9dffaac19ae</t>
-  </si>
-  <si>
-    <t>387a982c-b38d-4198-a200-a00e55697693</t>
-  </si>
-  <si>
-    <t>21fb471f-c95b-4f71-a068-f8615a32fe00</t>
+    <t>cf3b7ecc-1174-4007-ad37-6af41f4325f9</t>
+  </si>
+  <si>
+    <t>dbb4167a-7b7f-46aa-b63e-b6aca7e3ec0a</t>
+  </si>
+  <si>
+    <t>14f2856e-96ca-4945-9058-38f23556911f</t>
+  </si>
+  <si>
+    <t>4667e558-62d3-485e-8a2f-461931879bd6</t>
+  </si>
+  <si>
+    <t>73276c43-50a5-45c4-8598-b631972ec0ef</t>
+  </si>
+  <si>
+    <t>138043b7-9296-40b6-bb9f-af77d9374047</t>
+  </si>
+  <si>
+    <t>6da64f13-3237-4f72-a733-1cc76ea361e8</t>
   </si>
   <si>
     <t>Invalid timestamp "01/27/02 15:42" found in RECORDED_TIME</t>
@@ -543,7 +543,7 @@
     <t>01/27/02 15:42</t>
   </si>
   <si>
-    <t>19449a60-ffab-438a-bd89-a80357c1758f</t>
+    <t>9f1763cc-cbdb-468c-a436-7a70b4e315f6</t>
   </si>
   <si>
     <t>Invalid value "44250-9" found in QUESTION_CODE</t>
@@ -555,28 +555,28 @@
     <t>The QUESTION_CODE "44250-9" of QUESTION_CODE_DESCRIPTION "Little interest or pleasure in doing things?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>30a3f770-b3e5-4459-a034-6c8926c7231f</t>
-  </si>
-  <si>
-    <t>82b8db3b-7762-4ce2-9d39-7f99f825fbae</t>
-  </si>
-  <si>
-    <t>b368b7d9-d8ae-40cd-a215-874bb230cc9d</t>
-  </si>
-  <si>
-    <t>b22b0c1b-efae-4b3f-80e6-86bbab20a756</t>
-  </si>
-  <si>
-    <t>9f1bf01c-cc97-4276-9017-52ebaa5ea1ef</t>
-  </si>
-  <si>
-    <t>a0d29604-0097-4ebe-96fc-190861216639</t>
-  </si>
-  <si>
-    <t>ee112236-9519-4edc-a315-e2e1a30d6f4b</t>
-  </si>
-  <si>
-    <t>2789674f-f0fc-422f-9a7f-0247646291c2</t>
+    <t>85959c3d-5f97-41f6-a8d4-5558a0a3ffde</t>
+  </si>
+  <si>
+    <t>c09995e2-a81d-4c2f-8264-df31c5d91ce9</t>
+  </si>
+  <si>
+    <t>f6a6a254-7114-4e25-bbc0-e8bfb978b02a</t>
+  </si>
+  <si>
+    <t>2aa5cce0-a98d-4bfb-84b3-07fd8d2559a6</t>
+  </si>
+  <si>
+    <t>af12fd1c-2975-489d-81a6-e0c1b138f6b0</t>
+  </si>
+  <si>
+    <t>3571ce63-68f4-4dbf-b49a-390aea0241d0</t>
+  </si>
+  <si>
+    <t>1261d7ca-3896-4e7d-a05f-e7ad5f4f4eb7</t>
+  </si>
+  <si>
+    <t>aa522703-b495-45b7-91d3-38ddf24dc9ee</t>
   </si>
   <si>
     <t>Invalid value "95530-2" found in QUESTION_CODE</t>
@@ -588,34 +588,34 @@
     <t>The QUESTION_CODE "95530-2" of QUESTION_CODE_DESCRIPTION "How many times in the past year have you used prescription drugs for non-medical reasons?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>3c1a30fd-679b-40c4-bee8-67f783dd7e57</t>
-  </si>
-  <si>
-    <t>4f7f4107-51b3-4a28-b852-83c9bba80dde</t>
-  </si>
-  <si>
-    <t>514722d1-7ec0-4448-9e4a-c0b4ee0b3c29</t>
-  </si>
-  <si>
-    <t>8486e340-cc21-4f77-b4df-c7c336504dc0</t>
-  </si>
-  <si>
-    <t>e9ebbc27-6f31-4bbd-8f51-1bde9bd3c6a3</t>
-  </si>
-  <si>
-    <t>ade4a853-8c9a-4d06-b6d9-7a883df82473</t>
-  </si>
-  <si>
-    <t>8cf568a7-b03f-4a84-8327-8ac12ab7b0dc</t>
-  </si>
-  <si>
-    <t>0c52a2ab-c617-4883-af00-31a9f349d86e</t>
-  </si>
-  <si>
-    <t>647fce0b-4c0b-4cee-8e4b-848e526687c5</t>
-  </si>
-  <si>
-    <t>9e897be8-25d3-49bb-90e5-f4262f99eab3</t>
+    <t>18dbf305-d7b9-4aea-9996-a6e8c1bc90c6</t>
+  </si>
+  <si>
+    <t>ca13a2c5-bb8a-4409-bcf2-908ab6e2691e</t>
+  </si>
+  <si>
+    <t>215aee41-f0fa-4cfd-99e8-366be7f2e9a1</t>
+  </si>
+  <si>
+    <t>e4efb683-4e31-416e-b09a-5c7ed990bae8</t>
+  </si>
+  <si>
+    <t>a0c615c9-d1dd-4fb9-b075-f73ee2b382fb</t>
+  </si>
+  <si>
+    <t>d9a66f4b-c730-40fa-8260-9c8c088e4adc</t>
+  </si>
+  <si>
+    <t>7a1ac753-5106-403e-b204-2be8f379c7cc</t>
+  </si>
+  <si>
+    <t>31ffa4b5-990d-4f80-802c-a4194451bf17</t>
+  </si>
+  <si>
+    <t>0c0acf40-e9a5-4dcc-926c-38cbbb262935</t>
+  </si>
+  <si>
+    <t>7e0429e9-681f-45bf-a029-571142c593bc</t>
   </si>
   <si>
     <t>Invalid value "96842-0" found in QUESTION_CODE</t>
@@ -627,22 +627,22 @@
     <t>The QUESTION_CODE "96842-0" of QUESTION_CODE_DESCRIPTION "How many times in the past 12 months have you used tobacco products (like cigarettes, cigars, snuff, chew, electronic cigarettes)?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>6cf634a9-3f74-4147-8f08-63fa6520ceae</t>
-  </si>
-  <si>
-    <t>d566d765-cfdf-4057-afd0-a1873204aa03</t>
-  </si>
-  <si>
-    <t>3c0181f3-2d65-4ea5-909f-e6e9e2f7700d</t>
-  </si>
-  <si>
-    <t>38542657-b9f5-4210-ac6e-bdebf26522e2</t>
-  </si>
-  <si>
-    <t>4d4acf79-e170-4ff3-8ca1-82b2760733b8</t>
-  </si>
-  <si>
-    <t>5aa950cc-b2dc-45dc-b7ce-a86c66e9cf48</t>
+    <t>36895c4c-8a5f-4c5f-aa15-c5210ee8ae59</t>
+  </si>
+  <si>
+    <t>4e9d6ecf-c8ef-4f23-85be-68f59179cc57</t>
+  </si>
+  <si>
+    <t>bc882015-bb26-47f7-9285-30be66c23c31</t>
+  </si>
+  <si>
+    <t>102df668-587f-44ef-a67b-78e94ef0e5b7</t>
+  </si>
+  <si>
+    <t>7fc48b4d-e92e-4d2b-a489-126c5b021d72</t>
+  </si>
+  <si>
+    <t>595bef24-4546-4cdb-b233-7913ee3cd4fc</t>
   </si>
   <si>
     <t>Invalid value "68517-2" found in QUESTION_CODE</t>
@@ -654,19 +654,19 @@
     <t>The QUESTION_CODE "68517-2" of QUESTION_CODE_DESCRIPTION "How many times in the past 12 months have you had 5 or more drinks in a day (males) or 4 or more drinks in a day (females)?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>09762927-92b4-4994-8857-872d4e8abba0</t>
-  </si>
-  <si>
-    <t>eb593d95-ed21-455d-8c01-ec0648de1c1d</t>
-  </si>
-  <si>
-    <t>78378e31-3750-4ad9-b466-222573e047a1</t>
-  </si>
-  <si>
-    <t>db3c864c-841a-447c-b478-d2de1e9abf6d</t>
-  </si>
-  <si>
-    <t>899299eb-a3da-4cf2-aeeb-e192b96d96e1</t>
+    <t>0ab327b9-0d46-465b-ad45-1b7e6f1dc53f</t>
+  </si>
+  <si>
+    <t>cd2cee0a-a52a-4b58-99f7-1f05936e9d6c</t>
+  </si>
+  <si>
+    <t>8406f92b-7934-4153-b3b4-cc5f286b53ca</t>
+  </si>
+  <si>
+    <t>03df60e8-4414-430c-9d1b-6dd030bf3825</t>
+  </si>
+  <si>
+    <t>6cfa8140-a036-4e82-a8ae-e9890cb34877</t>
   </si>
   <si>
     <t>Invalid value "68516-4" found in QUESTION_CODE</t>
@@ -678,34 +678,34 @@
     <t>The QUESTION_CODE "68516-4" of QUESTION_CODE_DESCRIPTION "On average, how many minutes did you usually spend exercising at this level on one of those days?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>68decd91-a5c3-41f3-a67c-ba26e7744e59</t>
-  </si>
-  <si>
-    <t>c96b8f07-6f15-4e80-9d33-0e104b8bb29c</t>
-  </si>
-  <si>
-    <t>402ed204-c824-449f-8307-2aecdb67fe9a</t>
-  </si>
-  <si>
-    <t>4a2b7728-35a8-4174-b8d3-e1c2fc2dfed3</t>
-  </si>
-  <si>
-    <t>f79aa222-93e4-4002-8915-6482c02fdd20</t>
-  </si>
-  <si>
-    <t>42b57c4d-f0f9-45ca-bf4c-5685e9d8873e</t>
-  </si>
-  <si>
-    <t>1093aa5e-2f6b-4acd-b7a7-166f9d916706</t>
-  </si>
-  <si>
-    <t>7a4786bb-1f58-4386-a824-0bce8c0b8540</t>
-  </si>
-  <si>
-    <t>ff4f9851-1ba3-4124-bc6f-d746102d9e4d</t>
-  </si>
-  <si>
-    <t>4c91f909-640f-47ce-a05f-d611b43c07be</t>
+    <t>5d95bb27-f9af-4327-b6e4-f4edf4d22f41</t>
+  </si>
+  <si>
+    <t>c2274b2f-f783-46a3-9791-95ddd16b9844</t>
+  </si>
+  <si>
+    <t>b1158a96-7d03-4dac-b5b2-3b17fbc8c100</t>
+  </si>
+  <si>
+    <t>e3367ccc-807d-4bb4-bd2f-3527899958e1</t>
+  </si>
+  <si>
+    <t>6d981628-3848-442d-8c01-983e23343ed7</t>
+  </si>
+  <si>
+    <t>d06b3a88-54d2-4f08-b8bb-d6f28431031d</t>
+  </si>
+  <si>
+    <t>c69c0970-83cb-46da-8b1a-358363bcc070</t>
+  </si>
+  <si>
+    <t>6c257f25-c808-4f6c-942b-0b602ecb5015</t>
+  </si>
+  <si>
+    <t>874d1721-7c6c-4174-b7c7-af689e515da3</t>
+  </si>
+  <si>
+    <t>d31dfd3e-2992-428e-a220-e74b2b31ca91</t>
   </si>
   <si>
     <t>Invalid value "89555-7" found in QUESTION_CODE</t>
@@ -717,28 +717,28 @@
     <t>The QUESTION_CODE "89555-7" of QUESTION_CODE_DESCRIPTION "In the last 30 days, other than the activities you did for work, on average, how many days per week did you engage in moderate exercise (like walking fast, running, jogging, dancing, swimming, biking, or other similar activities)" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>e7441233-1e8c-45ca-96cd-afc57e241a50</t>
-  </si>
-  <si>
-    <t>a0dc28d6-1e37-4b32-89c4-7214ee0c77bf</t>
-  </si>
-  <si>
-    <t>4c0d512c-340b-4463-8431-8cd61db22fd5</t>
-  </si>
-  <si>
-    <t>a4c61193-ec02-4053-ac58-189f106ff070</t>
-  </si>
-  <si>
-    <t>6a19d8e1-3df7-4bfd-b3d8-fa0d3733d72e</t>
-  </si>
-  <si>
-    <t>7a523c50-47fb-418f-851f-60d9b574d924</t>
-  </si>
-  <si>
-    <t>7fc5b2a7-f246-4e0a-9378-541e9026226a</t>
-  </si>
-  <si>
-    <t>c6883bd1-6ef8-4dee-a97f-4fa0eef81dff</t>
+    <t>e046e991-8eb9-4e48-8ef4-f0513cebb7af</t>
+  </si>
+  <si>
+    <t>ea7f3d8a-b394-4c2a-bfe6-e23d8fa435dd</t>
+  </si>
+  <si>
+    <t>55834042-340c-4841-963c-1a3b29188bef</t>
+  </si>
+  <si>
+    <t>b86067ef-dfd2-48b4-a9a6-f4b779aa5907</t>
+  </si>
+  <si>
+    <t>a2884190-b5a2-46d1-a33e-5a5b7e44b1b9</t>
+  </si>
+  <si>
+    <t>a01630fb-36c5-43a6-b359-0cfbdc4c4688</t>
+  </si>
+  <si>
+    <t>8c659026-2121-49be-aa84-4c311eccbcdb</t>
+  </si>
+  <si>
+    <t>3e0d8a1d-1922-4c63-8c20-9ee6a89782b3</t>
   </si>
   <si>
     <t>Invalid value "96782-8" found in QUESTION_CODE</t>
@@ -750,10 +750,10 @@
     <t>The QUESTION_CODE "96782-8" of QUESTION_CODE_DESCRIPTION "Do you want help with school or training? For example, starting or completing job training or getting a high school diploma, GED or equivalent." is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>fea1c890-c144-4768-b042-913e3a49c8e0</t>
-  </si>
-  <si>
-    <t>b3fa3ccc-78ad-4fbc-8edd-3b4df4c8be62</t>
+    <t>c0256116-c5f6-4544-ba40-0849177cf3d3</t>
+  </si>
+  <si>
+    <t>4509604c-d6ba-4530-ac15-de8969bc89e7</t>
   </si>
   <si>
     <t>Invalid value "97027-7" found in QUESTION_CODE</t>
@@ -765,10 +765,10 @@
     <t>The QUESTION_CODE "97027-7" of QUESTION_CODE_DESCRIPTION "Do you speak a language other than English at home?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>ebfc677d-a077-400e-a88d-eaf0256fc1fc</t>
-  </si>
-  <si>
-    <t>4b121f66-615c-46b8-9b1e-324bebb1dccf</t>
+    <t>28f57a2f-8476-46ff-8029-441c7e1c0f9a</t>
+  </si>
+  <si>
+    <t>76a78d17-4089-481a-8e46-9215601f86d5</t>
   </si>
   <si>
     <t>Invalid value "93159-2" found in QUESTION_CODE</t>
@@ -780,19 +780,19 @@
     <t>The QUESTION_CODE "93159-2" of QUESTION_CODE_DESCRIPTION "How often do you feel lonely or isolated from those around you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>9491e2ef-e574-497b-8622-367d55b4a4ef</t>
-  </si>
-  <si>
-    <t>47418a66-0d96-43ae-8933-408e317a8ce8</t>
-  </si>
-  <si>
-    <t>5945fe21-df67-4444-b7ef-c4d889944ba6</t>
-  </si>
-  <si>
-    <t>feb08f78-945d-4925-b7e0-562152848b88</t>
-  </si>
-  <si>
-    <t>27520fcc-9da7-4e32-9252-ed1684e6687d</t>
+    <t>87a85d1a-119a-4a1d-a25b-9eb374b18a92</t>
+  </si>
+  <si>
+    <t>228a68a1-44c8-4e31-8996-4356a241ce03</t>
+  </si>
+  <si>
+    <t>ca806489-f13f-43bf-80e5-7899a24966d8</t>
+  </si>
+  <si>
+    <t>7fc0933a-f915-4874-a96e-b19641965fbe</t>
+  </si>
+  <si>
+    <t>7f1e730f-be4b-43aa-844d-21d191b9afe2</t>
   </si>
   <si>
     <t>Invalid value "96781-0" found in QUESTION_CODE</t>
@@ -804,16 +804,16 @@
     <t>The QUESTION_CODE "96781-0" of QUESTION_CODE_DESCRIPTION "If for any reason you need help with day-to-day activities such as bathing, preparing meals, shopping, managing finances, etc., do you get the help you need?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>a3cc0402-78ce-43b6-9e64-8ed8a2abf758</t>
-  </si>
-  <si>
-    <t>7fb1ff47-466d-4a68-b357-742c05f231c6</t>
-  </si>
-  <si>
-    <t>3f6f091d-0257-4a64-8706-0352c1963adb</t>
-  </si>
-  <si>
-    <t>4a73c804-5bd2-46f2-b839-84d5b8d95ccc</t>
+    <t>350b9aa1-7873-4b63-9682-7020a9d5f0d6</t>
+  </si>
+  <si>
+    <t>2e3c9f73-e922-4652-8225-83e6c2afcef1</t>
+  </si>
+  <si>
+    <t>2bdbf7c1-6e17-4e9b-8a06-0bb6e6729671</t>
+  </si>
+  <si>
+    <t>3b51f035-1b4e-4262-a4df-0e1120b17e93</t>
   </si>
   <si>
     <t>Invalid value "96780-2" found in QUESTION_CODE</t>
@@ -825,13 +825,13 @@
     <t>The QUESTION_CODE "96780-2" of QUESTION_CODE_DESCRIPTION "Do you want help finding or keeping work or a job?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>71ac4ea2-125d-4d77-a45d-b73e81b4e0e5</t>
-  </si>
-  <si>
-    <t>72d5d119-5d1f-41a2-b135-63d05692da73</t>
-  </si>
-  <si>
-    <t>6b9ab95c-c388-445d-a23a-b5332cc7a55c</t>
+    <t>1e042273-b252-4d12-aadd-5a931b74b910</t>
+  </si>
+  <si>
+    <t>ead2ffc2-fde5-4d3c-8745-4a606e4cd80e</t>
+  </si>
+  <si>
+    <t>13be2bb0-89ee-41a3-b953-c9c05d9c7c64</t>
   </si>
   <si>
     <t>Invalid value "76513-1" found in QUESTION_CODE</t>
@@ -843,13 +843,13 @@
     <t>The QUESTION_CODE "76513-1" of QUESTION_CODE_DESCRIPTION "How hard is it for you to pay for the very basics like food, housing, medical care, and heating? Would you say it is" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>8a08d0ca-921d-4e5b-b0f6-65d9a84bd59a</t>
-  </si>
-  <si>
-    <t>f48ac24c-797a-4c3c-b88b-a909b371e011</t>
-  </si>
-  <si>
-    <t>f128bb67-9e08-4aa9-870f-74d7c785e94a</t>
+    <t>f55722da-7e74-4439-b182-be317a739903</t>
+  </si>
+  <si>
+    <t>e26a9934-31bd-4fac-8cda-93e815206c92</t>
+  </si>
+  <si>
+    <t>0c245ecc-b68f-486b-a752-e17c6e105a5c</t>
   </si>
   <si>
     <t>Invalid value "95615-1" found in QUESTION_CODE</t>
@@ -861,19 +861,19 @@
     <t>The QUESTION_CODE "95615-1" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, scream or curse at you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>dcba302b-75a8-4311-887c-cb9a553b5b56</t>
-  </si>
-  <si>
-    <t>66c39655-6c04-42c7-a973-5880e85b86e3</t>
-  </si>
-  <si>
-    <t>9e97f7d4-2d5e-4c18-af64-29447d401861</t>
-  </si>
-  <si>
-    <t>1a65c494-d8e5-4460-acaa-6aafa68d7a1f</t>
-  </si>
-  <si>
-    <t>65d6836d-a955-4451-a69f-08364e895f1d</t>
+    <t>7723b547-20dd-42b8-8bb8-7a32177324a9</t>
+  </si>
+  <si>
+    <t>04e5d591-9cab-41be-9cbc-89bd4ef80c8f</t>
+  </si>
+  <si>
+    <t>d2f8836b-ac82-4c16-80be-b61cae2bee34</t>
+  </si>
+  <si>
+    <t>bbdd66a6-21da-4f65-9030-215153adcfcf</t>
+  </si>
+  <si>
+    <t>acfe0583-349c-4cfd-8a95-712d331ef9e0</t>
   </si>
   <si>
     <t>Invalid value "95616-9" found in QUESTION_CODE</t>
@@ -885,19 +885,19 @@
     <t>The QUESTION_CODE "95616-9" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, threaten you with harm?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>a25a3192-7bb3-4e1b-ae72-b370657e4120</t>
-  </si>
-  <si>
-    <t>4a33df0f-9d5c-48d1-b4e4-639defb890d3</t>
-  </si>
-  <si>
-    <t>14c49a04-7f27-4bcc-ab26-a163766bdda4</t>
-  </si>
-  <si>
-    <t>a94783b6-b248-448f-aee0-743e76ad2dcb</t>
-  </si>
-  <si>
-    <t>94829422-fb29-4c24-9c93-dec931d38027</t>
+    <t>51cf83b9-275a-47a1-b191-0be20bad2355</t>
+  </si>
+  <si>
+    <t>fe893f03-860c-4c93-b260-b864687a535e</t>
+  </si>
+  <si>
+    <t>99d42e3f-1fb5-4cb8-a5af-4bbeeb238d66</t>
+  </si>
+  <si>
+    <t>5a46dcd5-61c9-4770-a843-e08abe0f07af</t>
+  </si>
+  <si>
+    <t>1510c3c5-6ea0-4727-a54f-6c37c093cd10</t>
   </si>
   <si>
     <t>Invalid value "95617-7" found in QUESTION_CODE</t>
@@ -909,19 +909,19 @@
     <t>The QUESTION_CODE "95617-7" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, insult or talk down to you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>7444d6dc-d842-4f45-be24-5a2af15fb967</t>
-  </si>
-  <si>
-    <t>33695f5a-4a63-4fb1-ab11-5d48492ab4b0</t>
-  </si>
-  <si>
-    <t>e973cc9a-fc07-4c69-a7f2-d2011aea3185</t>
-  </si>
-  <si>
-    <t>87848db4-1b4e-4b3d-b44f-5d9a6d71075c</t>
-  </si>
-  <si>
-    <t>a8285eae-5ae2-4dd4-92ed-0be411e725d6</t>
+    <t>53e4f0f7-fb2a-4439-8b76-fb6de535773a</t>
+  </si>
+  <si>
+    <t>d9bd2720-628f-40a1-9726-60b29eacc547</t>
+  </si>
+  <si>
+    <t>90cbcc9c-8ff1-4749-8a1a-1585025883ce</t>
+  </si>
+  <si>
+    <t>7c62a06a-d774-49ca-b795-11abcfcdda3e</t>
+  </si>
+  <si>
+    <t>0e203110-5bae-4633-a394-8d5b56961d82</t>
   </si>
   <si>
     <t>Invalid value "95618-5" found in QUESTION_CODE</t>
@@ -933,19 +933,19 @@
     <t>The QUESTION_CODE "95618-5" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, physically hurt you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>4c1a9f2b-8c08-487d-ade1-86d4ea9801a5</t>
-  </si>
-  <si>
-    <t>d40477ee-7170-4a46-a8ed-39c7d9487212</t>
-  </si>
-  <si>
-    <t>4acf2f7c-e792-4c73-a3f7-d1b98a80e028</t>
-  </si>
-  <si>
-    <t>c631c8f1-4510-4396-843a-9a2d621c226e</t>
-  </si>
-  <si>
-    <t>2a135b2c-772f-44e1-b93d-d4241e988628</t>
+    <t>226ef428-913d-4210-a116-f65275fb5adb</t>
+  </si>
+  <si>
+    <t>0320e909-f0c3-44e5-a70d-9f78f79dd3cd</t>
+  </si>
+  <si>
+    <t>b4848954-585b-4485-a9fb-1deb64f8285c</t>
+  </si>
+  <si>
+    <t>3d3f9ee3-623c-411e-8209-9708dfabb7c7</t>
+  </si>
+  <si>
+    <t>eeb2cbcb-40d9-4b1b-9f8a-0858e4e8b12b</t>
   </si>
   <si>
     <t>Invalid value "96779-4" found in QUESTION_CODE</t>
@@ -957,13 +957,13 @@
     <t>The QUESTION_CODE "96779-4" of QUESTION_CODE_DESCRIPTION "In the past 12 months has the electric, gas, oil, or water company threatened to shut off services in your home?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>b65219e5-67be-49f4-b666-08dcf19f6ac4</t>
-  </si>
-  <si>
-    <t>344a45c8-584d-478e-9c62-3979727e0a4e</t>
-  </si>
-  <si>
-    <t>614c2af3-e344-415f-85c8-4c01296e967c</t>
+    <t>f32ecd3a-0296-4736-b171-55f9a7f796c1</t>
+  </si>
+  <si>
+    <t>6399f78e-84e5-4eea-b02b-18a4f95e2484</t>
+  </si>
+  <si>
+    <t>77fc3dac-a5cd-4ab7-bb56-0ff0cd939dab</t>
   </si>
   <si>
     <t>Invalid value "93030-5" found in QUESTION_CODE</t>
@@ -975,10 +975,10 @@
     <t>The QUESTION_CODE "93030-5" of QUESTION_CODE_DESCRIPTION "In the past 12 months, has lack of reliable transportation kept you from medical appointments, meetings, work or from getting things needed for daily living?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>5ba4cad2-93e7-4ad5-8201-c21f88510876</t>
-  </si>
-  <si>
-    <t>9bea84e8-35eb-4e61-bfbd-26eaf8be35b9</t>
+    <t>fd4f67d4-d54e-46ad-a1be-3efc78944e5b</t>
+  </si>
+  <si>
+    <t>9720ddbd-99cf-4e67-9ccd-8170d0acf84e</t>
   </si>
   <si>
     <t>Invalid value "88123-5" found in QUESTION_CODE</t>
@@ -990,13 +990,13 @@
     <t>The QUESTION_CODE "88123-5" of QUESTION_CODE_DESCRIPTION "Within the past 12 months, the food you bought just didn't last and you didn't have money to get more." is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>2450c9d4-9e71-459f-9cff-dc4cb7754c03</t>
-  </si>
-  <si>
-    <t>0e92569f-d4e0-4ab6-9880-46b7a67de43c</t>
-  </si>
-  <si>
-    <t>19a01fad-2dd3-4205-b6fc-54ed8722f980</t>
+    <t>5e47fc5e-fd16-4ca3-8aa6-693d5e78e2fc</t>
+  </si>
+  <si>
+    <t>7089d0f7-053a-4f9e-8233-2e25334cc3ee</t>
+  </si>
+  <si>
+    <t>365c4546-d3cc-4f92-9d8a-bb6069d7e37e</t>
   </si>
   <si>
     <t>Invalid value "96778-6" found in QUESTION_CODE</t>
@@ -1008,28 +1008,28 @@
     <t>The QUESTION_CODE "96778-6" of QUESTION_CODE_DESCRIPTION "Think about the place you live. Do you have problems with any of the following?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>cd2805c9-7f1d-4587-9be3-2a40a58cc649</t>
-  </si>
-  <si>
-    <t>387c4ed4-1677-4194-aa33-19ff745a8772</t>
-  </si>
-  <si>
-    <t>72b706a4-950a-4f54-a8c1-d779de46dbcd</t>
-  </si>
-  <si>
-    <t>89d2339c-ead3-4aff-8183-4ea6fe7d1c80</t>
-  </si>
-  <si>
-    <t>41ea2112-031b-4d4d-850b-8774a4be6304</t>
-  </si>
-  <si>
-    <t>df2f4d06-6ffb-4fb0-b20e-577c5561a889</t>
-  </si>
-  <si>
-    <t>c09ffb6f-4070-4c39-b129-301affe44d9f</t>
-  </si>
-  <si>
-    <t>7d41d228-cf85-4c77-9b60-434af97b78fd</t>
+    <t>c62bf1e9-0323-48de-93cc-24e5c282a1f4</t>
+  </si>
+  <si>
+    <t>090b4d5d-d8d7-4bf0-8a3c-66ca6c6b2062</t>
+  </si>
+  <si>
+    <t>1f49c97b-6ec5-4c7c-ae8c-0647498f8580</t>
+  </si>
+  <si>
+    <t>e8b5615c-8019-4fde-a0d4-cde166ee7912</t>
+  </si>
+  <si>
+    <t>314b893c-0bfa-4d43-9f35-4863a7ba92f7</t>
+  </si>
+  <si>
+    <t>06d693e3-da4d-4b02-9c90-28d46fe1e757</t>
+  </si>
+  <si>
+    <t>cd98dd3a-cda4-4b9c-90e7-c65011ee47f1</t>
+  </si>
+  <si>
+    <t>08dee596-4b55-443c-a132-95096baef18d</t>
   </si>
   <si>
     <t>Invalid value "71802-3" found in QUESTION_CODE</t>
@@ -1041,10 +1041,10 @@
     <t>The QUESTION_CODE "71802-3" of QUESTION_CODE_DESCRIPTION "What is your living situation today?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>8acc0107-6c08-4a36-b38b-e1d8e2116a9a</t>
-  </si>
-  <si>
-    <t>68c444b1-d8d5-42fb-991b-7e7334b504a1</t>
+    <t>78f67f03-0588-42f0-8bb4-9d6e84935d88</t>
+  </si>
+  <si>
+    <t>988a3fd7-8637-4ec8-a649-ae763485f7e5</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -1197,7 +1197,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>a853f09d-f2c0-4268-a8cb-251306ce09c8</t>
+    <t>c76cae54-6214-42e8-9af5-cd11cc221e3b</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
feat: update observation resource for generating FHIR Bundle based on SHINNY IG specification #67
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>a1bcd225-38c1-41dc-ba77-02cd2193d596</t>
+    <t>d581987c-0790-4ce6-9402-82aa0e578f2f</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -117,7 +117,7 @@
     <t/>
   </si>
   <si>
-    <t>2dbd073c-6684-4224-bb4c-a91ca15222a4</t>
+    <t>9786dcd4-83c0-40cf-9d88-6e7546b7206d</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -141,7 +141,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>0244304a-5deb-48da-875a-627182e9e89b</t>
+    <t>c42d5cf2-4eea-43bc-b41c-f0ada3d82ae3</t>
   </si>
   <si>
     <t>Invalid value "LA6729-3" found in ANSWER_CODE</t>
@@ -156,7 +156,7 @@
     <t>The ANSWER_CODE "LA6729-3" of ANSWER_CODE_DESCRIPTION "Sometimes true" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>026f475b-1f07-4fda-b482-105264f86fd2</t>
+    <t>6016edd8-ea21-4862-b337-20f06be2d78f</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -186,7 +186,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>7b8faadd-6850-401c-8b0c-2ac7dd11c42c</t>
+    <t>cd7d700d-8fa4-4c81-af62-8778878c7a4d</t>
   </si>
   <si>
     <t>Invalid value "UNK" found in SEX_AT_BIRTH_CODE</t>
@@ -201,7 +201,7 @@
     <t>The SEX_AT_BIRTH_CODE "UNK" of SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" is not matching with the SEX_AT_BIRTH_CODE of SEX_AT_BIRTH_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>6625dac4-cae1-4679-82c2-0917df6bf522</t>
+    <t>7b9e03b0-385c-49ac-94a4-d8c3c925a492</t>
   </si>
   <si>
     <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
@@ -219,7 +219,7 @@
     <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
   </si>
   <si>
-    <t>3ce331ee-5dc8-42d7-a7f7-b97ffd1c5751</t>
+    <t>e5e3d881-353d-4aed-a19d-b9ba6395a6c1</t>
   </si>
   <si>
     <t>Invalid value "1142-9" found in RACE_CODE</t>
@@ -234,7 +234,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>33d51eb2-8ad2-4328-824a-1f8b5f795cde</t>
+    <t>99e02555-2865-4552-86f0-159c2dc3721b</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -252,25 +252,25 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>2dcf1ec1-b9cd-4130-8f25-94815546c0eb</t>
-  </si>
-  <si>
-    <t>44463e7d-a7dc-419c-9637-6a35ea551d02</t>
-  </si>
-  <si>
-    <t>3011a340-e82b-4b7e-b2de-1c6ce6d7a64b</t>
-  </si>
-  <si>
-    <t>dbbad070-10bc-4ba3-8ab0-2ed53fb5db9b</t>
-  </si>
-  <si>
-    <t>7b0ebc60-137d-4566-91e6-3ccfc897a2fb</t>
-  </si>
-  <si>
-    <t>4b5d504e-fcaf-460a-9e41-d767f2be504f</t>
-  </si>
-  <si>
-    <t>28f5cba4-6f00-4644-9da8-7d0bd9552050</t>
+    <t>1b1f11e8-0d0b-4509-a43b-37ff16cbffc0</t>
+  </si>
+  <si>
+    <t>d53350f5-ad64-4db5-9aca-6a1c34110a31</t>
+  </si>
+  <si>
+    <t>e63329b5-6b65-44c9-852e-ee4e716d6fbd</t>
+  </si>
+  <si>
+    <t>becd9ce6-6fd6-4813-bced-b425a8c31ff3</t>
+  </si>
+  <si>
+    <t>12bc3ce1-3237-433c-ab40-25178edc4882</t>
+  </si>
+  <si>
+    <t>26cb79b8-48e5-41b5-9f26-54675d1c770d</t>
+  </si>
+  <si>
+    <t>06541c4a-2abd-4293-80e7-a8710ba096d6</t>
   </si>
   <si>
     <t>Invalid value "LA6571-9" found in ANSWER_CODE</t>
@@ -282,16 +282,16 @@
     <t>The ANSWER_CODE "LA6571-9" of ANSWER_CODE_DESCRIPTION "Nearly every day" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>89f31848-70e7-4d5c-9c2a-73ca02e3cdb7</t>
-  </si>
-  <si>
-    <t>b9e6e10f-eb9a-49e5-a3fa-6dea8584ecdc</t>
-  </si>
-  <si>
-    <t>d886d3e9-fc19-414d-b847-0ba764eaa70e</t>
-  </si>
-  <si>
-    <t>c4996409-8355-45b6-95a8-b721d815150a</t>
+    <t>99b0f6a8-6273-4ce1-9e64-c495b43fdf95</t>
+  </si>
+  <si>
+    <t>b9ee4ab4-a4d7-40b6-870b-bddd0c5eae59</t>
+  </si>
+  <si>
+    <t>d4aafff1-5a71-4e12-ad49-8f74f3707568</t>
+  </si>
+  <si>
+    <t>2d4cd45c-3134-43f1-bcb1-850edc931eae</t>
   </si>
   <si>
     <t>Invalid value "LA6569-3" found in ANSWER_CODE</t>
@@ -303,25 +303,25 @@
     <t>The ANSWER_CODE "LA6569-3" of ANSWER_CODE_DESCRIPTION "Several days" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>32556711-1f15-48ee-8b47-22aa919daab9</t>
-  </si>
-  <si>
-    <t>028f835f-37d1-4395-b2b1-de57d76803cd</t>
-  </si>
-  <si>
-    <t>efd473db-0aba-47e4-b2fb-01b4fa608999</t>
-  </si>
-  <si>
-    <t>23dd376f-566f-4e49-abbd-2779b2028319</t>
-  </si>
-  <si>
-    <t>d146a4dd-00da-442d-ba17-1fab3b3d84ac</t>
-  </si>
-  <si>
-    <t>013363e2-fe12-49f6-ba93-6c6afa64e762</t>
-  </si>
-  <si>
-    <t>64354630-7e22-48eb-a5ec-9b400ebbc5e9</t>
+    <t>1d0fc0c0-df09-4127-b443-a9cd1606eb1e</t>
+  </si>
+  <si>
+    <t>e5ccd776-17c8-4766-8afa-0afbce0732be</t>
+  </si>
+  <si>
+    <t>df7878c8-a62a-48fb-9f04-fe88ee3e7d94</t>
+  </si>
+  <si>
+    <t>d5642072-bbdd-4ce4-978e-32dd71bee55f</t>
+  </si>
+  <si>
+    <t>e3097184-0fa6-4e37-b54c-d220ae1e4416</t>
+  </si>
+  <si>
+    <t>8b6bce6f-1147-4562-bdd5-2f83366f7116</t>
+  </si>
+  <si>
+    <t>b5189876-7972-442d-95f5-f90870daac66</t>
   </si>
   <si>
     <t>Invalid value "69861-3" found in QUESTION_CODE</t>
@@ -333,19 +333,19 @@
     <t>The QUESTION_CODE "69861-3" of QUESTION_CODE_DESCRIPTION "Because of a physical, mental, or emotional condition, do you have difficulty doing errands alone such as visiting a physician's office or shopping" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>5147668f-02fa-43bf-a232-411b0011f374</t>
-  </si>
-  <si>
-    <t>356ca88d-410a-4803-ac69-47f536f47977</t>
-  </si>
-  <si>
-    <t>fa2ec750-ef9b-430e-accc-09a037cf049f</t>
-  </si>
-  <si>
-    <t>04f1fc8d-fe47-4689-80e1-3a6af42f3a25</t>
-  </si>
-  <si>
-    <t>99f54569-f1ed-4cf8-8b23-fb5f259ddd2a</t>
+    <t>92d4a412-1eff-43ce-b8b7-21a7aad86c1e</t>
+  </si>
+  <si>
+    <t>a22b4ab1-ad3b-4cdb-a79a-cc2a15af1582</t>
+  </si>
+  <si>
+    <t>38b12b40-b850-45ba-8534-e3df0be1fb95</t>
+  </si>
+  <si>
+    <t>a3784cc3-02e1-45a1-8b0f-a8896d6bdf9f</t>
+  </si>
+  <si>
+    <t>9406f52d-f6d5-4614-982e-1ff4792d4919</t>
   </si>
   <si>
     <t>Invalid value "LA31983-2" found in ANSWER_CODE</t>
@@ -357,7 +357,7 @@
     <t>The ANSWER_CODE "LA31983-2" of ANSWER_CODE_DESCRIPTION "I do not need or want help" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>afb5a289-b43c-448d-be33-ec669bf1ff4b</t>
+    <t>3815d48b-5dcc-4242-91cd-7ced54f119e4</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -369,10 +369,10 @@
     <t>Provide a value for POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>824464b1-0c1b-45f9-9d9c-e4a5116e20ee</t>
-  </si>
-  <si>
-    <t>d86d77e9-84b1-4d75-b7d6-82b100461f48</t>
+    <t>2e3c4911-d8b0-41dd-a2a3-c1d331796e60</t>
+  </si>
+  <si>
+    <t>52befe13-cd2b-4b55-bb0e-ac48b4c36ab2</t>
   </si>
   <si>
     <t>Invalid value "69858-9" found in QUESTION_CODE</t>
@@ -384,7 +384,7 @@
     <t>The QUESTION_CODE "69858-9" of QUESTION_CODE_DESCRIPTION "Because of a physical, mental, or emotional condition, do you have serious difficulty concentrating, remembering, or making decisions?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>f6452619-643c-4803-9934-d8fd5e3f39ce</t>
+    <t>eed12e3b-9053-4229-9870-1cdebbfb6823</t>
   </si>
   <si>
     <t>Invalid value "LA16644-9" found in ANSWER_CODE</t>
@@ -396,22 +396,22 @@
     <t>The ANSWER_CODE "LA16644-9" of ANSWER_CODE_DESCRIPTION "Fairly often" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>bbf0765f-ffa2-4700-9509-0d826e427157</t>
-  </si>
-  <si>
-    <t>d45208ae-beec-4494-a328-196bd7bdbc79</t>
-  </si>
-  <si>
-    <t>526116c7-4e05-4dc3-8a2b-549d9b3b2fe3</t>
-  </si>
-  <si>
-    <t>80b4e25d-ba60-43f3-8c30-894d9de52a3a</t>
-  </si>
-  <si>
-    <t>5b032a52-619d-40fd-b0bd-06faeee229f7</t>
-  </si>
-  <si>
-    <t>8654345f-2c5d-491d-8c4e-486967444406</t>
+    <t>754e11dd-db16-4678-87c2-d596eba882f3</t>
+  </si>
+  <si>
+    <t>b5a113ad-dda4-4b62-a5bc-b3ed9f95d7b2</t>
+  </si>
+  <si>
+    <t>25662acc-ac37-4d75-b78a-dbf86d7fcabd</t>
+  </si>
+  <si>
+    <t>27b76015-b643-41f3-8e3d-14b6bdf5640a</t>
+  </si>
+  <si>
+    <t>bf7251b9-ef69-4bdf-89f9-6254e91ad264</t>
+  </si>
+  <si>
+    <t>15847fe6-fb87-4a40-8b2a-43aafe4a1043</t>
   </si>
   <si>
     <t>Invalid value "93038-8" found in QUESTION_CODE</t>
@@ -423,25 +423,25 @@
     <t>The QUESTION_CODE "93038-8" of QUESTION_CODE_DESCRIPTION "Stress means a situation in which a person feels tense, restless, nervous, or anxious, or is unable to sleep at night because his or her mind is troubled all the time. Do you feel this kind of stress these days?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>767f2996-7ca0-4966-9d26-2ace48e272e6</t>
-  </si>
-  <si>
-    <t>93e03c23-a563-4441-bf83-da1750557c44</t>
-  </si>
-  <si>
-    <t>dc82faa1-2368-4be5-adb4-3bf887f76457</t>
-  </si>
-  <si>
-    <t>3abde441-aed7-4571-85af-52117905b126</t>
-  </si>
-  <si>
-    <t>eff18ffb-c6c3-4a47-8585-144989e29b43</t>
-  </si>
-  <si>
-    <t>40514b18-159d-4a5f-ac16-2adf6bde21da</t>
-  </si>
-  <si>
-    <t>312ef8f2-102c-457f-8acb-32dcdee2ade1</t>
+    <t>9b2e1792-88f3-4a41-8078-f7080e637df8</t>
+  </si>
+  <si>
+    <t>6f0cae53-547e-4713-87fb-16d8fce111d2</t>
+  </si>
+  <si>
+    <t>f6a0077e-8116-4ccf-91cf-d6db057a50b9</t>
+  </si>
+  <si>
+    <t>e9328f02-58f1-4b27-8bfb-3ea80f4dc23e</t>
+  </si>
+  <si>
+    <t>4b747da0-88f0-4f57-be70-4396244d457e</t>
+  </si>
+  <si>
+    <t>d676e89d-fd22-4947-bbaa-37da8cac1cc4</t>
+  </si>
+  <si>
+    <t>e72ffb9f-d50a-4c72-b0f2-f950c9644034</t>
   </si>
   <si>
     <t>Invalid value "LA32002-0" found in ANSWER_CODE</t>
@@ -453,31 +453,31 @@
     <t>The ANSWER_CODE "LA32002-0" of ANSWER_CODE_DESCRIPTION "Already shut off" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>40a6be8c-599c-458b-b9d5-84d852ca15b1</t>
-  </si>
-  <si>
-    <t>0c65eae8-d47c-4e00-b2cb-99c76621a0ec</t>
-  </si>
-  <si>
-    <t>4f70c607-e509-43b4-937d-5806775ba5cf</t>
-  </si>
-  <si>
-    <t>aba6753f-52d0-4a2d-acf1-cbdeff656287</t>
-  </si>
-  <si>
-    <t>d07efb67-2f11-4c57-a7b1-5118a03327b4</t>
-  </si>
-  <si>
-    <t>cec0699f-5a01-4cc5-bc7e-c5e688240bbc</t>
-  </si>
-  <si>
-    <t>2630f5fd-b9a5-4a7c-b8c7-bb7b9897d473</t>
-  </si>
-  <si>
-    <t>25266ec9-5a20-42e9-bd8b-598c4123d7c4</t>
-  </si>
-  <si>
-    <t>c1599033-6475-48e4-862b-0394eb7a66cc</t>
+    <t>017cabc5-2754-4be5-860e-5de15bab9594</t>
+  </si>
+  <si>
+    <t>853a5bfb-2a38-48de-a3ad-615344b4daf6</t>
+  </si>
+  <si>
+    <t>2e8d50b5-d694-428b-bf53-41945b60701a</t>
+  </si>
+  <si>
+    <t>b3f2b990-496f-4acb-be35-74c80b0d16d7</t>
+  </si>
+  <si>
+    <t>909ef15a-3b3c-4baa-97a5-cf79c19b97a8</t>
+  </si>
+  <si>
+    <t>e7db4778-f263-4e3b-97b1-2a4d593985b1</t>
+  </si>
+  <si>
+    <t>c6847d4b-cc04-42f0-8da9-7cd12298284b</t>
+  </si>
+  <si>
+    <t>64cf5fa4-ed2d-4c37-8526-cd56916d0b0b</t>
+  </si>
+  <si>
+    <t>792092a0-e67c-4fd1-a823-ad93faa9ad9d</t>
   </si>
   <si>
     <t>Invalid value "LA31997-2" found in ANSWER_CODE</t>
@@ -489,10 +489,10 @@
     <t>The ANSWER_CODE "LA31997-2" of ANSWER_CODE_DESCRIPTION "Lead paint or pipes" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>de1c606d-8abc-455a-947b-b0cf82c11418</t>
-  </si>
-  <si>
-    <t>d10943bf-66d3-43cd-ba7b-c48f5faf9b10</t>
+    <t>9cf9c3a1-a724-4cd0-a0c5-d6aa73869cc1</t>
+  </si>
+  <si>
+    <t>5c0c2ba0-3920-4bda-b095-e4303ad4814d</t>
   </si>
   <si>
     <t>Invalid value "44255-8" found in QUESTION_CODE</t>
@@ -504,7 +504,7 @@
     <t>The QUESTION_CODE "44255-8" of QUESTION_CODE_DESCRIPTION "Feeling down, depressed, or hopeless?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>f421ac6a-f469-4e56-855f-375546663940</t>
+    <t>0966bece-8eae-4ed3-9f7f-68bd3ae77230</t>
   </si>
   <si>
     <t>Invalid value "LA31994-9" found in ANSWER_CODE</t>
@@ -516,25 +516,25 @@
     <t>The ANSWER_CODE "LA31994-9" of ANSWER_CODE_DESCRIPTION "I have a place to live today, but I am worried about losing it in the future" is not matching with the ANSWER_CODE of ANSWER_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>cf3b7ecc-1174-4007-ad37-6af41f4325f9</t>
-  </si>
-  <si>
-    <t>dbb4167a-7b7f-46aa-b63e-b6aca7e3ec0a</t>
-  </si>
-  <si>
-    <t>14f2856e-96ca-4945-9058-38f23556911f</t>
-  </si>
-  <si>
-    <t>4667e558-62d3-485e-8a2f-461931879bd6</t>
-  </si>
-  <si>
-    <t>73276c43-50a5-45c4-8598-b631972ec0ef</t>
-  </si>
-  <si>
-    <t>138043b7-9296-40b6-bb9f-af77d9374047</t>
-  </si>
-  <si>
-    <t>6da64f13-3237-4f72-a733-1cc76ea361e8</t>
+    <t>a1ed3541-cdbc-4e02-b2a5-4531531f1e6b</t>
+  </si>
+  <si>
+    <t>c1b69c19-8287-4f5d-857c-d839cf627788</t>
+  </si>
+  <si>
+    <t>b92c0daa-2e2e-4fe6-b586-e625b96e1a5b</t>
+  </si>
+  <si>
+    <t>3cc0c4e4-f886-4456-a3ce-ecec4679aa54</t>
+  </si>
+  <si>
+    <t>a7d51c42-3f3f-4eb7-81f9-6d8eeb7a6f9d</t>
+  </si>
+  <si>
+    <t>d689ac33-1a27-47fa-af14-e27c86e97abd</t>
+  </si>
+  <si>
+    <t>30f2d4f6-d170-4097-b596-7785570d8629</t>
   </si>
   <si>
     <t>Invalid timestamp "01/27/02 15:42" found in RECORDED_TIME</t>
@@ -543,7 +543,7 @@
     <t>01/27/02 15:42</t>
   </si>
   <si>
-    <t>9f1763cc-cbdb-468c-a436-7a70b4e315f6</t>
+    <t>2039a4f8-cb67-4c35-86a0-a1d1ff53ee90</t>
   </si>
   <si>
     <t>Invalid value "44250-9" found in QUESTION_CODE</t>
@@ -555,28 +555,28 @@
     <t>The QUESTION_CODE "44250-9" of QUESTION_CODE_DESCRIPTION "Little interest or pleasure in doing things?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>85959c3d-5f97-41f6-a8d4-5558a0a3ffde</t>
-  </si>
-  <si>
-    <t>c09995e2-a81d-4c2f-8264-df31c5d91ce9</t>
-  </si>
-  <si>
-    <t>f6a6a254-7114-4e25-bbc0-e8bfb978b02a</t>
-  </si>
-  <si>
-    <t>2aa5cce0-a98d-4bfb-84b3-07fd8d2559a6</t>
-  </si>
-  <si>
-    <t>af12fd1c-2975-489d-81a6-e0c1b138f6b0</t>
-  </si>
-  <si>
-    <t>3571ce63-68f4-4dbf-b49a-390aea0241d0</t>
-  </si>
-  <si>
-    <t>1261d7ca-3896-4e7d-a05f-e7ad5f4f4eb7</t>
-  </si>
-  <si>
-    <t>aa522703-b495-45b7-91d3-38ddf24dc9ee</t>
+    <t>f4518ce7-d1fd-4db7-a6ea-a0e2ac705ab8</t>
+  </si>
+  <si>
+    <t>a581a358-4e11-4ad0-93ed-58bd2bbb7ef8</t>
+  </si>
+  <si>
+    <t>6bea34f0-0457-4e3d-9bcf-3225705d938f</t>
+  </si>
+  <si>
+    <t>5f060223-227c-44a4-9384-9e1e58a210db</t>
+  </si>
+  <si>
+    <t>894d8992-3133-4aee-8c19-d426a448cb38</t>
+  </si>
+  <si>
+    <t>bde3cd07-a715-4fd1-afd5-9e759eb1fb9a</t>
+  </si>
+  <si>
+    <t>ba81fdcd-6c46-4e65-bc3f-902abc62bda9</t>
+  </si>
+  <si>
+    <t>1332f845-af6d-4381-ae45-dd9943ae9d46</t>
   </si>
   <si>
     <t>Invalid value "95530-2" found in QUESTION_CODE</t>
@@ -588,34 +588,34 @@
     <t>The QUESTION_CODE "95530-2" of QUESTION_CODE_DESCRIPTION "How many times in the past year have you used prescription drugs for non-medical reasons?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>18dbf305-d7b9-4aea-9996-a6e8c1bc90c6</t>
-  </si>
-  <si>
-    <t>ca13a2c5-bb8a-4409-bcf2-908ab6e2691e</t>
-  </si>
-  <si>
-    <t>215aee41-f0fa-4cfd-99e8-366be7f2e9a1</t>
-  </si>
-  <si>
-    <t>e4efb683-4e31-416e-b09a-5c7ed990bae8</t>
-  </si>
-  <si>
-    <t>a0c615c9-d1dd-4fb9-b075-f73ee2b382fb</t>
-  </si>
-  <si>
-    <t>d9a66f4b-c730-40fa-8260-9c8c088e4adc</t>
-  </si>
-  <si>
-    <t>7a1ac753-5106-403e-b204-2be8f379c7cc</t>
-  </si>
-  <si>
-    <t>31ffa4b5-990d-4f80-802c-a4194451bf17</t>
-  </si>
-  <si>
-    <t>0c0acf40-e9a5-4dcc-926c-38cbbb262935</t>
-  </si>
-  <si>
-    <t>7e0429e9-681f-45bf-a029-571142c593bc</t>
+    <t>ec1ed839-b604-463e-a8b7-228ecccd6f4d</t>
+  </si>
+  <si>
+    <t>70333eaa-5432-4dd4-b3da-1b6067f39b56</t>
+  </si>
+  <si>
+    <t>6ed42d19-9391-451f-987b-b6428475f33c</t>
+  </si>
+  <si>
+    <t>ce6dfe18-8508-49ce-bcce-51511f64ffcd</t>
+  </si>
+  <si>
+    <t>be5ac01e-113e-4d13-b7bb-4d2fe3004d37</t>
+  </si>
+  <si>
+    <t>cf36567a-fa7e-4eac-a107-76db81050426</t>
+  </si>
+  <si>
+    <t>22e64b94-14f8-4f46-b014-313b15ad9f91</t>
+  </si>
+  <si>
+    <t>b7987cf3-eb60-4628-b912-f2924334e199</t>
+  </si>
+  <si>
+    <t>0795995a-d7c1-4d45-8b21-92884f4e13b2</t>
+  </si>
+  <si>
+    <t>76978555-375a-4864-9eed-d3bf8f866f24</t>
   </si>
   <si>
     <t>Invalid value "96842-0" found in QUESTION_CODE</t>
@@ -627,22 +627,22 @@
     <t>The QUESTION_CODE "96842-0" of QUESTION_CODE_DESCRIPTION "How many times in the past 12 months have you used tobacco products (like cigarettes, cigars, snuff, chew, electronic cigarettes)?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>36895c4c-8a5f-4c5f-aa15-c5210ee8ae59</t>
-  </si>
-  <si>
-    <t>4e9d6ecf-c8ef-4f23-85be-68f59179cc57</t>
-  </si>
-  <si>
-    <t>bc882015-bb26-47f7-9285-30be66c23c31</t>
-  </si>
-  <si>
-    <t>102df668-587f-44ef-a67b-78e94ef0e5b7</t>
-  </si>
-  <si>
-    <t>7fc48b4d-e92e-4d2b-a489-126c5b021d72</t>
-  </si>
-  <si>
-    <t>595bef24-4546-4cdb-b233-7913ee3cd4fc</t>
+    <t>30440734-5aa4-41ae-9eda-d25fd945ad9b</t>
+  </si>
+  <si>
+    <t>9049ecb4-c71f-493a-ac9a-3a03d7609f1a</t>
+  </si>
+  <si>
+    <t>a8b1bd01-11af-4deb-a3b8-9923560af0f8</t>
+  </si>
+  <si>
+    <t>2e9c43db-c153-4b1a-9670-0517df46bb89</t>
+  </si>
+  <si>
+    <t>1d3d763e-b02a-4237-99b9-09160fdd025e</t>
+  </si>
+  <si>
+    <t>bce8a8fd-3b3d-4964-9bca-8a9bccfccd94</t>
   </si>
   <si>
     <t>Invalid value "68517-2" found in QUESTION_CODE</t>
@@ -654,19 +654,19 @@
     <t>The QUESTION_CODE "68517-2" of QUESTION_CODE_DESCRIPTION "How many times in the past 12 months have you had 5 or more drinks in a day (males) or 4 or more drinks in a day (females)?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>0ab327b9-0d46-465b-ad45-1b7e6f1dc53f</t>
-  </si>
-  <si>
-    <t>cd2cee0a-a52a-4b58-99f7-1f05936e9d6c</t>
-  </si>
-  <si>
-    <t>8406f92b-7934-4153-b3b4-cc5f286b53ca</t>
-  </si>
-  <si>
-    <t>03df60e8-4414-430c-9d1b-6dd030bf3825</t>
-  </si>
-  <si>
-    <t>6cfa8140-a036-4e82-a8ae-e9890cb34877</t>
+    <t>0395db6d-9bb0-4f0a-8dd5-8738acb56078</t>
+  </si>
+  <si>
+    <t>58640cf0-4751-4432-a925-9c4602d0577a</t>
+  </si>
+  <si>
+    <t>ff66329e-db42-4df8-8038-b87c3db60c20</t>
+  </si>
+  <si>
+    <t>c21f7c06-b481-4b02-915c-74cd68f7f38e</t>
+  </si>
+  <si>
+    <t>c17bbb84-1e37-46d6-aefa-9d4c7c775304</t>
   </si>
   <si>
     <t>Invalid value "68516-4" found in QUESTION_CODE</t>
@@ -678,34 +678,34 @@
     <t>The QUESTION_CODE "68516-4" of QUESTION_CODE_DESCRIPTION "On average, how many minutes did you usually spend exercising at this level on one of those days?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>5d95bb27-f9af-4327-b6e4-f4edf4d22f41</t>
-  </si>
-  <si>
-    <t>c2274b2f-f783-46a3-9791-95ddd16b9844</t>
-  </si>
-  <si>
-    <t>b1158a96-7d03-4dac-b5b2-3b17fbc8c100</t>
-  </si>
-  <si>
-    <t>e3367ccc-807d-4bb4-bd2f-3527899958e1</t>
-  </si>
-  <si>
-    <t>6d981628-3848-442d-8c01-983e23343ed7</t>
-  </si>
-  <si>
-    <t>d06b3a88-54d2-4f08-b8bb-d6f28431031d</t>
-  </si>
-  <si>
-    <t>c69c0970-83cb-46da-8b1a-358363bcc070</t>
-  </si>
-  <si>
-    <t>6c257f25-c808-4f6c-942b-0b602ecb5015</t>
-  </si>
-  <si>
-    <t>874d1721-7c6c-4174-b7c7-af689e515da3</t>
-  </si>
-  <si>
-    <t>d31dfd3e-2992-428e-a220-e74b2b31ca91</t>
+    <t>3e62027a-9c6a-440c-9db9-027b51f13e76</t>
+  </si>
+  <si>
+    <t>cad83c8b-d824-421c-bdc9-f0aebd61e7fc</t>
+  </si>
+  <si>
+    <t>06a64437-1071-4ace-af4e-42ae3240f60a</t>
+  </si>
+  <si>
+    <t>8e676b28-c10e-473e-9eb4-e1f2d5c35825</t>
+  </si>
+  <si>
+    <t>71cb4322-e382-4ee4-aa0f-812186b9898a</t>
+  </si>
+  <si>
+    <t>69d13a1a-3190-4c68-a59f-3712588a1357</t>
+  </si>
+  <si>
+    <t>7d072c64-1895-44da-b1ca-fd9ed203256e</t>
+  </si>
+  <si>
+    <t>9880cdb5-fc78-491b-9523-f54c83847712</t>
+  </si>
+  <si>
+    <t>bd5a0e6f-cbe0-4b62-ad46-4f5aaf7989c3</t>
+  </si>
+  <si>
+    <t>fbf14e02-429c-404a-9288-8e6b818c0921</t>
   </si>
   <si>
     <t>Invalid value "89555-7" found in QUESTION_CODE</t>
@@ -717,28 +717,28 @@
     <t>The QUESTION_CODE "89555-7" of QUESTION_CODE_DESCRIPTION "In the last 30 days, other than the activities you did for work, on average, how many days per week did you engage in moderate exercise (like walking fast, running, jogging, dancing, swimming, biking, or other similar activities)" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>e046e991-8eb9-4e48-8ef4-f0513cebb7af</t>
-  </si>
-  <si>
-    <t>ea7f3d8a-b394-4c2a-bfe6-e23d8fa435dd</t>
-  </si>
-  <si>
-    <t>55834042-340c-4841-963c-1a3b29188bef</t>
-  </si>
-  <si>
-    <t>b86067ef-dfd2-48b4-a9a6-f4b779aa5907</t>
-  </si>
-  <si>
-    <t>a2884190-b5a2-46d1-a33e-5a5b7e44b1b9</t>
-  </si>
-  <si>
-    <t>a01630fb-36c5-43a6-b359-0cfbdc4c4688</t>
-  </si>
-  <si>
-    <t>8c659026-2121-49be-aa84-4c311eccbcdb</t>
-  </si>
-  <si>
-    <t>3e0d8a1d-1922-4c63-8c20-9ee6a89782b3</t>
+    <t>ac39de96-e56d-472f-bc41-39b45a0ba3d9</t>
+  </si>
+  <si>
+    <t>7c0aef64-c763-4756-931c-d5db0a2217e5</t>
+  </si>
+  <si>
+    <t>06428e77-0e8e-4cea-aafc-deb1fdc23360</t>
+  </si>
+  <si>
+    <t>3994e7ee-bf77-4235-bfe3-04fca9730660</t>
+  </si>
+  <si>
+    <t>253729f8-f135-4821-b41c-b4f79757738e</t>
+  </si>
+  <si>
+    <t>e7a3ae60-cf2f-4ed2-8da0-5607841d8cb5</t>
+  </si>
+  <si>
+    <t>7121cf04-8191-4217-8173-b171bad1783e</t>
+  </si>
+  <si>
+    <t>cfeab8dd-dddc-4b1d-98db-5afe572a06ff</t>
   </si>
   <si>
     <t>Invalid value "96782-8" found in QUESTION_CODE</t>
@@ -750,10 +750,10 @@
     <t>The QUESTION_CODE "96782-8" of QUESTION_CODE_DESCRIPTION "Do you want help with school or training? For example, starting or completing job training or getting a high school diploma, GED or equivalent." is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>c0256116-c5f6-4544-ba40-0849177cf3d3</t>
-  </si>
-  <si>
-    <t>4509604c-d6ba-4530-ac15-de8969bc89e7</t>
+    <t>b7f2f92b-7dc8-4ffe-bfa3-e88270b52a0f</t>
+  </si>
+  <si>
+    <t>6d122876-6085-4011-b2cd-e749ba46493f</t>
   </si>
   <si>
     <t>Invalid value "97027-7" found in QUESTION_CODE</t>
@@ -765,10 +765,10 @@
     <t>The QUESTION_CODE "97027-7" of QUESTION_CODE_DESCRIPTION "Do you speak a language other than English at home?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>28f57a2f-8476-46ff-8029-441c7e1c0f9a</t>
-  </si>
-  <si>
-    <t>76a78d17-4089-481a-8e46-9215601f86d5</t>
+    <t>ab8d6571-26d0-4f0d-b337-71ba5308b33a</t>
+  </si>
+  <si>
+    <t>2a8bc1b8-e21e-4225-b9b0-fa14d1354e4b</t>
   </si>
   <si>
     <t>Invalid value "93159-2" found in QUESTION_CODE</t>
@@ -780,19 +780,19 @@
     <t>The QUESTION_CODE "93159-2" of QUESTION_CODE_DESCRIPTION "How often do you feel lonely or isolated from those around you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>87a85d1a-119a-4a1d-a25b-9eb374b18a92</t>
-  </si>
-  <si>
-    <t>228a68a1-44c8-4e31-8996-4356a241ce03</t>
-  </si>
-  <si>
-    <t>ca806489-f13f-43bf-80e5-7899a24966d8</t>
-  </si>
-  <si>
-    <t>7fc0933a-f915-4874-a96e-b19641965fbe</t>
-  </si>
-  <si>
-    <t>7f1e730f-be4b-43aa-844d-21d191b9afe2</t>
+    <t>99888c27-2706-4cd7-845a-1d77279fde10</t>
+  </si>
+  <si>
+    <t>f87c97f1-480b-4bfd-af50-bde1eb4c9624</t>
+  </si>
+  <si>
+    <t>0518a6c5-b32b-4d13-9aee-cff332c8e55e</t>
+  </si>
+  <si>
+    <t>b02498f3-e165-47f6-9f4b-f4487ecab343</t>
+  </si>
+  <si>
+    <t>ef6eb984-3cd0-4e5a-b519-ad75cf44d8a8</t>
   </si>
   <si>
     <t>Invalid value "96781-0" found in QUESTION_CODE</t>
@@ -804,16 +804,16 @@
     <t>The QUESTION_CODE "96781-0" of QUESTION_CODE_DESCRIPTION "If for any reason you need help with day-to-day activities such as bathing, preparing meals, shopping, managing finances, etc., do you get the help you need?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>350b9aa1-7873-4b63-9682-7020a9d5f0d6</t>
-  </si>
-  <si>
-    <t>2e3c9f73-e922-4652-8225-83e6c2afcef1</t>
-  </si>
-  <si>
-    <t>2bdbf7c1-6e17-4e9b-8a06-0bb6e6729671</t>
-  </si>
-  <si>
-    <t>3b51f035-1b4e-4262-a4df-0e1120b17e93</t>
+    <t>576c6556-b963-46ab-a696-65c14bd833f3</t>
+  </si>
+  <si>
+    <t>5a742f4b-6397-4b20-a398-0faad5044ca2</t>
+  </si>
+  <si>
+    <t>658d64f7-828c-4b7d-aa1b-cf36ad8031d9</t>
+  </si>
+  <si>
+    <t>3c162475-ed60-4b1d-8029-d5753fe39784</t>
   </si>
   <si>
     <t>Invalid value "96780-2" found in QUESTION_CODE</t>
@@ -825,13 +825,13 @@
     <t>The QUESTION_CODE "96780-2" of QUESTION_CODE_DESCRIPTION "Do you want help finding or keeping work or a job?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>1e042273-b252-4d12-aadd-5a931b74b910</t>
-  </si>
-  <si>
-    <t>ead2ffc2-fde5-4d3c-8745-4a606e4cd80e</t>
-  </si>
-  <si>
-    <t>13be2bb0-89ee-41a3-b953-c9c05d9c7c64</t>
+    <t>9485159f-4fd1-4360-a13c-f96eeb3602be</t>
+  </si>
+  <si>
+    <t>540b5ba0-d25b-4b22-b18d-132b93a64804</t>
+  </si>
+  <si>
+    <t>9786b0bf-c65b-4cdd-aa91-19352ebf464d</t>
   </si>
   <si>
     <t>Invalid value "76513-1" found in QUESTION_CODE</t>
@@ -843,13 +843,13 @@
     <t>The QUESTION_CODE "76513-1" of QUESTION_CODE_DESCRIPTION "How hard is it for you to pay for the very basics like food, housing, medical care, and heating? Would you say it is" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>f55722da-7e74-4439-b182-be317a739903</t>
-  </si>
-  <si>
-    <t>e26a9934-31bd-4fac-8cda-93e815206c92</t>
-  </si>
-  <si>
-    <t>0c245ecc-b68f-486b-a752-e17c6e105a5c</t>
+    <t>8e16142e-2cda-4f6e-b9a3-9366a71be9ce</t>
+  </si>
+  <si>
+    <t>f1edff38-d6f9-4a95-8299-c1a7dfe7a596</t>
+  </si>
+  <si>
+    <t>c588e678-d52a-4d94-a27b-19f9cd7e1334</t>
   </si>
   <si>
     <t>Invalid value "95615-1" found in QUESTION_CODE</t>
@@ -861,19 +861,19 @@
     <t>The QUESTION_CODE "95615-1" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, scream or curse at you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>7723b547-20dd-42b8-8bb8-7a32177324a9</t>
-  </si>
-  <si>
-    <t>04e5d591-9cab-41be-9cbc-89bd4ef80c8f</t>
-  </si>
-  <si>
-    <t>d2f8836b-ac82-4c16-80be-b61cae2bee34</t>
-  </si>
-  <si>
-    <t>bbdd66a6-21da-4f65-9030-215153adcfcf</t>
-  </si>
-  <si>
-    <t>acfe0583-349c-4cfd-8a95-712d331ef9e0</t>
+    <t>f46b80fc-c6c5-4dab-9170-73e286406c93</t>
+  </si>
+  <si>
+    <t>088e0491-abd4-4945-aaba-3a0ca4d313dc</t>
+  </si>
+  <si>
+    <t>deced043-d11f-45a5-8095-92d80b0509e7</t>
+  </si>
+  <si>
+    <t>17634ee5-2b15-4172-b57f-121d60ae94f3</t>
+  </si>
+  <si>
+    <t>b0052510-47e2-43ff-a477-e88f8b705333</t>
   </si>
   <si>
     <t>Invalid value "95616-9" found in QUESTION_CODE</t>
@@ -885,19 +885,19 @@
     <t>The QUESTION_CODE "95616-9" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, threaten you with harm?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>51cf83b9-275a-47a1-b191-0be20bad2355</t>
-  </si>
-  <si>
-    <t>fe893f03-860c-4c93-b260-b864687a535e</t>
-  </si>
-  <si>
-    <t>99d42e3f-1fb5-4cb8-a5af-4bbeeb238d66</t>
-  </si>
-  <si>
-    <t>5a46dcd5-61c9-4770-a843-e08abe0f07af</t>
-  </si>
-  <si>
-    <t>1510c3c5-6ea0-4727-a54f-6c37c093cd10</t>
+    <t>2762daf7-8e1f-4f97-8de3-f0c525d8acfb</t>
+  </si>
+  <si>
+    <t>32d8aa93-e748-47f3-b93a-49663f719c04</t>
+  </si>
+  <si>
+    <t>3554a23c-eab0-40ac-bcd5-116498bbeed7</t>
+  </si>
+  <si>
+    <t>5a19942e-e2be-4e03-959a-8d7fc0e392bf</t>
+  </si>
+  <si>
+    <t>dea0a54f-565a-4535-b24a-f4fb48d4af03</t>
   </si>
   <si>
     <t>Invalid value "95617-7" found in QUESTION_CODE</t>
@@ -909,19 +909,19 @@
     <t>The QUESTION_CODE "95617-7" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, insult or talk down to you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>53e4f0f7-fb2a-4439-8b76-fb6de535773a</t>
-  </si>
-  <si>
-    <t>d9bd2720-628f-40a1-9726-60b29eacc547</t>
-  </si>
-  <si>
-    <t>90cbcc9c-8ff1-4749-8a1a-1585025883ce</t>
-  </si>
-  <si>
-    <t>7c62a06a-d774-49ca-b795-11abcfcdda3e</t>
-  </si>
-  <si>
-    <t>0e203110-5bae-4633-a394-8d5b56961d82</t>
+    <t>34cb5204-db65-4b52-bd7a-aec5a8645a08</t>
+  </si>
+  <si>
+    <t>b2346258-d471-4b05-bb80-4c62b31c0fc3</t>
+  </si>
+  <si>
+    <t>8830800a-95b1-4899-9c9d-3af05a20e718</t>
+  </si>
+  <si>
+    <t>421427ea-506a-4dd0-8767-f5207037f08d</t>
+  </si>
+  <si>
+    <t>fcb2227d-329e-456c-8da2-278f1b117300</t>
   </si>
   <si>
     <t>Invalid value "95618-5" found in QUESTION_CODE</t>
@@ -933,19 +933,19 @@
     <t>The QUESTION_CODE "95618-5" of QUESTION_CODE_DESCRIPTION "How often does anyone, including family and friends, physically hurt you?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>226ef428-913d-4210-a116-f65275fb5adb</t>
-  </si>
-  <si>
-    <t>0320e909-f0c3-44e5-a70d-9f78f79dd3cd</t>
-  </si>
-  <si>
-    <t>b4848954-585b-4485-a9fb-1deb64f8285c</t>
-  </si>
-  <si>
-    <t>3d3f9ee3-623c-411e-8209-9708dfabb7c7</t>
-  </si>
-  <si>
-    <t>eeb2cbcb-40d9-4b1b-9f8a-0858e4e8b12b</t>
+    <t>bc27af21-bc23-4cc5-a915-336fdc489049</t>
+  </si>
+  <si>
+    <t>e326b364-287f-4f18-897c-93fb93beb445</t>
+  </si>
+  <si>
+    <t>1b4a34f5-97e4-4d68-b61e-86ffcc551a15</t>
+  </si>
+  <si>
+    <t>4dc4c596-63e3-44ec-b9c3-ee2d6c6fc89a</t>
+  </si>
+  <si>
+    <t>08146eb7-2063-4b2d-a43a-f5ad6460fa8b</t>
   </si>
   <si>
     <t>Invalid value "96779-4" found in QUESTION_CODE</t>
@@ -957,13 +957,13 @@
     <t>The QUESTION_CODE "96779-4" of QUESTION_CODE_DESCRIPTION "In the past 12 months has the electric, gas, oil, or water company threatened to shut off services in your home?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>f32ecd3a-0296-4736-b171-55f9a7f796c1</t>
-  </si>
-  <si>
-    <t>6399f78e-84e5-4eea-b02b-18a4f95e2484</t>
-  </si>
-  <si>
-    <t>77fc3dac-a5cd-4ab7-bb56-0ff0cd939dab</t>
+    <t>9b1d938f-4822-459e-9c9a-9bc99e087d74</t>
+  </si>
+  <si>
+    <t>c4ab8ddf-c3d2-4304-98f3-d96e18c31bc4</t>
+  </si>
+  <si>
+    <t>3687effd-dacb-418c-aaae-d6df05bb54f6</t>
   </si>
   <si>
     <t>Invalid value "93030-5" found in QUESTION_CODE</t>
@@ -975,10 +975,10 @@
     <t>The QUESTION_CODE "93030-5" of QUESTION_CODE_DESCRIPTION "In the past 12 months, has lack of reliable transportation kept you from medical appointments, meetings, work or from getting things needed for daily living?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>fd4f67d4-d54e-46ad-a1be-3efc78944e5b</t>
-  </si>
-  <si>
-    <t>9720ddbd-99cf-4e67-9ccd-8170d0acf84e</t>
+    <t>31868d1d-06f7-4bbb-813f-4fb959a78171</t>
+  </si>
+  <si>
+    <t>e9ba6557-65ac-408e-b637-0b54ead40dce</t>
   </si>
   <si>
     <t>Invalid value "88123-5" found in QUESTION_CODE</t>
@@ -990,13 +990,13 @@
     <t>The QUESTION_CODE "88123-5" of QUESTION_CODE_DESCRIPTION "Within the past 12 months, the food you bought just didn't last and you didn't have money to get more." is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>5e47fc5e-fd16-4ca3-8aa6-693d5e78e2fc</t>
-  </si>
-  <si>
-    <t>7089d0f7-053a-4f9e-8233-2e25334cc3ee</t>
-  </si>
-  <si>
-    <t>365c4546-d3cc-4f92-9d8a-bb6069d7e37e</t>
+    <t>37eb7a76-d018-4548-857b-6b2ef8188979</t>
+  </si>
+  <si>
+    <t>1838630c-77d3-4e63-8bcf-a22d7e979b84</t>
+  </si>
+  <si>
+    <t>6370d234-804e-498a-ad2f-ef87b404eac9</t>
   </si>
   <si>
     <t>Invalid value "96778-6" found in QUESTION_CODE</t>
@@ -1008,28 +1008,28 @@
     <t>The QUESTION_CODE "96778-6" of QUESTION_CODE_DESCRIPTION "Think about the place you live. Do you have problems with any of the following?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>c62bf1e9-0323-48de-93cc-24e5c282a1f4</t>
-  </si>
-  <si>
-    <t>090b4d5d-d8d7-4bf0-8a3c-66ca6c6b2062</t>
-  </si>
-  <si>
-    <t>1f49c97b-6ec5-4c7c-ae8c-0647498f8580</t>
-  </si>
-  <si>
-    <t>e8b5615c-8019-4fde-a0d4-cde166ee7912</t>
-  </si>
-  <si>
-    <t>314b893c-0bfa-4d43-9f35-4863a7ba92f7</t>
-  </si>
-  <si>
-    <t>06d693e3-da4d-4b02-9c90-28d46fe1e757</t>
-  </si>
-  <si>
-    <t>cd98dd3a-cda4-4b9c-90e7-c65011ee47f1</t>
-  </si>
-  <si>
-    <t>08dee596-4b55-443c-a132-95096baef18d</t>
+    <t>a145fb39-0c8c-4548-8d2a-1890705c26e4</t>
+  </si>
+  <si>
+    <t>85c5a6ec-979f-4756-9a2c-56902d49f9ec</t>
+  </si>
+  <si>
+    <t>90e48fb2-6ad3-4ea4-a61b-4e160b15de8a</t>
+  </si>
+  <si>
+    <t>4c5244d5-6fae-4980-a9c2-8ac0e03e62f3</t>
+  </si>
+  <si>
+    <t>4f45f40e-64b6-4cc4-99d0-e3292636b7a4</t>
+  </si>
+  <si>
+    <t>6a2419f5-dc5f-47f8-9172-efae71ee75f8</t>
+  </si>
+  <si>
+    <t>7e01a46f-93a5-412d-a4e8-fb497c406675</t>
+  </si>
+  <si>
+    <t>b7f7b896-ef7d-4b39-810a-b44b88a85717</t>
   </si>
   <si>
     <t>Invalid value "71802-3" found in QUESTION_CODE</t>
@@ -1041,10 +1041,10 @@
     <t>The QUESTION_CODE "71802-3" of QUESTION_CODE_DESCRIPTION "What is your living situation today?" is not matching with the QUESTION_CODE of QUESTION_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>78f67f03-0588-42f0-8bb4-9d6e84935d88</t>
-  </si>
-  <si>
-    <t>988a3fd7-8637-4ec8-a649-ae763485f7e5</t>
+    <t>1387d1f1-7b75-4231-bd15-03d216a78b04</t>
+  </si>
+  <si>
+    <t>735876b7-9d53-451a-8cf0-e109a9b21ab8</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -1197,7 +1197,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>c76cae54-6214-42e8-9af5-cd11cc221e3b</t>
+    <t>53a28cc7-c24d-4f2b-9ec0-3ee8ea0f05a3</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
feat: modify data validation #66
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="224">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -96,7 +96,31 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>a5a0a85b-2f55-4587-938e-cf158fc7559e</t>
+    <t>1692bea9-e0a4-46bc-912e-921d08524dcc</t>
+  </si>
+  <si>
+    <t>Invalid Value</t>
+  </si>
+  <si>
+    <t>Value http://terminology.hl7.org/CodeSystem/v3-ActCode in ENCOUNTER_CLASS_CODE_SYSTEM not in allowed list ('http://terminology.hl7.org/ValueSet/v3-ActEncounterCode')</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_CLASS_CODE_SYSTEM</t>
+  </si>
+  <si>
+    <t>http://terminology.hl7.org/CodeSystem/v3-ActCode</t>
+  </si>
+  <si>
+    <t>Use only allowed values 'http://terminology.hl7.org/ValueSet/v3-ActEncounterCode' in ENCOUNTER_CLASS_CODE_SYSTEM</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Resolved By QE/QCS</t>
+  </si>
+  <si>
+    <t>986ce9cb-bfe8-4605-b55c-147bd0d1ea63</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -114,10 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>16607bff-5777-4028-ad0f-ffa8bf5166a3</t>
+    <t>a5346f2a-db69-4325-b11f-0a9ed6c6a722</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -144,7 +165,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>49d495db-6fab-4457-a42a-a5bc99aaaedf</t>
+    <t>09890ed6-ccf2-478f-ade7-9cf748010bcc</t>
   </si>
   <si>
     <t>Invalid ADMINISTRATIVE SEX CODE</t>
@@ -165,172 +186,133 @@
     <t>WARNING</t>
   </si>
   <si>
-    <t>Resolved By QE/QCS</t>
-  </si>
-  <si>
-    <t>97c4048a-4d1d-4dc1-927e-0b967106c3b3</t>
+    <t>c534c4da-80e0-4047-95d1-295b3402e324</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
   </si>
   <si>
-    <t>Invalid value "UNK" found in SEX_AT_BIRTH_CODE</t>
-  </si>
-  <si>
-    <t>SEX_AT_BIRTH_CODE</t>
+    <t>Invalid value "1142-9" found in RACE_CODE</t>
+  </si>
+  <si>
+    <t>RACE_CODE</t>
+  </si>
+  <si>
+    <t>1142-9</t>
+  </si>
+  <si>
+    <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>466799b7-a911-4c0d-be92-3c527c0d7e65</t>
+  </si>
+  <si>
+    <t>Invalid RACE CODE DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Invalid RACE CODE DESCRIPTION "Coquille" found in RACE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>RACE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>Coquille</t>
+  </si>
+  <si>
+    <t>Validate RACE CODE DESCRIPTION with race reference data</t>
+  </si>
+  <si>
+    <t>6dd3e498-c5b8-4f4c-a810-7dfd066cf2ed</t>
+  </si>
+  <si>
+    <t>Invalid Unique Medicaid Cin Per Mrn</t>
+  </si>
+  <si>
+    <t>Invalid Unique Medicaid Cin Per Mrn "QK65113L" found in MEDICAID_CIN</t>
+  </si>
+  <si>
+    <t>MEDICAID_CIN</t>
+  </si>
+  <si>
+    <t>QK65113L</t>
+  </si>
+  <si>
+    <t>Validate Unique Medicaid Cin Per Mrn</t>
+  </si>
+  <si>
+    <t>9ee63488-6365-47c3-92d6-2d83fa7bb0ff</t>
+  </si>
+  <si>
+    <t>2a0bd043-6c7d-4e5a-9676-0b4c0387b43b</t>
+  </si>
+  <si>
+    <t>2df4a9b4-8f55-44ad-b78f-b52ffbb56214</t>
+  </si>
+  <si>
+    <t>199967ec-72a3-402b-bac2-278226e2218d</t>
+  </si>
+  <si>
+    <t>Invalid value "X" found in ADMINISTRATIVE_SEX_CODE</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>The ADMINISTRATIVE_SEX_CODE "X" of ADMINISTRATIVE_SEX _CODE_DESCRIPTION "Other" is not matching with the ADMINISTRATIVE_SEX_CODE of ADMINISTRATIVE_SEX _CODE_DESCRIPTION in reference data</t>
+  </si>
+  <si>
+    <t>0f08e5f0-67df-4c18-93a0-bf267c6af2e9</t>
+  </si>
+  <si>
+    <t>aae32651-9577-4081-9339-95d21dcb95ae</t>
+  </si>
+  <si>
+    <t>6f773ae4-b9f4-47fd-a6d5-2563a6198331</t>
+  </si>
+  <si>
+    <t>168a77d8-34ba-46a8-963a-c3de7e7e290d</t>
+  </si>
+  <si>
+    <t>2e41c9a7-36f1-4b91-8914-5b919fc83363</t>
+  </si>
+  <si>
+    <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA')</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Use only allowed values 'Yes','No','NA' in POTENTIAL_NEED_INDICATED</t>
+  </si>
+  <si>
+    <t>488cd801-e4d5-46ac-ad8a-a3ad50c78679</t>
+  </si>
+  <si>
+    <t>Invalid value "UNK" found in ADMINISTRATIVE_SEX_CODE</t>
   </si>
   <si>
     <t>UNK</t>
   </si>
   <si>
-    <t>The SEX_AT_BIRTH_CODE "UNK" of SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" is not matching with the SEX_AT_BIRTH_CODE of SEX_AT_BIRTH_CODE_DESCRIPTION in reference data</t>
-  </si>
-  <si>
-    <t>403a915e-1c99-40a5-bcd3-07e763653fba</t>
-  </si>
-  <si>
-    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Invalid SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" found in SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Validate SEX_AT_BIRTH_CODE_DESCRIPTION with sex at birth reference data</t>
-  </si>
-  <si>
-    <t>b8abcddc-4526-4f24-a333-3286cc3723b0</t>
-  </si>
-  <si>
-    <t>Invalid value "1142-9" found in RACE_CODE</t>
-  </si>
-  <si>
-    <t>RACE_CODE</t>
-  </si>
-  <si>
-    <t>1142-9</t>
-  </si>
-  <si>
-    <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
-  </si>
-  <si>
-    <t>85d51026-b211-49e3-a236-83967e6f0335</t>
-  </si>
-  <si>
-    <t>Invalid RACE CODE DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Invalid RACE CODE DESCRIPTION "Coquille" found in RACE_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>RACE_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>Coquille</t>
-  </si>
-  <si>
-    <t>Validate RACE CODE DESCRIPTION with race reference data</t>
-  </si>
-  <si>
-    <t>2d5a6d99-fa27-44f3-ad4e-bc40fa8a99dd</t>
-  </si>
-  <si>
-    <t>Invalid Unique Medicaid Cin Per Mrn</t>
-  </si>
-  <si>
-    <t>Invalid Unique Medicaid Cin Per Mrn "QK65113L" found in MEDICAID_CIN</t>
-  </si>
-  <si>
-    <t>MEDICAID_CIN</t>
-  </si>
-  <si>
-    <t>QK65113L</t>
-  </si>
-  <si>
-    <t>Validate Unique Medicaid Cin Per Mrn</t>
-  </si>
-  <si>
-    <t>a170c5ea-d2dd-41fe-90db-161e3dc20c6b</t>
-  </si>
-  <si>
-    <t>0dfc5aab-f5da-47de-9cb5-68a6bd70ddfb</t>
-  </si>
-  <si>
-    <t>faa89b45-1dfe-4837-9a8a-7c523e479630</t>
-  </si>
-  <si>
-    <t>Invalid value "X" found in ADMINISTRATIVE_SEX_CODE</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>The ADMINISTRATIVE_SEX_CODE "X" of ADMINISTRATIVE_SEX _CODE_DESCRIPTION "Other" is not matching with the ADMINISTRATIVE_SEX_CODE of ADMINISTRATIVE_SEX _CODE_DESCRIPTION in reference data</t>
-  </si>
-  <si>
-    <t>ba64e48c-e986-4b6c-9413-bc717ad42d32</t>
-  </si>
-  <si>
-    <t>b21ff7a8-0925-4b1d-ac1e-e6aa6cf8b5b8</t>
-  </si>
-  <si>
-    <t>96cfdc1a-cb6c-4630-8600-7a25757c747a</t>
-  </si>
-  <si>
-    <t>a495149d-a2b6-4946-9dc1-405dc3800472</t>
-  </si>
-  <si>
-    <t>8c494cfb-bd54-4da9-98d8-ac67c9cf1054</t>
-  </si>
-  <si>
-    <t>4dc1f327-d77e-417e-8caf-502599b15226</t>
-  </si>
-  <si>
-    <t>Invalid Value</t>
-  </si>
-  <si>
-    <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA')</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Use only allowed values 'Yes','No','NA' in POTENTIAL_NEED_INDICATED</t>
-  </si>
-  <si>
-    <t>b627dee0-98d5-4917-90e7-bda5165e08f6</t>
-  </si>
-  <si>
-    <t>Invalid value "UNK" found in ADMINISTRATIVE_SEX_CODE</t>
-  </si>
-  <si>
     <t>The ADMINISTRATIVE_SEX_CODE "UNK" of ADMINISTRATIVE_SEX _CODE_DESCRIPTION "Undifferentiated" is not matching with the ADMINISTRATIVE_SEX_CODE of ADMINISTRATIVE_SEX _CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>bba823ec-7ea2-4dc9-b9ce-f144459856c1</t>
-  </si>
-  <si>
-    <t>3a99eb35-3b69-40a8-8ceb-7a080c276271</t>
-  </si>
-  <si>
-    <t>f8d94ae8-2885-4b96-ad63-c6104e33dc12</t>
-  </si>
-  <si>
-    <t>a3a66b75-319f-4071-a08c-4c0af694fcd7</t>
-  </si>
-  <si>
-    <t>72236ccc-e6c6-4e5a-ad7b-ae210580cd78</t>
-  </si>
-  <si>
-    <t>59f4e6ef-f2af-443c-b6de-9e7a83194aa9</t>
-  </si>
-  <si>
-    <t>f77fcbec-7d93-4469-b5b0-ce552a1945bf</t>
+    <t>af957b9a-9ba8-4cea-bb62-d47e98ed5788</t>
+  </si>
+  <si>
+    <t>0957f61d-de63-4f2e-b062-9459f57d52fa</t>
+  </si>
+  <si>
+    <t>341bdcae-d923-4d84-9f5d-38b8de72bf8d</t>
+  </si>
+  <si>
+    <t>f344f978-27a4-44fe-94c9-76ffcbfab431</t>
+  </si>
+  <si>
+    <t>ede95950-40f6-4cb8-931e-fdfaceda9798</t>
+  </si>
+  <si>
+    <t>29bcd30d-2cc5-40ba-a6a0-400d3e391d16</t>
   </si>
   <si>
     <t>Invalid value "vfdgvdfv" found in ADMINISTRATIVE_SEX_CODE</t>
@@ -339,34 +321,22 @@
     <t>The ADMINISTRATIVE_SEX_CODE "vfdgvdfv" of ADMINISTRATIVE_SEX _CODE_DESCRIPTION "Undifferentiated" is not matching with the ADMINISTRATIVE_SEX_CODE of ADMINISTRATIVE_SEX _CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>b2d8ee2e-85a5-441f-8d9c-d138e6c39327</t>
-  </si>
-  <si>
-    <t>7814c154-94fd-4c3c-a0d8-60b49c9badc2</t>
-  </si>
-  <si>
-    <t>152127cf-8c6d-4920-a440-182ae9b65eae</t>
-  </si>
-  <si>
-    <t>163944b9-5800-46cf-b065-86cc8e99442d</t>
-  </si>
-  <si>
-    <t>e46cc278-b36a-4275-84b8-20a6eb10d6de</t>
-  </si>
-  <si>
-    <t>1c1bfd21-ecfd-4b22-9dc9-83add8839370</t>
-  </si>
-  <si>
-    <t>cf3ca8d4-bb9d-49a8-9b30-62064689955a</t>
-  </si>
-  <si>
-    <t>Invalid value "unknown" found in SEX_AT_BIRTH_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>The SEX_AT_BIRTH_CODE_DESCRIPTION "unknown" of SEX_AT_BIRTH_CODE "UNK" is not matching with the SEX_AT_BIRTH_CODE_DESCRIPTION of SEX_AT_BIRTH_CODE in reference data</t>
-  </si>
-  <si>
-    <t>c179a217-1c1d-491b-9ca6-8212174d33b1</t>
+    <t>0cd5ab07-0015-47e4-870b-0ce627aeac43</t>
+  </si>
+  <si>
+    <t>16861563-78ba-4c93-86b4-93817530989f</t>
+  </si>
+  <si>
+    <t>e59c15ed-8c0d-40e4-aa08-b1a78ed33669</t>
+  </si>
+  <si>
+    <t>8f1d45a7-c538-404c-8812-2f51e977b151</t>
+  </si>
+  <si>
+    <t>eb89084e-b51a-4f7d-8115-158dc260ba73</t>
+  </si>
+  <si>
+    <t>568fb1f8-ac96-4202-b111-badaa69c558c</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -375,73 +345,139 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>3e55da91-e2f0-44fb-ac3a-e7f6cb23d1f3</t>
-  </si>
-  <si>
-    <t>eda230d3-6fc2-4c1e-882c-4725e428708d</t>
-  </si>
-  <si>
-    <t>b9dcd807-9b99-4cc5-a7a7-49e57e9a15c2</t>
-  </si>
-  <si>
-    <t>7b7f21a9-7a43-4386-8a5f-f907691e32a7</t>
-  </si>
-  <si>
-    <t>163ba05b-dca2-47ef-95ab-5f46ec367137</t>
-  </si>
-  <si>
-    <t>20c0046a-6326-403d-86d7-ffbef7410409</t>
-  </si>
-  <si>
-    <t>c5f2b522-44f0-48b0-8acb-72db8fd13374</t>
-  </si>
-  <si>
-    <t>d888942f-65de-40e0-a2da-33fac1d910a3</t>
-  </si>
-  <si>
-    <t>7a5fbc2f-2144-40c6-a72e-c9ed6c7af5f4</t>
-  </si>
-  <si>
-    <t>299115f4-d975-409f-abb1-24e42540d6e6</t>
-  </si>
-  <si>
-    <t>f25f2de1-f3cc-4b8a-8678-025c7bdc810a</t>
-  </si>
-  <si>
-    <t>ee9cc7e5-8c0b-4ade-83cf-e2f2a875d47f</t>
-  </si>
-  <si>
-    <t>4ac1012e-41be-431b-b309-4bd04bc38bd8</t>
-  </si>
-  <si>
-    <t>236a6349-f10b-477e-b1ec-677a5c15b602</t>
-  </si>
-  <si>
-    <t>a7f652b7-eae1-42f9-a4f0-99a3d73ec74b</t>
-  </si>
-  <si>
-    <t>ec98bc78-297f-4fdb-946b-483dcd76717e</t>
-  </si>
-  <si>
-    <t>21a1f300-bc96-479e-af76-df07ba6bb896</t>
-  </si>
-  <si>
-    <t>3514484e-fe04-4569-8bf6-1e79d7b5f1d6</t>
-  </si>
-  <si>
-    <t>00916e53-0b23-4a2a-bdfa-f243e1328e61</t>
-  </si>
-  <si>
-    <t>35aeac32-4442-43f1-9927-338fafdc93ed</t>
-  </si>
-  <si>
-    <t>3da32385-4ea6-4fb5-96b4-63e4e7322abf</t>
-  </si>
-  <si>
-    <t>34d6c7f5-a4a3-4b39-9e3f-4878f5114c74</t>
-  </si>
-  <si>
-    <t>a277f65f-4efd-48d2-b14b-b028e0d59165</t>
+    <t>1c76d8bb-054f-47d7-8665-075229775a23</t>
+  </si>
+  <si>
+    <t>588993fb-b2b3-4323-af9d-af874897819d</t>
+  </si>
+  <si>
+    <t>7b975a28-b0a9-41de-b7dd-28def8d778b2</t>
+  </si>
+  <si>
+    <t>90d3ef77-63b2-4a5b-83be-5eea615cc116</t>
+  </si>
+  <si>
+    <t>d35b314f-8cf8-4406-a9c1-52f843d7e43c</t>
+  </si>
+  <si>
+    <t>dd58e0f7-4e91-4492-80c3-31fffcf12cb8</t>
+  </si>
+  <si>
+    <t>2fd5a300-72dd-4a08-9dc3-4a6aa90b4519</t>
+  </si>
+  <si>
+    <t>b702a226-dea6-4929-bc13-4de58cc25731</t>
+  </si>
+  <si>
+    <t>7e4abb4e-6695-4889-b600-41c0579effe5</t>
+  </si>
+  <si>
+    <t>5f183fde-70bd-4ccd-8c32-26649afcf647</t>
+  </si>
+  <si>
+    <t>0dc55637-39ff-4e4f-9a8a-39f2ed49c8ee</t>
+  </si>
+  <si>
+    <t>fd703836-7655-4357-872d-58876c897aca</t>
+  </si>
+  <si>
+    <t>182dd371-4335-4ac7-b21b-d25b86111dab</t>
+  </si>
+  <si>
+    <t>0d704199-945a-4d92-acb1-5b8d33a43590</t>
+  </si>
+  <si>
+    <t>b1742745-95ea-4c4e-a182-359740c396bc</t>
+  </si>
+  <si>
+    <t>4f587d66-9baa-448a-a184-e61806c79374</t>
+  </si>
+  <si>
+    <t>15d795c9-ce95-4669-825d-11b80c9a067a</t>
+  </si>
+  <si>
+    <t>ec355a48-1d91-45d0-9040-7eb458648fd3</t>
+  </si>
+  <si>
+    <t>99484d3d-4f0a-415f-a5dd-a67269bd370a</t>
+  </si>
+  <si>
+    <t>9c6ce71d-5cf7-4e97-b290-db6773cb30c9</t>
+  </si>
+  <si>
+    <t>a3b65db1-6ed1-4a19-9aac-fd2a343e6099</t>
+  </si>
+  <si>
+    <t>e12c9161-c152-405c-aebe-b2dfc07d89e0</t>
+  </si>
+  <si>
+    <t>0e0f4fd8-261a-4379-8223-aa3abfc6d731</t>
+  </si>
+  <si>
+    <t>d2c65f5d-a214-4f96-9a99-6445b679ee22</t>
+  </si>
+  <si>
+    <t>73d74b99-71f3-4cd5-ae9a-a99a5eeea82c</t>
+  </si>
+  <si>
+    <t>3a9e4220-d474-4df6-97d5-3880b99b1809</t>
+  </si>
+  <si>
+    <t>f52cbd93-9b5b-431e-b056-2cfec471f8eb</t>
+  </si>
+  <si>
+    <t>2f87fb99-4859-4a03-8e3f-916bb7d805fc</t>
+  </si>
+  <si>
+    <t>b2968daa-64de-4aab-a45b-9e85591120b3</t>
+  </si>
+  <si>
+    <t>f823ee04-fcc9-4619-81d7-9821deb02837</t>
+  </si>
+  <si>
+    <t>d202cbb2-3e90-4480-b3dd-08f6c0756ef4</t>
+  </si>
+  <si>
+    <t>8397454d-5e40-4152-93bf-c963e0b7441b</t>
+  </si>
+  <si>
+    <t>6705e6bc-cdcc-4a1d-9b61-864630e38a8d</t>
+  </si>
+  <si>
+    <t>d847259c-9245-4c4d-a6ca-2f875fb4d73e</t>
+  </si>
+  <si>
+    <t>3a964dda-2f73-4d58-829d-0b6f8d64a8b8</t>
+  </si>
+  <si>
+    <t>3f196366-e49c-4a89-b3f9-a8d0b1e36e4c</t>
+  </si>
+  <si>
+    <t>0d0909e3-b202-4d21-9e52-efa7edea8f29</t>
+  </si>
+  <si>
+    <t>82643a2a-e15f-4955-bf80-834a356087ff</t>
+  </si>
+  <si>
+    <t>fe55d25c-867d-473c-9c48-458a84beba82</t>
+  </si>
+  <si>
+    <t>d76d2039-8dfa-4ca7-b0cf-8e1ac3ac20cb</t>
+  </si>
+  <si>
+    <t>4868e535-865c-485e-a867-90f138df9713</t>
+  </si>
+  <si>
+    <t>b466df89-97b9-4a28-8ac0-c3279a9a7ebb</t>
+  </si>
+  <si>
+    <t>8a11e4a6-cb54-4587-8986-d951752a3a0f</t>
+  </si>
+  <si>
+    <t>11a46304-4ad8-4d39-989c-47a402f15bed</t>
+  </si>
+  <si>
+    <t>a9edec7e-6387-44e4-8c83-ba776b32a240</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -594,7 +630,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>1ea5ce2a-92ab-4473-9875-001c63e649b4</t>
+    <t>b4be663b-ccef-49da-bd21-4955749d9a8c</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>
@@ -606,16 +642,16 @@
     <t>Provide a value for CONSENT</t>
   </si>
   <si>
-    <t>4ceaea17-f5f9-4f50-883c-0bf5989f6dba</t>
-  </si>
-  <si>
-    <t>227bceb7-98b8-4bf7-a434-cbc17096c642</t>
-  </si>
-  <si>
-    <t>1d3edb3f-ed4b-4d72-8b51-6ddf1624246f</t>
-  </si>
-  <si>
-    <t>cc774ff6-462c-4c4b-a8f8-f21c208ef3a7</t>
+    <t>07be4f9c-112f-4fec-8848-5cbd3dc82d3a</t>
+  </si>
+  <si>
+    <t>6d3d0889-6923-46d1-8885-7f65dbcc47e9</t>
+  </si>
+  <si>
+    <t>c6da2667-bb9f-4e75-9425-9b01c0a86500</t>
+  </si>
+  <si>
+    <t>aae0769b-cc66-4252-945a-fabe518c80f1</t>
   </si>
   <si>
     <t>Invalid value "Undifferentiated" found in ADMINISTRATIVE_SEX _CODE_DESCRIPTION</t>
@@ -630,13 +666,13 @@
     <t>The ADMINISTRATIVE_SEX _CODE_DESCRIPTION "Undifferentiated" of ADMINISTRATIVE_SEX_CODE "vfdgvdfv" is not matching with the ADMINISTRATIVE_SEX _CODE_DESCRIPTION of ADMINISTRATIVE_SEX_CODE in reference data</t>
   </si>
   <si>
-    <t>37138611-f2f2-4876-b4ed-f67c32ca9440</t>
+    <t>86e54486-7cc5-49b9-a97b-c9e10f29ac8e</t>
   </si>
   <si>
     <t>The ADMINISTRATIVE_SEX _CODE_DESCRIPTION "Undifferentiated" of ADMINISTRATIVE_SEX_CODE "UNK" is not matching with the ADMINISTRATIVE_SEX _CODE_DESCRIPTION of ADMINISTRATIVE_SEX_CODE in reference data</t>
   </si>
   <si>
-    <t>8fff981b-6993-4907-a323-e1c063e8256d</t>
+    <t>c09557c9-2c1a-447a-835c-0058bb800b07</t>
   </si>
   <si>
     <t>Invalid value "Other" found in ADMINISTRATIVE_SEX _CODE_DESCRIPTION</t>
@@ -822,7 +858,7 @@
         <v>30</v>
       </c>
       <c r="O2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="P2" t="s">
         <v>31</v>
@@ -836,6 +872,9 @@
       <c r="T2" t="s">
         <v>34</v>
       </c>
+      <c r="U2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -860,25 +899,28 @@
         <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O3">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>40</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -895,40 +937,34 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>44</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4">
+        <v>25</v>
+      </c>
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>46</v>
       </c>
-      <c r="O4">
-        <v>4</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
         <v>47</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" t="s">
-        <v>49</v>
-      </c>
-      <c r="T4" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5">
@@ -945,37 +981,40 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" t="s">
         <v>52</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>53</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5" t="s">
         <v>54</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>55</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>56</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>57</v>
       </c>
-      <c r="T5" t="s">
-        <v>34</v>
+      <c r="U5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -992,13 +1031,13 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L6" t="s">
         <v>58</v>
@@ -1039,34 +1078,34 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L7" t="s">
         <v>64</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="N7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O7">
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="T7" t="s">
         <v>34</v>
@@ -1086,37 +1125,40 @@
         <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Q8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="R8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="T8" t="s">
-        <v>34</v>
+        <v>57</v>
+      </c>
+      <c r="U8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -1133,40 +1175,40 @@
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="N9" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="O9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P9" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="Q9" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="R9" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="T9" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="U9" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
@@ -1192,25 +1234,25 @@
         <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="N10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O10">
         <v>13</v>
       </c>
       <c r="P10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="R10" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T10" t="s">
         <v>34</v>
@@ -1239,25 +1281,25 @@
         <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M11" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="N11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="O11">
         <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="R11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="T11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12">
@@ -1274,40 +1316,40 @@
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J12" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="M12" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="O12">
         <v>1</v>
       </c>
       <c r="P12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="Q12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="R12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="T12" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="U12" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -1324,34 +1366,34 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M13" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N13" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="O13">
         <v>2</v>
       </c>
       <c r="P13" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="Q13" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="R13" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="T13" t="s">
         <v>34</v>
@@ -1371,34 +1413,34 @@
         <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I14" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="N14" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="O14">
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="R14" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="T14" t="s">
         <v>34</v>
@@ -1418,37 +1460,40 @@
         <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I15" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M15" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N15" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="O15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="Q15" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="R15" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="T15" t="s">
         <v>34</v>
+      </c>
+      <c r="U15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -1465,34 +1510,34 @@
         <v>24</v>
       </c>
       <c r="H16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
+        <v>86</v>
+      </c>
+      <c r="M16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>38</v>
+      </c>
+      <c r="O16">
+        <v>14</v>
+      </c>
+      <c r="P16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>40</v>
+      </c>
+      <c r="R16" t="s">
         <v>41</v>
-      </c>
-      <c r="I16" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L16" t="s">
-        <v>90</v>
-      </c>
-      <c r="M16" t="s">
-        <v>70</v>
-      </c>
-      <c r="N16" t="s">
-        <v>71</v>
-      </c>
-      <c r="O16">
-        <v>2</v>
-      </c>
-      <c r="P16" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>73</v>
-      </c>
-      <c r="R16" t="s">
-        <v>74</v>
       </c>
       <c r="T16" t="s">
         <v>34</v>
@@ -1521,28 +1566,28 @@
         <v>27</v>
       </c>
       <c r="L17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="M17" t="s">
         <v>29</v>
       </c>
       <c r="N17" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="O17">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="P17" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="Q17" t="s">
-        <v>32</v>
+        <v>89</v>
       </c>
       <c r="R17" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="T17" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18">
@@ -1559,37 +1604,40 @@
         <v>24</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="I18" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="J18" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="L18" t="s">
+        <v>91</v>
+      </c>
+      <c r="M18" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" t="s">
         <v>92</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q18" t="s">
         <v>93</v>
       </c>
-      <c r="N18" t="s">
+      <c r="R18" t="s">
         <v>94</v>
       </c>
-      <c r="O18">
-        <v>7</v>
-      </c>
-      <c r="P18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>95</v>
-      </c>
-      <c r="R18" t="s">
-        <v>96</v>
-      </c>
       <c r="T18" t="s">
-        <v>40</v>
+        <v>57</v>
+      </c>
+      <c r="U18" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19">
@@ -1606,40 +1654,37 @@
         <v>24</v>
       </c>
       <c r="H19" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I19" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J19" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M19" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N19" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="O19">
         <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="Q19" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="R19" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="T19" t="s">
-        <v>50</v>
-      </c>
-      <c r="U19" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -1656,34 +1701,34 @@
         <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I20" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J20" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M20" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="N20" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="O20">
         <v>3</v>
       </c>
       <c r="P20" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="Q20" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="R20" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="T20" t="s">
         <v>34</v>
@@ -1703,37 +1748,40 @@
         <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I21" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J21" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="M21" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="N21" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="O21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P21" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="Q21" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="R21" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="T21" t="s">
         <v>34</v>
+      </c>
+      <c r="U21" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22">
@@ -1750,34 +1798,34 @@
         <v>24</v>
       </c>
       <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" t="s">
+        <v>98</v>
+      </c>
+      <c r="M22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O22">
+        <v>15</v>
+      </c>
+      <c r="P22" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>40</v>
+      </c>
+      <c r="R22" t="s">
         <v>41</v>
-      </c>
-      <c r="I22" t="s">
-        <v>42</v>
-      </c>
-      <c r="J22" t="s">
-        <v>43</v>
-      </c>
-      <c r="L22" t="s">
-        <v>102</v>
-      </c>
-      <c r="M22" t="s">
-        <v>53</v>
-      </c>
-      <c r="N22" t="s">
-        <v>65</v>
-      </c>
-      <c r="O22">
-        <v>3</v>
-      </c>
-      <c r="P22" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>67</v>
-      </c>
-      <c r="R22" t="s">
-        <v>68</v>
       </c>
       <c r="T22" t="s">
         <v>34</v>
@@ -1797,37 +1845,37 @@
         <v>24</v>
       </c>
       <c r="H23" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I23" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J23" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L23" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M23" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="N23" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="O23">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="P23" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="Q23" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="R23" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="T23" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24">
@@ -1844,37 +1892,40 @@
         <v>24</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="J24" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="L24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M24" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="N24" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="O24">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="P24" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="Q24" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="R24" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="T24" t="s">
-        <v>34</v>
+        <v>57</v>
+      </c>
+      <c r="U24" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="25">
@@ -1891,37 +1942,37 @@
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="J25" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="L25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M25" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="N25" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="O25">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P25" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="Q25" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="R25" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="T25" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26">
@@ -1938,40 +1989,37 @@
         <v>24</v>
       </c>
       <c r="H26" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I26" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J26" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M26" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="N26" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="O26">
         <v>4</v>
       </c>
       <c r="P26" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="Q26" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="R26" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
       <c r="T26" t="s">
-        <v>50</v>
-      </c>
-      <c r="U26" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27">
@@ -1988,37 +2036,40 @@
         <v>24</v>
       </c>
       <c r="H27" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I27" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J27" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="M27" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N27" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="O27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P27" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="Q27" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="R27" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="T27" t="s">
         <v>34</v>
+      </c>
+      <c r="U27" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28">
@@ -2035,34 +2086,34 @@
         <v>24</v>
       </c>
       <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L28" t="s">
+        <v>106</v>
+      </c>
+      <c r="M28" t="s">
+        <v>37</v>
+      </c>
+      <c r="N28" t="s">
+        <v>38</v>
+      </c>
+      <c r="O28">
+        <v>16</v>
+      </c>
+      <c r="P28" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>40</v>
+      </c>
+      <c r="R28" t="s">
         <v>41</v>
-      </c>
-      <c r="I28" t="s">
-        <v>42</v>
-      </c>
-      <c r="J28" t="s">
-        <v>43</v>
-      </c>
-      <c r="L28" t="s">
-        <v>110</v>
-      </c>
-      <c r="M28" t="s">
-        <v>59</v>
-      </c>
-      <c r="N28" t="s">
-        <v>60</v>
-      </c>
-      <c r="O28">
-        <v>4</v>
-      </c>
-      <c r="P28" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>62</v>
-      </c>
-      <c r="R28" t="s">
-        <v>63</v>
       </c>
       <c r="T28" t="s">
         <v>34</v>
@@ -2082,37 +2133,37 @@
         <v>24</v>
       </c>
       <c r="H29" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I29" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J29" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L29" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M29" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N29" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="O29">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="P29" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="Q29" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="R29" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="T29" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -2129,34 +2180,34 @@
         <v>24</v>
       </c>
       <c r="H30" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I30" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J30" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="M30" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="N30" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="O30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P30" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q30" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R30" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="T30" t="s">
         <v>34</v>
@@ -2185,7 +2236,7 @@
         <v>27</v>
       </c>
       <c r="L31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M31" t="s">
         <v>29</v>
@@ -2194,7 +2245,7 @@
         <v>30</v>
       </c>
       <c r="O31">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="P31" t="s">
         <v>31</v>
@@ -2208,6 +2259,9 @@
       <c r="T31" t="s">
         <v>34</v>
       </c>
+      <c r="U31" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -2232,28 +2286,28 @@
         <v>27</v>
       </c>
       <c r="L32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M32" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="N32" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="O32">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="P32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q32" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="R32" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="T32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33">
@@ -2270,37 +2324,37 @@
         <v>24</v>
       </c>
       <c r="H33" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I33" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M33" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N33" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="O33">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="P33" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="Q33" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="R33" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="T33" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34">
@@ -2317,34 +2371,34 @@
         <v>24</v>
       </c>
       <c r="H34" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I34" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J34" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="M34" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N34" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="O34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P34" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q34" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R34" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="T34" t="s">
         <v>34</v>
@@ -2373,7 +2427,7 @@
         <v>27</v>
       </c>
       <c r="L35" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="M35" t="s">
         <v>29</v>
@@ -2382,7 +2436,7 @@
         <v>30</v>
       </c>
       <c r="O35">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="P35" t="s">
         <v>31</v>
@@ -2396,6 +2450,9 @@
       <c r="T35" t="s">
         <v>34</v>
       </c>
+      <c r="U35" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
@@ -2420,28 +2477,28 @@
         <v>27</v>
       </c>
       <c r="L36" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="M36" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="N36" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="O36">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="P36" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q36" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="R36" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="T36" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37">
@@ -2458,37 +2515,37 @@
         <v>24</v>
       </c>
       <c r="H37" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I37" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J37" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L37" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="M37" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N37" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="O37">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="P37" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="Q37" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="R37" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="T37" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38">
@@ -2505,34 +2562,34 @@
         <v>24</v>
       </c>
       <c r="H38" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I38" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J38" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L38" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="M38" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N38" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="O38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P38" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q38" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R38" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="T38" t="s">
         <v>34</v>
@@ -2561,7 +2618,7 @@
         <v>27</v>
       </c>
       <c r="L39" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="M39" t="s">
         <v>29</v>
@@ -2570,7 +2627,7 @@
         <v>30</v>
       </c>
       <c r="O39">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="P39" t="s">
         <v>31</v>
@@ -2584,6 +2641,9 @@
       <c r="T39" t="s">
         <v>34</v>
       </c>
+      <c r="U39" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
@@ -2608,28 +2668,28 @@
         <v>27</v>
       </c>
       <c r="L40" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M40" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="N40" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="O40">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P40" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q40" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="R40" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="T40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41">
@@ -2646,37 +2706,37 @@
         <v>24</v>
       </c>
       <c r="H41" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I41" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J41" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L41" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="M41" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N41" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="O41">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="P41" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="Q41" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="R41" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="T41" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42">
@@ -2693,34 +2753,34 @@
         <v>24</v>
       </c>
       <c r="H42" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I42" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="J42" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L42" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="M42" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N42" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="O42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P42" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="Q42" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R42" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="T42" t="s">
         <v>34</v>
@@ -2749,7 +2809,7 @@
         <v>27</v>
       </c>
       <c r="L43" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="M43" t="s">
         <v>29</v>
@@ -2758,7 +2818,7 @@
         <v>30</v>
       </c>
       <c r="O43">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="P43" t="s">
         <v>31</v>
@@ -2772,6 +2832,9 @@
       <c r="T43" t="s">
         <v>34</v>
       </c>
+      <c r="U43" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
@@ -2796,28 +2859,28 @@
         <v>27</v>
       </c>
       <c r="L44" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="M44" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="N44" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="O44">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P44" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q44" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="R44" t="s">
-        <v>96</v>
+        <v>41</v>
       </c>
       <c r="T44" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45">
@@ -2834,37 +2897,40 @@
         <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I45" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J45" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L45" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="M45" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N45" t="s">
-        <v>116</v>
+        <v>30</v>
       </c>
       <c r="O45">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="P45" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="Q45" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="R45" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="T45" t="s">
         <v>34</v>
+      </c>
+      <c r="U45" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="46">
@@ -2881,34 +2947,34 @@
         <v>24</v>
       </c>
       <c r="H46" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" t="s">
+        <v>27</v>
+      </c>
+      <c r="L46" t="s">
+        <v>126</v>
+      </c>
+      <c r="M46" t="s">
+        <v>37</v>
+      </c>
+      <c r="N46" t="s">
+        <v>38</v>
+      </c>
+      <c r="O46">
+        <v>21</v>
+      </c>
+      <c r="P46" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>40</v>
+      </c>
+      <c r="R46" t="s">
         <v>41</v>
-      </c>
-      <c r="I46" t="s">
-        <v>42</v>
-      </c>
-      <c r="J46" t="s">
-        <v>43</v>
-      </c>
-      <c r="L46" t="s">
-        <v>132</v>
-      </c>
-      <c r="M46" t="s">
-        <v>53</v>
-      </c>
-      <c r="N46" t="s">
-        <v>119</v>
-      </c>
-      <c r="O46">
-        <v>4</v>
-      </c>
-      <c r="P46" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>73</v>
-      </c>
-      <c r="R46" t="s">
-        <v>120</v>
       </c>
       <c r="T46" t="s">
         <v>34</v>
@@ -2937,7 +3003,7 @@
         <v>27</v>
       </c>
       <c r="L47" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="M47" t="s">
         <v>29</v>
@@ -2946,7 +3012,7 @@
         <v>30</v>
       </c>
       <c r="O47">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="P47" t="s">
         <v>31</v>
@@ -2960,6 +3026,9 @@
       <c r="T47" t="s">
         <v>34</v>
       </c>
+      <c r="U47" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
@@ -2984,25 +3053,25 @@
         <v>27</v>
       </c>
       <c r="L48" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="M48" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="N48" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O48">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P48" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q48" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="R48" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T48" t="s">
         <v>34</v>
@@ -3031,7 +3100,7 @@
         <v>27</v>
       </c>
       <c r="L49" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="M49" t="s">
         <v>29</v>
@@ -3040,7 +3109,7 @@
         <v>30</v>
       </c>
       <c r="O49">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="P49" t="s">
         <v>31</v>
@@ -3054,6 +3123,9 @@
       <c r="T49" t="s">
         <v>34</v>
       </c>
+      <c r="U49" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
@@ -3078,25 +3150,25 @@
         <v>27</v>
       </c>
       <c r="L50" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="M50" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="N50" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O50">
         <v>23</v>
       </c>
       <c r="P50" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q50" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="R50" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T50" t="s">
         <v>34</v>
@@ -3125,7 +3197,7 @@
         <v>27</v>
       </c>
       <c r="L51" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="M51" t="s">
         <v>29</v>
@@ -3134,7 +3206,7 @@
         <v>30</v>
       </c>
       <c r="O51">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="P51" t="s">
         <v>31</v>
@@ -3148,6 +3220,9 @@
       <c r="T51" t="s">
         <v>34</v>
       </c>
+      <c r="U51" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
@@ -3172,25 +3247,25 @@
         <v>27</v>
       </c>
       <c r="L52" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="M52" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="N52" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O52">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P52" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q52" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="R52" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T52" t="s">
         <v>34</v>
@@ -3219,7 +3294,7 @@
         <v>27</v>
       </c>
       <c r="L53" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="M53" t="s">
         <v>29</v>
@@ -3228,7 +3303,7 @@
         <v>30</v>
       </c>
       <c r="O53">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="P53" t="s">
         <v>31</v>
@@ -3242,6 +3317,9 @@
       <c r="T53" t="s">
         <v>34</v>
       </c>
+      <c r="U53" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
@@ -3266,25 +3344,25 @@
         <v>27</v>
       </c>
       <c r="L54" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="M54" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="N54" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O54">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P54" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q54" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="R54" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T54" t="s">
         <v>34</v>
@@ -3313,7 +3391,7 @@
         <v>27</v>
       </c>
       <c r="L55" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="M55" t="s">
         <v>29</v>
@@ -3322,7 +3400,7 @@
         <v>30</v>
       </c>
       <c r="O55">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="P55" t="s">
         <v>31</v>
@@ -3336,6 +3414,9 @@
       <c r="T55" t="s">
         <v>34</v>
       </c>
+      <c r="U55" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
@@ -3360,25 +3441,25 @@
         <v>27</v>
       </c>
       <c r="L56" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="M56" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="N56" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="O56">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P56" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="Q56" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="R56" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T56" t="s">
         <v>34</v>
@@ -3407,7 +3488,7 @@
         <v>27</v>
       </c>
       <c r="L57" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="M57" t="s">
         <v>29</v>
@@ -3416,7 +3497,7 @@
         <v>30</v>
       </c>
       <c r="O57">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="P57" t="s">
         <v>31</v>
@@ -3430,6 +3511,9 @@
       <c r="T57" t="s">
         <v>34</v>
       </c>
+      <c r="U57" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
@@ -3445,25 +3529,37 @@
         <v>24</v>
       </c>
       <c r="H58" t="s">
-        <v>144</v>
+        <v>25</v>
       </c>
       <c r="I58" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="J58" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L58" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="M58" t="s">
-        <v>148</v>
+        <v>37</v>
       </c>
       <c r="N58" t="s">
-        <v>149</v>
+        <v>38</v>
+      </c>
+      <c r="O58">
+        <v>27</v>
+      </c>
+      <c r="P58" t="s">
+        <v>39</v>
       </c>
       <c r="Q58" t="s">
-        <v>145</v>
+        <v>40</v>
+      </c>
+      <c r="R58" t="s">
+        <v>41</v>
+      </c>
+      <c r="T58" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="59">
@@ -3480,25 +3576,40 @@
         <v>24</v>
       </c>
       <c r="H59" t="s">
-        <v>150</v>
+        <v>25</v>
       </c>
       <c r="I59" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="J59" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L59" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="M59" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N59" t="s">
-        <v>152</v>
+        <v>30</v>
+      </c>
+      <c r="O59">
+        <v>17</v>
+      </c>
+      <c r="P59" t="s">
+        <v>31</v>
       </c>
       <c r="Q59" t="s">
-        <v>145</v>
+        <v>32</v>
+      </c>
+      <c r="R59" t="s">
+        <v>33</v>
+      </c>
+      <c r="T59" t="s">
+        <v>34</v>
+      </c>
+      <c r="U59" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="60">
@@ -3515,25 +3626,37 @@
         <v>24</v>
       </c>
       <c r="H60" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="I60" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="J60" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L60" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="M60" t="s">
-        <v>148</v>
+        <v>37</v>
       </c>
       <c r="N60" t="s">
-        <v>155</v>
+        <v>38</v>
+      </c>
+      <c r="O60">
+        <v>28</v>
+      </c>
+      <c r="P60" t="s">
+        <v>39</v>
       </c>
       <c r="Q60" t="s">
-        <v>145</v>
+        <v>40</v>
+      </c>
+      <c r="R60" t="s">
+        <v>41</v>
+      </c>
+      <c r="T60" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="61">
@@ -3550,25 +3673,40 @@
         <v>24</v>
       </c>
       <c r="H61" t="s">
-        <v>156</v>
+        <v>25</v>
       </c>
       <c r="I61" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="J61" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L61" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="M61" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N61" t="s">
-        <v>158</v>
+        <v>30</v>
+      </c>
+      <c r="O61">
+        <v>18</v>
+      </c>
+      <c r="P61" t="s">
+        <v>31</v>
       </c>
       <c r="Q61" t="s">
-        <v>145</v>
+        <v>32</v>
+      </c>
+      <c r="R61" t="s">
+        <v>33</v>
+      </c>
+      <c r="T61" t="s">
+        <v>34</v>
+      </c>
+      <c r="U61" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="62">
@@ -3585,25 +3723,37 @@
         <v>24</v>
       </c>
       <c r="H62" t="s">
-        <v>159</v>
+        <v>25</v>
       </c>
       <c r="I62" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="J62" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L62" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="M62" t="s">
-        <v>148</v>
+        <v>37</v>
       </c>
       <c r="N62" t="s">
-        <v>161</v>
+        <v>38</v>
+      </c>
+      <c r="O62">
+        <v>29</v>
+      </c>
+      <c r="P62" t="s">
+        <v>39</v>
       </c>
       <c r="Q62" t="s">
-        <v>145</v>
+        <v>40</v>
+      </c>
+      <c r="R62" t="s">
+        <v>41</v>
+      </c>
+      <c r="T62" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="63">
@@ -3620,25 +3770,40 @@
         <v>24</v>
       </c>
       <c r="H63" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="I63" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="J63" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L63" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="M63" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N63" t="s">
-        <v>165</v>
+        <v>30</v>
+      </c>
+      <c r="O63">
+        <v>19</v>
+      </c>
+      <c r="P63" t="s">
+        <v>31</v>
       </c>
       <c r="Q63" t="s">
-        <v>163</v>
+        <v>32</v>
+      </c>
+      <c r="R63" t="s">
+        <v>33</v>
+      </c>
+      <c r="T63" t="s">
+        <v>34</v>
+      </c>
+      <c r="U63" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="64">
@@ -3655,25 +3820,37 @@
         <v>24</v>
       </c>
       <c r="H64" t="s">
-        <v>166</v>
+        <v>25</v>
       </c>
       <c r="I64" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="J64" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L64" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="M64" t="s">
-        <v>148</v>
+        <v>37</v>
       </c>
       <c r="N64" t="s">
-        <v>168</v>
+        <v>38</v>
+      </c>
+      <c r="O64">
+        <v>30</v>
+      </c>
+      <c r="P64" t="s">
+        <v>39</v>
       </c>
       <c r="Q64" t="s">
-        <v>163</v>
+        <v>40</v>
+      </c>
+      <c r="R64" t="s">
+        <v>41</v>
+      </c>
+      <c r="T64" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="65">
@@ -3690,25 +3867,40 @@
         <v>24</v>
       </c>
       <c r="H65" t="s">
-        <v>169</v>
+        <v>25</v>
       </c>
       <c r="I65" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="J65" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L65" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="M65" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N65" t="s">
-        <v>171</v>
+        <v>30</v>
+      </c>
+      <c r="O65">
+        <v>20</v>
+      </c>
+      <c r="P65" t="s">
+        <v>31</v>
       </c>
       <c r="Q65" t="s">
-        <v>163</v>
+        <v>32</v>
+      </c>
+      <c r="R65" t="s">
+        <v>33</v>
+      </c>
+      <c r="T65" t="s">
+        <v>34</v>
+      </c>
+      <c r="U65" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="66">
@@ -3725,25 +3917,40 @@
         <v>24</v>
       </c>
       <c r="H66" t="s">
-        <v>172</v>
+        <v>25</v>
       </c>
       <c r="I66" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="J66" t="s">
+        <v>27</v>
+      </c>
+      <c r="L66" t="s">
         <v>146</v>
       </c>
-      <c r="L66" t="s">
-        <v>173</v>
-      </c>
       <c r="M66" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N66" t="s">
-        <v>174</v>
+        <v>30</v>
+      </c>
+      <c r="O66">
+        <v>21</v>
+      </c>
+      <c r="P66" t="s">
+        <v>31</v>
       </c>
       <c r="Q66" t="s">
-        <v>163</v>
+        <v>32</v>
+      </c>
+      <c r="R66" t="s">
+        <v>33</v>
+      </c>
+      <c r="T66" t="s">
+        <v>34</v>
+      </c>
+      <c r="U66" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="67">
@@ -3760,25 +3967,40 @@
         <v>24</v>
       </c>
       <c r="H67" t="s">
-        <v>175</v>
+        <v>25</v>
       </c>
       <c r="I67" t="s">
-        <v>163</v>
+        <v>26</v>
       </c>
       <c r="J67" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L67" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="M67" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N67" t="s">
-        <v>177</v>
+        <v>30</v>
+      </c>
+      <c r="O67">
+        <v>22</v>
+      </c>
+      <c r="P67" t="s">
+        <v>31</v>
       </c>
       <c r="Q67" t="s">
-        <v>163</v>
+        <v>32</v>
+      </c>
+      <c r="R67" t="s">
+        <v>33</v>
+      </c>
+      <c r="T67" t="s">
+        <v>34</v>
+      </c>
+      <c r="U67" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="68">
@@ -3795,25 +4017,40 @@
         <v>24</v>
       </c>
       <c r="H68" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
       <c r="I68" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="J68" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L68" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="M68" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N68" t="s">
-        <v>181</v>
+        <v>30</v>
+      </c>
+      <c r="O68">
+        <v>23</v>
+      </c>
+      <c r="P68" t="s">
+        <v>31</v>
       </c>
       <c r="Q68" t="s">
-        <v>179</v>
+        <v>32</v>
+      </c>
+      <c r="R68" t="s">
+        <v>33</v>
+      </c>
+      <c r="T68" t="s">
+        <v>34</v>
+      </c>
+      <c r="U68" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="69">
@@ -3830,25 +4067,40 @@
         <v>24</v>
       </c>
       <c r="H69" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
       <c r="I69" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="J69" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L69" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="M69" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N69" t="s">
-        <v>184</v>
+        <v>30</v>
+      </c>
+      <c r="O69">
+        <v>24</v>
+      </c>
+      <c r="P69" t="s">
+        <v>31</v>
       </c>
       <c r="Q69" t="s">
-        <v>179</v>
+        <v>32</v>
+      </c>
+      <c r="R69" t="s">
+        <v>33</v>
+      </c>
+      <c r="T69" t="s">
+        <v>34</v>
+      </c>
+      <c r="U69" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="70">
@@ -3865,25 +4117,40 @@
         <v>24</v>
       </c>
       <c r="H70" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="I70" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="J70" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L70" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="M70" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N70" t="s">
-        <v>187</v>
+        <v>30</v>
+      </c>
+      <c r="O70">
+        <v>25</v>
+      </c>
+      <c r="P70" t="s">
+        <v>31</v>
       </c>
       <c r="Q70" t="s">
-        <v>179</v>
+        <v>32</v>
+      </c>
+      <c r="R70" t="s">
+        <v>33</v>
+      </c>
+      <c r="T70" t="s">
+        <v>34</v>
+      </c>
+      <c r="U70" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="71">
@@ -3900,25 +4167,40 @@
         <v>24</v>
       </c>
       <c r="H71" t="s">
-        <v>188</v>
+        <v>25</v>
       </c>
       <c r="I71" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="J71" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L71" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="M71" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N71" t="s">
-        <v>190</v>
+        <v>30</v>
+      </c>
+      <c r="O71">
+        <v>26</v>
+      </c>
+      <c r="P71" t="s">
+        <v>31</v>
       </c>
       <c r="Q71" t="s">
-        <v>179</v>
+        <v>32</v>
+      </c>
+      <c r="R71" t="s">
+        <v>33</v>
+      </c>
+      <c r="T71" t="s">
+        <v>34</v>
+      </c>
+      <c r="U71" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="72">
@@ -3935,25 +4217,40 @@
         <v>24</v>
       </c>
       <c r="H72" t="s">
-        <v>191</v>
+        <v>25</v>
       </c>
       <c r="I72" t="s">
-        <v>179</v>
+        <v>26</v>
       </c>
       <c r="J72" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="L72" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="M72" t="s">
-        <v>148</v>
+        <v>29</v>
       </c>
       <c r="N72" t="s">
-        <v>193</v>
+        <v>30</v>
+      </c>
+      <c r="O72">
+        <v>27</v>
+      </c>
+      <c r="P72" t="s">
+        <v>31</v>
       </c>
       <c r="Q72" t="s">
-        <v>179</v>
+        <v>32</v>
+      </c>
+      <c r="R72" t="s">
+        <v>33</v>
+      </c>
+      <c r="T72" t="s">
+        <v>34</v>
+      </c>
+      <c r="U72" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="73">
@@ -3970,31 +4267,40 @@
         <v>24</v>
       </c>
       <c r="H73" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I73" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J73" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L73" t="s">
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="M73" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N73" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="P73" t="s">
-        <v>196</v>
+        <v>31</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>32</v>
       </c>
       <c r="R73" t="s">
-        <v>197</v>
+        <v>33</v>
+      </c>
+      <c r="T73" t="s">
+        <v>34</v>
+      </c>
+      <c r="U73" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="74">
@@ -4011,31 +4317,40 @@
         <v>24</v>
       </c>
       <c r="H74" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I74" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J74" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L74" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="M74" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N74" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
       <c r="O74">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="P74" t="s">
-        <v>196</v>
+        <v>31</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>32</v>
       </c>
       <c r="R74" t="s">
-        <v>197</v>
+        <v>33</v>
+      </c>
+      <c r="T74" t="s">
+        <v>34</v>
+      </c>
+      <c r="U74" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="75">
@@ -4052,31 +4367,40 @@
         <v>24</v>
       </c>
       <c r="H75" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="I75" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="J75" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="L75" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
       <c r="M75" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N75" t="s">
-        <v>195</v>
+        <v>30</v>
       </c>
       <c r="O75">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="P75" t="s">
-        <v>196</v>
+        <v>31</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>32</v>
       </c>
       <c r="R75" t="s">
-        <v>197</v>
+        <v>33</v>
+      </c>
+      <c r="T75" t="s">
+        <v>34</v>
+      </c>
+      <c r="U75" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="76">
@@ -4093,31 +4417,25 @@
         <v>24</v>
       </c>
       <c r="H76" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="I76" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="J76" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="L76" t="s">
-        <v>200</v>
+        <v>159</v>
       </c>
       <c r="M76" t="s">
-        <v>36</v>
+        <v>160</v>
       </c>
       <c r="N76" t="s">
-        <v>195</v>
-      </c>
-      <c r="O76">
-        <v>1</v>
-      </c>
-      <c r="P76" t="s">
-        <v>196</v>
-      </c>
-      <c r="R76" t="s">
-        <v>197</v>
+        <v>161</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="77">
@@ -4134,34 +4452,25 @@
         <v>24</v>
       </c>
       <c r="H77" t="s">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="I77" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="J77" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="L77" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="M77" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="N77" t="s">
-        <v>202</v>
-      </c>
-      <c r="O77">
-        <v>4</v>
-      </c>
-      <c r="P77" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="Q77" t="s">
-        <v>204</v>
-      </c>
-      <c r="R77" t="s">
-        <v>205</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78">
@@ -4178,34 +4487,25 @@
         <v>24</v>
       </c>
       <c r="H78" t="s">
-        <v>41</v>
+        <v>165</v>
       </c>
       <c r="I78" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="J78" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="L78" t="s">
-        <v>206</v>
+        <v>166</v>
       </c>
       <c r="M78" t="s">
-        <v>53</v>
+        <v>160</v>
       </c>
       <c r="N78" t="s">
-        <v>202</v>
-      </c>
-      <c r="O78">
-        <v>3</v>
-      </c>
-      <c r="P78" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="Q78" t="s">
-        <v>204</v>
-      </c>
-      <c r="R78" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79">
@@ -4222,34 +4522,706 @@
         <v>24</v>
       </c>
       <c r="H79" t="s">
-        <v>41</v>
+        <v>168</v>
       </c>
       <c r="I79" t="s">
-        <v>42</v>
+        <v>157</v>
       </c>
       <c r="J79" t="s">
+        <v>158</v>
+      </c>
+      <c r="L79" t="s">
+        <v>169</v>
+      </c>
+      <c r="M79" t="s">
+        <v>160</v>
+      </c>
+      <c r="N79" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" t="s">
+        <v>23</v>
+      </c>
+      <c r="G80" t="s">
+        <v>24</v>
+      </c>
+      <c r="H80" t="s">
+        <v>171</v>
+      </c>
+      <c r="I80" t="s">
+        <v>157</v>
+      </c>
+      <c r="J80" t="s">
+        <v>158</v>
+      </c>
+      <c r="L80" t="s">
+        <v>172</v>
+      </c>
+      <c r="M80" t="s">
+        <v>160</v>
+      </c>
+      <c r="N80" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" t="s">
+        <v>24</v>
+      </c>
+      <c r="H81" t="s">
+        <v>174</v>
+      </c>
+      <c r="I81" t="s">
+        <v>175</v>
+      </c>
+      <c r="J81" t="s">
+        <v>158</v>
+      </c>
+      <c r="L81" t="s">
+        <v>176</v>
+      </c>
+      <c r="M81" t="s">
+        <v>160</v>
+      </c>
+      <c r="N81" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="G82" t="s">
+        <v>24</v>
+      </c>
+      <c r="H82" t="s">
+        <v>178</v>
+      </c>
+      <c r="I82" t="s">
+        <v>175</v>
+      </c>
+      <c r="J82" t="s">
+        <v>158</v>
+      </c>
+      <c r="L82" t="s">
+        <v>179</v>
+      </c>
+      <c r="M82" t="s">
+        <v>160</v>
+      </c>
+      <c r="N82" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" t="s">
+        <v>23</v>
+      </c>
+      <c r="G83" t="s">
+        <v>24</v>
+      </c>
+      <c r="H83" t="s">
+        <v>181</v>
+      </c>
+      <c r="I83" t="s">
+        <v>175</v>
+      </c>
+      <c r="J83" t="s">
+        <v>158</v>
+      </c>
+      <c r="L83" t="s">
+        <v>182</v>
+      </c>
+      <c r="M83" t="s">
+        <v>160</v>
+      </c>
+      <c r="N83" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="G84" t="s">
+        <v>24</v>
+      </c>
+      <c r="H84" t="s">
+        <v>184</v>
+      </c>
+      <c r="I84" t="s">
+        <v>175</v>
+      </c>
+      <c r="J84" t="s">
+        <v>158</v>
+      </c>
+      <c r="L84" t="s">
+        <v>185</v>
+      </c>
+      <c r="M84" t="s">
+        <v>160</v>
+      </c>
+      <c r="N84" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="G85" t="s">
+        <v>24</v>
+      </c>
+      <c r="H85" t="s">
+        <v>187</v>
+      </c>
+      <c r="I85" t="s">
+        <v>175</v>
+      </c>
+      <c r="J85" t="s">
+        <v>158</v>
+      </c>
+      <c r="L85" t="s">
+        <v>188</v>
+      </c>
+      <c r="M85" t="s">
+        <v>160</v>
+      </c>
+      <c r="N85" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>21</v>
+      </c>
+      <c r="B86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="G86" t="s">
+        <v>24</v>
+      </c>
+      <c r="H86" t="s">
+        <v>190</v>
+      </c>
+      <c r="I86" t="s">
+        <v>191</v>
+      </c>
+      <c r="J86" t="s">
+        <v>158</v>
+      </c>
+      <c r="L86" t="s">
+        <v>192</v>
+      </c>
+      <c r="M86" t="s">
+        <v>160</v>
+      </c>
+      <c r="N86" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="G87" t="s">
+        <v>24</v>
+      </c>
+      <c r="H87" t="s">
+        <v>194</v>
+      </c>
+      <c r="I87" t="s">
+        <v>191</v>
+      </c>
+      <c r="J87" t="s">
+        <v>158</v>
+      </c>
+      <c r="L87" t="s">
+        <v>195</v>
+      </c>
+      <c r="M87" t="s">
+        <v>160</v>
+      </c>
+      <c r="N87" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q87" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B88" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="G88" t="s">
+        <v>24</v>
+      </c>
+      <c r="H88" t="s">
+        <v>197</v>
+      </c>
+      <c r="I88" t="s">
+        <v>191</v>
+      </c>
+      <c r="J88" t="s">
+        <v>158</v>
+      </c>
+      <c r="L88" t="s">
+        <v>198</v>
+      </c>
+      <c r="M88" t="s">
+        <v>160</v>
+      </c>
+      <c r="N88" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q88" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>22</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" t="s">
+        <v>24</v>
+      </c>
+      <c r="H89" t="s">
+        <v>200</v>
+      </c>
+      <c r="I89" t="s">
+        <v>191</v>
+      </c>
+      <c r="J89" t="s">
+        <v>158</v>
+      </c>
+      <c r="L89" t="s">
+        <v>201</v>
+      </c>
+      <c r="M89" t="s">
+        <v>160</v>
+      </c>
+      <c r="N89" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q89" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>22</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="G90" t="s">
+        <v>24</v>
+      </c>
+      <c r="H90" t="s">
+        <v>203</v>
+      </c>
+      <c r="I90" t="s">
+        <v>191</v>
+      </c>
+      <c r="J90" t="s">
+        <v>158</v>
+      </c>
+      <c r="L90" t="s">
+        <v>204</v>
+      </c>
+      <c r="M90" t="s">
+        <v>160</v>
+      </c>
+      <c r="N90" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" t="s">
+        <v>22</v>
+      </c>
+      <c r="C91" t="s">
+        <v>23</v>
+      </c>
+      <c r="G91" t="s">
+        <v>24</v>
+      </c>
+      <c r="H91" t="s">
+        <v>48</v>
+      </c>
+      <c r="I91" t="s">
+        <v>49</v>
+      </c>
+      <c r="J91" t="s">
+        <v>50</v>
+      </c>
+      <c r="L91" t="s">
+        <v>206</v>
+      </c>
+      <c r="M91" t="s">
         <v>43</v>
       </c>
-      <c r="L79" t="s">
+      <c r="N91" t="s">
+        <v>207</v>
+      </c>
+      <c r="O91">
+        <v>4</v>
+      </c>
+      <c r="P91" t="s">
         <v>208</v>
       </c>
-      <c r="M79" t="s">
-        <v>53</v>
-      </c>
-      <c r="N79" t="s">
+      <c r="R91" t="s">
         <v>209</v>
       </c>
-      <c r="O79">
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C92" t="s">
+        <v>23</v>
+      </c>
+      <c r="G92" t="s">
+        <v>24</v>
+      </c>
+      <c r="H92" t="s">
+        <v>48</v>
+      </c>
+      <c r="I92" t="s">
+        <v>49</v>
+      </c>
+      <c r="J92" t="s">
+        <v>50</v>
+      </c>
+      <c r="L92" t="s">
+        <v>210</v>
+      </c>
+      <c r="M92" t="s">
+        <v>43</v>
+      </c>
+      <c r="N92" t="s">
+        <v>207</v>
+      </c>
+      <c r="O92">
+        <v>3</v>
+      </c>
+      <c r="P92" t="s">
+        <v>208</v>
+      </c>
+      <c r="R92" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" t="s">
+        <v>22</v>
+      </c>
+      <c r="C93" t="s">
+        <v>23</v>
+      </c>
+      <c r="G93" t="s">
+        <v>24</v>
+      </c>
+      <c r="H93" t="s">
+        <v>48</v>
+      </c>
+      <c r="I93" t="s">
+        <v>49</v>
+      </c>
+      <c r="J93" t="s">
+        <v>50</v>
+      </c>
+      <c r="L93" t="s">
+        <v>211</v>
+      </c>
+      <c r="M93" t="s">
+        <v>43</v>
+      </c>
+      <c r="N93" t="s">
+        <v>207</v>
+      </c>
+      <c r="O93">
+        <v>2</v>
+      </c>
+      <c r="P93" t="s">
+        <v>208</v>
+      </c>
+      <c r="R93" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" t="s">
+        <v>22</v>
+      </c>
+      <c r="C94" t="s">
+        <v>23</v>
+      </c>
+      <c r="G94" t="s">
+        <v>24</v>
+      </c>
+      <c r="H94" t="s">
+        <v>48</v>
+      </c>
+      <c r="I94" t="s">
+        <v>49</v>
+      </c>
+      <c r="J94" t="s">
+        <v>50</v>
+      </c>
+      <c r="L94" t="s">
+        <v>212</v>
+      </c>
+      <c r="M94" t="s">
+        <v>43</v>
+      </c>
+      <c r="N94" t="s">
+        <v>207</v>
+      </c>
+      <c r="O94">
         <v>1</v>
       </c>
-      <c r="P79" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>210</v>
-      </c>
-      <c r="R79" t="s">
-        <v>211</v>
+      <c r="P94" t="s">
+        <v>208</v>
+      </c>
+      <c r="R94" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>23</v>
+      </c>
+      <c r="G95" t="s">
+        <v>24</v>
+      </c>
+      <c r="H95" t="s">
+        <v>48</v>
+      </c>
+      <c r="I95" t="s">
+        <v>49</v>
+      </c>
+      <c r="J95" t="s">
+        <v>50</v>
+      </c>
+      <c r="L95" t="s">
+        <v>213</v>
+      </c>
+      <c r="M95" t="s">
+        <v>59</v>
+      </c>
+      <c r="N95" t="s">
+        <v>214</v>
+      </c>
+      <c r="O95">
+        <v>4</v>
+      </c>
+      <c r="P95" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q95" t="s">
+        <v>216</v>
+      </c>
+      <c r="R95" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" t="s">
+        <v>23</v>
+      </c>
+      <c r="G96" t="s">
+        <v>24</v>
+      </c>
+      <c r="H96" t="s">
+        <v>48</v>
+      </c>
+      <c r="I96" t="s">
+        <v>49</v>
+      </c>
+      <c r="J96" t="s">
+        <v>50</v>
+      </c>
+      <c r="L96" t="s">
+        <v>218</v>
+      </c>
+      <c r="M96" t="s">
+        <v>59</v>
+      </c>
+      <c r="N96" t="s">
+        <v>214</v>
+      </c>
+      <c r="O96">
+        <v>3</v>
+      </c>
+      <c r="P96" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q96" t="s">
+        <v>216</v>
+      </c>
+      <c r="R96" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" t="s">
+        <v>23</v>
+      </c>
+      <c r="G97" t="s">
+        <v>24</v>
+      </c>
+      <c r="H97" t="s">
+        <v>48</v>
+      </c>
+      <c r="I97" t="s">
+        <v>49</v>
+      </c>
+      <c r="J97" t="s">
+        <v>50</v>
+      </c>
+      <c r="L97" t="s">
+        <v>220</v>
+      </c>
+      <c r="M97" t="s">
+        <v>59</v>
+      </c>
+      <c r="N97" t="s">
+        <v>221</v>
+      </c>
+      <c r="O97">
+        <v>1</v>
+      </c>
+      <c r="P97" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q97" t="s">
+        <v>222</v>
+      </c>
+      <c r="R97" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: interpretation in observation #79
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>18f35809-12c4-4686-bbbd-d3340cce7601</t>
+    <t>acd21a00-9511-48f4-80c3-cead3641eab5</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>8f722592-e71d-4b05-8e7c-3b30bef89e70</t>
+    <t>a5176fc8-1b39-46ff-8a9e-3b2637ce576d</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>34df525a-32e5-493c-a1f4-d3408ee4c4d7</t>
+    <t>ecfc54ed-a1b2-4a03-a474-570f0327e13f</t>
   </si>
   <si>
     <t>Invalid Answer Code</t>
@@ -159,7 +159,7 @@
     <t>WARNING</t>
   </si>
   <si>
-    <t>9469f810-0689-4da8-a980-621368c15427</t>
+    <t>cc483033-701a-464d-870a-121c406d995d</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -186,7 +186,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>d472a582-0b4b-4120-aed9-301962c39103</t>
+    <t>ee9cf181-0c27-491e-b428-4bbdb13abf68</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -204,7 +204,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>99b97686-23ad-4866-8dff-640d5ed58c09</t>
+    <t>e5f726d2-a08a-4017-82fb-6f8adc775ad7</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -222,13 +222,13 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>a5a1d6bc-2ea0-4cc6-92e3-089e1bd9f240</t>
-  </si>
-  <si>
-    <t>7e822635-51ee-4273-8f34-a21a0784dd9b</t>
-  </si>
-  <si>
-    <t>dcdf57ff-b96c-4048-9640-bbf1db7f854d</t>
+    <t>649bff15-140d-4fc5-9a4d-12374ec0536d</t>
+  </si>
+  <si>
+    <t>d924d541-1f77-4a02-a05e-5b45713daef4</t>
+  </si>
+  <si>
+    <t>0014ef4d-b4f9-4bd5-bf4a-58eb318ac552</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "96842-0" and Answer Code "LA18891-4" are not matching with the reference data found in ANSWER_CODE</t>
@@ -237,10 +237,10 @@
     <t>LA18891-4</t>
   </si>
   <si>
-    <t>24e6e0e4-6c11-4ee1-9563-7c926f8e8790</t>
-  </si>
-  <si>
-    <t>7e505f38-0a8a-4f62-ac05-885d80f954fb</t>
+    <t>b0292c27-661a-41f7-b50c-98a14d950b10</t>
+  </si>
+  <si>
+    <t>1fbbbdd0-a252-49b1-81e2-4cbdba850ba3</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -249,13 +249,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>4444bdac-5b7c-477f-9753-084dbdcd4494</t>
-  </si>
-  <si>
-    <t>2eb16b50-6b3b-48ce-9cca-c9faed6f1cae</t>
-  </si>
-  <si>
-    <t>0f976ad7-b6ef-4794-a7a9-898954b41f6f</t>
+    <t>9c30ee6e-4f96-4361-85e8-c091c11e333b</t>
+  </si>
+  <si>
+    <t>b51e797e-6a03-4643-ad4f-bcee158c9f1b</t>
+  </si>
+  <si>
+    <t>6e9f267a-20c6-42a8-9a76-cd9c05265110</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "44255-8" and Answer Code "LA6569-3" are not matching with the reference data found in ANSWER_CODE</t>
@@ -264,7 +264,7 @@
     <t>LA6569-3</t>
   </si>
   <si>
-    <t>63caee03-619a-45e0-9b8b-adc8582bcd94</t>
+    <t>debeaf96-c691-4074-9c85-086be4208b84</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -276,13 +276,13 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>62f5530c-c0db-4c70-bff3-9ec6eda6e377</t>
-  </si>
-  <si>
-    <t>7f3ae49e-8eca-44cf-ad21-5db6632fc78c</t>
-  </si>
-  <si>
-    <t>0a20d09e-6a2e-4344-a426-810035742d85</t>
+    <t>f54a0b04-8459-472f-91cc-662eea6c7680</t>
+  </si>
+  <si>
+    <t>5d29a9e6-a8a5-447c-a52f-036c174e52ab</t>
+  </si>
+  <si>
+    <t>567dd62c-9034-4f3b-b4b3-a729c3c8e08e</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "96781-0" and Answer Code "LA31979-0" are not matching with the reference data found in ANSWER_CODE</t>
@@ -291,16 +291,16 @@
     <t>LA31979-0</t>
   </si>
   <si>
-    <t>19c1da9c-6315-4dc3-8a3a-3233bf564ac7</t>
-  </si>
-  <si>
-    <t>0db7fcac-77b7-4a7f-935a-345e23e9c06b</t>
-  </si>
-  <si>
-    <t>8c076cf1-86de-4ced-9141-c0c840179a1c</t>
-  </si>
-  <si>
-    <t>34dc9014-4813-4f8d-895d-4cc2c4b67ecd</t>
+    <t>aabf14f0-257f-43c9-a4fc-278a346ffa58</t>
+  </si>
+  <si>
+    <t>aab2cf71-dca1-452a-bf14-b56062d9d4f1</t>
+  </si>
+  <si>
+    <t>738e042b-2620-4c82-a642-a5beb55a6a02</t>
+  </si>
+  <si>
+    <t>1c8289ed-7608-4e6b-b7b6-082a8ff11ecf</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68524-8" and Answer Code "LA6270-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -309,31 +309,31 @@
     <t>LA6270-8</t>
   </si>
   <si>
-    <t>d3548573-63d9-4acb-9f4d-62480f2f062f</t>
-  </si>
-  <si>
-    <t>40ccd34a-ee04-42d0-88bf-9924dcce854f</t>
-  </si>
-  <si>
-    <t>6e724ffc-e219-4a40-8274-99d395a9535d</t>
-  </si>
-  <si>
-    <t>64045e52-a909-480a-8f12-c0061b176955</t>
+    <t>1aec4b08-791c-40ae-aa4e-099ba2df7423</t>
+  </si>
+  <si>
+    <t>8fa111e5-8af2-4396-9970-a746ee376c85</t>
+  </si>
+  <si>
+    <t>f0bf1e50-97bb-4706-9b9f-56b0cfb20bb4</t>
+  </si>
+  <si>
+    <t>47ca3904-83ea-435c-9b67-5cd16c013598</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68517-2" and Answer Code "LA6270-8" are not matching with the reference data found in ANSWER_CODE</t>
   </si>
   <si>
-    <t>d76bab4a-fdd5-4fbf-b79a-933e0c7671a7</t>
-  </si>
-  <si>
-    <t>68c2108d-5bb5-4e34-b61f-b79c5d70fa26</t>
-  </si>
-  <si>
-    <t>d48bed29-3aa3-470d-be47-9ad4c18faebd</t>
-  </si>
-  <si>
-    <t>43a1abc9-008f-4814-81a1-71913afd2058</t>
+    <t>c79778a9-cd6c-4572-ab3a-2bd0c469d359</t>
+  </si>
+  <si>
+    <t>1903820c-3c30-4de0-b42f-6e9d27440810</t>
+  </si>
+  <si>
+    <t>8518be33-0bb4-499b-aba0-c9dabb89a160</t>
+  </si>
+  <si>
+    <t>4ef19dd6-1c73-40e1-af0d-30f609cbe595</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "69858-9" and Answer Code "LA33-6" are not matching with the reference data found in ANSWER_CODE</t>
@@ -342,16 +342,16 @@
     <t>LA33-6</t>
   </si>
   <si>
-    <t>5e06ffda-e146-47b2-9952-13162bc2bc03</t>
-  </si>
-  <si>
-    <t>94f35b70-8d70-4fd5-b908-5633abda107d</t>
-  </si>
-  <si>
-    <t>f95afc54-2829-4f35-8e00-c19f919bdec2</t>
-  </si>
-  <si>
-    <t>709eec19-a26d-45ac-9753-d3a33b8e797d</t>
+    <t>6fd52d2e-5a6c-4ee5-8522-393aa7877a87</t>
+  </si>
+  <si>
+    <t>97a205b2-98f5-4fd7-8aef-c17415d402ec</t>
+  </si>
+  <si>
+    <t>693e6a04-3be5-494c-a9b1-67a69e30f51a</t>
+  </si>
+  <si>
+    <t>ac297eb7-8ac6-4052-acb2-4709ef7e0a31</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in ANSWER_CODE</t>
@@ -360,16 +360,16 @@
     <t>LA28853-2</t>
   </si>
   <si>
-    <t>f7789803-62b8-4452-a9e1-d3572387d7d1</t>
-  </si>
-  <si>
-    <t>f6fed19c-f5a7-4374-b3c6-258c13e874ce</t>
-  </si>
-  <si>
-    <t>236a2fda-352f-43ad-b215-7eb27b90aadf</t>
-  </si>
-  <si>
-    <t>2f69b10c-cc49-4409-80bc-082acc5c4f94</t>
+    <t>c3879b21-8ef5-4ffe-97ca-c00a6c45d849</t>
+  </si>
+  <si>
+    <t>7bd429b0-eae0-42fe-8eec-7d21ef655dfd</t>
+  </si>
+  <si>
+    <t>5b5d7707-1f12-4d58-a7ca-56e85111ca23</t>
+  </si>
+  <si>
+    <t>06b68a85-7976-4fa2-ba6f-a121eb363fca</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in ANSWER_CODE</t>
@@ -378,7 +378,7 @@
     <t>LA6571-9</t>
   </si>
   <si>
-    <t>5cb54e2e-d74a-40f9-b3d4-1c89d634192a</t>
+    <t>3dbd6b1d-ff17-40e6-8afc-81d4ef1331ea</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -393,13 +393,13 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>1f7c0114-dadb-463e-8e44-1fbe90dd1b19</t>
-  </si>
-  <si>
-    <t>9d2dbdfa-baa8-4b8f-b757-b2b7b6e859aa</t>
-  </si>
-  <si>
-    <t>1cf085f6-f7f2-4a9a-9103-82afdbc40947</t>
+    <t>32afeb54-8ad6-4827-b970-0046d04a7cc8</t>
+  </si>
+  <si>
+    <t>dd6dff5e-3389-4b43-8f65-7cb773adfb40</t>
+  </si>
+  <si>
+    <t>26851362-3e2d-4643-8dfe-765ab4e73f78</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "93038-8" and Answer Code "LA13902-4" are not matching with the reference data found in ANSWER_CODE</t>
@@ -408,7 +408,7 @@
     <t>LA13902-4</t>
   </si>
   <si>
-    <t>3c1521f8-b6e4-427c-a394-db4da2243e49</t>
+    <t>c14f5105-f52e-45d5-8ddf-f51df4ff658d</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44255-8" and Answer Code "LA6569-3" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
@@ -417,13 +417,13 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>282f9cca-a8d2-4563-93cf-0cf65e5862a4</t>
-  </si>
-  <si>
-    <t>ac11819e-1046-4c6b-9cee-811a34370e23</t>
-  </si>
-  <si>
-    <t>d87c1376-2c74-4ecb-8be1-d299e418fb9f</t>
+    <t>a48990c9-04c9-438c-a543-efe791b77dd7</t>
+  </si>
+  <si>
+    <t>6949647c-8eff-42de-9034-764d207e1b29</t>
+  </si>
+  <si>
+    <t>c82edfd8-1811-4947-ba2a-9447b2d7b77e</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "97027-7" and Answer Code "LA32-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -432,7 +432,7 @@
     <t>LA32-8</t>
   </si>
   <si>
-    <t>11939701-a721-4067-b850-70c0dd57d1ec</t>
+    <t>864f006f-3daf-407f-b3be-d7b4d9e795d2</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "69858-9" and Answer Code "LA33-6" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
@@ -441,10 +441,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>a0d31bb3-d1d2-4ba0-a1ea-e4bd750b3203</t>
-  </si>
-  <si>
-    <t>dc1b16bd-486e-437e-af94-42d64fc92142</t>
+    <t>e963b326-b443-4727-9cc1-aca1a9ef2f97</t>
+  </si>
+  <si>
+    <t>09811053-03e8-4351-b9ed-927889907f6c</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -453,25 +453,25 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>fea8e7fe-4105-4b7d-baba-0edae95646fc</t>
+    <t>5c4657dc-8cff-4f78-83f8-8356e608aada</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "69861-3" and Answer Code "LA32-8" are not matching with the reference data found in ANSWER_CODE</t>
   </si>
   <si>
-    <t>ddf2813a-fdb5-4e49-a5f3-f7f2072248ff</t>
+    <t>a73e0c04-7f06-400b-91f8-4a9d4553d99c</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>7119a7e7-526f-4987-bb34-7970ea26bf71</t>
-  </si>
-  <si>
-    <t>8a1b8e04-b5d7-483c-ab60-c1f3410bc1d5</t>
-  </si>
-  <si>
-    <t>6ef5e26d-765d-47a9-9999-21e06c523cac</t>
+    <t>9b213f1a-2551-4415-9b20-b98782006e5e</t>
+  </si>
+  <si>
+    <t>7a31426b-9330-4387-b9f0-a56a0603310a</t>
+  </si>
+  <si>
+    <t>edb2c003-6fd8-4b62-b87f-36be0eca2ab2</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "93159-2" and Answer Code "LA10044-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -480,190 +480,190 @@
     <t>LA10044-8</t>
   </si>
   <si>
-    <t>f0ea9208-cd26-46f9-834e-45a440999929</t>
+    <t>1611130b-33a0-4b1c-8e4e-694348e4a344</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "68524-8" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>c5d16bf4-bb77-43cd-812a-6d03dfa11f7f</t>
-  </si>
-  <si>
-    <t>b4c3394d-c042-442a-b2a7-11431727dc25</t>
-  </si>
-  <si>
-    <t>929c2fcb-5731-44f2-9eb8-038715fd63fc</t>
+    <t>a5505694-0081-4d4d-9da9-dc6eb0e4589c</t>
+  </si>
+  <si>
+    <t>c443079e-1771-4ccf-aeee-ba5f2ea821b7</t>
+  </si>
+  <si>
+    <t>6e63d31e-0fdb-41a7-bbf5-f2a9a005db6e</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>f0f97103-6f38-454e-bc3e-40ce70a0b180</t>
-  </si>
-  <si>
-    <t>9d15cc56-53a0-4f08-8f71-84d9ace82416</t>
-  </si>
-  <si>
-    <t>6ef391fa-a23f-455c-8dab-8064d32bf49a</t>
+    <t>0710b8b5-7b25-445e-a118-ab9bbbf436ee</t>
+  </si>
+  <si>
+    <t>ef391bf4-ad8e-488c-b4a6-9e92f7b612d1</t>
+  </si>
+  <si>
+    <t>801fa8dd-c990-4b62-9672-35b863b0b54d</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "76513-1" and Answer Code "LA15832-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>69a287c0-495c-436c-9baa-ecbb3c0c6ed9</t>
-  </si>
-  <si>
-    <t>c75c1085-b113-44f2-899f-00dc17008432</t>
-  </si>
-  <si>
-    <t>fb1122ca-f6d0-484d-8b96-749b2c8a2ca0</t>
+    <t>9b2f456d-f1ba-4638-a38c-d4d0add84488</t>
+  </si>
+  <si>
+    <t>79d3c887-6111-4ee2-bb15-356e02d5d5fa</t>
+  </si>
+  <si>
+    <t>6e176bde-3792-42f5-9d5c-45bf3c40ed0a</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>4271086d-1f1f-4de4-b2e3-163b0b5e7394</t>
-  </si>
-  <si>
-    <t>d64ad7a4-5762-4705-bf1e-b6231cf8a93d</t>
-  </si>
-  <si>
-    <t>8853e600-59db-4081-8fd0-0cffca526a10</t>
+    <t>558d1955-2fb8-4aea-ab86-a6dfdedf5dde</t>
+  </si>
+  <si>
+    <t>35509e26-087f-4b6c-9aec-e6c0fb2599d9</t>
+  </si>
+  <si>
+    <t>85699b23-56ed-424f-ab58-96d44ba3547d</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "97027-7" and Answer Code "LA32-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>5c699d09-afbb-469b-b3d1-642593c37da1</t>
-  </si>
-  <si>
-    <t>cf02082d-2405-4ea6-970a-644bb7d43823</t>
-  </si>
-  <si>
-    <t>5394fdb4-8b40-4961-9202-90aae64dfc85</t>
+    <t>1d2454c1-cb00-4203-aa0e-752a112c9d71</t>
+  </si>
+  <si>
+    <t>4566e1c7-b260-406e-9dc7-335d9b51e84a</t>
+  </si>
+  <si>
+    <t>936c6634-cf5c-4a84-a515-9efc0d7558a7</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>2a595655-da66-406d-935e-c15842bc23a2</t>
-  </si>
-  <si>
-    <t>87656cb0-b574-482f-ac26-30ecbbd14b53</t>
-  </si>
-  <si>
-    <t>89ba1e7a-413d-4c86-95d8-009fa86752ae</t>
+    <t>5f7a94ff-8d8e-4414-8974-ad3f4f3bfe33</t>
+  </si>
+  <si>
+    <t>0daea509-02a1-44ea-8f16-a6532f5aa2db</t>
+  </si>
+  <si>
+    <t>12b91a47-a951-44c6-9f5a-e4b64c1568bc</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>7e47d60d-aa93-4e8f-b5b8-0d9aa55b98be</t>
-  </si>
-  <si>
-    <t>60fad860-feb1-44dd-9d68-204b54b96fdf</t>
-  </si>
-  <si>
-    <t>4923dc54-100a-4bd7-b9fc-5eb7867a65c3</t>
+    <t>46c1984b-4591-4a2a-9f69-c6324793c3dd</t>
+  </si>
+  <si>
+    <t>1bf4ddd3-062f-4ade-95f7-3577f5129124</t>
+  </si>
+  <si>
+    <t>6528c3f4-4a64-42ba-89e5-14342d8d794b</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "96781-0" and Answer Code "LA31979-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>a6e60b9f-f570-4a9e-a956-4445459fc626</t>
-  </si>
-  <si>
-    <t>b895de91-8a9a-4acc-8aa3-2fe25f522190</t>
-  </si>
-  <si>
-    <t>f4ece211-1a3e-4dfc-ad7c-2b3d51d9c8e8</t>
+    <t>d60704d3-536a-41e8-bb32-15ea1431e18a</t>
+  </si>
+  <si>
+    <t>0eda4177-5608-49d4-9db9-5eb72a7b91fc</t>
+  </si>
+  <si>
+    <t>d0c95e55-c098-4dbc-a9c0-8779ae476660</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>0915beef-3bbc-441c-879f-a289a92af788</t>
-  </si>
-  <si>
-    <t>488135a0-bb4d-4ed6-83d5-f70b845fbee6</t>
-  </si>
-  <si>
-    <t>fed6f6fb-6623-447b-9097-33574a0ac4d1</t>
+    <t>6e1f2434-21a5-4b11-aeb1-af482a57392f</t>
+  </si>
+  <si>
+    <t>8037f2ef-e125-4bca-ac0e-be3ff1dc1474</t>
+  </si>
+  <si>
+    <t>59b9e6d9-e4e6-4636-8cc4-05d3854ffb21</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "93159-2" and Answer Code "LA10044-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>c79ea32f-dc13-4c16-a1e9-ad997ca2ec2b</t>
-  </si>
-  <si>
-    <t>5dc2cd86-31e3-4cf3-b572-d50a6e61d877</t>
-  </si>
-  <si>
-    <t>3006a651-8a3b-4361-bbe4-bfd120b6d1a3</t>
+    <t>2213cbde-f7cc-4943-bb6c-ba174cb0c4b5</t>
+  </si>
+  <si>
+    <t>56c2c6fc-4885-4142-afbd-d2f6aa719c90</t>
+  </si>
+  <si>
+    <t>12bee8c6-4dd7-45c5-8e55-eeb616020bf4</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>72279112-c5c0-478f-b522-de27343bc6a8</t>
-  </si>
-  <si>
-    <t>3a2231ab-3981-40f4-b4c5-9b535203c6aa</t>
-  </si>
-  <si>
-    <t>092db5f5-d166-4475-8bb0-7a98b1d4115d</t>
+    <t>3eb261de-9001-42e0-afb9-fd861cf16e75</t>
+  </si>
+  <si>
+    <t>1f761cd3-d176-4b7c-a102-bdcae8cb9f44</t>
+  </si>
+  <si>
+    <t>378b1777-5a10-4d4a-a442-059ce3d7c082</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "93038-8" and Answer Code "LA13902-4" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>73668bd9-3aad-4721-b4cd-50991f01b913</t>
-  </si>
-  <si>
-    <t>4f5be7f8-dfde-40f2-9a2a-9276690cf0b8</t>
-  </si>
-  <si>
-    <t>0ff813c8-6ca6-40d3-90e1-8a83aba8fe4c</t>
+    <t>ef76d150-9999-4877-a8b9-a142ae3f98a9</t>
+  </si>
+  <si>
+    <t>66f68cd5-c981-4ba0-95f4-dbc2a55972d5</t>
+  </si>
+  <si>
+    <t>1dbba41f-4527-4a81-afb7-b92f6bc0740a</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "69861-3" and Answer Code "LA32-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>566d1647-3598-4b8b-ad23-fa72324c716e</t>
-  </si>
-  <si>
-    <t>8a9ccda6-55ee-4185-a15e-4094c0cccd2a</t>
-  </si>
-  <si>
-    <t>ce68942c-1f9f-4753-8869-c8e4d2e6be80</t>
+    <t>37d1d80d-e7d0-4b6b-a1eb-d85aed2f6a4b</t>
+  </si>
+  <si>
+    <t>3bb2e3e3-6f3f-4c45-96b8-552880b2c669</t>
+  </si>
+  <si>
+    <t>4cd932df-49f6-42e5-9a66-5ccb03d5b1db</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "96842-0" and Answer Code "LA18891-4" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>92560696-f8a5-4120-9b32-a1a03de932d1</t>
-  </si>
-  <si>
-    <t>634118ee-3d99-47d1-9721-7d60d8ab06ae</t>
-  </si>
-  <si>
-    <t>be5cd47c-eefc-4bd4-878c-030dadf60962</t>
-  </si>
-  <si>
-    <t>34a504bb-63b1-483c-a99a-378da6092009</t>
-  </si>
-  <si>
-    <t>11f01971-da61-48db-a254-621419a49660</t>
-  </si>
-  <si>
-    <t>e00b7b88-7675-478f-8490-655a8c8cbd33</t>
-  </si>
-  <si>
-    <t>7a70f0fc-6794-4521-b20e-e092d0f4b956</t>
-  </si>
-  <si>
-    <t>8c6da3ba-e511-4559-ad92-54518500e979</t>
+    <t>fc5f02b3-048a-49eb-8a52-2c03c256d4b6</t>
+  </si>
+  <si>
+    <t>2e256766-2bed-40ae-9feb-599a5d131a5c</t>
+  </si>
+  <si>
+    <t>d8c10733-24f8-4d3d-aa76-1eb89b665be8</t>
+  </si>
+  <si>
+    <t>3e0aae8a-86c8-4b0b-925c-370dd8a8dedd</t>
+  </si>
+  <si>
+    <t>5c48bb3c-10d0-4da2-845b-1f76bfc5ff91</t>
+  </si>
+  <si>
+    <t>d456a5fe-9b10-4652-b169-5f0feacfef43</t>
+  </si>
+  <si>
+    <t>c12a0fb5-56f6-4bfb-8988-c40c2b976b47</t>
+  </si>
+  <si>
+    <t>2d3bf0d1-5f03-4b83-92ec-d8f13d74ff78</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -816,7 +816,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>26c90ffb-d623-406f-8808-67dc499faed9</t>
+    <t>99d7158e-91a4-4ed8-825e-4a351a2d7fa9</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
feat: update the generated FHIR json structure #82
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -81,7 +81,7 @@
     <t>7bab389e-54af-5a13-a39f-079abdc73a48</t>
   </si>
   <si>
-    <t>0.8.5</t>
+    <t>0.10.0</t>
   </si>
   <si>
     <t>Session 05269d28-15ae-5bd6-bd88-f949ccfa52d7 markdown diagnostics not provided (not completed?)</t>
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>acd21a00-9511-48f4-80c3-cead3641eab5</t>
+    <t>7d3130df-50b7-429c-8354-be2781c2e78b</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>a5176fc8-1b39-46ff-8a9e-3b2637ce576d</t>
+    <t>970f3a23-308f-4875-aeed-a9c8010732b4</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>ecfc54ed-a1b2-4a03-a474-570f0327e13f</t>
+    <t>2aa428f9-e8ca-4525-872f-bd6224121a31</t>
   </si>
   <si>
     <t>Invalid Answer Code</t>
@@ -159,7 +159,7 @@
     <t>WARNING</t>
   </si>
   <si>
-    <t>cc483033-701a-464d-870a-121c406d995d</t>
+    <t>5f7614c3-9e73-47e7-9bc9-99999364ae19</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -186,7 +186,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>ee9cf181-0c27-491e-b428-4bbdb13abf68</t>
+    <t>5f5046ce-d6bf-40f4-a113-90c87683310e</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -204,7 +204,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>e5f726d2-a08a-4017-82fb-6f8adc775ad7</t>
+    <t>0090848b-3389-4f3d-8899-9174dae0c622</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -222,13 +222,13 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>649bff15-140d-4fc5-9a4d-12374ec0536d</t>
-  </si>
-  <si>
-    <t>d924d541-1f77-4a02-a05e-5b45713daef4</t>
-  </si>
-  <si>
-    <t>0014ef4d-b4f9-4bd5-bf4a-58eb318ac552</t>
+    <t>63c20d3e-5a88-4cd1-a6ba-491850a65151</t>
+  </si>
+  <si>
+    <t>5c2f7272-f544-486c-8487-46b3ee126efc</t>
+  </si>
+  <si>
+    <t>6516c754-1959-41ad-80c2-689a5a13341f</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "96842-0" and Answer Code "LA18891-4" are not matching with the reference data found in ANSWER_CODE</t>
@@ -237,10 +237,10 @@
     <t>LA18891-4</t>
   </si>
   <si>
-    <t>b0292c27-661a-41f7-b50c-98a14d950b10</t>
-  </si>
-  <si>
-    <t>1fbbbdd0-a252-49b1-81e2-4cbdba850ba3</t>
+    <t>f7bbe4fd-9832-4732-9014-dab8cc90433c</t>
+  </si>
+  <si>
+    <t>79b706fc-a190-48de-a5be-38b9499c5ff4</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -249,13 +249,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>9c30ee6e-4f96-4361-85e8-c091c11e333b</t>
-  </si>
-  <si>
-    <t>b51e797e-6a03-4643-ad4f-bcee158c9f1b</t>
-  </si>
-  <si>
-    <t>6e9f267a-20c6-42a8-9a76-cd9c05265110</t>
+    <t>1bc36a0b-6bec-4d03-91b1-a77580353f2c</t>
+  </si>
+  <si>
+    <t>73ee848c-b9fc-4ee4-af18-a6a5140092c9</t>
+  </si>
+  <si>
+    <t>6d1a4149-7db8-479f-9b12-6a0a1ea06fa4</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "44255-8" and Answer Code "LA6569-3" are not matching with the reference data found in ANSWER_CODE</t>
@@ -264,7 +264,7 @@
     <t>LA6569-3</t>
   </si>
   <si>
-    <t>debeaf96-c691-4074-9c85-086be4208b84</t>
+    <t>8b14cf18-2ccd-4c7f-9146-d78f4d978131</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -276,13 +276,13 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>f54a0b04-8459-472f-91cc-662eea6c7680</t>
-  </si>
-  <si>
-    <t>5d29a9e6-a8a5-447c-a52f-036c174e52ab</t>
-  </si>
-  <si>
-    <t>567dd62c-9034-4f3b-b4b3-a729c3c8e08e</t>
+    <t>5485f038-d864-4f35-9576-c3fc3f94cc1c</t>
+  </si>
+  <si>
+    <t>edcc23eb-1679-48d7-ab2f-32ddbf286025</t>
+  </si>
+  <si>
+    <t>35cbf2f9-fb17-4ddc-881b-f249aad5c85a</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "96781-0" and Answer Code "LA31979-0" are not matching with the reference data found in ANSWER_CODE</t>
@@ -291,16 +291,16 @@
     <t>LA31979-0</t>
   </si>
   <si>
-    <t>aabf14f0-257f-43c9-a4fc-278a346ffa58</t>
-  </si>
-  <si>
-    <t>aab2cf71-dca1-452a-bf14-b56062d9d4f1</t>
-  </si>
-  <si>
-    <t>738e042b-2620-4c82-a642-a5beb55a6a02</t>
-  </si>
-  <si>
-    <t>1c8289ed-7608-4e6b-b7b6-082a8ff11ecf</t>
+    <t>c03ca390-ee24-4c08-b0f2-8084f2ea28bb</t>
+  </si>
+  <si>
+    <t>1524a424-a9a9-4dfa-89b1-00e74e3dc9d9</t>
+  </si>
+  <si>
+    <t>e0f7d99a-d838-4aad-8f55-ca83037ca84d</t>
+  </si>
+  <si>
+    <t>e3a8a36e-324a-4a21-8b3b-6b9e99e9bf47</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68524-8" and Answer Code "LA6270-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -309,31 +309,31 @@
     <t>LA6270-8</t>
   </si>
   <si>
-    <t>1aec4b08-791c-40ae-aa4e-099ba2df7423</t>
-  </si>
-  <si>
-    <t>8fa111e5-8af2-4396-9970-a746ee376c85</t>
-  </si>
-  <si>
-    <t>f0bf1e50-97bb-4706-9b9f-56b0cfb20bb4</t>
-  </si>
-  <si>
-    <t>47ca3904-83ea-435c-9b67-5cd16c013598</t>
+    <t>db33908d-84ab-48a0-8de9-a7344e2fdebc</t>
+  </si>
+  <si>
+    <t>7f2bd43e-efad-4166-a197-caca396c7645</t>
+  </si>
+  <si>
+    <t>edfad29c-cae4-45dc-a477-eb6d0b10520f</t>
+  </si>
+  <si>
+    <t>52a046f3-f40d-4bed-a3c2-9d46ed164066</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68517-2" and Answer Code "LA6270-8" are not matching with the reference data found in ANSWER_CODE</t>
   </si>
   <si>
-    <t>c79778a9-cd6c-4572-ab3a-2bd0c469d359</t>
-  </si>
-  <si>
-    <t>1903820c-3c30-4de0-b42f-6e9d27440810</t>
-  </si>
-  <si>
-    <t>8518be33-0bb4-499b-aba0-c9dabb89a160</t>
-  </si>
-  <si>
-    <t>4ef19dd6-1c73-40e1-af0d-30f609cbe595</t>
+    <t>1315191e-507c-4860-b5a8-49a930143651</t>
+  </si>
+  <si>
+    <t>fd8de152-86a8-4f5a-91fc-0e8ad6c03a7e</t>
+  </si>
+  <si>
+    <t>5a4e2085-7cdd-4aa2-8dc6-974c00ceb666</t>
+  </si>
+  <si>
+    <t>6c00a0c2-4871-457a-a490-46698eea8d18</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "69858-9" and Answer Code "LA33-6" are not matching with the reference data found in ANSWER_CODE</t>
@@ -342,16 +342,16 @@
     <t>LA33-6</t>
   </si>
   <si>
-    <t>6fd52d2e-5a6c-4ee5-8522-393aa7877a87</t>
-  </si>
-  <si>
-    <t>97a205b2-98f5-4fd7-8aef-c17415d402ec</t>
-  </si>
-  <si>
-    <t>693e6a04-3be5-494c-a9b1-67a69e30f51a</t>
-  </si>
-  <si>
-    <t>ac297eb7-8ac6-4052-acb2-4709ef7e0a31</t>
+    <t>408752d3-5563-40ee-a9d6-68f731bf48f9</t>
+  </si>
+  <si>
+    <t>7b0932d3-3fcc-434f-a3a2-ecd786fa5d13</t>
+  </si>
+  <si>
+    <t>b4a582bd-55b2-4988-b48a-c62c4b70a3d6</t>
+  </si>
+  <si>
+    <t>155f15b6-89ba-41b1-bf39-b3e0cc337de7</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in ANSWER_CODE</t>
@@ -360,16 +360,16 @@
     <t>LA28853-2</t>
   </si>
   <si>
-    <t>c3879b21-8ef5-4ffe-97ca-c00a6c45d849</t>
-  </si>
-  <si>
-    <t>7bd429b0-eae0-42fe-8eec-7d21ef655dfd</t>
-  </si>
-  <si>
-    <t>5b5d7707-1f12-4d58-a7ca-56e85111ca23</t>
-  </si>
-  <si>
-    <t>06b68a85-7976-4fa2-ba6f-a121eb363fca</t>
+    <t>5e900cf0-fcd1-438e-8bcd-23dce6a0d248</t>
+  </si>
+  <si>
+    <t>ef9164f5-5f5f-4a8c-a7cd-4ff1509a996b</t>
+  </si>
+  <si>
+    <t>e93f8c06-7e5e-49b0-9e12-5c52fe1ebb85</t>
+  </si>
+  <si>
+    <t>5bcdbb96-e63a-4f77-9bdf-767492bcfd44</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in ANSWER_CODE</t>
@@ -378,7 +378,7 @@
     <t>LA6571-9</t>
   </si>
   <si>
-    <t>3dbd6b1d-ff17-40e6-8afc-81d4ef1331ea</t>
+    <t>8bf8e88d-5c62-4921-a651-84a690d607f0</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -393,13 +393,13 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>32afeb54-8ad6-4827-b970-0046d04a7cc8</t>
-  </si>
-  <si>
-    <t>dd6dff5e-3389-4b43-8f65-7cb773adfb40</t>
-  </si>
-  <si>
-    <t>26851362-3e2d-4643-8dfe-765ab4e73f78</t>
+    <t>025b8512-4c75-4d04-88d2-8f926b3ad26a</t>
+  </si>
+  <si>
+    <t>76110869-eec6-43cc-a8a0-b8753a77d45c</t>
+  </si>
+  <si>
+    <t>5b41f561-a1e0-4f99-8da6-80bbf546da39</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "93038-8" and Answer Code "LA13902-4" are not matching with the reference data found in ANSWER_CODE</t>
@@ -408,7 +408,7 @@
     <t>LA13902-4</t>
   </si>
   <si>
-    <t>c14f5105-f52e-45d5-8ddf-f51df4ff658d</t>
+    <t>a1e06888-6e29-4858-b05c-64b3bfb14bbc</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44255-8" and Answer Code "LA6569-3" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
@@ -417,13 +417,13 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>a48990c9-04c9-438c-a543-efe791b77dd7</t>
-  </si>
-  <si>
-    <t>6949647c-8eff-42de-9034-764d207e1b29</t>
-  </si>
-  <si>
-    <t>c82edfd8-1811-4947-ba2a-9447b2d7b77e</t>
+    <t>d5d43fec-49d9-45de-b5a6-0d313887c5e5</t>
+  </si>
+  <si>
+    <t>d91c129e-dc2c-45c6-812d-7919a5f38b7a</t>
+  </si>
+  <si>
+    <t>067d8643-0b0f-4017-b27e-9b9223780315</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "97027-7" and Answer Code "LA32-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -432,7 +432,7 @@
     <t>LA32-8</t>
   </si>
   <si>
-    <t>864f006f-3daf-407f-b3be-d7b4d9e795d2</t>
+    <t>3f43598a-3824-42ec-ade3-f449cd4812a4</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "69858-9" and Answer Code "LA33-6" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
@@ -441,10 +441,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>e963b326-b443-4727-9cc1-aca1a9ef2f97</t>
-  </si>
-  <si>
-    <t>09811053-03e8-4351-b9ed-927889907f6c</t>
+    <t>e879406b-aa02-4284-ba23-b83f61df3720</t>
+  </si>
+  <si>
+    <t>b9278cc8-f222-4f39-9200-65c99c03bd2d</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -453,25 +453,25 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>5c4657dc-8cff-4f78-83f8-8356e608aada</t>
+    <t>5c853da9-aba7-4495-9948-3f062fa3fac8</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "69861-3" and Answer Code "LA32-8" are not matching with the reference data found in ANSWER_CODE</t>
   </si>
   <si>
-    <t>a73e0c04-7f06-400b-91f8-4a9d4553d99c</t>
+    <t>2a90d219-3dcf-40cf-b85a-03ec2e035e32</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>9b213f1a-2551-4415-9b20-b98782006e5e</t>
-  </si>
-  <si>
-    <t>7a31426b-9330-4387-b9f0-a56a0603310a</t>
-  </si>
-  <si>
-    <t>edb2c003-6fd8-4b62-b87f-36be0eca2ab2</t>
+    <t>d52121f1-231f-4329-beab-1ca316bdcd13</t>
+  </si>
+  <si>
+    <t>2b93b9ee-dd8e-475d-9183-03628907443b</t>
+  </si>
+  <si>
+    <t>fcccaf8f-55bb-4430-b8bc-39e41c55ac01</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "93159-2" and Answer Code "LA10044-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -480,190 +480,190 @@
     <t>LA10044-8</t>
   </si>
   <si>
-    <t>1611130b-33a0-4b1c-8e4e-694348e4a344</t>
+    <t>1eb8cd50-8dab-4b93-b30a-9c05a5b24696</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "68524-8" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>a5505694-0081-4d4d-9da9-dc6eb0e4589c</t>
-  </si>
-  <si>
-    <t>c443079e-1771-4ccf-aeee-ba5f2ea821b7</t>
-  </si>
-  <si>
-    <t>6e63d31e-0fdb-41a7-bbf5-f2a9a005db6e</t>
+    <t>362a9ba3-b775-4b2c-a44b-ee0e0701fdb8</t>
+  </si>
+  <si>
+    <t>e921b823-ce17-45d4-b389-1f7ea878370e</t>
+  </si>
+  <si>
+    <t>500f86a2-08c5-42eb-9583-0d5812b7281f</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>0710b8b5-7b25-445e-a118-ab9bbbf436ee</t>
-  </si>
-  <si>
-    <t>ef391bf4-ad8e-488c-b4a6-9e92f7b612d1</t>
-  </si>
-  <si>
-    <t>801fa8dd-c990-4b62-9672-35b863b0b54d</t>
+    <t>7103df56-e279-4012-a281-0e2114f9fa6f</t>
+  </si>
+  <si>
+    <t>87be461b-dd68-499f-b9d5-adebef433033</t>
+  </si>
+  <si>
+    <t>dd4081dd-3c95-4bb0-83bc-74afc385b6b2</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "76513-1" and Answer Code "LA15832-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>9b2f456d-f1ba-4638-a38c-d4d0add84488</t>
-  </si>
-  <si>
-    <t>79d3c887-6111-4ee2-bb15-356e02d5d5fa</t>
-  </si>
-  <si>
-    <t>6e176bde-3792-42f5-9d5c-45bf3c40ed0a</t>
+    <t>6a00c6da-9a2a-4aad-997f-f45be9997179</t>
+  </si>
+  <si>
+    <t>4f142396-71c2-4a8d-ac64-3e0fc5043a09</t>
+  </si>
+  <si>
+    <t>fdcba316-55b2-4385-9358-717507921100</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>558d1955-2fb8-4aea-ab86-a6dfdedf5dde</t>
-  </si>
-  <si>
-    <t>35509e26-087f-4b6c-9aec-e6c0fb2599d9</t>
-  </si>
-  <si>
-    <t>85699b23-56ed-424f-ab58-96d44ba3547d</t>
+    <t>c6c7efbf-93c5-43f9-a778-b0de7a6a4d89</t>
+  </si>
+  <si>
+    <t>3c3bea8b-a30e-411b-b2f6-84f738ba8a7a</t>
+  </si>
+  <si>
+    <t>97bb2498-4268-4777-a8bc-10cc4974de88</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "97027-7" and Answer Code "LA32-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>1d2454c1-cb00-4203-aa0e-752a112c9d71</t>
-  </si>
-  <si>
-    <t>4566e1c7-b260-406e-9dc7-335d9b51e84a</t>
-  </si>
-  <si>
-    <t>936c6634-cf5c-4a84-a515-9efc0d7558a7</t>
+    <t>ad494fe4-0a9d-44bd-8813-524062768d08</t>
+  </si>
+  <si>
+    <t>9fe506d8-6e9b-4ab6-9db6-449c814d229d</t>
+  </si>
+  <si>
+    <t>b71c98ad-bc7c-49d5-87f7-4c3b6ccbb89c</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>5f7a94ff-8d8e-4414-8974-ad3f4f3bfe33</t>
-  </si>
-  <si>
-    <t>0daea509-02a1-44ea-8f16-a6532f5aa2db</t>
-  </si>
-  <si>
-    <t>12b91a47-a951-44c6-9f5a-e4b64c1568bc</t>
+    <t>cf82cd2d-7973-4c20-ae2f-ae2655dbbc9a</t>
+  </si>
+  <si>
+    <t>0fede892-aced-4d19-a33d-4ab95b3dc2aa</t>
+  </si>
+  <si>
+    <t>0b328383-e38d-4efa-bfca-628edb277619</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>46c1984b-4591-4a2a-9f69-c6324793c3dd</t>
-  </si>
-  <si>
-    <t>1bf4ddd3-062f-4ade-95f7-3577f5129124</t>
-  </si>
-  <si>
-    <t>6528c3f4-4a64-42ba-89e5-14342d8d794b</t>
+    <t>b5298a09-0a07-411e-8ce8-2d94a760354d</t>
+  </si>
+  <si>
+    <t>5ae8ea3d-e4dd-4d15-ad93-287aae58fe55</t>
+  </si>
+  <si>
+    <t>a590e431-cb49-420c-bbf0-54269408bdff</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "96781-0" and Answer Code "LA31979-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>d60704d3-536a-41e8-bb32-15ea1431e18a</t>
-  </si>
-  <si>
-    <t>0eda4177-5608-49d4-9db9-5eb72a7b91fc</t>
-  </si>
-  <si>
-    <t>d0c95e55-c098-4dbc-a9c0-8779ae476660</t>
+    <t>6e4de5b2-20e6-4a63-af23-c956d30a0db6</t>
+  </si>
+  <si>
+    <t>b02edc1b-e15e-4b9e-b0b7-77f9ce798d64</t>
+  </si>
+  <si>
+    <t>57c1bb4c-92fb-45fd-87e3-3d524dfd9ab0</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>6e1f2434-21a5-4b11-aeb1-af482a57392f</t>
-  </si>
-  <si>
-    <t>8037f2ef-e125-4bca-ac0e-be3ff1dc1474</t>
-  </si>
-  <si>
-    <t>59b9e6d9-e4e6-4636-8cc4-05d3854ffb21</t>
+    <t>b78f0c90-163b-4ce2-95a6-f2e9d81ab56e</t>
+  </si>
+  <si>
+    <t>dd5294bc-9ea8-4a84-95a2-ad95b403b325</t>
+  </si>
+  <si>
+    <t>314f5962-e44d-4653-8973-6cdb4c1999c2</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "93159-2" and Answer Code "LA10044-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>2213cbde-f7cc-4943-bb6c-ba174cb0c4b5</t>
-  </si>
-  <si>
-    <t>56c2c6fc-4885-4142-afbd-d2f6aa719c90</t>
-  </si>
-  <si>
-    <t>12bee8c6-4dd7-45c5-8e55-eeb616020bf4</t>
+    <t>1f8ee814-7404-4c62-b13d-b8d3c95bcceb</t>
+  </si>
+  <si>
+    <t>5ca7f71c-47bd-414a-89bc-3328bee4b4f2</t>
+  </si>
+  <si>
+    <t>8a01c7c5-0485-4e55-bb58-91396edbf552</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>3eb261de-9001-42e0-afb9-fd861cf16e75</t>
-  </si>
-  <si>
-    <t>1f761cd3-d176-4b7c-a102-bdcae8cb9f44</t>
-  </si>
-  <si>
-    <t>378b1777-5a10-4d4a-a442-059ce3d7c082</t>
+    <t>bd608a13-dc4e-44da-9deb-417739471840</t>
+  </si>
+  <si>
+    <t>af37d7a2-20fd-458e-b4c4-8d1cbbb5efb3</t>
+  </si>
+  <si>
+    <t>73b970dc-d0f2-4d06-8d7e-1c54f6c9a4f6</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "93038-8" and Answer Code "LA13902-4" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>ef76d150-9999-4877-a8b9-a142ae3f98a9</t>
-  </si>
-  <si>
-    <t>66f68cd5-c981-4ba0-95f4-dbc2a55972d5</t>
-  </si>
-  <si>
-    <t>1dbba41f-4527-4a81-afb7-b92f6bc0740a</t>
+    <t>cc5e3cbf-6172-4906-8b0b-3707b3b1f83d</t>
+  </si>
+  <si>
+    <t>e2e3e84e-3239-4864-ac88-ac74797ed78a</t>
+  </si>
+  <si>
+    <t>3863779d-d94e-4751-8149-4fc135bbdb5e</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "69861-3" and Answer Code "LA32-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>37d1d80d-e7d0-4b6b-a1eb-d85aed2f6a4b</t>
-  </si>
-  <si>
-    <t>3bb2e3e3-6f3f-4c45-96b8-552880b2c669</t>
-  </si>
-  <si>
-    <t>4cd932df-49f6-42e5-9a66-5ccb03d5b1db</t>
+    <t>aa47fcde-2351-4337-98b3-62c425a72a75</t>
+  </si>
+  <si>
+    <t>9544db2e-42bc-4be7-a77e-03391b7aa215</t>
+  </si>
+  <si>
+    <t>4a2eb67a-88fa-438f-8085-292f5c25efc7</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "96842-0" and Answer Code "LA18891-4" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>fc5f02b3-048a-49eb-8a52-2c03c256d4b6</t>
-  </si>
-  <si>
-    <t>2e256766-2bed-40ae-9feb-599a5d131a5c</t>
-  </si>
-  <si>
-    <t>d8c10733-24f8-4d3d-aa76-1eb89b665be8</t>
-  </si>
-  <si>
-    <t>3e0aae8a-86c8-4b0b-925c-370dd8a8dedd</t>
-  </si>
-  <si>
-    <t>5c48bb3c-10d0-4da2-845b-1f76bfc5ff91</t>
-  </si>
-  <si>
-    <t>d456a5fe-9b10-4652-b169-5f0feacfef43</t>
-  </si>
-  <si>
-    <t>c12a0fb5-56f6-4bfb-8988-c40c2b976b47</t>
-  </si>
-  <si>
-    <t>2d3bf0d1-5f03-4b83-92ec-d8f13d74ff78</t>
+    <t>73034125-5056-4e70-964b-693962875c1d</t>
+  </si>
+  <si>
+    <t>52644959-5383-466d-9694-20c3a3156de7</t>
+  </si>
+  <si>
+    <t>0ada3647-1ff3-4aab-a783-9e5c19be20eb</t>
+  </si>
+  <si>
+    <t>a1492ef7-b2bf-4d10-a71f-04217cd95c12</t>
+  </si>
+  <si>
+    <t>eeb35705-edbe-474d-94b1-344809808c6c</t>
+  </si>
+  <si>
+    <t>53bf2850-4371-4999-8cd1-0a8a18248f65</t>
+  </si>
+  <si>
+    <t>6f4d082c-f89a-43e7-914c-165ce6a81828</t>
+  </si>
+  <si>
+    <t>1842614e-2880-4dad-8a20-6dc676159e7b</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -816,7 +816,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>99d7158e-91a4-4ed8-825e-4a351a2d7fa9</t>
+    <t>397cde6b-a7f0-4a29-9ab7-4519f9c41b80</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
fix: fix the generated FHIR json structure for encounter and gender #82
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>7d3130df-50b7-429c-8354-be2781c2e78b</t>
+    <t>09b7334a-1514-4de2-b36e-671858821b4f</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>970f3a23-308f-4875-aeed-a9c8010732b4</t>
+    <t>257bc1e3-35ac-4815-89e5-95244e2d51d6</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>2aa428f9-e8ca-4525-872f-bd6224121a31</t>
+    <t>2310954b-7aa5-44c1-9b20-e3a776857717</t>
   </si>
   <si>
     <t>Invalid Answer Code</t>
@@ -159,7 +159,7 @@
     <t>WARNING</t>
   </si>
   <si>
-    <t>5f7614c3-9e73-47e7-9bc9-99999364ae19</t>
+    <t>91b6a378-6b37-4b75-ae5a-b196a7fd6799</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -186,7 +186,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>5f5046ce-d6bf-40f4-a113-90c87683310e</t>
+    <t>d93cfdb2-6a85-44c9-bc64-02468b7f1b1f</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -204,7 +204,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>0090848b-3389-4f3d-8899-9174dae0c622</t>
+    <t>8a286c61-e57a-4c2e-90bf-34b068be4bb6</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -222,13 +222,13 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>63c20d3e-5a88-4cd1-a6ba-491850a65151</t>
-  </si>
-  <si>
-    <t>5c2f7272-f544-486c-8487-46b3ee126efc</t>
-  </si>
-  <si>
-    <t>6516c754-1959-41ad-80c2-689a5a13341f</t>
+    <t>92d6c614-7196-4c63-80f3-137ae4f34c30</t>
+  </si>
+  <si>
+    <t>03b6641e-17ae-428e-a19b-ed9fa33300a0</t>
+  </si>
+  <si>
+    <t>ffe9c8e8-8b86-4473-b860-922d2361d16d</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "96842-0" and Answer Code "LA18891-4" are not matching with the reference data found in ANSWER_CODE</t>
@@ -237,10 +237,10 @@
     <t>LA18891-4</t>
   </si>
   <si>
-    <t>f7bbe4fd-9832-4732-9014-dab8cc90433c</t>
-  </si>
-  <si>
-    <t>79b706fc-a190-48de-a5be-38b9499c5ff4</t>
+    <t>8ba636fc-b681-4c2a-80d6-dd0219d2cd7e</t>
+  </si>
+  <si>
+    <t>4356e83f-d708-496a-8c6b-ffe83779f9b6</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -249,13 +249,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>1bc36a0b-6bec-4d03-91b1-a77580353f2c</t>
-  </si>
-  <si>
-    <t>73ee848c-b9fc-4ee4-af18-a6a5140092c9</t>
-  </si>
-  <si>
-    <t>6d1a4149-7db8-479f-9b12-6a0a1ea06fa4</t>
+    <t>ffa827d9-5f1e-4b91-a168-aeb0b13bb274</t>
+  </si>
+  <si>
+    <t>c7999171-b179-445d-bc46-bd194d8907e9</t>
+  </si>
+  <si>
+    <t>11820fe1-94ee-4b33-b0d3-c52c662cf48f</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "44255-8" and Answer Code "LA6569-3" are not matching with the reference data found in ANSWER_CODE</t>
@@ -264,7 +264,7 @@
     <t>LA6569-3</t>
   </si>
   <si>
-    <t>8b14cf18-2ccd-4c7f-9146-d78f4d978131</t>
+    <t>6a22bbc2-3923-46e8-a348-18c416fc2ff6</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -276,13 +276,13 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>5485f038-d864-4f35-9576-c3fc3f94cc1c</t>
-  </si>
-  <si>
-    <t>edcc23eb-1679-48d7-ab2f-32ddbf286025</t>
-  </si>
-  <si>
-    <t>35cbf2f9-fb17-4ddc-881b-f249aad5c85a</t>
+    <t>80fac7d0-28db-4e02-9589-0fa17257fb7c</t>
+  </si>
+  <si>
+    <t>678fa32b-9d2e-4ef6-84cd-7ce6d01e867f</t>
+  </si>
+  <si>
+    <t>2a1c34ff-dd37-4ee8-b07e-a22b2cdd7346</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "96781-0" and Answer Code "LA31979-0" are not matching with the reference data found in ANSWER_CODE</t>
@@ -291,16 +291,16 @@
     <t>LA31979-0</t>
   </si>
   <si>
-    <t>c03ca390-ee24-4c08-b0f2-8084f2ea28bb</t>
-  </si>
-  <si>
-    <t>1524a424-a9a9-4dfa-89b1-00e74e3dc9d9</t>
-  </si>
-  <si>
-    <t>e0f7d99a-d838-4aad-8f55-ca83037ca84d</t>
-  </si>
-  <si>
-    <t>e3a8a36e-324a-4a21-8b3b-6b9e99e9bf47</t>
+    <t>4662a0a0-31ee-4be0-8ce3-9b38a410f956</t>
+  </si>
+  <si>
+    <t>f15353f2-2ee8-41a8-b605-4e8c883cc35e</t>
+  </si>
+  <si>
+    <t>bea12b49-8b58-48da-ae40-14950f146a97</t>
+  </si>
+  <si>
+    <t>4570ef72-4d1d-4bbb-ac2a-1a5b8b0bcf43</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68524-8" and Answer Code "LA6270-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -309,31 +309,31 @@
     <t>LA6270-8</t>
   </si>
   <si>
-    <t>db33908d-84ab-48a0-8de9-a7344e2fdebc</t>
-  </si>
-  <si>
-    <t>7f2bd43e-efad-4166-a197-caca396c7645</t>
-  </si>
-  <si>
-    <t>edfad29c-cae4-45dc-a477-eb6d0b10520f</t>
-  </si>
-  <si>
-    <t>52a046f3-f40d-4bed-a3c2-9d46ed164066</t>
+    <t>564795d4-2594-420b-9026-40c350dc8407</t>
+  </si>
+  <si>
+    <t>8bb86bb1-8d72-44d6-a560-25141a883036</t>
+  </si>
+  <si>
+    <t>99b95f78-9ad8-42a9-ad5a-44484fb0182a</t>
+  </si>
+  <si>
+    <t>5778974f-36ac-4681-b599-a4385343977a</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68517-2" and Answer Code "LA6270-8" are not matching with the reference data found in ANSWER_CODE</t>
   </si>
   <si>
-    <t>1315191e-507c-4860-b5a8-49a930143651</t>
-  </si>
-  <si>
-    <t>fd8de152-86a8-4f5a-91fc-0e8ad6c03a7e</t>
-  </si>
-  <si>
-    <t>5a4e2085-7cdd-4aa2-8dc6-974c00ceb666</t>
-  </si>
-  <si>
-    <t>6c00a0c2-4871-457a-a490-46698eea8d18</t>
+    <t>c0c70243-00b8-4411-8d91-8d9f38f93bed</t>
+  </si>
+  <si>
+    <t>1db43e86-ff82-4edc-86fd-bb4ec30ca66e</t>
+  </si>
+  <si>
+    <t>a1e856ec-ccd9-4831-9ff0-f07042ed67fa</t>
+  </si>
+  <si>
+    <t>8cdb8af7-12e0-40a7-92f4-d198df058427</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "69858-9" and Answer Code "LA33-6" are not matching with the reference data found in ANSWER_CODE</t>
@@ -342,16 +342,16 @@
     <t>LA33-6</t>
   </si>
   <si>
-    <t>408752d3-5563-40ee-a9d6-68f731bf48f9</t>
-  </si>
-  <si>
-    <t>7b0932d3-3fcc-434f-a3a2-ecd786fa5d13</t>
-  </si>
-  <si>
-    <t>b4a582bd-55b2-4988-b48a-c62c4b70a3d6</t>
-  </si>
-  <si>
-    <t>155f15b6-89ba-41b1-bf39-b3e0cc337de7</t>
+    <t>9c2eb6c8-384b-432d-a6ef-d8403771d2a2</t>
+  </si>
+  <si>
+    <t>8b03b509-7093-40bc-8434-a8bb0e863b8b</t>
+  </si>
+  <si>
+    <t>87692c93-012d-46df-9a34-c00c584ff1aa</t>
+  </si>
+  <si>
+    <t>9c58e938-6860-48d2-811b-7a808fab0100</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in ANSWER_CODE</t>
@@ -360,16 +360,16 @@
     <t>LA28853-2</t>
   </si>
   <si>
-    <t>5e900cf0-fcd1-438e-8bcd-23dce6a0d248</t>
-  </si>
-  <si>
-    <t>ef9164f5-5f5f-4a8c-a7cd-4ff1509a996b</t>
-  </si>
-  <si>
-    <t>e93f8c06-7e5e-49b0-9e12-5c52fe1ebb85</t>
-  </si>
-  <si>
-    <t>5bcdbb96-e63a-4f77-9bdf-767492bcfd44</t>
+    <t>35a25288-788d-4a44-8795-b32fe3cfa30e</t>
+  </si>
+  <si>
+    <t>ca2d65c6-d4c3-4ce0-8feb-b509e67aab4a</t>
+  </si>
+  <si>
+    <t>d52b5367-a67f-4c40-b3d2-3103b549415f</t>
+  </si>
+  <si>
+    <t>c9806066-7233-45af-92e5-908edd1beacd</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in ANSWER_CODE</t>
@@ -378,7 +378,7 @@
     <t>LA6571-9</t>
   </si>
   <si>
-    <t>8bf8e88d-5c62-4921-a651-84a690d607f0</t>
+    <t>98161028-ac3b-43f4-8786-5ca2aec3476f</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -393,13 +393,13 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>025b8512-4c75-4d04-88d2-8f926b3ad26a</t>
-  </si>
-  <si>
-    <t>76110869-eec6-43cc-a8a0-b8753a77d45c</t>
-  </si>
-  <si>
-    <t>5b41f561-a1e0-4f99-8da6-80bbf546da39</t>
+    <t>b3fc2e79-a20d-49a9-b5f7-65559ab2c2f1</t>
+  </si>
+  <si>
+    <t>10917618-5003-4daa-a7fc-a28d72a7d49c</t>
+  </si>
+  <si>
+    <t>888edf57-93cd-4561-b79e-66e20d7dabe0</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "93038-8" and Answer Code "LA13902-4" are not matching with the reference data found in ANSWER_CODE</t>
@@ -408,7 +408,7 @@
     <t>LA13902-4</t>
   </si>
   <si>
-    <t>a1e06888-6e29-4858-b05c-64b3bfb14bbc</t>
+    <t>d1868a5a-c510-457b-b519-74860bf9847a</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44255-8" and Answer Code "LA6569-3" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
@@ -417,13 +417,13 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>d5d43fec-49d9-45de-b5a6-0d313887c5e5</t>
-  </si>
-  <si>
-    <t>d91c129e-dc2c-45c6-812d-7919a5f38b7a</t>
-  </si>
-  <si>
-    <t>067d8643-0b0f-4017-b27e-9b9223780315</t>
+    <t>bae8f082-014e-4ba1-aa1b-d487e83421a1</t>
+  </si>
+  <si>
+    <t>18b3fc93-59e5-435e-b3c0-d42c7120c6bb</t>
+  </si>
+  <si>
+    <t>d394acae-f653-4e2b-b653-5bc4df0dbc57</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "97027-7" and Answer Code "LA32-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -432,7 +432,7 @@
     <t>LA32-8</t>
   </si>
   <si>
-    <t>3f43598a-3824-42ec-ade3-f449cd4812a4</t>
+    <t>c0e9df00-c3f3-49f3-be9e-108ad0df3235</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "69858-9" and Answer Code "LA33-6" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
@@ -441,10 +441,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>e879406b-aa02-4284-ba23-b83f61df3720</t>
-  </si>
-  <si>
-    <t>b9278cc8-f222-4f39-9200-65c99c03bd2d</t>
+    <t>80de24d2-5d78-4adf-ad6b-298bac6c0b48</t>
+  </si>
+  <si>
+    <t>0c6099a0-da26-4dd9-bb49-263672f992f5</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -453,25 +453,25 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>5c853da9-aba7-4495-9948-3f062fa3fac8</t>
+    <t>bb0d442b-2a9b-428f-a685-1fe48460f1a3</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "69861-3" and Answer Code "LA32-8" are not matching with the reference data found in ANSWER_CODE</t>
   </si>
   <si>
-    <t>2a90d219-3dcf-40cf-b85a-03ec2e035e32</t>
+    <t>fca78ffc-18eb-4374-a346-39061a1e26e2</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>d52121f1-231f-4329-beab-1ca316bdcd13</t>
-  </si>
-  <si>
-    <t>2b93b9ee-dd8e-475d-9183-03628907443b</t>
-  </si>
-  <si>
-    <t>fcccaf8f-55bb-4430-b8bc-39e41c55ac01</t>
+    <t>2217ed02-aee9-4123-bf65-54e608e2aaba</t>
+  </si>
+  <si>
+    <t>9d1367c5-58df-40c8-8905-87f663ec6241</t>
+  </si>
+  <si>
+    <t>eeacd526-85bd-4cdb-aa5d-a0142b9e7f49</t>
   </si>
   <si>
     <t>Provided Screening Code "97023-6", Question Code "93159-2" and Answer Code "LA10044-8" are not matching with the reference data found in ANSWER_CODE</t>
@@ -480,190 +480,190 @@
     <t>LA10044-8</t>
   </si>
   <si>
-    <t>1eb8cd50-8dab-4b93-b30a-9c05a5b24696</t>
+    <t>711f21eb-972b-43de-9f17-cb1358a6fe44</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "68524-8" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>362a9ba3-b775-4b2c-a44b-ee0e0701fdb8</t>
-  </si>
-  <si>
-    <t>e921b823-ce17-45d4-b389-1f7ea878370e</t>
-  </si>
-  <si>
-    <t>500f86a2-08c5-42eb-9583-0d5812b7281f</t>
+    <t>037a23ed-b1be-43d8-b546-8cc483b876b5</t>
+  </si>
+  <si>
+    <t>c23e2284-347a-45a6-bcc0-0a92c9c8a88c</t>
+  </si>
+  <si>
+    <t>843d6518-76e5-40b8-a7b3-75ae9d5910c3</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>7103df56-e279-4012-a281-0e2114f9fa6f</t>
-  </si>
-  <si>
-    <t>87be461b-dd68-499f-b9d5-adebef433033</t>
-  </si>
-  <si>
-    <t>dd4081dd-3c95-4bb0-83bc-74afc385b6b2</t>
+    <t>89cf9c31-4a08-41ba-a938-a058de10fa9a</t>
+  </si>
+  <si>
+    <t>85eb3468-c095-4f7d-bd07-b8effc1ce3f3</t>
+  </si>
+  <si>
+    <t>ae44a254-c516-4736-b38b-49bf97a8de17</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "76513-1" and Answer Code "LA15832-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>6a00c6da-9a2a-4aad-997f-f45be9997179</t>
-  </si>
-  <si>
-    <t>4f142396-71c2-4a8d-ac64-3e0fc5043a09</t>
-  </si>
-  <si>
-    <t>fdcba316-55b2-4385-9358-717507921100</t>
+    <t>d0d119bb-d7ad-47c2-9d75-5c4939270e5d</t>
+  </si>
+  <si>
+    <t>fb4b8e18-fe4d-43c4-99cb-71c8df90c721</t>
+  </si>
+  <si>
+    <t>7fc615f1-df1e-41a4-9605-b1d8f2887e9d</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>c6c7efbf-93c5-43f9-a778-b0de7a6a4d89</t>
-  </si>
-  <si>
-    <t>3c3bea8b-a30e-411b-b2f6-84f738ba8a7a</t>
-  </si>
-  <si>
-    <t>97bb2498-4268-4777-a8bc-10cc4974de88</t>
+    <t>71545c6e-cdd3-4d87-851b-5f7c473a52eb</t>
+  </si>
+  <si>
+    <t>348cc385-9a23-41ff-9ef2-b37e2deaf323</t>
+  </si>
+  <si>
+    <t>eb997444-68b6-469a-b2c5-1a52a78981b6</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "97027-7" and Answer Code "LA32-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>ad494fe4-0a9d-44bd-8813-524062768d08</t>
-  </si>
-  <si>
-    <t>9fe506d8-6e9b-4ab6-9db6-449c814d229d</t>
-  </si>
-  <si>
-    <t>b71c98ad-bc7c-49d5-87f7-4c3b6ccbb89c</t>
+    <t>06f7ad6a-821b-47b5-a4fa-511feb95c069</t>
+  </si>
+  <si>
+    <t>5e560bff-b904-4d3c-966c-4fc5e73ac6f7</t>
+  </si>
+  <si>
+    <t>c7a83500-2b26-41f8-a474-bed1a2563bab</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>cf82cd2d-7973-4c20-ae2f-ae2655dbbc9a</t>
-  </si>
-  <si>
-    <t>0fede892-aced-4d19-a33d-4ab95b3dc2aa</t>
-  </si>
-  <si>
-    <t>0b328383-e38d-4efa-bfca-628edb277619</t>
+    <t>e6c3af4d-6e42-4647-b232-2866c22e60cb</t>
+  </si>
+  <si>
+    <t>aa4b48d5-fd5b-4807-930d-e40e35a86364</t>
+  </si>
+  <si>
+    <t>3c91856b-c6fc-4359-ae44-6a5b51866f5c</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>b5298a09-0a07-411e-8ce8-2d94a760354d</t>
-  </si>
-  <si>
-    <t>5ae8ea3d-e4dd-4d15-ad93-287aae58fe55</t>
-  </si>
-  <si>
-    <t>a590e431-cb49-420c-bbf0-54269408bdff</t>
+    <t>4d6b304e-a1ce-417a-8488-3e0e6b1ce102</t>
+  </si>
+  <si>
+    <t>df247289-e4be-44fe-b6fc-4407b1bf2e99</t>
+  </si>
+  <si>
+    <t>ab699f75-21cb-4f69-8892-49127010a39d</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "96781-0" and Answer Code "LA31979-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>6e4de5b2-20e6-4a63-af23-c956d30a0db6</t>
-  </si>
-  <si>
-    <t>b02edc1b-e15e-4b9e-b0b7-77f9ce798d64</t>
-  </si>
-  <si>
-    <t>57c1bb4c-92fb-45fd-87e3-3d524dfd9ab0</t>
+    <t>74c97b9c-79ba-4f4f-b66e-537ec3ad2346</t>
+  </si>
+  <si>
+    <t>d81b5b77-5af0-4654-9705-74ee24a46fd4</t>
+  </si>
+  <si>
+    <t>cef5bd3b-fb7e-4851-bf39-c3027d536e66</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>b78f0c90-163b-4ce2-95a6-f2e9d81ab56e</t>
-  </si>
-  <si>
-    <t>dd5294bc-9ea8-4a84-95a2-ad95b403b325</t>
-  </si>
-  <si>
-    <t>314f5962-e44d-4653-8973-6cdb4c1999c2</t>
+    <t>a7c9f6ed-a681-4d52-ba32-01e6d018893e</t>
+  </si>
+  <si>
+    <t>12a9a0e2-3daa-45be-81ab-1593dde148ec</t>
+  </si>
+  <si>
+    <t>8779aafa-e18b-4af1-8749-0cdcf83f9358</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "93159-2" and Answer Code "LA10044-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>1f8ee814-7404-4c62-b13d-b8d3c95bcceb</t>
-  </si>
-  <si>
-    <t>5ca7f71c-47bd-414a-89bc-3328bee4b4f2</t>
-  </si>
-  <si>
-    <t>8a01c7c5-0485-4e55-bb58-91396edbf552</t>
+    <t>dc71351b-6d8d-4031-862c-34249f686a83</t>
+  </si>
+  <si>
+    <t>6438da93-f364-4881-8f60-2e0b5eefd5c8</t>
+  </si>
+  <si>
+    <t>4e9d069e-f036-499f-9c53-e2eb1624a31a</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>bd608a13-dc4e-44da-9deb-417739471840</t>
-  </si>
-  <si>
-    <t>af37d7a2-20fd-458e-b4c4-8d1cbbb5efb3</t>
-  </si>
-  <si>
-    <t>73b970dc-d0f2-4d06-8d7e-1c54f6c9a4f6</t>
+    <t>a5a50acd-c8bb-4384-9817-870013dbbc46</t>
+  </si>
+  <si>
+    <t>483d5484-1f8e-4a1c-984f-63b809a9588d</t>
+  </si>
+  <si>
+    <t>216bb252-4d64-41d9-b191-80d6e5334a4c</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "93038-8" and Answer Code "LA13902-4" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>cc5e3cbf-6172-4906-8b0b-3707b3b1f83d</t>
-  </si>
-  <si>
-    <t>e2e3e84e-3239-4864-ac88-ac74797ed78a</t>
-  </si>
-  <si>
-    <t>3863779d-d94e-4751-8149-4fc135bbdb5e</t>
+    <t>4edc032c-f374-4b49-be12-4ab481923798</t>
+  </si>
+  <si>
+    <t>f108702e-b61d-4d35-bc47-68d78ff93bfd</t>
+  </si>
+  <si>
+    <t>4fdff024-7e14-48b0-9254-e2b04893aad0</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "No", Screening Code "97023-6", Question Code "69861-3" and Answer Code "LA32-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>aa47fcde-2351-4337-98b3-62c425a72a75</t>
-  </si>
-  <si>
-    <t>9544db2e-42bc-4be7-a77e-03391b7aa215</t>
-  </si>
-  <si>
-    <t>4a2eb67a-88fa-438f-8085-292f5c25efc7</t>
+    <t>cbafd002-fe39-4a69-8094-ca8a4ef111b5</t>
+  </si>
+  <si>
+    <t>0cb25ecf-3771-4f9c-98a8-5234b577dad4</t>
+  </si>
+  <si>
+    <t>f243d14f-def2-4469-b206-3e461d75dded</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "Yes", Screening Code "97023-6", Question Code "96842-0" and Answer Code "LA18891-4" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>73034125-5056-4e70-964b-693962875c1d</t>
-  </si>
-  <si>
-    <t>52644959-5383-466d-9694-20c3a3156de7</t>
-  </si>
-  <si>
-    <t>0ada3647-1ff3-4aab-a783-9e5c19be20eb</t>
-  </si>
-  <si>
-    <t>a1492ef7-b2bf-4d10-a71f-04217cd95c12</t>
-  </si>
-  <si>
-    <t>eeb35705-edbe-474d-94b1-344809808c6c</t>
-  </si>
-  <si>
-    <t>53bf2850-4371-4999-8cd1-0a8a18248f65</t>
-  </si>
-  <si>
-    <t>6f4d082c-f89a-43e7-914c-165ce6a81828</t>
-  </si>
-  <si>
-    <t>1842614e-2880-4dad-8a20-6dc676159e7b</t>
+    <t>a43f158f-7a3e-4801-8852-e1e2505035ca</t>
+  </si>
+  <si>
+    <t>9d9ecca1-7776-4a00-99ce-ba50d95dfab2</t>
+  </si>
+  <si>
+    <t>2c7a77bb-3c13-42f3-b8f4-7c85401235b5</t>
+  </si>
+  <si>
+    <t>c4fa7a04-0f4e-45e9-acc1-4bf7b60322fb</t>
+  </si>
+  <si>
+    <t>d86f090b-e141-4840-83ab-bb706a7b29f6</t>
+  </si>
+  <si>
+    <t>648d0c48-32ce-41f8-81ee-8b1e1e2f1252</t>
+  </si>
+  <si>
+    <t>bd65676e-654c-406c-b241-49b0c50e4441</t>
+  </si>
+  <si>
+    <t>da1c08b4-5f36-4bcb-9c0f-1daf577732bb</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -816,7 +816,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>397cde6b-a7f0-4a29-9ab7-4519f9c41b80</t>
+    <t>b506f62c-2f97-4388-945d-6fe4bf4f8875</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
feat: update ahc-crosswalk csv file
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>4398cddc-d02e-45ea-bc5d-a791d0cc2adc</t>
+    <t>ea4b34aa-1a69-4e1e-bf29-6f3b529abe00</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>9f596510-c94b-4924-9d6a-0c55445d18b0</t>
+    <t>c951ee4c-8bd5-4d63-8349-76bd4baac952</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>44bfefd2-a8e2-4619-8ac2-73a8ff307fef</t>
+    <t>71a63c7c-0c0f-46be-87b9-926d0d008783</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -165,7 +165,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>8c59c0e3-d2b5-48a7-9ace-77c5f6fd543c</t>
+    <t>d8be4f17-a53c-4ca2-a597-14ab2abd93da</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -183,7 +183,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>22c619a0-63f3-4d09-a6d1-27e5b10edfe5</t>
+    <t>af9ac8bf-8c6e-4d63-b844-98b3047e6671</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -201,16 +201,16 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>a56db7dc-3b2e-466e-b7ac-f4f70e7c4628</t>
-  </si>
-  <si>
-    <t>1c3bb765-aa45-4960-baa0-b3a26da1aa47</t>
-  </si>
-  <si>
-    <t>a59a58cd-e377-414d-85f5-f492c2a506a2</t>
-  </si>
-  <si>
-    <t>4509e571-a68c-4256-b54e-a8dc9e068f7b</t>
+    <t>45d47ab9-4026-4e9f-ba3a-4a45e1a6d1bd</t>
+  </si>
+  <si>
+    <t>eeefb1f7-f9ee-41a3-8bb7-fddc7a101506</t>
+  </si>
+  <si>
+    <t>4aaaae80-62ed-48e4-be19-b5d0cf220c83</t>
+  </si>
+  <si>
+    <t>2d894ce0-a1f1-44e5-b711-43dc176b6d6c</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -219,13 +219,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>c5b0ab4d-3874-4ffa-b21e-63996884b54c</t>
-  </si>
-  <si>
-    <t>27d3c2f6-34ef-45bf-b2b7-74b7c7e9bb7d</t>
-  </si>
-  <si>
-    <t>c165dc6a-168a-4f05-98bb-9e7f094c4e16</t>
+    <t>862a6e77-1083-4f88-904f-f4251fe37fb3</t>
+  </si>
+  <si>
+    <t>4f9427dc-a8dc-46b4-86f6-27389849dd3a</t>
+  </si>
+  <si>
+    <t>b452e9f0-d693-4434-922f-07610b0d7343</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -237,58 +237,58 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>62234f03-b1d7-420f-a772-cbd8fb474445</t>
-  </si>
-  <si>
-    <t>d130e8e6-b121-4827-826c-11bba20a6739</t>
-  </si>
-  <si>
-    <t>74ed63e6-576f-4cdb-96ed-04d27da86214</t>
-  </si>
-  <si>
-    <t>7175152d-b2a4-4ede-986e-3ed77c5b73fc</t>
-  </si>
-  <si>
-    <t>a2ac4a39-a7b8-4923-9a2f-190c61cd2bef</t>
-  </si>
-  <si>
-    <t>f832a674-3866-4a8c-896b-924c2f88f2e0</t>
-  </si>
-  <si>
-    <t>a8b88cce-6ada-471c-82ba-c68fed5ded9d</t>
-  </si>
-  <si>
-    <t>077afc78-dad8-4732-b7c1-f27aee379134</t>
-  </si>
-  <si>
-    <t>b2574f5e-5b2d-4ee3-9ef2-2f7c9b5a0ed1</t>
-  </si>
-  <si>
-    <t>71ae0951-923f-47d3-bc48-0c3065895d39</t>
-  </si>
-  <si>
-    <t>1c824b0f-06ab-4ca3-8dc4-d8f1228a7534</t>
-  </si>
-  <si>
-    <t>8ec86cc4-3a5a-4e59-8499-7ed2ea02969f</t>
-  </si>
-  <si>
-    <t>c4c9c40a-ccde-4897-be82-3859a5e17c46</t>
-  </si>
-  <si>
-    <t>17dac939-1760-49c7-a108-49bbeac853a4</t>
-  </si>
-  <si>
-    <t>d55555e2-65c7-4de6-bbc0-1009e28daedb</t>
-  </si>
-  <si>
-    <t>69e2e2fc-fa4e-42bf-b315-8c31eaa8e1de</t>
-  </si>
-  <si>
-    <t>8847e610-0ae7-4e2e-a5cb-f42671352414</t>
-  </si>
-  <si>
-    <t>8551dfe0-b0a6-469b-8d94-4333d943b344</t>
+    <t>60aba70d-c7fa-4bc0-8081-cfa13de10583</t>
+  </si>
+  <si>
+    <t>772a619c-651f-463f-ba88-532452138666</t>
+  </si>
+  <si>
+    <t>cbe85f61-a7c2-443f-ae3d-51f2acccdc12</t>
+  </si>
+  <si>
+    <t>ab6c61b8-2a1d-4d14-bab7-75ecac746799</t>
+  </si>
+  <si>
+    <t>410c3569-86a9-4bbc-927b-5bf07a20df1b</t>
+  </si>
+  <si>
+    <t>c4799473-e0c4-4ad3-8d88-b57d53d1e2ca</t>
+  </si>
+  <si>
+    <t>30a8e7e9-60ee-4d32-970f-a4adb4cabb33</t>
+  </si>
+  <si>
+    <t>c005d20d-ef9b-4c75-a84e-e5e7228989c7</t>
+  </si>
+  <si>
+    <t>bff980f0-a6d5-40c1-af1c-80e97b3fd67b</t>
+  </si>
+  <si>
+    <t>9046b07a-1ab0-43e2-9eb2-9492c9591b24</t>
+  </si>
+  <si>
+    <t>05e6cf6e-dd16-4153-9e2e-8bdbc4d5e466</t>
+  </si>
+  <si>
+    <t>7eb80837-871f-43a1-aa5f-24da2735040c</t>
+  </si>
+  <si>
+    <t>df824644-b31c-448b-b3fa-9ce906f90aa6</t>
+  </si>
+  <si>
+    <t>7160b157-5599-4007-908c-1ac3066a452f</t>
+  </si>
+  <si>
+    <t>45e479a7-0809-4d88-a279-31cba9128289</t>
+  </si>
+  <si>
+    <t>daf9fc0f-c97e-4b23-9941-294d4931933c</t>
+  </si>
+  <si>
+    <t>56d78d61-99c6-4627-b03c-cf070b31dbfd</t>
+  </si>
+  <si>
+    <t>214f5c1d-90d5-43cf-b48e-92694262fd89</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -303,34 +303,34 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>4e9213ed-c72d-4f2b-b9ba-e351bf0a072c</t>
-  </si>
-  <si>
-    <t>1671f85a-1e6f-4e52-8caa-c9922156a498</t>
-  </si>
-  <si>
-    <t>308e5769-35f0-4575-a2ab-ec0b8a592ecc</t>
+    <t>4f4fb0ec-d17c-4756-8889-f2a27eae3a28</t>
+  </si>
+  <si>
+    <t>f2e98b1a-97e7-4a56-bdbb-cf024bac813f</t>
+  </si>
+  <si>
+    <t>f573016b-c933-4694-a254-fdd975460a59</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>3f64946d-ae0f-48a5-8b55-f7dab431d07b</t>
-  </si>
-  <si>
-    <t>0b0d4d04-fa9d-4d34-b4e5-0d38708ca284</t>
-  </si>
-  <si>
-    <t>f0d3290f-0695-4513-a865-33a2f77f76ab</t>
+    <t>1fa35da9-c562-4418-ab5c-9675bcb0c169</t>
+  </si>
+  <si>
+    <t>5b4721d1-5ebe-4dcc-a4e4-11f569607679</t>
+  </si>
+  <si>
+    <t>2bab4fd3-893a-4cae-a47a-03a5f52e81e3</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>b49c56e1-72d3-4f70-93c7-f8a5c8cad1d6</t>
-  </si>
-  <si>
-    <t>beb273c9-5ff8-457f-a2fa-baafab45baee</t>
+    <t>7e10905c-a5f2-4d8d-816c-46939bc7f288</t>
+  </si>
+  <si>
+    <t>1875bacf-0fea-4743-b355-20f897c62328</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -339,142 +339,142 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>222de68f-8ec9-4e6e-8f3d-0700e9ccbceb</t>
+    <t>398367a3-8e6f-4db1-8e4a-a27685203c79</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>847f6344-7deb-48b5-88d8-6b1de02a1608</t>
-  </si>
-  <si>
-    <t>482f2bdd-c08e-44ab-a867-ca9e7e860537</t>
-  </si>
-  <si>
-    <t>0a3186ed-b115-4886-b65d-8a0517884b0b</t>
+    <t>1c99b50d-3a59-4ab6-b58e-ad21188c3835</t>
+  </si>
+  <si>
+    <t>fe351f07-0fa9-43ce-94d0-2f69ef6a9209</t>
+  </si>
+  <si>
+    <t>c53bfa9f-b87c-4a90-a7e4-dfcab376428e</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>8279f5e9-9c8a-479e-a85e-0404ffb06d4b</t>
-  </si>
-  <si>
-    <t>b383ea60-3a65-4c75-b8ed-b5b02047e620</t>
-  </si>
-  <si>
-    <t>a97348c4-466c-4498-a1a4-87c4cbb42e7e</t>
+    <t>61cf0f84-634e-46f2-917c-cf99150fe9ab</t>
+  </si>
+  <si>
+    <t>47667083-d500-42f8-95e1-f7b14686b5b6</t>
+  </si>
+  <si>
+    <t>eb795860-b156-42f0-84eb-e4ec4e606efb</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>6711df7c-8bd6-41ad-be98-e2a27d3aa421</t>
-  </si>
-  <si>
-    <t>3b6b1d80-3eda-42cb-b6ee-4d87a5303996</t>
-  </si>
-  <si>
-    <t>3e5c3b0a-69ab-4c42-a938-636ccebedb7d</t>
+    <t>3210278e-c460-4bbc-bbcb-6a1b74a37b74</t>
+  </si>
+  <si>
+    <t>0f64d539-1d71-4ae6-a730-f08cc7349eef</t>
+  </si>
+  <si>
+    <t>dbac4637-04f7-4f73-967b-8e3aa0a55718</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>8e1802a8-90bb-4a9d-925b-7dcf7d8d4a71</t>
-  </si>
-  <si>
-    <t>7cc9dd65-ad06-4d4b-8cbb-ba1c04dfc91b</t>
-  </si>
-  <si>
-    <t>f2bb8026-9c74-43a3-a323-91c7f0d4f099</t>
+    <t>cd9cf62e-67d5-4245-81c4-0080f07e39eb</t>
+  </si>
+  <si>
+    <t>1c8fdd4f-a1f7-4a19-a824-ba621a45b257</t>
+  </si>
+  <si>
+    <t>51caecb9-122d-4ba1-902d-e9e047caa0f7</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>c9fd3a21-f648-4109-88d7-97b56edca893</t>
-  </si>
-  <si>
-    <t>9de47d7c-dcb2-46a8-a2c5-9b7c07807ee7</t>
-  </si>
-  <si>
-    <t>c0c4e945-bd39-4fb8-8288-c16591375aa6</t>
-  </si>
-  <si>
-    <t>b2ccf00c-77d2-4010-b59e-fe0e1d76fbc1</t>
-  </si>
-  <si>
-    <t>c7b44f8b-a9d9-4113-97f9-dfeaf7f4a318</t>
-  </si>
-  <si>
-    <t>68e20638-a529-4f46-b344-1d065e23bd10</t>
-  </si>
-  <si>
-    <t>7bf82214-d4b6-4dd2-9ea4-0dbd0614dc9c</t>
-  </si>
-  <si>
-    <t>8cd3b2c2-a172-4f3d-aba3-61383723aa2a</t>
-  </si>
-  <si>
-    <t>602beacc-1472-4202-9001-443624a8ab8d</t>
-  </si>
-  <si>
-    <t>cbe99ea0-5591-4dd1-8e28-159e372f9dac</t>
-  </si>
-  <si>
-    <t>5c85a3a0-4aed-4085-bf35-0d9e1538855d</t>
-  </si>
-  <si>
-    <t>e808c90a-eb42-4b29-87cd-515b77875b1e</t>
-  </si>
-  <si>
-    <t>899b55e2-ea80-41c3-a77e-b60fe4e33b9c</t>
-  </si>
-  <si>
-    <t>59328b74-efcf-4fc0-a2ca-07bb043359dd</t>
-  </si>
-  <si>
-    <t>612d719d-c234-4b95-836f-3805954bf287</t>
-  </si>
-  <si>
-    <t>bbd49771-4892-4552-a63a-0ee77dc658a7</t>
-  </si>
-  <si>
-    <t>6d8130e8-a251-49f7-b694-52ee5028ed8c</t>
-  </si>
-  <si>
-    <t>89e2add6-5e9e-4970-be06-2385e251829c</t>
-  </si>
-  <si>
-    <t>77b620a3-fe87-4595-be36-2c77b2beb12c</t>
-  </si>
-  <si>
-    <t>63647512-08e4-44ea-b30f-26c5f80eb757</t>
-  </si>
-  <si>
-    <t>eeedb57d-081d-4417-a510-900d4e3990c4</t>
-  </si>
-  <si>
-    <t>9c25280e-f3f9-4810-8da4-cf118a8dada0</t>
-  </si>
-  <si>
-    <t>04acd182-ba3a-436a-85e1-a99ad18c8e3b</t>
-  </si>
-  <si>
-    <t>ef28ae1f-fd92-4f13-8d26-ccccea44c408</t>
-  </si>
-  <si>
-    <t>5c8583b0-e1a9-45a7-94a3-954d35c0e558</t>
-  </si>
-  <si>
-    <t>39278902-8f66-433b-91cd-f9e54bddaafc</t>
-  </si>
-  <si>
-    <t>0de87cdf-1cbd-4bb6-8d5a-5a0f7edc0119</t>
-  </si>
-  <si>
-    <t>78e21599-04b1-4cb7-a267-efa8a6cd9f81</t>
+    <t>db8a38ed-cf83-400e-a4a5-192ea849872f</t>
+  </si>
+  <si>
+    <t>b9bee7a3-f016-43ab-9b6b-f35bc552c3c2</t>
+  </si>
+  <si>
+    <t>1f5d6c79-83c9-47ca-bf98-d76b4b6ead4a</t>
+  </si>
+  <si>
+    <t>7eb77061-590d-429c-9b4b-64b55cfe4dd4</t>
+  </si>
+  <si>
+    <t>18c10dd8-fd51-442a-9dbb-39d1c0167fbf</t>
+  </si>
+  <si>
+    <t>186ca05a-075a-4794-add0-3213127a815c</t>
+  </si>
+  <si>
+    <t>1223e4d2-10d1-4dff-b7eb-e3827f0a8f9d</t>
+  </si>
+  <si>
+    <t>fc437c56-50e1-40fa-aa1f-80e79639e079</t>
+  </si>
+  <si>
+    <t>1cd94cbe-b70e-4116-9df1-38fc42f61b0b</t>
+  </si>
+  <si>
+    <t>23d8e166-7251-4f8f-9318-834ae37de8f8</t>
+  </si>
+  <si>
+    <t>a7ca19f9-a69a-49bf-8f59-74ee70c52ee5</t>
+  </si>
+  <si>
+    <t>7e8dab49-1a1e-4129-9a02-a8792e278975</t>
+  </si>
+  <si>
+    <t>a0d0cde7-405d-4fb8-9dc6-cca1c554c20e</t>
+  </si>
+  <si>
+    <t>52a68fd9-0fe1-47d1-865f-7bf9a95adb3f</t>
+  </si>
+  <si>
+    <t>2069624f-6b41-43f1-b4c1-1bac0a8a095d</t>
+  </si>
+  <si>
+    <t>95d07939-143d-4313-bbac-884627573ef7</t>
+  </si>
+  <si>
+    <t>f47f4b43-2b14-4f01-b7a6-8be0fe0a7e3b</t>
+  </si>
+  <si>
+    <t>618e3bf6-8b2c-44b7-bf51-9695ae08356b</t>
+  </si>
+  <si>
+    <t>b7bc73cc-e366-4c33-b070-5ad394bcd805</t>
+  </si>
+  <si>
+    <t>ff083d1b-81e3-4ae4-97b7-1f95df6b650a</t>
+  </si>
+  <si>
+    <t>8b475a72-35ee-4570-b1c1-ca748fdd1ba0</t>
+  </si>
+  <si>
+    <t>dd17a62a-c8dd-4450-840c-c870137c0916</t>
+  </si>
+  <si>
+    <t>51521b14-8912-44e5-acf5-16a9c3e29ecd</t>
+  </si>
+  <si>
+    <t>96615a90-e365-4c1c-ac13-f47a36c7f607</t>
+  </si>
+  <si>
+    <t>2257fd37-edaf-4d07-b823-5a0174f51bd5</t>
+  </si>
+  <si>
+    <t>ad9c42f7-ec3f-4310-8e61-33e5d29716eb</t>
+  </si>
+  <si>
+    <t>0fc17170-2adb-4206-af1c-f8c8f04c81cf</t>
+  </si>
+  <si>
+    <t>a117ea99-445c-4a50-a703-081afc88f923</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -627,7 +627,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>7092cbe5-699f-4f3a-8ba0-deef5ca69c6d</t>
+    <t>402e96de-6b86-4346-a47b-259fb06965bf</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
feat: update ahc-crosswalk csv file #82
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>ea4b34aa-1a69-4e1e-bf29-6f3b529abe00</t>
+    <t>64e3e242-a920-4656-b133-1dcd8fa4fbcd</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>c951ee4c-8bd5-4d63-8349-76bd4baac952</t>
+    <t>88072bed-b6e6-41d0-ac92-40aae0641988</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>71a63c7c-0c0f-46be-87b9-926d0d008783</t>
+    <t>3a7b7ec9-c98d-4e64-9fcb-e9051dae800a</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -165,7 +165,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>d8be4f17-a53c-4ca2-a597-14ab2abd93da</t>
+    <t>2bc148ea-b314-4b5a-b282-01becf0d5723</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -183,7 +183,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>af9ac8bf-8c6e-4d63-b844-98b3047e6671</t>
+    <t>4a0c17b9-a0f8-4152-af17-eeee432b6fbe</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -201,16 +201,16 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>45d47ab9-4026-4e9f-ba3a-4a45e1a6d1bd</t>
-  </si>
-  <si>
-    <t>eeefb1f7-f9ee-41a3-8bb7-fddc7a101506</t>
-  </si>
-  <si>
-    <t>4aaaae80-62ed-48e4-be19-b5d0cf220c83</t>
-  </si>
-  <si>
-    <t>2d894ce0-a1f1-44e5-b711-43dc176b6d6c</t>
+    <t>b117452d-f333-4429-a599-c2f6031e812a</t>
+  </si>
+  <si>
+    <t>ba74db85-7a80-49c2-84bf-a617830b546d</t>
+  </si>
+  <si>
+    <t>80eb1571-3523-4dbd-9f95-beacf9f26400</t>
+  </si>
+  <si>
+    <t>245a6636-d16b-4ab9-9018-b7221db2e9d3</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -219,13 +219,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>862a6e77-1083-4f88-904f-f4251fe37fb3</t>
-  </si>
-  <si>
-    <t>4f9427dc-a8dc-46b4-86f6-27389849dd3a</t>
-  </si>
-  <si>
-    <t>b452e9f0-d693-4434-922f-07610b0d7343</t>
+    <t>eec57008-04bd-4a7d-a478-f59a3f00f1be</t>
+  </si>
+  <si>
+    <t>954587d9-f0f4-4ab7-aa99-9b70559bc7cc</t>
+  </si>
+  <si>
+    <t>aedab293-d339-469f-aea3-06bfe9b1b89e</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -237,58 +237,58 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>60aba70d-c7fa-4bc0-8081-cfa13de10583</t>
-  </si>
-  <si>
-    <t>772a619c-651f-463f-ba88-532452138666</t>
-  </si>
-  <si>
-    <t>cbe85f61-a7c2-443f-ae3d-51f2acccdc12</t>
-  </si>
-  <si>
-    <t>ab6c61b8-2a1d-4d14-bab7-75ecac746799</t>
-  </si>
-  <si>
-    <t>410c3569-86a9-4bbc-927b-5bf07a20df1b</t>
-  </si>
-  <si>
-    <t>c4799473-e0c4-4ad3-8d88-b57d53d1e2ca</t>
-  </si>
-  <si>
-    <t>30a8e7e9-60ee-4d32-970f-a4adb4cabb33</t>
-  </si>
-  <si>
-    <t>c005d20d-ef9b-4c75-a84e-e5e7228989c7</t>
-  </si>
-  <si>
-    <t>bff980f0-a6d5-40c1-af1c-80e97b3fd67b</t>
-  </si>
-  <si>
-    <t>9046b07a-1ab0-43e2-9eb2-9492c9591b24</t>
-  </si>
-  <si>
-    <t>05e6cf6e-dd16-4153-9e2e-8bdbc4d5e466</t>
-  </si>
-  <si>
-    <t>7eb80837-871f-43a1-aa5f-24da2735040c</t>
-  </si>
-  <si>
-    <t>df824644-b31c-448b-b3fa-9ce906f90aa6</t>
-  </si>
-  <si>
-    <t>7160b157-5599-4007-908c-1ac3066a452f</t>
-  </si>
-  <si>
-    <t>45e479a7-0809-4d88-a279-31cba9128289</t>
-  </si>
-  <si>
-    <t>daf9fc0f-c97e-4b23-9941-294d4931933c</t>
-  </si>
-  <si>
-    <t>56d78d61-99c6-4627-b03c-cf070b31dbfd</t>
-  </si>
-  <si>
-    <t>214f5c1d-90d5-43cf-b48e-92694262fd89</t>
+    <t>4f4fbb6d-a00b-42c0-8f1a-d7578dab55e5</t>
+  </si>
+  <si>
+    <t>709e1066-3b5a-4ef4-8ed2-0bde53e2a60d</t>
+  </si>
+  <si>
+    <t>08696ae1-5a23-4302-b382-481c05b385e2</t>
+  </si>
+  <si>
+    <t>17a0e57b-a3ef-41a3-a53a-051fa1ef1fe9</t>
+  </si>
+  <si>
+    <t>ac4639ee-2562-429a-9812-9753a60b2842</t>
+  </si>
+  <si>
+    <t>37e24e7b-8802-4b7d-a134-175ec924ada1</t>
+  </si>
+  <si>
+    <t>5e52c196-7363-4cf0-8b1b-acb6626c5691</t>
+  </si>
+  <si>
+    <t>cfdf72c7-fc71-4a18-873d-002448eda064</t>
+  </si>
+  <si>
+    <t>7d571e39-c1a9-4c4a-bbdb-ec03dce4b72d</t>
+  </si>
+  <si>
+    <t>93bca538-69cf-479c-91ad-68b23069fe65</t>
+  </si>
+  <si>
+    <t>d17843ce-f61b-43c2-815d-4b00a2985704</t>
+  </si>
+  <si>
+    <t>01ecddd4-e7b1-422d-9c05-9cb30d96ba47</t>
+  </si>
+  <si>
+    <t>cf38f500-1f61-48bc-9ee9-5f0251afdeb9</t>
+  </si>
+  <si>
+    <t>333025a1-fda3-4eb3-adc3-fd5e0af92343</t>
+  </si>
+  <si>
+    <t>bafc2f80-391f-4e74-a444-7282b5fff5bf</t>
+  </si>
+  <si>
+    <t>51ba1ff5-f15b-4890-b5e1-ef4a91c1c950</t>
+  </si>
+  <si>
+    <t>293b8dda-4357-4300-9ed1-61c5e492f5e5</t>
+  </si>
+  <si>
+    <t>45a4ab1f-bd06-48a8-af12-506f8034cb38</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -303,34 +303,34 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>4f4fb0ec-d17c-4756-8889-f2a27eae3a28</t>
-  </si>
-  <si>
-    <t>f2e98b1a-97e7-4a56-bdbb-cf024bac813f</t>
-  </si>
-  <si>
-    <t>f573016b-c933-4694-a254-fdd975460a59</t>
+    <t>0b583feb-d431-4445-b9bf-280bdeeb21e4</t>
+  </si>
+  <si>
+    <t>2211abfb-d08f-4e11-a17e-d0eb7e454d06</t>
+  </si>
+  <si>
+    <t>299b338b-9594-4675-941c-d5f39ed9ecd6</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>1fa35da9-c562-4418-ab5c-9675bcb0c169</t>
-  </si>
-  <si>
-    <t>5b4721d1-5ebe-4dcc-a4e4-11f569607679</t>
-  </si>
-  <si>
-    <t>2bab4fd3-893a-4cae-a47a-03a5f52e81e3</t>
+    <t>2c270a44-7657-40a9-9126-6bcb8af48eb1</t>
+  </si>
+  <si>
+    <t>49f80f75-c571-4bc4-8bf9-6996bbcaeda1</t>
+  </si>
+  <si>
+    <t>9f76fb3f-19f4-4cd0-8b46-6487cff10a12</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>7e10905c-a5f2-4d8d-816c-46939bc7f288</t>
-  </si>
-  <si>
-    <t>1875bacf-0fea-4743-b355-20f897c62328</t>
+    <t>5fd65387-eefe-4a98-912f-a3553859dd28</t>
+  </si>
+  <si>
+    <t>b8f61142-32b1-4053-8d3a-6e7d0a9c8be0</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -339,142 +339,142 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>398367a3-8e6f-4db1-8e4a-a27685203c79</t>
+    <t>8b373373-7de3-4842-abda-b2b4f5823848</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>1c99b50d-3a59-4ab6-b58e-ad21188c3835</t>
-  </si>
-  <si>
-    <t>fe351f07-0fa9-43ce-94d0-2f69ef6a9209</t>
-  </si>
-  <si>
-    <t>c53bfa9f-b87c-4a90-a7e4-dfcab376428e</t>
+    <t>d69760e5-ff96-45be-bd74-d05fbeed9b42</t>
+  </si>
+  <si>
+    <t>5ef9591e-e1b3-4c03-b49f-6f7f65a39340</t>
+  </si>
+  <si>
+    <t>d2a7953c-2ed0-489c-a613-4520aad7d7fe</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>61cf0f84-634e-46f2-917c-cf99150fe9ab</t>
-  </si>
-  <si>
-    <t>47667083-d500-42f8-95e1-f7b14686b5b6</t>
-  </si>
-  <si>
-    <t>eb795860-b156-42f0-84eb-e4ec4e606efb</t>
+    <t>9f3f1c46-cd40-4161-9c48-f80d1e2f9641</t>
+  </si>
+  <si>
+    <t>915bf3fa-e250-4df8-bdd7-eedb7d0f4dc8</t>
+  </si>
+  <si>
+    <t>4f875e73-a4f8-49ca-a53b-3cf822a4e8e6</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>3210278e-c460-4bbc-bbcb-6a1b74a37b74</t>
-  </si>
-  <si>
-    <t>0f64d539-1d71-4ae6-a730-f08cc7349eef</t>
-  </si>
-  <si>
-    <t>dbac4637-04f7-4f73-967b-8e3aa0a55718</t>
+    <t>b989dd6a-b211-4e39-9ec0-87e7d533e3c8</t>
+  </si>
+  <si>
+    <t>4591b529-657a-4625-82a4-7c4c26f9457b</t>
+  </si>
+  <si>
+    <t>4ce4f3f1-bc7b-4331-b476-1d7174dc132b</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>cd9cf62e-67d5-4245-81c4-0080f07e39eb</t>
-  </si>
-  <si>
-    <t>1c8fdd4f-a1f7-4a19-a824-ba621a45b257</t>
-  </si>
-  <si>
-    <t>51caecb9-122d-4ba1-902d-e9e047caa0f7</t>
+    <t>d0c16455-dd52-48af-adff-3aa9d9dbc10c</t>
+  </si>
+  <si>
+    <t>b2b4beea-9873-48e2-9882-233e697dc576</t>
+  </si>
+  <si>
+    <t>d8834c66-1e2c-4612-b195-d7fdcabd3ee9</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>db8a38ed-cf83-400e-a4a5-192ea849872f</t>
-  </si>
-  <si>
-    <t>b9bee7a3-f016-43ab-9b6b-f35bc552c3c2</t>
-  </si>
-  <si>
-    <t>1f5d6c79-83c9-47ca-bf98-d76b4b6ead4a</t>
-  </si>
-  <si>
-    <t>7eb77061-590d-429c-9b4b-64b55cfe4dd4</t>
-  </si>
-  <si>
-    <t>18c10dd8-fd51-442a-9dbb-39d1c0167fbf</t>
-  </si>
-  <si>
-    <t>186ca05a-075a-4794-add0-3213127a815c</t>
-  </si>
-  <si>
-    <t>1223e4d2-10d1-4dff-b7eb-e3827f0a8f9d</t>
-  </si>
-  <si>
-    <t>fc437c56-50e1-40fa-aa1f-80e79639e079</t>
-  </si>
-  <si>
-    <t>1cd94cbe-b70e-4116-9df1-38fc42f61b0b</t>
-  </si>
-  <si>
-    <t>23d8e166-7251-4f8f-9318-834ae37de8f8</t>
-  </si>
-  <si>
-    <t>a7ca19f9-a69a-49bf-8f59-74ee70c52ee5</t>
-  </si>
-  <si>
-    <t>7e8dab49-1a1e-4129-9a02-a8792e278975</t>
-  </si>
-  <si>
-    <t>a0d0cde7-405d-4fb8-9dc6-cca1c554c20e</t>
-  </si>
-  <si>
-    <t>52a68fd9-0fe1-47d1-865f-7bf9a95adb3f</t>
-  </si>
-  <si>
-    <t>2069624f-6b41-43f1-b4c1-1bac0a8a095d</t>
-  </si>
-  <si>
-    <t>95d07939-143d-4313-bbac-884627573ef7</t>
-  </si>
-  <si>
-    <t>f47f4b43-2b14-4f01-b7a6-8be0fe0a7e3b</t>
-  </si>
-  <si>
-    <t>618e3bf6-8b2c-44b7-bf51-9695ae08356b</t>
-  </si>
-  <si>
-    <t>b7bc73cc-e366-4c33-b070-5ad394bcd805</t>
-  </si>
-  <si>
-    <t>ff083d1b-81e3-4ae4-97b7-1f95df6b650a</t>
-  </si>
-  <si>
-    <t>8b475a72-35ee-4570-b1c1-ca748fdd1ba0</t>
-  </si>
-  <si>
-    <t>dd17a62a-c8dd-4450-840c-c870137c0916</t>
-  </si>
-  <si>
-    <t>51521b14-8912-44e5-acf5-16a9c3e29ecd</t>
-  </si>
-  <si>
-    <t>96615a90-e365-4c1c-ac13-f47a36c7f607</t>
-  </si>
-  <si>
-    <t>2257fd37-edaf-4d07-b823-5a0174f51bd5</t>
-  </si>
-  <si>
-    <t>ad9c42f7-ec3f-4310-8e61-33e5d29716eb</t>
-  </si>
-  <si>
-    <t>0fc17170-2adb-4206-af1c-f8c8f04c81cf</t>
-  </si>
-  <si>
-    <t>a117ea99-445c-4a50-a703-081afc88f923</t>
+    <t>f19bffe5-7445-46d7-8af7-081a49f7d65e</t>
+  </si>
+  <si>
+    <t>e27f8e68-8921-4b18-84f1-31e7619311f2</t>
+  </si>
+  <si>
+    <t>31be324e-b735-4fdf-85b9-a068e49bc899</t>
+  </si>
+  <si>
+    <t>77d22c7f-e343-4098-a72b-47f883cf7b81</t>
+  </si>
+  <si>
+    <t>7080a7ef-e9c8-40c5-baa1-86bd6ecc9b89</t>
+  </si>
+  <si>
+    <t>a740b3ca-515e-4e42-98a4-6d7686823a64</t>
+  </si>
+  <si>
+    <t>a23481a4-1851-4dfd-bab2-05026368f7f2</t>
+  </si>
+  <si>
+    <t>ea88aef5-4a7c-48c2-8b53-083e55a8bfd1</t>
+  </si>
+  <si>
+    <t>4f2da91d-61aa-49fc-be40-8c17ab51d0d3</t>
+  </si>
+  <si>
+    <t>0b5e72d4-a166-4be6-b4bc-0ed8a85009d5</t>
+  </si>
+  <si>
+    <t>c8d87316-519b-47fd-97b1-421daeb6aec1</t>
+  </si>
+  <si>
+    <t>fe07ebaf-2688-485a-84b2-11d7f403e294</t>
+  </si>
+  <si>
+    <t>6fe928f4-538e-4a1b-9cfa-43f3b93a6e2e</t>
+  </si>
+  <si>
+    <t>d01f2622-ac04-4837-8b5e-c1c16ec95d2b</t>
+  </si>
+  <si>
+    <t>4ae3b58c-399c-4fe0-b63c-15b157566145</t>
+  </si>
+  <si>
+    <t>fb5165d4-9d15-4f33-91d2-62afb36eaf09</t>
+  </si>
+  <si>
+    <t>c2c0ed9f-19ea-4e51-be5c-477248f45559</t>
+  </si>
+  <si>
+    <t>a419b6b3-1958-4de8-816f-08ecef2f3301</t>
+  </si>
+  <si>
+    <t>a28b6a74-17a1-4e62-84c2-5fe1a8368a0b</t>
+  </si>
+  <si>
+    <t>8f703b1a-0569-4de8-9038-73de3c01c7f8</t>
+  </si>
+  <si>
+    <t>ae5f7f93-e039-4547-a01c-39d8445c17d8</t>
+  </si>
+  <si>
+    <t>4a7eaabf-44b5-4e2f-987a-42c7d33d34db</t>
+  </si>
+  <si>
+    <t>180a3ef8-ed28-40dc-b97e-b6b6964fa6c5</t>
+  </si>
+  <si>
+    <t>fc143e71-9ced-4759-ae31-e78b81b424d9</t>
+  </si>
+  <si>
+    <t>ce31862f-7ee3-4860-bfc1-59e17f90fee0</t>
+  </si>
+  <si>
+    <t>04ace38b-fb5b-4053-9a47-32f0986113d8</t>
+  </si>
+  <si>
+    <t>e21d70c9-9daa-40e5-9d15-453d0241d43f</t>
+  </si>
+  <si>
+    <t>61e8bf9e-1a2c-4ad4-b3d4-e7ee8cf23683</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -627,7 +627,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>402e96de-6b86-4346-a47b-259fb06965bf</t>
+    <t>81d1190e-0aaf-4353-bd71-0211304eea98</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
fix: Demographic data CSV fields & FHIR structure issues reported #82 #88 #89
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>64e3e242-a920-4656-b133-1dcd8fa4fbcd</t>
+    <t>23fb7f2a-6a9c-4ea1-82f2-623ea4ba38f5</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>88072bed-b6e6-41d0-ac92-40aae0641988</t>
+    <t>1a5444e6-f505-4fb4-bf54-050f84516d6e</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>3a7b7ec9-c98d-4e64-9fcb-e9051dae800a</t>
+    <t>f772d4ce-83c6-4eac-8470-e2a809381ee8</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -165,7 +165,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>2bc148ea-b314-4b5a-b282-01becf0d5723</t>
+    <t>72d47d98-219f-4b69-82ac-8638befeb868</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -183,7 +183,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>4a0c17b9-a0f8-4152-af17-eeee432b6fbe</t>
+    <t>dbe638b1-724d-4104-9037-83d1da57449e</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -201,16 +201,16 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>b117452d-f333-4429-a599-c2f6031e812a</t>
-  </si>
-  <si>
-    <t>ba74db85-7a80-49c2-84bf-a617830b546d</t>
-  </si>
-  <si>
-    <t>80eb1571-3523-4dbd-9f95-beacf9f26400</t>
-  </si>
-  <si>
-    <t>245a6636-d16b-4ab9-9018-b7221db2e9d3</t>
+    <t>3305aeb2-9df5-4d71-9031-74c721b020d4</t>
+  </si>
+  <si>
+    <t>8c11661c-f148-463e-b7d4-6edcfc1a1d78</t>
+  </si>
+  <si>
+    <t>4379df56-8053-41f8-9c58-7ac9d1f7ba91</t>
+  </si>
+  <si>
+    <t>24a6496e-070c-4230-8c85-7e20e9bae756</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -219,13 +219,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>eec57008-04bd-4a7d-a478-f59a3f00f1be</t>
-  </si>
-  <si>
-    <t>954587d9-f0f4-4ab7-aa99-9b70559bc7cc</t>
-  </si>
-  <si>
-    <t>aedab293-d339-469f-aea3-06bfe9b1b89e</t>
+    <t>7009a27f-22c6-4041-b738-00c95dafe3a6</t>
+  </si>
+  <si>
+    <t>fd3cd4fe-456d-4d99-af1a-4671de0a1a04</t>
+  </si>
+  <si>
+    <t>5e332762-b7e9-4dc1-b80c-4e7e390f282c</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -237,58 +237,58 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>4f4fbb6d-a00b-42c0-8f1a-d7578dab55e5</t>
-  </si>
-  <si>
-    <t>709e1066-3b5a-4ef4-8ed2-0bde53e2a60d</t>
-  </si>
-  <si>
-    <t>08696ae1-5a23-4302-b382-481c05b385e2</t>
-  </si>
-  <si>
-    <t>17a0e57b-a3ef-41a3-a53a-051fa1ef1fe9</t>
-  </si>
-  <si>
-    <t>ac4639ee-2562-429a-9812-9753a60b2842</t>
-  </si>
-  <si>
-    <t>37e24e7b-8802-4b7d-a134-175ec924ada1</t>
-  </si>
-  <si>
-    <t>5e52c196-7363-4cf0-8b1b-acb6626c5691</t>
-  </si>
-  <si>
-    <t>cfdf72c7-fc71-4a18-873d-002448eda064</t>
-  </si>
-  <si>
-    <t>7d571e39-c1a9-4c4a-bbdb-ec03dce4b72d</t>
-  </si>
-  <si>
-    <t>93bca538-69cf-479c-91ad-68b23069fe65</t>
-  </si>
-  <si>
-    <t>d17843ce-f61b-43c2-815d-4b00a2985704</t>
-  </si>
-  <si>
-    <t>01ecddd4-e7b1-422d-9c05-9cb30d96ba47</t>
-  </si>
-  <si>
-    <t>cf38f500-1f61-48bc-9ee9-5f0251afdeb9</t>
-  </si>
-  <si>
-    <t>333025a1-fda3-4eb3-adc3-fd5e0af92343</t>
-  </si>
-  <si>
-    <t>bafc2f80-391f-4e74-a444-7282b5fff5bf</t>
-  </si>
-  <si>
-    <t>51ba1ff5-f15b-4890-b5e1-ef4a91c1c950</t>
-  </si>
-  <si>
-    <t>293b8dda-4357-4300-9ed1-61c5e492f5e5</t>
-  </si>
-  <si>
-    <t>45a4ab1f-bd06-48a8-af12-506f8034cb38</t>
+    <t>2106dd5f-bbf4-4953-8987-276acad055ae</t>
+  </si>
+  <si>
+    <t>ac9ce6b3-a435-4656-9479-389fdd5dd652</t>
+  </si>
+  <si>
+    <t>12cfa314-4c5c-45e2-a1c9-79e5d31329cb</t>
+  </si>
+  <si>
+    <t>e8128046-ca60-4932-95ab-56674ee7dd23</t>
+  </si>
+  <si>
+    <t>fe6e8e34-8aae-49ea-bc74-6a75e031b05a</t>
+  </si>
+  <si>
+    <t>8f1769be-b9ff-470c-b0ba-ed0d1b1c97dd</t>
+  </si>
+  <si>
+    <t>825edb45-da5d-4e71-b954-52f3ddc0957e</t>
+  </si>
+  <si>
+    <t>63b94fcd-375f-4a5a-8815-1a4d562fdbee</t>
+  </si>
+  <si>
+    <t>33ecd688-b39c-41c0-8519-ad86d3157257</t>
+  </si>
+  <si>
+    <t>b927a30a-d1dd-42cc-a515-563f9490e91e</t>
+  </si>
+  <si>
+    <t>7b65c2cf-0a0a-468a-9110-369ab9192dea</t>
+  </si>
+  <si>
+    <t>cba00a01-e1cd-46a7-a278-4c9aedbcc372</t>
+  </si>
+  <si>
+    <t>5dab577d-83dc-45db-ae48-793fa2301ec2</t>
+  </si>
+  <si>
+    <t>a0c5b76a-b6cf-4210-a317-cd268e0261f2</t>
+  </si>
+  <si>
+    <t>543be7af-d057-4d30-8ad9-471133f2ae6e</t>
+  </si>
+  <si>
+    <t>e450b46f-3e68-4f8d-ba48-54f23054f79d</t>
+  </si>
+  <si>
+    <t>cf3d1053-f6ce-42e6-9610-d85d69d621c4</t>
+  </si>
+  <si>
+    <t>4fcfd071-46b4-4f0f-98f2-745cc7d0e57d</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -303,34 +303,34 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>0b583feb-d431-4445-b9bf-280bdeeb21e4</t>
-  </si>
-  <si>
-    <t>2211abfb-d08f-4e11-a17e-d0eb7e454d06</t>
-  </si>
-  <si>
-    <t>299b338b-9594-4675-941c-d5f39ed9ecd6</t>
+    <t>6e0a2052-5d78-4b7d-9969-dbe5980ecf57</t>
+  </si>
+  <si>
+    <t>cbb27627-d1db-4cf4-85da-12610657dfca</t>
+  </si>
+  <si>
+    <t>c6813f05-fe68-47b9-b454-69facc02b939</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>2c270a44-7657-40a9-9126-6bcb8af48eb1</t>
-  </si>
-  <si>
-    <t>49f80f75-c571-4bc4-8bf9-6996bbcaeda1</t>
-  </si>
-  <si>
-    <t>9f76fb3f-19f4-4cd0-8b46-6487cff10a12</t>
+    <t>3ff99f77-a629-4ffb-9dfd-0e0c386fcd00</t>
+  </si>
+  <si>
+    <t>5b837cfa-2c99-4d99-9c70-cf397658e377</t>
+  </si>
+  <si>
+    <t>1411cf27-3598-47c6-8093-3d99e5e3a8fa</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>5fd65387-eefe-4a98-912f-a3553859dd28</t>
-  </si>
-  <si>
-    <t>b8f61142-32b1-4053-8d3a-6e7d0a9c8be0</t>
+    <t>4921d556-017b-42c3-922c-0849ff8b7553</t>
+  </si>
+  <si>
+    <t>77836f79-1d43-4f17-96a5-7230d1a82122</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -339,142 +339,142 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>8b373373-7de3-4842-abda-b2b4f5823848</t>
+    <t>d8054ee3-8c5f-46a5-9723-00551f37feed</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>d69760e5-ff96-45be-bd74-d05fbeed9b42</t>
-  </si>
-  <si>
-    <t>5ef9591e-e1b3-4c03-b49f-6f7f65a39340</t>
-  </si>
-  <si>
-    <t>d2a7953c-2ed0-489c-a613-4520aad7d7fe</t>
+    <t>381b5d4c-ee98-4bb1-b4f8-a7363639ea46</t>
+  </si>
+  <si>
+    <t>0cf8e999-ff7a-4dda-ae96-2760514c1cb7</t>
+  </si>
+  <si>
+    <t>cc375c51-c152-4626-8662-eba878668df7</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>9f3f1c46-cd40-4161-9c48-f80d1e2f9641</t>
-  </si>
-  <si>
-    <t>915bf3fa-e250-4df8-bdd7-eedb7d0f4dc8</t>
-  </si>
-  <si>
-    <t>4f875e73-a4f8-49ca-a53b-3cf822a4e8e6</t>
+    <t>57500dbf-377f-40d2-976a-c561e40cb632</t>
+  </si>
+  <si>
+    <t>dbde23d4-d66a-4820-8603-da4400657570</t>
+  </si>
+  <si>
+    <t>71041473-44ad-4cdd-85e6-c297e8c088b7</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>b989dd6a-b211-4e39-9ec0-87e7d533e3c8</t>
-  </si>
-  <si>
-    <t>4591b529-657a-4625-82a4-7c4c26f9457b</t>
-  </si>
-  <si>
-    <t>4ce4f3f1-bc7b-4331-b476-1d7174dc132b</t>
+    <t>8fff461b-93a1-42e8-8e81-07c78e81a043</t>
+  </si>
+  <si>
+    <t>d20c7a75-c109-4792-88be-22a70256e2fe</t>
+  </si>
+  <si>
+    <t>2cd08745-505c-4718-987a-5f7c89bc05a1</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>d0c16455-dd52-48af-adff-3aa9d9dbc10c</t>
-  </si>
-  <si>
-    <t>b2b4beea-9873-48e2-9882-233e697dc576</t>
-  </si>
-  <si>
-    <t>d8834c66-1e2c-4612-b195-d7fdcabd3ee9</t>
+    <t>568fcd18-4265-4d63-a08d-d6cb3320eebc</t>
+  </si>
+  <si>
+    <t>e28a1b92-816c-4102-a9c2-0c51db88e7ae</t>
+  </si>
+  <si>
+    <t>eeb19dbd-7a50-44d5-816f-d85c03f03876</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>f19bffe5-7445-46d7-8af7-081a49f7d65e</t>
-  </si>
-  <si>
-    <t>e27f8e68-8921-4b18-84f1-31e7619311f2</t>
-  </si>
-  <si>
-    <t>31be324e-b735-4fdf-85b9-a068e49bc899</t>
-  </si>
-  <si>
-    <t>77d22c7f-e343-4098-a72b-47f883cf7b81</t>
-  </si>
-  <si>
-    <t>7080a7ef-e9c8-40c5-baa1-86bd6ecc9b89</t>
-  </si>
-  <si>
-    <t>a740b3ca-515e-4e42-98a4-6d7686823a64</t>
-  </si>
-  <si>
-    <t>a23481a4-1851-4dfd-bab2-05026368f7f2</t>
-  </si>
-  <si>
-    <t>ea88aef5-4a7c-48c2-8b53-083e55a8bfd1</t>
-  </si>
-  <si>
-    <t>4f2da91d-61aa-49fc-be40-8c17ab51d0d3</t>
-  </si>
-  <si>
-    <t>0b5e72d4-a166-4be6-b4bc-0ed8a85009d5</t>
-  </si>
-  <si>
-    <t>c8d87316-519b-47fd-97b1-421daeb6aec1</t>
-  </si>
-  <si>
-    <t>fe07ebaf-2688-485a-84b2-11d7f403e294</t>
-  </si>
-  <si>
-    <t>6fe928f4-538e-4a1b-9cfa-43f3b93a6e2e</t>
-  </si>
-  <si>
-    <t>d01f2622-ac04-4837-8b5e-c1c16ec95d2b</t>
-  </si>
-  <si>
-    <t>4ae3b58c-399c-4fe0-b63c-15b157566145</t>
-  </si>
-  <si>
-    <t>fb5165d4-9d15-4f33-91d2-62afb36eaf09</t>
-  </si>
-  <si>
-    <t>c2c0ed9f-19ea-4e51-be5c-477248f45559</t>
-  </si>
-  <si>
-    <t>a419b6b3-1958-4de8-816f-08ecef2f3301</t>
-  </si>
-  <si>
-    <t>a28b6a74-17a1-4e62-84c2-5fe1a8368a0b</t>
-  </si>
-  <si>
-    <t>8f703b1a-0569-4de8-9038-73de3c01c7f8</t>
-  </si>
-  <si>
-    <t>ae5f7f93-e039-4547-a01c-39d8445c17d8</t>
-  </si>
-  <si>
-    <t>4a7eaabf-44b5-4e2f-987a-42c7d33d34db</t>
-  </si>
-  <si>
-    <t>180a3ef8-ed28-40dc-b97e-b6b6964fa6c5</t>
-  </si>
-  <si>
-    <t>fc143e71-9ced-4759-ae31-e78b81b424d9</t>
-  </si>
-  <si>
-    <t>ce31862f-7ee3-4860-bfc1-59e17f90fee0</t>
-  </si>
-  <si>
-    <t>04ace38b-fb5b-4053-9a47-32f0986113d8</t>
-  </si>
-  <si>
-    <t>e21d70c9-9daa-40e5-9d15-453d0241d43f</t>
-  </si>
-  <si>
-    <t>61e8bf9e-1a2c-4ad4-b3d4-e7ee8cf23683</t>
+    <t>855ad8d6-d82c-4912-82bd-c8f7ae6b6c15</t>
+  </si>
+  <si>
+    <t>fd93f280-5bf9-4d3c-8802-5dcc3ec8dbb9</t>
+  </si>
+  <si>
+    <t>b9ba049f-6f75-413f-8d3c-e15be59e1bd2</t>
+  </si>
+  <si>
+    <t>4955f804-2ad0-4e3b-a76b-ca09e89137cf</t>
+  </si>
+  <si>
+    <t>ff3c1f34-469e-40fb-bdc4-4980ec70eed9</t>
+  </si>
+  <si>
+    <t>41f4b5aa-01b7-46ed-951c-622e2adc39a3</t>
+  </si>
+  <si>
+    <t>da391883-92d9-4a36-b3aa-32d33ac6e15b</t>
+  </si>
+  <si>
+    <t>d8c667b3-0ec2-4c86-b0f0-e545a1c4dad5</t>
+  </si>
+  <si>
+    <t>849304f8-3de8-4ec9-b685-c95d4d00dde6</t>
+  </si>
+  <si>
+    <t>bebf1abc-dc5e-432e-8eb1-5281b628cb7e</t>
+  </si>
+  <si>
+    <t>5e5b90e3-bb6b-4a43-bbd6-56aeb720d6fe</t>
+  </si>
+  <si>
+    <t>6a580fcc-b6a9-49c0-b317-937f70b65f2b</t>
+  </si>
+  <si>
+    <t>ebc973e3-c637-45a0-94c8-e54b1c8daaea</t>
+  </si>
+  <si>
+    <t>3275935e-7408-42ea-8bca-d032bf5d82ad</t>
+  </si>
+  <si>
+    <t>28a49d02-f4e0-475e-b5b9-f247fcff9329</t>
+  </si>
+  <si>
+    <t>fe28baaa-e512-4918-8ffb-07b1632fb952</t>
+  </si>
+  <si>
+    <t>be5d723e-5b6c-4748-a0c0-25715493dae1</t>
+  </si>
+  <si>
+    <t>e3d5fdf7-c58a-4dc8-b2c6-f59bbe71ea72</t>
+  </si>
+  <si>
+    <t>305d8d3a-d319-486f-8fcc-0a2c3f26efd3</t>
+  </si>
+  <si>
+    <t>262e316a-5a33-4b8d-8a5a-2a6254bfde44</t>
+  </si>
+  <si>
+    <t>61304178-e0a9-46de-99c4-247de83a1c6c</t>
+  </si>
+  <si>
+    <t>b9bd9660-acc9-4098-8b3c-737824dfeea0</t>
+  </si>
+  <si>
+    <t>7b5a0490-acc4-4399-9e49-9c4883e89571</t>
+  </si>
+  <si>
+    <t>ba0ef346-179e-445c-b01a-40c02d31a576</t>
+  </si>
+  <si>
+    <t>8c255a5a-c62c-46cd-b507-5561cc50578f</t>
+  </si>
+  <si>
+    <t>bddbf100-5284-488a-a8e3-a4c2a9c437e9</t>
+  </si>
+  <si>
+    <t>f68585c2-56cb-47b6-87c5-b53e9a92ede2</t>
+  </si>
+  <si>
+    <t>de7c5407-bd0d-49b7-b76b-8191f6869804</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -627,7 +627,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>81d1190e-0aaf-4353-bd71-0211304eea98</t>
+    <t>353678b9-9a62-4dab-bdc0-f83a58107132</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
fix: Fix issue in fhir json generation for missing encounters #88
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -81,7 +81,7 @@
     <t>7bab389e-54af-5a13-a39f-079abdc73a48</t>
   </si>
   <si>
-    <t>0.10.1</t>
+    <t>0.10.2</t>
   </si>
   <si>
     <t>Session 05269d28-15ae-5bd6-bd88-f949ccfa52d7 markdown diagnostics not provided (not completed?)</t>
@@ -96,7 +96,7 @@
     <t>screening_20240307</t>
   </si>
   <si>
-    <t>23fb7f2a-6a9c-4ea1-82f2-623ea4ba38f5</t>
+    <t>9fd3e417-3582-46ba-95c3-00879067e726</t>
   </si>
   <si>
     <t>Invalid Value</t>
@@ -120,7 +120,7 @@
     <t>Resolved By QE/QCS</t>
   </si>
   <si>
-    <t>1a5444e6-f505-4fb4-bf54-050f84516d6e</t>
+    <t>2dc6e40d-6554-43c6-aad8-c8a180ffd722</t>
   </si>
   <si>
     <t>Invalid Date</t>
@@ -138,7 +138,7 @@
     <t>Please be sure to provide both a valid date and time.</t>
   </si>
   <si>
-    <t>f772d4ce-83c6-4eac-8470-e2a809381ee8</t>
+    <t>d1baf160-351e-4bc2-ba92-40e7d4170bd3</t>
   </si>
   <si>
     <t>Missing Mandatory Value</t>
@@ -165,7 +165,7 @@
     <t>admin_demographics_20240307</t>
   </si>
   <si>
-    <t>72d47d98-219f-4b69-82ac-8638befeb868</t>
+    <t>b7a39775-4cfe-417a-b8bb-206cccf78454</t>
   </si>
   <si>
     <t>Combination Not Matching</t>
@@ -183,7 +183,7 @@
     <t>The RACE_CODE "1142-9" of RACE_CODE_DESCRIPTION "Coquille" is not matching with the RACE_CODE of RACE_CODE_DESCRIPTION in reference data</t>
   </si>
   <si>
-    <t>dbe638b1-724d-4104-9037-83d1da57449e</t>
+    <t>a3901164-c413-4cda-b0a4-c3ea8aef4832</t>
   </si>
   <si>
     <t>Invalid RACE CODE DESCRIPTION</t>
@@ -201,16 +201,16 @@
     <t>Validate RACE CODE DESCRIPTION with race reference data</t>
   </si>
   <si>
-    <t>3305aeb2-9df5-4d71-9031-74c721b020d4</t>
-  </si>
-  <si>
-    <t>8c11661c-f148-463e-b7d4-6edcfc1a1d78</t>
-  </si>
-  <si>
-    <t>4379df56-8053-41f8-9c58-7ac9d1f7ba91</t>
-  </si>
-  <si>
-    <t>24a6496e-070c-4230-8c85-7e20e9bae756</t>
+    <t>303931bf-eb91-49b9-ad4f-d0e1beadb13a</t>
+  </si>
+  <si>
+    <t>e1d31992-a452-4822-b96a-918b282dc82d</t>
+  </si>
+  <si>
+    <t>6dce7fc7-a4e4-42e4-a971-a65dae0efc58</t>
+  </si>
+  <si>
+    <t>a75f49ac-025f-4b2a-a9cf-a1ed766f934e</t>
   </si>
   <si>
     <t>Invalid value "Coquille" found in RACE_CODE_DESCRIPTION</t>
@@ -219,13 +219,13 @@
     <t>The RACE_CODE_DESCRIPTION "Coquille" of RACE_CODE "1142-9" is not matching with the RACE_CODE_DESCRIPTION of RACE_CODE in reference data</t>
   </si>
   <si>
-    <t>7009a27f-22c6-4041-b738-00c95dafe3a6</t>
-  </si>
-  <si>
-    <t>fd3cd4fe-456d-4d99-af1a-4671de0a1a04</t>
-  </si>
-  <si>
-    <t>5e332762-b7e9-4dc1-b80c-4e7e390f282c</t>
+    <t>60d973e9-5bd8-4e77-925b-0b7f61aabcb5</t>
+  </si>
+  <si>
+    <t>8529fa01-9219-4cd1-8a7a-7288a1b43a56</t>
+  </si>
+  <si>
+    <t>458691ba-4886-470a-86b4-40cb38d14df4</t>
   </si>
   <si>
     <t>Value N/A in POTENTIAL_NEED_INDICATED not in allowed list ('Yes','No','NA','yes','no','na')</t>
@@ -237,58 +237,58 @@
     <t>Use only allowed values 'Yes','No','NA','yes','no','na' in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>2106dd5f-bbf4-4953-8987-276acad055ae</t>
-  </si>
-  <si>
-    <t>ac9ce6b3-a435-4656-9479-389fdd5dd652</t>
-  </si>
-  <si>
-    <t>12cfa314-4c5c-45e2-a1c9-79e5d31329cb</t>
-  </si>
-  <si>
-    <t>e8128046-ca60-4932-95ab-56674ee7dd23</t>
-  </si>
-  <si>
-    <t>fe6e8e34-8aae-49ea-bc74-6a75e031b05a</t>
-  </si>
-  <si>
-    <t>8f1769be-b9ff-470c-b0ba-ed0d1b1c97dd</t>
-  </si>
-  <si>
-    <t>825edb45-da5d-4e71-b954-52f3ddc0957e</t>
-  </si>
-  <si>
-    <t>63b94fcd-375f-4a5a-8815-1a4d562fdbee</t>
-  </si>
-  <si>
-    <t>33ecd688-b39c-41c0-8519-ad86d3157257</t>
-  </si>
-  <si>
-    <t>b927a30a-d1dd-42cc-a515-563f9490e91e</t>
-  </si>
-  <si>
-    <t>7b65c2cf-0a0a-468a-9110-369ab9192dea</t>
-  </si>
-  <si>
-    <t>cba00a01-e1cd-46a7-a278-4c9aedbcc372</t>
-  </si>
-  <si>
-    <t>5dab577d-83dc-45db-ae48-793fa2301ec2</t>
-  </si>
-  <si>
-    <t>a0c5b76a-b6cf-4210-a317-cd268e0261f2</t>
-  </si>
-  <si>
-    <t>543be7af-d057-4d30-8ad9-471133f2ae6e</t>
-  </si>
-  <si>
-    <t>e450b46f-3e68-4f8d-ba48-54f23054f79d</t>
-  </si>
-  <si>
-    <t>cf3d1053-f6ce-42e6-9610-d85d69d621c4</t>
-  </si>
-  <si>
-    <t>4fcfd071-46b4-4f0f-98f2-745cc7d0e57d</t>
+    <t>7e90c9a5-e4ad-41a1-8bd5-997e7ca346ad</t>
+  </si>
+  <si>
+    <t>fc045f6a-41d9-46db-a729-7f2af5061fcb</t>
+  </si>
+  <si>
+    <t>03775aee-13d6-4217-aee8-0cbd84ed2213</t>
+  </si>
+  <si>
+    <t>411db574-fcbc-4adb-a5b9-98304503b359</t>
+  </si>
+  <si>
+    <t>44904906-191b-4bd6-9f4e-e339985b4562</t>
+  </si>
+  <si>
+    <t>628e8f26-7094-4d02-b963-4a420f9980dc</t>
+  </si>
+  <si>
+    <t>7a16a168-aa27-426a-a2c8-bdedc085a3cc</t>
+  </si>
+  <si>
+    <t>f857ef5b-e9c2-440d-b0be-b5658daeb055</t>
+  </si>
+  <si>
+    <t>1c2a17e7-2c9e-4362-8bd9-2cb140510355</t>
+  </si>
+  <si>
+    <t>9a80c399-b3fa-4b35-b1a7-f4c311ad2d65</t>
+  </si>
+  <si>
+    <t>ffdaf977-7c72-480b-8a1f-486cf8c06938</t>
+  </si>
+  <si>
+    <t>40642f3e-d6b5-4d5a-8521-e2a2089881f8</t>
+  </si>
+  <si>
+    <t>fffdb8a8-65db-4f70-8a2a-c7cab63b1359</t>
+  </si>
+  <si>
+    <t>ca9da0c6-a511-437e-afd0-22d6746a845e</t>
+  </si>
+  <si>
+    <t>b9f32bba-e240-4125-8aad-170cafe91366</t>
+  </si>
+  <si>
+    <t>0a91b605-b54d-4eaa-ad16-08d2d4e86e49</t>
+  </si>
+  <si>
+    <t>76f680ab-b8d0-43d1-8566-346e7c636b3f</t>
+  </si>
+  <si>
+    <t>000b63ad-edf9-4db5-82c7-d75d4640c704</t>
   </si>
   <si>
     <t>Invalid value in POTENTIAL_NEED_INDICATED</t>
@@ -303,34 +303,34 @@
     <t>Validate Potential Need Indicated, Screening Code, Question Code and Answer Code with ahc cross walk reference data</t>
   </si>
   <si>
-    <t>6e0a2052-5d78-4b7d-9969-dbe5980ecf57</t>
-  </si>
-  <si>
-    <t>cbb27627-d1db-4cf4-85da-12610657dfca</t>
-  </si>
-  <si>
-    <t>c6813f05-fe68-47b9-b454-69facc02b939</t>
+    <t>d2050cb1-dc13-41cd-8f8e-08759a473bac</t>
+  </si>
+  <si>
+    <t>0fe06e09-16ba-4983-8afc-7f5c3ba9878f</t>
+  </si>
+  <si>
+    <t>691c4eb1-c5a0-42fb-bf51-f713b271fbab</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95618-5" and Answer Code "LA10066-1" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>3ff99f77-a629-4ffb-9dfd-0e0c386fcd00</t>
-  </si>
-  <si>
-    <t>5b837cfa-2c99-4d99-9c70-cf397658e377</t>
-  </si>
-  <si>
-    <t>1411cf27-3598-47c6-8093-3d99e5e3a8fa</t>
+    <t>852d66ab-ebbe-4ceb-91f5-9c67749ada3a</t>
+  </si>
+  <si>
+    <t>cad7516f-cd2a-46c4-99d5-edb0bc26bbed</t>
+  </si>
+  <si>
+    <t>f99c8ba0-40cc-4561-9eb0-17ced4c9feb8</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95615-1" and Answer Code "LA10082-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>4921d556-017b-42c3-922c-0849ff8b7553</t>
-  </si>
-  <si>
-    <t>77836f79-1d43-4f17-96a5-7230d1a82122</t>
+    <t>455a067d-70ab-495e-b295-c7bc2ee90ec8</t>
+  </si>
+  <si>
+    <t>9f48f3f4-fc97-4d57-bd3f-93bbc5324b12</t>
   </si>
   <si>
     <t>Invalid timestamp "03/05/94 13:08" found in RECORDED_TIME</t>
@@ -339,142 +339,142 @@
     <t>03/05/94 13:08</t>
   </si>
   <si>
-    <t>d8054ee3-8c5f-46a5-9723-00551f37feed</t>
+    <t>43fc1838-ced3-4aa3-bb19-73098f3b9d62</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95616-9" and Answer Code "LA16644-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>381b5d4c-ee98-4bb1-b4f8-a7363639ea46</t>
-  </si>
-  <si>
-    <t>0cf8e999-ff7a-4dda-ae96-2760514c1cb7</t>
-  </si>
-  <si>
-    <t>cc375c51-c152-4626-8662-eba878668df7</t>
+    <t>5ae98409-8df3-4c15-9569-f03ee21b415c</t>
+  </si>
+  <si>
+    <t>4372558f-1383-4ecf-b839-e12bcce5a2b5</t>
+  </si>
+  <si>
+    <t>4bb0f8d1-23c6-4aca-8dbc-42e108b9fc06</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "68516-4" and Answer Code "LA28853-2" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>57500dbf-377f-40d2-976a-c561e40cb632</t>
-  </si>
-  <si>
-    <t>dbde23d4-d66a-4820-8603-da4400657570</t>
-  </si>
-  <si>
-    <t>71041473-44ad-4cdd-85e6-c297e8c088b7</t>
+    <t>5f445ad8-8db0-4925-b7bf-6c85df877131</t>
+  </si>
+  <si>
+    <t>bc53fd75-c097-4fc2-afe5-4e7cf0a3b064</t>
+  </si>
+  <si>
+    <t>3597a11a-0e5c-4d37-b6ad-f18b1b9ecbcf</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "96777-8", Question Code "95617-7" and Answer Code "LA6270-8" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>8fff461b-93a1-42e8-8e81-07c78e81a043</t>
-  </si>
-  <si>
-    <t>d20c7a75-c109-4792-88be-22a70256e2fe</t>
-  </si>
-  <si>
-    <t>2cd08745-505c-4718-987a-5f7c89bc05a1</t>
+    <t>09a9b03d-ccb8-42ce-8008-305a8734e3f5</t>
+  </si>
+  <si>
+    <t>5abf28d6-ae38-4903-9bf8-1d987127a05f</t>
+  </si>
+  <si>
+    <t>3f227d63-66bc-46e3-a857-df8762cd5aad</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "NULL", Screening Code "97023-6", Question Code "44250-9" and Answer Code "LA6571-9" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>568fcd18-4265-4d63-a08d-d6cb3320eebc</t>
-  </si>
-  <si>
-    <t>e28a1b92-816c-4102-a9c2-0c51db88e7ae</t>
-  </si>
-  <si>
-    <t>eeb19dbd-7a50-44d5-816f-d85c03f03876</t>
+    <t>60825e9e-01d9-4a71-923d-7ff542de3859</t>
+  </si>
+  <si>
+    <t>0b3a2b49-665e-48fc-a339-8b6e36a946d7</t>
+  </si>
+  <si>
+    <t>efc679f5-9851-4c4d-98fb-79d4e5a53706</t>
   </si>
   <si>
     <t>Provided Potential Need Indicated "N/A", Screening Code "97023-6", Question Code "89555-7" and Answer Code "LA6113-0" are not matching with the reference data found in POTENTIAL_NEED_INDICATED</t>
   </si>
   <si>
-    <t>855ad8d6-d82c-4912-82bd-c8f7ae6b6c15</t>
-  </si>
-  <si>
-    <t>fd93f280-5bf9-4d3c-8802-5dcc3ec8dbb9</t>
-  </si>
-  <si>
-    <t>b9ba049f-6f75-413f-8d3c-e15be59e1bd2</t>
-  </si>
-  <si>
-    <t>4955f804-2ad0-4e3b-a76b-ca09e89137cf</t>
-  </si>
-  <si>
-    <t>ff3c1f34-469e-40fb-bdc4-4980ec70eed9</t>
-  </si>
-  <si>
-    <t>41f4b5aa-01b7-46ed-951c-622e2adc39a3</t>
-  </si>
-  <si>
-    <t>da391883-92d9-4a36-b3aa-32d33ac6e15b</t>
-  </si>
-  <si>
-    <t>d8c667b3-0ec2-4c86-b0f0-e545a1c4dad5</t>
-  </si>
-  <si>
-    <t>849304f8-3de8-4ec9-b685-c95d4d00dde6</t>
-  </si>
-  <si>
-    <t>bebf1abc-dc5e-432e-8eb1-5281b628cb7e</t>
-  </si>
-  <si>
-    <t>5e5b90e3-bb6b-4a43-bbd6-56aeb720d6fe</t>
-  </si>
-  <si>
-    <t>6a580fcc-b6a9-49c0-b317-937f70b65f2b</t>
-  </si>
-  <si>
-    <t>ebc973e3-c637-45a0-94c8-e54b1c8daaea</t>
-  </si>
-  <si>
-    <t>3275935e-7408-42ea-8bca-d032bf5d82ad</t>
-  </si>
-  <si>
-    <t>28a49d02-f4e0-475e-b5b9-f247fcff9329</t>
-  </si>
-  <si>
-    <t>fe28baaa-e512-4918-8ffb-07b1632fb952</t>
-  </si>
-  <si>
-    <t>be5d723e-5b6c-4748-a0c0-25715493dae1</t>
-  </si>
-  <si>
-    <t>e3d5fdf7-c58a-4dc8-b2c6-f59bbe71ea72</t>
-  </si>
-  <si>
-    <t>305d8d3a-d319-486f-8fcc-0a2c3f26efd3</t>
-  </si>
-  <si>
-    <t>262e316a-5a33-4b8d-8a5a-2a6254bfde44</t>
-  </si>
-  <si>
-    <t>61304178-e0a9-46de-99c4-247de83a1c6c</t>
-  </si>
-  <si>
-    <t>b9bd9660-acc9-4098-8b3c-737824dfeea0</t>
-  </si>
-  <si>
-    <t>7b5a0490-acc4-4399-9e49-9c4883e89571</t>
-  </si>
-  <si>
-    <t>ba0ef346-179e-445c-b01a-40c02d31a576</t>
-  </si>
-  <si>
-    <t>8c255a5a-c62c-46cd-b507-5561cc50578f</t>
-  </si>
-  <si>
-    <t>bddbf100-5284-488a-a8e3-a4c2a9c437e9</t>
-  </si>
-  <si>
-    <t>f68585c2-56cb-47b6-87c5-b53e9a92ede2</t>
-  </si>
-  <si>
-    <t>de7c5407-bd0d-49b7-b76b-8191f6869804</t>
+    <t>e146e43c-d072-435f-afd4-d257467eb7c5</t>
+  </si>
+  <si>
+    <t>e4283e08-dd82-4e8e-81f6-1459548407d3</t>
+  </si>
+  <si>
+    <t>f6566695-9564-412a-9b30-f1ca756ec324</t>
+  </si>
+  <si>
+    <t>e0046b1e-d7b7-4130-a750-12f5e9f6b1e9</t>
+  </si>
+  <si>
+    <t>b3630b75-695c-42fc-b6e3-4b1ed114c7cd</t>
+  </si>
+  <si>
+    <t>70118710-d1cf-451a-ad9f-b026a99f83f8</t>
+  </si>
+  <si>
+    <t>093771f8-b04f-4160-b211-96780736d3e9</t>
+  </si>
+  <si>
+    <t>24bc18d7-e8e8-4bdb-90db-c64184a559a3</t>
+  </si>
+  <si>
+    <t>4382f6da-5b1f-4ce2-950f-5090cbf9c8f3</t>
+  </si>
+  <si>
+    <t>0bc27811-4640-4391-ba21-aaa584255af4</t>
+  </si>
+  <si>
+    <t>c9d3df1f-f4f4-400b-ac90-42ab06c86eff</t>
+  </si>
+  <si>
+    <t>2fb74a0e-9bfa-4aa2-b077-bbc3ddc38483</t>
+  </si>
+  <si>
+    <t>b1c31bb6-6dd0-4ddc-a304-17e0648af64c</t>
+  </si>
+  <si>
+    <t>33617cda-dc6b-4010-a697-898da30b86d4</t>
+  </si>
+  <si>
+    <t>ed45fc53-dbeb-4e35-8ff9-89ddb40a05df</t>
+  </si>
+  <si>
+    <t>9c134df2-3342-4a86-a564-87f384badcde</t>
+  </si>
+  <si>
+    <t>fde877e1-3d43-48aa-880d-ee9d938409e1</t>
+  </si>
+  <si>
+    <t>8059d9d0-cea6-4ae2-b81c-4079faa11dbc</t>
+  </si>
+  <si>
+    <t>b02a7600-4e97-4088-af56-2caadfca079f</t>
+  </si>
+  <si>
+    <t>705e0968-d621-49f4-86d9-e7a495b978ea</t>
+  </si>
+  <si>
+    <t>1423673a-0da4-4ce7-a276-a2cda6102cdf</t>
+  </si>
+  <si>
+    <t>868799e5-46d1-4f7b-8f62-a661561d3aa5</t>
+  </si>
+  <si>
+    <t>4fad556f-7ba5-488d-b519-b2963704d522</t>
+  </si>
+  <si>
+    <t>23ce14b7-d7d1-4350-84e9-8951856defdf</t>
+  </si>
+  <si>
+    <t>fb9cc18f-b28b-45fc-99d1-040f368efb21</t>
+  </si>
+  <si>
+    <t>95aa3c19-e160-485e-a085-ac883cff8162</t>
+  </si>
+  <si>
+    <t>d8402606-7b3d-4892-809b-5bfae72697ca</t>
+  </si>
+  <si>
+    <t>a3f29ad4-58f4-4197-b8d9-47d5fd0032f6</t>
   </si>
   <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
@@ -627,7 +627,7 @@
     <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
   <si>
-    <t>353678b9-9a62-4dab-bdc0-f83a58107132</t>
+    <t>33002cfe-91b5-4229-8808-b6204c335c5a</t>
   </si>
   <si>
     <t>Mandatory field CONSENT is empty</t>

</xml_diff>

<commit_message>
feat: add fields PHONE and SSN in demographic data #178
</commit_message>
<xml_diff>
--- a/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
+++ b/support/assurance/ahc-hrsn-elt/screening/results-test-e2e/diagnostics.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>orch_session_id</t>
   </si>
@@ -42,7 +42,7 @@
     <t>ingest_table_name</t>
   </si>
   <si>
-    <t>elaboration_1</t>
+    <t>elaboration:1</t>
   </si>
   <si>
     <t>orch_session_issue_id</t>
@@ -66,13 +66,13 @@
     <t>remediation</t>
   </si>
   <si>
-    <t>elaboration_2</t>
+    <t>elaboration:2</t>
   </si>
   <si>
     <t>disposition</t>
   </si>
   <si>
-    <t>remediation_1</t>
+    <t>remediation:1</t>
   </si>
   <si>
     <t>05269d28-15ae-5bd6-bd88-f949ccfa52d7</t>
@@ -81,160 +81,217 @@
     <t>7bab389e-54af-5a13-a39f-079abdc73a48</t>
   </si>
   <si>
-    <t>0.23.7</t>
+    <t>0.30.1</t>
   </si>
   <si>
     <t>Session 05269d28-15ae-5bd6-bd88-f949ccfa52d7 markdown diagnostics not provided (not completed?)</t>
   </si>
   <si>
+    <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/DEMOGRAPHIC_DATA_qcs-test-20240531-testcase1.csv</t>
+  </si>
+  <si>
+    <t>admin_demographics_qcs_test_20240531_testcase1</t>
+  </si>
+  <si>
+    <t>39528fc7-f7be-4f39-bb69-4fc384283adb</t>
+  </si>
+  <si>
+    <t>Missing Mandatory Value</t>
+  </si>
+  <si>
+    <t>Mandatory field MPI_ID is empty</t>
+  </si>
+  <si>
+    <t>MPI_ID</t>
+  </si>
+  <si>
+    <t>Provide a value for MPI_ID</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Resolved By QE/QCS</t>
+  </si>
+  <si>
+    <t>8b7c669c-1795-5f6b-8f3a-3e502b74c628</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/QE_ADMIN_DATA_qcs-test-20240531-testcase1.csv</t>
+  </si>
+  <si>
+    <t>qe_admin_data_qcs_test_20240531_testcase1</t>
+  </si>
+  <si>
+    <t>58095c08-ceb3-44f7-9b7b-6864aae4081e</t>
+  </si>
+  <si>
+    <t>Invalid Value</t>
+  </si>
+  <si>
+    <t>Value SCN in ORGANIZATION_TYPE not in allowed list ('prov','dept','team','govt','ins','pay','edu','reli','crs','cg','bus','other','laboratory','imaging','pharmacy','health-information-network','health-data-aggregator')</t>
+  </si>
+  <si>
+    <t>ORGANIZATION_TYPE</t>
+  </si>
+  <si>
+    <t>SCN</t>
+  </si>
+  <si>
+    <t>Use only allowed values 'prov','dept','team','govt','ins','pay','edu','reli','crs','cg','bus','other','laboratory','imaging','pharmacy','health-information-network','health-data-aggregator' in ORGANIZATION_TYPE</t>
+  </si>
+  <si>
     <t>641dff51-97fd-56b3-8443-c1ed568a6d66</t>
   </si>
   <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
+  </si>
+  <si>
+    <t>Sheet Missing</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>47277588-99e8-59f5-8384-b24344a86073</t>
+  </si>
+  <si>
+    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
+  </si>
+  <si>
+    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
+  </si>
+  <si>
+    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Question_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
+  </si>
+  <si>
+    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
+  </si>
+  <si>
+    <t>99e72a60-96ab-5ef1-a3af-3e7759777664</t>
+  </si>
+  <si>
+    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
+  </si>
+  <si>
+    <t>e36daa69-3c63-5384-b6a7-03fa3b00641d</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Admin_Demographic' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>89f7ec04-277a-5799-afaa-a70d0f2a8ed5</t>
+  </si>
+  <si>
+    <t>c60cf3db-b1bf-5103-b278-b0c128ce924a</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Screening' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>b2a7c7e8-5ffe-5f28-8112-4eb7abb6397f</t>
+  </si>
+  <si>
+    <t>b10e248d-8c94-59ec-83fc-a1249dd3b111</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>5222b730-9add-5b52-b0c9-6f2506b0af9d</t>
+  </si>
+  <si>
+    <t>fa7874f6-f848-572b-a9ab-9db4c8d5e959</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Question_Reference' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>c302047e-21cf-5059-a32c-e81a9bd3a9b9</t>
+  </si>
+  <si>
+    <t>3252fee6-3a9a-5f4c-81c6-739201046d79</t>
+  </si>
+  <si>
+    <t>Excel workbook sheet 'Answer_Reference' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
+  </si>
+  <si>
+    <t>78d6a904-035e-54ae-8ac2-ca5cdf3f75f7</t>
+  </si>
+  <si>
     <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx</t>
   </si>
   <si>
-    <t>ERROR</t>
-  </si>
-  <si>
-    <t>d70a4700-6b40-52fc-a7a2-69ef0d7f69ff</t>
-  </si>
-  <si>
-    <t>Sheet Missing</t>
+    <t>9860873a-c387-5d98-9930-4ff296eb7192</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Admin_Demographic' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
   </si>
   <si>
-    <t>47277588-99e8-59f5-8384-b24344a86073</t>
-  </si>
-  <si>
-    <t>58b22e99-5854-53bf-adbe-08e67df99b85</t>
+    <t>d5d6e25d-81b4-5f98-8b91-ea2dbc155a9c</t>
+  </si>
+  <si>
+    <t>46171763-bd21-57a8-a403-0785f72643cf</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Screening' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
   </si>
   <si>
-    <t>a26ce332-3ced-5623-861d-23a2ef78e4a9</t>
-  </si>
-  <si>
-    <t>bc0c03b5-d1ba-5301-850f-5e4c42c1bf09</t>
+    <t>4971a2f5-06a3-5898-823d-364145d3b9a5</t>
+  </si>
+  <si>
+    <t>c2c0cbca-70cb-54f6-9dc7-66b47c4f3157</t>
   </si>
   <si>
     <t>Excel workbook sheet 'QE_Admin_Data' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
   </si>
   <si>
-    <t>ae477ba1-c7f1-5f34-847a-50bddb7130aa</t>
-  </si>
-  <si>
-    <t>8aad9cfa-b1a2-5fb1-a6ab-613a79a7e839</t>
+    <t>8640a4b5-53ef-506e-bcde-83f00315d4b2</t>
+  </si>
+  <si>
+    <t>544998d3-58c5-5f65-9dc8-9f998508495f</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Question_Reference' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
   </si>
   <si>
-    <t>b41ccd27-9a4f-5cc8-9c5d-b55242d90fb0</t>
-  </si>
-  <si>
-    <t>7ef8bdeb-fd56-5eb9-a09b-ef15ce18dc49</t>
+    <t>0adb81bc-3df2-5f86-99cc-2d20e1dd5efd</t>
+  </si>
+  <si>
+    <t>10d0290c-b2eb-581e-b627-b5b8fcbb830f</t>
   </si>
   <si>
     <t>Excel workbook sheet 'Answer_Reference' not found in 'JRCHC_SDOH HEL_Report 2452_ran 020124DeIdent.xlsx' (available: JRCHC_SDOH HEL_Report 2452_ran )</t>
-  </si>
-  <si>
-    <t>86b4a49e-7378-5159-9f41-b005208c31bc</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/jrchc-hrsn-file-spec.xlsx</t>
-  </si>
-  <si>
-    <t>a530fe1b-57ef-5a90-8bea-835ece2483da</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Admin_Demographic' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
-  </si>
-  <si>
-    <t>a3fe7098-8ae8-5612-81ac-cbe10780c19b</t>
-  </si>
-  <si>
-    <t>99e72a60-96ab-5ef1-a3af-3e7759777664</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Screening' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
-  </si>
-  <si>
-    <t>e36daa69-3c63-5384-b6a7-03fa3b00641d</t>
-  </si>
-  <si>
-    <t>89f7ec04-277a-5799-afaa-a70d0f2a8ed5</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
-  </si>
-  <si>
-    <t>c60cf3db-b1bf-5103-b278-b0c128ce924a</t>
-  </si>
-  <si>
-    <t>b2a7c7e8-5ffe-5f28-8112-4eb7abb6397f</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Question_Reference' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
-  </si>
-  <si>
-    <t>b10e248d-8c94-59ec-83fc-a1249dd3b111</t>
-  </si>
-  <si>
-    <t>5222b730-9add-5b52-b0c9-6f2506b0af9d</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Answer_Reference' not found in 'jrchc-hrsn-file-spec.xlsx' (available: Original Report, HeL LOINC Mapping)</t>
-  </si>
-  <si>
-    <t>fa7874f6-f848-572b-a9ab-9db4c8d5e959</t>
-  </si>
-  <si>
-    <t>support/assurance/ahc-hrsn-elt/screening/synthetic-content/synthetic-fail-excel-01.xlsx</t>
-  </si>
-  <si>
-    <t>c302047e-21cf-5059-a32c-e81a9bd3a9b9</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Admin_Demographic' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>3252fee6-3a9a-5f4c-81c6-739201046d79</t>
-  </si>
-  <si>
-    <t>78d6a904-035e-54ae-8ac2-ca5cdf3f75f7</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Screening' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>9860873a-c387-5d98-9930-4ff296eb7192</t>
-  </si>
-  <si>
-    <t>d5d6e25d-81b4-5f98-8b91-ea2dbc155a9c</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'QE_Admin_Data' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>46171763-bd21-57a8-a403-0785f72643cf</t>
-  </si>
-  <si>
-    <t>4971a2f5-06a3-5898-823d-364145d3b9a5</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Question_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
-  </si>
-  <si>
-    <t>c2c0cbca-70cb-54f6-9dc7-66b47c4f3157</t>
-  </si>
-  <si>
-    <t>8640a4b5-53ef-506e-bcde-83f00315d4b2</t>
-  </si>
-  <si>
-    <t>Excel workbook sheet 'Answer_Reference' not found in 'synthetic-fail-excel-01.xlsx' (available: Sheet1)</t>
   </si>
 </sst>
 </file>
@@ -410,8 +467,20 @@
       <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
-        <v>26</v>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -428,25 +497,37 @@
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" t="s">
         <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -463,25 +544,25 @@
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="Q4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -498,25 +579,25 @@
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="Q5" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -533,25 +614,25 @@
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L6" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="Q6" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7">
@@ -568,25 +649,25 @@
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
         <v>45</v>
-      </c>
-      <c r="M7" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="8">
@@ -603,25 +684,25 @@
         <v>24</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="Q8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
@@ -638,25 +719,25 @@
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="I9" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="J9" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L9" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="Q9" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10">
@@ -673,25 +754,25 @@
         <v>24</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L10" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="M10" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="Q10" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11">
@@ -708,25 +789,25 @@
         <v>24</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L11" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="M11" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N11" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="Q11" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12">
@@ -743,25 +824,25 @@
         <v>24</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="M12" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N12" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="Q12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -778,25 +859,25 @@
         <v>24</v>
       </c>
       <c r="H13" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" t="s">
         <v>63</v>
       </c>
-      <c r="I13" t="s">
-        <v>60</v>
-      </c>
       <c r="J13" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="M13" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N13" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="Q13" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -813,25 +894,25 @@
         <v>24</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="M14" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N14" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="Q14" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
@@ -848,25 +929,25 @@
         <v>24</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L15" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="M15" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N15" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="Q15" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -883,25 +964,95 @@
         <v>24</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="I16" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="M16" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="N16" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="Q16" t="s">
-        <v>60</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M17" t="s">
+        <v>48</v>
+      </c>
+      <c r="N17" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" t="s">
+        <v>46</v>
+      </c>
+      <c r="L18" t="s">
+        <v>92</v>
+      </c>
+      <c r="M18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>